<commit_message>
Improvment for converting to ISO dates, treatment of Precision parameter
</commit_message>
<xml_diff>
--- a/Dev/Calendar_LambdaModule.xlsx
+++ b/Dev/Calendar_LambdaModule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dbb3931c8741440f/Projects/Datachord/Excel-Lambda-Calendar/Dev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="102901" documentId="8_{EC863CD5-8208-420A-82DC-FA001A6233C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3AF7C85F-1D7D-4AE5-8C7C-0B99ECCF8E55}"/>
+  <xr:revisionPtr revIDLastSave="113384" documentId="8_{EC863CD5-8208-420A-82DC-FA001A6233C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C646520D-1E85-428A-982D-0071F118EFC8}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="806" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="806" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CALENDAR_LOGICAL" sheetId="1" r:id="rId1"/>
@@ -23,13 +23,13 @@
     <sheet name="CALENDAR_EXTENTS" sheetId="21" r:id="rId8"/>
     <sheet name="CALENDAR_PARSING" sheetId="11" r:id="rId9"/>
     <sheet name="CALENDAR_TEXT" sheetId="12" r:id="rId10"/>
-    <sheet name="CALENDAR_Conversion_ISO" sheetId="8" r:id="rId11"/>
-    <sheet name="CALENDAR_Conversion_EDate" sheetId="13" r:id="rId12"/>
-    <sheet name="CALENDAR_Conversion_Fmts" sheetId="14" r:id="rId13"/>
+    <sheet name="CALENDAR_CONVERSION_ISO" sheetId="8" r:id="rId11"/>
+    <sheet name="CALENDAR_CONVERSION_EDATE" sheetId="13" r:id="rId12"/>
+    <sheet name="CALENDAR_CONVERSION_USDATE" sheetId="14" r:id="rId13"/>
   </sheets>
   <definedNames>
     <definedName name="CALENDAR.ADD_TIMESPAN">_xlfn.LAMBDA(_xlpm.YearCE,_xlpm.Month,_xlpm.Day,_xlpm.Time,_xlpm.AddYears,_xlpm.AddMonths,_xlpm.AddDays,_xlpm.AddTime,_xlop.TimeZoneOffset,_xlop.JulianCalendar, IF((_xlpm.YearCE = "") * (_xlpm.Month = "") * (_xlpm.Day = "") * (_xlpm.Time = ""), "", IF(NOT(ISNUMBER(_xlpm.YearCE)) + NOT(ISNUMBER(_xlpm.Month)) + NOT(ISNUMBER(_xlpm.Day)), {#VALUE!}, IF(NOT(CALENDAR.IS_VALID_DATE(_xlpm.YearCE, _xlpm.Month, _xlpm.Day, _xlpm.JulianCalendar)), {#VALUE!}, IF(MOD(_xlpm.Day, 1) &gt; 0, {#NUM!}, _xlfn.LET(_xlpm._tzo, N(_xlpm.TimeZoneOffset), IF(ABS(_xlpm._tzo) &gt; 900, {#NUM!}, _xlfn.LET(_xlpm._addYears, INT(N(_xlpm.AddYears)), _xlpm._fAddYears, N(_xlpm.AddYears) - _xlpm._addYears, _xlpm._sMonths, N(_xlpm.AddMonths) + (_xlpm._fAddYears * 12), _xlpm._addMonths, INT(_xlpm._sMonths), _xlpm._fAddMonths, _xlpm._sMonths - _xlpm._addMonths, _xlpm._zMonths, _xlpm.Month + _xlpm._addMonths - 1, _xlpm._rMonth, MOD(_xlpm._zMonths, 12) + 1, _xlpm._rYear, _xlpm.YearCE + _xlpm._addYears + INT(_xlpm._zMonths / 12), _xlpm._avgDaysMonth, IF(N(_xlpm.JulianCalendar), 30.4375, 30.436875), _xlpm._mDays, ROUND(_xlpm._fAddMonths * _xlpm._avgDaysMonth, 0), _xlpm._baseJDate, CALENDAR.JULIAN_DATE(_xlpm._rYear, _xlpm._rMonth, 1, 0, _xlpm._tzo, _xlpm.JulianCalendar) - 1, _xlpm._sDays, _xlpm.Day + _xlpm._mDays + N(_xlpm.AddDays) + N(_xlpm.Time) + N(_xlpm.AddTime), _xlpm._baseJDate + _xlpm._sDays))))))))</definedName>
-    <definedName name="CALENDAR.CALENDAR_FROM_JDATE">_xlfn.LAMBDA(_xlpm.JDate,_xlop.TimeZoneOffset,_xlop.Precision,_xlop.JulianCalendar, IF(_xlpm.JDate = "", {"","","",""}, IF(NOT(ISNUMBER(_xlpm.JDate)), {#VALUE!,#VALUE!,#VALUE!,#VALUE!}, _xlfn.LET(_xlpm._jdnLocal, CALENDAR.JDATE_TO_JDN_LOCAL(_xlpm.JDate, _xlpm.TimeZoneOffset), IF(ISERROR(INDEX(_xlpm._jdnLocal, 1, 1)), {#NUM!,#NUM!,#NUM!,#NUM!}, _xlfn.LET(_xlpm._precision, N(_xlpm.Precision), _xlpm._localTime, _xlfn.IFS(_xlpm._precision &lt;= 0, INDEX(_xlpm._jdnLocal, 1, 2), _xlpm._precision = 1, ROUND(INDEX(_xlpm._jdnLocal, 1, 2), 0), _xlpm._precision = 2, ROUND(INDEX(_xlpm._jdnLocal, 1, 2) * 24, 0) / 24, _xlpm._precision = 3, ROUND(INDEX(_xlpm._jdnLocal, 1, 2) * 1440, 0) / 1440, _xlpm._precision = 4, ROUND(INDEX(_xlpm._jdnLocal, 1, 2) * 86400, 0) / 86400, TRUE, ROUND(INDEX(_xlpm._jdnLocal, 1, 2) * 86400000, 0) / 86400000), _xlpm._rLocalTime, MOD(_xlpm._localTime, 1), _xlpm._rJDN, INDEX(_xlpm._jdnLocal, 1, 1) + INT(_xlpm._localTime), _xlpm._localDate, CALENDAR.JDN_TO_CALENDAR_DATE(_xlpm._rJDN, _xlpm.JulianCalendar), _xlfn.HSTACK(_xlpm._localDate, _xlpm._rLocalTime)))))))</definedName>
+    <definedName name="CALENDAR.CALENDAR_FROM_JDATE">_xlfn.LAMBDA(_xlpm.JDate,_xlop.TimeZoneOffset,_xlop.Precision,_xlop.JulianCalendar, IF(_xlpm.JDate = "", {"","","",""}, IF(NOT(ISNUMBER(_xlpm.JDate)), {#VALUE!,#VALUE!,#VALUE!,#VALUE!}, _xlfn.LET(_xlpm._jdnLocal, CALENDAR.JDATE_TO_JDN_LOCAL(_xlpm.JDate, _xlpm.TimeZoneOffset), IF(ISERROR(INDEX(_xlpm._jdnLocal, 1, 1)), {#NUM!,#NUM!,#NUM!,#NUM!}, _xlfn.LET(_xlpm._precision, N(_xlpm.Precision), _xlpm._localTime, _xlfn.IFS(_xlpm._precision &lt;= 0, INDEX(_xlpm._jdnLocal, 1, 2), _xlpm._precision = 1, ROUND(INDEX(_xlpm._jdnLocal, 1, 2), 0), _xlpm._precision = 2, ROUND(INDEX(_xlpm._jdnLocal, 1, 2) * 24, 0) / 24, _xlpm._precision = 3, ROUND(INDEX(_xlpm._jdnLocal, 1, 2) * 1440, 0) / 1440, _xlpm._precision = 4, ROUND(INDEX(_xlpm._jdnLocal, 1, 2) * 86400, 0) / 86400, TRUE, ROUND(INDEX(_xlpm._jdnLocal, 1, 2) * 86400, 3) / 86400), _xlpm._rLocalTime, MOD(_xlpm._localTime, 1), _xlpm._rJDN, INDEX(_xlpm._jdnLocal, 1, 1) + INT(_xlpm._localTime), _xlpm._localDate, CALENDAR.JDN_TO_CALENDAR_DATE(_xlpm._rJDN, _xlpm.JulianCalendar), _xlfn.HSTACK(_xlpm._localDate, _xlpm._rLocalTime)))))))</definedName>
     <definedName name="CALENDAR.CONVERT_WEEKDAY_NUMBER">_xlfn.LAMBDA(_xlpm.DayOfWeek,_xlop.ISOtoTraditional, IF(_xlpm.DayOfWeek = "", "", IF(NOT(ISNUMBER(_xlpm.DayOfWeek)), {#VALUE!}, _xlfn.LET(_xlpm._givenDoW, INT(N(_xlpm.DayOfWeek)), _xlpm._fromISO, N(_xlpm.ISOtoTraditional) &lt;&gt; 0, _xlpm._shiftDoW, _xlpm._givenDoW + IF(_xlpm._fromISO, 0, -2), MOD(_xlpm._shiftDoW, 7) + 1))))</definedName>
     <definedName name="CALENDAR.DAY_OF_WEEK">_xlfn.LAMBDA(_xlpm.JDN, IF(_xlpm.JDN = "", "", IF(NOT(ISNUMBER(_xlpm.JDN)), {#VALUE!}, _xlfn.LET(_xlpm._jdn, INT(_xlpm.JDN), MOD(_xlpm._jdn, 7) + 1))))</definedName>
     <definedName name="CALENDAR.DAYS_IN_MONTH">_xlfn.LAMBDA(_xlpm.Month,_xlop.YearCE,_xlop.JulianCalendar, IF(_xlpm.Month = "", "", IF(NOT(ISNUMBER(_xlpm.Month)), {#VALUE!}, _xlfn.LET(_xlpm._month, INT(_xlpm.Month), _xlfn.IFS(_xlpm._month &lt; 1, {#NUM!}, _xlpm._month &gt; 12, {#NUM!}, _xlpm._month = 2, _xlfn.LET(_xlpm._leapDay, IF(ISNUMBER(_xlpm.YearCE), N(CALENDAR.IS_LEAP_YEAR(_xlpm.YearCE, _xlpm.JulianCalendar)), 0), 28 + _xlpm._leapDay), _xlpm._month &lt;= 7, 30 + MOD(_xlpm._month, 2), TRUE, 31 - MOD(_xlpm._month, 2))))))</definedName>
@@ -58,11 +58,11 @@
     <definedName name="CALENDAR.EXTENT_OF_QUARTERS">_xlfn.LAMBDA(_xlpm.JDate1,_xlpm.JDate2,_xlop.TimeZoneOffset,_xlop.MonthOffset,_xlop.JulianCalendar, IF((_xlpm.JDate1 = "") * (_xlpm.JDate2 = ""), "", IF(NOT(ISNUMBER(_xlpm.JDate1)) + NOT(ISNUMBER(_xlpm.JDate2)), {#VALUE!}, _xlfn.LET(_xlpm._tzo, N(_xlpm.TimeZoneOffset), _xlpm._monthOffset, ROUND(N(_xlpm.MonthOffset), 0), IF((ABS(_xlpm._tzo) &gt; 900) + (_xlpm._monthOffset &lt; -6) + (_xlpm._monthOffset &gt; 3), {#NUM!}, _xlfn.LET(_xlpm._sign, IF(_xlpm.JDate2 &gt;= _xlpm.JDate1, 1, -1), _xlpm._jdnLocal_Start, CALENDAR.JDATE_TO_JDN_LOCAL(IF(_xlpm._sign = 1, _xlpm.JDate1, _xlpm.JDate2), _xlpm._tzo), _xlpm._jdnLocal_End, CALENDAR.JDATE_TO_JDN_LOCAL(IF(_xlpm._sign = 1, _xlpm.JDate2, _xlpm.JDate1), _xlpm._tzo), _xlpm._quarterDate_Start, CALENDAR.JDN_TO_QUARTER_DATE(INDEX(_xlpm._jdnLocal_Start, 1, 1), _xlpm._monthOffset, _xlpm.JulianCalendar), _xlpm._quarterDate_End, CALENDAR.JDN_TO_QUARTER_DATE(INDEX(_xlpm._jdnLocal_End, 1, 1), _xlpm._monthOffset, _xlpm.JulianCalendar), _xlpm._deltaYear, INDEX(_xlpm._quarterDate_End, 1, 1) - INDEX(_xlpm._quarterDate_Start, 1, 1), _xlpm._deltaQuarter, INDEX(_xlpm._quarterDate_End, 1, 2) - INDEX(_xlpm._quarterDate_Start, 1, 2), _xlpm._diffQuarters, (_xlpm._deltaYear * 4) + _xlpm._deltaQuarter, _xlpm._sign * (_xlpm._diffQuarters + 1)))))))</definedName>
     <definedName name="CALENDAR.EXTENT_OF_WEEKS">_xlfn.LAMBDA(_xlpm.JDate1,_xlpm.JDate2,_xlop.TimeZoneOffset, IF((_xlpm.JDate1 = "") * (_xlpm.JDate2 = ""), "", IF(NOT(ISNUMBER(_xlpm.JDate1)) + NOT(ISNUMBER(_xlpm.JDate2)), {#VALUE!}, _xlfn.LET(_xlpm._tzo, N(_xlpm.TimeZoneOffset), IF(ABS(_xlpm._tzo) &gt; 900, {#NUM!}, _xlfn.LET(_xlpm._sign, IF(_xlpm.JDate2 &gt;= _xlpm.JDate1, 1, -1), _xlpm._jdnLocal_Start, CALENDAR.JDATE_TO_JDN_LOCAL(IF(_xlpm._sign = 1, _xlpm.JDate1, _xlpm.JDate2), _xlpm._tzo), _xlpm._jdnLocal_End, CALENDAR.JDATE_TO_JDN_LOCAL(IF(_xlpm._sign = 1, _xlpm.JDate2, _xlpm.JDate1), _xlpm._tzo), _xlpm._jdnMonday_Start, INDEX(_xlpm._jdnLocal_Start, 1, 1) + 1 - CALENDAR.DAY_OF_WEEK(INDEX(_xlpm._jdnLocal_Start, 1, 1)), _xlpm._jdnMonday_End, INDEX(_xlpm._jdnLocal_End, 1, 1) + 1 - CALENDAR.DAY_OF_WEEK(INDEX(_xlpm._jdnLocal_End, 1, 1)), _xlpm._sign * INT((_xlpm._jdnMonday_End - _xlpm._jdnMonday_Start) / 7 + 1)))))))</definedName>
     <definedName name="CALENDAR.EXTENT_OF_YEARS">_xlfn.LAMBDA(_xlpm.JDate1,_xlpm.JDate2,_xlop.TimeZoneOffset,_xlop.JulianCalendar, IF((_xlpm.JDate1 = "") * (_xlpm.JDate2 = ""), "", IF(NOT(ISNUMBER(_xlpm.JDate1)) + NOT(ISNUMBER(_xlpm.JDate2)), {#VALUE!}, _xlfn.LET(_xlpm._tzo, N(_xlpm.TimeZoneOffset), IF((ABS(_xlpm._tzo) &gt; 900), {#NUM!}, _xlfn.LET(_xlpm._sign, IF(_xlpm.JDate2 &gt;= _xlpm.JDate1, 1, -1), _xlpm._jdnLocal_Start, CALENDAR.JDATE_TO_JDN_LOCAL(IF(_xlpm._sign = 1, _xlpm.JDate1, _xlpm.JDate2), _xlpm._tzo), _xlpm._jdnLocal_End, CALENDAR.JDATE_TO_JDN_LOCAL(IF(_xlpm._sign = 1, _xlpm.JDate2, _xlpm.JDate1), _xlpm._tzo), _xlpm._date_Start, CALENDAR.JDN_TO_CALENDAR_DATE(INDEX(_xlpm._jdnLocal_Start, 1, 1), _xlpm.JulianCalendar), _xlpm._date_End, CALENDAR.JDN_TO_CALENDAR_DATE(INDEX(_xlpm._jdnLocal_End, 1, 1), _xlpm.JulianCalendar), _xlpm._deltaYear, INDEX(_xlpm._date_End, 1, 1) - INDEX(_xlpm._date_Start, 1, 1), _xlpm._sign * (_xlpm._deltaYear + 1)))))))</definedName>
-    <definedName name="CALENDAR.FORMAT_ISO_DATE">_xlfn.LAMBDA(_xlpm.YearCE,_xlpm.Month,_xlpm.Day,_xlop.Time,_xlop.TimeZoneOffset,_xlop.Precision,_xlop.NoZulu,_xlop.JulianCalendar, IF((_xlpm.YearCE = "") * (_xlpm.Month = "") * (_xlpm.Day = ""), "", IF(NOT(ISNUMBER(_xlpm.YearCE)) + NOT(ISNUMBER(_xlpm.Month)) + NOT(ISNUMBER(_xlpm.Day)), {#VALUE!}, IF(NOT(CALENDAR.IS_VALID_DATE(_xlpm.YearCE, _xlpm.Month, _xlpm.Day, _xlpm.JulianCalendar)), {#VALUE!}, _xlfn.LET(_xlpm.fnResolveTime, _xlfn.LAMBDA(_xlpm._time, IF(NOT(ISNUMBER(_xlpm._time)), _xlfn.HSTACK(_xlpm.YearCE, _xlpm.Month, _xlpm.Day, ""), _xlfn.LET(_xlpm._usePrecision, IF(N(_xlpm.Precision) &gt; 5, 5, 4), CALENDAR.RESOLVE_DATE(_xlpm.YearCE, _xlpm.Month, _xlpm.Day, _xlpm._time, _xlpm._usePrecision, _xlpm.JulianCalendar)))), _xlpm.fnFormatYear, _xlfn.LAMBDA(_xlpm._year, _xlfn.LET(_xlpm._yearFmt, IF((_xlpm._year &gt;= 1000) * (_xlpm._year &lt;= 9999), "0000;" &amp; _xlfn.UNICHAR(8722) &amp; "0000", "+0000;" &amp; _xlfn.UNICHAR(8722) &amp; "0000;+0000"), TEXT(_xlpm._year, _xlpm._yearFmt))), _xlpm.fnFormatTime, _xlfn.LAMBDA(_xlpm._time, IF(NOT(ISNUMBER(_xlpm._time)), "", _xlfn.LET(_xlpm._seconds, ROUND(_xlpm._time * 86400, 3), _xlpm._showPrecision, IF(N(_xlpm.Precision) &gt; 0, _xlpm.Precision, _xlfn.IFS(_xlpm._seconds = 0, 2, MOD(_xlpm._seconds, 1) &gt; 0, 5, MOD(_xlpm._seconds / 60, 1) &gt; 0, 4, MOD(_xlpm._seconds / 3600, 1) &gt; 0, 3, TRUE, 2)), IF(_xlpm._showPrecision = 1, "", _xlfn.LET(_xlpm._fmt, _xlfn.IFS(_xlpm._showPrecision = 2, "HH", _xlpm._showPrecision = 3, "HH:mm", _xlpm._showPrecision = 4, "HH:mm:ss", TRUE, "HH:mm:ss.000"), "T" &amp; TEXT(_xlpm._time, _xlpm._fmt)))))), _xlpm.fnFormatTZ, _xlfn.LAMBDA(_xlpm._tzo, IF(NOT(ISNUMBER(_xlpm._tzo)), "", IF((_xlpm._tzo = 0) * (N(_xlpm.NoZulu) = 0), "Z", _xlfn.LET(_xlpm._tzFmt, IF(MOD(_xlpm._tzo, 1) = 0, "HH:mm", "HH:mm:ss"), _xlpm._sign, IF(_xlpm._tzo &gt;= 0, "+", _xlfn.UNICHAR(8722)), _xlpm._sign &amp; TEXT(ABS(_xlpm._tzo) / 1440, _xlpm._tzFmt))))), _xlpm._rDate, _xlpm.fnResolveTime(_xlpm.Time), _xlpm._sYear, _xlpm.fnFormatYear(INDEX(_xlpm._rDate, 1, 1)), _xlpm._sMonth, TEXT(INDEX(_xlpm._rDate, 1, 2), "00"), _xlpm._sDay, TEXT(INDEX(_xlpm._rDate, 1, 3), "00"), _xlpm._sTime, _xlpm.fnFormatTime(INDEX(_xlpm._rDate, 1, 4)), _xlpm._sTZ, _xlpm.fnFormatTZ(_xlpm.TimeZoneOffset), _xlfn.CONCAT(_xlpm._sYear, "-", _xlpm._sMonth, "-", _xlpm._sDay, _xlpm._sTime, _xlpm._sTZ))))))</definedName>
+    <definedName name="CALENDAR.FORMAT_ISO_DATE">_xlfn.LAMBDA(_xlpm.YearCE,_xlpm.Month,_xlpm.Day,_xlop.Time,_xlop.TimeZoneOffset,_xlop.Precision,_xlop.NoZulu,_xlop.JulianCalendar, IF((_xlpm.YearCE = "") * (_xlpm.Month = "") * (_xlpm.Day = ""), "", IF(NOT(ISNUMBER(_xlpm.YearCE)) + NOT(ISNUMBER(_xlpm.Month)) + NOT(ISNUMBER(_xlpm.Day)), {#VALUE!}, IF(NOT(CALENDAR.IS_VALID_DATE(_xlpm.YearCE, _xlpm.Month, _xlpm.Day, _xlpm.JulianCalendar)), {#VALUE!}, _xlfn.LET(_xlpm.fnFormatYear, _xlfn.LAMBDA(_xlpm._year, _xlfn.LET(_xlpm._yearFmt, IF((_xlpm._year &gt;= 1000) * (_xlpm._year &lt;= 9999), "0000;" &amp; _xlfn.UNICHAR(8722) &amp; "0000", "+0000;" &amp; _xlfn.UNICHAR(8722) &amp; "0000;+0000"), TEXT(_xlpm._year, _xlpm._yearFmt))), _xlpm.fnFormatTime, _xlfn.LAMBDA(_xlpm._time,_xlpm._precision, IF(_xlpm._precision = 1, "", _xlfn.LET(_xlpm._showPrecision, IF(_xlpm._precision &gt; 1, _xlpm._precision, _xlfn.LET(_xlpm._seconds, ROUND(_xlpm._time * 86400, 3), _xlfn.IFS(_xlpm._seconds = 0, 3, MOD(_xlpm._seconds, 1) &gt; 0, 5, MOD(_xlpm._seconds / 60, 1) &gt; 0, 4, TRUE, 3))), IF(_xlpm._showPrecision = 1, "", _xlfn.LET(_xlpm._fmt, _xlfn.IFS(_xlpm._showPrecision = 2, "HH", _xlpm._showPrecision = 3, "HH:mm", _xlpm._showPrecision = 4, "HH:mm:ss", TRUE, "HH:mm:ss.000"), "T" &amp; TEXT(_xlpm._time, _xlpm._fmt)))))), _xlpm.fnFormatTZ, _xlfn.LAMBDA(_xlpm._tzo, IF(NOT(ISNUMBER(_xlpm._tzo)), "", IF((_xlpm._tzo = 0) * (N(_xlpm.NoZulu) = 0), "Z", _xlfn.LET(_xlpm._tzFmt, IF(MOD(_xlpm._tzo, 1) = 0, "HH:mm", "HH:mm:ss"), _xlpm._sign, IF(_xlpm._tzo &gt;= 0, "+", _xlfn.UNICHAR(8722)), _xlpm._sign &amp; TEXT(ABS(_xlpm._tzo) / 1440, _xlpm._tzFmt))))), _xlpm._hasTime, ((MOD(_xlpm.Day, 1) &gt; 0) + ISNUMBER(_xlpm.Time)) &gt; 0, _xlpm._usePrecision, _xlfn.IFS(NOT(_xlpm._hasTime), 1, NOT(ISNUMBER(_xlpm.Precision)), 3, TRUE, INT(_xlpm.Precision)), _xlpm._rDate, CALENDAR.RESOLVE_DATE(_xlpm.YearCE, _xlpm.Month, _xlpm.Day, _xlpm.Time, _xlpm._usePrecision, _xlpm.JulianCalendar), _xlpm._sYear, _xlpm.fnFormatYear(INDEX(_xlpm._rDate, 1, 1)), _xlpm._sMonth, TEXT(INDEX(_xlpm._rDate, 1, 2), "00"), _xlpm._sDay, TEXT(INDEX(_xlpm._rDate, 1, 3), "00"), _xlpm._sTime, _xlpm.fnFormatTime(INDEX(_xlpm._rDate, 1, 4), _xlpm._usePrecision), _xlpm._sTZ, _xlpm.fnFormatTZ(_xlpm.TimeZoneOffset), _xlfn.CONCAT(_xlpm._sYear, "-", _xlpm._sMonth, "-", _xlpm._sDay, _xlpm._sTime, _xlpm._sTZ))))))</definedName>
     <definedName name="CALENDAR.FORMAT_LITERARY_DATE">_xlfn.LAMBDA(_xlpm.YearCE,_xlpm.Month,_xlpm.Day,_xlop.Time,_xlop.Short,_xlop.InternationalEnglish,_xlop.AlwaysShowEra,_xlop.JulianCalendar, IF((_xlpm.YearCE = "") * (_xlpm.Month = "") * (_xlpm.Day = ""), "", IF(NOT(ISNUMBER(_xlpm.Month)) + (NOT(ISNUMBER(_xlpm.YearCE)) * NOT(ISNUMBER(_xlpm.Day))), #VALUE!, _xlfn.LET(_xlpm._yearCE, IF(_xlpm.YearCE = "", 2000, _xlpm.YearCE), _xlpm._day, IF(_xlpm.Day = "", 1, _xlpm.Day), IF(NOT(CALENDAR.IS_VALID_DATE(_xlpm._yearCE, _xlpm.Month, _xlpm._day, _xlpm.JulianCalendar)), #VALUE!, _xlfn.LET(_xlpm._rDate, IF(NOT(ISNUMBER(_xlpm.Time)), _xlfn.HSTACK(_xlpm._yearCE, _xlpm.Month, _xlpm._day, ""), CALENDAR.RESOLVE_DATE(_xlpm._yearCE, _xlpm.Month, _xlpm._day, _xlpm.Time, 3, _xlpm.JulianCalendar)), _xlpm._sMonth, CALENDAR.MONTH_NAME(INDEX(_xlpm._rDate, 1, 2), _xlpm.Short, _xlpm.InternationalEnglish), _xlpm._sDay, IF(ISNUMBER(_xlpm.Day), " " &amp; INDEX(_xlpm._rDate, 1, 3), ""), _xlpm._sYear, IF(ISNUMBER(_xlpm.YearCE), ", " &amp; CALENDAR.FORMAT_LITERARY_YEAR(INDEX(_xlpm._rDate, 1, 1), _xlpm.AlwaysShowEra), ""), _xlpm._sTime, IF(ISNUMBER(_xlpm.Time), ", " &amp; TEXT(INDEX(_xlpm._rDate, 1, 4), "h:mm AM/PM"), ""), _xlfn.CONCAT(_xlpm._sMonth, _xlpm._sDay, _xlpm._sYear, _xlpm._sTime)))))))</definedName>
     <definedName name="CALENDAR.FORMAT_LITERARY_YEAR">_xlfn.LAMBDA(_xlpm.YearCE,_xlop.AlwaysShowEra, IF(_xlpm.YearCE = "", "", _xlfn.LET(_xlpm._yearCE, INT(_xlpm.YearCE), _xlpm._isCE, _xlpm._yearCE &gt;= 1, _xlpm._year, IF(_xlpm._isCE, _xlpm._yearCE, 1 - _xlpm._yearCE), _xlpm._suffix, _xlfn.IFS(NOT(_xlpm._isCE), " BCE", _xlpm._yearCE &lt; 1000, " CE", N(_xlpm.AlwaysShowEra) &lt;&gt; 0, " CE", TRUE, ""), _xlpm._year &amp; _xlpm._suffix)))</definedName>
     <definedName name="CALENDAR.FORMAT_MIL_DTG">_xlfn.LAMBDA(_xlpm.Year,_xlpm.Month,_xlpm.Day,_xlpm.Time,_xlop.TimeZoneOffset,_xlop.Short, IF((_xlpm.Year = "") * (_xlpm.Month = "") * (_xlpm.Day = "") * (_xlpm.Time = ""), "", IF(NOT(ISNUMBER(_xlpm.Day)), {#VALUE!}, _xlfn.LET(_xlpm._local, _xlpm.TimeZoneOffset = "", _xlpm._tzo, N(_xlpm.TimeZoneOffset), _xlpm.fnInvalidParams, _xlfn.LAMBDA(_xlfn.IFS(ABS(_xlpm._tzo) &gt; 900, TRUE, IF(ISNUMBER(_xlpm.Year), ((_xlpm.Year &lt; 1951) + (_xlpm.Year &gt; 2050)), FALSE), TRUE, (((_xlpm.Year = "") * (_xlpm.Month = "")) + N(CALENDAR.IS_VALID_DATE(_xlpm.Year, _xlpm.Month, _xlpm.Day, 0))) = 0, TRUE, TRUE, FALSE)), _xlpm.fnFmtTime, _xlfn.LAMBDA(_xlpm._time,_xlpm._short, _xlfn.LET(_xlpm._timeFmt, IF(_xlpm._short, "HHmm", "HHmmss"), TEXT(_xlpm._time, _xlpm._timeFmt))), _xlpm.fnResolveMilitaryTZ, _xlfn.LAMBDA(_xlfn.IFS(_xlpm._local, _xlfn.HSTACK(N(_xlpm.Time), "J"), _xlpm._tzo &gt; 720, _xlfn.LET(_xlpm._shiftTZO, _xlpm._tzo - 720, _xlpm._time, N(_xlpm.Time) - (_xlpm._shiftTZO / 1440), _xlfn.HSTACK(_xlpm._time, "M")), _xlpm._tzo &lt; -720, _xlfn.LET(_xlpm._shiftTZO, _xlpm._tzo + 720, _xlpm._time, N(_xlpm.Time) - (_xlpm._shiftTZO / 1440), _xlfn.HSTACK(_xlpm._time, "Y")), TRUE, _xlfn.LET(_xlpm._militaryTZO, SIGN(_xlpm._tzo) * MROUND(ABS(_xlpm._tzo), 60), _xlpm._shiftTZO, _xlpm._tzo - _xlpm._militaryTZO, _xlpm._time, N(_xlpm.Time) - (_xlpm._shiftTZO / 1440), _xlpm._idx, INT(_xlpm._militaryTZO / 60) + 13, _xlpm._militaryTZ, CHOOSE(_xlpm._idx, "Y", "X", "W", "V", "U", "T", "S", "R", "Q", "P", "O", "N", "Z", "A", "B", "C", "D", "E", "F", "G", "H", "I", "K", "L", "M"), _xlfn.HSTACK(_xlpm._time, _xlpm._militaryTZ)))), IF(_xlpm.fnInvalidParams(), {"#NUM!!"}, _xlfn.LET(_xlpm._militaryTime, _xlpm.fnResolveMilitaryTZ(), _xlpm._rDate, IF(_xlpm.Year = "", CALENDAR.RESOLVE_DATE(2000, 3, _xlpm.Day, INDEX(_xlpm._militaryTime, 1, 1), 3), CALENDAR.RESOLVE_DATE(_xlpm.Year, _xlpm.Month, _xlpm.Day, INDEX(_xlpm._militaryTime, 1, 1), 3)), _xlpm._sDay, TEXT(INDEX(_xlpm._rDate, 3), "00"), IF(_xlpm.Year = "", _xlfn.CONCAT(_xlpm._sDay, _xlpm.fnFmtTime(INDEX(_xlpm._rDate, 4), 1), INDEX(_xlpm._militaryTime, 1, 2)), _xlfn.LET(_xlpm._sTime, _xlpm.fnFmtTime(INDEX(_xlpm._rDate, 4), N(_xlpm.Short)), _xlpm._sMonth, UPPER(CALENDAR.MONTH_NAME(INDEX(_xlpm._rDate, 2), 1, 1)), _xlpm._sYY, RIGHT(TEXT(INDEX(_xlpm._rDate, 1), "00"), 2), _xlfn.CONCAT(_xlpm._sDay, _xlpm._sTime, INDEX(_xlpm._militaryTime, 1, 2), _xlpm._sMonth, _xlpm._sYY)))))))))</definedName>
-    <definedName name="CALENDAR.FORMAT_US_DATE">_xlfn.LAMBDA(_xlpm.YearCE,_xlpm.Month,_xlpm.Day,_xlop.Time,_xlop.Separator,_xlop.Precision,_xlop.JulianCalendar, IF((_xlpm.YearCE = "") * (_xlpm.Month = "") * (_xlpm.Day = ""), "", IF(NOT(ISNUMBER(_xlpm.YearCE)) + NOT(ISNUMBER(_xlpm.Month)) + NOT(ISNUMBER(_xlpm.Day)), #VALUE!, IF(NOT(CALENDAR.IS_VALID_DATE(_xlpm.YearCE, _xlpm.Month, _xlpm.Day, _xlpm.JulianCalendar)), #VALUE!, _xlfn.LET(_xlpm.fnFormatTime, _xlfn.LAMBDA(_xlpm._time, IF(NOT(ISNUMBER(_xlpm._time)), "", _xlfn.LET(_xlpm._seconds, ROUND(_xlpm._time * 86400, 3), _xlpm._showPrecision, IF(N(_xlpm.Precision) &gt; 0, _xlpm.Precision, _xlfn.IFS(_xlpm._seconds = 0, 3, MOD(_xlpm._seconds, 1) &gt; 0, 5, MOD(_xlpm._seconds / 60, 1) &gt; 0, 4, TRUE, 3)), IF(_xlpm._showPrecision = 1, "", _xlfn.LET(_xlpm._fmt, _xlfn.IFS(_xlpm._showPrecision = 2, "h AM/PM", _xlpm._showPrecision = 3, "h:mm AM/PM", _xlpm._showPrecision = 4, "h:mm:ss AM/PM", TRUE, "h:mm:ss.000 AM/PM"), " " &amp; TEXT(_xlpm._time, _xlpm._fmt)))))), _xlpm._separator, IF(_xlpm.Separator = "", "/", _xlfn.LET(_xlpm._char1, LEFT(_xlpm.Separator, 1), IF(IFERROR(FIND(_xlpm._char1, ",./-_"), 0) &gt; 0, _xlpm._char1, "/"))), _xlpm._usePrecision, IF(N(_xlpm.Precision) &gt;= 5, 5, 4), _xlpm._rDate, IF(NOT(ISNUMBER(_xlpm.Time)), _xlfn.HSTACK(_xlpm.YearCE, _xlpm.Month, _xlpm.Day, ""), CALENDAR.RESOLVE_DATE(_xlpm.YearCE, _xlpm.Month, _xlpm.Day, _xlpm.Time, _xlpm._usePrecision, _xlpm.JulianCalendar)), _xlpm._sYear, TEXT(INDEX(_xlpm._rDate, 1, 1), "0000;" &amp; _xlfn.UNICHAR(8722) &amp; "0000;0000"), _xlpm._sMonth, INDEX(_xlpm._rDate, 1, 2), _xlpm._sDay, TEXT(INDEX(_xlpm._rDate, 1, 3), "00"), _xlpm._sTime, _xlpm.fnFormatTime(INDEX(_xlpm._rDate, 1, 4)), _xlfn.CONCAT(_xlpm._sMonth, _xlpm._separator, _xlpm._sDay, _xlpm._separator, _xlpm._sYear, _xlpm._sTime))))))</definedName>
+    <definedName name="CALENDAR.FORMAT_US_DATE">_xlfn.LAMBDA(_xlpm.YearCE,_xlpm.Month,_xlpm.Day,_xlop.Time,_xlop.Separator,_xlop.Precision,_xlop.JulianCalendar, IF((_xlpm.YearCE = "") * (_xlpm.Month = "") * (_xlpm.Day = ""), "", IF(NOT(ISNUMBER(_xlpm.YearCE)) + NOT(ISNUMBER(_xlpm.Month)) + NOT(ISNUMBER(_xlpm.Day)), #VALUE!, IF(NOT(CALENDAR.IS_VALID_DATE(_xlpm.YearCE, _xlpm.Month, _xlpm.Day, _xlpm.JulianCalendar)), #VALUE!, _xlfn.LET(_xlpm.fnFormatTime, _xlfn.LAMBDA(_xlpm._time,_xlpm._precision, IF(_xlpm._precision = 1, "", _xlfn.LET(_xlpm._showPrecision, IF(_xlpm._precision &gt; 1, _xlpm._precision, _xlfn.LET(_xlpm._seconds, ROUND(_xlpm._time * 86400, 3), _xlfn.IFS(_xlpm._seconds = 0, 3, MOD(_xlpm._seconds, 1) &gt; 0, 5, MOD(_xlpm._seconds / 60, 1) &gt; 0, 4, TRUE, 3))), IF(_xlpm._showPrecision = 1, "", _xlfn.LET(_xlpm._fmt, _xlfn.IFS(_xlpm._showPrecision = 2, "h AM/PM", _xlpm._showPrecision = 3, "h:mm AM/PM", _xlpm._showPrecision = 4, "h:mm:ss AM/PM", TRUE, "h:mm:ss.000 AM/PM"), " " &amp; TEXT(_xlpm._time, _xlpm._fmt)))))), _xlpm._separator, IF(_xlpm.Separator = "", "/", _xlfn.LET(_xlpm._char1, LEFT(_xlpm.Separator, 1), IF(IFERROR(FIND(_xlpm._char1, ",./-_"), 0) &gt; 0, _xlpm._char1, "/"))), _xlpm._hasTime, ((MOD(_xlpm.Day, 1) &gt; 0) + ISNUMBER(_xlpm.Time)) &gt; 0, _xlpm._usePrecision, _xlfn.IFS(NOT(_xlpm._hasTime), 1, NOT(ISNUMBER(_xlpm.Precision)), 3, TRUE, INT(_xlpm.Precision)), _xlpm._rDate, CALENDAR.RESOLVE_DATE(_xlpm.YearCE, _xlpm.Month, _xlpm.Day, _xlpm.Time, _xlpm._usePrecision, _xlpm.JulianCalendar), _xlpm._sYear, TEXT(INDEX(_xlpm._rDate, 1, 1), "0000;" &amp; _xlfn.UNICHAR(8722) &amp; "0000;0000"), _xlpm._sMonth, INDEX(_xlpm._rDate, 1, 2), _xlpm._sDay, TEXT(INDEX(_xlpm._rDate, 1, 3), "00"), _xlpm._sTime, _xlpm.fnFormatTime(INDEX(_xlpm._rDate, 1, 4), _xlpm._usePrecision), _xlfn.CONCAT(_xlpm._sMonth, _xlpm._separator, _xlpm._sDay, _xlpm._separator, _xlpm._sYear, _xlpm._sTime))))))</definedName>
     <definedName name="CALENDAR.GREGORIAN_TO_JULIAN">_xlfn.LAMBDA(_xlpm.YearCE,_xlpm.Month,_xlpm.Day, _xlfn.LET(_xlpm._JDN, CALENDAR.JULIAN_DAY_NUMBER(_xlpm.YearCE, _xlpm.Month, _xlpm.Day, 0), _xlfn.IFS(ISERROR(_xlpm._JDN), {#VALUE!,#VALUE!,#VALUE!}, _xlpm._JDN = "", {"","",""}, TRUE, CALENDAR.JDN_TO_CALENDAR_DATE(_xlpm._JDN, 1))))</definedName>
     <definedName name="CALENDAR.HMS_TO_TIME_DECIMAL">_xlfn.LAMBDA(_xlpm.Sign,_xlpm.Hours,_xlpm.Minutes,_xlpm.Seconds, IF((_xlpm.Hours = "") * (_xlpm.Minutes = "") * (_xlpm.Seconds = ""), "", IF((NOT(ISNUMBER(_xlpm.Sign)) * (_xlpm.Sign &lt;&gt; "")) + (NOT(ISNUMBER(_xlpm.Hours)) * (_xlpm.Hours &lt;&gt; "")) + (NOT(ISNUMBER(_xlpm.Minutes)) * (_xlpm.Minutes &lt;&gt; "")) + (NOT(ISNUMBER(_xlpm.Seconds)) * (_xlpm.Seconds &lt;&gt; "")), {#VALUE!}, _xlfn.LET(_xlpm._hours, N(_xlpm.Hours), _xlpm._minutes, N(_xlpm.Minutes), _xlpm._seconds, N(_xlpm.Seconds), IF((_xlpm._hours = 0) * (_xlpm._minutes = 0) * (_xlpm._seconds = 0), 0, _xlfn.LET(_xlpm._sign, IF(N(_xlpm.Sign) &lt; 0, -1, 1), _xlpm._sign * ((_xlpm._hours / 24) + (_xlpm._minutes / 1440) + (_xlpm._seconds / 86400))))))))</definedName>
     <definedName name="CALENDAR.IS_LEAP_YEAR">_xlfn.LAMBDA(_xlpm.YearCE,_xlop.JulianCalendar, IF(_xlpm.YearCE = "", "", IF(NOT(ISNUMBER(_xlpm.YearCE)), {#VALUE!}, _xlfn.LET(_xlpm._yearCE, INT(_xlpm.YearCE), IF(N(_xlpm.JulianCalendar) = 0, _xlfn.IFS(MOD(_xlpm._yearCE, 400) = 0, TRUE, MOD(_xlpm._yearCE, 100) = 0, FALSE, TRUE, MOD(_xlpm._yearCE, 4) = 0), MOD(_xlpm._yearCE, 4) = 0)))))</definedName>
@@ -108,7 +108,6 @@
     <definedName name="CALENDAR.YEAR_COMMON_ERA">_xlfn.LAMBDA(_xlpm.Year,_xlpm.BCE, IF(_xlpm.Year = "", "", IF(NOT(ISNUMBER(_xlpm.Year)), {#VALUE!}, _xlfn.LET(_xlpm._year, INT(_xlpm.Year), IF(_xlpm._year &lt; 1, {#NUM!}, IF(N(_xlpm.BCE), 1 - _xlpm._year, _xlpm._year))))))</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1318,7 +1317,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="17">
+  <numFmts count="19">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="ddd\ d/mm/yyyy"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
@@ -1336,6 +1335,8 @@
     <numFmt numFmtId="178" formatCode="0.000000000"/>
     <numFmt numFmtId="179" formatCode="[h]:mm:ss.000"/>
     <numFmt numFmtId="180" formatCode="0.00000000000000000"/>
+    <numFmt numFmtId="187" formatCode="0.000000000000000"/>
+    <numFmt numFmtId="189" formatCode="h:mm:ss.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -1774,7 +1775,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="272">
+  <cellXfs count="273">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2068,6 +2069,20 @@
     <xf numFmtId="169" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="169" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="0" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2083,24 +2098,11 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="187" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="189" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -2824,9 +2826,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3267,9 +3267,11 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B77C6453-1F3B-4A73-95D5-04255835D86E}">
-  <dimension ref="A1:J90"/>
+  <dimension ref="A1:J92"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="F77" sqref="F77"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3673,17 +3675,19 @@
         <v>25</v>
       </c>
       <c r="D34" s="12">
-        <v>1.25</v>
+        <v>1.78</v>
       </c>
       <c r="E34" s="12">
         <v>0</v>
       </c>
-      <c r="F34" s="12"/>
+      <c r="F34" s="12">
+        <v>1</v>
+      </c>
       <c r="G34" s="12"/>
       <c r="H34" s="12"/>
       <c r="I34" s="13" t="str" cm="1">
         <f t="array" ref="I34">CALENDAR.FORMAT_ISO_DATE(A34,B34,C34,D34,E34,F34,G34,H34)</f>
-        <v>2023-05-26T06Z</v>
+        <v>2023-05-27Z</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -3768,176 +3772,196 @@
         <v>2100-02-29T00:00:00+01:00</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="87">
+        <v>2023</v>
+      </c>
+      <c r="B38" s="49">
+        <v>5</v>
+      </c>
+      <c r="C38" s="49">
+        <v>31</v>
+      </c>
+      <c r="D38" s="49">
+        <v>0</v>
+      </c>
+      <c r="E38" s="49">
+        <v>570</v>
+      </c>
+      <c r="F38" s="49">
+        <v>0</v>
+      </c>
+      <c r="G38" s="49"/>
+      <c r="H38" s="49"/>
+      <c r="I38" s="84" t="str" cm="1">
+        <f t="array" ref="I38">CALENDAR.FORMAT_ISO_DATE(A38,B38,C38,D38,E38,F38,G38,H38)</f>
+        <v>2023-05-31T00:00+09:30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="88">
+        <v>2100</v>
+      </c>
+      <c r="B39" s="52">
+        <v>2</v>
+      </c>
+      <c r="C39" s="52">
+        <v>28</v>
+      </c>
+      <c r="D39" s="52">
+        <v>0.99999999900000003</v>
+      </c>
+      <c r="E39" s="52">
+        <v>60</v>
+      </c>
+      <c r="F39" s="52">
+        <v>4</v>
+      </c>
+      <c r="G39" s="52"/>
+      <c r="H39" s="52">
+        <v>1</v>
+      </c>
+      <c r="I39" s="86" t="str" cm="1">
+        <f t="array" ref="I39">CALENDAR.FORMAT_ISO_DATE(A39,B39,C39,D39,E39,F39,G39,H39)</f>
+        <v>2100-02-29T00:00:00+01:00</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B42" s="6" t="s">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B44" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="C42" s="24" t="s">
+      <c r="C44" s="24" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="8"/>
-      <c r="B43" s="9"/>
-      <c r="C43" s="10" t="str" cm="1">
-        <f t="array" ref="C43">CALENDAR.FORMAT_LITERARY_YEAR(A43,B43)</f>
-        <v/>
-      </c>
-      <c r="E43" s="114"/>
-      <c r="F43" s="115"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B44" s="12"/>
-      <c r="C44" s="13" t="e" cm="1">
-        <f t="array" ref="C44">CALENDAR.FORMAT_LITERARY_YEAR(A44,B44)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E44" s="103"/>
-    </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="8">
-        <v>1</v>
-      </c>
+      <c r="A45" s="8"/>
       <c r="B45" s="9"/>
       <c r="C45" s="10" t="str" cm="1">
         <f t="array" ref="C45">CALENDAR.FORMAT_LITERARY_YEAR(A45,B45)</f>
-        <v>1 CE</v>
-      </c>
+        <v/>
+      </c>
+      <c r="E45" s="114"/>
+      <c r="F45" s="115"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="11">
-        <v>0</v>
+      <c r="A46" s="11" t="s">
+        <v>3</v>
       </c>
       <c r="B46" s="12"/>
-      <c r="C46" s="13" t="str" cm="1">
+      <c r="C46" s="13" t="e" cm="1">
         <f t="array" ref="C46">CALENDAR.FORMAT_LITERARY_YEAR(A46,B46)</f>
-        <v>1 BCE</v>
-      </c>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E46" s="103"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="8">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B47" s="9"/>
       <c r="C47" s="10" t="str" cm="1">
         <f t="array" ref="C47">CALENDAR.FORMAT_LITERARY_YEAR(A47,B47)</f>
+        <v>1 CE</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="11">
+        <v>0</v>
+      </c>
+      <c r="B48" s="12"/>
+      <c r="C48" s="13" t="str" cm="1">
+        <f t="array" ref="C48">CALENDAR.FORMAT_LITERARY_YEAR(A48,B48)</f>
+        <v>1 BCE</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="8">
+        <v>-1</v>
+      </c>
+      <c r="B49" s="9"/>
+      <c r="C49" s="10" t="str" cm="1">
+        <f t="array" ref="C49">CALENDAR.FORMAT_LITERARY_YEAR(A49,B49)</f>
         <v>2 BCE</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="87">
-        <v>900</v>
-      </c>
-      <c r="B48" s="49"/>
-      <c r="C48" s="84" t="str" cm="1">
-        <f t="array" ref="C48">CALENDAR.FORMAT_LITERARY_YEAR(A48,B48)</f>
-        <v>900 CE</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="88">
-        <v>1800</v>
-      </c>
-      <c r="B49" s="52"/>
-      <c r="C49" s="86" t="str" cm="1">
-        <f t="array" ref="C49">CALENDAR.FORMAT_LITERARY_YEAR(A49,B49)</f>
-        <v>1800</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="87">
-        <v>2000</v>
-      </c>
-      <c r="B50" s="49">
-        <v>1</v>
-      </c>
+        <v>900</v>
+      </c>
+      <c r="B50" s="49"/>
       <c r="C50" s="84" t="str" cm="1">
         <f t="array" ref="C50">CALENDAR.FORMAT_LITERARY_YEAR(A50,B50)</f>
+        <v>900 CE</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="88">
+        <v>1800</v>
+      </c>
+      <c r="B51" s="52"/>
+      <c r="C51" s="86" t="str" cm="1">
+        <f t="array" ref="C51">CALENDAR.FORMAT_LITERARY_YEAR(A51,B51)</f>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="87">
+        <v>2000</v>
+      </c>
+      <c r="B52" s="49">
+        <v>1</v>
+      </c>
+      <c r="C52" s="84" t="str" cm="1">
+        <f t="array" ref="C52">CALENDAR.FORMAT_LITERARY_YEAR(A52,B52)</f>
         <v>2000 CE</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
+    <row r="55" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B55" s="6" t="s">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B57" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C55" s="6" t="s">
+      <c r="C57" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D55" s="6" t="s">
+      <c r="D57" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="E55" s="6" t="s">
+      <c r="E57" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F55" s="6" t="s">
+      <c r="F57" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="G55" s="6" t="s">
+      <c r="G57" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="H55" s="6" t="s">
+      <c r="H57" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I55" s="24" t="s">
+      <c r="I57" s="24" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="8"/>
-      <c r="B56" s="9"/>
-      <c r="C56" s="9"/>
-      <c r="D56" s="9"/>
-      <c r="E56" s="9"/>
-      <c r="F56" s="9"/>
-      <c r="G56" s="9"/>
-      <c r="H56" s="9"/>
-      <c r="I56" s="10" t="str" cm="1">
-        <f t="array" ref="I56">CALENDAR.FORMAT_LITERARY_DATE(A56,B56,C56,D56,E56,F56,G56,H56)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B57" s="12"/>
-      <c r="C57" s="12"/>
-      <c r="D57" s="12"/>
-      <c r="E57" s="12"/>
-      <c r="F57" s="12"/>
-      <c r="G57" s="12"/>
-      <c r="H57" s="12"/>
-      <c r="I57" s="13" t="e" cm="1">
-        <f t="array" ref="I57">CALENDAR.FORMAT_LITERARY_DATE(A57,B57,C57,D57,E57,F57,G57,H57)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="8">
-        <v>2023</v>
-      </c>
-      <c r="B58" s="9">
-        <v>5</v>
-      </c>
+      <c r="A58" s="8"/>
+      <c r="B58" s="9"/>
       <c r="C58" s="9"/>
       <c r="D58" s="9"/>
       <c r="E58" s="9"/>
@@ -3946,128 +3970,108 @@
       <c r="H58" s="9"/>
       <c r="I58" s="10" t="str" cm="1">
         <f t="array" ref="I58">CALENDAR.FORMAT_LITERARY_DATE(A58,B58,C58,D58,E58,F58,G58,H58)</f>
-        <v>May, 2023</v>
+        <v/>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="11"/>
-      <c r="B59" s="12">
-        <v>5</v>
-      </c>
-      <c r="C59" s="12">
-        <v>12</v>
-      </c>
+      <c r="A59" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B59" s="12"/>
+      <c r="C59" s="12"/>
       <c r="D59" s="12"/>
       <c r="E59" s="12"/>
       <c r="F59" s="12"/>
       <c r="G59" s="12"/>
       <c r="H59" s="12"/>
-      <c r="I59" s="13" t="str" cm="1">
+      <c r="I59" s="13" t="e" cm="1">
         <f t="array" ref="I59">CALENDAR.FORMAT_LITERARY_DATE(A59,B59,C59,D59,E59,F59,G59,H59)</f>
-        <v>May 12</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="8">
-        <v>-200</v>
+        <v>2023</v>
       </c>
       <c r="B60" s="9">
-        <v>2</v>
-      </c>
-      <c r="C60" s="9">
-        <v>29</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C60" s="9"/>
       <c r="D60" s="9"/>
       <c r="E60" s="9"/>
       <c r="F60" s="9"/>
       <c r="G60" s="9"/>
-      <c r="H60" s="9">
-        <v>1</v>
-      </c>
+      <c r="H60" s="9"/>
       <c r="I60" s="10" t="str" cm="1">
         <f t="array" ref="I60">CALENDAR.FORMAT_LITERARY_DATE(A60,B60,C60,D60,E60,F60,G60,H60)</f>
+        <v>May, 2023</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="11"/>
+      <c r="B61" s="12">
+        <v>5</v>
+      </c>
+      <c r="C61" s="12">
+        <v>12</v>
+      </c>
+      <c r="D61" s="12"/>
+      <c r="E61" s="12"/>
+      <c r="F61" s="12"/>
+      <c r="G61" s="12"/>
+      <c r="H61" s="12"/>
+      <c r="I61" s="13" t="str" cm="1">
+        <f t="array" ref="I61">CALENDAR.FORMAT_LITERARY_DATE(A61,B61,C61,D61,E61,F61,G61,H61)</f>
+        <v>May 12</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="8">
+        <v>-200</v>
+      </c>
+      <c r="B62" s="9">
+        <v>2</v>
+      </c>
+      <c r="C62" s="9">
+        <v>29</v>
+      </c>
+      <c r="D62" s="9"/>
+      <c r="E62" s="9"/>
+      <c r="F62" s="9"/>
+      <c r="G62" s="9"/>
+      <c r="H62" s="9">
+        <v>1</v>
+      </c>
+      <c r="I62" s="10" t="str" cm="1">
+        <f t="array" ref="I62">CALENDAR.FORMAT_LITERARY_DATE(A62,B62,C62,D62,E62,F62,G62,H62)</f>
         <v>February 29, 201 BCE</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="87">
-        <v>2000</v>
-      </c>
-      <c r="B61" s="49">
-        <v>1</v>
-      </c>
-      <c r="C61" s="49">
-        <v>1</v>
-      </c>
-      <c r="D61" s="49">
-        <v>0.25</v>
-      </c>
-      <c r="E61" s="49"/>
-      <c r="F61" s="49"/>
-      <c r="G61" s="49"/>
-      <c r="H61" s="49"/>
-      <c r="I61" s="84" t="str" cm="1">
-        <f t="array" ref="I61">CALENDAR.FORMAT_LITERARY_DATE(A61,B61,C61,D61,E61,F61,G61,H61)</f>
-        <v>January 1, 2000, 6:00 AM</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="88">
-        <v>2000</v>
-      </c>
-      <c r="B62" s="52">
-        <v>1</v>
-      </c>
-      <c r="C62" s="52">
-        <v>1</v>
-      </c>
-      <c r="D62" s="52">
-        <v>1.25</v>
-      </c>
-      <c r="E62" s="52">
-        <v>1</v>
-      </c>
-      <c r="F62" s="52"/>
-      <c r="G62" s="52">
-        <v>1</v>
-      </c>
-      <c r="H62" s="52"/>
-      <c r="I62" s="86" t="str" cm="1">
-        <f t="array" ref="I62">CALENDAR.FORMAT_LITERARY_DATE(A62,B62,C62,D62,E62,F62,G62,H62)</f>
-        <v>Jan 2, 2000 CE, 6:00 AM</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="87">
-        <v>1900</v>
+        <v>2000</v>
       </c>
       <c r="B63" s="49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C63" s="49">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="D63" s="49">
-        <v>0.99999998999999995</v>
-      </c>
-      <c r="E63" s="49">
-        <v>1</v>
-      </c>
+        <v>0.25</v>
+      </c>
+      <c r="E63" s="49"/>
       <c r="F63" s="49"/>
-      <c r="G63" s="49">
-        <v>1</v>
-      </c>
-      <c r="H63" s="49">
-        <v>1</v>
-      </c>
+      <c r="G63" s="49"/>
+      <c r="H63" s="49"/>
       <c r="I63" s="84" t="str" cm="1">
         <f t="array" ref="I63">CALENDAR.FORMAT_LITERARY_DATE(A63,B63,C63,D63,E63,F63,G63,H63)</f>
-        <v>Feb 29, 1900 CE, 12:00 AM</v>
+        <v>January 1, 2000, 6:00 AM</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="88">
-        <v>100</v>
+        <v>2000</v>
       </c>
       <c r="B64" s="52">
         <v>1</v>
@@ -4081,126 +4085,140 @@
       <c r="E64" s="52">
         <v>1</v>
       </c>
-      <c r="F64" s="52">
-        <v>1</v>
-      </c>
+      <c r="F64" s="52"/>
       <c r="G64" s="52">
         <v>1</v>
       </c>
       <c r="H64" s="52"/>
       <c r="I64" s="86" t="str" cm="1">
         <f t="array" ref="I64">CALENDAR.FORMAT_LITERARY_DATE(A64,B64,C64,D64,E64,F64,G64,H64)</f>
+        <v>Jan 2, 2000 CE, 6:00 AM</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="87">
+        <v>1900</v>
+      </c>
+      <c r="B65" s="49">
+        <v>2</v>
+      </c>
+      <c r="C65" s="49">
+        <v>28</v>
+      </c>
+      <c r="D65" s="49">
+        <v>0.99999998999999995</v>
+      </c>
+      <c r="E65" s="49">
+        <v>1</v>
+      </c>
+      <c r="F65" s="49"/>
+      <c r="G65" s="49">
+        <v>1</v>
+      </c>
+      <c r="H65" s="49">
+        <v>1</v>
+      </c>
+      <c r="I65" s="84" t="str" cm="1">
+        <f t="array" ref="I65">CALENDAR.FORMAT_LITERARY_DATE(A65,B65,C65,D65,E65,F65,G65,H65)</f>
+        <v>Feb 29, 1900 CE, 12:00 AM</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="88">
+        <v>100</v>
+      </c>
+      <c r="B66" s="52">
+        <v>1</v>
+      </c>
+      <c r="C66" s="52">
+        <v>1</v>
+      </c>
+      <c r="D66" s="52">
+        <v>1.25</v>
+      </c>
+      <c r="E66" s="52">
+        <v>1</v>
+      </c>
+      <c r="F66" s="52">
+        <v>1</v>
+      </c>
+      <c r="G66" s="52">
+        <v>1</v>
+      </c>
+      <c r="H66" s="52"/>
+      <c r="I66" s="86" t="str" cm="1">
+        <f t="array" ref="I66">CALENDAR.FORMAT_LITERARY_DATE(A66,B66,C66,D66,E66,F66,G66,H66)</f>
         <v>Jan 2, 100 CE, 6:00 AM</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A67" s="1" t="s">
+    <row r="69" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B69" s="6" t="s">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B71" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C69" s="6" t="s">
+      <c r="C71" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D69" s="6" t="s">
+      <c r="D71" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="E69" s="6" t="s">
+      <c r="E71" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="F69" s="6" t="s">
+      <c r="F71" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G69" s="6" t="s">
+      <c r="G71" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H69" s="24" t="s">
+      <c r="H71" s="24" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="8"/>
-      <c r="B70" s="9"/>
-      <c r="C70" s="9"/>
-      <c r="D70" s="9"/>
-      <c r="E70" s="9"/>
-      <c r="F70" s="9"/>
-      <c r="G70" s="9"/>
-      <c r="H70" s="10" t="str" cm="1">
-        <f t="array" ref="H70">CALENDAR.FORMAT_US_DATE(A70,B70,C70,D70,E70,F70,G70)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B71" s="12"/>
-      <c r="C71" s="12"/>
-      <c r="D71" s="12"/>
-      <c r="E71" s="12"/>
-      <c r="F71" s="12"/>
-      <c r="G71" s="12"/>
-      <c r="H71" s="13" t="e" cm="1">
-        <f t="array" ref="H71">CALENDAR.FORMAT_US_DATE(A71,B71,C71,D71,E71,F71,G71)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="8">
-        <v>2023</v>
-      </c>
-      <c r="B72" s="9">
-        <v>5</v>
-      </c>
-      <c r="C72" s="9">
-        <v>25</v>
-      </c>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="8"/>
+      <c r="B72" s="9"/>
+      <c r="C72" s="9"/>
       <c r="D72" s="9"/>
       <c r="E72" s="9"/>
       <c r="F72" s="9"/>
       <c r="G72" s="9"/>
       <c r="H72" s="10" t="str" cm="1">
         <f t="array" ref="H72">CALENDAR.FORMAT_US_DATE(A72,B72,C72,D72,E72,F72,G72)</f>
-        <v>5/25/2023</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="11">
-        <v>2100</v>
-      </c>
-      <c r="B73" s="12">
-        <v>2</v>
-      </c>
-      <c r="C73" s="12">
-        <v>29</v>
-      </c>
+        <v/>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B73" s="12"/>
+      <c r="C73" s="12"/>
       <c r="D73" s="12"/>
       <c r="E73" s="12"/>
       <c r="F73" s="12"/>
-      <c r="G73" s="12">
-        <v>1</v>
-      </c>
-      <c r="H73" s="13" t="str" cm="1">
+      <c r="G73" s="12"/>
+      <c r="H73" s="13" t="e" cm="1">
         <f t="array" ref="H73">CALENDAR.FORMAT_US_DATE(A73,B73,C73,D73,E73,F73,G73)</f>
-        <v>2/29/2100</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="8">
-        <v>1987</v>
+        <v>2023</v>
       </c>
       <c r="B74" s="9">
         <v>5</v>
       </c>
       <c r="C74" s="9">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="D74" s="9"/>
       <c r="E74" s="9"/>
@@ -4208,315 +4226,359 @@
       <c r="G74" s="9"/>
       <c r="H74" s="10" t="str" cm="1">
         <f t="array" ref="H74">CALENDAR.FORMAT_US_DATE(A74,B74,C74,D74,E74,F74,G74)</f>
+        <v>5/25/2023</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="11">
+        <v>2100</v>
+      </c>
+      <c r="B75" s="12">
+        <v>2</v>
+      </c>
+      <c r="C75" s="12">
+        <v>29</v>
+      </c>
+      <c r="D75" s="12"/>
+      <c r="E75" s="12"/>
+      <c r="F75" s="12"/>
+      <c r="G75" s="12">
+        <v>1</v>
+      </c>
+      <c r="H75" s="13" t="str" cm="1">
+        <f t="array" ref="H75">CALENDAR.FORMAT_US_DATE(A75,B75,C75,D75,E75,F75,G75)</f>
+        <v>2/29/2100</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="8">
+        <v>1987</v>
+      </c>
+      <c r="B76" s="9">
+        <v>5</v>
+      </c>
+      <c r="C76" s="9">
+        <v>12</v>
+      </c>
+      <c r="D76" s="9"/>
+      <c r="E76" s="9"/>
+      <c r="F76" s="9">
+        <v>0</v>
+      </c>
+      <c r="G76" s="9"/>
+      <c r="H76" s="10" t="str" cm="1">
+        <f t="array" ref="H76">CALENDAR.FORMAT_US_DATE(A76,B76,C76,D76,E76,F76,G76)</f>
         <v>5/12/1987</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="87">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="87">
         <v>2000</v>
       </c>
-      <c r="B75" s="49">
-        <v>1</v>
-      </c>
-      <c r="C75" s="49">
+      <c r="B77" s="49">
+        <v>1</v>
+      </c>
+      <c r="C77" s="49">
         <v>31</v>
       </c>
-      <c r="D75" s="49">
+      <c r="D77" s="49">
         <v>1.25</v>
       </c>
-      <c r="E75" s="49"/>
-      <c r="F75" s="49"/>
-      <c r="G75" s="49"/>
-      <c r="H75" s="84" t="str" cm="1">
-        <f t="array" ref="H75">CALENDAR.FORMAT_US_DATE(A75,B75,C75,D75,E75,F75,G75)</f>
-        <v>2/01/2000 6:00 AM</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" s="88">
-        <v>2100</v>
-      </c>
-      <c r="B76" s="52">
-        <v>2</v>
-      </c>
-      <c r="C76" s="52">
-        <v>28</v>
-      </c>
-      <c r="D76" s="125">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="E76" s="127" t="s">
-        <v>154</v>
-      </c>
-      <c r="F76" s="52">
-        <v>5</v>
-      </c>
-      <c r="G76" s="52">
-        <v>1</v>
-      </c>
-      <c r="H76" s="86" t="str" cm="1">
-        <f t="array" ref="H76">CALENDAR.FORMAT_US_DATE(A76,B76,C76,D76,E76,F76,G76)</f>
-        <v>2-28-2100 12:00:00.864 AM</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" s="87">
-        <v>2100</v>
-      </c>
-      <c r="B77" s="49">
-        <v>2</v>
-      </c>
-      <c r="C77" s="49">
-        <v>28</v>
-      </c>
-      <c r="D77" s="49">
-        <v>1.9999999900000001</v>
-      </c>
       <c r="E77" s="49"/>
-      <c r="F77" s="49">
-        <v>3</v>
-      </c>
-      <c r="G77" s="49">
-        <v>1</v>
-      </c>
+      <c r="F77" s="49"/>
+      <c r="G77" s="49"/>
       <c r="H77" s="84" t="str" cm="1">
         <f t="array" ref="H77">CALENDAR.FORMAT_US_DATE(A77,B77,C77,D77,E77,F77,G77)</f>
-        <v>3/01/2100 12:00 AM</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2/01/2000 6:00 AM</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="88">
-        <v>-385</v>
+        <v>2100</v>
       </c>
       <c r="B78" s="52">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C78" s="52">
-        <v>12</v>
-      </c>
-      <c r="D78" s="52">
-        <v>0.25</v>
-      </c>
-      <c r="E78" s="52"/>
-      <c r="F78" s="52"/>
-      <c r="G78" s="52"/>
+        <v>28</v>
+      </c>
+      <c r="D78" s="125">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="E78" s="127" t="s">
+        <v>154</v>
+      </c>
+      <c r="F78" s="52">
+        <v>0</v>
+      </c>
+      <c r="G78" s="52">
+        <v>1</v>
+      </c>
       <c r="H78" s="86" t="str" cm="1">
         <f t="array" ref="H78">CALENDAR.FORMAT_US_DATE(A78,B78,C78,D78,E78,F78,G78)</f>
-        <v>5/12/−0385 6:00 AM</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A81" s="1" t="s">
+        <v>2-28-2100 12:00:00.864 AM</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="87">
+        <v>2100</v>
+      </c>
+      <c r="B79" s="49">
+        <v>2</v>
+      </c>
+      <c r="C79" s="49">
+        <v>28</v>
+      </c>
+      <c r="D79" s="49">
+        <v>1.9999999900000001</v>
+      </c>
+      <c r="E79" s="49"/>
+      <c r="F79" s="49">
+        <v>4</v>
+      </c>
+      <c r="G79" s="49">
+        <v>1</v>
+      </c>
+      <c r="H79" s="84" t="str" cm="1">
+        <f t="array" ref="H79">CALENDAR.FORMAT_US_DATE(A79,B79,C79,D79,E79,F79,G79)</f>
+        <v>3/01/2100 12:00:00 AM</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" s="88">
+        <v>-385</v>
+      </c>
+      <c r="B80" s="52">
+        <v>5</v>
+      </c>
+      <c r="C80" s="52">
+        <v>12</v>
+      </c>
+      <c r="D80" s="52">
+        <v>0.25</v>
+      </c>
+      <c r="E80" s="52"/>
+      <c r="F80" s="52">
+        <v>5</v>
+      </c>
+      <c r="G80" s="52"/>
+      <c r="H80" s="86" t="str" cm="1">
+        <f t="array" ref="H80">CALENDAR.FORMAT_US_DATE(A80,B80,C80,D80,E80,F80,G80)</f>
+        <v>5/12/−0385 6:00:00.000 AM</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A83" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A83" s="22" t="s">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B83" s="6" t="s">
+      <c r="B85" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C83" s="6" t="s">
+      <c r="C85" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D83" s="6" t="s">
+      <c r="D85" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="E83" s="6" t="s">
+      <c r="E85" s="6" t="s">
         <v>385</v>
       </c>
-      <c r="F83" s="6"/>
-      <c r="G83" s="6" t="s">
+      <c r="F85" s="6"/>
+      <c r="G85" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="H83" s="6" t="s">
+      <c r="H85" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="I83" s="6" t="s">
+      <c r="I85" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J83" s="37" t="s">
+      <c r="J85" s="37" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A84" s="8"/>
-      <c r="B84" s="9"/>
-      <c r="C84" s="9"/>
-      <c r="D84" s="9"/>
-      <c r="E84" s="9"/>
-      <c r="F84" s="9"/>
-      <c r="G84" s="9"/>
-      <c r="H84" s="9"/>
-      <c r="I84" s="9"/>
-      <c r="J84" s="10" t="str" cm="1">
-        <f t="array" ref="J84">CALENDAR.FORMAT_MIL_DTG(A84,B84,C84,G84,H84,I84)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A85" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B85" s="12"/>
-      <c r="C85" s="12"/>
-      <c r="D85" s="12"/>
-      <c r="E85" s="12"/>
-      <c r="F85" s="12"/>
-      <c r="G85" s="12"/>
-      <c r="H85" s="12"/>
-      <c r="I85" s="12"/>
-      <c r="J85" s="13" t="e" cm="1">
-        <f t="array" ref="J85">CALENDAR.FORMAT_MIL_DTG(A85,B85,C85,G85,H85,I85)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A86" s="8">
-        <v>2000</v>
-      </c>
-      <c r="B86" s="9">
-        <v>2</v>
-      </c>
-      <c r="C86" s="9">
-        <v>29</v>
-      </c>
-      <c r="D86" s="9">
-        <v>1</v>
-      </c>
-      <c r="E86" s="264">
-        <v>0.1986111111111111</v>
-      </c>
+      <c r="A86" s="8"/>
+      <c r="B86" s="9"/>
+      <c r="C86" s="9"/>
+      <c r="D86" s="9"/>
+      <c r="E86" s="9"/>
       <c r="F86" s="9"/>
-      <c r="G86" s="267">
-        <f>E86*D86</f>
-        <v>0.1986111111111111</v>
-      </c>
-      <c r="H86" s="9">
-        <v>106</v>
-      </c>
+      <c r="G86" s="9"/>
+      <c r="H86" s="9"/>
       <c r="I86" s="9"/>
       <c r="J86" s="10" t="str" cm="1">
         <f t="array" ref="J86">CALENDAR.FORMAT_MIL_DTG(A86,B86,C86,G86,H86,I86)</f>
-        <v>29050000BFEB00</v>
+        <v/>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A87" s="11">
-        <v>2023</v>
-      </c>
-      <c r="B87" s="12">
+      <c r="A87" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B87" s="12"/>
+      <c r="C87" s="12"/>
+      <c r="D87" s="12"/>
+      <c r="E87" s="12"/>
+      <c r="F87" s="12"/>
+      <c r="G87" s="12"/>
+      <c r="H87" s="12"/>
+      <c r="I87" s="12"/>
+      <c r="J87" s="13" t="e" cm="1">
+        <f t="array" ref="J87">CALENDAR.FORMAT_MIL_DTG(A87,B87,C87,G87,H87,I87)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="8">
+        <v>2000</v>
+      </c>
+      <c r="B88" s="9">
         <v>2</v>
       </c>
-      <c r="C87" s="12">
-        <v>1</v>
-      </c>
-      <c r="D87" s="12">
-        <v>1</v>
-      </c>
-      <c r="E87" s="265">
-        <v>0.15973379629629628</v>
-      </c>
-      <c r="F87" s="12"/>
-      <c r="G87" s="268">
-        <f t="shared" ref="G87:G90" si="0">E87*D87</f>
-        <v>0.15973379629629628</v>
-      </c>
-      <c r="H87" s="12">
-        <v>900</v>
-      </c>
-      <c r="I87" s="12">
-        <v>1</v>
-      </c>
-      <c r="J87" s="13" t="str" cm="1">
-        <f t="array" ref="J87">CALENDAR.FORMAT_MIL_DTG(A87,B87,C87,G87,H87,I87)</f>
-        <v>010050MFEB23</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A88" s="8"/>
-      <c r="B88" s="9"/>
       <c r="C88" s="9">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="D88" s="9">
         <v>1</v>
       </c>
-      <c r="E88" s="264">
-        <v>0.28819444444444448</v>
+      <c r="E88" s="255">
+        <v>0.1986111111111111</v>
       </c>
       <c r="F88" s="9"/>
-      <c r="G88" s="267">
-        <f t="shared" si="0"/>
-        <v>0.28819444444444448</v>
-      </c>
-      <c r="H88" s="9"/>
+      <c r="G88" s="258">
+        <f>E88*D88</f>
+        <v>0.1986111111111111</v>
+      </c>
+      <c r="H88" s="9">
+        <v>106</v>
+      </c>
       <c r="I88" s="9"/>
       <c r="J88" s="10" t="str" cm="1">
         <f t="array" ref="J88">CALENDAR.FORMAT_MIL_DTG(A88,B88,C88,G88,H88,I88)</f>
+        <v>29050000BFEB00</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="11">
+        <v>2023</v>
+      </c>
+      <c r="B89" s="12">
+        <v>2</v>
+      </c>
+      <c r="C89" s="12">
+        <v>1</v>
+      </c>
+      <c r="D89" s="12">
+        <v>1</v>
+      </c>
+      <c r="E89" s="256">
+        <v>0.15973379629629628</v>
+      </c>
+      <c r="F89" s="12"/>
+      <c r="G89" s="259">
+        <f t="shared" ref="G89:G92" si="0">E89*D89</f>
+        <v>0.15973379629629628</v>
+      </c>
+      <c r="H89" s="12">
+        <v>900</v>
+      </c>
+      <c r="I89" s="12">
+        <v>1</v>
+      </c>
+      <c r="J89" s="13" t="str" cm="1">
+        <f t="array" ref="J89">CALENDAR.FORMAT_MIL_DTG(A89,B89,C89,G89,H89,I89)</f>
+        <v>010050MFEB23</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="8"/>
+      <c r="B90" s="9"/>
+      <c r="C90" s="9">
+        <v>12</v>
+      </c>
+      <c r="D90" s="9">
+        <v>1</v>
+      </c>
+      <c r="E90" s="255">
+        <v>0.28819444444444448</v>
+      </c>
+      <c r="F90" s="9"/>
+      <c r="G90" s="258">
+        <f t="shared" si="0"/>
+        <v>0.28819444444444448</v>
+      </c>
+      <c r="H90" s="9"/>
+      <c r="I90" s="9"/>
+      <c r="J90" s="10" t="str" cm="1">
+        <f t="array" ref="J90">CALENDAR.FORMAT_MIL_DTG(A90,B90,C90,G90,H90,I90)</f>
         <v>120655J</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A89" s="87">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="87">
         <v>1951</v>
       </c>
-      <c r="B89" s="49">
-        <v>1</v>
-      </c>
-      <c r="C89" s="49">
+      <c r="B91" s="49">
+        <v>1</v>
+      </c>
+      <c r="C91" s="49">
         <v>31</v>
       </c>
-      <c r="D89" s="49">
+      <c r="D91" s="49">
         <v>-1</v>
       </c>
-      <c r="E89" s="266">
+      <c r="E91" s="257">
         <v>0.5</v>
       </c>
-      <c r="F89" s="49"/>
-      <c r="G89" s="269">
+      <c r="F91" s="49"/>
+      <c r="G91" s="260">
         <f t="shared" si="0"/>
         <v>-0.5</v>
       </c>
-      <c r="H89" s="49">
+      <c r="H91" s="49">
         <v>-570</v>
       </c>
-      <c r="I89" s="49">
-        <v>1</v>
-      </c>
-      <c r="J89" s="84" t="str" cm="1">
-        <f t="array" ref="J89">CALENDAR.FORMAT_MIL_DTG(A89,B89,C89,G89,H89,I89)</f>
+      <c r="I91" s="49">
+        <v>1</v>
+      </c>
+      <c r="J91" s="84" t="str" cm="1">
+        <f t="array" ref="J91">CALENDAR.FORMAT_MIL_DTG(A91,B91,C91,G91,H91,I91)</f>
         <v>301130WJAN51</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A90" s="88">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="88">
         <v>2051</v>
       </c>
-      <c r="B90" s="52">
+      <c r="B92" s="52">
         <v>5</v>
       </c>
-      <c r="C90" s="52">
+      <c r="C92" s="52">
         <v>11</v>
       </c>
-      <c r="D90" s="52">
-        <v>1</v>
-      </c>
-      <c r="E90" s="271">
-        <v>0</v>
-      </c>
-      <c r="F90" s="52"/>
-      <c r="G90" s="270">
+      <c r="D92" s="52">
+        <v>1</v>
+      </c>
+      <c r="E92" s="262">
+        <v>0</v>
+      </c>
+      <c r="F92" s="52"/>
+      <c r="G92" s="261">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H90" s="52">
+      <c r="H92" s="52">
         <v>60</v>
       </c>
-      <c r="I90" s="52"/>
-      <c r="J90" s="86" t="str" cm="1">
-        <f t="array" ref="J90">CALENDAR.FORMAT_MIL_DTG(A90,B90,C90,G90,H90,I90)</f>
+      <c r="I92" s="52"/>
+      <c r="J92" s="86" t="str" cm="1">
+        <f t="array" ref="J92">CALENDAR.FORMAT_MIL_DTG(A92,B92,C92,G92,H92,I92)</f>
         <v>#NUM!!</v>
       </c>
     </row>
@@ -4531,10 +4593,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16E3E4D4-B3E5-4714-8C51-665E20588021}">
-  <dimension ref="A1:K50"/>
+  <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4543,7 +4605,7 @@
     <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.28515625" customWidth="1"/>
     <col min="4" max="4" width="20.140625" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" customWidth="1"/>
     <col min="6" max="6" width="37" customWidth="1"/>
     <col min="7" max="7" width="28.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="17.85546875" bestFit="1" customWidth="1"/>
@@ -4700,7 +4762,7 @@
         <v>116</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>52</v>
+        <v>94</v>
       </c>
       <c r="E15" s="75"/>
     </row>
@@ -4892,7 +4954,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="132">
-        <v>2460003.8645833302</v>
+        <v>2460003.8645833801</v>
       </c>
       <c r="B37" s="69"/>
       <c r="C37" s="69"/>
@@ -4905,19 +4967,17 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="130">
-        <v>2460241.9999999902</v>
-      </c>
-      <c r="B38" s="70">
-        <v>570</v>
-      </c>
+        <v>2460241.4999999902</v>
+      </c>
+      <c r="B38" s="70"/>
       <c r="C38" s="70">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D38" s="70"/>
       <c r="E38" s="70"/>
       <c r="F38" s="63" t="str" cm="1">
         <f t="array" ref="F38">CALENDAR.JDATE_TO_ISODATE(A38,B38,C38,D38,E38)</f>
-        <v>2023-10-24T21:30:00+09:30</v>
+        <v>2023-10-23T23:59:59.999</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -5004,7 +5064,9 @@
         <v>0.86458332999999998</v>
       </c>
       <c r="C47" s="69"/>
-      <c r="D47" s="69"/>
+      <c r="D47" s="69">
+        <v>0</v>
+      </c>
       <c r="E47" s="69"/>
       <c r="F47" s="69"/>
       <c r="G47" s="61" t="str" cm="1">
@@ -5073,6 +5135,10 @@
         <f t="array" ref="G50">CALENDAR.JDN_LOCAL_TO_ISODATE(A50,B50,C50,D50,E50,F50)</f>
         <v>2023-10-10T02:30−09:00</v>
       </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E58" s="269"/>
+      <c r="F58" s="268"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5084,8 +5150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9869958-2389-4900-93D5-8B88BB2FBA8B}">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5139,7 +5205,9 @@
         <v>45039.585590277777</v>
       </c>
       <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
+      <c r="C5" s="69">
+        <v>0</v>
+      </c>
       <c r="D5" s="69"/>
       <c r="E5" s="69"/>
       <c r="F5" s="61" t="str" cm="1">
@@ -5500,9 +5568,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC6F0ADE-E8AE-4C89-8078-86F8FAD36319}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5601,7 +5667,9 @@
         <v>45039.585590277777</v>
       </c>
       <c r="B15" s="69"/>
-      <c r="C15" s="12"/>
+      <c r="C15" s="12">
+        <v>0</v>
+      </c>
       <c r="D15" s="120" t="str" cm="1">
         <f t="array" ref="D15">CALENDAR.EDATE_TO_USDATE(A15,B15,C15)</f>
         <v>4/23/2023 2:03:15 PM</v>
@@ -5640,10 +5708,12 @@
       <c r="B18" s="70" t="s">
         <v>154</v>
       </c>
-      <c r="C18" s="16"/>
+      <c r="C18" s="16">
+        <v>4</v>
+      </c>
       <c r="D18" s="136" t="str" cm="1">
         <f t="array" ref="D18">CALENDAR.EDATE_TO_USDATE(A18,B18,C18)</f>
-        <v>3-14-2100 12:00 AM</v>
+        <v>3-14-2100 12:00:00 AM</v>
       </c>
     </row>
   </sheetData>
@@ -8908,11 +8978,11 @@
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="249" t="s">
+      <c r="A16" s="263" t="s">
         <v>219</v>
       </c>
-      <c r="B16" s="249"/>
-      <c r="C16" s="249"/>
+      <c r="B16" s="263"/>
+      <c r="C16" s="263"/>
       <c r="D16" cm="1">
         <f t="array" ref="D16:O16">{90,89,92,91,92,92,92,92,91,92,92,90}</f>
         <v>90</v>
@@ -8952,36 +9022,36 @@
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="250" t="s">
+      <c r="A18" s="264" t="s">
         <v>206</v>
       </c>
-      <c r="B18" s="252" t="s">
+      <c r="B18" s="266" t="s">
         <v>218</v>
       </c>
-      <c r="C18" s="253"/>
-      <c r="D18" s="253"/>
-      <c r="E18" s="253"/>
-      <c r="G18" s="252" t="s">
+      <c r="C18" s="267"/>
+      <c r="D18" s="267"/>
+      <c r="E18" s="267"/>
+      <c r="G18" s="266" t="s">
         <v>234</v>
       </c>
-      <c r="H18" s="253"/>
-      <c r="I18" s="253"/>
-      <c r="J18" s="253"/>
-      <c r="L18" s="252" t="s">
+      <c r="H18" s="267"/>
+      <c r="I18" s="267"/>
+      <c r="J18" s="267"/>
+      <c r="L18" s="266" t="s">
         <v>218</v>
       </c>
-      <c r="M18" s="253"/>
-      <c r="N18" s="253"/>
-      <c r="O18" s="253"/>
-      <c r="Q18" s="252" t="s">
+      <c r="M18" s="267"/>
+      <c r="N18" s="267"/>
+      <c r="O18" s="267"/>
+      <c r="Q18" s="266" t="s">
         <v>192</v>
       </c>
-      <c r="R18" s="253"/>
-      <c r="S18" s="253"/>
-      <c r="T18" s="253"/>
+      <c r="R18" s="267"/>
+      <c r="S18" s="267"/>
+      <c r="T18" s="267"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="251"/>
+      <c r="A19" s="265"/>
       <c r="B19" s="77">
         <v>1</v>
       </c>
@@ -10473,8 +10543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{248533E1-DB7C-4A47-A754-1372CF539763}">
   <dimension ref="A1:O99"/>
   <sheetViews>
-    <sheetView topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+    <sheetView topLeftCell="C46" workbookViewId="0">
+      <selection activeCell="J66" sqref="J66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11116,17 +11186,13 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B65" s="12">
-        <v>0</v>
-      </c>
+      <c r="B65" s="12"/>
       <c r="C65" s="12"/>
-      <c r="D65" s="45">
-        <v>0</v>
-      </c>
+      <c r="D65" s="45"/>
       <c r="E65" s="12" t="e" cm="1">
         <f t="array" ref="E65:H65">CALENDAR.CALENDAR_FROM_JDATE(A65,B65,C65,D65)</f>
         <v>#VALUE!</v>
@@ -11141,17 +11207,13 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="54">
-        <v>2460000</v>
-      </c>
-      <c r="B66" s="9">
-        <v>0</v>
-      </c>
+        <v>2460000.0428907899</v>
+      </c>
+      <c r="B66" s="9"/>
       <c r="C66" s="9"/>
-      <c r="D66" s="44">
-        <v>0</v>
-      </c>
+      <c r="D66" s="44"/>
       <c r="E66" s="9" cm="1">
         <f t="array" ref="E66:H66">CALENDAR.CALENDAR_FROM_JDATE(A66,B66,C66,D66)</f>
         <v>2023</v>
@@ -11163,10 +11225,11 @@
         <v>24</v>
       </c>
       <c r="H66" s="116">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.54289078991860151</v>
+      </c>
+      <c r="J66" s="272"/>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="55">
         <v>2458908.125</v>
       </c>
@@ -11174,9 +11237,7 @@
         <v>540</v>
       </c>
       <c r="C67" s="49"/>
-      <c r="D67" s="50">
-        <v>0</v>
-      </c>
+      <c r="D67" s="50"/>
       <c r="E67" s="49" cm="1">
         <f t="array" ref="E67:H67">CALENDAR.CALENDAR_FROM_JDATE(A67,B67,C67,D67)</f>
         <v>2020</v>
@@ -11190,8 +11251,9 @@
       <c r="H67" s="118">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L67" s="270"/>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="56">
         <v>2251766.3665999998</v>
       </c>
@@ -11217,8 +11279,9 @@
       <c r="H68" s="119">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="L68" s="271"/>
+    </row>
+    <row r="71" spans="1:12" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>315</v>
       </c>
@@ -11226,7 +11289,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="22" t="s">
         <v>87</v>
       </c>
@@ -11246,7 +11309,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="237"/>
       <c r="B74" s="9" t="str" cm="1">
         <f t="array" ref="B74:E74">CALENDAR.TIME_DECIMAL_TO_HMS(A74)</f>
@@ -11266,7 +11329,7 @@
         <v/>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="238">
         <v>0.5</v>
       </c>
@@ -11288,7 +11351,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="237">
         <v>1.25</v>
       </c>
@@ -11310,7 +11373,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="239">
         <v>0</v>
       </c>
@@ -11332,7 +11395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="240">
         <v>-1.7532654320000001</v>
       </c>
@@ -18418,11 +18481,11 @@
       <c r="B4" s="181">
         <v>45078.75</v>
       </c>
-      <c r="C4" s="254" cm="1">
+      <c r="C4" s="9" cm="1">
         <f t="array" ref="C4">_xlfn.IFS(A4=B4,0,B4&gt;A4,1,TRUE,-1)</f>
         <v>1</v>
       </c>
-      <c r="D4" s="254">
+      <c r="D4" s="9">
         <f>C4*(ABS(INT(B4)-INT(A4))+1)</f>
         <v>2</v>
       </c>
@@ -18435,7 +18498,7 @@
         <v>2460097.25</v>
       </c>
       <c r="G4" s="9"/>
-      <c r="H4" s="254" cm="1">
+      <c r="H4" s="9" cm="1">
         <f t="array" ref="H4">CALENDAR.EXTENT_OF_DAYS(E4,F4,G4)</f>
         <v>2</v>
       </c>
@@ -18452,11 +18515,11 @@
       <c r="B5" s="183">
         <v>45078</v>
       </c>
-      <c r="C5" s="255" cm="1">
+      <c r="C5" s="12" cm="1">
         <f t="array" ref="C5">_xlfn.IFS(A5=B5,0,B5&gt;A5,1,TRUE,-1)</f>
         <v>1</v>
       </c>
-      <c r="D5" s="255">
+      <c r="D5" s="12">
         <f t="shared" ref="D5:D6" si="0">C5*(ABS(INT(B5)-INT(A5))+1)</f>
         <v>2</v>
       </c>
@@ -18469,7 +18532,7 @@
         <v>2460096.5</v>
       </c>
       <c r="G5" s="12"/>
-      <c r="H5" s="255" cm="1">
+      <c r="H5" s="12" cm="1">
         <f t="array" ref="H5">CALENDAR.EXTENT_OF_DAYS(E5,F5,G5)</f>
         <v>2</v>
       </c>
@@ -18485,30 +18548,30 @@
       <c r="B6" s="229">
         <v>45077.25</v>
       </c>
-      <c r="C6" s="257" cm="1">
+      <c r="C6" s="249" cm="1">
         <f t="array" ref="C6">_xlfn.IFS(A6=B6,0,B6&gt;A6,1,TRUE,-1)</f>
         <v>-1</v>
       </c>
-      <c r="D6" s="257">
+      <c r="D6" s="249">
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-      <c r="E6" s="258" cm="1">
+      <c r="E6" s="250" cm="1">
         <f t="array" ref="E6">CALENDAR.EDATE_TO_JDATE(A6,G6)</f>
         <v>2460097.6666666665</v>
       </c>
-      <c r="F6" s="258" cm="1">
+      <c r="F6" s="250" cm="1">
         <f t="array" ref="F6">CALENDAR.EDATE_TO_JDATE(B6,G6)</f>
         <v>2460096.1666666665</v>
       </c>
-      <c r="G6" s="259">
+      <c r="G6" s="249">
         <v>-600</v>
       </c>
-      <c r="H6" s="257" cm="1">
+      <c r="H6" s="249" cm="1">
         <f t="array" ref="H6">CALENDAR.EXTENT_OF_DAYS(E6,F6,G6)</f>
         <v>-2</v>
       </c>
-      <c r="I6" s="260" t="b">
+      <c r="I6" s="251" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -18554,11 +18617,11 @@
       <c r="B12" s="181">
         <v>45081.999988425923</v>
       </c>
-      <c r="C12" s="254" cm="1">
+      <c r="C12" s="9" cm="1">
         <f t="array" ref="C12">_xlfn.IFS(A12=B12,0,B12&gt;A12,1,TRUE,-1)</f>
         <v>1</v>
       </c>
-      <c r="D12" s="254">
+      <c r="D12" s="9">
         <f>C12*INT(((INT(B12-WEEKDAY(B12,3))-INT(A12-WEEKDAY(A12,3)))/7)+1)</f>
         <v>1</v>
       </c>
@@ -18571,7 +18634,7 @@
         <v>2460100.499988426</v>
       </c>
       <c r="G12" s="9"/>
-      <c r="H12" s="254" cm="1">
+      <c r="H12" s="9" cm="1">
         <f t="array" ref="H12">CALENDAR.EXTENT_OF_WEEKS(E12,F12,G12)</f>
         <v>1</v>
       </c>
@@ -18587,11 +18650,11 @@
       <c r="B13" s="183">
         <v>45077.25</v>
       </c>
-      <c r="C13" s="255" cm="1">
+      <c r="C13" s="12" cm="1">
         <f t="array" ref="C13">_xlfn.IFS(A13=B13,0,B13&gt;A13,1,TRUE,-1)</f>
         <v>-1</v>
       </c>
-      <c r="D13" s="255">
+      <c r="D13" s="12">
         <f t="shared" ref="D13:D15" si="3">C13*INT(((INT(B13-WEEKDAY(B13,3))-INT(A13-WEEKDAY(A13,3)))/7)+1)</f>
         <v>-1</v>
       </c>
@@ -18604,7 +18667,7 @@
         <v>2460095.75</v>
       </c>
       <c r="G13" s="12"/>
-      <c r="H13" s="255" cm="1">
+      <c r="H13" s="12" cm="1">
         <f t="array" ref="H13">CALENDAR.EXTENT_OF_WEEKS(E13,F13,G13)</f>
         <v>-1</v>
       </c>
@@ -18620,11 +18683,11 @@
       <c r="B14" s="181">
         <v>45413.75</v>
       </c>
-      <c r="C14" s="254" cm="1">
+      <c r="C14" s="9" cm="1">
         <f t="array" ref="C14">_xlfn.IFS(A14=B14,0,B14&gt;A14,1,TRUE,-1)</f>
         <v>1</v>
       </c>
-      <c r="D14" s="254">
+      <c r="D14" s="9">
         <f t="shared" si="3"/>
         <v>53</v>
       </c>
@@ -18639,7 +18702,7 @@
       <c r="G14" s="9">
         <v>-600</v>
       </c>
-      <c r="H14" s="254" cm="1">
+      <c r="H14" s="9" cm="1">
         <f t="array" ref="H14">CALENDAR.EXTENT_OF_WEEKS(E14,F14,G14)</f>
         <v>53</v>
       </c>
@@ -18655,11 +18718,11 @@
       <c r="B15" s="185">
         <v>45077.25</v>
       </c>
-      <c r="C15" s="256" cm="1">
+      <c r="C15" s="49" cm="1">
         <f t="array" ref="C15">_xlfn.IFS(A15=B15,0,B15&gt;A15,1,TRUE,-1)</f>
         <v>1</v>
       </c>
-      <c r="D15" s="256">
+      <c r="D15" s="49">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
@@ -18674,7 +18737,7 @@
       <c r="G15" s="49">
         <v>570</v>
       </c>
-      <c r="H15" s="256" cm="1">
+      <c r="H15" s="49" cm="1">
         <f t="array" ref="H15">CALENDAR.EXTENT_OF_WEEKS(E15,F15,G15)</f>
         <v>5</v>
       </c>
@@ -18724,11 +18787,11 @@
       <c r="B21" s="181">
         <v>45081.999988425923</v>
       </c>
-      <c r="C21" s="254" cm="1">
+      <c r="C21" s="9" cm="1">
         <f t="array" ref="C21">_xlfn.IFS(A21=B21,0,B21&gt;A21,1,TRUE,-1)</f>
         <v>1</v>
       </c>
-      <c r="D21" s="254">
+      <c r="D21" s="9">
         <f t="shared" ref="D21:D22" si="4">IF(C21=0,1,_xlfn.LET(_xlpm._s,IF(C21=1,A21,B21),_xlpm._e,IF(C21=-1,A21,B21),C21*((YEAR(_xlpm._e)-YEAR(_xlpm._s))*12+MONTH(_xlpm._e)-MONTH(_xlpm._s)+1)))</f>
         <v>2</v>
       </c>
@@ -18741,7 +18804,7 @@
         <v>2460100.499988426</v>
       </c>
       <c r="G21" s="9"/>
-      <c r="H21" s="254" cm="1">
+      <c r="H21" s="9" cm="1">
         <f t="array" ref="H21">CALENDAR.EXTENT_OF_MONTHS(E21,F21,G21)</f>
         <v>2</v>
       </c>
@@ -18757,11 +18820,11 @@
       <c r="B22" s="183">
         <v>45077.25</v>
       </c>
-      <c r="C22" s="255" cm="1">
+      <c r="C22" s="12" cm="1">
         <f t="array" ref="C22">_xlfn.IFS(A22=B22,0,B22&gt;A22,1,TRUE,-1)</f>
         <v>-1</v>
       </c>
-      <c r="D22" s="255">
+      <c r="D22" s="12">
         <f t="shared" si="4"/>
         <v>-2</v>
       </c>
@@ -18774,7 +18837,7 @@
         <v>2460095.75</v>
       </c>
       <c r="G22" s="12"/>
-      <c r="H22" s="255" cm="1">
+      <c r="H22" s="12" cm="1">
         <f t="array" ref="H22">CALENDAR.EXTENT_OF_MONTHS(E22,F22,G22)</f>
         <v>-2</v>
       </c>
@@ -18790,11 +18853,11 @@
       <c r="B23" s="181">
         <v>45413.75</v>
       </c>
-      <c r="C23" s="254" cm="1">
+      <c r="C23" s="9" cm="1">
         <f t="array" ref="C23">_xlfn.IFS(A23=B23,0,B23&gt;A23,1,TRUE,-1)</f>
         <v>1</v>
       </c>
-      <c r="D23" s="254">
+      <c r="D23" s="9">
         <f>IF(C23=0,1,_xlfn.LET(_xlpm._s,IF(C23=1,A23,B23),_xlpm._e,IF(C23=-1,A23,B23),C23*((YEAR(_xlpm._e)-YEAR(_xlpm._s))*12+MONTH(_xlpm._e)-MONTH(_xlpm._s)+1)))</f>
         <v>13</v>
       </c>
@@ -18809,7 +18872,7 @@
       <c r="G23" s="9">
         <v>-600</v>
       </c>
-      <c r="H23" s="254" cm="1">
+      <c r="H23" s="9" cm="1">
         <f t="array" ref="H23">CALENDAR.EXTENT_OF_MONTHS(E23,F23,G23)</f>
         <v>13</v>
       </c>
@@ -18825,11 +18888,11 @@
       <c r="B24" s="185">
         <v>44347.25</v>
       </c>
-      <c r="C24" s="256" cm="1">
+      <c r="C24" s="49" cm="1">
         <f t="array" ref="C24">_xlfn.IFS(A24=B24,0,B24&gt;A24,1,TRUE,-1)</f>
         <v>-1</v>
       </c>
-      <c r="D24" s="256">
+      <c r="D24" s="49">
         <f t="shared" ref="D24" si="6">IF(C24=0,1,_xlfn.LET(_xlpm._s,IF(C24=1,A24,B24),_xlpm._e,IF(C24=-1,A24,B24),C24*((YEAR(_xlpm._e)-YEAR(_xlpm._s))*12+MONTH(_xlpm._e)-MONTH(_xlpm._s)+1)))</f>
         <v>-25</v>
       </c>
@@ -18844,7 +18907,7 @@
       <c r="G24" s="49">
         <v>570</v>
       </c>
-      <c r="H24" s="256" cm="1">
+      <c r="H24" s="49" cm="1">
         <f t="array" ref="H24">CALENDAR.EXTENT_OF_MONTHS(E24,F24,G24)</f>
         <v>-25</v>
       </c>
@@ -18921,43 +18984,43 @@
       <c r="B30" s="181">
         <v>44593.75</v>
       </c>
-      <c r="C30" s="254" cm="1">
+      <c r="C30" s="9" cm="1">
         <f t="array" ref="C30">_xlfn.IFS(A30=B30,0,B30&gt;A30,1,TRUE,-1)</f>
         <v>-1</v>
       </c>
-      <c r="D30" s="261">
+      <c r="D30" s="252">
         <f>INT(IF(C30&gt;=0,A30,B30))</f>
         <v>44593</v>
       </c>
-      <c r="E30" s="254">
-        <f>MONTH(D30)-N(P30)-1</f>
+      <c r="E30" s="9">
+        <f t="shared" ref="E30:E35" si="7">MONTH(D30)-N(P30)-1</f>
         <v>2</v>
       </c>
-      <c r="F30" s="254">
+      <c r="F30" s="9">
         <f>YEAR(D30)+INT(E30/12)</f>
         <v>2022</v>
       </c>
-      <c r="G30" s="254">
+      <c r="G30" s="9">
         <f>MOD(INT(E30/3),4)+1</f>
         <v>1</v>
       </c>
-      <c r="H30" s="261">
+      <c r="H30" s="252">
         <f>INT(IF(C30&gt;=0,B30,A30))</f>
         <v>44910</v>
       </c>
-      <c r="I30" s="254">
+      <c r="I30" s="9">
         <f>MONTH(H30)-N(P30)-1</f>
         <v>12</v>
       </c>
-      <c r="J30" s="254">
+      <c r="J30" s="9">
         <f>YEAR(H30)+INT(I30/12)</f>
         <v>2023</v>
       </c>
-      <c r="K30" s="254">
+      <c r="K30" s="9">
         <f>MOD(INT(I30/3),4)+1</f>
         <v>1</v>
       </c>
-      <c r="L30" s="254">
+      <c r="L30" s="9">
         <f>C30*((J30-F30)*4+K30-G30+1)</f>
         <v>-5</v>
       </c>
@@ -18973,12 +19036,12 @@
       <c r="P30" s="9">
         <v>-1</v>
       </c>
-      <c r="Q30" s="254" cm="1">
+      <c r="Q30" s="9" cm="1">
         <f t="array" ref="Q30">CALENDAR.EXTENT_OF_QUARTERS(M30,N30,O30,P30)</f>
         <v>-5</v>
       </c>
       <c r="R30" s="176" t="b">
-        <f>L30=Q30</f>
+        <f t="shared" ref="R30:R35" si="8">L30=Q30</f>
         <v>1</v>
       </c>
     </row>
@@ -18989,44 +19052,44 @@
       <c r="B31" s="183">
         <v>44593.75</v>
       </c>
-      <c r="C31" s="255" cm="1">
+      <c r="C31" s="12" cm="1">
         <f t="array" ref="C31">_xlfn.IFS(A31=B31,0,B31&gt;A31,1,TRUE,-1)</f>
         <v>-1</v>
       </c>
-      <c r="D31" s="262">
-        <f t="shared" ref="D31:D35" si="7">INT(IF(C31&gt;=0,A31,B31))</f>
+      <c r="D31" s="253">
+        <f t="shared" ref="D31:D35" si="9">INT(IF(C31&gt;=0,A31,B31))</f>
         <v>44593</v>
       </c>
-      <c r="E31" s="255">
-        <f>MONTH(D31)-N(P31)-1</f>
-        <v>0</v>
-      </c>
-      <c r="F31" s="255">
-        <f t="shared" ref="F31:F35" si="8">YEAR(D31)+INT(E31/12)</f>
+      <c r="E31" s="12">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F31" s="12">
+        <f t="shared" ref="F31:F35" si="10">YEAR(D31)+INT(E31/12)</f>
         <v>2022</v>
       </c>
-      <c r="G31" s="255">
-        <f t="shared" ref="G31:G35" si="9">MOD(INT(E31/3),4)+1</f>
-        <v>1</v>
-      </c>
-      <c r="H31" s="262">
-        <f t="shared" ref="H31:H35" si="10">INT(IF(C31&gt;=0,B31,A31))</f>
+      <c r="G31" s="12">
+        <f t="shared" ref="G31:G35" si="11">MOD(INT(E31/3),4)+1</f>
+        <v>1</v>
+      </c>
+      <c r="H31" s="253">
+        <f t="shared" ref="H31:H35" si="12">INT(IF(C31&gt;=0,B31,A31))</f>
         <v>44910</v>
       </c>
-      <c r="I31" s="255">
-        <f t="shared" ref="I31:I35" si="11">MONTH(H31)-N(P31)-1</f>
+      <c r="I31" s="12">
+        <f t="shared" ref="I31:I35" si="13">MONTH(H31)-N(P31)-1</f>
         <v>10</v>
       </c>
-      <c r="J31" s="255">
-        <f t="shared" ref="J31:J35" si="12">YEAR(H31)+INT(I31/12)</f>
+      <c r="J31" s="12">
+        <f t="shared" ref="J31:J35" si="14">YEAR(H31)+INT(I31/12)</f>
         <v>2022</v>
       </c>
-      <c r="K31" s="255">
-        <f t="shared" ref="K31:K35" si="13">MOD(INT(I31/3),4)+1</f>
+      <c r="K31" s="12">
+        <f t="shared" ref="K31:K35" si="15">MOD(INT(I31/3),4)+1</f>
         <v>4</v>
       </c>
-      <c r="L31" s="255">
-        <f t="shared" ref="L31:L35" si="14">C31*((J31-F31)*4+K31-G31+1)</f>
+      <c r="L31" s="12">
+        <f t="shared" ref="L31:L35" si="16">C31*((J31-F31)*4+K31-G31+1)</f>
         <v>-4</v>
       </c>
       <c r="M31" s="155" cm="1">
@@ -19041,12 +19104,12 @@
       <c r="P31" s="12">
         <v>1</v>
       </c>
-      <c r="Q31" s="255" cm="1">
+      <c r="Q31" s="12" cm="1">
         <f t="array" ref="Q31">CALENDAR.EXTENT_OF_QUARTERS(M31,N31,O31,P31)</f>
         <v>-4</v>
       </c>
       <c r="R31" s="177" t="b">
-        <f>L31=Q31</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -19057,44 +19120,44 @@
       <c r="B32" s="181">
         <v>45413.75</v>
       </c>
-      <c r="C32" s="254" cm="1">
+      <c r="C32" s="9" cm="1">
         <f t="array" ref="C32">_xlfn.IFS(A32=B32,0,B32&gt;A32,1,TRUE,-1)</f>
         <v>1</v>
       </c>
-      <c r="D32" s="261">
+      <c r="D32" s="252">
+        <f t="shared" si="9"/>
+        <v>44967</v>
+      </c>
+      <c r="E32" s="9">
         <f t="shared" si="7"/>
-        <v>44967</v>
-      </c>
-      <c r="E32" s="254">
-        <f>MONTH(D32)-N(P32)-1</f>
-        <v>1</v>
-      </c>
-      <c r="F32" s="254">
-        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="F32" s="9">
+        <f t="shared" si="10"/>
         <v>2023</v>
       </c>
-      <c r="G32" s="254">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="H32" s="261">
-        <f t="shared" si="10"/>
+      <c r="G32" s="9">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="H32" s="252">
+        <f t="shared" si="12"/>
         <v>45413</v>
       </c>
-      <c r="I32" s="254">
-        <f t="shared" si="11"/>
+      <c r="I32" s="9">
+        <f t="shared" si="13"/>
         <v>4</v>
       </c>
-      <c r="J32" s="254">
-        <f t="shared" si="12"/>
+      <c r="J32" s="9">
+        <f t="shared" si="14"/>
         <v>2024</v>
       </c>
-      <c r="K32" s="254">
-        <f t="shared" si="13"/>
+      <c r="K32" s="9">
+        <f t="shared" si="15"/>
         <v>2</v>
       </c>
-      <c r="L32" s="254">
-        <f t="shared" si="14"/>
+      <c r="L32" s="9">
+        <f t="shared" si="16"/>
         <v>6</v>
       </c>
       <c r="M32" s="154" cm="1">
@@ -19109,12 +19172,12 @@
         <v>-600</v>
       </c>
       <c r="P32" s="9"/>
-      <c r="Q32" s="254" cm="1">
+      <c r="Q32" s="9" cm="1">
         <f t="array" ref="Q32">CALENDAR.EXTENT_OF_QUARTERS(M32,N32,O32,P32)</f>
         <v>6</v>
       </c>
       <c r="R32" s="176" t="b">
-        <f>L32=Q32</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -19125,44 +19188,44 @@
       <c r="B33" s="185">
         <v>45413.75</v>
       </c>
-      <c r="C33" s="256" cm="1">
+      <c r="C33" s="49" cm="1">
         <f t="array" ref="C33">_xlfn.IFS(A33=B33,0,B33&gt;A33,1,TRUE,-1)</f>
         <v>1</v>
       </c>
-      <c r="D33" s="263">
+      <c r="D33" s="254">
+        <f t="shared" si="9"/>
+        <v>45000</v>
+      </c>
+      <c r="E33" s="49">
         <f t="shared" si="7"/>
-        <v>45000</v>
-      </c>
-      <c r="E33" s="256">
-        <f>MONTH(D33)-N(P33)-1</f>
         <v>2</v>
       </c>
-      <c r="F33" s="256">
-        <f t="shared" si="8"/>
+      <c r="F33" s="49">
+        <f t="shared" si="10"/>
         <v>2023</v>
       </c>
-      <c r="G33" s="256">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="H33" s="263">
-        <f t="shared" si="10"/>
+      <c r="G33" s="49">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="H33" s="254">
+        <f t="shared" si="12"/>
         <v>45413</v>
       </c>
-      <c r="I33" s="256">
-        <f t="shared" si="11"/>
+      <c r="I33" s="49">
+        <f t="shared" si="13"/>
         <v>4</v>
       </c>
-      <c r="J33" s="256">
-        <f t="shared" si="12"/>
+      <c r="J33" s="49">
+        <f t="shared" si="14"/>
         <v>2024</v>
       </c>
-      <c r="K33" s="256">
-        <f t="shared" si="13"/>
+      <c r="K33" s="49">
+        <f t="shared" si="15"/>
         <v>2</v>
       </c>
-      <c r="L33" s="256">
-        <f t="shared" si="14"/>
+      <c r="L33" s="49">
+        <f t="shared" si="16"/>
         <v>6</v>
       </c>
       <c r="M33" s="156" cm="1">
@@ -19177,12 +19240,12 @@
         <v>570</v>
       </c>
       <c r="P33" s="49"/>
-      <c r="Q33" s="256" cm="1">
+      <c r="Q33" s="49" cm="1">
         <f t="array" ref="Q33">CALENDAR.EXTENT_OF_QUARTERS(M33,N33,O33,P33)</f>
         <v>6</v>
       </c>
       <c r="R33" s="178" t="b">
-        <f>L33=Q33</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -19193,44 +19256,44 @@
       <c r="B34" s="181">
         <v>45047.75</v>
       </c>
-      <c r="C34" s="254" cm="1">
+      <c r="C34" s="9" cm="1">
         <f t="array" ref="C34">_xlfn.IFS(A34=B34,0,B34&gt;A34,1,TRUE,-1)</f>
         <v>1</v>
       </c>
-      <c r="D34" s="261">
+      <c r="D34" s="252">
+        <f t="shared" si="9"/>
+        <v>45031</v>
+      </c>
+      <c r="E34" s="9">
         <f t="shared" si="7"/>
-        <v>45031</v>
-      </c>
-      <c r="E34" s="254">
-        <f>MONTH(D34)-N(P34)-1</f>
         <v>9</v>
       </c>
-      <c r="F34" s="254">
-        <f t="shared" si="8"/>
+      <c r="F34" s="9">
+        <f t="shared" si="10"/>
         <v>2023</v>
       </c>
-      <c r="G34" s="254">
-        <f t="shared" si="9"/>
+      <c r="G34" s="9">
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
-      <c r="H34" s="261">
-        <f t="shared" si="10"/>
+      <c r="H34" s="252">
+        <f t="shared" si="12"/>
         <v>45047</v>
       </c>
-      <c r="I34" s="254">
-        <f t="shared" si="11"/>
+      <c r="I34" s="9">
+        <f t="shared" si="13"/>
         <v>10</v>
       </c>
-      <c r="J34" s="254">
-        <f t="shared" si="12"/>
+      <c r="J34" s="9">
+        <f t="shared" si="14"/>
         <v>2023</v>
       </c>
-      <c r="K34" s="254">
-        <f t="shared" si="13"/>
+      <c r="K34" s="9">
+        <f t="shared" si="15"/>
         <v>4</v>
       </c>
-      <c r="L34" s="254">
-        <f t="shared" si="14"/>
+      <c r="L34" s="9">
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="M34" s="154" cm="1">
@@ -19247,12 +19310,12 @@
       <c r="P34" s="9">
         <v>-6</v>
       </c>
-      <c r="Q34" s="254" cm="1">
+      <c r="Q34" s="9" cm="1">
         <f t="array" ref="Q34">CALENDAR.EXTENT_OF_QUARTERS(M34,N34,O34,P34)</f>
         <v>1</v>
       </c>
       <c r="R34" s="176" t="b">
-        <f>L34=Q34</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -19263,44 +19326,44 @@
       <c r="B35" s="185">
         <v>45170.75</v>
       </c>
-      <c r="C35" s="256" cm="1">
+      <c r="C35" s="49" cm="1">
         <f t="array" ref="C35">_xlfn.IFS(A35=B35,0,B35&gt;A35,1,TRUE,-1)</f>
         <v>1</v>
       </c>
-      <c r="D35" s="263">
+      <c r="D35" s="254">
+        <f t="shared" si="9"/>
+        <v>45061</v>
+      </c>
+      <c r="E35" s="49">
         <f t="shared" si="7"/>
-        <v>45061</v>
-      </c>
-      <c r="E35" s="256">
-        <f>MONTH(D35)-N(P35)-1</f>
         <v>10</v>
       </c>
-      <c r="F35" s="256">
-        <f t="shared" si="8"/>
+      <c r="F35" s="49">
+        <f t="shared" si="10"/>
         <v>2023</v>
       </c>
-      <c r="G35" s="256">
-        <f t="shared" si="9"/>
+      <c r="G35" s="49">
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
-      <c r="H35" s="263">
-        <f t="shared" si="10"/>
+      <c r="H35" s="254">
+        <f t="shared" si="12"/>
         <v>45170</v>
       </c>
-      <c r="I35" s="256">
-        <f t="shared" si="11"/>
+      <c r="I35" s="49">
+        <f t="shared" si="13"/>
         <v>14</v>
       </c>
-      <c r="J35" s="256">
-        <f t="shared" si="12"/>
+      <c r="J35" s="49">
+        <f t="shared" si="14"/>
         <v>2024</v>
       </c>
-      <c r="K35" s="256">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-      <c r="L35" s="256">
-        <f t="shared" si="14"/>
+      <c r="K35" s="49">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="L35" s="49">
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="M35" s="156" cm="1">
@@ -19317,12 +19380,12 @@
       <c r="P35" s="49">
         <v>-6</v>
       </c>
-      <c r="Q35" s="256" cm="1">
+      <c r="Q35" s="49" cm="1">
         <f t="array" ref="Q35">CALENDAR.EXTENT_OF_QUARTERS(M35,N35,O35,P35)</f>
         <v>2</v>
       </c>
       <c r="R35" s="178" t="b">
-        <f>L35=Q35</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -19367,11 +19430,11 @@
       <c r="B41" s="181">
         <v>45081.999988425923</v>
       </c>
-      <c r="C41" s="254" cm="1">
+      <c r="C41" s="9" cm="1">
         <f t="array" ref="C41">_xlfn.IFS(A41=B41,0,B41&gt;A41,1,TRUE,-1)</f>
         <v>1</v>
       </c>
-      <c r="D41" s="254">
+      <c r="D41" s="9">
         <f>C41*(ABS(YEAR(B41)-YEAR(A41))+1)</f>
         <v>1</v>
       </c>
@@ -19384,12 +19447,12 @@
         <v>2460100.499988426</v>
       </c>
       <c r="G41" s="9"/>
-      <c r="H41" s="254" cm="1">
+      <c r="H41" s="9" cm="1">
         <f t="array" ref="H41">CALENDAR.EXTENT_OF_MONTHS(E41,F41,G41)</f>
         <v>2</v>
       </c>
       <c r="I41" s="176" t="b">
-        <f t="shared" ref="I41:I44" si="15">D41=H41</f>
+        <f t="shared" ref="I41:I44" si="17">D41=H41</f>
         <v>0</v>
       </c>
     </row>
@@ -19400,12 +19463,12 @@
       <c r="B42" s="183">
         <v>45077.25</v>
       </c>
-      <c r="C42" s="255" cm="1">
+      <c r="C42" s="12" cm="1">
         <f t="array" ref="C42">_xlfn.IFS(A42=B42,0,B42&gt;A42,1,TRUE,-1)</f>
         <v>-1</v>
       </c>
-      <c r="D42" s="255">
-        <f t="shared" ref="D42:D44" si="16">C42*(ABS(YEAR(B42)-YEAR(A42))+1)</f>
+      <c r="D42" s="12">
+        <f t="shared" ref="D42:D44" si="18">C42*(ABS(YEAR(B42)-YEAR(A42))+1)</f>
         <v>-1</v>
       </c>
       <c r="E42" s="155" cm="1">
@@ -19417,12 +19480,12 @@
         <v>2460095.75</v>
       </c>
       <c r="G42" s="12"/>
-      <c r="H42" s="255" cm="1">
+      <c r="H42" s="12" cm="1">
         <f t="array" ref="H42">CALENDAR.EXTENT_OF_MONTHS(E42,F42,G42)</f>
         <v>-2</v>
       </c>
       <c r="I42" s="177" t="b">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -19433,12 +19496,12 @@
       <c r="B43" s="181">
         <v>45413.75</v>
       </c>
-      <c r="C43" s="254" cm="1">
+      <c r="C43" s="9" cm="1">
         <f t="array" ref="C43">_xlfn.IFS(A43=B43,0,B43&gt;A43,1,TRUE,-1)</f>
         <v>1</v>
       </c>
-      <c r="D43" s="254">
-        <f t="shared" si="16"/>
+      <c r="D43" s="9">
+        <f t="shared" si="18"/>
         <v>2</v>
       </c>
       <c r="E43" s="154" cm="1">
@@ -19452,12 +19515,12 @@
       <c r="G43" s="9">
         <v>-600</v>
       </c>
-      <c r="H43" s="254" cm="1">
+      <c r="H43" s="9" cm="1">
         <f t="array" ref="H43">CALENDAR.EXTENT_OF_MONTHS(E43,F43,G43)</f>
         <v>13</v>
       </c>
       <c r="I43" s="176" t="b">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -19468,12 +19531,12 @@
       <c r="B44" s="185">
         <v>44347.25</v>
       </c>
-      <c r="C44" s="256" cm="1">
+      <c r="C44" s="49" cm="1">
         <f t="array" ref="C44">_xlfn.IFS(A44=B44,0,B44&gt;A44,1,TRUE,-1)</f>
         <v>-1</v>
       </c>
-      <c r="D44" s="256">
-        <f t="shared" si="16"/>
+      <c r="D44" s="49">
+        <f t="shared" si="18"/>
         <v>-3</v>
       </c>
       <c r="E44" s="156" cm="1">
@@ -19487,12 +19550,12 @@
       <c r="G44" s="49">
         <v>570</v>
       </c>
-      <c r="H44" s="256" cm="1">
+      <c r="H44" s="49" cm="1">
         <f t="array" ref="H44">CALENDAR.EXTENT_OF_MONTHS(E44,F44,G44)</f>
         <v>-25</v>
       </c>
       <c r="I44" s="178" t="b">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -20659,7 +20722,7 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<AFEJSONBlob xmlns="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0">ewAiAHMAYwBoAGUAbQBhACIAOgAiAGgAdAB0AHAAOgAvAC8AcwBjAGgAZQBtAGEAcwAuAGEAZAB2AGEAbgBjAGUAZABmAG8AcgBtAHUAbABhAGUAbgB2AGkAcgBvAG4AbQBlAG4AdAAuAG8AZgBmAGkAYwBlAGEAcABwAHMALgBsAGkAdgBlAC4AYwBvAG0ALwBhAGYAZQBwAHIAbwBqAGUAYwB0AHMALwAwAC4AMgAiACwAIgBmAGkAbABlAHMAIgA6AFsAewAiAHAAYQB0AGgAIgA6ACIALwBwAHIAbwBqAGUAYwB0AHMALwBXAG8AcgBrAGIAbwBvAGsAIgAsACIAdABlAHgAdAAiADoAIgAiAH0ALAB7ACIAcABhAHQAaAAiADoAIgAvAHAAcgBvAGoAZQBjAHQAcwAvAEMAQQBMAEUATgBEAEEAUgAiACwAIgB0AGUAeAB0ACIAOgAiAC8AKgAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAXABuACMAIABDAEEATABFAE4ARABBAFIAIAB2ADEAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABNAG8AZAB1AGwAZQAgAGYAbwByACAAdwBvAHIAawBpAG4AZwAgAHcAaQB0AGgAIABkAGEAdABlAHMAIABpAG4AIAB0AGgAZQAgAEcAcgBlAGcAbwByAGkAYQBuACAAYQBuAGQAIABKAHUAbABpAGEAbgAgAGMAYQBsAGUAbgBkAGEAcgBzACAAbwB1AHQAcwBpAGQAZQAgAHQAaABlACAAcgBhAG4AZwBlACAAbwBmACAAdABoAGUAIABFAHgAYwBlAGwAIAAgACAAIAAgACMAXABuACMAIABEAGEAdABlAC8AVABpAG0AZQAgAHQAeQBwAGUALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABNAG8AZAB1AGwAZQAgAEQAZQBwAGUAbgBkAGUAbgBjAGkAZQBzADoAIABOAG8AbgBlACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABMAE8ARwBJAEMAQQBMACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIAAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAgACMAXABuACMAIABJAFMAXwBMAEUAQQBQAF8AWQBFAEEAUgAgACAAIAAgACAAIAAgACAAIAAgACAAVABlAHMAdABzACAAaQBmACAAYQAgAHkAZQBhAHIAIABpAG4AYwBsAHUAZABlAHMAIABhACAAbABlAGEAcAAgAGQAYQB5ACAAaQBuACAAdABoAGUAIABnAGkAdgBlAG4AIABjAGEAbABlAG4AZABhAHIALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABJAFMAXwBWAEEATABJAEQAXwBEAEEAVABFACAAIAAgACAAIAAgACAAIAAgACAAVABlAHMAdABzACAAaQBmACAAYQAgAGQAYQB0AGUAIABpAHMAIAB2AGEAbABpAGQAIABmAG8AcgAgAHQAaABlACAAZwBpAHYAZQBuACAAYwBhAGwAZQBuAGQAYQByAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABJAFMAXwBWAEEATABJAEQAXwBUAEkATQBFACAAIAAgACAAIAAgACAAIAAgACAAVABlAHMAdABzACAAaQBmACAAYQAgAHQAaQBtAGUAIABpAHMAIAB2AGEAbABpAGQAIABpAG4AIAB0AGgAZQAgADIANAAgAGgAbwB1AHIAIAB0AGkAbQBlAGsAZQBlAHAAaQBuAGcAIABzAHkAcwB0AGUAbQAuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABDAEEATABFAE4ARABBAFIAIABEAEEAVABFAFMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIAAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAgACMAXABuACMAIABZAEUAQQBSAF8AQwBPAE0ATQBPAE4AXwBFAFIAQQAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHkAZQBhAHIAIAB2AGEAbAB1AGUAIAByAGUAbABhAHQAaQB2AGUAIAB0AG8AIAB0AGgAZQAgAEMAbwBtAG0AbwBuACAARQByAGEALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABEAEEAWQBTAF8ASQBOAF8AWQBFAEEAUgAgACAAIAAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAG4AdQBtAGIAZQByACAAbwBmACAAZABhAHkAcwAgAGkAbgAgAHQAaABlACAAZwBpAHYAZQBuACAAeQBlAGEAcgAgAG8AZgAgAHQAaABlACAAcwBwAGUAYwBpAGYAaQBlAGQAIABjAGEAbABlAG4AZABhAHIALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABEAEEAWQBTAF8ASQBOAF8ATQBPAE4AVABIACAAIAAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAG4AdQBtAGIAZQByACAAbwBmACAAZABhAHkAcwAgAGkAbgAgAHQAaABlACAAZwBpAHYAZQBuACAAbQBvAG4AdABoACAAYQBuAGQAIAB5AGUAYQByACAAbwBmACAAdABoAGUAIABzAHAAZQBjAGkAZgBpAGUAZAAgAGMAYQBsAGUAbgBkAGEAcgAuACAAIAAgACMAXABuACMAIABKAFUATABJAEEATgBfAEQAQQBZAF8ATgBVAE0AQgBFAFIAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByACAAbwBmACAAdABoAGUAIABwAHIAbwB2AGkAZABlAGQAIABkAGEAdABlACAAaQBuACAAdABoAGUAIABzAHAAZQBjAGkAZgBpAGUAZAAgAGMAYQBsAGUAbgBkAGEAcgAuACAAIAAgACMAXABuACMAIABKAEQATgBfAFQATwBfAEMAQQBMAEUATgBEAEEAUgBfAEQAQQBUAEUAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAAZABhAHQAZQAgAGYAcgBvAG0AIAB0AGgAZQAgAGcAaQB2AGUAbgAgAEoAdQBsAGkAYQBuACAARABhAHkAIABOAHUAbQBiAGUAcgAgAGkAbgAgAHQAaABlACAAcwBwAGUAYwBpAGYAaQBlAGQAIABjAGEAbABlAG4AZABhAHIALgAgACAAIAAgACMAXABuACMAIABKAEQATgBfAFQATwBfAE8AUgBEAEkATgBBAEwAXwBEAEEAVABFACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAAeQBlAGEAcgAsACAAbwByAGQAaQBuAGEAbAAgAGQAYQB5ACAAbwBmACAAeQBlAGEAcgAgAGEAbgBkACAAZABhAHkAcwAgAGkAbgAgAHQAaABlACAAeQBlAGEAcgAgAGYAcgBvAG0AIAB0AGgAZQAgAGcAaQB2AGUAbgAgACAAIAAgACAAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByACAAaQBuACAAdABoAGUAIABzAHAAZQBjAGkAZgBpAGUAZAAgAGMAYQBsAGUAbgBkAGEAcgAuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABPAFIARABJAE4AQQBMAF8ARABBAFQARQBfAFQATwBfAEoARABOACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByACAAbwBmACAAdABoAGUAIABwAHIAbwB2AGkAZABlAGQAIABvAHIAZABpAG4AYQBsACAAZABhAHQAZQAgAGkAbgAgAHQAaABlACAAcwBwAGUAYwBpAGYAaQBlAGQAIAAgACAAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAYwBhAGwAZQBuAGQAYQByAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABHAFIARQBHAE8AUgBJAEEATgBfAFQATwBfAEoAVQBMAEkAQQBOACAAIAAgACAAVAByAGEAbgBzAGwAYQB0AGUAcwAgAGEAIABkAGEAdABlACAAaQBuACAAdABoAGUAIABHAHIAZQBnAG8AcgBpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByACAAdABvACAAdABoAGUAIABKAHUAbABpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAYwBhAGwAZQBuAGQAYQByAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABKAFUATABJAEEATgBfAFQATwBfAEcAUgBFAEcATwBSAEkAQQBOACAAIAAgACAAVAByAGEAbgBzAGwAYQB0AGUAcwAgAGEAIABkAGEAdABlACAAaQBuACAAdABoAGUAIABKAHUAbABpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByACAAdABvACAAdABoAGUAIABHAHIAZQBnAG8AcgBpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAYwBhAGwAZQBuAGQAYQByAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABTAEUAQwBVAEwAQQBSAF8ARABJAEYARgBFAFIARQBOAEMARQAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAAbgB1AG0AYgBlAHIAIABvAGYAIABkAGEAeQBzACAAdABoAGUAIABHAHIAZQBnAG8AcgBpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByACAAaQBzACAAYQBoAGUAYQBkACAAbwBmACAAdABoAGUAIAAgACAAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASgB1AGwAaQBhAG4AIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAgAGYAbwByACAAYQAgAGcAaQB2AGUAbgAgAGQAYQB0AGUALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABXAEUARQBLAFMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIAAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAgACMAXABuACMAIABEAEEAWQBfAE8ARgBfAFcARQBFAEsAIAAgACAAIAAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAGEAbgAgAGkAbgB0AGUAZwBlAHIAIABmAG8AcgAgAHQAaABlACAAZABhAHkAIABvAGYAIAB0AGgAZQAgAHcAZQBlAGsAIABmAG8AcgAgAGEAIABnAGkAdgBlAG4AIABKAHUAbABpAGEAbgAgAEQAYQB5ACAATgB1AG0AYgBlAHIALgAgACAAIAAgACAAIAAgACMAXABuACMAIABDAE8ATgBWAEUAUgBUAF8AVwBFAEUASwBEAEEAWQBfAE4AVQBNAEIARQBSACAAUgBlAHQAdQByAG4AcwAgAGEAbgAgAGkAbgB0AGUAZwBlAHIAIABmAG8AcgAgAHQAaABlACAAZABhAHkAIABvAGYAIAB0AGgAZQAgAHcAZQBlAGsAIABmAHIAbwBtACAAdABoAGUAIAB0AHIAYQBkAGkAdABvAG4AYQBsACAAbgB1AG0AYgBlAHIAaQBuAGcAIABzAGMAaABlAG0AZQAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAdABvACAAdABoAGUAIABJAFMATwAgAGQAZQBmAGkAbgBpAHQAaQBvAG4ALAAgAG8AcgAgAHYAaQBjAGUAIAB2AGUAcgBzAGEALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABXAEUARQBLAEQAQQBZAF8ATwBGAF8ATQBPAE4AVABIACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAGEAIABKAHUAbABpAGEAbgAgAEQAYQB5ACAATgB1AG0AYgBlAHIAIABmAG8AcgAgAGEAIABnAGkAdgBlAG4AIABkAGEAeQAgAG8AZgAgAHcAZQBlAGsALAAgAGEAbgBkACAAYQAgAHIAZQBsAGEAdABpAHYAZQAgAHcAZQBlAGsAIABmAG8AcgAgACAAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAdABoAGUAIABtAG8AbgB0AGgAIABhAG4AZAAgAHkAZQBhAHIAIABvAGYAIAB0AGgAZQAgAHMAcABlAGMAaQBmAGkAZQBkACAAYwBhAGwAZQBuAGQAYQByAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABXAEUARQBLAFMAXwBJAE4AXwBZAEUAQQBSACAAIAAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAAYwBvAHUAbgB0ACAAbwBmACAASQBTAE8AIABkAGUAZgBpAG4AZQBkACAAdwBlAGUAawBzACAAaQBuACAAYQAgAGcAaQB2AGUAbgAgAHkAZQBhAHIAIABvAGYAIAB0AGgAZQAgAHMAcABlAGMAaQBmAGkAZQBkACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAYwBhAGwAZQBuAGQAYQByAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABXAEUARQBLAF8ARABBAFQARQBfAFQATwBfAEoARABOACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByACAAbwBmACAAdABoAGUAIABwAHIAbwB2AGkAZABlAGQAIAB3AGUAZQBrACAAZABhAHQAZQAgAGkAbgAgAHQAaABlACAAcwBwAGUAYwBpAGYAaQBlAGQAIAAgACAAIAAgACAAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAYwBhAGwAZQBuAGQAYQByAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABKAEQATgBfAFQATwBfAFcARQBFAEsAXwBEAEEAVABFACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAAeQBlAGEAcgAsACAASQBTAE8AIABkAGUAZgBpAG4AZQBkACAAdwBlAGUAawAgAG4AdQBtAGIAZQByACwAIABkAGEAeQAgAG8AZgAgAHQAaABlACAAdwBlAGUAawAsACAAYQBuAGQAIAB3AGUAZQBrAHMAIABpAG4AIAB0AGgAZQAgACAAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAeQBlAGEAcgAgAGYAbwByACAAdABoAGUAIABnAGkAdgBlAG4AIABKAHUAbABpAGEAbgAgAEQAYQB5ACAATgB1AG0AYgBlAHIAIABpAG4AIAB0AGgAZQAgAHMAcABlAGMAaQBmAGkAZQBkACAAYwBhAGwAZQBuAGQAYQByAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABXAEUARQBLAF8ATgBVAE0AQgBFAFIAIAAgACAAIAAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAASQBTAE8AIABkAGUAZgBpAG4AZQBkACAAdwBlAGUAawAgAG4AdQBtAGIAZQByACAAZgBvAHIAIABhACAAZwBpAHYAZQBuACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByACAAaQBuACAAdABoAGUAIAAgACAAIAAgACAAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAcwBwAGUAYwBpAGYAaQBlAGQAIABjAGEAbABlAG4AZABhAHIALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABRAFUAQQBSAFQARQBSAFMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIAAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAgACMAXABuACMAIABEAEEAWQBTAF8ASQBOAF8AUQBVAEEAUgBUAEUAUgAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAAYwBvAHUAbgB0ACAAbwBmACAAZABhAHkAcwAgAGkAbgAgAGEAIABxAHUAYQByAHQAZQByACAAbwBmACAAYQAgAGcAaQB2AGUAbgAgAHkAZQBhAHIAIABvAGYAIAB0AGgAZQAgAHMAcABlAGMAaQBmAGkAZQBkACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAYwBhAGwAZQBuAGQAYQByAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABKAEQATgBfAFQATwBfAFEAVQBBAFIAVABFAFIAXwBEAEEAVABFACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAAeQBlAGEAcgAsACAAcQB1AGEAcgB0AGUAcgAsACAAZABhAHkAIABvAGYAIABxAHUAYQByAHQAZQByACAAYQBuAGQAIABkAGEAeQBzACAAaQBuACAAdABoAGUAIABxAHUAYQByAHQAZQByACAAZgBvAHIAIAB0AGgAZQAgAGcAaQB2AGUAbgAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByACAAaQBuACAAdABoAGUAIABzAHAAZQBjAGkAZgBpAGUAZAAgAGMAYQBsAGUAbgBkAGEAcgAuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABRAFUAQQBSAFQARQBSAF8ARABBAFQARQBfAFQATwBfAEoARABOACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByACAAbwBmACAAdABoAGUAIABwAHIAbwB2AGkAZABlAGQAIABxAHUAYQByAHQAZQByACAAZABhAHQAZQAgAGkAbgAgAHQAaABlACAAcwBwAGUAYwBpAGYAaQBlAGQAIAAgACAAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAYwBhAGwAZQBuAGQAYQByAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABEAEEAVABFACAAQQBOAEQAIABUAEkATQBFACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIAAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAgACMAXABuACMAIABKAEQATgBfAFUAVABDAF8AVABPAF8ASgBEAEEAVABFACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAASgB1AGwAaQBhAG4AIABEAGEAdABlACAAZwBpAHYAZQBuACAAYQBuACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByACAAYQBuAGQAIAB0AGkAbQBlACAAbwBmACAAZABhAHkAIABpAG4AIABVAFQAQwAuACAAIAAgACAAIAAgACMAXABuACMAIABKAEQATgBfAEwATwBDAEEATABfAFQATwBfAEoARABBAFQARQAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAASgB1AGwAaQBhAG4AIABEAGEAdABlACAAZwBpAHYAZQBuACAAYQAgAGwAbwBjAGEAbAAgAEoAdQBsAGkAYQBuACAARABhAHkAIABOAHUAbQBiAGUAcgAgAGEAbgBkACAAbABvAGMAYQBsACAAdABpAG0AZQAgAG8AZgAgAGQAYQB5ACAAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAdwBpAHQAaAAgAHQAaQBtAGUAIAB6AG8AbgBlACAAbwBmAGYAcwBlAHQAIABpAG4AIABtAGkAbgB1AHQAZQBzAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABKAEQAQQBUAEUAXwBUAE8AXwBKAEQATgBfAFUAVABDACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByACAAYQBuAGQAIAB0AGkAbQBlACAAbwBmACAAZABhAHkAIABpAG4AIABVAFQAQwAgAG8AZgAgAGEAIABnAGkAdgBlAG4AIABKAHUAbABpAGEAbgAgAEQAYQB0AGUALgAgACAAIAAgACMAXABuACMAIABKAEQAQQBUAEUAXwBUAE8AXwBKAEQATgBfAEwATwBDAEEATAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAAbABvAGMAYQBsACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByACAAYQBuAGQAIAB0AGkAbQBlACAAbwBmACAAZABhAHkAIABvAGYAIABhACAAZwBpAHYAZQBuACAASgB1AGwAaQBhAG4AIABEAGEAdABlAC4AIAAgACAAIAAgACMAXABuACMAIABKAFUATABJAEEATgBfAEQAQQBUAEUAIAAgACAAIAAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAASgB1AGwAaQBhAG4AIABEAGEAdABlACAAbwBmACAAdABoAGUAIABwAHIAbwB2AGkAZABlAGQAIABjAGEAbABlAG4AZABhAHIAIABkAGEAdABlACAAYQBuAGQAIAB0AGkAbQBlACAAbwBmACAAZABhAHkALgAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABDAEEATABFAE4ARABBAFIAXwBGAFIATwBNAF8ASgBEAEEAVABFACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAAYwBhAGwAZQBuAGQAYQByACAAZABhAHQAZQAgAGEAbgBkACAAbABvAGMAYQBsACAAdABpAG0AZQAgAG8AZgAgAGQAYQB5ACAAZgBvAHIAIABhACAAZwBpAHYAZQBuACAASgB1AGwAaQBhAG4AIABEAGEAdABlACAAYQBuAGQAIAAgACAAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAdABpAG0AZQAgAHoAbwBuAGUAIABvAGYAZgBzAGUAdAAuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABUAEkATQBFAF8ARABFAEMASQBNAEEATABfAFQATwBfAEgATQBTACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAAMgA0ACAAaABvAHUAcgAgAHQAaQBtAGUAawBlAGUAcABpAG4AZwAgAHIAZQBwAHIAZQBzAGUAbgB0AGEAdABpAG8AbgAgAG8AZgAgAGEAIABkAGUAYwBpAG0AYQBsACAAdABpAG0AZQAgAHYAYQBsAHUAZQAuACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABIAE0AUwBfAFQATwBfAFQASQBNAEUAXwBEAEUAQwBJAE0AQQBMACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAGEAIABkAGUAYwBpAG0AYQBsACAAdABpAG0AZQAgAGEAcwAgAGEAIABmAHIAYQBjAHQAaQBvAG4AIABvAGYAIABhACAAZABhAHkAIABmAHIAbwBtACAAYQAgADIANAAgAGgAbwB1AHIAIAB0AGkAbQBlAGsAZQBlAHAAaQBuAGcAIAB2AGEAbAB1AGUAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAbwBmACAAdABpAG0AZQAuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuAFwAbgAjACAAQQBEAEQAXwBUAEkATQBFAFMAUABBAE4AIAAgACAAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAEoAdQBsAGkAYQBuACAARABhAHQAZQAgAG8AZgAgAHQAaABlACAAYQBkAGQAaQB0AGkAbwBuACAAbwBmACAAdABoAGUAIABwAHIAbwB2AGkAZABlAGQAIABjAGEAbABlAG4AZABhAHIAIABkAGEAdABlACAAYQBuAGQAIAB0AGkAbQBlACAAIAAjAFwAbgAjACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAG8AZgAgAGQAYQB5ACAAYQBuAGQAIABhACAAdABpAG0AZQBzAHAAYQBuACAAYwBvAG0AcABsAGkAYwBhAHQAaQBvAG4ALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAAUgBFAFMATwBMAFYARQBfAEQAQQBUAEUAIAAgACAAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIABhACAAYwBhAGwAZQBuAGQAYQByACAAZABhAHQAZQAgAGYAcgBvAG0AIABwAHIAbwB2AGkAZABlAGQAIABkAGUAYwBpAG0AYQBsACAAeQBlAGEAcgAsACAAbQBvAG4AdABoAHMALAAgAGQAYQB5AHMAIABhAG4AZAAgAHQAaQBtAGUALgAgACAAIAAgACAAIAAjAFwAbgAjACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARABFAEwAVABBACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AIAAjAFwAbgAjACAARABFAEwAVABBAF8ASQBOAFQARQBSAFYAQQBMACAAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHQAaQBtAGUAcwBwAGEAbgAgAGQAaQBmAGYAZQByAGUAbgBjAGUAIABiAGUAdAB3AGUAZQBuACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMAIABpAG4AIAB0AGgAZQAgAHMAcABlAGMAaQBmAGkAZQBkACAAdQBuAGkAdABzAC4AIAAgACAAIAAjAFwAbgAjACAARABFAEwAVABBAF8ASABPAFUAUgBTACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHQAaQBtAGUAcwBwAGEAbgAgAGQAaQBmAGYAZQByAGUAbgBjAGUAIABiAGUAdAB3AGUAZQBuACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMAIABpAG4AIABoAG8AdQByAHMALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARABFAEwAVABBAF8ATQBJAE4AVQBUAEUAUwAgACAAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHQAaQBtAGUAcwBwAGEAbgAgAGQAaQBmAGYAZQByAGUAbgBjAGUAIABiAGUAdAB3AGUAZQBuACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMAIABpAG4AIABtAGkAbgB1AHQAZQBzAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARABFAEwAVABBAF8AUwBFAEMATwBOAEQAUwAgACAAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHQAaQBtAGUAcwBwAGEAbgAgAGQAaQBmAGYAZQByAGUAbgBjAGUAIABiAGUAdAB3AGUAZQBuACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMAIABpAG4AIABzAGUAYwBvAG4AZABzAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARABFAEwAVABBAF8ASABPAFUAUgBfAE0ASQBOAF8AUwBFAEMAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHQAaQBtAGUAcwBwAGEAbgAgAGQAaQBmAGYAZQByAGUAbgBjAGUAIABiAGUAdAB3AGUAZQBuACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMAIABpAG4AIABoAG8AdQByAHMALAAgAG0AaQBuAHUAdABlAHMAIABhAG4AZAAgACAAIAAgACAAIAAjAFwAbgAjACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHMAZQBjAG8AbgBkAHMALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARABFAEwAVABBAF8ARABBAFkAUwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHQAaQBtAGUAcwBwAGEAbgAgAGQAaQBmAGYAZQByAGUAbgBjAGUAIABiAGUAdAB3AGUAZQBuACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMAIABpAG4AIABkAGEAeQBzAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARABFAEwAVABBAF8AVwBFAEUASwBTACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHQAaQBtAGUAcwBwAGEAbgAgAGQAaQBmAGYAZQByAGUAbgBjAGUAIABiAGUAdAB3AGUAZQBuACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMAIABpAG4AIAB3AGUAZQBrAHMALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARABFAEwAVABBAF8ATQBPAE4AVABIAFMAIAAgACAAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHQAaQBtAGUAcwBwAGEAbgAgAGQAaQBmAGYAZQByAGUAbgBjAGUAIABiAGUAdAB3AGUAZQBuACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMAIABpAG4AIABtAG8AbgB0AGgAcwAuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARABFAEwAVABBAF8AUQBVAEEAUgBUAEUAUgBTACAAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHQAaQBtAGUAcwBwAGEAbgAgAGQAaQBmAGYAZQByAGUAbgBjAGUAIABiAGUAdAB3AGUAZQBuACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMAIABpAG4AIABxAHUAYQByAHQAZQByAHMALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARABFAEwAVABBAF8AWQBFAEEAUgBTACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHQAaQBtAGUAcwBwAGEAbgAgAGQAaQBmAGYAZQByAGUAbgBjAGUAIABiAGUAdAB3AGUAZQBuACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMAIABpAG4AIAB5AGUAYQByAHMALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARABFAEwAVABBAF8AVwBFAEUASwBfAEQAQQBZAFMAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHQAaQBtAGUAcwBwAGEAbgAgAGQAaQBmAGYAZQByAGUAbgBjAGUAIABiAGUAdAB3AGUAZQBuACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMAIABpAG4AIAB3AGUAZQBrAHMAIABhAG4AZAAgAGQAYQB5AHMALgAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARABFAEwAVABBAF8AWQBFAEEAUgBfAFcARQBFAEsAXwBEAEEAWQBTACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHQAaQBtAGUAcwBwAGEAbgAgAGQAaQBmAGYAZQByAGUAbgBjAGUAIABiAGUAdAB3AGUAZQBuACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMAIABpAG4AIAB5AGUAYQByAHMALAAgAHcAZQBlAGsAcwAgAGEAbgBkACAAZABhAHkAcwAuACAAIAAjAFwAbgAjACAARABFAEwAVABBAF8ATQBPAE4AVABIAF8ARABBAFkAUwAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHQAaQBtAGUAcwBwAGEAbgAgAGQAaQBmAGYAZQByAGUAbgBjAGUAIABiAGUAdAB3AGUAZQBuACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMAIABpAG4AIABtAG8AbgB0AGgAcwAgAGEAbgBkACAAZABhAHkAcwAuACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARABFAEwAVABBAF8AUQBVAEEAUgBUAEUAUgBfAEQAQQBZAFMAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHQAaQBtAGUAcwBwAGEAbgAgAGQAaQBmAGYAZQByAGUAbgBjAGUAIABiAGUAdAB3AGUAZQBuACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMAIABpAG4AIABxAHUAYQByAHQAZQByAHMAIABhAG4AZAAgAGQAYQB5AHMALgAgACAAIAAgACAAIAAjAFwAbgAjACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARQBYAFQARQBOAFQAUwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AIAAjAFwAbgAjACAARQBYAFQARQBOAFQAXwBPAEYAXwBEAEEAWQBTACAAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAGkAbgBjAGwAdQBzAGkAdgBlACAAZQB4AHQAZQBuAHQAIABvAGYAIABkAGEAeQBzACAAcwBwAGEAbgBuAGUAZAAgAGIAeQAgAHQAdwBvACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARQBYAFQARQBOAFQAXwBPAEYAXwBXAEUARQBLAFMAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAGkAbgBjAGwAdQBzAGkAdgBlACAAZQB4AHQAZQBuAHQAIABvAGYAIAB3AGUAZQBrAHMAIABzAHAAYQBuAG4AZQBkACAAYgB5ACAAdAB3AG8AIABKAHUAbABpAGEAbgAgAEQAYQB0AGUAcwAuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARQBYAFQARQBOAFQAXwBPAEYAXwBNAE8ATgBUAEgAUwAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAGkAbgBjAGwAdQBzAGkAdgBlACAAZQB4AHQAZQBuAHQAIABvAGYAIABtAG8AbgB0AGgAcwAgAHMAcABhAG4AbgBlAGQAIABiAHkAIAB0AHcAbwAgAEoAdQBsAGkAYQBuACAARABhAHQAZQBzAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARQBYAFQARQBOAFQAXwBPAEYAXwBRAFUAQQBSAFQARQBSAFMAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAGkAbgBjAGwAdQBzAGkAdgBlACAAZQB4AHQAZQBuAHQAIABvAGYAIABxAHUAYQByAHQAZQByAHMAIABzAHAAYQBuAG4AZQBkACAAYgB5ACAAdAB3AG8AIABKAHUAbABpAGEAbgAgAEQAYQB0AGUAcwAuACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARQBYAFQARQBOAFQAXwBPAEYAXwBZAEUAQQBSAFMAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAGkAbgBjAGwAdQBzAGkAdgBlACAAZQB4AHQAZQBuAHQAIABvAGYAIAB5AGUAYQByAHMAIABzAHAAYQBuAG4AZQBkACAAYgB5ACAAdAB3AG8AIABKAHUAbABpAGEAbgAgAEQAYQB0AGUAcwAuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAAUABBAFIAUwBJAE4ARwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AIAAjAFwAbgAjACAAUABBAFIAUwBFAF8ASQBTAE8AXwBEAEEAVABFACAAIAAgACAAIAAgACAAIAAgAFAAYQByAHMAZQBzACAAYQBuACAASQBTAE8AIABmAG8AcgBtAGEAdAB0AGUAZAAgAGQAYQB0AGUAIABpAG4AdABvACAAcgBlAHMAcABlAGMAdABpAHYAZQAgAHAAYQByAHQAcwAgAG8AZgAgAHkAZQBhAHIALAAgAG0AbwBuAHQAaAAsACAAZABhAHkALAAgAHQAaQBtAGUAIABvAGYAIAAjAFwAbgAjACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAGQAYQB5ACAAYQBuAGQAIAB0AGkAbQBlACAAegBvAG4AZQAgAG8AZgBmAHMAZQB0ACAAaQBuACAAbQBpAG4AdQB0AGUAcwAgAGYAcgBvAG0AIABVAFQAQwAuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAAUABBAFIAUwBFAF8AVwBFAEUASwBEAEEAWQAgACAAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIABhACAAbgB1AG0AYgBlAHIAIAByAGUAcAByAGUAcwBlAG4AdABpAG4AZwAgAHQAaABlACAAZABhAHkAIABvAGYAIAB0AGgAZQAgAHcAZQBlAGsAIABmAHIAbwBtACAAYQAgAGcAaQB2AGUAbgAgAHQAZQB4AHQAIAB3AGUAZQBrAGQAYQB5ACAAIAAgACAAIAAjAFwAbgAjACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAG4AYQBtAGUALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAAUABBAFIAUwBFAF8ATQBPAE4AVABIACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIABhACAAbgB1AG0AYgBlAHIAIAByAGUAcAByAGUAcwBlAG4AdABpAG4AZwAgAHQAaABlACAAbQBvAG4AdABoACAAbwBmACAAeQBlAGEAcgAgAGYAcgBvAG0AIABhACAAZwBpAHYAZQBuACAAbQBvAG4AdABoACAAbgBhAG0AZQAuACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAAUABBAFIAUwBFAF8ATABJAFQARQBSAEEAUgBZAF8AWQBFAEEAUgAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIABhACAAbgB1AG0AYgBlAHIAIAByAGUAcAByAGUAcwBlAG4AdABpAG4AZwAgAHQAaABlACAAeQBlAGEAcgAgAHIAZQBsAGEAdABpAHYAZQAgAHQAbwAgAHQAaABlACAAYwBvAG0AbQBvAG4AIABlAHIAYQAgAGYAcgBvAG0AIABhACAAZwBpAHYAZQBuACAAIAAjAFwAbgAjACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAGwAaQB0AGUAcgBhAHIAeQAgAHkAZQBhAHIALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAAUABBAFIAUwBFAF8ATABJAFQARQBSAEEAUgBZAF8ARABBAFQARQAgACAAIAAgAFAAYQByAHMAZQBzACAAYQAgAGwAaQB0AGUAcgBhAHIAeQAgAGQAYQB0AGUAIABpAG4AdABvACAAcgBlAHMAcABlAGMAdABpAHYAZQAgAHAAYQByAHQAcwAgAG8AZgAgAHkAZQBhAHIALAAgAG0AbwBuAHQAaAAsACAAZABhAHkAIABhAG4AZAAgAHQAaQBtAGUAIABvAGYAIAAgACAAIAAjAFwAbgAjACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAGQAYQB5AC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAAUABBAFIAUwBFAF8AVQBTAF8ARABBAFQARQAgACAAIAAgACAAIAAgACAAIAAgAFAAYQByAHMAZQBzACAAYQAgAFUAUwAgAGYAbwByAG0AYQB0AHQAZQBkACAAZABhAHQAZQAgAGkAbgB0AG8AIAByAGUAcwBwAGUAYwB0AGkAdgBlACAAcABhAHIAdABzACAAbwBmACAAeQBlAGEAcgAsACAAbQBvAG4AdABoACwAIABkAGEAeQAgAGEAbgBkACAAdABpAG0AZQAgACAAIAAjAFwAbgAjACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAG8AZgAgAGQAYQB5AC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAAUABBAFIAUwBFAF8ATQBJAEwAXwBEAFQARwAgACAAIAAgACAAIAAgACAAIAAgAFAAYQByAHMAZQBzACAAYQAgAGQAYQB0AGUALQB0AGkAbQBlACAAZwByAG8AdQBwACAAaQBuACAAdABoAGUAIABmAG8AcgBtAGEAdAAgAHUAcwBlAGQAIABiAHkAIABVAFMAIABNAGkAbABpAHQAYQByAHkAIABtAGUAcwBzAGEAZwBlACAAdAByAGEAZgBmAGkAYwAsACAAIAAgACAAIAAjAFwAbgAjACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAGkAbgB0AG8AIAByAGUAcwBwAGUAYwB0AGkAdgBlACAAcABhAHIAdABzACAAbwBmACAAeQBlAGEAcgAsACAAbQBvAG4AdABoACwAIABkAGEAeQAsACAAdABpAG0AZQAgAG8AZgAgAGQAYQB5ACAAYQBuAGQAIAB0AGkAbQBlACAAegBvAG4AZQAgAG8AZgBmAHMAZQB0ACAAaQBuACAAIAAjAFwAbgAjACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAG0AaQBuAHUAdABlAHMAIABmAHIAbwBtACAAVQBUAEMALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAAVABFAFgAVAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AIAAjAFwAbgAjACAAVwBFAEUASwBEAEEAWQBfAE4AQQBNAEUAIAAgACAAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIABuAGEAbQBlACAAbwBmACAAYQBuACAASQBTAE8AIABkAGEAeQAgAG8AZgAgAHcAZQBlAGsAIABuAHUAbQBiAGUAcgAgAGEAcwAgAHQAZQB4AHQALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAATQBPAE4AVABIAF8ATgBBAE0ARQAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIABuAGEAbQBlACAAbwBmACAAbQBvAG4AdABoAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARgBPAFIATQBBAFQAXwBJAFMATwBfAEQAQQBUAEUAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIABhACAAZABhAHQAZQAgAGEAcwAgAHQAZQB4AHQAIABpAG4AIABJAFMATwAgAGYAbwByAG0AYQB0AC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARgBPAFIATQBBAFQAXwBMAEkAVABFAFIAQQBSAFkAXwBZAEUAQQBSACAAIAAgAFIAZQB0AHUAcgBuAHMAIABhACAAeQBlAGEAcgAgAGYAbwByAG0AYQB0AHQAZQBkACAAaQBuACAAbABpAHQAZQByAGEAcgB5ACAAcwB0AHkAbABlAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARgBPAFIATQBBAFQAXwBMAEkAVABFAFIAQQBSAFkAXwBEAEEAVABFACAAIAAgAFIAZQB0AHUAcgBuAHMAIABhACAAZABhAHQAZQAgAGYAbwByAG0AYQB0AHQAZQBkACAAaQBuACAAbABpAHQAZQByAGEAcgB5ACAAcwB0AHkAbABlAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARgBPAFIATQBBAFQAXwBVAFMAXwBEAEEAVABFACAAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIABhACAAZABhAHQAZQAgAGYAbwByAG0AYQB0AHQAZQBkACAAaQBuACAAdABoAGUAIABVAFMAIABzAHQAeQBsAGUALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARgBPAFIATQBBAFQAXwBNAEkATABfAEQAVABHACAAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIABhACAAZABhAHQAZQAtAHQAaQBtAGUAIABnAHIAbwB1AHAAIABmAG8AcgBtAGEAdAB0AGUAZAAgAGkAbgAgAFUAUwAgAE0AaQBsAGkAdABhAHIAeQAgAG0AZQBzAHMAYQBnAGUAIAB0AHIAYQBmAGYAaQBjACAAcwB0AHkAbABlAC4AIAAgACAAIAAgACAAIAAjAFwAbgAjACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAAQwBvAG4AdgBlAHIAcwBpAG8AbgBzACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AIAAjAFwAbgAjACAASQBTAE8ARABBAFQARQBfAFQATwBfAEoARABOAF8ATABPAEMAQQBMACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAEoAdQBsAGkAYQBuACAARABhAHkAIABOAHUAbQBiAGUAcgAgAGEAbgBkACAAbABvAGMAYQBsACAAdABpAG0AZQAgAGYAbwByACAAYQAgAGQAYQB0AGUAIABhAG4AZAAgAHQAaQBtAGUAIABwAHIAbwB2AGkAZABlAGQAIABpAG4AIAAgACAAIAAjAFwAbgAjACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkAUwBPACAAZgBvAHIAbQBhAHQALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAASQBTAE8ARABBAFQARQBfAFQATwBfAEoARABBAFQARQAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAEoAdQBsAGkAYQBuACAARABhAHQAZQAgAGYAbwByACAAYQAgAGQAYQB0AGUAIABhAG4AZAAgAHQAaQBtAGUAIABwAHIAbwB2AGkAZABlAGQAIABpAG4AIABJAFMATwAgAGYAbwByAG0AYQB0AC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAASQBTAE8ARABBAFQARQBfAFQATwBfAEUARABBAFQARQAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIABhAG4AIABFAHgAYwBlAGwAIABEAGEAdABlAC8AVABpAG0AZQAgAGYAbwByACAAYQAgAGQAYQB0AGUAIABhAG4AZAAgAHQAaQBtAGUAIABwAHIAbwB2AGkAZABlAGQAIABpAG4AIABJAFMATwAgAGYAbwByAG0AYQB0AC4AIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAASgBEAEEAVABFAF8AVABPAF8ASQBTAE8ARABBAFQARQAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIABJAFMATwAgAGYAbwByAG0AYQB0ACAAZABhAHQAZQAsACAAdABpAG0AZQAgAGEAbgBkACAAdABpAG0AZQAgAHoAbwBuAGUAIABvAGYAZgBzAGUAdAAgAGYAcgBvAG0AIABhACAAIABKAHUAbABpAGEAbgAgAEQAYQB0AGUALgAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAASgBEAE4AXwBMAE8AQwBBAEwAXwBUAE8AXwBJAFMATwBEAEEAVABFACAAIAAgAFIAZQB0AHUAcgBuAHMAIABJAFMATwAgAGYAbwByAG0AYQB0ACAAZABhAHQAZQAsACAAdABpAG0AZQAgAGEAbgBkACAAdABpAG0AZQAgAHoAbwBuAGUAIABvAGYAZgBzAGUAdAAgAGYAbwByACAAdABoAGUAIABwAHIAbwB2AGkAZABlAGQAIABKAHUAbABpAGEAbgAgAEQAYQB5ACAAIAAjAFwAbgAjACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAE4AdQBtAGIAZQByACAAYQBuAGQAIABsAG8AYwBhAGwAIAB0AGkAbQBlAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARQBEAEEAVABFAF8AVABPAF8ASQBTAE8ARABBAFQARQAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIABJAFMATwAgAGYAbwByAG0AYQB0ACAAZABhAHQAZQAsACAAdABpAG0AZQAgAGEAbgBkACAAdABpAG0AZQAgAHoAbwBuAGUAIABvAGYAZgBzAGUAdAAgAGYAcgBvAG0AIABhAG4AIABFAHgAYwBlAGwAIABEAGEAdABlAC8AVABpAG0AZQAuACAAIAAgACAAIAAjAFwAbgAjACAARQBEAEEAVABFAF8AVABPAF8ASgBEAEEAVABFACAAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAEoAdQBsAGkAYQBuACAARABhAHQAZQAgAGYAbwByACAAdABoAGUAIABwAHIAbwB2AGkAZABlAGQAIABFAHgAYwBlAGwAIABEAGEAdABlAC8AVABpAG0AZQAuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARQBEAEEAVABFAF8AVABPAF8ASgBEAE4AXwBMAE8AQwBBAEwAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAEoAdQBsAGkAYQBuACAARABhAHkAIABOAHUAbQBiAGUAcgAgAGEAbgBkACAAbABvAGMAYQBsACAAdABpAG0AZQAgAGYAbwByACAAdABoAGUAIABwAHIAbwB2AGkAZABlAGQAIABFAHgAYwBlAGwAIABEAGEAdABlAC8AVABpAG0AZQAuACAAIAAjAFwAbgAjACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAASgBEAE4AXwBMAE8AQwBBAEwAXwBUAE8AXwBFAEQAQQBUAEUAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIABhAG4AIABFAHgAYwBlAGwAIABEAGEAdABlAC8AVABpAG0AZQAgAGYAbwByACAAdABoAGUAIABwAHIAbwB2AGkAZABlAGQAIABKAHUAbABpAGEAbgAgAEQAYQB5ACAATgB1AG0AYgBlAHIAIABhAG4AZAAgAGwAbwBjAGEAbAAgAHQAaQBtAGUALgAgACAAIAAjAFwAbgAjACAASgBEAEEAVABFAF8AVABPAF8ARQBEAEEAVABFACAAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIABhAG4AIABFAHgAYwBlAGwAIABEAGEAdABlAC8AVABpAG0AZQAgAGYAbwByACAAdABoAGUAIABwAHIAbwB2AGkAZABlAGQAIABKAHUAbABpAGEAbgAgAEQAYQB0AGUALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAAVQBTAEQAQQBUAEUAXwBUAE8AXwBFAEQAQQBUAEUAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIABhAG4AIABFAHgAYwBlAGwAIABEAGEAdABlAC8AVABpAG0AZQAgAGYAbwByACAAdABoAGUAIABwAHIAbwB2AGkAZABlAGQAIABVAFMAIABmAG8AcgBtAGEAdAAgAGQAYQB0AGUAIABhAG4AZAAgAHQAaQBtAGUALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARQBEAEEAVABFAF8AVABPAF8AVQBTAEQAQQBUAEUAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIABhACAAVQBTACAAZgBvAHIAbQBhAHQAIABkAGEAdABlACAAYQBuAGQAIAB0AGkAbQBlACAAZgBvAHIAIAB0AGgAZQAgAHAAcgBvAHYAaQBkAGUAZAAgAEUAeABjAGUAbAAgAEQAYQB0AGUALwBUAGkAbQBlAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAKgAvAFwAbgBcAG4AXABuAFwAbgAvACoAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjAFwAbgAjACAATABPAEcASQBDAEEATAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAKgAvAFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEkAUwBfAEwARQBBAFAAXwBZAEUAQQBSAFwAbgBcAG4AVABlAHMAdABzACAAaQBmACAAYQAgAHkAZQBhAHIAIABpAG4AYwBsAHUAZABlAHMAIABhACAAbABlAGEAcAAgAGQAYQB5ACAAaQBuACAAdABoAGUAIABnAGkAdgBlAG4AIABjAGEAbABlAG4AZABhAHIALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAYgBvAG8AbABlAGEAbgAgAHwAIABuAHUAbABsACAAaQBmACAAZQBtAHAAdAB5AFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AWQBlAGEAcgBDAEUAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgAFkAZQBhAHIAIABpAG4AIABDAG8AbQBtAG8AbgAgAEUAcgBhAC4AIABOAG8AdABlACAAdABoAGEAdAAgADEAIABCAEMAIAA9ACAAMAAgAEMARQAsACAAMgAgAEIAQwAgAD0AIAAtADEAIABDAEUAXABuAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0AIAB8ACAAcwB3AGkAdABjAGgAIAAgAHwAIABDAGEAbABjAHUAbABhAHQAZQAgAGYAbwByACAAdABoAGUAIABKAHUAbABpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AIABEAGUAZgBhAHUAbAB0ACAAaQBzACAARwByAGUAZwBvAHIAaQBhAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBJAFMAXwBMAEUAQQBQAF8AWQBFAEEAUgAgAD0AIABMAEEATQBCAEQAQQAoAFkAZQBhAHIAQwBFACwAIABbAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACwAXABuACAAIAAgACAASQBGACgAWQBlAGEAcgBDAEUAIAA9ACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABZAGUAYQByAEMARQApACkALAAgAHsAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AGUAYQByAEMARQAsACAASQBOAFQAKABZAGUAYQByAEMARQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABOACgASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByACkAIAA9ACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGAFMAKABNAE8ARAAoAF8AeQBlAGEAcgBDAEUALAAgADQAMAAwACkAIAA9ACAAMAAsACAAVABSAFUARQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABNAE8ARAAoAF8AeQBlAGEAcgBDAEUALAAgADEAMAAwACkAIAA9ACAAMAAsACAARgBBAEwAUwBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALAAgAE0ATwBEACgAXwB5AGUAYQByAEMARQAsACAANAApACAAPQAgADAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABNAE8ARAAoAF8AeQBlAGEAcgBDAEUALAAgADQAKQAgAD0AIAAwAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEkAUwBfAFYAQQBMAEkARABfAEQAQQBUAEUAXABuAFwAbgBUAGUAcwB0AHMAIABpAGYAIABhACAAZABhAHQAZQAgAGkAcwAgAHYAYQBsAGkAZAAgAGYAbwByACAAdABoAGUAIABnAGkAdgBlAG4AIABjAGEAbABlAG4AZABhAHIALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAYgBvAG8AbABlAGEAbgAgAHwAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBZAGUAYQByAEMARQAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAAgACAAIAAgACAAIAAgACAAfAAgAFkAZQBhAHIAIABpAG4AIABDAG8AbQBtAG8AbgAgAEUAcgBhAC4AIABOAG8AdABlACAAdABoAGEAdAAgADEAIABCAEMAIAA9ACAAMAAgAEMARQAsACAAMgAgAEIAQwAgAD0AIAAtADEAIABDAEUAXABuAE0AbwBuAHQAaAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMQAuAC4AMQAyAF0AIAB8ACAATQBvAG4AdABoACAAbwBmACAAeQBlAGEAcgBcAG4ARABhAHkAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAWwAxAC4ALgAzADIAKQAgAHwAIABEAGEAeQAgAG8AZgAgAG0AbwBuAHQAaABcAG4AWwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAgAHwAIABzAHcAaQB0AGMAaAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABDAGEAbABjAHUAbABhAHQAZQAgAGYAbwByACAAdABoAGUAIABKAHUAbABpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AIABEAGUAZgBhAHUAbAB0ACAAaQBzACAARwByAGUAZwBvAHIAaQBhAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ASQBTAF8AVgBBAEwASQBEAF8ARABBAFQARQAgAD0AIABMAEEATQBCAEQAQQAoAFkAZQBhAHIAQwBFACwAIABNAG8AbgB0AGgALAAgAEQAYQB5ACwAIABbAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACwAXABuACAAIAAgACAASQBGACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABZAGUAYQByAEMARQApACkAIAArACAATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABNAG8AbgB0AGgAKQApACAAKwAgAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgARABhAHkAKQApACwAXABuACAAIAAgACAAIAAgACAAIABGAEEATABTAEUALAAgAC8ALwAgAGMAYQBuAG4AbwB0ACAAbwBtAG0AaQB0ACAAeQBlAGEAcgAsACAAbQBvAG4AdABoACAAbwByACAAZABhAHkAXABuACAAIAAgACAAIAAgACAAIABJAEYAKAAoAE0ATwBEACgAWQBlAGEAcgBDAEUALAAgADEAKQAgAD4AIAAwACkAIAArACAAKABNAE8ARAAoAE0AbwBuAHQAaAAsACAAMQApACAAPgAgADAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABGAEEATABTAEUALAAgAC8ALwAgAHkAZQBhAHIAIABhAG4AZAAgAG0AbwBuAHQAaAAgAGMAYQBuAG4AbwB0ACAAYgBlACAAZgByAGEAYwB0AGkAbwBuAGEAbABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAYQB5ACwAIABJAE4AVAAoAEQAYQB5ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAGQAYQB5ACAAPAAgADEALAAgAEYAQQBMAFMARQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQBzAEkAbgBNAG8AbgB0AGgALAAgAEQAQQBZAFMAXwBJAE4AXwBNAE8ATgBUAEgAKABNAG8AbgB0AGgALAAgAFkAZQBhAHIAQwBFACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABJAFMARQBSAFIATwBSACgAXwBkAGEAeQBzAEkAbgBNAG8AbgB0AGgAKQAsACAARgBBAEwAUwBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQAgADwAPQAgAF8AZABhAHkAcwBJAG4ATQBvAG4AdABoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ASQBTAF8AVgBBAEwASQBEAF8AVABJAE0ARQBcAG4AXABuAFQAZQBzAHQAcwAgAGkAZgAgAGEAIAB0AGkAbQBlACAAaQBzACAAdgBhAGwAaQBkACAAaQBuACAAdABoAGUAIAAyADQAIABoAG8AdQByACAAdABpAG0AZQBrAGUAZQBwAGkAbgBnACAAcwB5AHMAdABlAG0ALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAYgBvAG8AbABlAGEAbgAgAHwAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBIAG8AdQByACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAWwAwAC4ALgAyADQAKQAgAHwAIABGAHIAYQBjAHQAaQBvAG4AYQBsACAAYQBsAGwAbwB3AGUAZAAgAGkAZgAgAG0AaQBuAHUAdABlACAAYQBuAGQAIABzAGUAYwBvAG4AZAAgAGUAbQBwAHQAeQAuAFwAbgBNAGkAbgB1AHQAZQAgAHwAIABkAGUAYwBpAG0AYQBsACAAWwAwAC4ALgA2ADAAKQAgAHwAIABGAHIAYQBjAHQAaQBvAG4AYQBsACAAYQBsAGwAbwB3AGUAZAAgAGkAZgAgAHMAZQBjAG8AbgBkACAAZQBtAHAAdAB5AC4AXABuAFMAZQBjAG8AbgBkACAAfAAgAGQAZQBjAGkAbQBhAGwAIABbADAALgAuADYAMAApACAAfAAgAEYAcgBhAGMAdABpAG8AbgBhAGwAIABhAGwAbABvAHcAZQBkAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBcAG4ASQBTAF8AVgBBAEwASQBEAF8AVABJAE0ARQAgAD0AIABMAEEATQBCAEQAQQAoAEgAbwB1AHIALAAgAE0AaQBuAHUAdABlACwAIABTAGUAYwBvAG4AZAAsAFwAbgAgACAAIAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIABJAFMATgBVAE0AQgBFAFIAKABIAG8AdQByACkAIAAqACAASQBTAE4AVQBNAEIARQBSACgATQBpAG4AdQB0AGUAKQAgACoAIABJAFMATgBVAE0AQgBFAFIAKABTAGUAYwBvAG4AZAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKABNAE8ARAAoAEgAbwB1AHIALAAgADEAKQAgAD4AIAAwACkAIAArACAAKABNAE8ARAAoAE0AaQBuAHUAdABlACwAIAAxACkAIAA+ACAAMAApACwAIABGAEEATABTAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoAEgAbwB1AHIAIAA8ACAAMAApACAAKwAgACgASABvAHUAcgAgAD4AIAAyADMAKQAsACAARgBBAEwAUwBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKABNAGkAbgB1AHQAZQAgADwAIAAwACkAIAArACAAKABNAGkAbgB1AHQAZQAgAD4AIAA1ADkAKQAsACAARgBBAEwAUwBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKABTAGUAYwBvAG4AZAAgADwAIAAwACkAIAArACAAKABTAGUAYwBvAG4AZAAgAD4APQAgADYAMAApACwAIABGAEEATABTAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAIABUAFIAVQBFAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIABJAFMATgBVAE0AQgBFAFIAKABIAG8AdQByACkAIAAqACAASQBTAE4AVQBNAEIARQBSACgATQBpAG4AdQB0AGUAKQAgACoAIAAoAFMAZQBjAG8AbgBkACAAPQAgAFwAIgBcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAUwAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAE0ATwBEACgASABvAHUAcgAsACAAMQApACAAPgAgADAALAAgAEYAQQBMAFMARQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgASABvAHUAcgAgADwAIAAwACkAIAArACAAKABIAG8AdQByACAAPgAgADIAMwApACwAIABGAEEATABTAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoAE0AaQBuAHUAdABlACAAPAAgADAAKQAgACsAIAAoAE0AaQBuAHUAdABlACAAPgA9ACAANgAwACkALAAgAEYAQQBMAFMARQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALAAgAFQAUgBVAEUAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgAEkAUwBOAFUATQBCAEUAUgAoAEgAbwB1AHIAKQAgACoAIAAoAE0AaQBuAHUAdABlACAAPQAgAFwAIgBcACIAKQAgACoAIAAoAFMAZQBjAG8AbgBkACAAPQAgAFwAIgBcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoACgASABvAHUAcgAgAD4APQAgADAAKQAgACoAIAAoAEgAbwB1AHIAIAA8ACAAMgA0ACkAKQAgADwAPgAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACgASABvAHUAcgAgAD0AIABcACIAXAAiACkAIAAqACAASQBTAE4AVQBNAEIARQBSACgATQBpAG4AdQB0AGUAKQAgACoAIABJAFMATgBVAE0AQgBFAFIAKABTAGUAYwBvAG4AZAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATQBPAEQAKABNAGkAbgB1AHQAZQAsACAAMQApACAAPgAgADAALAAgAEYAQQBMAFMARQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgATQBpAG4AdQB0AGUAIAA8ACAAMAApACAAKwAgACgATQBpAG4AdQB0AGUAIAA+ACAANQA5ACkALAAgAEYAQQBMAFMARQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgAUwBlAGMAbwBuAGQAIAA8ACAAMAApACAAKwAgACgAUwBlAGMAbwBuAGQAIAA+AD0AIAA2ADAAKQAsACAARgBBAEwAUwBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABSAFUARQAsACAAVABSAFUARQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAKABIAG8AdQByACAAPQAgAFwAIgBcACIAKQAgACoAIABJAFMATgBVAE0AQgBFAFIAKABNAGkAbgB1AHQAZQApACAAKgAgACgAUwBlAGMAbwBuAGQAIAA9ACAAXAAiAFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgAKABNAGkAbgB1AHQAZQAgAD4APQAgADAAKQAgACoAIAAoAE0AaQBuAHUAdABlACAAPAAgADYAMAApACkAIAA8AD4AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAoAEgAbwB1AHIAIAA9ACAAXAAiAFwAIgApACAAKgAgACgATQBpAG4AdQB0AGUAIAA9ACAAXAAiAFwAIgApACAAKgAgAEkAUwBOAFUATQBCAEUAUgAoAFMAZQBjAG8AbgBkACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKAAoAFMAZQBjAG8AbgBkACAAPgA9ACAAMAApACAAKgAgACgAUwBlAGMAbwBuAGQAIAA8ACAANgAwACkAKQAgADwAPgAgADAALABcAG4AIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALAAgAEYAQQBMAFMARQBcAG4AIAAgACAAIAApAFwAbgApADsAIAAgACAAIAAgACAAIAAgAFwAbgBcAG4AXABuAFwAbgAvACoAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjAFwAbgAjACAAQwBBAEwARQBOAEQAQQBSACAARABBAFQARQBTACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAKgAvAFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFkARQBBAFIAXwBDAE8ATQBNAE8ATgBfAEUAUgBBAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAHkAZQBhAHIAIAB2AGEAbAB1AGUAIAByAGUAbABhAHQAaQB2AGUAIAB0AG8AIAB0AGgAZQAgAEMAbwBtAG0AbwBuACAARQByAGEALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIAAxACAAQwBFACAAPQAgADEALAAgADEAIABCAEMARQAgAD0AIAAwACwAIAAyACAAQgBDAEUAIAA9ACAALQAxAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AWQBlAGEAcgAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADEALgAuAF0AIAB8ACAAUABvAHMAaQB0AGkAdgBlACAAbgBvAG4ALQB6AGUAcgBvACAAaQBuAHQAZQBnAGUAcgAuAFwAbgBCAEMARQAgACAAIAB8ACAAcwB3AGkAdABjAGgAIAAgACAAIAAgACAAIAAgAHwAIABCAGUAZgBvAHIAZQAgAEMAbwBtAG0AbwBuACAARQByAGEALgBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4AWQBFAEEAUgBfAEMATwBNAE0ATwBOAF8ARQBSAEEAIAA9ACAATABBAE0AQgBEAEEAKABZAGUAYQByACwAIABCAEMARQAsAFwAbgAgACAAIAAgAEkARgAoAFkAZQBhAHIAIAA9ACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABZAGUAYQByACkAKQAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIALAAgAEkATgBUACgAWQBlAGEAcgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwB5AGUAYQByACAAPAAgADEALAAgAHsAIwBOAFUATQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAE4AKABCAEMARQApACwAIAAxACAALQAgAF8AeQBlAGEAcgAsACAAXwB5AGUAYQByACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEQAQQBZAFMAXwBJAE4AXwBZAEUAQQBSAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAG4AdQBtAGIAZQByACAAbwBmACAAZABhAHkAcwAgAGkAbgAgAHQAaABlACAAZwBpAHYAZQBuACAAeQBlAGEAcgAgAG8AZgAgAHQAaABlACAAcwBwAGUAYwBpAGYAaQBlAGQAIABjAGEAbABlAG4AZABhAHIALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMwA2ADUALAAzADYANgBdAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AWQBlAGEAcgBDAEUAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAFkAZQBhAHIAIABpAG4AIABDAG8AbQBtAG8AbgAgAEUAcgBhAC4AIABOAG8AdABlACAAdABoAGEAdAAgADEAIABCAEMAIAA9ACAAMAAgAEMARQAsACAAMgAgAEIAQwAgAD0AIAAtADEAIABDAEUAXABuAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0AIAB8ACAAcwB3AGkAdABjAGgAIAAgAHwAIABDAGEAbABjAHUAbABhAHQAZQAgAGYAbwByACAAdABoAGUAIABKAHUAbABpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AIABEAGUAZgBhAHUAbAB0ACAAaQBzACAARwByAGUAZwBvAHIAaQBhAG4AIABwAHIAbwBsAGUAcAB0AGkAYwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgAGMAYQBsAGUAbgBkAGEAcgAuAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBEAEEAWQBTAF8ASQBOAF8AWQBFAEEAUgAgAD0AIABMAEEATQBCAEQAQQAoAFkAZQBhAHIAQwBFACwAIABbAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACwAXABuACAAIAAgACAASQBGACgAWQBlAGEAcgBDAEUAIAA9ACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABZAGUAYQByAEMARQApACkALAAgAHsAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAEkAUwBfAEwARQBBAFAAXwBZAEUAQQBSACgAWQBlAGEAcgBDAEUALAAgAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAMwA2ADYALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAzADYANQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEQAQQBZAFMAXwBJAE4AXwBNAE8ATgBUAEgAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAbgB1AG0AYgBlAHIAIABvAGYAIABkAGEAeQBzACAAaQBuACAAdABoAGUAIABnAGkAdgBlAG4AIABtAG8AbgB0AGgAIABhAG4AZAAgAHkAZQBhAHIAIABvAGYAIAB0AGgAZQAgAHMAcABlAGMAaQBmAGkAZQBkACAAYwBhAGwAZQBuAGQAYQByAC4AXABuAFwAbgBPAHUAdABwAHUAdABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADEALgAuADMAMQBdAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ATQBvAG4AdABoACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAWwAxAC4ALgAxADIAXQAgAHwAIABNAG8AbgB0AGgAIABvAGYAIAB5AGUAYQByAFwAbgBbAFkAZQBhAHIAQwBFAF0AIAAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAAgACAAIAAgACAAIAAgACAAfAAgAFkAZQBhAHIAIABpAG4AIABDAG8AbQBtAG8AbgAgAEUAcgBhAC4AIABOAG8AdABlACAAdABoAGEAdAAgADEAIABCAEMAIAA9ACAAMAAgAEMARQAsACAAMgAgAEIAQwAgAD0AIAAtADEAIABDAEUAXABuAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0AIAB8ACAAcwB3AGkAdABjAGgAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAQwBhAGwAYwB1AGwAYQB0AGUAIABmAG8AcgAgAHQAaABlACAASgB1AGwAaQBhAG4AIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuACAARABlAGYAYQB1AGwAdAAgAGkAcwAgAEcAcgBlAGcAbwByAGkAYQBuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEQAQQBZAFMAXwBJAE4AXwBNAE8ATgBUAEgAIAA9ACAATABBAE0AQgBEAEEAKABNAG8AbgB0AGgALAAgAFsAWQBlAGEAcgBDAEUAXQAsACAAWwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAsAFwAbgAgACAAIAAgAEkARgAoAE0AbwBuAHQAaAA9AFwAIgBcACIALAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgATQBvAG4AdABoACkAKQAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AbwBuAHQAaAAsACAASQBOAFQAKABNAG8AbgB0AGgAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AbwBuAHQAaAAgADwAIAAxACwAIAB7ACMATgBVAE0AIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AbwBuAHQAaAAgAD4AIAAxADIALAAgAHsAIwBOAFUATQAhAH0ALABcAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABGAGUAYgByAHUAYQByAHkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AbwBuAHQAaAAgAD0AIAAyACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBsAGUAYQBwAEQAYQB5ACwAIABJAEYAKABJAFMATgBVAE0AQgBFAFIAKABZAGUAYQByAEMARQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABOACgASQBTAF8ATABFAEEAUABfAFkARQBBAFIAKABZAGUAYQByAEMARQAsACAASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAMABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAMgA4ACAAKwAgAF8AbABlAGEAcABEAGEAeQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAEoAYQBuACwAIABNAGEAcgAsACAAQQBwAHIALAAgAE0AYQB5ACwAIABKAHUAbgAsACAASgB1AGwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AbwBuAHQAaAAgADwAPQAgADcALAAgADMAMAAgACsAIABNAE8ARAAoAF8AbQBvAG4AdABoACwAIAAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAQQB1AGcALAAgAFMAZQBwACwAIABPAGMAdAAsACAATgBvAHYALAAgAEQAZQBjAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABSAFUARQAsACAAMwAxACAALQAgAE0ATwBEACgAXwBtAG8AbgB0AGgALAAgADIAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEoAVQBMAEkAQQBOAF8ARABBAFkAXwBOAFUATQBCAEUAUgBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAEoAdQBsAGkAYQBuACAARABhAHkAIABOAHUAbQBiAGUAcgAgAG8AZgAgAHQAaABlACAAcAByAG8AdgBpAGQAZQBkACAAZABhAHQAZQAgAGkAbgAgAHQAaABlACAAcwBwAGUAYwBpAGYAaQBlAGQAIABjAGEAbABlAG4AZABhAHIALgBcAG4ATgBvAHQAZQAgAHQAaABlACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByACAAaQBzACAAYQBuACAAaQBuAHQAZQBnAGUAcgAgAHQAeQBwAGUAIABhAG4AZAAgAGkAcwAgAGEAbgAgAG8AcgBkAGkAbgBhAGwAIABkAGEAeQAgAG4AdQBtAGIAZQByACAAcgBlAGYAZQByAGUAbgBjAGUAZAAgAGYAcgBvAG0AIABKAGEAbgB1AGEAcgB5ACAAMQAsAFwAbgA0ADcAMQAzACAAQgBDACAAaQBuACAAdABoAGUAIABwAHIAbwBsAGUAcAB0AGkAYwAgAEoAdQBsAGkAYQBuACAAYwBhAGwAZQBuAGQAYQByAC4AIABJAHQAIABkAG8AZQBzACAAbgBvAHQAIABpAG4AYwBsAHUAZABlACAAYQBuAHkAIAB2AGEAbAB1AGUAIABmAG8AcgAgAHQAaQBtAGUAIABvAGYAIABkAGEAeQAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAEoAdQBsAGkAYQBuACAARABhAHkAIABOAHUAbQBiAGUAcgBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFkAZQBhAHIAQwBFACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgACAAIAAgACAAIAAgACAAIAB8ACAAWQBlAGEAcgAgAGkAbgAgAEMAbwBtAG0AbwBuACAARQByAGEALgAgAE4AbwB0AGUAIAB0AGgAYQB0ACAAMQAgAEIAQwAgAD0AIAAwACAAQwBFACwAIAAyACAAQgBDACAAPQAgAC0AMQAgAEMARQBcAG4ATQBvAG4AdABoACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAWwAxAC4ALgAxADIAXQAgAHwAIABNAG8AbgB0AGgAIABvAGYAIAB5AGUAYQByAFwAbgBEAGEAeQAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIABbADEALgAuADMAMgApACAAfAAgAEQAYQB5ACAAbwBmACAAbQBvAG4AdABoAFwAbgBbAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACAAfAAgAHMAdwBpAHQAYwBoACAAIAAgACAAIAAgACAAIAAgACAAfAAgAEMAYQBsAGMAdQBsAGEAdABlACAAZgBvAHIAIAB0AGgAZQAgAEoAdQBsAGkAYQBuACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgAgAEQAZQBmAGEAdQBsAHQAIABpAHMAIABHAHIAZQBnAG8AcgBpAGEAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABwAHIAbwBsAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ASgBVAEwASQBBAE4AXwBEAEEAWQBfAE4AVQBNAEIARQBSACAAPQAgAEwAQQBNAEIARABBACgAWQBlAGEAcgBDAEUALAAgAE0AbwBuAHQAaAAsACAARABhAHkALAAgAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0ALABcAG4AIAAgACAAIABJAEYAKAAoAFkAZQBhAHIAQwBFACAAPQAgAFwAIgBcACIAKQAgACoAIAAoAE0AbwBuAHQAaAAgAD0AIABcACIAXAAiACkAIAAqACAAKABEAGEAeQAgAD0AIABcACIAXAAiACkALAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAF8AVgBBAEwASQBEAF8ARABBAFQARQAoAFkAZQBhAHIAQwBFACwAIABNAG8AbgB0AGgALAAgAEQAYQB5ACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQApACwAIAB7ACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkALAAgAEkATgBUACgARABhAHkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZwByAGUAZwBvAHIAaQBhAG4ALAAgAE4AKABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAgAD0AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBZAEUAQQBSADQAOAAwADEAQgBDAEUALAAgAC0ANAA4ADAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8ARwA0ADgAMAAxAEIAQwBFAF8ASgBEACwAIAAtADMAMgAwADQANQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8ASgA0ADgAMAAxAEIAQwBFAF8ASgBEACwAIAAtADMAMgAwADgAMwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8ARABhAHkAcwBJAG4ANQBNAG8AbgB0AGgAcwBGAHIAbwBtAE0AYQByAGMAaAAsACAAMQA1ADMALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGEALAAgAEkATgBUACgAKAAxADQAIAAtACAATQBvAG4AdABoACkAIAAvACAAMQAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkALAAgACgAWQBlAGEAcgBDAEUAIAAtACAAXwBZAEUAQQBSADQAOAAwADEAQgBDAEUAIAAtACAAXwBhACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0ALAAgACgATQBvAG4AdABoACAAKwAgADEAMgAgACoAIABfAGEAIAAtACAAMwApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB4ACwAIAAzADYANQAgACoAIABfAHkAIAArACAASQBOAFQAKABfAHkAIAAvACAANAApACAAKwAgAEkATgBUACgAKABfAEQAYQB5AHMASQBuADUATQBvAG4AdABoAHMARgByAG8AbQBNAGEAcgBjAGgAIAAqACAAXwBtACAAKwAgADIAKQAgAC8AIAA1ACkAIAArACAAXwBkAGEAeQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBnAHIAZQBnAG8AcgBpAGEAbgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB4ACAAKwAgAF8ARwA0ADgAMAAxAEIAQwBFAF8ASgBEACAALQAgAEkATgBUACgAXwB5ACAALwAgADEAMAAwACkAIAArACAASQBOAFQAKABfAHkAIAAvACAANAAwADAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB4ACAAKwAgAF8ASgA0ADgAMAAxAEIAQwBFAF8ASgBEAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBKAEQATgBfAFQATwBfAEMAQQBMAEUATgBEAEEAUgBfAEQAQQBUAEUAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIABkAGEAdABlACAAZgByAG8AbQAgAHQAaABlACAAZwBpAHYAZQBuACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByACAAaQBuACAAdABoAGUAIABzAHAAZQBjAGkAZgBpAGUAZAAgAGMAYQBsAGUAbgBkAGEAcgAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABpAG4AdABlAGcAZQByACAAIAAgACAAIAAgACAAIAAgAHwAIABZAGUAYQByACAAaQBuACAAQwBvAG0AbQBvAG4AIABFAHIAYQAuACAATgBvAHQAZQAgAHQAaABhAHQAIAAxACAAQgBDACAAPQAgADAAIABDAEUALAAgADIAIABCAEMAIAA9ACAALQAxACAAQwBFAFwAbgAgADIAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMQAuAC4AMQAyAF0AIAB8ACAATQBvAG4AdABoAFwAbgAgADMAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMQAuAC4AMwAxAF0AIAB8ACAARABhAHkAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBKAEQATgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByACAAZgBvAHIAIAB0AGgAZQAgAGMAYQBsAGUAbgBkAGEAcgAgAGQAYQB5AFwAbgBbAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACAAfAAgAHMAdwBpAHQAYwBoACAAIAB8ACAAQwBhAGwAYwB1AGwAYQB0AGUAIABmAG8AcgAgAHQAaABlACAASgB1AGwAaQBhAG4AIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuACAARABlAGYAYQB1AGwAdAAgAGkAcwAgAEcAcgBlAGcAbwByAGkAYQBuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ASgBEAE4AXwBUAE8AXwBDAEEATABFAE4ARABBAFIAXwBEAEEAVABFACAAPQAgAEwAQQBNAEIARABBACgASgBEAE4ALAAgAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0ALABcAG4AIAAgACAAIABJAEYAKABKAEQATgAgAD0AIABcACIAXAAiACwAIAB7AFwAIgBcACIALAAgAFwAIgBcACIALAAgAFwAIgBcACIAfQAsAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABKAEQATgApACkALAAgAHsAIwBWAEEATABVAEUAIQAsACAAIwBWAEEATABVAEUAIQAsACAAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBqAGQAbgAsACAASQBOAFQAKABKAEQATgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBnAHIAZQBnAG8AcgBpAGEAbgAsACAATgAoAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgApACAAPQAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAFkARQBBAFIANAA4ADAAMQBCAEMARQAsACAALQA0ADgAMAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBEAGEAeQBzAEkAbgA0AFkAZQBhAHIALAAgADEANAA2ADEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAEQAYQB5AHMASQBuAFkAZQBhAHIALAAgADMANgA1ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBNAG8AbgB0AGgAQwBvAHIAcgBlAGMAdABpAG8AbgBEAGEAeQBzACwAIAAzADAAOAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8ARABhAHkAcwBJAG4ANABNAG8AbgB0AGgAcwAsACAAMQAyADIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAEQAYQB5AHMASQBuADUATQBvAG4AdABoAHMARgByAG8AbQBNAGEAcgBjAGgALAAgADEANQAzACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBnAHIAZQBnAG8AcgBpAGEAbgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBHADQAOAAwADEAQgBDAEUAXwBKAEQAMAAsACAALQAzADIAMAA0ADUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBHAHIAZQBnAEQAYQB5AHMASQBuADQAMAAwAFkAZQBhAHIALAAgADEANAA2ADAAOQA3ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8ARwByAGUAZwBEAGEAeQBzAEkAbgAxADAAMABZAGUAYQByACwAIAAzADYANQAyADQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQBzADAALAAgAF8AagBkAG4AIAAtACAAXwBHADQAOAAwADEAQgBDAEUAXwBKAEQAMAAgAC0AIAAxACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcQB1AGEAZABDAGUAbgB0ACwAIABJAE4AVAAoAF8AZABhAHkAcwAwACAALwAgAF8ARwByAGUAZwBEAGEAeQBzAEkAbgA0ADAAMABZAGUAYQByACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQBzADEALAAgAF8AZABhAHkAcwAwACAALQAgAF8AcQB1AGEAZABDAGUAbgB0ACAAKgAgAF8ARwByAGUAZwBEAGEAeQBzAEkAbgA0ADAAMABZAGUAYQByACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcgBlAG0AQwBlAG4AdAAsACAASQBOAFQAKAAoAEkATgBUACgAXwBkAGEAeQBzADEAIAAvACAAXwBHAHIAZQBnAEQAYQB5AHMASQBuADEAMAAwAFkAZQBhAHIAKQAgACsAIAAxACkAIAAqACAAMAAuADcANQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkAcwAyACwAIABfAGQAYQB5AHMAMQAgAC0AIABfAHIAZQBtAEMAZQBuAHQAIAAqACAAXwBHAHIAZQBnAEQAYQB5AHMASQBuADEAMAAwAFkAZQBhAHIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBxAHUAYQBkAFkAcgAsACAASQBOAFQAKABfAGQAYQB5AHMAMgAgAC8AIABfAEQAYQB5AHMASQBuADQAWQBlAGEAcgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkAcwAzACwAIABfAGQAYQB5AHMAMgAgAC0AIABfAHEAdQBhAGQAWQByACAAKgAgAF8ARABhAHkAcwBJAG4ANABZAGUAYQByACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcgBlAG0AWQByACwAIABJAE4AVAAoACgASQBOAFQAKABfAGQAYQB5AHMAMwAgAC8AIABfAEQAYQB5AHMASQBuAFkAZQBhAHIAKQAgACsAIAAxACkAIAAqACAAMAAuADcANQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkAcwA0ACwAIABfAGQAYQB5AHMAMwAgAC0AIABfAHIAZQBtAFkAcgAgACoAIABfAEQAYQB5AHMASQBuAFkAZQBhAHIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5ACwAIABfAHEAdQBhAGQAQwBlAG4AdAAgACoAIAA0ADAAMAAgACsAIABfAHIAZQBtAEMAZQBuAHQAIAAqACAAMQAwADAAIAArACAAXwBxAHUAYQBkAFkAcgAgACoAIAA0ACAAKwAgAF8AcgBlAG0AWQByACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbQAsACAASQBOAFQAKAAoAF8AZABhAHkAcwA0ACAAKgAgADUAIAArACAAXwBNAG8AbgB0AGgAQwBvAHIAcgBlAGMAdABpAG8AbgBEAGEAeQBzACkAIAAvACAAXwBEAGEAeQBzAEkAbgA1AE0AbwBuAHQAaABzAEYAcgBvAG0ATQBhAHIAYwBoACkAIAAtACAAMgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAYQB5ACwAIABfAGQAYQB5AHMANAAgAC0AIABJAE4AVAAoACgAXwBtACAAKwAgADQAKQAgACoAIABfAEQAYQB5AHMASQBuADUATQBvAG4AdABoAHMARgByAG8AbQBNAGEAcgBjAGgAIAAvACAANQApACAAKwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAEQAYQB5AHMASQBuADQATQBvAG4AdABoAHMAIAArACAAMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIALAAgAF8AWQBFAEEAUgA0ADgAMAAxAEIAQwBFACAAKwAgAF8AeQAgACsAIABJAE4AVAAoACgAXwBtACAAKwAgADIAKQAgAC8AIAAxADIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AbwBuAHQAaAAsACAATQBPAEQAKABfAG0AIAArACAAMgAsACAAMQAyACkAIAArACAAMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAF8AeQBlAGEAcgAsACAAXwBtAG8AbgB0AGgALAAgAF8AZABhAHkAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8ASgA0ADgAMAAxAEIAQwBFAF8ASgBEADAALAAgAC0AMwAyADAAOAAzACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkAcwAwACwAIABfAGoAZABuACAALQAgAF8ASgA0ADgAMAAxAEIAQwBFAF8ASgBEADAAIAAtACAAMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHEAdQBhAGQAWQByACwAIABJAE4AVAAoAF8AZABhAHkAcwAwACAALwAgAF8ARABhAHkAcwBJAG4ANABZAGUAYQByACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQBzADEALAAgAF8AZABhAHkAcwAwACAALQAgAF8AcQB1AGEAZABZAHIAIAAqACAAXwBEAGEAeQBzAEkAbgA0AFkAZQBhAHIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwByAGUAbQBZAHIALAAgAEkATgBUACgAKABJAE4AVAAoAF8AZABhAHkAcwAxACAALwAgAF8ARABhAHkAcwBJAG4AWQBlAGEAcgApACAAKwAgADEAKQAgACoAIAAwAC4ANwA1ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQBzADIALAAgAF8AZABhAHkAcwAxACAALQAgAF8AcgBlAG0AWQByACAAKgAgAF8ARABhAHkAcwBJAG4AWQBlAGEAcgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkALAAgAF8AcQB1AGEAZABZAHIAIAAqACAANAAgACsAIABfAHIAZQBtAFkAcgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0ALAAgAEkATgBUACgAKABfAGQAYQB5AHMAMgAgACoAIAA1ACAAKwAgAF8ATQBvAG4AdABoAEMAbwByAHIAZQBjAHQAaQBvAG4ARABhAHkAcwApACAALwAgAF8ARABhAHkAcwBJAG4ANQBNAG8AbgB0AGgAcwBGAHIAbwBtAE0AYQByAGMAaAApACAALQAgADIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQAsACAAXwBkAGEAeQBzADIAIAAtACAASQBOAFQAKAAoAF8AbQAgACsAIAA0ACkAIAAqACAAXwBEAGEAeQBzAEkAbgA1AE0AbwBuAHQAaABzAEYAcgBvAG0ATQBhAHIAYwBoACAALwAgADUAKQAgACsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBEAGEAeQBzAEkAbgA0AE0AbwBuAHQAaABzACAAKwAgADEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AGUAYQByACwAIABfAFkARQBBAFIANAA4ADAAMQBCAEMARQAgACsAIABfAHkAIAArACAASQBOAFQAKAAoAF8AbQAgACsAIAAyACkAIAAvACAAMQAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBtAG8AbgB0AGgALAAgAE0ATwBEACgAXwBtACAAKwAgADIALAAgADEAMgApACAAKwAgADEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABfAHkAZQBhAHIALAAgAF8AbQBvAG4AdABoACwAIABfAGQAYQB5ACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBKAEQATgBfAFQATwBfAE8AUgBEAEkATgBBAEwAXwBEAEEAVABFAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAHQAaABlACAAeQBlAGEAcgAsACAAbwByAGQAaQBuAGEAbAAgAGQAYQB5ACAAbwBmACAAeQBlAGEAcgAgAGEAbgBkACAAZABhAHkAcwAgAGkAbgAgAHQAaABlACAAeQBlAGEAcgAgAGYAcgBvAG0AIAB0AGgAZQAgAGcAaQB2AGUAbgAgAEoAdQBsAGkAYQBuACAARABhAHkAIABOAHUAbQBiAGUAcgAgAGkAbgAgAHQAaABlACAAcwBwAGUAYwBpAGYAaQBlAGQAXABuAGMAYQBsAGUAbgBkAGEAcgAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABpAG4AdABlAGcAZQByACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAWQBlAGEAcgAgAGkAbgAgAEMAbwBtAG0AbwBuACAARQByAGEALgAgAE4AbwB0AGUAIAB0AGgAYQB0ACAAMQAgAEIAQwAgAD0AIAAwACAAQwBFACwAIAAyACAAQgBDACAAPQAgAC0AMQAgAEMARQBcAG4AIAAyACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADEALgAuADMANgA2AF0AIAAgAHwAIABPAHIAZABpAG4AYQBsACAAZABhAHkAXABuACAAMwAgAHwAIABpAG4AdABlAGcAZQByACAAWwAzADYANQAsADMANgA2AF0AIAB8ACAARABhAHkAcwAgAGkAbgAgAHkAZQBhAHIAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBKAEQATgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByACAAZgBvAHIAIAB0AGgAZQAgAGMAYQBsAGUAbgBkAGEAcgAgAGQAYQB5AFwAbgBbAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACAAfAAgAHMAdwBpAHQAYwBoACAAIAB8ACAAQwBhAGwAYwB1AGwAYQB0AGUAIABmAG8AcgAgAHQAaABlACAASgB1AGwAaQBhAG4AIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuACAARABlAGYAYQB1AGwAdAAgAGkAcwAgAEcAcgBlAGcAbwByAGkAYQBuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ASgBEAE4AXwBUAE8AXwBPAFIARABJAE4AQQBMAF8ARABBAFQARQAgAD0AIABMAEEATQBCAEQAQQAoAEoARABOACwAIABbAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACwAXABuACAAIAAgACAASQBGACgASgBEAE4AIAA9ACAAXAAiAFwAIgAsACAAewBcACIAXAAiACwAIABcACIAXAAiACwAIABcACIAXAAiAH0ALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgASgBEAE4AKQApACwAIAB7ACMAVgBBAEwAVQBFACEALAAgACMAVgBBAEwAVQBFACEALAAgACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AagBkAG4ALAAgAEkATgBUACgASgBEAE4AKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHQAZQAsACAASgBEAE4AXwBUAE8AXwBDAEEATABFAE4ARABBAFIAXwBEAEEAVABFACgAXwBqAGQAbgAsACAASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIAQwBFACwAIABJAE4ARABFAFgAKABfAGQAYQB0AGUALAAgADEALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AagBkAG4AWQBlAGEAcgBTAHQAYQByAHQALAAgAEoAVQBMAEkAQQBOAF8ARABBAFkAXwBOAFUATQBCAEUAUgAoAF8AeQBlAGEAcgBDAEUALAAgADEALAAgADEALAAgAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBvAHIAZABpAG4AYQBsAEQAYQB5ACwAIABfAGoAZABuACAALQAgAF8AagBkAG4AWQBlAGEAcgBTAHQAYQByAHQAIAArACAAMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkAcwBJAG4AWQBlAGEAcgAsACAARABBAFkAUwBfAEkATgBfAFkARQBBAFIAKABfAHkAZQBhAHIAQwBFACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIAQwBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG8AcgBkAGkAbgBhAGwARABhAHkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkAcwBJAG4AWQBlAGEAcgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBPAFIARABJAE4AQQBMAF8ARABBAFQARQBfAFQATwBfAEoARABOAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAHQAaABlACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByACAAbwBmACAAdABoAGUAIABwAHIAbwB2AGkAZABlAGQAIABvAHIAZABpAG4AYQBsACAAZABhAHQAZQAgAGkAbgAgAHQAaABlACAAcwBwAGUAYwBpAGYAaQBlAGQAIABjAGEAbABlAG4AZABhAHIALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIABKAHUAbABpAGEAbgAgAEQAYQB5ACAATgB1AG0AYgBlAHIAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBZAGUAYQByAEMARQAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAWQBlAGEAcgAgAGkAbgAgAEMAbwBtAG0AbwBuACAARQByAGEALgAgAE4AbwB0AGUAIAB0AGgAYQB0ACAAMQAgAEIAQwAgAD0AIAAwACAAQwBFACwAIAAyACAAQgBDACAAPQAgAC0AMQAgAEMARQBcAG4ATwByAGQAaQBuAGEAbABEAGEAeQAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAWwAxAC4ALgAzADYANgApACAAfAAgAEQAYQB5ACAAbwBmACAAeQBlAGEAcgAsACAAYwBhAHIAcgBpAGUAcwAgAGkAZgAgAHIAYQBuAGcAZQAgAGUAeABjAGUAZQBkAGUAZABcAG4AWwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAgAHwAIABzAHcAaQB0AGMAaAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAEMAYQBsAGMAdQBsAGEAdABlACAAZgBvAHIAIAB0AGgAZQAgAEoAdQBsAGkAYQBuACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgAgAEQAZQBmAGEAdQBsAHQAIABpAHMAIABHAHIAZQBnAG8AcgBpAGEAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAE8AUgBEAEkATgBBAEwAXwBEAEEAVABFAF8AVABPAF8ASgBEAE4AIAA9ACAATABBAE0AQgBEAEEAKABZAGUAYQByAEMARQAsACAATwByAGQAaQBuAGEAbABEAGEAeQAsACAAWwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAsAFwAbgAgACAAIAAgAEkARgAoACgAWQBlAGEAcgBDAEUAIAA9ACAAXAAiAFwAIgApACAAKgAgACgATwByAGQAaQBuAGEAbABEAGEAeQAgAD0AIABcACIAXAAiACkALAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgAWQBlAGEAcgBDAEUAKQApACAAKwAgAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgATwByAGQAaQBuAGEAbABEAGEAeQApACkALAAgAHsAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBvAHIAZABpAG4AYQBsAEQAYQB5ACwAIABJAE4AVAAoAE8AcgBkAGkAbgBhAGwARABhAHkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AagBkAG4AWQBlAGEAcgBTAHQAYQByAHQALAAgAEoAVQBMAEkAQQBOAF8ARABBAFkAXwBOAFUATQBCAEUAUgAoAFkAZQBhAHIAQwBFACwAIAAxACwAIAAxACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AagBkAG4AWQBlAGEAcgBTAHQAYQByAHQAIAArACAAXwBvAHIAZABpAG4AYQBsAEQAYQB5ACAALQAgADEAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBHAFIARQBHAE8AUgBJAEEATgBfAFQATwBfAEoAVQBMAEkAQQBOAFwAbgBcAG4AVAByAGEAbgBzAGwAYQB0AGUAcwAgAGEAIABkAGEAdABlACAAaQBuACAAdABoAGUAIABHAHIAZQBnAG8AcgBpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByACAAdABvACAAdABoAGUAIABKAHUAbABpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AXABuAFwAbgBPAHUAdABwAHUAdABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAGkAbgB0AGUAZwBlAHIAIAAgACAAIAAgACAAIAAgACAAfAAgAFkAZQBhAHIAIABpAG4AIABDAG8AbQBtAG8AbgAgAEUAcgBhAC4AIABOAG8AdABlACAAdABoAGEAdAAgADEAIABCAEMAIAA9ACAAMAAgAEMARQAsACAAMgAgAEIAQwAgAD0AIAAtADEAIABDAEUAXABuACAAMgAgAHwAIABpAG4AdABlAGcAZQByACAAWwAxAC4ALgAxADIAXQAgAHwAIABNAG8AbgB0AGgAXABuACAAMwAgAHwAIABpAG4AdABlAGcAZQByACAAWwAxAC4ALgAzADEAXQAgAHwAIABEAGEAeQBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFkAZQBhAHIAQwBFACAAfAAgAGkAbgB0AGUAZwBlAHIAIAAgACAAIAAgACAAIAAgACAAfAAgAFkAZQBhAHIAIABpAG4AIABDAG8AbQBtAG8AbgAgAEUAcgBhAC4AIABOAG8AdABlACAAdABoAGEAdAAgADEAIABCAEMAIAA9ACAAMAAgAEMARQAsACAAMgAgAEIAQwAgAD0AIAAtADEAIABDAEUAXABuAE0AbwBuAHQAaAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADEALgAuADEAMgBdACAAfAAgAFwAbgBEAGEAeQAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAWwAxAC4ALgAzADIAKQAgAHwAIABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ARwBSAEUARwBPAFIASQBBAE4AXwBUAE8AXwBKAFUATABJAEEATgAgAD0AIABMAEEATQBCAEQAQQAoAFkAZQBhAHIAQwBFACwAIABNAG8AbgB0AGgALAAgAEQAYQB5ACwAXABuACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgAF8ASgBEAE4ALAAgAEoAVQBMAEkAQQBOAF8ARABBAFkAXwBOAFUATQBCAEUAUgAoAFkAZQBhAHIAQwBFACwAIABNAG8AbgB0AGgALAAgAEQAYQB5ACwAIAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgBTACgASQBTAEUAUgBSAE8AUgAoAF8ASgBEAE4AKQAsACAAewAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBKAEQATgAgAD0AIABcACIAXAAiACwAIAB7AFwAIgBcACIALAAgAFwAIgBcACIALAAgAFwAIgBcACIAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAIABKAEQATgBfAFQATwBfAEMAQQBMAEUATgBEAEEAUgBfAEQAQQBUAEUAKABfAEoARABOACwAIAAxACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBKAFUATABJAEEATgBfAFQATwBfAEcAUgBFAEcATwBSAEkAQQBOAFwAbgBcAG4AVAByAGEAbgBzAGwAYQB0AGUAcwAgAGEAIABkAGEAdABlACAAaQBuACAAdABoAGUAIABKAHUAbABpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByACAAdABvACAAdABoAGUAIABHAHIAZQBnAG8AcgBpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AXABuAFwAbgBPAHUAdABwAHUAdABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAGkAbgB0AGUAZwBlAHIAIAAgACAAIAAgACAAIAAgACAAfAAgAFkAZQBhAHIAIABpAG4AIABDAG8AbQBtAG8AbgAgAEUAcgBhAC4AIABOAG8AdABlACAAdABoAGEAdAAgADEAIABCAEMAIAA9ACAAMAAgAEMARQAsACAAMgAgAEIAQwAgAD0AIAAtADEAIABDAEUAXABuACAAMgAgAHwAIABpAG4AdABlAGcAZQByACAAWwAxAC4ALgAxADIAXQAgAHwAIABNAG8AbgB0AGgAXABuACAAMwAgAHwAIABpAG4AdABlAGcAZQByACAAWwAxAC4ALgAzADEAXQAgAHwAIABEAGEAeQBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFkAZQBhAHIAQwBFACAAfAAgAGkAbgB0AGUAZwBlAHIAIAAgACAAIAAgACAAIAAgACAAfAAgAFkAZQBhAHIAIABpAG4AIABDAG8AbQBtAG8AbgAgAEUAcgBhAC4AIABOAG8AdABlACAAdABoAGEAdAAgADEAIABCAEMAIAA9ACAAMAAgAEMARQAsACAAMgAgAEIAQwAgAD0AIAAtADEAIABDAEUAXABuAE0AbwBuAHQAaAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADEALgAuADEAMgBdACAAfAAgAFwAbgBEAGEAeQAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAWwAxAC4ALgAzADIAKQAgAHwAIABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ASgBVAEwASQBBAE4AXwBUAE8AXwBHAFIARQBHAE8AUgBJAEEATgAgAD0AIABMAEEATQBCAEQAQQAoAFkAZQBhAHIAQwBFACwAIABNAG8AbgB0AGgALAAgAEQAYQB5ACwAXABuACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgAF8ASgBEAE4ALAAgAEoAVQBMAEkAQQBOAF8ARABBAFkAXwBOAFUATQBCAEUAUgAoAFkAZQBhAHIAQwBFACwAIABNAG8AbgB0AGgALAAgAEQAYQB5ACwAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgBTACgASQBTAEUAUgBSAE8AUgAoAF8ASgBEAE4AKQAsACAAewAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBKAEQATgAgAD0AIABcACIAXAAiACwAIAB7AFwAIgBcACIALAAgAFwAIgBcACIALAAgAFwAIgBcACIAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAIABKAEQATgBfAFQATwBfAEMAQQBMAEUATgBEAEEAUgBfAEQAQQBUAEUAKABfAEoARABOACwAIAAwACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBTAEUAQwBVAEwAQQBSAF8ARABJAEYARgBFAFIARQBOAEMARQBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAG4AdQBtAGIAZQByACAAbwBmACAAZABhAHkAcwAgAHQAaABlACAARwByAGUAZwBvAHIAaQBhAG4AIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAgAGkAcwAgAGEAaABlAGEAZAAgAG8AZgAgAHQAaABlACAASgB1AGwAaQBhAG4AIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAgAGYAbwByAFwAbgBhACAAZwBpAHYAZQBuACAAZABhAHQAZQAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAEQAYQB5AHMAIABkAGkAZgBmAGUAcgBlAG4AYwBlAC4AIABOAGUAZwBhAHQAaQB2AGUAIAB2AGEAbAB1AGUAcwAgAGEAcgBlACAAdwBoAGUAbgAgAHQAaABlACAASgB1AGwAaQBhAG4AIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGUAcgAgAGkAcwAgAGEAaABlAGEAZAAuAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AWQBlAGEAcgBDAEUAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAAgACAAIAAgACAAIAAgACAAfAAgAFkAZQBhAHIAIABpAG4AIABDAG8AbQBtAG8AbgAgAEUAcgBhAC4AIABOAG8AdABlACAAdABoAGEAdAAgADEAIABCAEMAIAA9ACAAMAAgAEMARQAsACAAMgAgAEIAQwAgAD0AIAAtADEAIABDAEUAXABuAE0AbwBuAHQAaAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAWwAxAC4ALgAxADIAXQAgAHwAIABcAG4ARABhAHkAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIABbADEALgAuADMAMgApACAAfAAgAFwAbgBbAEYAcgBvAG0ASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0AIAB8ACAAcwB3AGkAdABjAGgAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAUAByAG8AdgBpAGQAZQBkACAAZABhAHQAZQAgAGkAcwAgAGkAbgAgAEoAdQBsAGkAYQBuACAAYwBhAGwAZQBuAGQAYQByAC4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABEAGUAZgBhAHUAbAB0ACAAaQBzACAAdABoAGUAIABHAHIAZQBnAG8AcgBpAGEAbgAgAGMAYQBsAGUAbgBkAGEAcgAuAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBTAEUAQwBVAEwAQQBSAF8ARABJAEYARgBFAFIARQBOAEMARQAgAD0AIABMAEEATQBCAEQAQQAoAFkAZQBhAHIAQwBFACwAIABNAG8AbgB0AGgALAAgAEQAYQB5ACwAIABbAEYAcgBvAG0ASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0ALABcAG4AIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAXwBkAGEAeQAsACAASQBOAFQAKABEAGEAeQApACwAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABOACgARgByAG8AbQBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAgAD0AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAEYAcgBvAG0AIABHAHIAZQBnAG8AcgBpAGEAbgAgAGMAYQBsAGUAbgBkAGEAcgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAEoARABOAF8ARwAsACAASgBVAEwASQBBAE4AXwBEAEEAWQBfAE4AVQBNAEIARQBSACgAWQBlAGEAcgBDAEUALAAgAE0AbwBuAHQAaAAsACAAXwBkAGEAeQAsACAAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgASQBTAEUAUgBSAE8AUgAoAF8ASgBEAE4AXwBHACkALAAgAHsAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAEoARABOAF8ARwAgAD0AIABcACIAXAAiACwAIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBKAEQATgBfAEoALAAgAEkARgAoACgATQBvAG4AdABoACAAPQAgADIAKQAgACoAIAAoAF8AZABhAHkAIAA9ACAAMgA5ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAEkAUwBfAEwARQBBAFAAXwBZAEUAQQBSACgAWQBlAGEAcgBDAEUALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABKAFUATABJAEEATgBfAEQAQQBZAF8ATgBVAE0AQgBFAFIAKABZAGUAYQByAEMARQAsACAAMgAsACAAMgA5ACwAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASgBVAEwASQBBAE4AXwBEAEEAWQBfAE4AVQBNAEIARQBSACgAWQBlAGEAcgBDAEUALAAgADIALAAgADIAOAAsACAAMQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASgBVAEwASQBBAE4AXwBEAEEAWQBfAE4AVQBNAEIARQBSACgAWQBlAGEAcgBDAEUALAAgAE0AbwBuAHQAaAAsACAAXwBkAGEAeQAsACAAMQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAEoARABOAF8ASgAgAC0AIABfAEoARABOAF8ARwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAARgByAG8AbQAgAEoAdQBsAGkAYQBuACAAYwBhAGwAZQBuAGQAYQByAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHQAZQBfAEcALAAgAEoAVQBMAEkAQQBOAF8AVABPAF8ARwBSAEUARwBPAFIASQBBAE4AKABZAGUAYQByAEMARQAsACAATQBvAG4AdABoACwAIABfAGQAYQB5ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABJAFMARQBSAFIATwBSACgASQBOAEQARQBYACgAXwBkAGEAdABlAF8ARwAsACAAMQAsACAAMQApACkALAAgAHsAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABJAE4ARABFAFgAKABfAGQAYQB0AGUAXwBHACwAIAAxACwAIAAxACkAIAA9ACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABTAEUAQwBVAEwAQQBSAF8ARABJAEYARgBFAFIARQBOAEMARQAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkATgBEAEUAWAAoAF8AZABhAHQAZQBfAEcALAAgADEALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkATgBEAEUAWAAoAF8AZABhAHQAZQBfAEcALAAgADEALAAgADIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkATgBEAEUAWAAoAF8AZABhAHQAZQBfAEcALAAgADEALAAgADMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAFwAbgBcAG4AXABuAFwAbgBcAG4AXABuAC8AKgAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAXABuACMAIABXAEUARQBLAFMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAqAC8AXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ARABBAFkAXwBPAEYAXwBXAEUARQBLAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAGEAbgAgAGkAbgB0AGUAZwBlAHIAIABmAG8AcgAgAHQAaABlACAAZABhAHkAIABvAGYAIAB0AGgAZQAgAHcAZQBlAGsAIABmAG8AcgAgAGEAIABnAGkAdgBlAG4AIABKAHUAbABpAGEAbgAgAEQAYQB5ACAATgB1AG0AYgBlAHIALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMQAuAC4ANwBdACAAfAAgAEkAUwBPACAAZABhAHkAIABvAGYAIAB3AGUAZQBrACAAbgB1AG0AYgBlAHIAXABuACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAATQBvAG4AZABhAHkALgAuAFMAdQBuAGQAYQB5AFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ASgBEAE4AIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIABKAHUAbABpAGEAbgAgAEQAYQB5ACAATgB1AG0AYgBlAHIAIABmAG8AcgAgAHQAaABlACAAYwBhAGwAZQBuAGQAYQByACAAZABhAHkAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEQAQQBZAF8ATwBGAF8AVwBFAEUASwAgAD0AIABMAEEATQBCAEQAQQAoAEoARABOACwAXABuACAAIAAgACAASQBGACgASgBEAE4AIAA9ACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABKAEQATgApACkALAAgAHsAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBqAGQAbgAsACAASQBOAFQAKABKAEQATgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATQBPAEQAKABfAGoAZABuACwAIAA3ACkAIAArACAAMQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEMATwBOAFYARQBSAFQAXwBXAEUARQBLAEQAQQBZAF8ATgBVAE0AQgBFAFIAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAYQBuACAAaQBuAHQAZQBnAGUAcgAgAGYAbwByACAAdABoAGUAIABkAGEAeQAgAG8AZgAgAHQAaABlACAAdwBlAGUAawAgAGYAcgBvAG0AIAB0AGgAZQAgAHQAcgBhAGQAaQB0AG8AbgBhAGwAIABuAHUAbQBiAGUAcgBpAG4AZwAgAHMAYwBoAGUAbQBlACAAdABvACAAdABoAGUAIABJAFMATwAgAGQAZQBmAGkAbgBpAHQAaQBvAG4ALAAgAG8AcgBcAG4AdgBpAGMAZQAgAHYAZQByAHMAYQAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAFcAZQBlAGsAZABhAHkAIABuAHUAbQBiAGUAcgBcAG4AIAAgACAAfAAgAFsAMQAuAC4ANwBdACAAIAB8ACAAIAAgACAAfAAgAEkAUwBPACAAIAAgACAAIAAgACAAfAAgAFQAcgBhAGQAaQB0AGkAbwBhAGwAXABuACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAgADEAIAB8ACAATQBvAG4AZABhAHkAIAAgACAAIAB8ACAAUwB1AG4AZABhAHkAIABcAG4AIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAyACAAfAAgAFQAdQBlAHMAZABhAHkAIAAgACAAfAAgAE0AbwBuAGQAYQB5ACAAXABuACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgACAAMwAgAHwAIABXAGUAZABuAGUAcwBkAGEAeQAgAHwAIABUAHUAZQBzAGQAYQB5AFwAbgAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAgADQAIAB8ACAAVABoAHUAcgBzAGQAYQB5ACAAIAB8ACAAVwBlAGQAbgBlAHMAZABhAHkAXABuACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgACAANQAgAHwAIABGAHIAaQBkAGEAeQAgACAAIAAgAHwAIABUAGgAdQByAHMAZABhAHkAXABuACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgACAANgAgAHwAIABTAGEAdAB1AHIAZABhAHkAIAAgAHwAIABGAHIAaQBkAGEAeQBcAG4AIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAA3ACAAfAAgAFMAdQBuAGQAYQB5ACAAIAAgACAAfAAgAFMAYQB0AHUAcgBkAGEAeQBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEQAYQB5AE8AZgBXAGUAZQBrACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADEALgAuADcAXQAgAHwAIABEAGEAeQAgAG8AZgAgAHcAZQBlAGsAIABuAHUAbQBiAGUAcgBcAG4AWwBJAFMATwB0AG8AVAByAGEAZABpAHQAaQBvAG4AYQBsAF0AIAB8ACAAcwB3AGkAdABjAGgAIAAgACAAIAAgACAAIAAgACAAfAAgAFIAZQB0AHUAcgBuACAAZABhAHkAIABvAGYAIAB3AGUAZQBrACAAdQBzAGkAbgBnACAAdAByAGEAZABpAHQAaQBvAG4AYQBsACAAbgB1AG0AYgBlAHIAaQBuAGcAIABzAGMAaABlAG0AZQAsACAAYQBzAHMAdQBtAGkAbgBnACAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABEAGEAeQBPAGYAVwBlAGUAawAgAHcAYQBzACAAcAByAG8AdgBpAGQAZQBkACAAYQBjAGMAbwByAGQAaQBuAGcAIAB0AG8AIABJAFMATwAgAGQAZQBmAGkAbgBpAHQAaQBvAG4ALgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAEQAZQBmAGEAdQBsAHQAIABpAHMAIAB0AG8AIAByAGUAdAB1AHIAbgAgAGkAbgAgAEkAUwBPACAAZABlAGYAaQBuAGkAdABpAG8AbgAsACAAYQBzAHMAdQBtAGkAbgBnACAARABhAHkATwBmAFcAZQBlAGsAIAB3AGEAcwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAHAAcgBvAHYAaQBkAGUAZAAgAGEAYwBjAG8AcgBkAGkAbgBnACAAdABvACAAdABoAGUAIAB0AHIAYQBkAGkAdABpAG8AbgBhAGwAIABuAHUAbQBiAGUAcgBpAG4AZwAgAHMAYwBoAGUAbQBlAC4AXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEMATwBOAFYARQBSAFQAXwBXAEUARQBLAEQAQQBZAF8ATgBVAE0AQgBFAFIAIAA9ACAATABBAE0AQgBEAEEAKABEAGEAeQBPAGYAVwBlAGUAawAsACAAWwBJAFMATwB0AG8AVAByAGEAZABpAHQAaQBvAG4AYQBsAF0ALABcAG4AIAAgACAAIABJAEYAKABEAGEAeQBPAGYAVwBlAGUAawAgAD0AIABcACIAXAAiACwAIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEQAYQB5AE8AZgBXAGUAZQBrACkAKQAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGcAaQB2AGUAbgBEAG8AVwAsACAASQBOAFQAKABOACgARABhAHkATwBmAFcAZQBlAGsAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBmAHIAbwBtAEkAUwBPACwAIABOACgASQBTAE8AdABvAFQAcgBhAGQAaQB0AGkAbwBuAGEAbAApACAAPAA+ACAAMAAsACAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGgAaQBmAHQARABvAFcALAAgAF8AZwBpAHYAZQBuAEQAbwB3ACAAKwAgAEkARgAoAF8AZgByAG8AbQBJAFMATwAsACAAMAAsACAALQAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABNAE8ARAAoAF8AcwBoAGkAZgB0AEQAbwB3ACwAIAA3ACkAIAArACAAMQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFcARQBFAEsARABBAFkAXwBPAEYAXwBNAE8ATgBUAEgAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAYQAgAEoAdQBsAGkAYQBuACAARABhAHkAIABOAHUAbQBiAGUAcgAgAGYAbwByACAAYQAgAGcAaQB2AGUAbgAgAGQAYQB5ACAAbwBmACAAdwBlAGUAawAsACAAYQBuAGQAIABhACAAcgBlAGwAYQB0AGkAdgBlACAAdwBlAGUAawAgAGYAbwByACAAdABoAGUAIABtAG8AbgB0AGgAIABhAG4AZAAgAHkAZQBhAHIAIABvAGYAIAB0AGgAZQBcAG4AcwBwAGUAYwBpAGYAaQBlAGQAIABjAGEAbABlAG4AZABhAHIALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIABKAHUAbABpAGEAbgAgAEQAYQB5ACAATgB1AG0AYgBlAHIAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBZAGUAYQByAEMARQAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAAgACAAIAAgACAAIAAgACAAfAAgAFkAZQBhAHIAIABpAG4AIABDAG8AbQBtAG8AbgAgAEUAcgBhAC4AIABOAG8AdABlACAAdABoAGEAdAAgADEAIABCAEMAIAA9ACAAMAAgAEMARQAsACAAMgAgAEIAQwAgAD0AIAAtADEAIABDAEUAXABuAE0AbwBuAHQAaAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMQAuAC4AMQAyAF0AIAB8ACAATQBvAG4AdABoACAAbwBmACAAdABoAGUAIAB5AGUAYQByAFwAbgBXAGUAZQBrAE8AZgBNAG8AbgB0AGgAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAAgACAAIAAgACAAIAAgACAAfAAgAFcAZQBlAGsAIABpAG4AIAB0AGgAZQAgAG0AbwBuAHQAaAAuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAE4AbwB0AGUAIABpAGYAIAB0AGgAZQAgAHIAZQBmAGUAcgBlAG4AYwBlACAAZQB4AGMAZQBlAGQAcwAgAHQAaABlACAAYgBvAHUAbgBkAHMAIABvAGYAIAB0AGgAZQAgAG0AbwBuAHQAaAAsACAAYQBuAG8AdABoAGUAcgAgAG0AbwBuAHQAaABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAB3AGkAbABsACAAYgBlACAAcgBlAHQAdQByAG4AZQBkAC4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAxACAALQAgAGYAaQByAHMAdAAgAHcAZQBlAGsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAyACAALQAgAHMAZQBjAG8AbgBkACAAdwBlAGUAawBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgADMAIAAtACAAdABoAGkAcgBkACAAdwBlAGUAawBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgADQAIAAtACAAZgBvAHUAcgB0AGgAIAB3AGUAZQBrAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAANQAgAC0AIABmAGkAZgB0AGgAIAB3AGUAZQBrAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAMAAgAC0AIABsAGEAcwB0ACAAdwBlAGUAawBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAtADEAIAAtACAAcwBlAGMAbwBuAGQAIAB0AG8AIABsAGEAcwB0ACAAdwBlAGUAawBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAtADIAIAAtACAAdABoAGkAcgBkACAAdABvACAAbABhAHMAdAAgAHcAZQBlAGsAXABuAEkAUwBPAFcAZQBlAGsARABhAHkAIAAgACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgAFsAMQAuAC4ANwBdACAAIAB8ACAASQBTAE8AIABkAGEAeQAgAG8AZgAgAHcAZQBlAGsAIABuAHUAbQBiAGUAcgAgAE0AbwBuAGQAYQB5AC4ALgBTAHUAbgBkAGEAeQBcAG4AWwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAgAHwAIABzAHcAaQB0AGMAaAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABDAGEAbABjAHUAbABhAHQAZQAgAGYAbwByACAAdABoAGUAIABKAHUAbABpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AIABEAGUAZgBhAHUAbAB0ACAAaQBzACAARwByAGUAZwBvAHIAaQBhAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgBcAG4AIAAgACAAIABcAG4ARQB4AGEAbQBwAGwAZQBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBXAEUARQBLAEQAQQBZAF8ATwBGAF8ATQBPAE4AVABIACgAMgAwADIAMwAsACAANgAsACAAMAAsACAANwApAFwAbgBSAGUAdAB1AHIAbgBzADoAIABKAEQATgAgADIANAA2ADAAMQAyADEAIAAoADIANQAvADAANgAvADIAMAAyADMAKQAgAGkAZQAuACAAdABoAGUAIABsAGEAcwB0ACAAUwB1AG4AZABhAHkAIABvAGYAIABKAHUAbgBlACAAMgAwADIAMwBcAG4AXABuAFcARQBFAEsARABBAFkAXwBPAEYAXwBNAE8ATgBUAEgAKAAyADAAMgAzACwAIAAxACwAIAAyACwAIAAyACkAXABuAFIAZQB0AHUAcgBuAHMAOgAgAEoARABOACAAMgA0ADUAOQA5ADUANQAgACgAMQAwAC8AMAAxAC8AMgAwADIAMwApACAAaQBlAC4AIAB0AGgAZQAgAHMAZQBjAG8AbgBkACAAVAB1AGUAcwBkAGEAeQAgAG8AZgAgAEoAYQBuAHUAYQByAHkAIAAyADAAMgAzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBXAEUARQBLAEQAQQBZAF8ATwBGAF8ATQBPAE4AVABIACAAPQAgAEwAQQBNAEIARABBACgAWQBlAGEAcgBDAEUALAAgAE0AbwBuAHQAaAAsACAAVwBlAGUAawBPAGYATQBvAG4AdABoACwAIABJAFMATwBXAGUAZQBrAEQAYQB5ACwAIABbAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACwAXABuACAAIAAgACAASQBGACgAKABZAGUAYQByAEMARQAgAD0AIABcACIAXAAiACkAIAAqACAAKABNAG8AbgB0AGgAIAA9ACAAXAAiAFwAIgApACAAKgAgACgAVwBlAGUAawBPAGYATQBvAG4AdABoACAAPQAgAFwAIgBcACIAKQAgACoAIAAoAEkAUwBPAFcAZQBlAGsARABhAHkAIAA9ACAAXAAiAFwAIgApACwAIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAFkAZQBhAHIAQwBFACkAKQAgACsAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAE0AbwBuAHQAaAApACkAIAArACAATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABXAGUAZQBrAE8AZgBNAG8AbgB0AGgAKQApACAAKwAgAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgASQBTAE8AVwBlAGUAawBEAGEAeQApACkALAAgAHsAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoACgATQBPAEQAKABZAGUAYQByAEMARQAsACAAMQApACAAPgAgADAAKQAgACsAIAAoAE0ATwBEACgATQBvAG4AdABoACwAIAAxACkAIAA+ACAAMAApACAAKwAgACgATQBPAEQAKABXAGUAZQBrAE8AZgBNAG8AbgB0AGgALAAgADEAKQAgAD4AIAAwACkALAAgAHsAIwBOAFUATQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBtAG8AbgB0AGgALAAgAE0AbwBuAHQAaAAgACsAIABOACgAVwBlAGUAawBPAGYATQBvAG4AdABoACAAPAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBpAHMAbwBEAG8AVwAsACAATQBPAEQAKABJAE4AVAAoAEkAUwBPAFcAZQBlAGsARABhAHkAKQAgAC0AIAAxACwAIAA3ACkAIAArACAAMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBmAGkAcgBzAHQATwBmAE0AbwBuAHQAaAAsACAASgBVAEwASQBBAE4AXwBEAEEAWQBfAE4AVQBNAEIARQBSACgAWQBlAGEAcgBDAEUALAAgAF8AbQBvAG4AdABoACwAIAAxACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBmAGkAcgBzAHQARABvAFcALAAgAEQAQQBZAF8ATwBGAF8AVwBFAEUASwAoAF8AZgBpAHIAcwB0AE8AZgBNAG8AbgB0AGgAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBmAGkAcgBzAHQATwBmAE0AbwBuAHQAaAAgACsAIAAoACgAVwBlAGUAawBPAGYATQBvAG4AdABoACAALQAgADEAKQAgACoAIAA3ACkAIAArACAATQBPAEQAKABfAGkAcwBvAEQAbwB3ACAALQAgAF8AZgBpAHIAcwB0AEQAbwBXACwAIAA3ACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFcARQBFAEsAUwBfAEkATgBfAFkARQBBAFIAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIABjAG8AdQBuAHQAIABvAGYAIABJAFMATwAgAGQAZQBmAGkAbgBlAGQAIAB3AGUAZQBrAHMAIABpAG4AIABhACAAZwBpAHYAZQBuACAAeQBlAGEAcgAgAG8AZgAgAHQAaABlACAAcwBwAGUAYwBpAGYAaQBlAGQAIABjAGEAbABlAG4AZABhAHIALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsANQAyACwANQAzAF0AXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBZAGUAYQByAEMARQAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAAWQBlAGEAcgAgAGkAbgAgAEMAbwBtAG0AbwBuACAARQByAGEALgAgAE4AbwB0AGUAIAB0AGgAYQB0ACAAMQAgAEIAQwAgAD0AIAAwACAAQwBFACwAIAAyACAAQgBDACAAPQAgAC0AMQAgAEMARQBcAG4AWwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAgAHwAIABzAHcAaQB0AGMAaAAgACAAfAAgAEMAYQBsAGMAdQBsAGEAdABlACAAZgBvAHIAIAB0AGgAZQAgAEoAdQBsAGkAYQBuACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgAgAEQAZQBmAGEAdQBsAHQAIABpAHMAIABHAHIAZQBnAG8AcgBpAGEAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAFcARQBFAEsAUwBfAEkATgBfAFkARQBBAFIAIAA9ACAATABBAE0AQgBEAEEAKABZAGUAYQByAEMARQAsACAAWwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAsAFwAbgAgACAAIAAgAEkARgAoAFkAZQBhAHIAQwBFACAAPQAgAFwAIgBcACIALAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgAWQBlAGEAcgBDAEUAKQApACwAIAB7ACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZwByAGUAZwBvAHIAaQBhAG4ALAAgAE4AKABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAgAD0AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAZgBuAEwAYQBzAHQAVwBlAGUAawBEAGEAeQBPAGYAWQBlAGEAcgAsACAATABBAE0AQgBEAEEAKABfAHkAZQBhAHIAQwBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAYQB5AFAAcgBlAGMAZQBzAHMAaQBvAG4ALAAgAEkARgAoAF8AZwByAGUAZwBvAHIAaQBhAG4ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIAQwBFACAAKwAgAEkATgBUACgAXwB5AGUAYQByAEMARQAgAC8AIAA0ACkAIAAtACAASQBOAFQAKABfAHkAZQBhAHIAQwBFACAALwAgADEAMAAwACkAIAArACAASQBOAFQAKABfAHkAZQBhAHIAQwBFACAALwAgADQAMAAwACkAIAArACAANgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AeQBlAGEAcgBDAEUAIAArACAASQBOAFQAKABfAHkAZQBhAHIAQwBFACAALwAgADQAKQAgACsAIAA0AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAE0ATwBEACgAXwBkAGEAeQBQAHIAZQBjAGUAcwBzAGkAbwBuACwAIAA3ACkAIAArACAAMQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIAQwBFACwAIABJAE4AVAAoAFkAZQBhAHIAQwBFACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAbwB3AEwAYQBzAHQARABhAHkALAAgAGYAbgBMAGEAcwB0AFcAZQBlAGsARABhAHkATwBmAFkAZQBhAHIAKABfAHkAZQBhAHIAQwBFACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABvAHcATABhAHMAdABEAGEAeQAgAD0AIAA0ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABpAGYAIABsAGEAcwB0ACAAZABhAHkAIABvAGYAIAB5AGUAYQByACAAaQBzACAAYQAgAFQAaAB1AHIAcwBkAGEAeQAsACAAdABoAGUAbgAgAGgAYQBzACAAYQBuACAAZQB4AHQAcgBhACAAdwBlAGUAawBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADUAMwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAG8AdwBMAGEAcwB0AEQAYQB5AFAAcgBlAHYALAAgAGYAbgBMAGEAcwB0AFcAZQBlAGsARABhAHkATwBmAFkAZQBhAHIAKABfAHkAZQBhAHIAQwBFACAALQAgADEAKQAgACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABvAHcATABhAHMAdABEAGEAeQBQAHIAZQB2ACAAPQAgADMALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABpAGYAIABsAGEAcwB0ACAAZABhAHkAIABvAGYAIABwAHIAZQB2AGkAbwB1AHMAIAB5AGUAYQByACAAaQBzACAAYQAgAFcAZQBkAG4AZQBzAGQAYQB5ACwAIAB0AGgAZQBuACAAaABhAHMAIABhAG4AIABlAHgAdAByAGEAIAB3AGUAZQBrAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADUAMwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAG8AdABoAGUAcgB3AGkAcwBlAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADUAMgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFcARQBFAEsAXwBEAEEAVABFAF8AVABPAF8ASgBEAE4AXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIABKAHUAbABpAGEAbgAgAEQAYQB5ACAATgB1AG0AYgBlAHIAIABvAGYAIAB0AGgAZQAgAHAAcgBvAHYAaQBkAGUAZAAgAHcAZQBlAGsAIABkAGEAdABlACAAaQBuACAAdABoAGUAIABzAHAAZQBjAGkAZgBpAGUAZAAgAGMAYQBsAGUAbgBkAGEAcgAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAEoAdQBsAGkAYQBuACAARABhAHkAIABOAHUAbQBiAGUAcgBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFkAZQBhAHIAQwBFACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgACAAIAAgACAAIAAgACAAIAB8ACAAWQBlAGEAcgAgAGkAbgAgAEMAbwBtAG0AbwBuACAARQByAGEALgAgAE4AbwB0AGUAIAB0AGgAYQB0ACAAMQAgAEIAQwAgAD0AIAAwACAAQwBFACwAIAAyACAAQgBDACAAPQAgAC0AMQAgAEMARQBcAG4ASQBTAE8AVwBlAGUAawAgACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAWwAxAC4ALgA1ADMAXQAgAHwAIABJAFMATwAgAGQAZQBmAGkAbgBlAGQAIAB3AGUAZQBrACAAbgB1AG0AYgBlAHIAIABvAGYAIAB0AGgAZQAgAHkAZQBhAHIAXABuAEkAUwBPAFcAZQBlAGsARABhAHkAIAAgACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgAFsAMQAuAC4ANwBdACAAIAB8ACAASQBTAE8AIABkAGUAZgBpAG4AZQBkACAAZABhAHkAIABvAGYAIAB3AGUAZQBrACAATQBvAG4AZABhAHkALgAuAFMAdQBuAGQAYQB5AFwAbgBbAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACAAfAAgAHMAdwBpAHQAYwBoACAAIAAgACAAIAAgACAAIAAgACAAfAAgAEMAYQBsAGMAdQBsAGEAdABlACAAZgBvAHIAIAB0AGgAZQAgAEoAdQBsAGkAYQBuACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgAgAEQAZQBmAGEAdQBsAHQAIABpAHMAIABHAHIAZQBnAG8AcgBpAGEAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBXAEUARQBLAF8ARABBAFQARQBfAFQATwBfAEoARABOACAAPQAgAEwAQQBNAEIARABBACgAWQBlAGEAcgBDAEUALAAgAEkAUwBPAFcAZQBlAGsALAAgAEkAUwBPAFcAZQBlAGsARABhAHkALAAgAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0ALABcAG4AIAAgACAAIABJAEYAKAAoAFkAZQBhAHIAQwBFACAAPQAgAFwAIgBcACIAKQAgACoAIAAoAEkAUwBPAFcAZQBlAGsAIAA9ACAAXAAiAFwAIgApACAAKgAgACgASQBTAE8AVwBlAGUAawBEAGEAeQAgAD0AIABcACIAXAAiACkALAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgAWQBlAGEAcgBDAEUAKQApACAAKwAgAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgASQBTAE8AVwBlAGUAawApACkAIAArACAATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABJAFMATwBXAGUAZQBrAEQAYQB5ACkAKQAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGkAbgB2AGEAbABpAGQALAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABNAE8ARAAoAFkAZQBhAHIAQwBFACwAIAAxACkAIAA+ACAAMAAsACAAVABSAFUARQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATQBPAEQAKABJAFMATwBXAGUAZQBrACwAIAAxACkAIAA+ACAAMAAsACAAVABSAFUARQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBTAE8AVwBlAGUAawAgADwAIAAxACwAIABUAFIAVQBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAFMATwBXAGUAZQBrACAAPgAgADUAMwAsACAAVABSAFUARQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBTAE8AVwBlAGUAawAgAD0AIAA1ADMALAAgACgAVwBFAEUASwBTAF8ASQBOAF8AWQBFAEEAUgAoAFkAZQBhAHIAQwBFACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAgADwAIAA1ADMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABSAFUARQAsACAARgBBAEwAUwBFAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAGkAbgB2AGEAbABpAGQALAAgAHsAIwBOAFUATQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBoAGkAZgB0AEIAeQBXAGUAZQBrAHMALAAgACgASQBTAE8AVwBlAGUAawAgAC0AIAAxACkAIAAqACAANwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaABpAGYAdABEAGEAeQBPAGYAVwBlAGUAawAsACAATQBPAEQAKABJAE4AVAAoAEkAUwBPAFcAZQBlAGsARABhAHkAKQAgAC0AIAAxACwAIAA3ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBqAGQAbgBGAGkAcgBzAHQARABhAHkAWQBlAGEAcgAsACAASgBVAEwASQBBAE4AXwBEAEEAWQBfAE4AVQBNAEIARQBSACgAWQBlAGEAcgBDAEUALAAgADEALAAgADEALAAgAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZgBpAHIAcwB0AFcAZQBlAGsARABhAHkALAAgAEQAQQBZAF8ATwBGAF8AVwBFAEUASwAoAF8AagBkAG4ARgBpAHIAcwB0AEQAYQB5AFkAZQBhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIAQwBvAHIAcgBlAGMAdABpAG8AbgAsACAATQBPAEQAKAA0ACAALQAgAF8AZgBpAHIAcwB0AFcAZQBlAGsARABhAHkALAAgADcAKQAgAC0AIAAzACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AagBkAG4ARgBpAHIAcwB0AEQAYQB5AFkAZQBhAHIAIAArACAAXwB5AGUAYQByAEMAbwByAHIAZQBjAHQAaQBvAG4AIAArACAAXwBzAGgAaQBmAHQAQgB5AFcAZQBlAGsAcwAgACsAIABfAHMAaABpAGYAdABEAGEAeQBPAGYAVwBlAGUAawAgAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ASgBEAE4AXwBUAE8AXwBXAEUARQBLAF8ARABBAFQARQBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHkAZQBhAHIALAAgAEkAUwBPACAAZABlAGYAaQBuAGUAZAAgAHcAZQBlAGsAIABuAHUAbQBiAGUAcgAsACAAZABhAHkAIABvAGYAIAB0AGgAZQAgAHcAZQBlAGsALAAgAGEAbgBkACAAdwBlAGUAawBzACAAaQBuACAAdABoAGUAIAB5AGUAYQByACAAZgBvAHIAIAB0AGgAZQAgAGcAaQB2AGUAbgAgAEoAdQBsAGkAYQBuACAARABhAHkAXABuAE4AdQBtAGIAZQByACAAaQBuACAAdABoAGUAIABzAHAAZQBjAGkAZgBpAGUAZAAgAGMAYQBsAGUAbgBkAGEAcgAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABpAG4AdABlAGcAZQByACAAIAAgACAAIAAgACAAIAAgAHwAIABZAGUAYQByAEMARQBcAG4AIAAyACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADEALgAuADUAMwBdACAAfAAgAEkAUwBPACAAdwBlAGUAawAgAG4AdQBtAGIAZQByAFwAbgAgADMAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMQAuAC4ANwBdACAAIAB8ACAASQBTAE8AIABkAGEAeQAgAG8AZgAgAHcAZQBlAGsAIABNAG8AbgBkAGEAeQAuAC4AUwB1AG4AZABhAHkAXABuACAANAAgAHwAIABpAG4AdABlAGcAZQByACAAWwA1ADIALAA1ADMAXQAgAHwAIABJAFMATwAgAHcAZQBlAGsAcwAgAGkAbgAgAHkAZQBhAHIAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBKAEQATgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByACAAZgBvAHIAIAB0AGgAZQAgAGMAYQBsAGUAbgBkAGEAcgAgAGQAYQB5AFwAbgBbAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACAAfAAgAHMAdwBpAHQAYwBoACAAIAB8ACAAQwBhAGwAYwB1AGwAYQB0AGUAIABmAG8AcgAgAHQAaABlACAASgB1AGwAaQBhAG4AIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuACAARABlAGYAYQB1AGwAdAAgAGkAcwAgAEcAcgBlAGcAbwByAGkAYQBuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ASgBEAE4AXwBUAE8AXwBXAEUARQBLAF8ARABBAFQARQAgAD0AIABMAEEATQBCAEQAQQAoAEoARABOACwAIABbAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACwAXABuACAAIAAgACAASQBGACgASgBEAE4AIAA9ACAAXAAiAFwAIgAsACAAewBcACIAXAAiACwAIABcACIAXAAiACwAIABcACIAXAAiACwAIABcACIAXAAiAH0ALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgASgBEAE4AKQApACwAIAB7ACMAVgBBAEwAVQBFACEALAAgACMAVgBBAEwAVQBFACEALAAgACMAVgBBAEwAVQBFACEALAAgACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AagBkAG4ALAAgAEkATgBUACgASgBEAE4AKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYwBhAGwARABhAHQAZQAsACAASgBEAE4AXwBUAE8AXwBDAEEATABFAE4ARABBAFIAXwBEAEEAVABFACgAXwBqAGQAbgAsACAASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIAQwBFACwAIABJAE4ARABFAFgAKABfAGMAYQBsAEQAYQB0AGUALAAgADEALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkATwBmAFcAZQBlAGsALAAgAEQAQQBZAF8ATwBGAF8AVwBFAEUASwAoAF8AagBkAG4AKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkATwBmAFkAZQBhAHIALAAgAF8AagBkAG4AIAAtACAASgBVAEwASQBBAE4AXwBEAEEAWQBfAE4AVQBNAEIARQBSACgAXwB5AGUAYQByAEMARQAsACAAMQAsACAAMQAsACAASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByACkAIAArACAAMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbgBvAG0AaQBuAGEAbABXAGUAZQBrACwAIABJAE4AVAAoACgAXwBkAGEAeQBPAGYAWQBlAGEAcgAgAC0AIABfAGQAYQB5AE8AZgBXAGUAZQBrACAAKwAgADEAMAApACAALwAgADcAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABsAGEAcwB0ACAAdwBlAGUAawAgAG8AZgAgAHAAcgBlAHYAaQBvAHUAcwAgAHkAZQBhAHIAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG4AbwBtAGkAbgBhAGwAVwBlAGUAawAgAD0AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB3AGUAZQBrAHMASQBuAFkAZQBhAHIALAAgAFcARQBFAEsAUwBfAEkATgBfAFkARQBBAFIAKABfAHkAZQBhAHIAQwBFACAALQAgADEALAAgAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgApACwAIABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AGUAYQByAEMARQAgAC0AIAAxACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHcAZQBlAGsAcwBJAG4AWQBlAGEAcgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQBPAGYAVwBlAGUAawAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB3AGUAZQBrAHMASQBuAFkAZQBhAHIAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABpAGYAIAB0AGgAaQBzACAAeQBlAGEAcgAgAGQAbwBlAHMAIABuAG8AdAAgAGgAYQB2AGUAIAA1ADMAIAB3AGUAZQBrAHMALAAgAHQAaABlAG4AIABpAHMAIAB0AGgAZQAgAGYAaQByAHMAdAAgAHcAZQBlAGsAIABvAGYAIABmAG8AbABsAG8AdwBpAG4AZwAgAHkAZQBhAHIAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG4AbwBtAGkAbgBhAGwAVwBlAGUAawAgAD0AIAA1ADMALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAVwBFAEUASwBTAF8ASQBOAF8AWQBFAEEAUgAoAF8AeQBlAGEAcgBDAEUALAAgAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgApACAAPQAgADUAMwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIAQwBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAA1ADMALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkATwBmAFcAZQBlAGsALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADUAMwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdwBlAGUAawBzAEkAbgBZAGUAYQByACwAIABXAEUARQBLAFMAXwBJAE4AXwBZAEUAQQBSACgAXwB5AGUAYQByAEMARQAgACsAIAAxACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AGUAYQByAEMARQAgACsAIAAxACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQBPAGYAVwBlAGUAawAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHcAZQBlAGsAcwBJAG4AWQBlAGEAcgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB3AGUAZQBrAHMASQBuAFkAZQBhAHIALAAgAFcARQBFAEsAUwBfAEkATgBfAFkARQBBAFIAKABfAHkAZQBhAHIAQwBFACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIAQwBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG4AbwBtAGkAbgBhAGwAVwBlAGUAawAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQBPAGYAVwBlAGUAawAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB3AGUAZQBrAHMASQBuAFkAZQBhAHIAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFcARQBFAEsAXwBOAFUATQBCAEUAUgBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAEkAUwBPACAAZABlAGYAaQBuAGUAZAAgAHcAZQBlAGsAIABuAHUAbQBiAGUAcgAgAGYAbwByACAAYQAgAGcAaQB2AGUAbgAgAEoAdQBsAGkAYQBuACAARABhAHkAIABOAHUAbQBiAGUAcgAgAGkAbgAgAHQAaABlACAAcwBwAGUAYwBpAGYAaQBlAGQAIABjAGEAbABlAG4AZABhAHIALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMQAuAC4ANQAzAF0AIAB8ACAASQBTAE8AIAB3AGUAZQBrACAAbgB1AG0AYgBlAHIAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBKAEQATgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByAC4AXABuAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0AIAB8ACAAcwB3AGkAdABjAGgAIAAgAHwAIABDAGEAbABjAHUAbABhAHQAZQAgAGYAbwByACAAdABoAGUAIABKAHUAbABpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AIABEAGUAZgBhAHUAbAB0ACAAaQBzACAARwByAGUAZwBvAHIAaQBhAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBXAEUARQBLAF8ATgBVAE0AQgBFAFIAIAA9ACAATABBAE0AQgBEAEEAKABKAEQATgAsACAAWwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAsAFwAbgAgACAAIAAgAEkARgAoAEoARABOACAAPQAgAFwAIgBcACIALAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgASgBEAE4AKQApACwAIAB7ACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdwBlAGUAawBEAGEAdABlACwAIABKAEQATgBfAFQATwBfAFcARQBFAEsAXwBEAEEAVABFACgASgBEAE4ALAAgAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAQwBIAE8ATwBTAEUAQwBPAEwAUwAoAF8AdwBlAGUAawBEAGEAdABlACwAIAAyACkAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAFwAbgBcAG4AXABuAFwAbgBcAG4ALwAqACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwBcAG4AIwAgAFEAVQBBAFIAVABFAFIAUwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACoALwBcAG4AXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBEAEEAWQBTAF8ASQBOAF8AUQBVAEEAUgBUAEUAUgBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAGMAbwB1AG4AdAAgAG8AZgAgAGQAYQB5AHMAIABpAG4AIABhACAAcQB1AGEAcgB0AGUAcgAgAG8AZgAgAGEAIABnAGkAdgBlAG4AIAB5AGUAYQByACAAbwBmACAAdABoAGUAIABzAHAAZQBjAGkAZgBpAGUAZAAgAGMAYQBsAGUAbgBkAGEAcgAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABpAG4AdABlAGcAZQByACAAWwA4ADkALgAuADkAMgBdAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AUQB1AGEAcgB0AGUAcgAgACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAWwAxAC4ALgA0AF0AIAAgAHwAIABRAHUAYQByAHQAZQByACAAbwBmACAAdABoAGUAIAB5AGUAYQByACAAMQAuAC4ANAAsACAAdAByAGEAbgBzAGkAdABpAHYAZQAsACAAZQB4AGMAZQBlAGQAaQBuAGcAIAByAGEAbgBnAGUAIAB3AGkAbABsACAAYwBhAHIAcgB5ACAAdABvACAAeQBlAGEAcgAuAFwAbgBbAEYAaQBzAGMAYQBsAFkAZQBhAHIAQwBFAF0AIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAAgACAAIAAgACAAIAAgACAAfAAgAFkAZQBhAHIAIABpAG4AIABDAG8AbQBtAG8AbgAgAEUAcgBhAC4AIABOAG8AdABlACAAdABoAGEAdAAgADEAIABCAEMAIAA9ACAAMAAgAEMARQAsACAAMgAgAEIAQwAgAD0AIAAtADEAIABDAEUAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAVwBoAGUAbgAgAG0AbwBuAHQAaAAgAG8AZgBmAHMAZQB0ACAAaQBzACAAbgBvAG4ALQB6AGUAcgBvACAAdABoAGUAIABmAGkAcwBjAGEAbAAgAHkAZQBhAHIAIABzAHAAYQBuAHMAIABjAGEAbABlAG4AZABhAHIAIAB5AGUAYQByAHMAIABhAG4AZABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABpAHMAIABkAGUAZgBpAG4AZQBkACAAYQBzACAAdABoAGUAIAB5AGUAYQByACAAdwBoAGUAcgBlACAASgB1AG4AZQAgAGYAYQBsAGwAcwAuAFwAbgBbAE0AbwBuAHQAaABPAGYAZgBzAGUAdABdACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbAC0ANgAuAC4AMwBdACAAfAAgAFEAdQBhAHIAdABlAHIAIABtAG8AbgB0AGgAIABvAGYAZgBzAGUAdAAgAGYAcgBvAG0AIABKAGEAbgB1AGEAcgBhAHkAXABuAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0AIAB8ACAAcwB3AGkAdABjAGgAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAQwBhAGwAYwB1AGwAYQB0AGUAIABmAG8AcgAgAHQAaABlACAASgB1AGwAaQBhAG4AIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuACAARABlAGYAYQB1AGwAdAAgAGkAcwAgAEcAcgBlAGcAbwByAGkAYQBuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AXABuAFwAbgBFAHgAYQBtAHAAbABlAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEQAQQBZAFMAXwBJAE4AXwBRAFUAQQBSAFQARQBSACgAMwAsACAAMgAwADIAMAAsACAALQA2ACkAXABuAFIAZQB0AHUAcgBuAHMAOgAgADkAMQBcAG4AaQAuAGUALgAgADMAcgBkACAAcQB1AGEAcgB0AGUAcgAgAHMAdABhAHIAdABpAG4AZwAgAGYAcgBvAG0AIABKAHUAbAB5ACAAMgAwADEAOQAsACAAbgBhAG0AZQBsAHkAIABKAGEAbgAsACAARgBlAGIALAAgAE0AYQByACAAMgAwADIAMAAgAHcAaQB0AGgAIAAzADEALAAgADIAOQAsACAAMwAxACAAZABhAHkAcwAgAHIAZQBzAHAAZQBjAHQAaQB2AGUAbAB5AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBEAEEAWQBTAF8ASQBOAF8AUQBVAEEAUgBUAEUAUgAgAD0AIABMAEEATQBCAEQAQQAoAFEAdQBhAHIAdABlAHIALAAgAFsARgBpAHMAYwBhAGwAWQBlAGEAcgBDAEUAXQAsACAAWwBNAG8AbgB0AGgATwBmAGYAcwBlAHQAXQAsACAAWwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAsAFwAbgAgACAAIAAgAEkARgAoAFEAdQBhAHIAdABlAHIAIAA9ACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABRAHUAYQByAHQAZQByACkAKQAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgATQBPAEQAKABRAHUAYQByAHQAZQByACwAIAAxACkAIAA+ACAAMAAsACAAewAjAE4AVQBNACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AbwBuAHQAaABPAGYAZgBzAGUAdAAsACAAUgBPAFUATgBEACgATgAoAE0AbwBuAHQAaABPAGYAZgBzAGUAdAApACwAIAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoACgAXwBtAG8AbgB0AGgATwBmAGYAcwBlAHQAIAA8ACAALQA2ACkAIAArACAAKABfAG0AbwBuAHQAaABPAGYAZgBzAGUAdAAgAD4AIAAzACkALAAgAHsAIwBOAFUATQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHEAdQBhAHIAdABlAHIALAAgAE0ATwBEACgASQBOAFQAKABRAHUAYQByAHQAZQByACkAIAAtACAAMQAsACAANAApACwAIAAvAC8AIAAwAC4ALgAzAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkAcwBJAG4AUQB1AGEAcgB0AGUAcgBDAHkAYwBsAGkAYwBhAGwALAAgAHsAOQAwACwAOAA5ACwAOQAyACwAOQAxACwAOQAyACwAOQAyACwAOQAyACwAOQAyACwAOQAxACwAOQAyACwAOQAyACwAOQAwAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHEAdQBhAHIAdABlAHIAVwBpAHQAaABGAGUAYgAsACAASQBOAFQAKABNAE8ARAAoADEAIAAtACAAXwBtAG8AbgB0AGgATwBmAGYAcwBlAHQALAAgADEAMgApACAALwAgADMAKQAsACAAIAAvAC8AIAAwAC4ALgAzAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcQB1AGEAcgB0AGUAcgBQAHIAZQBjAGUAcwBzAGkAbwBuACwAIABNAE8ARAAoAF8AbQBvAG4AdABoAE8AZgBmAHMAZQB0ACAAKwAgACgAXwBxAHUAYQByAHQAZQByACAAKgAgADMAKQAsACAAMQAyACkAIAArACAAMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbgBvAG0AaQBuAGEAbABEAGEAeQBzAEkAbgBRAHUAYQByAHQAZQByACwAIABJAE4ARABFAFgAKABfAGQAYQB5AHMASQBuAFEAdQBhAHIAdABlAHIAQwB5AGMAbABpAGMAYQBsACwAIAAxACwAIABfAHEAdQBhAHIAdABlAHIAUAByAGUAYwBlAHMAcwBpAG8AbgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBsAGUAYQBwAEQAYQB5ACwAIABJAEYAKABJAFMATgBVAE0AQgBFAFIAKABGAGkAcwBjAGEAbABZAGUAYQByAEMARQApACAAKgAgACgAXwBxAHUAYQByAHQAZQByAFcAaQB0AGgARgBlAGIAIAA9ACAAXwBxAHUAYQByAHQAZQByACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AeQBlAGEAcgBPAGYARgBlAGIALAAgAEkATgBUACgARgBpAHMAYwBhAGwAWQBlAGEAcgBDAEUAKQAgACsAIABOACgAXwBxAHUAYQByAHQAZQByACAAPQAgADMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABOACgASQBTAF8ATABFAEEAUABfAFkARQBBAFIAKABfAHkAZQBhAHIATwBmAEYAZQBiACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAMABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBuAG8AbQBpAG4AYQBsAEQAYQB5AHMASQBuAFEAdQBhAHIAdABlAHIAIAArACAAXwBsAGUAYQBwAEQAYQB5AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AUQBVAEEAUgBUAEUAUgBfAEQAQQBUAEUAXwBUAE8AXwBKAEQATgBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAEoAdQBsAGkAYQBuACAARABhAHkAIABOAHUAbQBiAGUAcgAgAG8AZgAgAHQAaABlACAAcAByAG8AdgBpAGQAZQBkACAAcQB1AGEAcgB0AGUAcgAgAGQAYQB0AGUAIABpAG4AIAB0AGgAZQAgAHMAcABlAGMAaQBmAGkAZQBkACAAYwBhAGwAZQBuAGQAYQByAC4AXABuAFwAbgBPAHUAdABwAHUAdABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ARgBpAHMAYwBhAGwAWQBlAGEAcgBDAEUAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAIAAgACAAIAAgACAAIAAgAHwAIABZAGUAYQByACAAaQBuACAAQwBvAG0AbQBvAG4AIABFAHIAYQAuACAATgBvAHQAZQAgAHQAaABhAHQAIAAxACAAQgBDACAAPQAgADAAIABDAEUALAAgADIAIABCAEMAIAA9ACAALQAxACAAQwBFAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAFcAaABlAG4AIABtAG8AbgB0AGgAIABvAGYAZgBzAGUAdAAgAGkAcwAgAG4AbwBuAC0AegBlAHIAbwAgAHQAaABlACAAZgBpAHMAYwBhAGwAIAB5AGUAYQByACAAcwBwAGEAbgBzACAAYwBhAGwAZQBuAGQAYQByACAAeQBlAGEAcgBzACAAYQBuAGQAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAaQBzACAAZABlAGYAaQBuAGUAZAAgAGEAcwAgAHQAaABlACAAeQBlAGEAcgAgAHcAaABlAHIAZQAgAEoAdQBuAGUAIABmAGEAbABsAHMALgBcAG4AUQB1AGEAcgB0AGUAcgAgACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAWwAxAC4ALgA0AF0AIAAgAHwAIABRAHUAYQByAHQAZQByACAAbwBmACAAdABoAGUAIAB5AGUAYQByACAAMQAuAC4ANAAsACAAdAByAGEAbgBzAGkAdABpAHYAZQAsACAAZQB4AGMAZQBlAGQAaQBuAGcAIAByAGEAbgBnAGUAIAB3AGkAbABsACAAYwBhAHIAcgB5ACAAdABvACAAeQBlAGEAcgAuAFwAbgBEAGEAeQBPAGYAUQB1AGEAcgB0AGUAcgAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIABbADEALgAuADkAMgBdACAAfAAgAE8AcgBkAGkAbgBhAGwAIABkAGEAeQAgAG8AZgAgAHQAaABlACAAcQB1AGEAcgB0AGUAcgAsACAAZQB4AGMAZQBlAGQAaQBuAGcAIAByAGEAbgBnAGUAIAB3AGkAbABsACAAYwBhAHIAcgB5AFwAbgBbAE0AbwBuAHQAaABPAGYAZgBzAGUAdABdACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbAC0ANgAuAC4AMwBdACAAfAAgAFEAdQBhAHIAdABlAHIAIABtAG8AbgB0AGgAIABvAGYAZgBzAGUAdAAgAGYAcgBvAG0AIABKAGEAbgB1AGEAcgB5AFwAbgBbAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACAAfAAgAHMAdwBpAHQAYwBoACAAIAAgACAAIAAgACAAIAAgACAAfAAgAEMAYQBsAGMAdQBsAGEAdABlACAAZgBvAHIAIAB0AGgAZQAgAEoAdQBsAGkAYQBuACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgAgAEQAZQBmAGEAdQBsAHQAIABpAHMAIABHAHIAZQBnAG8AcgBpAGEAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBRAFUAQQBSAFQARQBSAF8ARABBAFQARQBfAFQATwBfAEoARABOACAAPQAgAEwAQQBNAEIARABBACgARgBpAHMAYwBhAGwAWQBlAGEAcgBDAEUALAAgAFEAdQBhAHIAdABlAHIALAAgAEQAYQB5AE8AZgBRAHUAYQByAHQAZQByACwAIABbAE0AbwBuAHQAaABPAGYAZgBzAGUAdABdACwAIABbAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACwAXABuACAAIAAgACAASQBGACgAKABGAGkAcwBjAGEAbABZAGUAYQByAEMARQAgAD0AIABcACIAXAAiACkAIAAqACAAKABRAHUAYQByAHQAZQByACAAPQAgAFwAIgBcACIAKQAgACoAIAAoAEQAYQB5AE8AZgBRAHUAYQByAHQAZQByACAAPQAgAFwAIgBcACIAKQAsACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABGAGkAcwBjAGEAbABZAGUAYQByAEMARQApACkAIAArACAATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABRAHUAYQByAHQAZQByACkAKQAgACsAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEQAYQB5AE8AZgBRAHUAYQByAHQAZQByACkAKQAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgATQBPAEQAKABRAHUAYQByAHQAZQByACwAIAAxACkAIAA+ACAAMAAsACAAewAjAE4AVQBNACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AbwBuAHQAaABPAGYAZgBzAGUAdAAsACAAUgBPAFUATgBEACgATgAoAE0AbwBuAHQAaABPAGYAZgBzAGUAdAApACwAIAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoACgAXwBtAG8AbgB0AGgATwBmAGYAcwBlAHQAIAA8ACAALQA2ACkAIAArACAAKABfAG0AbwBuAHQAaABPAGYAZgBzAGUAdAAgAD4AIAAzACkALAAgAHsAIwBOAFUATQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGYAaQBzAGMAYQBsAFkAZQBhAHIAQwBFACwAIABJAE4AVAAoAEYAaQBzAGMAYQBsAFkAZQBhAHIAQwBFACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHEAdQBhAHIAdABlAHIALAAgAEkATgBUACgAUQB1AGEAcgB0AGUAcgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGgAaQBmAHQATQBvAG4AdABoACwAIAAoAF8AcQB1AGEAcgB0AGUAcgAgAC0AIAAxACkAIAAqACAAMwAgACsAIABfAG0AbwBuAHQAaABPAGYAZgBzAGUAdAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AeQBlAGEAcgBDAEUALAAgAF8AZgBpAHMAYwBhAGwAWQBlAGEAcgBDAEUAIAArACAASQBOAFQAKABfAHMAaABpAGYAdABNAG8AbgB0AGgAIAAvACAAMQAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AbwBuAHQAaAAsACAATQBPAEQAKABfAHMAaABpAGYAdABNAG8AbgB0AGgALAAgADEAMgApACAAKwAgADEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGYAaQByAHMAdABEAGEAeQBPAGYAUQB1AGEAcgB0AGUAcgAsACAASgBVAEwASQBBAE4AXwBEAEEAWQBfAE4AVQBNAEIARQBSACgAXwB5AGUAYQByAEMARQAsACAAXwBtAG8AbgB0AGgALAAgADEALAAgAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBmAGkAcgBzAHQARABhAHkATwBmAFEAdQBhAHIAdABlAHIAIAAtACAAMQAgACsAIABJAE4AVAAoAEQAYQB5AE8AZgBRAHUAYQByAHQAZQByACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAIAAgACAAIABcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEoARABOAF8AVABPAF8AUQBVAEEAUgBUAEUAUgBfAEQAQQBUAEUAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIABmAGkAcwBjAGEAbAAgAHkAZQBhAHIALAAgAHEAdQBhAHIAdABlAHIALAAgAGQAYQB5ACAAbwBmACAAcQB1AGEAcgB0AGUAcgAgAGEAbgBkACAAZABhAHkAcwAgAGkAbgAgAHQAaABlACAAcQB1AGEAcgB0AGUAcgAgAGYAbwByACAAdABoAGUAIABnAGkAdgBlAG4AIABKAHUAbABpAGEAbgAgAEQAYQB5ACAATgB1AG0AYgBlAHIAXABuAGkAbgAgAHQAaABlACAAcwBwAGUAYwBpAGYAaQBlAGQAIABjAGEAbABlAG4AZABhAHIALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAaQBuAHQAZQBnAGUAcgAgACAAIAAgACAAIAAgACAAIAAgAHwAIABGAGkAcwBjAGEAbABZAGUAYQByAEMARQBcAG4AIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAVwBoAGUAbgAgAG0AbwBuAHQAaAAgAG8AZgBmAHMAZQB0ACAAaQBzACAAbgBvAG4ALQB6AGUAcgBvACAAdABoAGUAIABmAGkAcwBjAGEAbAAgAHkAZQBhAHIAIABzAHAAYQBuAHMAIABjAGEAbABlAG4AZABhAHIAIAB5AGUAYQByAHMAIABhAG4AZABcAG4AIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAaQBzACAAZABlAGYAaQBuAGUAZAAgAGEAcwAgAHQAaABlACAAeQBlAGEAcgAgAHcAaABlAHIAZQAgAEoAdQBuAGUAIABmAGEAbABsAHMALgBcAG4AIAAyACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADEALgAuADQAXQAgACAAIAB8ACAAUQB1AGEAcgB0AGUAcgBcAG4AIAAzACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADEALgAuADkAMgBdACAAIAB8ACAARABhAHkAIABvAGYAIABxAHUAYQByAHQAZQByAFwAbgAgADQAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAOAA5AC4ALgA5ADIAXQAgAHwAIABEAGEAeQBzACAAaQBuACAAcQB1AGEAcgB0AGUAcgBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEoARABOACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgACAAIAAgACAAIAAgACAAIAB8ACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByACAAZgBvAHIAIAB0AGgAZQAgAGMAYQBsAGUAbgBkAGEAcgAgAGQAYQB5AFwAbgBbAE0AbwBuAHQAaABPAGYAZgBzAGUAdABdACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbAC0ANgAuAC4AMwBdACAAfAAgAFEAdQBhAHIAdABlAHIAIABtAG8AbgB0AGgAIABvAGYAZgBzAGUAdAAgAGYAcgBvAG0AIABKAGEAbgB1AGEAcgB5AC4AXABuAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0AIAB8ACAAcwB3AGkAdABjAGgAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAQwBhAGwAYwB1AGwAYQB0AGUAIABmAG8AcgAgAHQAaABlACAASgB1AGwAaQBhAG4AIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuACAARABlAGYAYQB1AGwAdAAgAGkAcwAgAEcAcgBlAGcAbwByAGkAYQBuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEoARABOAF8AVABPAF8AUQBVAEEAUgBUAEUAUgBfAEQAQQBUAEUAIAA9ACAATABBAE0AQgBEAEEAKABKAEQATgAsACAAWwBNAG8AbgB0AGgATwBmAGYAcwBlAHQAXQAsACAAWwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAsAFwAbgAgACAAIAAgAEkARgAoAEoARABOACAAPQAgAFwAIgBcACIALAAgAHsAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgB9ACwAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEoARABOACkAKQAsACAAewAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AbwBuAHQAaABPAGYAZgBzAGUAdAAsACAAUgBPAFUATgBEACgATgAoAE0AbwBuAHQAaABPAGYAZgBzAGUAdAApACwAIAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKAAoAF8AbQBvAG4AdABoAE8AZgBmAHMAZQB0ACAAPAAgAC0ANgApACAAKwAgACgAXwBtAG8AbgB0AGgATwBmAGYAcwBlAHQAIAA+ACAAMwApACwAIAB7ACMATgBVAE0AIQAsACAAIwBOAFUATQAhACwAIAAjAE4AVQBNACEALAAgACMATgBVAE0AIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGoAZABuACwAIABJAE4AVAAoAEoARABOACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBjAGEAbABEAGEAdABlACwAIABKAEQATgBfAFQATwBfAEMAQQBMAEUATgBEAEEAUgBfAEQAQQBUAEUAKABfAGoAZABuACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaABpAGYAdABNAG8AbgB0AGgALAAgAEkATgBEAEUAWAAoAF8AYwBhAGwARABhAHQAZQAsACAAMQAsACAAMgApACAALQAgADEAIAAtACAAXwBtAG8AbgB0AGgATwBmAGYAcwBlAHQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBmAGkAcwBjAGEAbABZAGUAYQByACwAIABJAE4ARABFAFgAKABfAGMAYQBsAEQAYQB0AGUALAAgADEALAAgADEAKQAgACsAIABJAE4AVAAoAF8AcwBoAGkAZgB0AE0AbwBuAHQAaAAgAC8AIAAxADIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHoAZQByAG8AQgBhAHMAZQBkAEYAaQBzAGMAYQBsAE0AbwBuAHQAaAAsACAATQBPAEQAKABfAHMAaABpAGYAdABNAG8AbgB0AGgALAAgADEAMgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcQB1AGEAcgB0AGUAcgAsACAASQBOAFQAKABfAHoAZQByAG8AQgBhAHMAZQBkAEYAaQBzAGMAYQBsAE0AbwBuAHQAaAAgAC8AIAAzACkAIAArACAAMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGoAZABuAEYAaQByAHMAdABEAGEAeQBRAHUAYQByAHQAZQByACwAIABRAFUAQQBSAFQARQBSAF8ARABBAFQARQBfAFQATwBfAEoARABOACgAXwBmAGkAcwBjAGEAbABZAGUAYQByACwAIABfAHEAdQBhAHIAdABlAHIALAAgADEALAAgAF8AbQBvAG4AdABoAE8AZgBmAHMAZQB0ACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAYQB5AE8AZgBRAHUAYQByAHQAZQByACwAIABfAGoAZABuACAALQAgAF8AagBkAG4ARgBpAHIAcwB0AEQAYQB5AFEAdQBhAHIAdABlAHIAIAArACAAMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAYQB5AHMASQBuAFEAdQBhAHIAdABlAHIALAAgAEQAQQBZAFMAXwBJAE4AXwBRAFUAQQBSAFQARQBSACgAXwBxAHUAYQByAHQAZQByACwAIABfAGYAaQBzAGMAYQBsAFkAZQBhAHIALAAgAF8AbQBvAG4AdABoAE8AZgBmAHMAZQB0ACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZgBpAHMAYwBhAGwAWQBlAGEAcgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcQB1AGEAcgB0AGUAcgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkATwBmAFEAdQBhAHIAdABlAHIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAYQB5AHMASQBuAFEAdQBhAHIAdABlAHIAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAFwAbgBcAG4AXABuAFwAbgBcAG4AXABuAFwAbgBcAG4ALwAqACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwBcAG4AIwAgAEQAQQBUAEUAIABBAE4ARAAgAFQASQBNAEUAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACoALwBcAG4AXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBKAEQATgBfAFUAVABDAF8AVABPAF8ASgBEAEEAVABFAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAHQAaABlACAASgB1AGwAaQBhAG4AIABEAGEAdABlACAAZwBpAHYAZQBuACAAYQBuACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByACAAYQBuAGQAIAB0AGkAbQBlACAAbwBmACAAZABhAHkAIABpAG4AIABVAFQAQwAuAFwAbgBOAG8AdABlACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMAIABhAHIAZQAgAGEAbAB3AGEAeQBzACAAaQBuACAAVQBUAEMALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIABKAHUAbABpAGEAbgAgAEQAYQB0AGUAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBKAEQATgAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAIAAgACAAIAAgACAAIAB8ACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByAC4AXABuAFsAVABpAG0AZQBVAFQAQwBdACAAfAAgAGQAZQBjAGkAbQBhAGwAIABbADAALgAuADEAKQAgAHwAIABUAGkAbQBlACAAbwBmACAAZABhAHkAIABpAG4AIABVAFQAQwAgAGEAcwAgAGQAZQBjAGkAbQBhAGwAIABmAHIAYQBjAHQAaQBvAG4AIABvAHIAIABFAHgAYwBlAGwAIABEAGEAdABlAC8AVABpAG0AZQAgAHQAeQBwAGUALgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAEMAYQByAHIAaQBlAHMAIABpAGYAIAByAGEAbgBnAGUAIABpAHMAIABlAHgAYwBlAGUAZABlAGQALgBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ASgBEAE4AXwBVAFQAQwBfAFQATwBfAEoARABBAFQARQAgAD0AIABMAEEATQBCAEQAQQAoAEoARABOACwAIABbAFQAaQBtAGUAVQBUAEMAXQAsAFwAbgAgACAAIAAgAEkARgAoACgASgBEAE4AIAA9ACAAXAAiAFwAIgApACAAKgAgACgAVABpAG0AZQBVAFQAQwAgAD0AIABcACIAXAAiACkALAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgASgBEAE4AKQApACAAKwAgACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABUAGkAbQBlAFUAVABDACkAKQAgACoAIAAoAFQAaQBtAGUAVQBUAEMAIAA8AD4AIABcACIAXAAiACkAKQAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgATQBPAEQAKABKAEQATgAsACAAMQApACAAPgAgADAALAAgAHsAIwBOAFUATQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABKAEQATgAgAC0AIAAwAC4ANQAgACsAIABOACgAVABpAG0AZQBVAFQAQwApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBKAEQATgBfAEwATwBDAEEATABfAFQATwBfAEoARABBAFQARQBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAEoAdQBsAGkAYQBuACAARABhAHQAZQAgAGcAaQB2AGUAbgAgAGEAIABsAG8AYwBhAGwAIABKAHUAbABpAGEAbgAgAEQAYQB5ACAATgB1AG0AYgBlAHIAIABhAG4AZAAgAGwAbwBjAGEAbAAgAHQAaQBtAGUAIABvAGYAIABkAGEAeQAgAHcAaQB0AGgAIAB0AGkAbQBlACAAegBvAG4AZQAgAG8AZgBmAHMAZQB0ACAAaQBuAFwAbgBtAGkAbgB1AHQAZQBzAC4AIABOAG8AdABlACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMAIABhAHIAZQAgAGEAbAB3AGEAeQBzACAAaQBuACAAVQBUAEMALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIABKAHUAbABpAGEAbgAgAEQAYQB0AGUAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBMAG8AYwBhAGwASgBEAE4AIAAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAAgACAAIAAgACAAIAAgAHwAIABMAG8AYwBhAGwAIABKAHUAbABpAGEAbgAgAEQAYQB5ACAATgB1AG0AYgBlAHIALgBcAG4ATABvAGMAYQBsAFQAaQBtAGUAIAAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAWwAwAC4ALgAxACkAIAB8ACAATABvAGMAYQBsACAAdABpAG0AZQAgAG8AZgAgAGQAYQB5ACAAYQBzACAAZABlAGMAaQBtAGEAbAAgAGYAcgBhAGMAdABpAG8AbgAgAG8AcgAgAEUAeABjAGUAbAAgAEQAYQB0AGUALwBUAGkAbQBlACAAdAB5AHAAZQAuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABDAGEAcgByAGkAZQBzACAAaQBzACAAcgBhAG4AZwBlACAAaQBzACAAZQB4AGMAZQBlAGQAZQBkAC4AXABuAFsAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0AF0AIAB8ACAAZABlAGMAaQBtAGEAbAAgACAAIAAgACAAIAAgACAAfAAgAFQAaQBtAGUAIAB6AG8AbgBlACAAbwBmAGYAcwBlAHQAIABpAG4AIABtAGkAbgB1AHQAZQBzACAAZgByAG8AbQAgAFUAVABDAC4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAWwAtADkAMAAwAC4ALgA5ADAAMABdACAAIAAgACAAfAAgAEEAcwBzAHUAbQBlAGQAIAB0AG8AIABiAGUAIABVAFQAQwAgAGkAZgAgAG8AbQBtAGkAdAB0AGUAZAAuAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBKAEQATgBfAEwATwBDAEEATABfAFQATwBfAEoARABBAFQARQAgAD0AIABMAEEATQBCAEQAQQAoAEwAbwBjAGEAbABKAEQATgAsACAATABvAGMAYQBsAFQAaQBtAGUALAAgAFsAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0AF0ALABcAG4AIAAgACAAIABJAEYAKAAoAEwAbwBjAGEAbABKAEQATgAgAD0AIABcACIAXAAiACkAIAAqACAAKABMAG8AYwBhAGwAVABpAG0AZQAgAD0AIABcACIAXAAiACkALAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgATABvAGMAYQBsAEoARABOACkAKQAgACsAIAAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgATABvAGMAYQBsAFQAaQBtAGUAKQApACAAKgAgACgATABvAGMAYQBsAFQAaQBtAGUAIAA8AD4AIABcACIAXAAiACkAKQAgACsAIAAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0ACkAKQAgACoAIAAoAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdAAgADwAPgAgAFwAIgBcACIAKQApACwAIAB7ACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABNAE8ARAAoAEwAbwBjAGEAbABKAEQATgAsACAAMQApACAAPgAgADAALAAgAHsAIwBOAFUATQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AHoAbwAsACAATgAoAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdAApACAALwAgADEANAA0ADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAEEAQgBTACgAXwB0AHoAbwApACAAPgAgADAALgA2ADIANQAsACAAewAjAE4AVQBNACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAG8AYwBhAGwASgBEAE4AIAAtACAAMAAuADUAIAArACAATgAoAEwAbwBjAGEAbABUAGkAbQBlACkAIAAtACAAXwB0AHoAbwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEoARABBAFQARQBfAFQATwBfAEoARABOAF8AVQBUAEMAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIABKAHUAbABpAGEAbgAgAEQAYQB5ACAATgB1AG0AYgBlAHIAIABhAG4AZAAgAHQAaQBtAGUAIABvAGYAIABkAGEAeQAgAGkAbgAgAFUAVABDACAAbwBmACAAYQAgAGcAaQB2AGUAbgAgAEoAdQBsAGkAYQBuACAARABhAHQAZQAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABpAG4AdABlAGcAZQByACAAIAAgACAAIAAgACAAIAB8ACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByAFwAbgAgADIAIAB8ACAAZABlAGMAaQBtAGEAbAAgAFsAMAAuAC4AMQApACAAfAAgAFQAaQBtAGUAIABvAGYAIABkAGEAeQAgAGkAbgAgAFUAVABDAC4AIABEAGUAYwBpAG0AYQBsACAAZgByAGEAYwB0AGkAbwBuACwAIABpAG0AcABsAGkAYwBpAHQAbAB5ACAAYwBvAG4AdgBlAHIAdABzACAAdABvACAARQB4AGMAZQBsACAARABhAHQAZQAvAFQAaQBtAGUAIAB0AHkAcABlAC4AXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBKAEQAYQB0AGUAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIABKAHUAbABpAGEAbgAgAEQAYQB0AGUAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEoARABBAFQARQBfAFQATwBfAEoARABOAF8AVQBUAEMAIAA9ACAATABBAE0AQgBEAEEAKABKAEQAYQB0AGUALABcAG4AIAAgACAAIABJAEYAKABKAEQAYQB0AGUAIAA9ACAAXAAiAFwAIgAsACAAewBcACIAXAAiACwAIABcACIAXAAiAH0ALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgASgBEAGEAdABlACkAKQAsACAAewAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaABpAGYAdABVAFQAQwAsACAASgBEAGEAdABlACAAKwAgADAALgA1ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBKAEQATgAsACAASQBOAFQAKABfAHMAaABpAGYAdABVAFQAQwApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBVAFQAQwAsACAAXwBzAGgAaQBmAHQAVQBUAEMAIAAtACAAXwBKAEQATgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXwBKAEQATgAsACAAXwBVAFQAQwApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ASgBEAEEAVABFAF8AVABPAF8ASgBEAE4AXwBMAE8AQwBBAEwAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIABsAG8AYwBhAGwAIABKAHUAbABpAGEAbgAgAEQAYQB5ACAATgB1AG0AYgBlAHIAIABhAG4AZAAgAHQAaQBtAGUAIABvAGYAIABkAGEAeQAgAG8AZgAgAGEAIABnAGkAdgBlAG4AIABKAHUAbABpAGEAbgAgAEQAYQB0AGUALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAaQBuAHQAZQBnAGUAcgAgACAAIAAgACAAIAAgACAAfAAgAEwAbwBjAGEAbAAgAEoAdQBsAGkAYQBuACAARABhAHkAIABOAHUAbQBiAGUAcgBcAG4AIAAyACAAfAAgAGQAZQBjAGkAbQBhAGwAIABbADAALgAuADEAKQAgAHwAIABMAG8AYwBhAGwAIAB0AGkAbQBlACAAbwBmACAAZABhAHkALgAgAEQAZQBjAGkAbQBhAGwAIABmAHIAYQBjAHQAaQBvAG4ALAAgAGkAbQBwAGwAaQBjAGkAdABsAHkAIABjAG8AbgB2AGUAcgB0AHMAIAB0AG8AIABFAHgAYwBlAGwAIABEAGEAdABlAC8AVABpAG0AZQAgAHQAeQBwAGUALgBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEoARABhAHQAZQAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgACAAIAAgACAAfAAgAEoAdQBsAGkAYQBuACAARABhAHQAZQBcAG4AWwBUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQAXQAgAHwAIABkAGUAYwBpAG0AYQBsACAAIAAgACAAIAB8ACAAVABpAG0AZQAgAHoAbwBuAGUAIABvAGYAZgBzAGUAdAAgAGkAbgAgAG0AaQBuAHUAdABlAHMAIABmAHIAbwBtACAAVQBUAEMALgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABbAC0AOQAwADAALgAuADkAMAAwAF0AIAB8ACAAQQBzAHMAdQBtAGUAZAAgAHQAbwAgAGIAZQAgAFUAVABDACAAaQBmACAAbwBtAG0AaQB0AHQAZQBkAC4AXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEoARABBAFQARQBfAFQATwBfAEoARABOAF8ATABPAEMAQQBMACAAPQAgAEwAQQBNAEIARABBACgASgBEAGEAdABlACwAIABbAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdABdACwAXABuACAAIAAgACAASQBGACgASgBEAGEAdABlACAAPQAgAFwAIgBcACIALAAgAHsAXAAiAFwAIgAsACAAXAAiAFwAIgB9ACwAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEoARABhAHQAZQApACkAIAArACAAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdAApACkAIAAqACAAKABUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQAIAA8AD4AIABcACIAXAAiACkAKQAsACAAewAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBvACwAIABOACgAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0ACkAIAAvACAAMQA0ADQAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAEEAQgBTACgAXwB0AHoAbwApACAAPgAgADAALgA2ADIANQAsACAAewAjAE4AVQBNACEALAAgACMATgBVAE0AIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGgAaQBmAHQATABvAGMAYQBsACwAIABKAEQAYQB0AGUAIAArACAAMAAuADUAIAArACAAXwB0AHoAbwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGwAbwBjAGEAbABKAEQATgAsACAASQBOAFQAKABfAHMAaABpAGYAdABMAG8AYwBhAGwAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGwAbwBjAGEAbABUAGkAbQBlACwAIABfAHMAaABpAGYAdABMAG8AYwBhAGwAIAAtACAAXwBsAG8AYwBhAGwASgBEAE4ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABfAGwAbwBjAGEAbABKAEQATgAsACAAXwBsAG8AYwBhAGwAVABpAG0AZQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ASgBVAEwASQBBAE4AXwBEAEEAVABFAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAHQAaABlACAASgB1AGwAaQBhAG4AIABEAGEAdABlACAAbwBmACAAdABoAGUAIABwAHIAbwB2AGkAZABlAGQAIABjAGEAbABlAG4AZABhAHIAIABkAGEAdABlACAAYQBuAGQAIAB0AGkAbQBlACAAbwBmACAAZABhAHkALgBcAG4ATgBvAHQAZQAgAEoAdQBsAGkAYQBuACAARABhAHQAZQBzACAAYQByAGUAIABhAGwAdwBhAHkAcwAgAGkAbgAgAFUAVABDAC4AXABuAFwAbgBPAHUAdABwAHUAdABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAASgB1AGwAaQBhAG4AIABEAGEAdABlAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AWQBlAGEAcgBDAEUAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAIAAgACAAIAAgACAAIAAgAHwAIABZAGUAYQByACAAaQBuACAAQwBvAG0AbQBvAG4AIABFAHIAYQAuACAATgBvAHQAZQAgAHQAaABhAHQAIAAxACAAQgBDACAAPQAgADAAIABDAEUALAAgADIAIABCAEMAIAA9ACAALQAxACAAQwBFAFwAbgBNAG8AbgB0AGgAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADEALgAuADEAMgBdACAAfAAgAE0AbwBuAHQAaABcAG4ARABhAHkAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAWwAxAC4ALgAzADEAXQAgAHwAIABEAGEAeQBcAG4AVABpAG0AZQAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAWwAwAC4ALgAxACkAIAAgAHwAIABUAGkAbQBlACAAbwBmACAAZABhAHkAIABhAHMAIABkAGUAYwBpAG0AYQBsACAAZgByAGEAYwB0AGkAbwBuACAAbwByACAARQB4AGMAZQBsACAARABhAHQAZQAvAFQAaQBtAGUAIAB0AHkAcABlAC4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAQwBhAHIAcgBpAGUAcwAgAGkAZgAgAHIAYQBuAGcAZQAgAGkAcwAgAGUAeABjAGUAZQBkAGUAZAAuAFwAbgBbAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdABdACAAfAAgAGQAZQBjAGkAbQBhAGwAIAAgACAAIAAgACAAIAAgACAAfAAgAFQAaQBtAGUAIAB6AG8AbgBlACAAbwBmAGYAcwBlAHQAIABpAG4AIABtAGkAbgB1AHQAZQBzACAAZgByAG8AbQAgAFUAVABDAC4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAWwAtADkAMAAwAC4ALgA5ADAAMABdACAAIAAgACAAIAB8ACAAQQBzAHMAdQBtAGUAZAAgAHQAbwAgAGIAZQAgAFUAVABDACAAaQBmACAAbwBtAG0AaQB0AHQAZQBkAC4AXABuAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0AIAB8ACAAcwB3AGkAdABjAGgAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAQwBhAGwAYwB1AGwAYQB0AGUAIABpAG4AIAB0AGgAZQAgAEoAdQBsAGkAYQBuACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgAgAEQAZQBmAGEAdQBsAHQAIABpAHMAIABHAHIAZQBnAG8AcgBpAGEAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBKAFUATABJAEEATgBfAEQAQQBUAEUAIAA9ACAATABBAE0AQgBEAEEAKABZAGUAYQByAEMARQAsACAATQBvAG4AdABoACwAIABEAGEAeQAsACAAVABpAG0AZQAsACAAWwBUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQAXQAsACAAWwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAsAFwAbgAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAF8AVgBBAEwASQBEAF8ARABBAFQARQAoAFkAZQBhAHIAQwBFACwAIABNAG8AbgB0AGgALAAgAEQAYQB5ACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQApACwAIAB7ACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgATQBPAEQAKABEAGEAeQAsACAAMQApACAAPgAgADAALAAgAHsAIwBOAFUATQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBvACwAIABOACgAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABBAEIAUwAoAF8AdAB6AG8AKQAgAD4AIAA5ADAAMAAsACAAewAjAE4AVQBNACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkAUABhAHIAdAAsACAASQBOAFQAKABOACgAVABpAG0AZQApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AG8AZAAsACAATgAoAFQAaQBtAGUAKQAgAC0AIABfAGQAYQB5AFAAYQByAHQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBqAGQAbgAsACAAXwBkAGEAeQBQAGEAcgB0ACAAKwAgAEoAVQBMAEkAQQBOAF8ARABBAFkAXwBOAFUATQBCAEUAUgAoAFkAZQBhAHIAQwBFACwAIABNAG8AbgB0AGgALAAgAEQAYQB5ACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABKAEQATgBfAEwATwBDAEEATABfAFQATwBfAEoARABBAFQARQAoAF8AagBkAG4ALAAgAF8AdABvAGQALAAgAF8AdAB6AG8AKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEMAQQBMAEUATgBEAEEAUgBfAEYAUgBPAE0AXwBKAEQAQQBUAEUAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIABjAGEAbABlAG4AZABhAHIAIABkAGEAdABlACAAYQBuAGQAIABsAG8AYwBhAGwAIAB0AGkAbQBlACAAbwBmACAAZABhAHkAIABmAG8AcgAgAGEAIABnAGkAdgBlAG4AIABKAHUAbABpAGEAbgAgAEQAYQB0AGUAIABhAG4AZAAgAHQAaQBtAGUAIAB6AG8AbgBlACAAbwBmAGYAcwBlAHQALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAaQBuAHQAZQBnAGUAcgAgACAAIAAgACAAIAAgACAAIAB8ACAAWQBlAGEAcgBDAEUAXABuACAAMgAgAHwAIABpAG4AdABlAGcAZQByACAAWwAxAC4ALgAxADIAXQAgAHwAIABNAG8AbgB0AGgAXABuACAAMwAgAHwAIABpAG4AdABlAGcAZQByACAAWwAxAC4ALgAzADEAXQAgAHwAIABEAGEAeQBcAG4AIAA0ACAAfAAgAGQAZQBjAGkAbQBhAGwAIABbADAALgAuADEAKQAgACAAfAAgAEwAbwBjAGEAbAAgAHQAaQBtAGUAIABvAGYAIABkAGEAeQAuACAARABlAGMAaQBtAGEAbAAgAGYAcgBhAGMAdABpAG8AbgAsACAAaQBtAHAAbABpAGMAaQB0AGwAeQAgAGMAbwBuAHYAZQByAHQAcwAgAHQAbwAgAEUAeABjAGUAbAAgAEQAYQB0AGUALwBUAGkAbQBlACAAdAB5AHAAZQAuAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ASgBEAGEAdABlACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAIAAgACAAIAB8ACAASgB1AGwAaQBhAG4AIABEAGEAdABlAC4AIABOAG8AdABlACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMAIABhAHIAZQAgAGEAbAB3AGEAeQBzACAAaQBuACAAVQBUAEMALgBcAG4AWwBUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQAXQAgAHwAIABkAGUAYwBpAG0AYQBsACAAIAAgACAAIAB8ACAAVABpAG0AZQAgAHoAbwBuAGUAIABvAGYAZgBzAGUAdAAgAGkAbgAgAG0AaQBuAHUAdABlAHMAIABmAHIAbwBtACAAVQBUAEMALgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABbAC0AOQAwADAALgAuADkAMAAwAF0AIAB8ACAAQQBzAHMAdQBtAGUAZAAgAHQAbwAgAGIAZQAgAFUAVABDACAAaQBmACAAbwBtAG0AaQB0AHQAZQBkAC4AXABuAFsAUAByAGUAYwBpAHMAaQBvAG4AXQAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgACAAIAAgACAAfAAgAFMAZQBsAGUAYwB0ACAAcAByAGUAYwBpAHMAaQBvAG4AIABsAGUAdgBlAGwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAwACAALQAgAEYAbABvAGEAdABpAG4AZwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADEAIAAtACAARABhAHkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAyACAALQAgAEgAbwB1AHIAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAzACAALQAgAE0AaQBuAHUAdABlAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAANAAgAC0AIABTAGUAYwBvAG4AZABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADUAIAAtACAATQBpAGwAbABpAHMAZQBjAG8AbgBkAFwAbgBbAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACAAfAAgAHMAdwBpAHQAYwBoACAAIAAgACAAIAAgAHwAIABDAGEAbABjAHUAbABhAHQAZQAgAGkAbgAgAHQAaABlACAASgB1AGwAaQBhAG4AIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuACAARABlAGYAYQB1AGwAdAAgAGkAcwAgAEcAcgBlAGcAbwByAGkAYQBuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBDAEEATABFAE4ARABBAFIAXwBGAFIATwBNAF8ASgBEAEEAVABFACAAPQAgAEwAQQBNAEIARABBACgASgBEAGEAdABlACwAIABbAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdABdACwAIABbAFAAcgBlAGMAaQBzAGkAbwBuAF0ALAAgAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0ALABcAG4AIAAgACAAIABJAEYAKABKAEQAYQB0AGUAIAA9ACAAXAAiAFwAIgAsACAAewBcACIAXAAiACwAIABcACIAXAAiACwAIABcACIAXAAiACwAIABcACIAXAAiAH0ALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgASgBEAGEAdABlACkAKQAsACAAewAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGoAZABuAEwAbwBjAGEAbAAsACAASgBEAEEAVABFAF8AVABPAF8ASgBEAE4AXwBMAE8AQwBBAEwAKABKAEQAYQB0AGUALAAgAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgASQBTAEUAUgBSAE8AUgAoAEkATgBEAEUAWAAoAF8AagBkAG4ATABvAGMAYQBsACwAIAAxACwAIAAxACkAKQAsACAAewAjAE4AVQBNACEALAAgACMATgBVAE0AIQAsACAAIwBOAFUATQAhACwAIAAjAE4AVQBNACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBwAHIAZQBjAGkAcwBpAG8AbgAsACAATgAoAFAAcgBlAGMAaQBzAGkAbwBuACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBsAG8AYwBhAGwAVABpAG0AZQAsACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHAAcgBlAGMAaQBzAGkAbwBuACAAPAA9ACAAMAAsACAASQBOAEQARQBYACgAXwBqAGQAbgBMAG8AYwBhAGwALAAgADEALAAgADIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcAByAGUAYwBpAHMAaQBvAG4AIAA9ACAAMQAsACAAUgBPAFUATgBEACgASQBOAEQARQBYACgAXwBqAGQAbgBMAG8AYwBhAGwALAAgADEALAAgADIAKQAsACAAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBwAHIAZQBjAGkAcwBpAG8AbgAgAD0AIAAyACwAIABSAE8AVQBOAEQAKABJAE4ARABFAFgAKABfAGoAZABuAEwAbwBjAGEAbAAsACAAMQAsACAAMgApACAAKgAgADIANAAsACAAMAApACAALwAgADIANAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcAByAGUAYwBpAHMAaQBvAG4AIAA9ACAAMwAsACAAUgBPAFUATgBEACgASQBOAEQARQBYACgAXwBqAGQAbgBMAG8AYwBhAGwALAAgADEALAAgADIAKQAgACoAIAAxADQANAAwACwAIAAwACkAIAAvACAAMQA0ADQAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcAByAGUAYwBpAHMAaQBvAG4AIAA9ACAANAAsACAAUgBPAFUATgBEACgASQBOAEQARQBYACgAXwBqAGQAbgBMAG8AYwBhAGwALAAgADEALAAgADIAKQAgACoAIAA4ADYANAAwADAALAAgADAAKQAgAC8AIAA4ADYANAAwADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAIABSAE8AVQBOAEQAKABJAE4ARABFAFgAKABfAGoAZABuAEwAbwBjAGEAbAAsACAAMQAsACAAMgApACAAKgAgADgANgA0ADAAMAAwADAAMAAsACAAMAApACAALwAgADgANgA0ADAAMAAwADAAMABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHIATABvAGMAYQBsAFQAaQBtAGUALAAgAE0ATwBEACgAXwBsAG8AYwBhAGwAVABpAG0AZQAsACAAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcgBKAEQATgAsACAASQBOAEQARQBYACgAXwBqAGQAbgBMAG8AYwBhAGwALAAgADEALAAgADEAKQAgACsAIABJAE4AVAAoAF8AbABvAGMAYQBsAFQAaQBtAGUAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGwAbwBjAGEAbABEAGEAdABlACwAIABKAEQATgBfAFQATwBfAEMAQQBMAEUATgBEAEEAUgBfAEQAQQBUAEUAKABfAHIASgBEAE4ALAAgAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXwBsAG8AYwBhAGwARABhAHQAZQAsACAAXwByAEwAbwBjAGEAbABUAGkAbQBlACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBUAEkATQBFAF8ARABFAEMASQBNAEEATABfAFQATwBfAEgATQBTAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAHQAaABlACAAMgA0ACAAaABvAHUAcgAgAHQAaQBtAGUAawBlAGUAcABpAG4AZwAgAHIAZQBwAHIAZQBzAGUAbgB0AGEAdABpAG8AbgAgAG8AZgAgAGEAIABkAGUAYwBpAG0AYQBsACAAdABpAG0AZQAgAHYAYQBsAHUAZQAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABpAG4AdABlAGcAZQByACAAWwAtADEALAAwACwAMQBdACAAfAAgAFMAaQBnAG4AXABuACAAMgAgAHwAIABpAG4AdABlAGcAZQByACAAWwAwAC4ALgBdACAAIAAgACAAfAAgAEgAbwB1AHIAcwBcAG4AIAAzACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADAALgAuADUAOQBdACAAIAB8ACAATQBpAG4AdQB0AGUAcwBcAG4AIAA0ACAAfAAgAGQAZQBjAGkAbQBhAGwAIABbADAALgAuADYAMAApACAAIAB8ACAAUwBlAGMAbwBuAGQAcwBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFQAaQBtAGUAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIABUAGkAbQBlACAAYQBzACAAZgByAGEAYwB0AGkAbwBuACAAbwBmACAAYQAgAGQAYQB5ACAAKAAyADQAIABoAG8AdQByAHMAKQAuACAASQBtAHAAbABpAGMAaQB0AGwAeQAgAGMAbwBuAHYAZQByAHQAcwAgAGYAcgBvAG0AIABFAHgAYwBlAGwAIABEAGEAdABlAC8AVABpAG0AZQAgAHQAeQBwAGUAIABmAG8AcgBcAG4AIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgAG4AbwBuAC0AbgBlAGcAYQB0AGkAdgBlACAAdgBhAGwAdQBlAHMALgAgAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBUAEkATQBFAF8ARABFAEMASQBNAEEATABfAFQATwBfAEgATQBTACAAPQAgAEwAQQBNAEIARABBACgAVABpAG0AZQAsAFwAbgAgACAAIAAgAEkARgAoAFQAaQBtAGUAIAA9ACAAXAAiAFwAIgAsACAAewBcACIAXAAiACwAIABcACIAXAAiACwAIABcACIAXAAiACwAIABcACIAXAAiAH0ALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgAVABpAG0AZQApACkALAAgAHsAIwBWAEEATABVAEUAIQAsACAAIwBWAEEATABVAEUAIQAsACAAIwBWAEEATABVAEUAIQAsACAAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAcgBvAHUAbgBkACAAdABvACAAbQBpAGwAbABpAHMAZQBjAG8AbgBkAHMALAAgAHMAYwBhAGwAZQAgAHQAbwAgAHMAZQBjAG8AbgBkAHMAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGUAYwBvAG4AZABzACwAIABSAE8AVQBOAEQAKABUAGkAbQBlACAAKgAgADgANgA0ADAAMAAsACAAMwApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBzAGUAYwBvAG4AZABzACAAPQAgADAALAAgAHsAMAAsACAAMAAsACAAMAAsACAAMAB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaQBnAG4ALAAgAFMASQBHAE4AKABfAHMAZQBjAG8AbgBkAHMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGEAYgBzAFMAZQBjAG8AbgBkAHMALAAgAEEAQgBTACgAXwBzAGUAYwBvAG4AZABzACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGUAYwBvAG4AZABQAGEAcgB0ACwAIABNAE8ARAAoAF8AYQBiAHMAUwBlAGMAbwBuAGQAcwAsACAANgAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBtAGkAbgB1AHQAZQBzACwAIABJAE4AVAAoACgAXwBhAGIAcwBTAGUAYwBvAG4AZABzACAALQAgAF8AcwBlAGMAbwBuAGQAUABhAHIAdAApACAALwAgADYAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbQBpAG4AdQB0AGUAUABhAHIAdAAsACAATQBPAEQAKABfAG0AaQBuAHUAdABlAHMALAAgADYAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AaABvAHUAcgBQAGEAcgB0ACwAIABJAE4AVAAoACgAXwBtAGkAbgB1AHQAZQBzACAALQAgAF8AbQBpAG4AdQB0AGUAUABhAHIAdAApACAALwAgADYAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGkAZwBuACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBoAG8AdQByAFAAYQByAHQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AaQBuAHUAdABlAFAAYQByAHQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAZQBjAG8AbgBkAFAAYQByAHQAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBIAE0AUwBfAFQATwBfAFQASQBNAEUAXwBEAEUAQwBJAE0AQQBMAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAGEAIABkAGUAYwBpAG0AYQBsACAAdABpAG0AZQAgAGEAcwAgAGEAIABmAHIAYQBjAHQAaQBvAG4AIABvAGYAIABhACAAZABhAHkAIABmAHIAbwBtACAAYQAgADIANAAgAGgAbwB1AHIAIAB0AGkAbQBlAGsAZQBlAHAAaQBuAGcAIAB2AGEAbAB1AGUAIABvAGYAIAB0AGkAbQBlAC4AXABuAFwAbgBPAHUAdABwAHUAdABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAASQBtAHAAbABpAGMAaQB0AGwAeQAgAGMAbwBuAHYAZQByAHQAcwAgAHQAbwAgAEUAeABjAGUAbAAgAEQAYQB0AGUALwBUAGkAbQBlACAAdAB5AHAAZQAgAGYAbwByACAAbgBvAG4ALQBuAGUAZwBhAHQAaQB2AGUAIAB2AGEAbAB1AGUAcwAuAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AUwBpAGcAbgAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAWwAtADEALAAwACwAMQBdACAAfABcAG4ASABvAHUAcgBzACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAWwAwAC4ALgBdACAAIAAgACAAfABcAG4ATQBpAG4AdQB0AGUAcwAgAHwAIABpAG4AdABlAGcAZQByACAAWwAwAC4ALgA1ADkAXQAgACAAfABcAG4AUwBlAGMAbwBuAGQAcwAgAHwAIABkAGUAYwBpAG0AYQBsACAAWwAwAC4ALgA2ADAAKQAgACAAfABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ASABNAFMAXwBUAE8AXwBUAEkATQBFAF8ARABFAEMASQBNAEEATAAgAD0AIABMAEEATQBCAEQAQQAoAFMAaQBnAG4ALAAgAEgAbwB1AHIAcwAsACAATQBpAG4AdQB0AGUAcwAsACAAUwBlAGMAbwBuAGQAcwAsAFwAbgAgACAAIAAgAEkARgAoACgASABvAHUAcgBzACAAPQAgAFwAIgBcACIAKQAgACoAIAAoAE0AaQBuAHUAdABlAHMAIAA9ACAAXAAiAFwAIgApACAAKgAgACgAUwBlAGMAbwBuAGQAcwAgAD0AIABcACIAXAAiACkALAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABTAGkAZwBuACkAKQAgACoAIAAoAFMAaQBnAG4AIAA8AD4AIABcACIAXAAiACkAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKwAgACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABIAG8AdQByAHMAKQApACAAKgAgACgASABvAHUAcgBzACAAPAA+ACAAXAAiAFwAIgApACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACsAIAAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgATQBpAG4AdQB0AGUAcwApACkAIAAqACAAKABNAGkAbgB1AHQAZQBzACAAPAA+ACAAXAAiAFwAIgApACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACsAIAAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgAUwBlAGMAbwBuAGQAcwApACkAIAAqACAAKABTAGUAYwBvAG4AZABzACAAPAA+ACAAXAAiAFwAIgApACkALAAgAHsAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBoAG8AdQByAHMALAAgAE4AKABIAG8AdQByAHMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbQBpAG4AdQB0AGUAcwAsACAATgAoAE0AaQBuAHUAdABlAHMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBlAGMAbwBuAGQAcwAsACAATgAoAFMAZQBjAG8AbgBkAHMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoACgAXwBoAG8AdQByAHMAIAA9ACAAMAApACAAKgAgACgAXwBtAGkAbgB1AHQAZQBzACAAPQAgADAAKQAgACoAIAAoAF8AcwBlAGMAbwBuAGQAcwAgAD0AIAAwACkALAAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBpAGcAbgAsACAASQBGACgATgAoAFMAaQBnAG4AKQAgADwAIAAwACwAIAAtADEALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaQBnAG4AIAAqACAAKAAoAF8AaABvAHUAcgBzACAALwAgADIANAApACAAKwAgACgAXwBtAGkAbgB1AHQAZQBzACAALwAgADEANAA0ADAAKQAgACsAIAAoAF8AcwBlAGMAbwBuAGQAcwAgAC8AIAA4ADYANAAwADAAKQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AQQBEAEQAXwBUAEkATQBFAFMAUABBAE4AXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIABKAHUAbABpAGEAbgAgAEQAYQB0AGUAIABvAGYAIAB0AGgAZQAgAGEAZABkAGkAdABpAG8AbgAgAG8AZgAgAHQAaABlACAAcAByAG8AdgBpAGQAZQBkACAAYwBhAGwAZQBuAGQAYQByACAAZABhAHQAZQAgAGEAbgBkACAAdABpAG0AZQAgAG8AZgAgAGQAYQB5ACAAYQBuAGQAIABhACAAdABpAG0AZQBzAHAAYQBuACAAYwBvAG0AcABsAGkAYwBhAHQAaQBvAG4ALgBcAG4ATgBvAHQAZQAgAEoAdQBsAGkAYQBuACAARABhAHQAZQBzACAAYQByAGUAIABhAGwAdwBhAHkAcwAgAGkAbgAgAFUAVABDAC4AXABuAFwAbgBPAHUAdABwAHUAdABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAASgB1AGwAaQBhAG4AIABEAGEAdABlAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AWQBlAGEAcgBDAEUAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAIAAgACAAIAAgACAAIAAgAHwAIABZAGUAYQByACAAaQBuACAAQwBvAG0AbQBvAG4AIABFAHIAYQAuACAATgBvAHQAZQAgAHQAaABhAHQAIAAxACAAQgBDACAAPQAgADAAIABDAEUALAAgADIAIABCAEMAIAA9ACAALQAxACAAQwBFAFwAbgBNAG8AbgB0AGgAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADEALgAuADEAMgBdACAAfAAgAE0AbwBuAHQAaABcAG4ARABhAHkAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAWwAxAC4ALgAzADEAXQAgAHwAIABEAGEAeQBcAG4AVABpAG0AZQAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAWwAwAC4ALgAxACkAIAAgAHwAIABMAG8AYwBhAGwAIAB0AGkAbQBlACAAbwBmACAAZABhAHkAIABhAHMAIABkAGUAYwBpAG0AYQBsACAAZgByAGEAYwB0AGkAbwBuACAAbwByACAARQB4AGMAZQBsACAARABhAHQAZQAvAFQAaQBtAGUAIAB0AHkAcABlAC4AXABuAEEAZABkAFkAZQBhAHIAcwAgACAAIAAgACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgACAAIAAgACAAIAAgACAAIAB8ACAAQQBkAGQAIAB5AGUAYQByAHMAIAB0AGkAbQBlAHMAcABhAG4ALgAgAEYAcgBhAGMAdABpAG8AbgBhAGwAIABwAGEAcgB0ACAAYwBhAHIAcgBpAGUAcwAgAHQAbwAgAG0AbwBuAHQAaAAgAGEAbgBkACAAZABhAHkALgBcAG4AQQBkAGQATQBvAG4AdABoAHMAIAAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAIAAgACAAIAAgACAAIAAgAHwAIABBAGQAZAAgAG0AbwBuAHQAaABzACAAdABpAG0AZQBzAHAAYQBuAC4AIABGAHIAYQBjAHQAaQBvAG4AYQBsACAAcABhAHIAdAAgAGMAYQByAHIAaQBlAHMAIAB0AG8AIABkAGEAeQAuAFwAbgBBAGQAZABEAGEAeQBzACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAAgACAAIAAgACAAIAAgACAAfAAgAEEAZABkACAAZABhAHkAcwAgAHQAaQBtAGUAcwBwAGEAbgAuACAARgByAGEAYwB0AGkAbwBuAGEAbAAgAHAAYQByAHQAIABjAGEAcgByAGkAZQBzACAAdABvACAAdABpAG0AZQAuAFwAbgBBAGQAZABUAGkAbQBlACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAAgACAAIAAgACAAIAAgACAAfAAgAEEAZABkACAAdABpAG0AZQBzAHAAYQBuAC4AXABuAFsAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0AF0AIAB8ACAAZABlAGMAaQBtAGEAbAAgACAAIAAgACAAIAAgACAAIAB8ACAAVABpAG0AZQAgAHoAbwBuAGUAIABvAGYAZgBzAGUAdAAgAGkAbgAgAG0AaQBuAHUAdABlAHMAIABmAHIAbwBtACAAVQBUAEMALgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABbAC0AOQAwADAALgAuADkAMAAwAF0AIAAgACAAIAAgAHwAIABBAHMAcwB1AG0AZQBkACAAdABvACAAYgBlACAAVQBUAEMAIABpAGYAIABvAG0AbQBpAHQAdABlAGQALgBcAG4AWwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAgAHwAIABzAHcAaQB0AGMAaAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABDAGEAbABjAHUAbABhAHQAZQAgAGkAbgAgAHQAaABlACAASgB1AGwAaQBhAG4AIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuACAARABlAGYAYQB1AGwAdAAgAGkAcwAgAEcAcgBlAGcAbwByAGkAYQBuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEEARABEAF8AVABJAE0ARQBTAFAAQQBOACAAPQAgAEwAQQBNAEIARABBACgAWQBlAGEAcgBDAEUALAAgAE0AbwBuAHQAaAAsACAARABhAHkALAAgAFQAaQBtAGUALAAgAEEAZABkAFkAZQBhAHIAcwAsACAAQQBkAGQATQBvAG4AdABoAHMALAAgAEEAZABkAEQAYQB5AHMALAAgAEEAZABkAFQAaQBtAGUALAAgAFsAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0AF0ALAAgAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0ALABcAG4AIAAgACAAIABJAEYAKAAoAFkAZQBhAHIAQwBFACAAPQAgAFwAIgBcACIAKQAgACoAIAAoAE0AbwBuAHQAaAAgAD0AIABcACIAXAAiACkAIAAqACAAKABEAGEAeQAgAD0AIABcACIAXAAiACkAIAAqACAAKABUAGkAbQBlACAAPQAgAFwAIgBcACIAKQAsACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABZAGUAYQByAEMARQApACkAIAArACAATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABNAG8AbgB0AGgAKQApACAAKwAgAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgARABhAHkAKQApACwAIAB7ACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBfAFYAQQBMAEkARABfAEQAQQBUAEUAKABZAGUAYQByAEMARQAsACAATQBvAG4AdABoACwAIABEAGEAeQAsACAASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByACkAKQAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABNAE8ARAAoAEQAYQB5ACwAIAAxACkAIAA+ACAAMAAsACAAewAjAE4AVQBNACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AHoAbwAsACAATgAoAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAEEAQgBTACgAXwB0AHoAbwApACAAPgAgADkAMAAwACwAIAB7ACMATgBVAE0AIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYQBkAGQAWQBlAGEAcgBzACwAIABJAE4AVAAoAE4AKABBAGQAZABZAGUAYQByAHMAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGYAQQBkAGQAWQBlAGEAcgBzACwAIABOACgAQQBkAGQAWQBlAGEAcgBzACkAIAAtACAAXwBhAGQAZABZAGUAYQByAHMALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBNAG8AbgB0AGgAcwAsACAATgAoAEEAZABkAE0AbwBuAHQAaABzACkAIAArACAAKABfAGYAQQBkAGQAWQBlAGEAcgBzACAAKgAgADEAMgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGEAZABkAE0AbwBuAHQAaABzACwAIABJAE4AVAAoAF8AcwBNAG8AbgB0AGgAcwApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGYAQQBkAGQATQBvAG4AdABoAHMALAAgAF8AcwBNAG8AbgB0AGgAcwAgAC0AIABfAGEAZABkAE0AbwBuAHQAaABzACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHoATQBvAG4AdABoAHMALAAgAE0AbwBuAHQAaAAgACsAIABfAGEAZABkAE0AbwBuAHQAaABzACAALQAgADEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcgBNAG8AbgB0AGgALAAgAE0ATwBEACgAXwB6AE0AbwBuAHQAaABzACwAIAAxADIAKQAgACsAIAAxACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHIAWQBlAGEAcgAsACAAWQBlAGEAcgBDAEUAIAArACAAXwBhAGQAZABZAGUAYQByAHMAIAArACAASQBOAFQAKABfAHoATQBvAG4AdABoAHMAIAAvACAAMQAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYQB2AGcARABhAHkAcwBNAG8AbgB0AGgALAAgAEkARgAoAE4AKABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsACAAMwAwAC4ANAAzADcANQAsACAAMwAwAC4ANAAzADYAOAA3ADUAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBtAEQAYQB5AHMALAAgAFIATwBVAE4ARAAoAF8AZgBBAGQAZABNAG8AbgB0AGgAcwAgACoAIABfAGEAdgBnAEQAYQB5AHMATQBvAG4AdABoACwAIAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYgBhAHMAZQBKAEQAYQB0AGUALAAgAEoAVQBMAEkAQQBOAF8ARABBAFQARQAoAF8AcgBZAGUAYQByACwAIABfAHIATQBvAG4AdABoACwAIAAxACwAIAAwACwAIABfAHQAegBvACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAgAC0AIAAxACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMARABhAHkAcwAsACAARABhAHkAIAArACAAXwBtAEQAYQB5AHMAIAArACAATgAoAEEAZABkAEQAYQB5AHMAKQAgACsAIABOACgAVABpAG0AZQApACAAKwAgAE4AKABBAGQAZABUAGkAbQBlACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYgBhAHMAZQBKAEQAYQB0AGUAIAArACAAXwBzAEQAYQB5AHMAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFIARQBTAE8ATABWAEUAXwBEAEEAVABFAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAGEAIABjAGEAbABlAG4AZABhAHIAIABkAGEAdABlACAAZgByAG8AbQAgAHAAcgBvAHYAaQBkAGUAZAAgAGQAZQBjAGkAbQBhAGwAIAB5AGUAYQByACwAIABtAG8AbgB0AGgAcwAsACAAZABhAHkAcwAgAGEAbgBkACAAdABpAG0AZQAuAFwAbgBOAG8AdABlACAAbQBvAG4AdABoAHMAIABhAG4AZAAgAGQAYQB5AHMAIABhAHIAZQAgAG4AbwB0ACAAYgBvAHUAbgBkAGUAZAAgAGIAeQAgAHQAaABlACAAYwBhAGwAZQBuAGQAYQByAC4AXABuAFwAbgBPAHUAdABwAHUAdABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAGkAbgB0AGUAZwBlAHIAIAAgACAAIAAgACAAIAAgACAAfAAgAFkAZQBhAHIAQwBFAFwAbgAgADIAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMQAuAC4AMQAyAF0AIAB8ACAATQBvAG4AdABoAFwAbgAgADMAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMQAuAC4AMwAxAF0AIAB8ACAARABhAHkAXABuACAANAAgAHwAIABkAGUAYwBpAG0AYQBsACAAWwAwAC4ALgAxACkAXQAgAHwAIABMAG8AYwBhAGwAIAB0AGkAbQBlACAAbwBmACAAZABhAHkALgAgAEQAZQBjAGkAbQBhAGwAIABmAHIAYQBjAHQAaQBvAG4ALAAgAGkAbQBwAGwAaQBjAGkAdABsAHkAIABjAG8AbgB2AGUAcgB0AHMAIAB0AG8AIABFAHgAYwBlAGwAIABEAGEAdABlAC8AVABpAG0AZQAgAHQAeQBwAGUALgBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFkAZQBhAHIAQwBFACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIABZAGUAYQByACAAaQBuACAAQwBvAG0AbQBvAG4AIABFAHIAYQAuACAATgBvAHQAZQAgAHQAaABhAHQAIAAxACAAQgBDACAAPQAgADAAIABDAEUALAAgADIAIABCAEMAIAA9ACAALQAxACAAQwBFAFwAbgBNAG8AbgB0AGgAcwAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAATQBvAG4AdABoAHMAXABuAEQAYQB5AHMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIABEAGEAeQBzAFwAbgBUAGkAbQBlACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAATABvAGMAYQBsACAAdABpAG0AZQAgAG8AZgAgAGQAYQB5ACAAYQBzACAAZABlAGMAaQBtAGEAbAAgAGYAcgBhAGMAdABpAG8AbgAgAG8AcgAgAEUAeABjAGUAbAAgAEQAYQB0AGUALwBUAGkAbQBlACAAdAB5AHAAZQAuAFwAbgBbAFAAcgBlAGMAaQBzAGkAbwBuAF0AIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAAUwBlAGwAZQBjAHQAIABwAHIAZQBjAGkAcwBpAG8AbgAgAGwAZQB2AGUAbABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAwACAALQAgAEYAbABvAGEAdABpAG4AZwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAxACAALQAgAEQAYQB5AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADIAIAAtACAASABvAHUAcgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAzACAALQAgAE0AaQBuAHUAdABlAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADQAIAAtACAAUwBlAGMAbwBuAGQAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAANQAgAC0AIABNAGkAbABsAGkAcwBlAGMAbwBuAGQAXABuAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0AIAB8ACAAcwB3AGkAdABjAGgAIAAgAHwAIABDAGEAbABjAHUAbABhAHQAZQAgAGkAbgAgAHQAaABlACAASgB1AGwAaQBhAG4AIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuACAARABlAGYAYQB1AGwAdAAgAGkAcwAgAEcAcgBlAGcAbwByAGkAYQBuACAAcAByAG8AbABlAHAAdABpAGMAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIABjAGEAbABlAG4AZABhAHIALgBcAG4AXABuAEUAeABhAG0AcABsAGUAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AUgBFAFMATwBMAFYARQBfAEQAQQBUAEUAKAAyADAAMgAzACwAIAAyADUALAAgADMAMwAuADUALAAgAC0AMQAuADUAKQBcAG4AUgBlAHQAdQByAG4AcwA6ACAAewAyADAAMgA1ACwAIAAyACwAIAAxACwAIAAwAH0AXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAFIARQBTAE8ATABWAEUAXwBEAEEAVABFACAAPQAgAEwAQQBNAEIARABBACgAWQBlAGEAcgBDAEUALAAgAE0AbwBuAHQAaABzACwAIABEAGEAeQBzACwAIABUAGkAbQBlACwAIABbAFAAcgBlAGMAaQBzAGkAbwBuAF0ALAAgAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0ALABcAG4AIAAgACAAIABJAEYAKAAoAFkAZQBhAHIAQwBFACAAPQAgAFwAIgBcACIAKQAgACoAIAAoAE0AbwBuAHQAaABzACAAPQAgAFwAIgBcACIAKQAgACoAIAAoAEQAYQB5AHMAIAA9ACAAXAAiAFwAIgApACAAKgAgACgAVABpAG0AZQAgAD0AIABcACIAXAAiACkALAAgAHsAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgB9ACwAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAFkAZQBhAHIAQwBFACkAKQAgACsAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAE0AbwBuAHQAaABzACkAKQAgACsAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEQAYQB5AHMAKQApACwAIAB7ACMAVgBBAEwAVQBFACEALAAgACMAVgBBAEwAVQBFACEALAAgACMAVgBBAEwAVQBFACEALAAgACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AeQBlAGEAcgBDAEUALAAgAEkATgBUACgAWQBlAGEAcgBDAEUAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYQBkAGQAWQBlAGEAcgBzACwAIABZAGUAYQByAEMARQAgAC0AIABfAHkAZQBhAHIAQwBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBhAGQAZABNAG8AbgB0AGgAcwAsACAATQBvAG4AdABoAHMAIAAtACAAMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYQBkAGQARABhAHkAcwAsACAARABhAHkAcwAgAC0AIAAxACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBqAEQAYQB0AGUALAAgAEEARABEAF8AVABJAE0ARQBTAFAAQQBOACgAXwB5AGUAYQByAEMARQAsACAAMQAsACAAMQAsACAAMAAsACAAXwBhAGQAZABZAGUAYQByAHMALAAgAF8AYQBkAGQATQBvAG4AdABoAHMALAAgAF8AYQBkAGQARABhAHkAcwAsACAAVABpAG0AZQAsACAAMAAsACAASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABDAEEATABFAE4ARABBAFIAXwBGAFIATwBNAF8ASgBEAEEAVABFACgAXwBqAEQAYQB0AGUALAAgADAALAAgAFAAcgBlAGMAaQBzAGkAbwBuACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAFwAbgBcAG4AXABuAFwAbgAvACoAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjAFwAbgAjACAARABFAEwAVABBAFMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAKgAvAFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEQARQBMAFQAQQBfAEgATwBVAFIAUwBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHQAaQBtAGUAcwBwAGEAbgAgAGQAaQBmAGYAZQByAGUAbgBjAGUAIABiAGUAdAB3AGUAZQBuACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMAIABpAG4AIABoAG8AdQByAHMALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIABEAGkAZgBmAGUAcgBlAG4AYwBlACAAaQBuACAAaABvAHUAcgBzAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ASgBEAGEAdABlADEAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIABcAG4ASgBEAGEAdABlADIAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ARABFAEwAVABBAF8ASABPAFUAUgBTACAAPQAgAEwAQQBNAEIARABBACgASgBEAGEAdABlADEALAAgAEoARABhAHQAZQAyACwAXABuACAAIAAgACAASQBGACgAKABKAEQAYQB0AGUAMQAgAD0AIABcACIAXAAiACkAIAAqACAAKABKAEQAYQB0AGUAMgAgAD0AIABcACIAXAAiACkALAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgASgBEAGEAdABlADEAKQApACAAKwAgAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgASgBEAGEAdABlADIAKQApACwAIAB7ACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoAEoARABhAHQAZQAyACAALQAgAEoARABhAHQAZQAxACkAIAAqACAAMgA0AFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ARABFAEwAVABBAF8ATQBJAE4AVQBUAEUAUwBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHQAaQBtAGUAcwBwAGEAbgAgAGQAaQBmAGYAZQByAGUAbgBjAGUAIABiAGUAdAB3AGUAZQBuACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMAIABpAG4AIABtAGkAbgB1AHQAZQBzAC4AXABuAFwAbgBPAHUAdABwAHUAdABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAARABpAGYAZgBlAHIAZQBuAGMAZQAgAGkAbgAgAG0AaQBuAHUAdABlAHMAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBKAEQAYQB0AGUAMQAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgAFwAbgBKAEQAYQB0AGUAMgAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBEAEUATABUAEEAXwBNAEkATgBVAFQARQBTACAAPQAgAEwAQQBNAEIARABBACgASgBEAGEAdABlADEALAAgAEoARABhAHQAZQAyACwAXABuACAAIAAgACAASQBGACgAKABKAEQAYQB0AGUAMQAgAD0AIABcACIAXAAiACkAIAAqACAAKABKAEQAYQB0AGUAMgAgAD0AIABcACIAXAAiACkALAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgASgBEAGEAdABlADEAKQApACAAKwAgAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgASgBEAGEAdABlADIAKQApACwAIAB7ACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoAEoARABhAHQAZQAyACAALQAgAEoARABhAHQAZQAxACkAIAAqACAAMQA0ADQAMABcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEQARQBMAFQAQQBfAFMARQBDAE8ATgBEAFMAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIAB0AGkAbQBlAHMAcABhAG4AIABkAGkAZgBmAGUAcgBlAG4AYwBlACAAYgBlAHQAdwBlAGUAbgAgAEoAdQBsAGkAYQBuACAARABhAHQAZQBzACAAaQBuACAAcwBlAGMAbwBuAGQAcwAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgAEQAaQBmAGYAZQByAGUAbgBjAGUAIABpAG4AIABzAGUAYwBvAG4AZABzAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ASgBEAGEAdABlADEAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIABcAG4ASgBEAGEAdABlADIAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ARABFAEwAVABBAF8AUwBFAEMATwBOAEQAUwAgAD0AIABMAEEATQBCAEQAQQAoAEoARABhAHQAZQAxACwAIABKAEQAYQB0AGUAMgAsAFwAbgAgACAAIAAgAEkARgAoACgASgBEAGEAdABlADEAIAA9ACAAXAAiAFwAIgApACAAKgAgACgASgBEAGEAdABlADIAIAA9ACAAXAAiAFwAIgApACwAIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEoARABhAHQAZQAxACkAKQAgACsAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEoARABhAHQAZQAyACkAKQAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKABKAEQAYQB0AGUAMgAgAC0AIABKAEQAYQB0AGUAMQApACAAKgAgADgANgA0ADAAMABcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEQARQBMAFQAQQBfAEgATwBVAFIAXwBNAEkATgBfAFMARQBDAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAHQAaABlACAAdABpAG0AZQBzAHAAYQBuACAAZABpAGYAZgBlAHIAZQBuAGMAZQAgAGIAZQB0AHcAZQBlAG4AIABKAHUAbABpAGEAbgAgAEQAYQB0AGUAcwAgAGkAbgAgAGgAbwB1AHIAcwAsACAAbQBpAG4AdQB0AGUAcwAgAGEAbgBkACAAcwBlAGMAbwBuAGQAcwAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABpAG4AdABlAGcAZQByACAAWwAtADEALAAwACwAMQBdACAAfAAgAFMAaQBnAG4AXABuACAAMgAgAHwAIABpAG4AdABlAGcAZQByACAAWwAwAC4ALgBdACAAIAAgACAAfAAgAEQAZQBsAHQAYQAgAGgAbwB1AHIAcwBcAG4AIAAzACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADAALgAuADUAOQBdACAAIAB8ACAARABlAGwAdABhACAAbQBpAG4AdQB0AGUAcwBcAG4AIAA0ACAAfAAgAGQAZQBjAGkAbQBhAGwAIABbADAALgAuADYAMAApACAAIAB8ACAARABlAGwAdABhACAAcwBlAGMAbwBuAGQAcwBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEoARABhAHQAZQAxACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAAXABuAEoARABhAHQAZQAyACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEQARQBMAFQAQQBfAEgATwBVAFIAXwBNAEkATgBfAFMARQBDACAAPQAgAEwAQQBNAEIARABBACgASgBEAGEAdABlADEALAAgAEoARABhAHQAZQAyACwAXABuACAAIAAgACAASQBGACgAKABKAEQAYQB0AGUAMQAgAD0AIABcACIAXAAiACkAIAAqACAAKABKAEQAYQB0AGUAMgAgAD0AIABcACIAXAAiACkALAAgAHsAXAAiAFwAIgAsAFwAIgBcACIALABcACIAXAAiACwAXAAiAFwAIgB9ACwAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEoARABhAHQAZQAxACkAKQAgACsAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEoARABhAHQAZQAyACkAKQAsACAAewAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABJAE0ARQBfAEQARQBDAEkATQBBAEwAXwBUAE8AXwBIAE0AUwAoAEoARABhAHQAZQAyACAALQAgAEoARABhAHQAZQAxACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBEAEUATABUAEEAXwBEAEEAWQBTAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAHQAaABlACAAdABpAG0AZQBzAHAAYQBuACAAZABpAGYAZgBlAHIAZQBuAGMAZQAgAGIAZQB0AHcAZQBlAG4AIABKAHUAbABpAGEAbgAgAEQAYQB0AGUAcwAgAGkAbgAgAGQAYQB5AHMALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIABEAGkAZgBmAGUAcgBlAG4AYwBlACAAaQBuACAAZABhAHkAcwBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEoARABhAHQAZQAxACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAAXABuAEoARABhAHQAZQAyACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEQARQBMAFQAQQBfAEQAQQBZAFMAIAA9ACAATABBAE0AQgBEAEEAKABKAEQAYQB0AGUAMQAsACAASgBEAGEAdABlADIALABcAG4AIAAgACAAIABJAEYAKAAoAEoARABhAHQAZQAxACAAPQAgAFwAIgBcACIAKQAgACoAIAAoAEoARABhAHQAZQAyACAAPQAgAFwAIgBcACIAKQAsACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABKAEQAYQB0AGUAMQApACkAIAArACAATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABKAEQAYQB0AGUAMgApACkALAAgAHsAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgASgBEAGEAdABlADIAIAAtACAASgBEAGEAdABlADEAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEQARQBMAFQAQQBfAFcARQBFAEsAUwBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHQAaQBtAGUAcwBwAGEAbgAgAGQAaQBmAGYAZQByAGUAbgBjAGUAIABiAGUAdAB3AGUAZQBuACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMAIABpAG4AIAB3AGUAZQBrAHMALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIABEAGkAZgBmAGUAcgBlAG4AYwBlACAAaQBuACAAdwBlAGUAawBzAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ASgBEAGEAdABlADEAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAXABuAEoARABhAHQAZQAyACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBEAEUATABUAEEAXwBXAEUARQBLAFMAIAA9ACAATABBAE0AQgBEAEEAKABKAEQAYQB0AGUAMQAsACAASgBEAGEAdABlADIALABcAG4AIAAgACAAIABJAEYAKAAoAEoARABhAHQAZQAxACAAPQAgAFwAIgBcACIAKQAgACoAIAAoAEoARABhAHQAZQAyACAAPQAgAFwAIgBcACIAKQAsACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABKAEQAYQB0AGUAMQApACkAIAArACAATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABKAEQAYQB0AGUAMgApACkALAAgAHsAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgASgBEAGEAdABlADIAIAAtACAASgBEAGEAdABlADEAKQAgAC8AIAA3AFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ARABFAEwAVABBAF8ATQBPAE4AVABIAFMAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIAB0AGkAbQBlAHMAcABhAG4AIABkAGkAZgBmAGUAcgBlAG4AYwBlACAAYgBlAHQAdwBlAGUAbgAgAEoAdQBsAGkAYQBuACAARABhAHQAZQBzACAAaQBuACAAbQBvAG4AdABoAHMALgBcAG4AVwBoAGUAcgBlACAAdABoAGUAIABkAGkAZgBmAGUAcgBlAG4AYwBlACAAaQBuAGMAbAB1AGQAZQBzACAAcABhAHIAdABpAGEAbAAgAG0AbwBuAHQAaABzACwAIAB0AGgAZQAgAGYAcgBhAGMAdABpAG8AbgAgAGkAcwAgAGMAYQBsAGMAdQBsAGEAdABlAGQAIABvAG4AIAB0AGgAZQAgAGIAYQBzAGkAcwAgAG8AZgAgAGQAYQB5AHMAIABpAG4AIAB0AGgAZQAgAG0AbwBuAHQAaABcAG4AbwBmACAAdABoAGUAIABjAGEAbABlAG4AZABhAHIALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIABEAGkAZgBmAGUAcgBlAG4AYwBlACAAaQBuACAAbQBvAG4AdABoAHMAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBKAEQAYQB0AGUAMQAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAAgACAAIAAgAHwAXABuAEoARABhAHQAZQAyACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgACAAIAAgACAAfABcAG4AWwBUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQAXQAgAHwAIABkAGUAYwBpAG0AYQBsACAAIAAgACAAIAB8ACAAVABpAG0AZQAgAHoAbwBuAGUAIABvAGYAZgBzAGUAdAAgAGkAbgAgAG0AaQBuAHUAdABlAHMAIABmAHIAbwBtACAAVQBUAEMALgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABbAC0AOQAwADAALgAuADkAMAAwAF0AIAB8ACAAQQBzAHMAdQBtAGUAZAAgAHQAbwAgAGIAZQAgAFUAVABDACAAaQBmACAAbwBtAG0AaQB0AHQAZQBkAC4AXABuAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0AIAB8ACAAcwB3AGkAdABjAGgAIAAgACAAIAAgACAAfAAgAEMAYQBsAGMAdQBsAGEAdABlACAAaQBuACAAdABoAGUAIABKAHUAbABpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AIABEAGUAZgBhAHUAbAB0ACAAaQBzACAARwByAGUAZwBvAHIAaQBhAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEQARQBMAFQAQQBfAE0ATwBOAFQASABTACAAPQAgAEwAQQBNAEIARABBACgASgBEAGEAdABlADEALAAgAEoARABhAHQAZQAyACwAIABbAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdABdACwAIABbAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACwAXABuACAAIAAgACAASQBGACgAKABKAEQAYQB0AGUAMQAgAD0AIABcACIAXAAiACkAIAAqACAAKABKAEQAYQB0AGUAMgAgAD0AIABcACIAXAAiACkALAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgASgBEAGEAdABlADEAKQApACAAKwAgAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgASgBEAGEAdABlADIAKQApACwAIAB7ACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdAB6AG8ALAAgAE4AKABUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAEEAQgBTACgAXwB0AHoAbwApACAAPgAgADkAMAAwACwAIAB7ACMATgBVAE0AIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaQBnAG4ALAAgAEkARgAoAEoARABhAHQAZQAyACAAPgA9ACAASgBEAGEAdABlADEALAAgADEALAAgAC0AMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AagBkAG4ATABvAGMAYQBsAF8AUwB0AGEAcgB0ACwAIABKAEQAQQBUAEUAXwBUAE8AXwBKAEQATgBfAEwATwBDAEEATAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAF8AcwBpAGcAbgAgAD0AIAAxACwAIABKAEQAYQB0AGUAMQAsACAASgBEAGEAdABlADIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdAB6AG8AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBqAGQAbgBMAG8AYwBhAGwAXwBFAG4AZAAsACAASgBEAEEAVABFAF8AVABPAF8ASgBEAE4AXwBMAE8AQwBBAEwAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAHMAaQBnAG4AIAA9ACAAMQAsACAASgBEAGEAdABlADIALAAgAEoARABhAHQAZQAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBvAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHQAZQBfAFMAdABhAHIAdAAsACAASgBEAE4AXwBUAE8AXwBDAEEATABFAE4ARABBAFIAXwBEAEEAVABFACgASQBOAEQARQBYACgAXwBqAGQAbgBMAG8AYwBhAGwAXwBTAHQAYQByAHQALAAgADEALAAgADEAKQAsACAASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAdABlAF8ARQBuAGQALAAgAEoARABOAF8AVABPAF8AQwBBAEwARQBOAEQAQQBSAF8ARABBAFQARQAoAEkATgBEAEUAWAAoAF8AagBkAG4ATABvAGMAYQBsAF8ARQBuAGQALAAgADEALAAgADEAKQAsACAASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGUAbAB0AGEAWQBlAGEAcgAsACAASQBOAEQARQBYACgAXwBkAGEAdABlAF8ARQBuAGQALAAgADEALAAgADEAKQAgAC0AIABJAE4ARABFAFgAKABfAGQAYQB0AGUAXwBTAHQAYQByAHQALAAgADEALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAZQBsAHQAYQBNAG8AbgB0AGgALAAgAEkATgBEAEUAWAAoAF8AZABhAHQAZQBfAEUAbgBkACwAIAAxACwAIAAyACkAIAAtACAASQBOAEQARQBYACgAXwBkAGEAdABlAF8AUwB0AGEAcgB0ACwAIAAxACwAIAAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGkAZgBmAE0AbwBuAHQAaABzACwAIAAoAF8AZABlAGwAdABhAFkAZQBhAHIAIAAqACAAMQAyACkAIAArACAAXwBkAGUAbAB0AGEATQBvAG4AdABoACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkAcwBNAG8AbgB0AGgAXwBTAHQAYQByAHQALAAgAEQAQQBZAFMAXwBJAE4AXwBNAE8ATgBUAEgAKABJAE4ARABFAFgAKABfAGQAYQB0AGUAXwBTAHQAYQByAHQALAAgADEALAAgADIAKQAsACAASQBOAEQARQBYACgAXwBkAGEAdABlAF8AUwB0AGEAcgB0ACwAIAAxACwAIAAxACkALAAgAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkAcwBNAG8AbgB0AGgAXwBFAG4AZAAsACAARABBAFkAUwBfAEkATgBfAE0ATwBOAFQASAAoAEkATgBEAEUAWAAoAF8AZABhAHQAZQBfAEUAbgBkACwAIAAxACwAIAAyACkALAAgAEkATgBEAEUAWAAoAF8AZABhAHQAZQBfAEUAbgBkACwAIAAxACwAIAAxACkALAAgAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcABhAHIAdABpAGEAbABNAG8AbgB0AGgAXwBTAHQAYQByAHQALAAgACgASQBOAEQARQBYACgAXwBkAGEAdABlAF8AUwB0AGEAcgB0ACwAIAAxACwAIAAzACkAIAAtACAAMQAgACsAIABJAE4ARABFAFgAKABfAGoAZABuAEwAbwBjAGEAbABfAFMAdABhAHIAdAAsACAAMQAsACAAMgApACkAIAAvACAAXwBkAGEAeQBzAE0AbwBuAHQAaABfAFMAdABhAHIAdAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHAAYQByAHQAaQBhAGwATQBvAG4AdABoAF8ARQBuAGQALAAgACgASQBOAEQARQBYACgAXwBkAGEAdABlAF8ARQBuAGQALAAgADEALAAgADMAKQAgAC0AIAAxACAAKwAgAEkATgBEAEUAWAAoAF8AagBkAG4ATABvAGMAYQBsAF8ARQBuAGQALAAgADEALAAgADIAKQApACAALwAgAF8AZABhAHkAcwBNAG8AbgB0AGgAXwBFAG4AZAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaQBnAG4AIAAqACAAKABfAGQAaQBmAGYATQBvAG4AdABoAHMAIAAtACAAXwBwAGEAcgB0AGkAYQBsAE0AbwBuAHQAaABfAFMAdABhAHIAdAAgACsAIABfAHAAYQByAHQAaQBhAGwATQBvAG4AdABoAF8ARQBuAGQAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEQARQBMAFQAQQBfAFEAVQBBAFIAVABFAFIAUwBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHQAaQBtAGUAcwBwAGEAbgAgAGQAaQBmAGYAZQByAGUAbgBjAGUAIABiAGUAdAB3AGUAZQBuACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMAIABpAG4AIABxAHUAYQByAHQAZQByAHMALgBcAG4AVwBoAGUAcgBlACAAdABoAGUAIABkAGkAZgBmAGUAcgBlAG4AYwBlACAAaQBuAGMAbAB1AGQAZQBzACAAcABhAHIAdABpAGEAbAAgAHEAdQBhAHIAdABlAHIAcwAsACAAdABoAGUAIABmAHIAYQBjAHQAaQBvAG4AIABpAHMAIABjAGEAbABjAHUAbABhAHQAZQBkACAAbwBuACAAdABoAGUAIABiAGEAcwBpAHMAIABvAGYAIABkAGEAeQBzACAAaQBuACAAdABoAGUAXABuAHEAdQBhAHIAdABlAHIAIABvAGYAIAB0AGgAZQAgAGMAYQBsAGUAbgBkAGEAcgAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgAEQAaQBmAGYAZQByAGUAbgBjAGUAIABpAG4AIABxAHUAYQByAHQAZQByAHMAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBKAEQAYQB0AGUAMQAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAAgACAAIAAgACAAIAAgACAAfAAgAFwAbgBKAEQAYQB0AGUAMgAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAAgACAAIAAgACAAIAAgACAAfAAgAFwAbgBbAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdABdACAAfAAgAGQAZQBjAGkAbQBhAGwAIAAgACAAIAAgACAAIAAgACAAfAAgAFQAaQBtAGUAIAB6AG8AbgBlACAAbwBmAGYAcwBlAHQAIABpAG4AIABtAGkAbgB1AHQAZQBzACAAZgByAG8AbQAgAFUAVABDAC4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAWwAtADkAMAAwAC4ALgA5ADAAMABdACAAIAAgACAAIAB8ACAAQQBzAHMAdQBtAGUAZAAgAHQAbwAgAGIAZQAgAFUAVABDACAAaQBmACAAbwBtAG0AaQB0AHQAZQBkAC4AXABuAFsATQBvAG4AdABoAE8AZgBmAHMAZQB0AF0AIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsALQA2AC4ALgAzAF0AIAB8ACAAUQB1AGEAcgB0AGUAcgAgAG0AbwBuAHQAaAAgAG8AZgBmAHMAZQB0ACAAZgByAG8AbQAgAEoAYQBuAHUAYQByAHkALgBcAG4AWwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAgAHwAIABzAHcAaQB0AGMAaAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABDAGEAbABjAHUAbABhAHQAZQAgAGkAbgAgAHQAaABlACAASgB1AGwAaQBhAG4AIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuACAARABlAGYAYQB1AGwAdAAgAGkAcwAgAEcAcgBlAGcAbwByAGkAYQBuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEQARQBMAFQAQQBfAFEAVQBBAFIAVABFAFIAUwAgAD0AIABMAEEATQBCAEQAQQAoAEoARABhAHQAZQAxACwAIABKAEQAYQB0AGUAMgAsACAAWwBUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQAXQAsACAAWwBNAG8AbgB0AGgATwBmAGYAcwBlAHQAXQAsACAAWwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAsAFwAbgAgACAAIAAgAEkARgAoACgASgBEAGEAdABlADEAIAA9ACAAXAAiAFwAIgApACAAKgAgACgASgBEAGEAdABlADIAIAA9ACAAXAAiAFwAIgApACwAIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEoARABhAHQAZQAxACkAKQAgACsAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEoARABhAHQAZQAyACkAKQAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBvACwAIABOACgAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AbwBuAHQAaABPAGYAZgBzAGUAdAAsACAAUgBPAFUATgBEACgATgAoAE0AbwBuAHQAaABPAGYAZgBzAGUAdAApACwAIAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKAAoAEEAQgBTACgAXwB0AHoAbwApACAAPgAgADkAMAAwACkAIAArACAAKABfAG0AbwBuAHQAaABPAGYAZgBzAGUAdAAgADwAIAAtADYAKQAgACsAIAAoAF8AbQBvAG4AdABoAE8AZgBmAHMAZQB0ACAAPgAgADMAKQAsACAAewAjAE4AVQBNACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGkAZwBuACwAIABJAEYAKABKAEQAYQB0AGUAMgAgAD4APQAgAEoARABhAHQAZQAxACwAIAAxACwAIAAtADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGoAZABuAEwAbwBjAGEAbABfAFMAdABhAHIAdAAsACAASgBEAEEAVABFAF8AVABPAF8ASgBEAE4AXwBMAE8AQwBBAEwAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAHMAaQBnAG4AIAA9ACAAMQAsACAASgBEAGEAdABlADEALAAgAEoARABhAHQAZQAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBvAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AagBkAG4ATABvAGMAYQBsAF8ARQBuAGQALAAgAEoARABBAFQARQBfAFQATwBfAEoARABOAF8ATABPAEMAQQBMACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBzAGkAZwBuACAAPQAgADEALAAgAEoARABhAHQAZQAyACwAIABKAEQAYQB0AGUAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AHoAbwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHEAdQBhAHIAdABlAHIARABhAHQAZQBfAFMAdABhAHIAdAAsACAASgBEAE4AXwBUAE8AXwBRAFUAQQBSAFQARQBSAF8ARABBAFQARQAoAEkATgBEAEUAWAAoAF8AagBkAG4ATABvAGMAYQBsAF8AUwB0AGEAcgB0ACwAIAAxACwAIAAxACkALAAgAF8AbQBvAG4AdABoAE8AZgBmAHMAZQB0ACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHEAdQBhAHIAdABlAHIARABhAHQAZQBfAEUAbgBkACwAIABKAEQATgBfAFQATwBfAFEAVQBBAFIAVABFAFIAXwBEAEEAVABFACgASQBOAEQARQBYACgAXwBqAGQAbgBMAG8AYwBhAGwAXwBFAG4AZAAsACAAMQAsACAAMQApACwAIABfAG0AbwBuAHQAaABPAGYAZgBzAGUAdAAsACAASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGUAbAB0AGEAWQBlAGEAcgAsACAASQBOAEQARQBYACgAXwBxAHUAYQByAHQAZQByAEQAYQB0AGUAXwBFAG4AZAAsACAAMQAsACAAMQApACAALQAgAEkATgBEAEUAWAAoAF8AcQB1AGEAcgB0AGUAcgBEAGEAdABlAF8AUwB0AGEAcgB0ACwAIAAxACwAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGUAbAB0AGEAUQB1AGEAcgB0AGUAcgAsACAASQBOAEQARQBYACgAXwBxAHUAYQByAHQAZQByAEQAYQB0AGUAXwBFAG4AZAAsACAAMQAsACAAMgApACAALQAgAEkATgBEAEUAWAAoAF8AcQB1AGEAcgB0AGUAcgBEAGEAdABlAF8AUwB0AGEAcgB0ACwAIAAxACwAIAAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGkAZgBmAFEAdQBhAHIAdABlAHIAcwAsACAAKABfAGQAZQBsAHQAYQBZAGUAYQByACAAKgAgADQAKQAgACsAIABfAGQAZQBsAHQAYQBRAHUAYQByAHQAZQByACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcABhAHIAdABpAGEAbABRAHUAYQByAHQAZQByAF8AUwB0AGEAcgB0ACwAIAAoAEkATgBEAEUAWAAoAF8AcQB1AGEAcgB0AGUAcgBEAGEAdABlAF8AUwB0AGEAcgB0ACwAIAAxACwAIAAzACkAIAAtACAAMQAgACsAIABJAE4ARABFAFgAKABfAGoAZABuAEwAbwBjAGEAbABfAFMAdABhAHIAdAAsACAAMQAsACAAMgApACkAIAAvACAASQBOAEQARQBYACgAXwBxAHUAYQByAHQAZQByAEQAYQB0AGUAXwBTAHQAYQByAHQALAAgADEALAAgADQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHAAYQByAHQAaQBhAGwAUQB1AGEAcgB0AGUAcgBfAEUAbgBkACwAIAAoAEkATgBEAEUAWAAoAF8AcQB1AGEAcgB0AGUAcgBEAGEAdABlAF8ARQBuAGQALAAgADEALAAgADMAKQAgAC0AIAAxACAAKwAgAEkATgBEAEUAWAAoAF8AagBkAG4ATABvAGMAYQBsAF8ARQBuAGQALAAgADEALAAgADIAKQApACAALwAgAEkATgBEAEUAWAAoAF8AcQB1AGEAcgB0AGUAcgBEAGEAdABlAF8ARQBuAGQALAAgADEALAAgADQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaQBnAG4AIAAqACAAKABfAGQAaQBmAGYAUQB1AGEAcgB0AGUAcgBzACAALQAgAF8AcABhAHIAdABpAGEAbABRAHUAYQByAHQAZQByAF8AUwB0AGEAcgB0ACAAKwAgAF8AcABhAHIAdABpAGEAbABRAHUAYQByAHQAZQByAF8ARQBuAGQAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEQARQBMAFQAQQBfAFkARQBBAFIAUwBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHQAaQBtAGUAcwBwAGEAbgAgAGQAaQBmAGYAZQByAGUAbgBjAGUAIABiAGUAdAB3AGUAZQBuACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMAIABpAG4AIAB5AGUAYQByAHMALgBcAG4AVwBoAGUAcgBlACAAdABoAGUAIABkAGkAZgBmAGUAcgBlAG4AYwBlACAAaQBuAGMAbAB1AGQAZQBzACAAcABhAHIAdABpAGEAbAAgAHkAZQBhAHIAcwAsACAAdABoAGUAIABmAHIAYQBjAHQAaQBvAG4AIABpAHMAIABjAGEAbABjAHUAbABhAHQAZQBkACAAbwBuACAAdABoAGUAIABiAGEAcwBpAHMAIABvAGYAIABkAGEAeQBzACAAaQBuACAAdABoAGUAXABuAHkAZQBhAHIAIABvAGYAIAB0AGgAZQAgAGMAYQBsAGUAbgBkAGEAcgAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgAEQAaQBmAGYAZQByAGUAbgBjAGUAIABpAG4AIAB5AGUAYQByAHMAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBKAEQAYQB0AGUAMQAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAAgACAAIAAgAHwAIABcAG4ASgBEAGEAdABlADIAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAIAAgACAAIAB8ACAAXABuAFsAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0AF0AIAB8ACAAZABlAGMAaQBtAGEAbAAgACAAIAAgACAAfAAgAFQAaQBtAGUAIAB6AG8AbgBlACAAbwBmAGYAcwBlAHQAIABpAG4AIABtAGkAbgB1AHQAZQBzACAAZgByAG8AbQAgAFUAVABDAC4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAWwAtADkAMAAwAC4ALgA5ADAAMABdACAAfAAgAEEAcwBzAHUAbQBlAGQAIAB0AG8AIABiAGUAIABVAFQAQwAgAGkAZgAgAG8AbQBtAGkAdAB0AGUAZAAuAFwAbgBbAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACAAfAAgAHMAdwBpAHQAYwBoACAAIAAgACAAIAAgAHwAIABDAGEAbABjAHUAbABhAHQAZQAgAGkAbgAgAHQAaABlACAASgB1AGwAaQBhAG4AIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuACAARABlAGYAYQB1AGwAdAAgAGkAcwAgAEcAcgBlAGcAbwByAGkAYQBuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBEAEUATABUAEEAXwBZAEUAQQBSAFMAIAA9ACAATABBAE0AQgBEAEEAKABKAEQAYQB0AGUAMQAsACAASgBEAGEAdABlADIALAAgAFsAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0AF0ALAAgAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0ALABcAG4AIAAgACAAIABJAEYAKAAoAEoARABhAHQAZQAxACAAPQAgAFwAIgBcACIAKQAgACoAIAAoAEoARABhAHQAZQAyACAAPQAgAFwAIgBcACIAKQAsACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABKAEQAYQB0AGUAMQApACkAIAArACAATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABKAEQAYQB0AGUAMgApACkALAAgAHsAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AHoAbwAsACAATgAoAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAQQBCAFMAKABfAHQAegBvACkAIAA+ACAAOQAwADAALAAgAHsAIwBOAFUATQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBpAGcAbgAsACAASQBGACgASgBEAGEAdABlADIAIAA+AD0AIABKAEQAYQB0AGUAMQAsACAAMQAsACAALQAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBqAGQAbgBMAG8AYwBhAGwAXwBTAHQAYQByAHQALAAgAEoARABBAFQARQBfAFQATwBfAEoARABOAF8ATABPAEMAQQBMACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBzAGkAZwBuACAAPQAgADEALAAgAEoARABhAHQAZQAxACwAIABKAEQAYQB0AGUAMgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AHoAbwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGoAZABuAEwAbwBjAGEAbABfAEUAbgBkACwAIABKAEQAQQBUAEUAXwBUAE8AXwBKAEQATgBfAEwATwBDAEEATAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAF8AcwBpAGcAbgAgAD0AIAAxACwAIABKAEQAYQB0AGUAMgAsACAASgBEAGEAdABlADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdAB6AG8AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBvAHIAZABpAG4AYQBsAEQAYQB0AGUAXwBTAHQAYQByAHQALAAgAEoARABOAF8AVABPAF8ATwBSAEQASQBOAEEATABfAEQAQQBUAEUAKABJAE4ARABFAFgAKABfAGoAZABuAEwAbwBjAGEAbABfAFMAdABhAHIAdAAsACAAMQAsACAAMQApACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG8AcgBkAGkAbgBhAGwARABhAHQAZQBfAEUAbgBkACwAIABKAEQATgBfAFQATwBfAE8AUgBEAEkATgBBAEwAXwBEAEEAVABFACgASQBOAEQARQBYACgAXwBqAGQAbgBMAG8AYwBhAGwAXwBFAG4AZAAsACAAMQAsACAAMQApACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAZQBsAHQAYQBZAGUAYQByACwAIABJAE4ARABFAFgAKABfAG8AcgBkAGkAbgBhAGwARABhAHQAZQBfAEUAbgBkACwAIAAxACwAIAAxACkAIAAtACAASQBOAEQARQBYACgAXwBvAHIAZABpAG4AYQBsAEQAYQB0AGUAXwBTAHQAYQByAHQALAAgADEALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHAAYQByAHQAaQBhAGwAWQBlAGEAcgBfAFMAdABhAHIAdAAsACAAKABJAE4ARABFAFgAKABfAG8AcgBkAGkAbgBhAGwARABhAHQAZQBfAFMAdABhAHIAdAAsACAAMQAsACAAMgApACAALQAgADEAIAArACAASQBOAEQARQBYACgAXwBqAGQAbgBMAG8AYwBhAGwAXwBTAHQAYQByAHQALAAgADEALAAgADIAKQApACAALwAgAEkATgBEAEUAWAAoAF8AbwByAGQAaQBuAGEAbABEAGEAdABlAF8AUwB0AGEAcgB0ACwAIAAxACwAIAAzACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBwAGEAcgB0AGkAYQBsAFkAZQBhAHIAXwBFAG4AZAAsACAAKABJAE4ARABFAFgAKABfAG8AcgBkAGkAbgBhAGwARABhAHQAZQBfAEUAbgBkACwAIAAxACwAIAAyACkAIAAtACAAMQAgACsAIABJAE4ARABFAFgAKABfAGoAZABuAEwAbwBjAGEAbABfAEUAbgBkACwAIAAxACwAIAAyACkAKQAgAC8AIABJAE4ARABFAFgAKABfAG8AcgBkAGkAbgBhAGwARABhAHQAZQBfAEUAbgBkACwAIAAxACwAIAAzACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGkAZwBuACAAKgAgACgAXwBkAGUAbAB0AGEAWQBlAGEAcgAgAC0AIABfAHAAYQByAHQAaQBhAGwAWQBlAGEAcgBfAFMAdABhAHIAdAAgACsAIABfAHAAYQByAHQAaQBhAGwAWQBlAGEAcgBfAEUAbgBkACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ARABFAEwAVABBAF8AVwBFAEUASwBfAEQAQQBZAFMAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIAB0AGkAbQBlAHMAcABhAG4AIABkAGkAZgBmAGUAcgBlAG4AYwBlACAAYgBlAHQAdwBlAGUAbgAgAEoAdQBsAGkAYQBuACAARABhAHQAZQBzACAAaQBuACAAdwBlAGUAawBzACAAYQBuAGQAIABkAGEAeQBzAC4AXABuAFwAbgBPAHUAdABwAHUAdABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbAC0AMQAsADAALAAxAF0AIAB8ACAAUwBpAGcAbgBcAG4AIAAzACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADAALgAuAF0AIAAgACAAIAB8ACAARABlAGwAdABhACAAdwBlAGUAawBzACAAXABuACAANAAgAHwAIABkAGUAYwBpAG0AYQBsACAAWwAwAC4ALgA3ACkAIAAgACAAfAAgAEQAZQBsAHQAYQAgAGQAYQB5AHMAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBKAEQAYQB0AGUAMQAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgAFwAbgBKAEQAYQB0AGUAMgAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBEAEUATABUAEEAXwBXAEUARQBLAF8ARABBAFkAUwAgAD0AIABMAEEATQBCAEQAQQAoAEoARABhAHQAZQAxACwAIABKAEQAYQB0AGUAMgAsAFwAbgAgACAAIAAgAEkARgAoACgASgBEAGEAdABlADEAIAA9ACAAXAAiAFwAIgApACAAKgAgACgASgBEAGEAdABlADIAIAA9ACAAXAAiAFwAIgApACwAIAB7AFwAIgBcACIALAAgAFwAIgBcACIALAAgAFwAIgBcACIAfQAsAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABKAEQAYQB0AGUAMQApACkAIAArACAATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABKAEQAYQB0AGUAMgApACkALAAgAHsAIwBWAEEATABVAEUAIQAsACAAIwBWAEEATABVAEUAIQAsACAAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGkAZgBmAEQAYQB5AHMALAAgACgASgBEAGEAdABlADIAIAAtACAASgBEAGEAdABlADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAF8AZABpAGYAZgBEAGEAeQBzACAAPQAgADAALAAgAHsAMAAsACAAMAAsACAAMAB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaQBnAG4ALAAgAEkARgAoAF8AZABpAGYAZgBEAGEAeQBzACAAPgA9ACAAMAAsACAAMQAsACAALQAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBhAGIAcwBEAGkAZgBmAEQAYQB5AHMALAAgAF8AcwBpAGcAbgAgACoAIABfAGQAaQBmAGYARABhAHkAcwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAZQBsAHQAYQBXAGUAZQBrACwAIABJAE4AVAAoAF8AYQBiAHMARABpAGYAZgBEAGEAeQBzACAALwAgADcAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAZQBsAHQAYQBEAGEAeQAsACAATQBPAEQAKABfAGEAYgBzAEQAaQBmAGYARABhAHkAcwAsACAANwApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGkAZwBuACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGUAbAB0AGEAVwBlAGUAawAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABlAGwAdABhAEQAYQB5AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ARABFAEwAVABBAF8AWQBFAEEAUgBfAFcARQBFAEsAXwBEAEEAWQBTAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAHQAaABlACAAdABpAG0AZQBzAHAAYQBuACAAZABpAGYAZgBlAHIAZQBuAGMAZQAgAGIAZQB0AHcAZQBlAG4AIABKAHUAbABpAGEAbgAgAEQAYQB0AGUAcwAgAGkAbgAgAHkAZQBhAHIAcwAsACAAdwBlAGUAawBzACwAIABhAG4AZAAgAGQAYQB5AHMALgBcAG4ATgBvAHQAZQAgAHQAaABlACAAbgB1AG0AYgBlAHIAIABvAGYAIAB3AGUAZQBrAHMAIABwAGUAcgAgAHkAZQBhAHIAIABhAG4AIAB2AGEAcgB5ACAAYgBlAHQAdwBlAGUAbgAgADUAMgAgAGEAbgBkACAANQAzAC4AIABJAGYAIABhAG4AIABhAGIAcwBvAGwAdQB0AGUAIABuAHUAbQBiAGUAcgAgAG8AZgAgAHcAZQBlAGsAcwAgAGkAcwAgAGIAZQBpAG4AZwAgAHMAbwB1AGcAaAB0AFwAbgB0AGgAZQBuACAAdQBzAGUAIABlAGkAdABoAGUAcgAgAEQARQBMAFQAQQBfAFcARQBFAEsAXwBEAEEAWQBTACAAbwByACAARABFAEwAVABBAF8AVwBFAEUASwBTACAAZgB1AG4AYwB0AGkAbwBuAHMALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsALQAxACwAMAAsADEAXQAgAHwAIABTAGkAZwBuAFwAbgAgADIAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMAAuAC4AXQAgACAAIAAgAHwAIABEAGUAbAB0AGEAIAB5AGUAYQByAHMAXABuACAAMwAgAHwAIABpAG4AdABlAGcAZQByACAAWwAwAC4ALgA1ADIAXQAgACAAfAAgAEQAZQBsAHQAYQAgAHcAZQBlAGsAcwAgAFwAbgAgADQAIAB8ACAAZABlAGMAaQBtAGEAbAAgAFsAMAAuAC4ANwApACAAIAAgAHwAIABEAGUAbAB0AGEAIABkAGEAeQBzAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ASgBEAGEAdABlADEAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAIAAgACAAIAB8ACAAXABuAEoARABhAHQAZQAyACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgACAAIAAgACAAfAAgAFwAbgBbAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdABdACAAfAAgAGQAZQBjAGkAbQBhAGwAIAAgACAAIAAgAHwAIABUAGkAbQBlACAAegBvAG4AZQAgAG8AZgBmAHMAZQB0ACAAaQBuACAAbQBpAG4AdQB0AGUAcwAgAGYAcgBvAG0AIABVAFQAQwAuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAFsALQA5ADAAMAAuAC4AOQAwADAAXQAgAHwAIABBAHMAcwB1AG0AZQBkACAAdABvACAAYgBlACAAVQBUAEMAIABpAGYAIABvAG0AbQBpAHQAdABlAGQALgBcAG4AWwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAgAHwAIABzAHcAaQB0AGMAaAAgACAAIAAgACAAIAB8ACAAQwBhAGwAYwB1AGwAYQB0AGUAIABpAG4AIAB0AGgAZQAgAEoAdQBsAGkAYQBuACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgAgAEQAZQBmAGEAdQBsAHQAIABpAHMAIABHAHIAZQBnAG8AcgBpAGEAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ARABFAEwAVABBAF8AWQBFAEEAUgBfAFcARQBFAEsAXwBEAEEAWQBTACAAPQAgAEwAQQBNAEIARABBACgASgBEAGEAdABlADEALAAgAEoARABhAHQAZQAyACwAIABbAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdABdACwAIABbAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACwAXABuACAAIAAgACAASQBGACgAKABKAEQAYQB0AGUAMQAgAD0AIABcACIAXAAiACkAIAAqACAAKABKAEQAYQB0AGUAMgAgAD0AIABcACIAXAAiACkALAAgAHsAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgB9ACwAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEoARABhAHQAZQAxACkAKQAgACsAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEoARABhAHQAZQAyACkAKQAsACAAewAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBvACwAIABOACgAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABBAEIAUwAoAF8AdAB6AG8AKQAgAD4AIAA5ADAAMAAsACAAewAjAE4AVQBNACEALAAgACMATgBVAE0AIQAsACAAIwBOAFUATQAhACwAIAAjAE4AVQBNACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgASgBEAGEAdABlADIAIAA9ACAASgBEAGEAdABlADEALAAgAHsAMAAsACAAMAAsACAAMAAsACAAMAB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGkAZwBuACwAIABJAEYAKABKAEQAYQB0AGUAMgAgAD4APQAgAEoARABhAHQAZQAxACwAIAAxACwAIAAtADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AagBkAG4ATABvAGMAYQBsAF8AUwB0AGEAcgB0ACwAIABKAEQAQQBUAEUAXwBUAE8AXwBKAEQATgBfAEwATwBDAEEATAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBzAGkAZwBuACAAPQAgADEALAAgAEoARABhAHQAZQAxACwAIABKAEQAYQB0AGUAMgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBvAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGoAZABuAEwAbwBjAGEAbABfAEUAbgBkACwAIABKAEQAQQBUAEUAXwBUAE8AXwBKAEQATgBfAEwATwBDAEEATAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBzAGkAZwBuACAAPQAgADEALAAgAEoARABhAHQAZQAyACwAIABKAEQAYQB0AGUAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBvAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB3AGUAZQBrAEQAYQB0AGUAXwBTAHQAYQByAHQALAAgAEoARABOAF8AVABPAF8AVwBFAEUASwBfAEQAQQBUAEUAKABJAE4ARABFAFgAKABfAGoAZABuAEwAbwBjAGEAbABfAFMAdABhAHIAdAAsACAAMQAsACAAMQApACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdwBlAGUAawBEAGEAdABlAF8ARQBuAGQALAAgAEoARABOAF8AVABPAF8AVwBFAEUASwBfAEQAQQBUAEUAKABJAE4ARABFAFgAKABfAGoAZABuAEwAbwBjAGEAbABfAEUAbgBkACwAIAAxACwAIAAxACkALAAgAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGUAbAB0AGEAWQBlAGEAcgAsACAASQBOAEQARQBYACgAXwB3AGUAZQBrAEQAYQB0AGUAXwBFAG4AZAAsACAAMQAsACAAMQApACAALQAgAEkATgBEAEUAWAAoAF8AdwBlAGUAawBEAGEAdABlAF8AUwB0AGEAcgB0ACwAIAAxACwAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAZQBsAHQAYQBXAGUAZQBrACwAIABJAE4ARABFAFgAKABfAHcAZQBlAGsARABhAHQAZQBfAEUAbgBkACwAIAAxACwAIAAyACkAIAAtACAASQBOAEQARQBYACgAXwB3AGUAZQBrAEQAYQB0AGUAXwBTAHQAYQByAHQALAAgADEALAAgADIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABlAGwAdABhAEQAYQB5ACwAIABJAE4ARABFAFgAKABfAHcAZQBlAGsARABhAHQAZQBfAEUAbgBkACwAIAAxACwAIAAzACkAIAAtACAASQBOAEQARQBYACgAXwB3AGUAZQBrAEQAYQB0AGUAXwBTAHQAYQByAHQALAAgADEALAAgADMAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACsAIABJAE4ARABFAFgAKABfAGoAZABuAEwAbwBjAGEAbABfAEUAbgBkACwAIAAxACwAIAAyACkAIAAtACAASQBOAEQARQBYACgAXwBqAGQAbgBMAG8AYwBhAGwAXwBTAHQAYQByAHQALAAgADEALAAgADIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAZQBsAHQAYQBEAGEAeQAyACwAIABNAE8ARAAoAF8AZABlAGwAdABhAEQAYQB5ACwAIAA3ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAZQBsAHQAYQBXAGUAZQBrADIALAAgAF8AZABlAGwAdABhAFcAZQBlAGsAIAArACAASQBOAFQAKABfAGQAZQBsAHQAYQBEAGEAeQAgAC8AIAA3ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAGQAZQBsAHQAYQBXAGUAZQBrADIAIAA+AD0AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaQBnAG4ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGUAbAB0AGEAWQBlAGEAcgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAZQBsAHQAYQBXAGUAZQBrADIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGUAbAB0AGEARABhAHkAMgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBpAGcAbgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAZQBsAHQAYQBZAGUAYQByACAALQAgADEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGUAbAB0AGEAVwBlAGUAawAyACAAKwAgAEkATgBEAEUAWAAoAF8AdwBlAGUAawBEAGEAdABlAF8AUwB0AGEAcgB0ACwAIAAxACwAIAA0ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGUAbAB0AGEARABhAHkAMgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEQARQBMAFQAQQBfAE0ATwBOAFQASABfAEQAQQBZAFMAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIAB0AGkAbQBlAHMAcABhAG4AIABkAGkAZgBmAGUAcgBlAG4AYwBlACAAYgBlAHQAdwBlAGUAbgAgAEoAdQBsAGkAYQBuACAARABhAHQAZQBzACAAaQBuACAAbQBvAG4AdABoAHMAIABhAG4AZAAgAGQAYQB5AHMALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsALQAxACwAMAAsADEAXQAgAHwAIABTAGkAZwBuAFwAbgAgADIAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMAAuAC4AXQAgACAAIAAgAHwAIABEAGUAbAB0AGEAIABtAG8AbgB0AGgAcwBcAG4AIAAzACAAfAAgAGQAZQBjAGkAbQBhAGwAIABbADAALgAuADMAMQApACAAIAB8ACAARABlAGwAdABhACAAZABhAHkAcwBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEoARABhAHQAZQAxACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgACAAIAAgACAAfAAgAFwAbgBKAEQAYQB0AGUAMgAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAAgACAAIAAgAHwAIABcAG4AWwBUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQAXQAgAHwAIABkAGUAYwBpAG0AYQBsACAAIAAgACAAIAB8ACAAVABpAG0AZQAgAHoAbwBuAGUAIABvAGYAZgBzAGUAdAAgAGkAbgAgAG0AaQBuAHUAdABlAHMAIABmAHIAbwBtACAAVQBUAEMALgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABbAC0AOQAwADAALgAuADkAMAAwAF0AIAB8ACAAQQBzAHMAdQBtAGUAZAAgAHQAbwAgAGIAZQAgAFUAVABDACAAaQBmACAAbwBtAG0AaQB0AHQAZQBkAC4AXABuAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0AIAB8ACAAcwB3AGkAdABjAGgAIAAgACAAIAAgACAAfAAgAEMAYQBsAGMAdQBsAGEAdABlACAAaQBuACAAdABoAGUAIABKAHUAbABpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AIABEAGUAZgBhAHUAbAB0ACAAaQBzACAARwByAGUAZwBvAHIAaQBhAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEQARQBMAFQAQQBfAE0ATwBOAFQASABfAEQAQQBZAFMAIAA9ACAATABBAE0AQgBEAEEAKABKAEQAYQB0AGUAMQAsACAASgBEAGEAdABlADIALAAgAFsAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0AF0ALAAgAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0ALABcAG4AIAAgACAAIABJAEYAKAAoAEoARABhAHQAZQAxACAAPQAgAFwAIgBcACIAKQAgACoAIAAoAEoARABhAHQAZQAyACAAPQAgAFwAIgBcACIAKQAsACAAewBcACIAXAAiACwAIABcACIAXAAiACwAIABcACIAXAAiAH0ALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgASgBEAGEAdABlADEAKQApACAAKwAgAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgASgBEAGEAdABlADIAKQApACwAIAB7ACMAVgBBAEwAVQBFACEALAAgACMAVgBBAEwAVQBFACEALAAgACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdAB6AG8ALAAgAE4AKABUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAEEAQgBTACgAXwB0AHoAbwApACAAPgAgADkAMAAwACwAIAB7ACMATgBVAE0AIQAsACAAIwBOAFUATQAhACwAIAAjAE4AVQBNACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgASgBEAGEAdABlADIAIAA9ACAASgBEAGEAdABlADEALAAgAHsAMAAsACAAMAAsACAAMAB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGkAZwBuACwAIABJAEYAKABKAEQAYQB0AGUAMgAgAD4APQAgAEoARABhAHQAZQAxACwAIAAxACwAIAAtADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AagBkAG4ATABvAGMAYQBsAF8AUwB0AGEAcgB0ACwAIABKAEQAQQBUAEUAXwBUAE8AXwBKAEQATgBfAEwATwBDAEEATAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBzAGkAZwBuACAAPQAgADEALAAgAEoARABhAHQAZQAxACwAIABKAEQAYQB0AGUAMgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBvAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGoAZABuAEwAbwBjAGEAbABfAEUAbgBkACwAIABKAEQAQQBUAEUAXwBUAE8AXwBKAEQATgBfAEwATwBDAEEATAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBzAGkAZwBuACAAPQAgADEALAAgAEoARABhAHQAZQAyACwAIABKAEQAYQB0AGUAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBvAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAdABlAF8AUwB0AGEAcgB0ACwAIABKAEQATgBfAFQATwBfAEMAQQBMAEUATgBEAEEAUgBfAEQAQQBUAEUAKABJAE4ARABFAFgAKABfAGoAZABuAEwAbwBjAGEAbABfAFMAdABhAHIAdAAsACAAMQAsACAAMQApACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHQAZQBfAEUAbgBkACwAIABKAEQATgBfAFQATwBfAEMAQQBMAEUATgBEAEEAUgBfAEQAQQBUAEUAKABJAE4ARABFAFgAKABfAGoAZABuAEwAbwBjAGEAbABfAEUAbgBkACwAIAAxACwAIAAxACkALAAgAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGUAbAB0AGEAWQBlAGEAcgAsACAASQBOAEQARQBYACgAXwBkAGEAdABlAF8ARQBuAGQALAAgADEALAAgADEAKQAgAC0AIABJAE4ARABFAFgAKABfAGQAYQB0AGUAXwBTAHQAYQByAHQALAAgADEALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABlAGwAdABhAE0AbwBuAHQAaAAsACAASQBOAEQARQBYACgAXwBkAGEAdABlAF8ARQBuAGQALAAgADEALAAgADIAKQAgAC0AIABJAE4ARABFAFgAKABfAGQAYQB0AGUAXwBTAHQAYQByAHQALAAgADEALAAgADIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABpAGYAZgBNAG8AbgB0AGgAcwAsACAAKABfAGQAZQBsAHQAYQBZAGUAYQByACAAKgAgADEAMgApACAAKwAgAF8AZABlAGwAdABhAE0AbwBuAHQAaAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABlAGwAdABhAEQAYQB5ACwAIABJAE4ARABFAFgAKABfAGQAYQB0AGUAXwBFAG4AZAAsACAAMQAsACAAMwApACAALQAgAEkATgBEAEUAWAAoAF8AZABhAHQAZQBfAFMAdABhAHIAdAAsACAAMQAsACAAMwApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKwAgAEkATgBEAEUAWAAoAF8AagBkAG4ATABvAGMAYQBsAF8ARQBuAGQALAAgADEALAAgADIAKQAgAC0AIABJAE4ARABFAFgAKABfAGoAZABuAEwAbwBjAGEAbABfAFMAdABhAHIAdAAsACAAMQAsACAAMgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAF8AZABlAGwAdABhAEQAYQB5ACAAPAAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkAcwBNAG8AbgB0AGgAXwBTAHQAYQByAHQALAAgAEQAQQBZAFMAXwBJAE4AXwBNAE8ATgBUAEgAKABJAE4ARABFAFgAKABfAGQAYQB0AGUAXwBTAHQAYQByAHQALAAgADEALAAgADIAKQAsACAASQBOAEQARQBYACgAXwBkAGEAdABlAF8AUwB0AGEAcgB0ACwAIAAxACwAIAAxACkALAAgAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGkAZwBuACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGkAZgBmAE0AbwBuAHQAaABzACAALQAgADEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAYQB5AHMATQBvAG4AdABoAF8AUwB0AGEAcgB0ACAAKwAgAF8AZABlAGwAdABhAEQAYQB5AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGkAZwBuACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABpAGYAZgBNAG8AbgB0AGgAcwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAZQBsAHQAYQBEAGEAeQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEQARQBMAFQAQQBfAFEAVQBBAFIAVABFAFIAXwBEAEEAWQBTAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAHQAaABlACAAdABpAG0AZQBzAHAAYQBuACAAZABpAGYAZgBlAHIAZQBuAGMAZQAgAGIAZQB0AHcAZQBlAG4AIABKAHUAbABpAGEAbgAgAEQAYQB0AGUAcwAgAGkAbgAgAHEAdQBhAHIAdABlAHIAcwAgAGEAbgBkACAAZABhAHkAcwAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABpAG4AdABlAGcAZQByACAAWwAtADEALAAwACwAMQBdACAAfAAgAFMAaQBnAG4AXABuACAAMgAgAHwAIABpAG4AdABlAGcAZQByACAAWwAwAC4ALgBdACAAIAAgACAAfAAgAEQAZQBsAHQAYQAgAHEAdQBhAHIAdABlAHIAcwBcAG4AIAAzACAAfAAgAGQAZQBjAGkAbQBhAGwAIABbADAALgAuADkAMgApACAAIAB8ACAARABlAGwAdABhACAAZABhAHkAcwBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEoARABhAHQAZQAxACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgACAAIAAgACAAIAAgACAAIAB8ACAAXABuAEoARABhAHQAZQAyACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgACAAIAAgACAAIAAgACAAIAB8ACAAXABuAFsAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0AF0AIAB8ACAAZABlAGMAaQBtAGEAbAAgACAAIAAgACAAIAAgACAAIAB8ACAAVABpAG0AZQAgAHoAbwBuAGUAIABvAGYAZgBzAGUAdAAgAGkAbgAgAG0AaQBuAHUAdABlAHMAIABmAHIAbwBtACAAVQBUAEMALgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABbAC0AOQAwADAALgAuADkAMAAwAF0AIAAgACAAIAAgAHwAIABBAHMAcwB1AG0AZQBkACAAdABvACAAYgBlACAAVQBUAEMAIABpAGYAIABvAG0AbQBpAHQAdABlAGQALgBcAG4AWwBNAG8AbgB0AGgATwBmAGYAcwBlAHQAXQAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAWwAtADYALgAuADMAXQAgAHwAIABRAHUAYQByAHQAZQByACAAbQBvAG4AdABoACAAbwBmAGYAcwBlAHQAIABmAHIAbwBtACAASgBhAG4AdQBhAHIAeQAuAFwAbgBbAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACAAfAAgAHMAdwBpAHQAYwBoACAAIAAgACAAIAAgACAAIAAgACAAfAAgAEMAYQBsAGMAdQBsAGEAdABlACAAaQBuACAAdABoAGUAIABKAHUAbABpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AIABEAGUAZgBhAHUAbAB0ACAAaQBzACAARwByAGUAZwBvAHIAaQBhAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ARABFAEwAVABBAF8AUQBVAEEAUgBUAEUAUgBfAEQAQQBZAFMAIAA9ACAATABBAE0AQgBEAEEAKABKAEQAYQB0AGUAMQAsACAASgBEAGEAdABlADIALAAgAFsAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0AF0ALAAgAFsATQBvAG4AdABoAE8AZgBmAHMAZQB0AF0ALAAgAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0ALABcAG4AIAAgACAAIABJAEYAKAAoAEoARABhAHQAZQAxACAAPQAgAFwAIgBcACIAKQAgACoAIAAoAEoARABhAHQAZQAyACAAPQAgAFwAIgBcACIAKQAsACAAewBcACIAXAAiACwAIABcACIAXAAiACwAIABcACIAXAAiAH0ALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgASgBEAGEAdABlADEAKQApACAAKwAgAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgASgBEAGEAdABlADIAKQApACwAIAB7ACMAVgBBAEwAVQBFACEALAAgACMAVgBBAEwAVQBFACEALAAgACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdAB6AG8ALAAgAE4AKABUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbQBvAG4AdABoAE8AZgBmAHMAZQB0ACwAIABSAE8AVQBOAEQAKABOACgATQBvAG4AdABoAE8AZgBmAHMAZQB0ACkALAAgADAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoACgAQQBCAFMAKABfAHQAegBvACkAIAA+ACAAOQAwADAAKQAgACsAIAAoAF8AbQBvAG4AdABoAE8AZgBmAHMAZQB0ACAAPAAgAC0ANgApACAAKwAgACgAXwBtAG8AbgB0AGgATwBmAGYAcwBlAHQAIAA+ACAAMwApACwAIAB7ACMATgBVAE0AIQAsACAAIwBOAFUATQAhACwAIAAjAE4AVQBNACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgASgBEAGEAdABlADIAIAA9ACAASgBEAGEAdABlADEALAAgAHsAIAAwACwAIAAwACAALAAwAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaQBnAG4ALAAgAEkARgAoAEoARABhAHQAZQAxACAAPgAgAEoARABhAHQAZQAyACwAIAAtADEALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AagBkAG4ATABvAGMAYQBsAF8AUwB0AGEAcgB0ACwAIABKAEQAQQBUAEUAXwBUAE8AXwBKAEQATgBfAEwATwBDAEEATAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBzAGkAZwBuACAAPQAgADEALAAgAEoARABhAHQAZQAxACwAIABKAEQAYQB0AGUAMgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBvAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGoAZABuAEwAbwBjAGEAbABfAEUAbgBkACwAIABKAEQAQQBUAEUAXwBUAE8AXwBKAEQATgBfAEwATwBDAEEATAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBzAGkAZwBuACAAPQAgADEALAAgAEoARABhAHQAZQAyACwAIABKAEQAYQB0AGUAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBvAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHEAdQBhAHIAdABlAHIARABhAHQAZQBfAFMAdABhAHIAdAAsACAASgBEAE4AXwBUAE8AXwBRAFUAQQBSAFQARQBSAF8ARABBAFQARQAoAEkATgBEAEUAWAAoAF8AagBkAG4ATABvAGMAYQBsAF8AUwB0AGEAcgB0ACwAIAAxACwAIAAxACkALAAgAF8AbQBvAG4AdABoAE8AZgBmAHMAZQB0ACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcQB1AGEAcgB0AGUAcgBEAGEAdABlAF8ARQBuAGQALAAgAEoARABOAF8AVABPAF8AUQBVAEEAUgBUAEUAUgBfAEQAQQBUAEUAKABJAE4ARABFAFgAKABfAGoAZABuAEwAbwBjAGEAbABfAEUAbgBkACwAIAAxACwAIAAxACkALAAgAF8AbQBvAG4AdABoAE8AZgBmAHMAZQB0ACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABlAGwAdABhAFkAZQBhAHIALAAgAEkATgBEAEUAWAAoAF8AcQB1AGEAcgB0AGUAcgBEAGEAdABlAF8ARQBuAGQALAAgADEALAAgADEAKQAgAC0AIABJAE4ARABFAFgAKABfAHEAdQBhAHIAdABlAHIARABhAHQAZQBfAFMAdABhAHIAdAAsACAAMQAsACAAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGUAbAB0AGEAUQB1AGEAcgB0AGUAcgAsACAASQBOAEQARQBYACgAXwBxAHUAYQByAHQAZQByAEQAYQB0AGUAXwBFAG4AZAAsACAAMQAsACAAMgApACAALQAgAEkATgBEAEUAWAAoAF8AcQB1AGEAcgB0AGUAcgBEAGEAdABlAF8AUwB0AGEAcgB0ACwAIAAxACwAIAAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAaQBmAGYAUQB1AGEAcgB0AGUAcgBzACwAIAAoAF8AZABlAGwAdABhAFkAZQBhAHIAIAAqACAANAApACAAKwAgAF8AZABlAGwAdABhAFEAdQBhAHIAdABlAHIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAZQBsAHQAYQBEAGEAeQAsACAASQBOAEQARQBYACgAXwBxAHUAYQByAHQAZQByAEQAYQB0AGUAXwBFAG4AZAAsACAAMQAsACAAMwApACAALQAgAEkATgBEAEUAWAAoAF8AcQB1AGEAcgB0AGUAcgBEAGEAdABlAF8AUwB0AGEAcgB0ACwAIAAxACwAIAAzACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAArACAASQBOAEQARQBYACgAXwBqAGQAbgBMAG8AYwBhAGwAXwBFAG4AZAAsACAAMQAsACAAMgApACAALQAgAEkATgBEAEUAWAAoAF8AagBkAG4ATABvAGMAYQBsAF8AUwB0AGEAcgB0ACwAIAAxACwAIAAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBkAGUAbAB0AGEARABhAHkAIAA8ACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQBzAFEAdQBhAHIAdABlAHIAXwBTAHQAYQByAHQALAAgAEkATgBEAEUAWAAoAF8AcQB1AGEAcgB0AGUAcgBEAGEAdABlAF8AUwB0AGEAcgB0ACwAIAAxACwAIAA0ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaQBnAG4ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAaQBmAGYAUQB1AGEAcgB0AGUAcgBzACAALQAgADEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAYQB5AHMAUQB1AGEAcgB0AGUAcgBfAFMAdABhAHIAdAAgACsAIABfAGQAZQBsAHQAYQBEAGEAeQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBpAGcAbgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAaQBmAGYAUQB1AGEAcgB0AGUAcgBzACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABlAGwAdABhAEQAYQB5AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ARABFAEwAVABBAF8ASQBOAFQARQBSAFYAQQBMAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAHQAaABlACAAdABpAG0AZQBzAHAAYQBuACAAZABpAGYAZgBlAHIAZQBuAGMAZQAgAGIAZQB0AHcAZQBlAG4AIABKAHUAbABpAGEAbgAgAEQAYQB0AGUAcwAgAGkAbgAgAHQAaABlACAAcwBwAGUAYwBpAGYAaQBlAGQAIAB1AG4AaQB0AHMALgBcAG4AXABuAE8AdQB0AHAAdQB0ACAAdwBoAGUAcgBlACAAVQBuAGkAdABzACAAPQAgAEgALAAgAE4ALAAgAFMALAAgAEQALAAgAFcALAAgAE0ALAAgAFEALAAgAFkAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgAEQAZQBsAHQAYQAgAHUAbgBpAHQAcwAgAGQAZQBjAGkAbQBhAGwAXABuAFwAbgBPAHUAdABwAHUAdAAgAHcAaABlAHIAZQAgAFUAbgBpAHQAcwAgAD0AIABIAE0AUwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbAC0AMQAsADAALAAxAF0AIAB8ACAAUwBpAGcAbgBcAG4AIAAyACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADAALgAuAF0AIAAgACAAIAB8ACAARABlAGwAdABhACAAaABvAHUAcgBzAFwAbgAgADMAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMAAuAC4ANQA5AF0AIAAgAHwAIABEAGUAbAB0AGEAIABtAGkAbgB1AHQAZQBzAFwAbgAgADQAIAB8ACAAZABlAGMAaQBtAGEAbAAgAFsAMAAuAC4ANgAwACkAIAAgAHwAIABEAGUAbAB0AGEAIABzAGUAYwBvAG4AZABzAFwAbgBcAG4ATwB1AHQAcAB1AHQAIAB3AGgAZQByAGUAIABVAG4AaQB0AHMAIAA9ACAARABIAE0AUwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbAC0AMQAsADAALAAxAF0AIAB8ACAAUwBpAGcAbgBcAG4AIAAyACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADAALgAuAF0AIAAgACAAIAB8ACAARABlAGwAdABhACAAZABhAHkAcwBcAG4AIAAzACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADAALgAuADIAMwBdACAAIAB8ACAARABlAGwAdABhACAAaABvAHUAcgBzAFwAbgAgADQAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMAAuAC4ANQA5AF0AIAAgAHwAIABEAGUAbAB0AGEAIABtAGkAbgB1AHQAZQBzAFwAbgAgADUAIAB8ACAAZABlAGMAaQBtAGEAbAAgAFsAMAAuAC4ANgAwACkAIAAgAHwAIABEAGUAbAB0AGEAIABzAGUAYwBvAG4AZABzAFwAbgBcAG4ATwB1AHQAcAB1AHQAIAB3AGgAZQByAGUAIABVAG4AaQB0AHMAIAA9ACAAVwBEACwAIABNAEQALAAgAFEARABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbAC0AMQAsADAALAAxAF0AIAAgACAAIAAgAHwAIABTAGkAZwBuAFwAbgAgADIAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMAAuAC4AXQAgACAAIAAgACAAIAAgACAAfAAgAEQAZQBsAHQAYQAgAHcAZQBlAGsAcwAvAG0AbwBuAHQAaABzAC8AcQB1AGEAcgB0AGUAcgBzAFwAbgAgADMAIAB8ACAAZABlAGMAaQBtAGEAbAAgAFsAMAAuAC4ANwAvADMAMQAvADkAMgApACAAfAAgAEQAZQBsAHQAYQAgAGQAYQB5AHMAXABuAFwAbgBPAHUAdABwAHUAdAAgAHcAaABlAHIAZQAgAFUAbgBpAHQAcwAgAD0AIABZAFcARAAsACAAWQBNAEQALAAgAFkAUQBEAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsALQAxACwAMAAsADEAXQAgACAAIAAgACAAfAAgAFMAaQBnAG4AXABuACAAMgAgAHwAIABpAG4AdABlAGcAZQByACAAWwAwAC4ALgBdACAAIAAgACAAIAAgACAAIAB8ACAARABlAGwAdABhACAAeQBlAGEAcgBzAFwAbgAgADMAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMAAuAC4ANQAyAC8AMQAyAC8ANABdACAAfAAgAEQAZQBsAHQAYQAgAHcAZQBlAGsAcwAvAG0AbwBuAHQAaABzAC8AcQB1AGEAcgB0AGUAcgBzAFwAbgAgADQAIAB8ACAAZABlAGMAaQBtAGEAbAAgAFsAMAAuAC4ANwAvADMAMQAvADkAMgApACAAfAAgAEQAZQBsAHQAYQAgAGQAYQB5AHMAXABuAFwAbgBPAHUAdABwAHUAdAAgAHcAaABlAHIAZQAgAFUAbgBpAHQAcwAgAD0AIABZAE0ARABIAE0AUwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbAC0AMQAsADAALAAxAF0AIAB8ACAAUwBpAGcAbgBcAG4AIAAyACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADAALgAuAF0AIAAgACAAIAB8ACAARABlAGwAdABhACAAeQBlAGEAcgBzAFwAbgAgADMAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMAAuAC4AMQAyAF0AIAAgAHwAIABEAGUAbAB0AGEAIABtAG8AbgB0AGgAcwBcAG4AIAA0ACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADAALgAuADMAMABdACAAIAB8ACAARABlAGwAdABhACAAZABhAHkAcwBcAG4AIAA1ACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADAALgAuADIAMwBdACAAIAB8ACAARABlAGwAdABhACAAaABvAHUAcgBzAFwAbgAgADYAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMAAuAC4ANQA5AF0AIAAgAHwAIABEAGUAbAB0AGEAIABtAGkAbgB1AHQAZQBzAFwAbgAgADcAIAB8ACAAZABlAGMAaQBtAGEAbAAgAFsAMAAuAC4ANgAwACkAIAAgAHwAIABEAGUAbAB0AGEAIABzAGUAYwBvAG4AZABzAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AVQBuAGkAdABzACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAB0AGUAeAB0ACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAASAAgAC0AIABoAG8AdQByAHMAIABkAGUAYwBpAG0AYQBsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIABOACAALQAgAG0AaQBuAHUAdABlAHMAIABkAGUAYwBpAG0AYQBsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIABTACAALQAgAHMAZQBjAG8AbgBkAHMAIABkAGUAYwBpAG0AYQBsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIABEACAALQAgAGQAYQB5AHMAIABkAGUAYwBpAG0AYQBsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIABXACAALQAgAHcAZQBlAGsAcwAgAGQAZQBjAGkAbQBhAGwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgAE0AIAAtACAAbQBvAG4AdABoAHMAIABkAGUAYwBpAG0AYQBsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIABRACAALQAgAHEAdQBhAHIAdABlAHIAcwAgAGQAZQBjAGkAbQBhAGwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgAFkAIAAtACAAeQBlAGEAcgBzACAAZABlAGMAaQBtAGEAbABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIABIAE0AUwAgAC0AIABoAG8AdQByAHMALAAgAG0AaQBuAHUAdABlAHMALAAgAHMAZQBjAG8AbgBkAHMAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgAEQASABNAFMAIAAtACAAZABhAHkAcwAsACAAaABvAHUAcgBzACwAIABtAGkAbgB1AHQAZQBzACwAIABzAGUAYwBvAG4AZABzAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAVwBEACAALQAgAHcAZQBlAGsAcwAgAGEAbgBkACAAZABhAHkAcwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgAE0ARAAgAC0AIABtAG8AbgB0AGgAcwAgAGEAbgBkACAAZABhAHkAcwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgAFEARAAgAC0AIABxAHUAYQByAHQAZQByAHMAIABhAG4AZAAgAGQAYQB5AHMAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAWQBXAEQAIAAtACAAeQBlAGEAcgBzACwAIAB3AGUAZQBrAHMALAAgAGQAYQB5AHMAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAWQBNAEQAIAAtACAAeQBlAGEAcgBzACwAIABtAG8AbgB0AGgAcwAsACAAZABhAHkAcwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIABZAFEARAAgAC0AIAB5AGUAYQByAHMALAAgAHEAdQBhAHIAdABlAHIAcwAsACAAZABhAHkAcwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABZAE0ARABIAE0AUwAgAC0AIAB5AGUAYQByAHMALAAgAG0AbwBuAHQAaABzACwAIABkAGEAeQBzACwAIABoAG8AdQByAHMALAAgAG0AaQBuAHUAdABlAHMALAAgAHMAZQBjAG8AbgBkAHMAXABuAEoARABhAHQAZQAxACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgACAAIAAgACAAIAAgACAAIAB8ACAAXABuAEoARABhAHQAZQAyACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgACAAIAAgACAAIAAgACAAIAB8ACAAXABuAFsAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0AF0AIAB8ACAAZABlAGMAaQBtAGEAbAAgACAAIAAgACAAIAAgACAAIAB8ACAAVABpAG0AZQAgAHoAbwBuAGUAIABvAGYAZgBzAGUAdAAgAGkAbgAgAG0AaQBuAHUAdABlAHMAIABmAHIAbwBtACAAVQBUAEMALgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABbAC0AOQAwADAALgAuADkAMAAwAF0AIAAgACAAIAAgAHwAIABBAHMAcwB1AG0AZQBkACAAdABvACAAYgBlACAAVQBUAEMAIABpAGYAIABvAG0AbQBpAHQAdABlAGQALgBcAG4AWwBNAG8AbgB0AGgATwBmAGYAcwBlAHQAXQAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAWwAtADYALgAuADMAXQAgAHwAIABRAHUAYQByAHQAZQByACAAbQBvAG4AdABoACAAbwBmAGYAcwBlAHQAIABmAHIAbwBtACAASgBhAG4AdQBhAHIAeQAuAFwAbgBbAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACAAfAAgAHMAdwBpAHQAYwBoACAAIAAgACAAIAAgACAAIAAgACAAfAAgAEMAYQBsAGMAdQBsAGEAdABlACAAaQBuACAAdABoAGUAIABKAHUAbABpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AIABEAGUAZgBhAHUAbAB0ACAAaQBzACAARwByAGUAZwBvAHIAaQBhAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ARABFAEwAVABBAF8ASQBOAFQARQBSAFYAQQBMACAAPQAgAEwAQQBNAEIARABBACgAVQBuAGkAdABzACwAIABKAEQAYQB0AGUAMQAsACAASgBEAGEAdABlADIALAAgAFsAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0AF0ALAAgAFsATQBvAG4AdABoAE8AZgBmAHMAZQB0AF0ALAAgAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0ALABcAG4AIAAgACAAIABJAEYAUwAoAFwAbgAgACAAIAAgACAAIAAgACAAVQBuAGkAdABzACAAPQAgAFwAIgBcACIALAAgAHsAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIABVAG4AaQB0AHMAIAA9ACAAXAAiAEgAXAAiACwAIABEAEUATABUAEEAXwBIAE8AVQBSAFMAKABKAEQAYQB0AGUAMQAsACAASgBEAGEAdABlADIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAVQBuAGkAdABzACAAPQAgAFwAIgBOAFwAIgAsACAARABFAEwAVABBAF8ATQBJAE4AVQBUAEUAUwAoAEoARABhAHQAZQAxACwAIABKAEQAYQB0AGUAMgApACwAXABuACAAIAAgACAAIAAgACAAIABVAG4AaQB0AHMAIAA9ACAAXAAiAFMAXAAiACwAIABEAEUATABUAEEAXwBTAEUAQwBPAE4ARABTACgASgBEAGEAdABlADEALAAgAEoARABhAHQAZQAyACkALABcAG4AIAAgACAAIAAgACAAIAAgAFUAbgBpAHQAcwAgAD0AIABcACIASABNAFMAXAAiACwAIABEAEUATABUAEEAXwBIAE8AVQBSAF8ATQBJAE4AXwBTAEUAQwAoAEoARABhAHQAZQAxACwAIABKAEQAYQB0AGUAMgApACwAXABuACAAIAAgACAAIAAgACAAIABVAG4AaQB0AHMAIAA9ACAAXAAiAEQAXAAiACwAIABEAEUATABUAEEAXwBEAEEAWQBTACgASgBEAGEAdABlADEALAAgAEoARABhAHQAZQAyACkALABcAG4AIAAgACAAIAAgACAAIAAgAFUAbgBpAHQAcwAgAD0AIABcACIAVwBcACIALAAgAEQARQBMAFQAQQBfAFcARQBFAEsAUwAoAEoARABhAHQAZQAxACwAIABKAEQAYQB0AGUAMgApACwAXABuACAAIAAgACAAIAAgACAAIABVAG4AaQB0AHMAIAA9ACAAXAAiAE0AXAAiACwAIABEAEUATABUAEEAXwBNAE8ATgBUAEgAUwAoAEoARABhAHQAZQAxACwAIABKAEQAYQB0AGUAMgAsACAAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0ACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAVQBuAGkAdABzACAAPQAgAFwAIgBRAFwAIgAsACAARABFAEwAVABBAF8AUQBVAEEAUgBUAEUAUgBTACgASgBEAGEAdABlADEALAAgAEoARABhAHQAZQAyACwAIABUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQALAAgAE0AbwBuAHQAaABPAGYAZgBzAGUAdAAsACAASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByACkALABcAG4AIAAgACAAIAAgACAAIAAgAFUAbgBpAHQAcwAgAD0AIABcACIAWQBcACIALAAgAEQARQBMAFQAQQBfAFkARQBBAFIAUwAoAEoARABhAHQAZQAxACwAIABKAEQAYQB0AGUAMgAsACAAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0ACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAVQBuAGkAdABzACAAPQAgAFwAIgBXAEQAXAAiACwAIABEAEUATABUAEEAXwBXAEUARQBLAF8ARABBAFkAUwAoAEoARABhAHQAZQAxACwAIABKAEQAYQB0AGUAMgApACwAXABuACAAIAAgACAAIAAgACAAIABVAG4AaQB0AHMAIAA9ACAAXAAiAFkAVwBEAFwAIgAsACAARABFAEwAVABBAF8AWQBFAEEAUgBfAFcARQBFAEsAXwBEAEEAWQBTACgASgBEAGEAdABlADEALAAgAEoARABhAHQAZQAyACwAIABUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQALAAgAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgApACwAXABuACAAIAAgACAAIAAgACAAIABVAG4AaQB0AHMAIAA9ACAAXAAiAE0ARABcACIALAAgAEQARQBMAFQAQQBfAE0ATwBOAFQASABfAEQAQQBZAFMAKABKAEQAYQB0AGUAMQAsACAASgBEAGEAdABlADIALAAgAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdAAsACAASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByACkALABcAG4AIAAgACAAIAAgACAAIAAgAFUAbgBpAHQAcwAgAD0AIABcACIAUQBEAFwAIgAsACAARABFAEwAVABBAF8AUQBVAEEAUgBUAEUAUgBfAEQAQQBZAFMAKABKAEQAYQB0AGUAMQAsACAASgBEAGEAdABlADIALAAgAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdAAsACAATQBvAG4AdABoAE8AZgBmAHMAZQB0ACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAVQBuAGkAdABzACAAPQAgAFwAIgBEAEgATQBTAFwAIgAsACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGgAbQBzACwAIABEAEUATABUAEEAXwBIAE8AVQBSAF8ATQBJAE4AXwBTAEUAQwAoAEoARABhAHQAZQAxACwAIABKAEQAYQB0AGUAMgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQBzACwAIABJAE4AVAAoAEkATgBEAEUAWAAoAF8AaABtAHMALAAgADEALAAgADIAKQAgAC8AIAAyADQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AaABvAHUAcgBzACwAIABJAE4ARABFAFgAKABfAGgAbQBzACwAIAAxACwAIAAyACkAIAAtACAAXwBkAGEAeQBzACAAKgAgADIANAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAE4ARABFAFgAKABfAGgAbQBzACwAIAAxACwAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkAcwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBoAG8AdQByAHMALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkATgBEAEUAWAAoAF8AaABtAHMALAAgADEALAAgADMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBOAEQARQBYACgAXwBoAG0AcwAsACAAMQAsACAANAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgAFUAbgBpAHQAcwAgAD0AIABcACIAWQBNAEQAXAAiACwAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbQBvAG4AdABoAEQAYQB5AHMALAAgAEQARQBMAFQAQQBfAE0ATwBOAFQASABfAEQAQQBZAFMAKABKAEQAYQB0AGUAMQAsACAASgBEAGEAdABlADIALAAgAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdAAsACAASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIAcwAsACAASQBOAFQAKABJAE4ARABFAFgAKABfAG0AbwBuAHQAaABEAGEAeQBzACwAIAAxACwAIAAyACkAIAAvACAAMQAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AbwBuAHQAaABzACwAIABJAE4ARABFAFgAKABfAG0AbwBuAHQAaABEAGEAeQBzACwAIAAxACwAIAAyACkAIAAtACAAXwB5AGUAYQByAHMAIAAqACAAMQAyACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkATgBEAEUAWAAoAF8AbQBvAG4AdABoAEQAYQB5AHMALAAgADEALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AGUAYQByAHMALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbQBvAG4AdABoAHMALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkATgBEAEUAWAAoAF8AbQBvAG4AdABoAEQAYQB5AHMALAAgADEALAAgADMAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIABVAG4AaQB0AHMAIAA9ACAAXAAiAFkAUQBEAFwAIgAsACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHEAdQBhAHIAdABlAHIARABhAHkAcwAsACAARABFAEwAVABBAF8AUQBVAEEAUgBUAEUAUgBfAEQAQQBZAFMAKABKAEQAYQB0AGUAMQAsACAASgBEAGEAdABlADIALAAgAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdAAsACAASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIAcwAsACAASQBOAFQAKABJAE4ARABFAFgAKABfAHEAdQBhAHIAdABlAHIARABhAHkAcwAsACAAMQAsACAAMgApACAALwAgADQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcQB1AGEAcgB0AGUAcgBzACwAIABJAE4ARABFAFgAKABfAHEAdQBhAHIAdABlAHIARABhAHkAcwAsACAAMQAsACAAMgApACAALQAgAF8AeQBlAGEAcgBzACAAKgAgADQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBOAEQARQBYACgAXwBxAHUAYQByAHQAZQByAEQAYQB5AHMALAAgADEALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AGUAYQByAHMALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcQB1AGEAcgB0AGUAcgBzACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAE4ARABFAFgAKABfAHEAdQBhAHIAdABlAHIARABhAHkAcwAsACAAMQAsACAAMwApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgAFUAbgBpAHQAcwAgAD0AIABcACIAWQBNAEQASABNAFMAXAAiACwAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbQBvAG4AdABoAEQAYQB5AHMALAAgAEQARQBMAFQAQQBfAE0ATwBOAFQASABfAEQAQQBZAFMAKABKAEQAYQB0AGUAMQAsACAASgBEAGEAdABlADIALAAgAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdAAsACAASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIAcwAsACAASQBOAFQAKABJAE4ARABFAFgAKABfAG0AbwBuAHQAaABEAGEAeQBzACwAIAAxACwAIAAyACkAIAAvACAAMQAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AbwBuAHQAaABzACwAIABJAE4ARABFAFgAKABfAG0AbwBuAHQAaABEAGEAeQBzACwAIAAxACwAIAAyACkAIAAtACAAXwB5AGUAYQByAHMAIAAqACAAMQAyACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQBzACwAIABJAE4AVAAoAEkATgBEAEUAWAAoAF8AbQBvAG4AdABoAEQAYQB5AHMALAAgADEALAAgADMAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AGkAbQBlACwAIABJAE4ARABFAFgAKABfAG0AbwBuAHQAaABEAGEAeQBzACwAIAAxACwAIAAzACkAIAAtACAAXwBkAGEAeQBzACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBoAG0AcwAsACAAVABJAE0ARQBfAEQARQBDAEkATQBBAEwAXwBUAE8AXwBIAE0AUwAoAF8AdABpAG0AZQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkATgBEAEUAWAAoAF8AbQBvAG4AdABoAEQAYQB5AHMALAAgADEALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AGUAYQByAHMALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbQBvAG4AdABoAHMALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkAcwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAARABSAE8AUAAoAF8AaABtAHMALAAsACAAMQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALAAgAHsAIwBWAEEATABVAEUAIQB9AFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAFwAbgBcAG4AXABuAFwAbgBcAG4AXABuAFwAbgBcAG4AXABuAFwAbgBcAG4ALwAqACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwBcAG4AIwAgAEUAWABUAEUATgBUAFMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACoALwBcAG4AXABuAFwAbgBcAG4AXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBFAFgAVABFAE4AVABfAE8ARgBfAEQAQQBZAFMAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIABpAG4AYwBsAHUAcwBpAHYAZQAgAGUAeAB0AGUAbgB0ACAAbwBmACAAZABhAHkAcwAgAHMAcABhAG4AbgBlAGQAIABiAHkAIAB0AHcAbwAgAEoAdQBsAGkAYQBuACAARABhAHQAZQBzAC4AXABuAFwAbgBPAHUAdABwAHUAdABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAARQB4AHQAZQBuAHQAIABvAGYAIABkAGEAeQBzAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ASgBEAGEAdABlADEAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAIAAgACAAIAB8ACAAXABuAEoARABhAHQAZQAyACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgACAAIAAgACAAfAAgAFwAbgBbAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdABdACAAfAAgAGQAZQBjAGkAbQBhAGwAIAAgACAAIAAgAHwAIABUAGkAbQBlACAAegBvAG4AZQAgAG8AZgBmAHMAZQB0ACAAaQBuACAAbQBpAG4AdQB0AGUAcwAgAGYAcgBvAG0AIABVAFQAQwAuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAFsALQA5ADAAMAAuAC4AOQAwADAAXQAgAHwAIABBAHMAcwB1AG0AZQBkACAAdABvACAAYgBlACAAVQBUAEMAIABpAGYAIABvAG0AbQBpAHQAdABlAGQALgBcAG4AXABuAEUAeABhAG0AcABsAGUAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ARQBYAFQARQBOAFQAXwBEAEEAWQBTACgASgBVAEwASQBBAE4AXwBEAEEAVABFACgAMgAwADIAMwAsADEALAAxACwAVABJAE0ARQAoADIAMwAsADUAOQAsADUANQApACkALAAgAEoAVQBMAEkAQQBOAF8ARABBAFQARQAoADIAMAAyADMALAAxACwAMgAsAFQASQBNAEUAKAAwACwAMAAsADUAKQApACkAXABuAD0AIAAyACAAIABpAC4AZQAuACAAMgAgAGQAYQB5AHMAIABiAGUAYwBhAHUAcwBlACAAdABoAGUAIAAxADAAIABzAGUAYwBvAG4AZAAgAHQAaQBtAGUAcwBwAGEAbgAgAGMAcgBvAHMAcwBlAHMAIAB0AGgAZQAgAGQAYQB5ACAAYgBvAHUAbgBkAGEAcgB5AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBFAFgAVABFAE4AVABfAE8ARgBfAEQAQQBZAFMAIAA9ACAATABBAE0AQgBEAEEAKABKAEQAYQB0AGUAMQAsACAASgBEAGEAdABlADIALAAgAFsAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0AF0ALABcAG4AIAAgACAAIABJAEYAKAAoAEoARABhAHQAZQAxACAAPQAgAFwAIgBcACIAKQAgACoAIAAoAEoARABhAHQAZQAyACAAPQAgAFwAIgBcACIAKQAsACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABKAEQAYQB0AGUAMQApACkAIAArACAATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABKAEQAYQB0AGUAMgApACkALAAgAHsAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AHoAbwAsACAATgAoAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAQQBCAFMAKABfAHQAegBvACkAIAA+ACAAOQAwADAALAAgAHsAIwBOAFUATQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBpAGcAbgAsACAASQBGACgASgBEAGEAdABlADIAIAA+AD0AIABKAEQAYQB0AGUAMQAsACAAMQAsACAALQAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBqAGQAbgBMAG8AYwBhAGwAMQAsACAASgBEAEEAVABFAF8AVABPAF8ASgBEAE4AXwBMAE8AQwBBAEwAKABKAEQAYQB0AGUAMQAsACAAXwB0AHoAbwApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AagBkAG4ATABvAGMAYQBsADIALAAgAEoARABBAFQARQBfAFQATwBfAEoARABOAF8ATABPAEMAQQBMACgASgBEAGEAdABlADIALAAgAF8AdAB6AG8AKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAZQBsAHQAYQBEAGEAeQAsACAASQBOAEQARQBYACgAXwBqAGQAbgBMAG8AYwBhAGwAMgAsACAAMQAsACAAMQApACAALQAgAEkATgBEAEUAWAAoAF8AagBkAG4ATABvAGMAYQBsADEALAAgADEALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaQBnAG4AIAAqACAAKABBAEIAUwAoAF8AZABlAGwAdABhAEQAYQB5ACkAIAArACAAMQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEUAWABUAEUATgBUAF8ATwBGAF8AVwBFAEUASwBTAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAHQAaABlACAAaQBuAGMAbAB1AHMAaQB2AGUAIABlAHgAdABlAG4AdAAgAG8AZgAgAHcAZQBlAGsAcwAgAHMAcABhAG4AbgBlAGQAIABiAHkAIAB0AHcAbwAgAEoAdQBsAGkAYQBuACAARABhAHQAZQBzAC4AXABuAFwAbgBPAHUAdABwAHUAdABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAARQB4AHQAZQBuAHQAIABvAGYAIAB3AGUAZQBrAHMAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBKAEQAYQB0AGUAMQAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAAgACAAIAAgAHwAIABcAG4ASgBEAGEAdABlADIAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAIAAgACAAIAB8ACAAXABuAFsAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0AF0AIAB8ACAAZABlAGMAaQBtAGEAbAAgACAAIAAgACAAfAAgAFQAaQBtAGUAIAB6AG8AbgBlACAAbwBmAGYAcwBlAHQAIABpAG4AIABtAGkAbgB1AHQAZQBzACAAZgByAG8AbQAgAFUAVABDAC4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAWwAtADkAMAAwAC4ALgA5ADAAMABdACAAfAAgAEEAcwBzAHUAbQBlAGQAIAB0AG8AIABiAGUAIABVAFQAQwAgAGkAZgAgAG8AbQBtAGkAdAB0AGUAZAAuAFwAbgBcAG4ARQB4AGEAbQBwAGwAZQBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBFAFgAVABFAE4AVABfAEQAQQBZAFMAKABKAFUATABJAEEATgBfAEQAQQBUAEUAKAAyADAAMgAzACwANgAsADQALABUAEkATQBFACgAMgAzACwANQA5ACwANQA1ACkAKQAsACAASgBVAEwASQBBAE4AXwBEAEEAVABFACgAMgAwADIAMwAsADYALAA1ACwAVABJAE0ARQAoADAALAAwACwANQApACkAKQBcAG4APQAgADIAIAAgAGkALgBlAC4AIAAyACAAdwBlAGUAawBzACAAYgBlAGMAYQB1AHMAZQAgAHQAaABlACAAMQAwACAAcwBlAGMAbwBuAGQAIAB0AGkAbQBlAHMAcABhAG4AIABjAHIAbwBzAHMAZQBzACAAdABoAGUAIAB3AGUAZQBrACAAYgBvAHUAbgBkAGEAcgB5AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBFAFgAVABFAE4AVABfAE8ARgBfAFcARQBFAEsAUwAgAD0AIABMAEEATQBCAEQAQQAoAEoARABhAHQAZQAxACwAIABKAEQAYQB0AGUAMgAsACAAWwBUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQAXQAsAFwAbgAgACAAIAAgAEkARgAoACgASgBEAGEAdABlADEAIAA9ACAAXAAiAFwAIgApACAAKgAgACgASgBEAGEAdABlADIAIAA9ACAAXAAiAFwAIgApACwAIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEoARABhAHQAZQAxACkAKQAgACsAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEoARABhAHQAZQAyACkAKQAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBvACwAIABOACgAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABBAEIAUwAoAF8AdAB6AG8AKQAgAD4AIAA5ADAAMAAsACAAewAjAE4AVQBNACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGkAZwBuACwAIABJAEYAKABKAEQAYQB0AGUAMgAgAD4APQAgAEoARABhAHQAZQAxACwAIAAxACwAIAAtADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGoAZABuAEwAbwBjAGEAbABfAFMAdABhAHIAdAAsACAASgBEAEEAVABFAF8AVABPAF8ASgBEAE4AXwBMAE8AQwBBAEwAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAHMAaQBnAG4AIAA9ACAAMQAsACAASgBEAGEAdABlADEALAAgAEoARABhAHQAZQAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBvAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AagBkAG4ATABvAGMAYQBsAF8ARQBuAGQALAAgAEoARABBAFQARQBfAFQATwBfAEoARABOAF8ATABPAEMAQQBMACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBzAGkAZwBuACAAPQAgADEALAAgAEoARABhAHQAZQAyACwAIABKAEQAYQB0AGUAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AHoAbwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGoAZABuAE0AbwBuAGQAYQB5AF8AUwB0AGEAcgB0ACwAIABJAE4ARABFAFgAKABfAGoAZABuAEwAbwBjAGEAbABfAFMAdABhAHIAdAAsACAAMQAsACAAMQApACAAKwAgADEAIAAtACAARABBAFkAXwBPAEYAXwBXAEUARQBLACgASQBOAEQARQBYACgAXwBqAGQAbgBMAG8AYwBhAGwAXwBTAHQAYQByAHQALAAgADEALAAgADEAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AagBkAG4ATQBvAG4AZABhAHkAXwBFAG4AZAAsACAASQBOAEQARQBYACgAXwBqAGQAbgBMAG8AYwBhAGwAXwBFAG4AZAAsACAAMQAsACAAMQApACAAKwAgADEAIAAtACAARABBAFkAXwBPAEYAXwBXAEUARQBLACgASQBOAEQARQBYACgAXwBqAGQAbgBMAG8AYwBhAGwAXwBFAG4AZAAsACAAMQAsACAAMQApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGkAZwBuACAAKgAgAEkATgBUACgAKABfAGoAZABuAE0AbwBuAGQAYQB5AF8ARQBuAGQAIAAtACAAXwBqAGQAbgBNAG8AbgBkAGEAeQBfAFMAdABhAHIAdAApACAALwAgADcAIAArACAAMQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ARQBYAFQARQBOAFQAXwBPAEYAXwBNAE8ATgBUAEgAUwBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAGkAbgBjAGwAdQBzAGkAdgBlACAAZQB4AHQAZQBuAHQAIABvAGYAIABtAG8AbgB0AGgAcwAgAHMAcABhAG4AbgBlAGQAIABiAHkAIAB0AHcAbwAgAEoAdQBsAGkAYQBuACAARABhAHQAZQBzAC4AXABuAFwAbgBPAHUAdABwAHUAdABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAARQB4AHQAZQBuAHQAIABvAGYAIABtAG8AbgB0AGgAcwBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEoARABhAHQAZQAxACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgACAAIAAgACAAfABcAG4ASgBEAGEAdABlADIAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAIAAgACAAIAB8AFwAbgBbAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdABdACAAfAAgAGQAZQBjAGkAbQBhAGwAIAAgACAAIAAgAHwAIABUAGkAbQBlACAAegBvAG4AZQAgAG8AZgBmAHMAZQB0ACAAaQBuACAAbQBpAG4AdQB0AGUAcwAgAGYAcgBvAG0AIABVAFQAQwAuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAFsALQA5ADAAMAAuAC4AOQAwADAAXQAgAHwAIABBAHMAcwB1AG0AZQBkACAAdABvACAAYgBlACAAVQBUAEMAIABpAGYAIABvAG0AbQBpAHQAdABlAGQALgBcAG4AWwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAgAHwAIABzAHcAaQB0AGMAaAAgACAAIAAgACAAIAB8ACAAQwBhAGwAYwB1AGwAYQB0AGUAIABpAG4AIAB0AGgAZQAgAEoAdQBsAGkAYQBuACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgAgAEQAZQBmAGEAdQBsAHQAIABpAHMAIABHAHIAZQBnAG8AcgBpAGEAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ARQBYAFQARQBOAFQAXwBPAEYAXwBNAE8ATgBUAEgAUwAgAD0AIABMAEEATQBCAEQAQQAoAEoARABhAHQAZQAxACwAIABKAEQAYQB0AGUAMgAsACAAWwBUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQAXQAsACAAWwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAsAFwAbgAgACAAIAAgAEkARgAoACgASgBEAGEAdABlADEAIAA9ACAAXAAiAFwAIgApACAAKgAgACgASgBEAGEAdABlADIAIAA9ACAAXAAiAFwAIgApACwAIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEoARABhAHQAZQAxACkAKQAgACsAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEoARABhAHQAZQAyACkAKQAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBvACwAIABOACgAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABBAEIAUwAoAF8AdAB6AG8AKQAgAD4AIAA5ADAAMAAsACAAewAjAE4AVQBNACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGkAZwBuACwAIABJAEYAKABKAEQAYQB0AGUAMgAgAD4APQAgAEoARABhAHQAZQAxACwAIAAxACwAIAAtADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGoAZABuAEwAbwBjAGEAbABfAFMAdABhAHIAdAAsACAASgBEAEEAVABFAF8AVABPAF8ASgBEAE4AXwBMAE8AQwBBAEwAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAHMAaQBnAG4AIAA9ACAAMQAsACAASgBEAGEAdABlADEALAAgAEoARABhAHQAZQAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBvAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AagBkAG4ATABvAGMAYQBsAF8ARQBuAGQALAAgAEoARABBAFQARQBfAFQATwBfAEoARABOAF8ATABPAEMAQQBMACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBzAGkAZwBuACAAPQAgADEALAAgAEoARABhAHQAZQAyACwAIABKAEQAYQB0AGUAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AHoAbwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAYQB0AGUAXwBTAHQAYQByAHQALAAgAEoARABOAF8AVABPAF8AQwBBAEwARQBOAEQAQQBSAF8ARABBAFQARQAoAEkATgBEAEUAWAAoAF8AagBkAG4ATABvAGMAYQBsAF8AUwB0AGEAcgB0ACwAIAAxACwAIAAxACkALAAgAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHQAZQBfAEUAbgBkACwAIABKAEQATgBfAFQATwBfAEMAQQBMAEUATgBEAEEAUgBfAEQAQQBUAEUAKABJAE4ARABFAFgAKABfAGoAZABuAEwAbwBjAGEAbABfAEUAbgBkACwAIAAxACwAIAAxACkALAAgAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABlAGwAdABhAFkAZQBhAHIALAAgAEkATgBEAEUAWAAoAF8AZABhAHQAZQBfAEUAbgBkACwAIAAxACwAIAAxACkAIAAtACAASQBOAEQARQBYACgAXwBkAGEAdABlAF8AUwB0AGEAcgB0ACwAIAAxACwAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGUAbAB0AGEATQBvAG4AdABoACwAIABJAE4ARABFAFgAKABfAGQAYQB0AGUAXwBFAG4AZAAsACAAMQAsACAAMgApACAALQAgAEkATgBEAEUAWAAoAF8AZABhAHQAZQBfAFMAdABhAHIAdAAsACAAMQAsACAAMgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABpAGYAZgBNAG8AbgB0AGgAcwAsACAAKABfAGQAZQBsAHQAYQBZAGUAYQByACAAKgAgADEAMgApACAAKwAgAF8AZABlAGwAdABhAE0AbwBuAHQAaAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaQBnAG4AIAAqACAAKABfAGQAaQBmAGYATQBvAG4AdABoAHMAIAArACAAMQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ARQBYAFQARQBOAFQAXwBPAEYAXwBRAFUAQQBSAFQARQBSAFMAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIABpAG4AYwBsAHUAcwBpAHYAZQAgAGUAeAB0AGUAbgB0ACAAbwBmACAAcQB1AGEAcgB0AGUAcgBzACAAcwBwAGEAbgBuAGUAZAAgAGIAeQAgAHQAdwBvACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIABFAHgAdABlAG4AdAAgAG8AZgAgAHEAdQBhAHIAdABlAHIAcwBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEoARABhAHQAZQAxACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgACAAIAAgACAAIAAgACAAIAB8AFwAbgBKAEQAYQB0AGUAMgAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAAgACAAIAAgACAAIAAgACAAfABcAG4AWwBUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQAXQAgAHwAIABkAGUAYwBpAG0AYQBsACAAIAAgACAAIAAgACAAIAAgAHwAIABUAGkAbQBlACAAegBvAG4AZQAgAG8AZgBmAHMAZQB0ACAAaQBuACAAbQBpAG4AdQB0AGUAcwAgAGYAcgBvAG0AIABVAFQAQwAuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAFsALQA5ADAAMAAuAC4AOQAwADAAXQAgACAAIAAgACAAfAAgAEEAcwBzAHUAbQBlAGQAIAB0AG8AIABiAGUAIABVAFQAQwAgAGkAZgAgAG8AbQBtAGkAdAB0AGUAZAAuAFwAbgBbAE0AbwBuAHQAaABPAGYAZgBzAGUAdABdACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbAC0ANgAuAC4AMwBdACAAfAAgAFEAdQBhAHIAdABlAHIAIABtAG8AbgB0AGgAIABvAGYAZgBzAGUAdAAgAGYAcgBvAG0AIABKAGEAbgB1AGEAcgB5AC4AXABuAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0AIAB8ACAAcwB3AGkAdABjAGgAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAQwBhAGwAYwB1AGwAYQB0AGUAIABpAG4AIAB0AGgAZQAgAEoAdQBsAGkAYQBuACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgAgAEQAZQBmAGEAdQBsAHQAIABpAHMAIABHAHIAZQBnAG8AcgBpAGEAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBFAFgAVABFAE4AVABfAE8ARgBfAFEAVQBBAFIAVABFAFIAUwAgAD0AIABMAEEATQBCAEQAQQAoAEoARABhAHQAZQAxACwAIABKAEQAYQB0AGUAMgAsACAAWwBUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQAXQAsACAAWwBNAG8AbgB0AGgATwBmAGYAcwBlAHQAXQAsACAAWwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAsAFwAbgAgACAAIAAgAEkARgAoACgASgBEAGEAdABlADEAIAA9ACAAXAAiAFwAIgApACAAKgAgACgASgBEAGEAdABlADIAIAA9ACAAXAAiAFwAIgApACwAIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEoARABhAHQAZQAxACkAKQAgACsAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEoARABhAHQAZQAyACkAKQAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBvACwAIABOACgAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AbwBuAHQAaABPAGYAZgBzAGUAdAAsACAAUgBPAFUATgBEACgATgAoAE0AbwBuAHQAaABPAGYAZgBzAGUAdAApACwAIAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKAAoAEEAQgBTACgAXwB0AHoAbwApACAAPgAgADkAMAAwACkAIAArACAAKABfAG0AbwBuAHQAaABPAGYAZgBzAGUAdAAgADwAIAAtADYAKQAgACsAIAAoAF8AbQBvAG4AdABoAE8AZgBmAHMAZQB0ACAAPgAgADMAKQAsACAAewAjAE4AVQBNACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGkAZwBuACwAIABJAEYAKABKAEQAYQB0AGUAMgAgAD4APQAgAEoARABhAHQAZQAxACwAIAAxACwAIAAtADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGoAZABuAEwAbwBjAGEAbABfAFMAdABhAHIAdAAsACAASgBEAEEAVABFAF8AVABPAF8ASgBEAE4AXwBMAE8AQwBBAEwAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAHMAaQBnAG4AIAA9ACAAMQAsACAASgBEAGEAdABlADEALAAgAEoARABhAHQAZQAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBvAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AagBkAG4ATABvAGMAYQBsAF8ARQBuAGQALAAgAEoARABBAFQARQBfAFQATwBfAEoARABOAF8ATABPAEMAQQBMACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBzAGkAZwBuACAAPQAgADEALAAgAEoARABhAHQAZQAyACwAIABKAEQAYQB0AGUAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AHoAbwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHEAdQBhAHIAdABlAHIARABhAHQAZQBfAFMAdABhAHIAdAAsACAASgBEAE4AXwBUAE8AXwBRAFUAQQBSAFQARQBSAF8ARABBAFQARQAoAEkATgBEAEUAWAAoAF8AagBkAG4ATABvAGMAYQBsAF8AUwB0AGEAcgB0ACwAIAAxACwAIAAxACkALAAgAF8AbQBvAG4AdABoAE8AZgBmAHMAZQB0ACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHEAdQBhAHIAdABlAHIARABhAHQAZQBfAEUAbgBkACwAIABKAEQATgBfAFQATwBfAFEAVQBBAFIAVABFAFIAXwBEAEEAVABFACgASQBOAEQARQBYACgAXwBqAGQAbgBMAG8AYwBhAGwAXwBFAG4AZAAsACAAMQAsACAAMQApACwAIABfAG0AbwBuAHQAaABPAGYAZgBzAGUAdAAsACAASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGUAbAB0AGEAWQBlAGEAcgAsACAASQBOAEQARQBYACgAXwBxAHUAYQByAHQAZQByAEQAYQB0AGUAXwBFAG4AZAAsACAAMQAsACAAMQApACAALQAgAEkATgBEAEUAWAAoAF8AcQB1AGEAcgB0AGUAcgBEAGEAdABlAF8AUwB0AGEAcgB0ACwAIAAxACwAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGUAbAB0AGEAUQB1AGEAcgB0AGUAcgAsACAASQBOAEQARQBYACgAXwBxAHUAYQByAHQAZQByAEQAYQB0AGUAXwBFAG4AZAAsACAAMQAsACAAMgApACAALQAgAEkATgBEAEUAWAAoAF8AcQB1AGEAcgB0AGUAcgBEAGEAdABlAF8AUwB0AGEAcgB0ACwAIAAxACwAIAAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGkAZgBmAFEAdQBhAHIAdABlAHIAcwAsACAAKABfAGQAZQBsAHQAYQBZAGUAYQByACAAKgAgADQAKQAgACsAIABfAGQAZQBsAHQAYQBRAHUAYQByAHQAZQByACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBpAGcAbgAgACoAIAAoAF8AZABpAGYAZgBRAHUAYQByAHQAZQByAHMAIAArACAAMQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ARQBYAFQARQBOAFQAXwBPAEYAXwBZAEUAQQBSAFMAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIABpAG4AYwBsAHUAcwBpAHYAZQAgAGUAeAB0AGUAbgB0ACAAbwBmACAAeQBlAGEAcgBzACAAcwBwAGEAbgBuAGUAZAAgAGIAeQAgAHQAdwBvACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIABFAHgAdABlAG4AdAAgAG8AZgAgAHEAdQBhAHIAdABlAHIAcwBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEoARABhAHQAZQAxACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgACAAIAAgACAAIAAgACAAIAB8AFwAbgBKAEQAYQB0AGUAMgAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAAgACAAIAAgACAAIAAgACAAfABcAG4AWwBUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQAXQAgAHwAIABkAGUAYwBpAG0AYQBsACAAIAAgACAAIAAgACAAIAAgAHwAIABUAGkAbQBlACAAegBvAG4AZQAgAG8AZgBmAHMAZQB0ACAAaQBuACAAbQBpAG4AdQB0AGUAcwAgAGYAcgBvAG0AIABVAFQAQwAuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAFsALQA5ADAAMAAuAC4AOQAwADAAXQAgACAAIAAgACAAfAAgAEEAcwBzAHUAbQBlAGQAIAB0AG8AIABiAGUAIABVAFQAQwAgAGkAZgAgAG8AbQBtAGkAdAB0AGUAZAAuAFwAbgBbAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACAAfAAgAHMAdwBpAHQAYwBoACAAIAAgACAAIAAgACAAIAAgACAAfAAgAEMAYQBsAGMAdQBsAGEAdABlACAAaQBuACAAdABoAGUAIABKAHUAbABpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AIABEAGUAZgBhAHUAbAB0ACAAaQBzACAARwByAGUAZwBvAHIAaQBhAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ARQBYAFQARQBOAFQAXwBPAEYAXwBZAEUAQQBSAFMAIAA9ACAATABBAE0AQgBEAEEAKABKAEQAYQB0AGUAMQAsACAASgBEAGEAdABlADIALAAgAFsAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0AF0ALAAgAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0ALABcAG4AIAAgACAAIABJAEYAKAAoAEoARABhAHQAZQAxACAAPQAgAFwAIgBcACIAKQAgACoAIAAoAEoARABhAHQAZQAyACAAPQAgAFwAIgBcACIAKQAsACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABKAEQAYQB0AGUAMQApACkAIAArACAATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABKAEQAYQB0AGUAMgApACkALAAgAHsAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AHoAbwAsACAATgAoAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAKABBAEIAUwAoAF8AdAB6AG8AKQAgAD4AIAA5ADAAMAApACwAIAB7ACMATgBVAE0AIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaQBnAG4ALAAgAEkARgAoAEoARABhAHQAZQAyACAAPgA9ACAASgBEAGEAdABlADEALAAgADEALAAgAC0AMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AagBkAG4ATABvAGMAYQBsAF8AUwB0AGEAcgB0ACwAIABKAEQAQQBUAEUAXwBUAE8AXwBKAEQATgBfAEwATwBDAEEATAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAF8AcwBpAGcAbgAgAD0AIAAxACwAIABKAEQAYQB0AGUAMQAsACAASgBEAGEAdABlADIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdAB6AG8AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBqAGQAbgBMAG8AYwBhAGwAXwBFAG4AZAAsACAASgBEAEEAVABFAF8AVABPAF8ASgBEAE4AXwBMAE8AQwBBAEwAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAHMAaQBnAG4AIAA9ACAAMQAsACAASgBEAGEAdABlADIALAAgAEoARABhAHQAZQAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBvAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHQAZQBfAFMAdABhAHIAdAAsACAASgBEAE4AXwBUAE8AXwBDAEEATABFAE4ARABBAFIAXwBEAEEAVABFACgASQBOAEQARQBYACgAXwBqAGQAbgBMAG8AYwBhAGwAXwBTAHQAYQByAHQALAAgADEALAAgADEAKQAsACAASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAdABlAF8ARQBuAGQALAAgAEoARABOAF8AVABPAF8AQwBBAEwARQBOAEQAQQBSAF8ARABBAFQARQAoAEkATgBEAEUAWAAoAF8AagBkAG4ATABvAGMAYQBsAF8ARQBuAGQALAAgADEALAAgADEAKQAsACAASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGUAbAB0AGEAWQBlAGEAcgAsACAASQBOAEQARQBYACgAXwBkAGEAdABlAF8ARQBuAGQALAAgADEALAAgADEAKQAgAC0AIABJAE4ARABFAFgAKABfAGQAYQB0AGUAXwBTAHQAYQByAHQALAAgADEALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaQBnAG4AIAAqACAAKABfAGQAZQBsAHQAYQBZAGUAYQByACAAKwAgADEAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAFwAbgBcAG4AXABuAFwAbgBcAG4AXABuAC8AKgAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAXABuACMAIABQAEEAUgBTAEkATgBHACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAqAC8AXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AUABBAFIAUwBFAF8ASQBTAE8AXwBEAEEAVABFAFwAbgBcAG4AUABhAHIAcwBlAHMAIABhAG4AIABJAFMATwAgAGYAbwByAG0AYQB0AHQAZQBkACAAZABhAHQAZQAgAGkAbgB0AG8AIAByAGUAcwBwAGUAYwB0AGkAdgBlACAAcABhAHIAdABzACAAbwBmACAAeQBlAGEAcgAsACAAbQBvAG4AdABoACwAIABkAGEAeQAsACAAdABpAG0AZQAgAG8AZgAgAGQAYQB5ACAAYQBuAGQAIAB0AGkAbQBlACAAegBvAG4AZQAgAG8AZgBmAHMAZQB0AFwAbgBpAG4AIABtAGkAbgB1AHQAZQBzACAAZgByAG8AbQAgAFUAVABDAC4AXABuAFwAbgBPAHUAdABwAHUAdABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAGkAbgB0AGUAZwBlAHIAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAWQBlAGEAcgBcAG4AIAAyACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADEALgAuADEAMgBdACAAIAAgACAAIAB8ACAATQBvAG4AdABoAFwAbgAgADMAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMQAuAC4AMwAxAF0AIAAgACAAIAAgAHwAIABEAGEAeQBcAG4AIAA0ACAAfAAgAGQAZQBjAGkAbQBhAGwAIABbADAALgAuADEAKQAgACAAIAAgACAAIAB8ACAAVABpAG0AZQBcAG4AIAA1ACAAfAAgAGQAZQBjAGkAbQBhAGwAIABbAC0AOQAwADAALgAuADkAMAAwAF0AIAB8ACAAVABpAG0AZQAgAHoAbwBuAGUAIABvAGYAZgBzAGUAdAAgAG0AaQBuAHUAdABlAHMAIABmAHIAbwBtACAAVQBUAEMAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBJAFMATwBEAGEAdABlACAAIAAgACAAIAAgACAAIAAgACAAfAAgAHQAZQB4AHQAIAAgACAAfAAgAEQAYQB0AGUAIABpAG4AIABJAFMATwAgAGYAbwByAG0AYQB0ACAAaQBlAC4AIAB5AHkAeQB5AC0ATQBNAC0AZABkAFQAaABoADoAbQBtADoAcwBzACsAaABoADoAbQBtAFwAbgBbAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACAAfAAgAHMAdwBpAHQAYwBoACAAfAAgAEMAYQBsAGMAdQBsAGEAdABlACAAaQBuACAAdABoAGUAIABKAHUAbABpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AIABEAGUAZgBhAHUAbAB0ACAAaQBzACAARwByAGUAZwBvAHIAaQBhAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAB8ACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgBcAG4AXABuAEUAeABhAG0AcABsAGUAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AUABBAFIAUwBFAF8ASQBTAE8AXwBEAEEAVABFACgAXAAiADIAMAAyADMALQAwADUALQAyADMAXAAiACkAXABuAFIAZQB0AHUAcgBuAHMAOgAgAHsAMgAwADIAMwAsACAANQAsACAAMgAzACwAIABcACIAXAAiACwAIABcACIAXAAiAH0AXABuAFwAbgBQAEEAUgBTAEUAXwBJAFMATwBfAEQAQQBUAEUAKABcACIAMgAwADIAMwAtADAANQAtADIAMwBUADAANgA6ADAAMABcACIAKQBcAG4AUgBlAHQAdQByAG4AcwA6ACAAewAyADAAMgAzACwAIAA1ACwAIAAyADMALAAgADAALgAyADUALAAgAFwAIgBcACIAfQBcAG4AXABuAFAAQQBSAFMARQBfAEkAUwBPAF8ARABBAFQARQAoAFwAIgAyADAAMgAzAC0AMAA1AC0AMgAzAFQAMAA2ADoAMAAwACsAMAA5ADoAMwAwAFwAIgApAFwAbgBSAGUAdAB1AHIAbgBzADoAIAB7ADIAMAAyADMALAAgADUALAAgADIAMwAsACAAMAAuADIANQAsACAANQA3ADAAfQBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4AUABBAFIAUwBFAF8ASQBTAE8AXwBEAEEAVABFACAAPQAgAEwAQQBNAEIARABBACgASQBTAE8ARABhAHQAZQAsACAAWwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAsAFwAbgAgACAAIAAgAEkARgAoAEkAUwBPAEQAYQB0AGUAIAA9ACAAXAAiAFwAIgAsACAAewBcACIAXAAiACwAIABcACIAXAAiACwAIABcACIAXAAiACwAIABcACIAXAAiACwAIABcACIAXAAiAH0ALABcAG4AIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAGYAbgBDAG8AdQBuAHQAQwBoAGEAcgBzACwAIABMAEEATQBCAEQAQQAoAEMAaABhAHIAQQByAHIAYQB5ACwAIABUAGUAeAB0ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAGUAeAB0ACAAPQAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcgBlAG0AbwB2AGUAZAAsACAAUgBFAEQAVQBDAEUAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAGUAeAB0ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAQwBoAGEAcgBBAHIAcgBhAHkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEEATQBCAEQAQQAoAF8AYQBjAGMALAAgAF8AYwB1AHIAcgAsACAAUwBVAEIAUwBUAEkAVABVAFQARQAoAF8AYQBjAGMALAAgAF8AYwB1AHIAcgAsACAAXAAiAFwAIgApACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAE4AKABUAGUAeAB0ACkAIAAtACAATABFAE4AKABfAHIAZQBtAG8AdgBlAGQAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAZgBuAEYAaQBuAGQATgB0AGgAQwBoAGEAcgBQAG8AcwAsACAATABBAE0AQgBEAEEAKABDAGgAYQByAHMALAAgAFQAZQB4AHQALAAgAE4ALAAgAFsAUwB0AGEAcgB0AFAAbwBzAF0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABOACgAUwB0AGEAcgB0AFAAbwBzACkAIAA+ACAATABFAE4AKABUAGUAeAB0ACkALAAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZgByAG8AbQBQAG8AcwAsACAASQBGACgATgAoAFMAdABhAHIAdABQAG8AcwApACAAPAA9ACAAMAAsACAAMAAsACAATgAoAFMAdABhAHIAdABQAG8AcwApACAALQAgADEAKQAsACAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdABlAHgAdAAsACAASQBGACgAXwBmAHIAbwBtAFAAbwBzACAAPQAgADAALAAgAFQAZQB4AHQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABSAEkARwBIAFQAKABUAGUAeAB0ACwAIABMAEUATgAoAFQAZQB4AHQAKQAgAC0AIABfAGYAcgBvAG0AUABvAHMAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGMAaABhAHIAQwBvAHUAbgB0ACwAIABMAEUATgAoAEMAaABhAHIAcwApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbgAsACAASQBOAFQAKABOACgATgApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAKABfAGMAaABhAHIAQwBvAHUAbgB0ACAAPQAgADAAKQAgACsAIAAoAF8AbgAgAD0AIAAwACkALAAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBjAGgAYQByAHMALAAgAE0ASQBEACgAQwBoAGEAcgBzACwAIABTAEUAUQBVAEUATgBDAEUAKAAxACwAIABfAGMAaABhAHIAQwBvAHUAbgB0ACkALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBmAGkAbgBkAEMAbwB1AG4AdAAsACAAZgBuAEMAbwB1AG4AdABDAGgAYQByAHMAKABfAGMAaABhAHIAcwAsACAAXwB0AGUAeAB0ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAF8AZgBpAG4AZABDAG8AdQBuAHQAIAA8ACAAQQBCAFMAKABfAG4AKQAsACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAG4AdABoACAAYwBhAG4AIABjAG8AdQBuAHQAIABmAHIAbwBtACAAZQBuAGQAIABiAGEAYwBrAHcAYQByAGQAcwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG4AdABoACwAIABJAEYAKABfAG4AIAA+ACAAMAAsACAAXwBuACwAIABfAGYAaQBuAGQAQwBvAHUAbgB0ACAAKwAgAF8AbgAgACsAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG4AdABoAFAAbwBzACwAIABSAEUARABVAEMARQAoADAALAAgAFMARQBRAFUARQBOAEMARQAoADEALAAgAF8AbgB0AGgAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABBAE0AQgBEAEEAKABfAGEAYwBjACwAIABfAGMAdQByAHIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBhAGMAYwAgADwAIAAwACwAIAAtADEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBuAGUAeAB0AFAAbwBzAEMAaABhAHIAcwAsACAASQBGAEUAUgBSAE8AUgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABGAEkATgBEACgAXwBjAGgAYQByAHMALAAgAF8AdABlAHgAdAAsACAAXwBhAGMAYwAgACsAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAMABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbgBlAHgAdABQAG8AcwAsACAATQBJAE4AKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAARgBJAEwAVABFAFIAKABfAG4AZQB4AHQAUABvAHMAQwBoAGEAcgBzACwAIABfAG4AZQB4AHQAUABvAHMAQwBoAGEAcgBzACAAPgAgADAALAAgADAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAF8AbgBlAHgAdABQAG8AcwAgAD0AIAAwACwAIAAtADEALAAgAF8AbgBlAHgAdABQAG8AcwApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAG4AdABoAFAAbwBzACAAPgAgADAALAAgAF8AbgB0AGgAUABvAHMAIAArACAAXwBmAHIAbwBtAFAAbwBzACAALAAgADAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAZgBuAEkAbgB2AGEAbABpAGQAQwBoAGEAcgBzACwAIABMAEEATQBCAEQAQQAoAF8AdABlAHgAdAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGMAaABhAHIAUwBlAHQALAAgAFwAIgArACwALQAuADAAMQAyADMANAA1ADYANwA4ADkAOgBUAFcAWgBcACIAIAAmACAAVQBOAEkAQwBIAEEAUgAoADgANwAyADIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBlAHMAYwBhAHAAZQBUAGUAeAB0ACwAIABTAFUAQgBTAFQASQBUAFUAVABFACgAUwBVAEIAUwBUAEkAVABVAFQARQAoAF8AdABlAHgAdAAsACAAXAAiACYAXAAiACwAIABcACIAJgBhAG0AcAA7AFwAIgApACwAIABcACIAPABcACIALAAgAFwAIgAmAGwAdAA7AFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHgAbQBsACwAIABcACIAPAB0AD4APABzAD4AXAAiACAAJgAgAF8AZQBzAGMAYQBwAGUAVABlAHgAdAAgACYAIABcACIAPAAvAHMAPgA8AC8AdAA+AFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB4AHAAYQB0AGgALAAgAFwAIgAvAC8AcwBbAHQAcgBhAG4AcwBsAGEAdABlACgALgAsACcAXAAiACAAJgAgAF8AYwBoAGEAcgBTAGUAdAAgACYAIABcACIAJwAsACcAJwApAD0AJwAnAF0AXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAFMARQBSAFIATwBSACgARgBJAEwAVABFAFIAWABNAEwAKABfAHgAbQBsACwAIABfAHgAcABhAHQAaAApACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAZgBuAFAAYQByAHMAZQBEAGEAdABlACwAIABMAEEATQBCAEQAQQAoAF8AZABhAHQAZQBQAGEAcgB0ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZgBpAHIAcwB0AEMAaABhAHIALAAgAEwARQBGAFQAKABfAGQAYQB0AGUAUABhAHIAdAAsACAAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGkAcwBTAGkAZwBuAGUAZAAsACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBmAGkAcgBzAHQAQwBoAGEAcgAgAD0AIABcACIAKwBcACIALAAgAFQAUgBVAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBmAGkAcgBzAHQAQwBoAGEAcgAgAD0AIABcACIALQBcACIALAAgAFQAUgBVAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBmAGkAcgBzAHQAQwBoAGEAcgAgAD0AIABVAE4ASQBDAEgAQQBSACgAOAA3ADIAMgApACwAIABUAFIAVQBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALAAgAEYAQQBMAFMARQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBpAGcAbgAsACAASQBGACgAXwBpAHMAUwBpAGcAbgBlAGQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGYAaQByAHMAdABDAGgAYQByACAAPQAgAFwAIgAtAFwAIgAsACAALQAxACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBmAGkAcgBzAHQAQwBoAGEAcgAgAD0AIABVAE4ASQBDAEgAQQBSACgAOAA3ADIAMgApACwAIAAtADEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAIAAxAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAIAAxAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB1AG4AUwBpAGcAbgBlAGQALAAgAEkARgAoAF8AaQBzAFMAaQBnAG4AZQBkACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFIASQBHAEgAVAAoAF8AZABhAHQAZQBQAGEAcgB0ACwAIABMAEUATgAoAF8AZABhAHQAZQBQAGEAcgB0ACkAIAAtACAAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHQAZQBQAGEAcgB0AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBwAG8AcwAxACwAIABJAEYARQBSAFIATwBSACgARgBJAE4ARAAoAFwAIgAtAFwAIgAsACAAXwB1AG4AUwBpAGcAbgBlAGQAKQAsACAAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAHAAbwBzADEAIAA8ACAANQAsACAAewAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHAAbwBzADIALAAgAEkARgBFAFIAUgBPAFIAKABGAEkATgBEACgAXAAiAC0AXAAiACwAIABfAHUAbgBTAGkAZwBuAGUAZAAsACAAXwBwAG8AcwAxACAAKwAgADEAKQAsACAAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBwAG8AcwAyACAALQAgAF8AcABvAHMAMQAgADwAPgAgADMALAAgAHsAIwBWAEEATABVAEUAIQAsACAAIwBWAEEATABVAEUAIQAsACAAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIALAAgAF8AcwBpAGcAbgAgACoAIABJAE4AVAAoAFYAQQBMAFUARQAoAEwARQBGAFQAKABfAHUAbgBTAGkAZwBuAGUAZAAsACAAXwBwAG8AcwAxACAALQAgADEAKQApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBtAG8AbgB0AGgALAAgAEkATgBUACgAVgBBAEwAVQBFACgATQBJAEQAKABfAHUAbgBTAGkAZwBuAGUAZAAsACAAXwBwAG8AcwAxACAAKwAgADEALAAgAF8AcABvAHMAMgAtACAAXwBwAG8AcwAxACAALQAgADEAKQApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQAsACAASQBOAFQAKABWAEEATABVAEUAKABSAEkARwBIAFQAKABfAHUAbgBTAGkAZwBuAGUAZAAsACAATABFAE4AKABfAHUAbgBTAGkAZwBuAGUAZAApACAALQAgAF8AcABvAHMAMgApACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABJAFMAXwBWAEEATABJAEQAXwBEAEEAVABFACgAXwB5AGUAYQByACwAIABfAG0AbwBuAHQAaAAsACAAXwBkAGEAeQAsACAASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAF8AeQBlAGEAcgAsACAAXwBtAG8AbgB0AGgALAAgAF8AZABhAHkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHsAIwBWAEEATABVAEUAIQAsACAAIwBWAEEATABVAEUAIQAsACAAIwBWAEEATABVAEUAIQB9AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABmAG4AVABpAG0AZQBEAGUAYwBpAG0AYQBsACwAIABMAEEATQBCAEQAQQAoAF8AaABvAHUAcgAsACAAXwBtAGkAbgB1AHQAZQAsACAAXwBzAGUAYwBvAG4AZAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGkAcwBJAG4AVgBhAGwAaQBkACwAIABJAEYAUwAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGgAbwB1AHIAIAA8ACAAMAAsACAAVABSAFUARQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGgAbwB1AHIAIAA+ACAAMgA0ACwAIABUAFIAVQBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgAXwBoAG8AdQByACAAPQAgADIANAApACAAKgAgACgAKABfAG0AaQBuAHUAdABlACAAPgAgADAAKQAgACsAIAAoAF8AcwBlAGMAbwBuAGQAIAA+ACAAMAApACkALAAgAFQAUgBVAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBtAGkAbgB1AHQAZQAgADwAIAAwACwAIABUAFIAVQBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbQBpAG4AdQB0AGUAIAA+AD0AIAA2ADAALAAgAFQAUgBVAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGUAYwBvAG4AZAAgADwAIAAwACwAIABUAFIAVQBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBlAGMAbwBuAGQAIAA+AD0AIAA2ADAALAAgAFQAUgBVAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABSAFUARQAsACAARgBBAEwAUwBFAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAF8AaQBzAEkAbgB2AGEAbABpAGQALAAgAHsAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgAXwBoAG8AdQByACAALwAgADIANAApACAAKwAgACgAXwBtAGkAbgB1AHQAZQAvACAAMQA0ADQAMAApACAAKwAgACgAXwBzAGUAYwBvAG4AZAAgAC8AIAA4ADYANAAwADAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAZgBuAFAAYQByAHMAZQBUAGkAbQBlACwAIABMAEEATQBCAEQAQQAoAF8AdABpAG0AZQBQAGEAcgB0ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbABlAG4ALAAgAEwARQBOACgAXwB0AGkAbQBlAFAAYQByAHQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBsAGUAbgAgAD0AIAAyACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAGYAbgBUAGkAbQBlAEQAZQBjAGkAbQBhAGwAKABWAEEATABVAEUAKABfAHQAaQBtAGUAUABhAHIAdAApACwAIAAwACwAIAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBsAGUAbgAgAD0AIAA1ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAE0ASQBEACgAXwB0AGkAbQBlAFAAYQByAHQALAAgADMALAAgADEAKQAgADwAPgAgAFwAIgA6AFwAIgAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABmAG4AVABpAG0AZQBEAGUAYwBpAG0AYQBsACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABWAEEATABVAEUAKABMAEUARgBUACgAXwB0AGkAbQBlAFAAYQByAHQALAAgADIAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABWAEEATABVAEUAKABSAEkARwBIAFQAKABfAHQAaQBtAGUAUABhAHIAdAAsACAAMgApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGwAZQBuACAAPQAgADgALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgATQBJAEQAKABfAHQAaQBtAGUAUABhAHIAdAAsACAAMwAsACAAMQApACAAPAA+ACAAXAAiADoAXAAiACwAIAB7ACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAE0ASQBEACgAXwB0AGkAbQBlAFAAYQByAHQALAAgADYALAAgADEAKQAgADwAPgAgAFwAIgA6AFwAIgAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAGYAbgBUAGkAbQBlAEQAZQBjAGkAbQBhAGwAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVgBBAEwAVQBFACgATABFAEYAVAAoAF8AdABpAG0AZQBQAGEAcgB0ACwAIAAyACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABWAEEATABVAEUAKABNAEkARAAoAF8AdABpAG0AZQBQAGEAcgB0ACwAIAA0ACwAIAAyACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABWAEEATABVAEUAKABSAEkARwBIAFQAKABfAHQAaQBtAGUAUABhAHIAdAAsACAAMgApACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKABfAGwAZQBuACAAPgA9ACAAMQAwACkAIAAqACAAKABfAGwAZQBuACAAPAA9ACAAMQAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgATQBJAEQAKABfAHQAaQBtAGUAUABhAHIAdAAsACAAMwAsACAAMQApACAAPAA+ACAAXAAiADoAXAAiACwAIAB7ACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAE0ASQBEACgAXwB0AGkAbQBlAFAAYQByAHQALAAgADYALAAgADEAKQAgADwAPgAgAFwAIgA6AFwAIgAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAE0ASQBEACgAXwB0AGkAbQBlAFAAYQByAHQALAAgADkALAAgADEAKQAgADwAPgAgAFwAIgAuAFwAIgAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGkAbgB0AFMAZQBjACwAIABJAE4AVAAoAFYAQQBMAFUARQAoAE0ASQBEACgAXwB0AGkAbQBlAFAAYQByAHQALAAgADcALAAgADIAKQApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAZQBjAFAAbABhAGMAZQBzACwAIABfAGwAZQBuACAALQAgADkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGYAcgBhAGMAUwBlAGMALAAgAEkATgBUACgAVgBBAEwAVQBFACgAUgBJAEcASABUACgAXwB0AGkAbQBlAFAAYQByAHQALAAgAF8AZABlAGMAUABsAGEAYwBlAHMAKQApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAZQBjAFMAZQBjACwAIABfAGkAbgB0AFMAZQBjACAAKwAgACgAXwBmAHIAYQBjAFMAZQBjACAALwAgACgAMQAwACAAXgAgAF8AZABlAGMAUABsAGEAYwBlAHMAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAZgBuAFQAaQBtAGUARABlAGMAaQBtAGEAbAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVgBBAEwAVQBFACgATABFAEYAVAAoAF8AdABpAG0AZQBQAGEAcgB0ACwAIAAyACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVgBBAEwAVQBFACgATQBJAEQAKABfAHQAaQBtAGUAUABhAHIAdAAsACAANAAsACAAMgApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABlAGMAUwBlAGMAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAIAB7ACMAVgBBAEwAVQBFACEAfQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABmAG4AVABaAG0AaQBuAHUAdABlAHMALAAgAEwAQQBNAEIARABBACgAXwBzAGkAZwBuACwAIABfAGgAbwB1AHIALAAgAF8AbQBpAG4AdQB0AGUALAAgAF8AcwBlAGMAbwBuAGQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBhAGIAcwBNAGkAbgBzACwAIAAoAF8AaABvAHUAcgAgACoAIAA2ADAAKQAgACsAIABfAG0AaQBuAHUAdABlACAAKwAgACgAXwBzAGUAYwBvAG4AZAAgAC8AIAA2ADAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBhAGIAcwBNAGkAbgBzACAAPgAgADkAMAAwACwAIAB7ACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaQBnAG4AIAAqACAAXwBhAGIAcwBNAGkAbgBzAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABmAG4AUABhAHIAcwBlAFQAWgAsACAATABBAE0AQgBEAEEAKABfAFQAWgBwAGEAcgB0ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAVQBQAFAARQBSACgAXwBUAFoAcABhAHIAdAApACAAPQAgAFwAIgBaAFwAIgAsACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBmAGkAcgBzAHQAQwBoAGEAcgAsACAATABFAEYAVAAoAF8AVABaAHAAYQByAHQALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaQBnAG4ALAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBmAGkAcgBzAHQAQwBoAGEAcgAgAD0AIABcACIALQBcACIALAAgAC0AMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZgBpAHIAcwB0AEMAaABhAHIAIAA9ACAAVQBOAEkAQwBIAEEAUgAoADgANwAyADIAKQAsACAALQAxACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABSAFUARQAsACAAMQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGwAZQBuACwAIABMAEUATgAoAF8AVABaAHAAYQByAHQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAUwAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbABlAG4AIAA9ACAAMwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAGYAbgBUAFoAbQBpAG4AdQB0AGUAcwAoAF8AcwBpAGcAbgAsACAAVgBBAEwAVQBFACgAUgBJAEcASABUACgAXwBUAFoAcABhAHIAdAAsACAAMgApACkALAAgADAALAAgADAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbABlAG4AIAA9ACAANgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAE0ASQBEACgAXwBUAFoAcABhAHIAdAAsACAANAAsACAAMQApACAAPAA+ACAAXAAiADoAXAAiACwAIAB7ACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAZgBuAFQAWgBtAGkAbgB1AHQAZQBzACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBpAGcAbgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABWAEEATABVAEUAKABNAEkARAAoAF8AVABaAHAAYQByAHQALAAgADIALAAgADIAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFYAQQBMAFUARQAoAFIASQBHAEgAVAAoAF8AVABaAHAAYQByAHQALAAgADIAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGwAZQBuACAAPQAgADkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABNAEkARAAoAF8AVABaAHAAYQByAHQALAAgADQALAAgADEAKQAgADwAPgAgAFwAIgA6AFwAIgAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAE0ASQBEACgAXwBUAFoAcABhAHIAdAAsACAANwAsACAAMQApACAAPAA+ACAAXAAiADoAXAAiACwAIAB7ACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABmAG4AVABaAG0AaQBuAHUAdABlAHMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaQBnAG4ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABWAEEATABVAEUAKABNAEkARAAoAF8AVABaAHAAYQByAHQALAAgADIALAAgADIAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVgBBAEwAVQBFACgATQBJAEQAKABfAFQAWgBwAGEAcgB0ACwAIAA1ACwAIAAyACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFYAQQBMAFUARQAoAFIASQBHAEgAVAAoAF8AVABaAHAAYQByAHQALAAgADIAKQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABSAFUARQAsACAAewAjAFYAQQBMAFUARQAhAH0AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAGYAbgBJAG4AdgBhAGwAaQBkAEMAaABhAHIAcwAoAEkAUwBPAEQAYQB0AGUAKQAsACAAewAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBUAHAAbwBzACwAIABJAEYARQBSAFIATwBSACgARgBJAE4ARAAoAFwAIgBUAFwAIgAsACAASQBTAE8ARABhAHQAZQApACwAIAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAF8AVABwAG8AcwAgAD0AIAAwACwAIABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABmAG4AUABhAHIAcwBlAEQAYQB0AGUAKABJAFMATwBEAGEAdABlACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiAFwAIgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHQAZQAsACAAZgBuAFAAYQByAHMAZQBEAGEAdABlACgATABFAEYAVAAoAEkAUwBPAEQAYQB0AGUALAAgAF8AVABwAG8AcwAgAC0AIAAxACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AVABaAHAAbwBzACwAIABmAG4ARgBpAG4AZABOAHQAaABDAGgAYQByAFAAbwBzACgAXAAiAFoAKwAtAFwAIgAgACYAIABVAE4ASQBDAEgAQQBSACgAOAA3ADIAMgApACwAIABJAFMATwBEAGEAdABlACwAIAAtADEALAAgAF8AVABwAG8AcwApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBUAFoAcABvAHMAIAA9ACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAZgBuAFAAYQByAHMAZQBEAGEAdABlACgATABFAEYAVAAoAEkAUwBPAEQAYQB0AGUALAAgAF8AVABwAG8AcwAgAC0AIAAxACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABmAG4AUABhAHIAcwBlAFQAaQBtAGUAKABSAEkARwBIAFQAKABJAFMATwBEAGEAdABlACwAIABMAEUATgAoAEkAUwBPAEQAYQB0AGUAKQAgAC0AIABfAFQAcABvAHMAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBcACIAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABmAG4AUABhAHIAcwBlAEQAYQB0AGUAKABMAEUARgBUACgASQBTAE8ARABhAHQAZQAsACAAXwBUAHAAbwBzACAALQAgADEAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAGYAbgBQAGEAcgBzAGUAVABpAG0AZQAoAE0ASQBEACgASQBTAE8ARABhAHQAZQAsACAAXwBUAHAAbwBzACAAKwAgADEALAAgAF8AVABaAFAAbwBzACAALQAgAF8AVABwAG8AcwAgAC0AIAAxACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABmAG4AUABhAHIAcwBlAFQAWgAoAFIASQBHAEgAVAAoAEkAUwBPAEQAYQB0AGUALAAgAEwARQBOACgASQBTAE8ARABhAHQAZQApACAALQAgAF8AVABaAHAAbwBzACAAKwAgADEAKQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AUABBAFIAUwBFAF8AVwBFAEUASwBEAEEAWQBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIABhACAAbgB1AG0AYgBlAHIAIAByAGUAcAByAGUAcwBlAG4AdABpAG4AZwAgAHQAaABlACAAZABhAHkAIABvAGYAIAB0AGgAZQAgAHcAZQBlAGsAIABmAHIAbwBtACAAYQAgAGcAaQB2AGUAbgAgAHQAZQB4AHQAIAB3AGUAZQBrAGQAYQB5ACAAbgBhAG0AZQAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAEQAYQB5ACAAbwBmACAAdwBlAGUAawBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEQAYQB5AE8AZgBXAGUAZQBrACAAIAAgACAAIAAgACAAfAAgAHQAZQB4AHQAIAAgACAAIAB8ACAARABhAHkAIABvAGYAIAB3AGUAZQBrACAAbgBhAG0AZQBcAG4AWwBOAHUAbQBiAGUAcgBTAGMAaABlAG0AZQBdACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIABSAGUAdAB1AHIAbgAgAGQAYQB5ACAAbwBmACAAdwBlAGUAawAgAHUAcwBpAG4AZwAgAG4AdQBtAGIAZQByAGkAbgBnACAAcwBjAGgAZQBtAGUAOgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAMQAgAC0AIAAxAC4ALgA3ACAAUwB1AG4AZABhAHkALgAuAFMAYQB0AHUAcgBkAGEAeQAgACgAZABlAGYAYQB1AGwAdAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAyACAALQAgADEALgAuADcAIABNAG8AbgBkAGEAeQAuAC4AUwB1AG4AZABhAHkAIAAgACAAKABJAFMATwAgADgANgAwADEAIABkAGUAZgBpAG4AaQB0AGkAbwBuACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADMAIAAtACAAMAAuAC4ANgAgAE0AbwBuAGQAYQB5AC4ALgBTAHUAbgBkAGEAeQBcAG4ARQB4AGEAbQBwAGwAZQBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBQAEEAUgBTAEUAXwBXAEUARQBLAEQAQQBZACgAXAAiAFMAYQB0AHUAcgBkAGEAeQBcACIAKQBcAG4AUgBlAHQAdQByAG4AcwA6ACAANwBcAG4AXABuAFAAQQBSAFMARQBfAFcARQBFAEsARABBAFkAKABcACIATQBvAG4AXAAiACwAIAAzACkAXABuAFIAZQB0AHUAcgBuAHMAOgAgADAAXABuAFwAbgBQAEEAUgBTAEUAXwBXAEUARQBLAEQAQQBZACgAXAAiAFQAaAB1AHIAcwBcACIALAAgADEAKQBcAG4AUgBlAHQAdQByAG4AcwA6ACAAIwBWAEEATABVAEUAIQBcAG4AXABuAFAAQQBSAFMARQBfAFcARQBFAEsARABBAFkAKABcACIAVgBlAG4AXAAiACwAIAAyACkAXABuAFIAZQB0AHUAcgBuAHMAOgAgADUAIAAoAGkAZgAgAGwAbwBjAGEAbAAgAGwAYQBuAGcAdQBhAGcAZQAgAGkAcwAgAHMAZQB0ACAAdABvACAASQB0AGEAbABpAGEAbgApAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBQAEEAUgBTAEUAXwBXAEUARQBLAEQAQQBZACAAPQAgAEwAQQBNAEIARABBACgARABhAHkATwBmAFcAZQBlAGsALAAgAFsATgB1AG0AYgBlAHIAUwBjAGgAZQBtAGUAXQAsAFwAbgAgACAAIAAgAEkARgAoAEQAYQB5AE8AZgBXAGUAZQBrACAAPQAgAFwAIgBcACIALAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAGYAbgBNAGEAdABjAGgASQBuAHQARQBuAGcALAAgAEwAQQBNAEIARABBACgARABvAFcALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAG8AdwAsACAASQBGACgATABFAE4AKABEAGEAeQBPAGYAVwBlAGUAawApACAAPQAgADMALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAWABNAEEAVABDAEgAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABEAGEAeQBPAGYAVwBlAGUAawAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAUwB1AG4AXAAiADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIATQBvAG4AXAAiADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAVAB1AGUAXAAiADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAVwBlAGQAXAAiADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAVABoAHUAXAAiADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIARgByAGkAXAAiADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAUwBhAHQAXAAiAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAH0AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAWABNAEEAVABDAEgAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABEAGEAeQBPAGYAVwBlAGUAawAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAUwB1AG4AZABhAHkAXAAiADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIATQBvAG4AZABhAHkAXAAiADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAVAB1AGUAcwBkAGEAeQBcACIAOwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBXAGUAZABuAGUAcwBkAGEAeQBcACIAOwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBUAGgAdQByAHMAZABhAHkAXAAiADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIARgByAGkAZABhAHkAXAAiADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAUwBhAHQAdQByAGQAYQB5AFwAIgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB9AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGAE4AQQAoAF8AZABvAHcALAAgADAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAGYAbgBNAGEAdABjAGgATABvAGMAYQBsAEwAYQBuAGcALAAgAEwAQQBNAEIARABBACgARABvAFcALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQBzACwAIABTAEUAUQBVAEUATgBDAEUAKAA3ACwAIAAxACwAIAAzADYANQAyADcAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAG8AdwAsACAASQBGACgATABFAE4AKABEAGEAeQBPAGYAVwBlAGUAawApACAAPQAgADMALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAWABNAEEAVABDAEgAKABEAGEAeQBPAGYAVwBlAGUAawAsACAAVABFAFgAVAAoAF8AZABhAHkAcwAsACAAXAAiAGQAZABkAFwAIgApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAWABNAEEAVABDAEgAKABEAGEAeQBPAGYAVwBlAGUAawAsACAAVABFAFgAVAAoAF8AZABhAHkAcwAsACAAXAAiAGQAZABkAGQAXAAiACkAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgBOAEEAKABfAGQAbwB3ACwAIAAwACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAcgBhAGQARABvAFcALAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBpAGQAeAAsACAAZgBuAE0AYQB0AGMAaABJAG4AdABFAG4AZwAoAEQAYQB5AE8AZgBXAGUAZQBrACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAGkAZAB4ACAAPgAgADAALAAgAF8AaQBkAHgALAAgAGYAbgBNAGEAdABjAGgATABvAGMAYQBsAEwAYQBuAGcAKABEAGEAeQBPAGYAVwBlAGUAawApACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGMAaABlAG0AZQAsACAASQBOAFQAKABOACgATgB1AG0AYgBlAHIAUwBjAGgAZQBtAGUAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AHIAYQBkAEQAbwBXACAAPQAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAVgBBAEwAVQBFACEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAYwBoAGUAbQBlACAAPAA9ACAAMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AHIAYQBkAEQAbwBXACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGMAaABlAG0AZQAgAD4APQAgADMALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAE0ATwBEACgAXwB0AHIAYQBkAEQAbwBXACAALQAgADIALAAgADcAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAE0ATwBEACgAXwB0AHIAYQBkAEQAbwBXACAALQAgADIALAAgADcAKQAgACsAIAAxAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBQAEEAUgBTAEUAXwBNAE8ATgBUAEgAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAYQAgAG4AdQBtAGIAZQByACAAcgBlAHAAcgBlAHMAZQBuAHQAaQBuAGcAIAB0AGgAZQAgAG0AbwBuAHQAaAAgAG8AZgAgAHkAZQBhAHIAIABmAHIAbwBtACAAYQAgAGcAaQB2AGUAbgAgAHQAZQB4AHQAIABtAG8AbgB0AGgAIABuAGEAbQBlAC4AXABuAFwAbgBPAHUAdABwAHUAdABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADEALgAuADEAMgBdACAAfAAgAE0AbwBuAHQAaABcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAE0AbwBuAHQAaABOAGEAbQBlACAAfAAgAHQAZQB4AHQAIAB8ACAATQBvAG4AdABoACAAbgBhAG0AZQBcAG4AXABuAEUAeABhAG0AcABsAGUAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AUABBAFIAUwBFAF8ATQBPAE4AVABIACgAXAAiAEYAZQBiAFwAIgApAFwAbgBSAGUAdAB1AHIAbgBzADoAIAAyAFwAbgBcAG4AUABBAFIAUwBFAF8ATQBPAE4AVABIACgAXAAiAEoAYQBuAHUAYQByAHkAXAAiACkAXABuAFIAZQB0AHUAcgBuAHMAOgAgADEAXABuAFwAbgBQAEEAUgBTAEUAXwBNAE8ATgBUAEgAKABcACIASgBcACIAKQBcAG4AUgBlAHQAdQByAG4AcwA6ACAAIwBWAEEATABVAEUAIQBcAG4AXABuAFAAQQBSAFMARQBfAE0ATwBOAFQASAAoAFwAIgBNAGEAcgB6AG8AXAAiACkAXABuAFIAZQB0AHUAcgBuAHMAOgAgADMAIAAoAGkAZgAgAGwAbwBjAGEAbAAgAGwAYQBuAGcAdQBhAGcAZQAgAGkAcwAgAHMAZQB0ACAAdABvACAASQB0AGEAbABpAGEAbgApAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBQAEEAUgBTAEUAXwBNAE8ATgBUAEgAIAA9ACAATABBAE0AQgBEAEEAKABNAG8AbgB0AGgATgBhAG0AZQAsAFwAbgAgACAAIAAgAEkARgAoAE0AbwBuAHQAaABOAGEAbQBlACAAPQAgAFwAIgBcACIALAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdAByAHkATQBvAG4AdABoACwAIABNAG8AbgB0AGgATgBhAG0AZQAgACYAIABcACIAIAAyADAAMAAwAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABNAE8ATgBUAEgAKABEAEEAVABFAFYAQQBMAFUARQAoAF8AdAByAHkATQBvAG4AdABoACkAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AUABBAFIAUwBFAF8ATABJAFQARQBSAEEAUgBZAF8AWQBFAEEAUgBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIABhACAAbgB1AG0AYgBlAHIAIAByAGUAcAByAGUAcwBlAG4AdABpAG4AZwAgAHQAaABlACAAeQBlAGEAcgAgAHIAZQBsAGEAdABpAHYAZQAgAHQAbwAgAHQAaABlACAAYwBvAG0AbQBvAG4AIABlAHIAYQAgAGYAcgBvAG0AIABhACAAZwBpAHYAZQBuACAAbABpAHQAZQByAGEAcgB5ACAAeQBlAGEAcgAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAFkAZQBhAHIAQwBFAC4AIABOAG8AdABlACAAdABoAGEAdAAgADEAIABCAEMAIAA9ACAAMAAgAEMARQAsACAAMgAgAEIAQwAgAD0AIAAtADEAIABDAEUAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBMAGkAdABlAHIAYQByAHkAWQBlAGEAcgAgAHwAIAB0AGUAeAB0ACAAfAAgAEwAaQB0AGUAcgBhAHIAeQAgAHkAZQBhAHIAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAFAAQQBSAFMARQBfAEwASQBUAEUAUgBBAFIAWQBfAFkARQBBAFIAIAA9ACAATABBAE0AQgBEAEEAKABMAGkAdABlAHIAYQByAHkAWQBlAGEAcgAsAFwAbgAgACAAIAAgAEkARgAoAEwAaQB0AGUAcgBhAHIAeQBZAGUAYQByACAAPQAgAFwAIgBcACIALAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAGYAbgBZAGUAYQByAFYAYQBsAHUAZQAsACAATABBAE0AQgBEAEEAKABfAHQAZQB4AHQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBjAGgAYQByADEALAAgAEwARQBGAFQAKABfAHQAZQB4AHQALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGkAZwBuACwAIABJAEYAUwAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGMAaABhAHIAMQAgAD0AIABcACIAKwBcACIALAAgADEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBjAGgAYQByADEAIAA9ACAAXAAiAC0AXAAiACwAIAAtADEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVQBOAEkAQwBPAEQARQAoAF8AYwBoAGEAcgAxACkAIAA9ACAAOAA3ADIAMgAsACAALQAxACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALAAgAFwAIgBcACIAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAHMAaQBnAG4AIAA9ACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAE4AVAAoAFYAQQBMAFUARQAoAF8AdABlAHgAdAApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGkAZwBuACAAKgAgAEkATgBUACgAVgBBAEwAVQBFACgAUgBJAEcASABUACgAXwB0AGUAeAB0ACwAIABMAEUATgAoAF8AdABlAHgAdAApACAALQAxACkAKQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGwAaQB0AFkAZQBhAHIALAAgAFMAVQBCAFMAVABJAFQAVQBUAEUAKABTAFUAQgBTAFQASQBUAFUAVABFACgATABpAHQAZQByAGEAcgB5AFkAZQBhAHIALAAgAFwAIgAsAFwAIgAsACAAXAAiAFwAIgApACwAIABcACIAIABcACIALAAgAFwAIgBcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIAQwBFACwAIABJAEYAUwAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFIASQBHAEgAVAAoAF8AbABpAHQAWQBlAGEAcgAsACAAMwApACAAPQAgAFwAIgBCAEMARQBcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBZAGUAYQByACwAIABMAEUARgBUACgAXwBsAGkAdABZAGUAYQByACwAIABMAEUATgAoAF8AbABpAHQAWQBlAGEAcgApACAALQAgADMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAxACAALQAgAGYAbgBZAGUAYQByAFYAYQBsAHUAZQAoAF8AcwBZAGUAYQByACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAUgBJAEcASABUACgAXwBsAGkAdABZAGUAYQByACwAIAAyACkAIAA9ACAAXAAiAEMARQBcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBZAGUAYQByACwAIABMAEUARgBUACgAXwBsAGkAdABZAGUAYQByACwAIABMAEUATgAoAF8AbABpAHQAWQBlAGEAcgApACAALQAgADIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABmAG4AWQBlAGEAcgBWAGEAbAB1AGUAKABfAHMAWQBlAGEAcgApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALAAgAGYAbgBZAGUAYQByAFYAYQBsAHUAZQAoAF8AbABpAHQAWQBlAGEAcgApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYARQBSAFIATwBSACgAXwB5AGUAYQByAEMARQAsACAAewAjAFYAQQBMAFUARQAhAH0AKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AUABBAFIAUwBFAF8ATABJAFQARQBSAEEAUgBZAF8ARABBAFQARQBcAG4AXABuAFAAYQByAHMAZQBzACAAYQAgAGwAaQB0AGUAcgBhAHIAeQAgAGQAYQB0AGUAIABpAG4AdABvACAAcgBlAHMAcABlAGMAdABpAHYAZQAgAHAAYQByAHQAcwAgAG8AZgAgAHkAZQBhAHIALAAgAG0AbwBuAHQAaAAsACAAZABhAHkAIABhAG4AZAAgAHQAaQBtAGUAIABvAGYAIABkAGEAeQAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABpAG4AdABlAGcAZQByACAAIAAgACAAIAAgACAAIAAgAHwAIABZAGUAYQByAFwAbgAgADIAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMQAuAC4AMQAyAF0AIAB8ACAATQBvAG4AdABoAFwAbgAgADMAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMQAuAC4AMwAxAF0AIAB8ACAARABhAHkAXABuACAANAAgAHwAIABkAGUAYwBpAG0AYQBsACAAWwAwAC4ALgAxACkAIAAgAHwAIABUAGkAbQBlAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ATABpAHQAZQByAGEAcgB5AEQAYQB0AGUAIAB8ACAAdABlAHgAdAAgAHwAIABMAGkAdABlAHIAYQByAHkAIABkAGEAdABlACAAYQBuAGQAIAB0AGkAbQBlAFwAbgBcAG4ARQB4AGEAbQBwAGwAZQBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBQAEEAUgBTAEUAXwBMAEkAVABFAFIAQQBSAFkAXwBEAEEAVABFACgAXAAiAEYAZQBiACAAMgA1ACwAIAAyADAAMQA0ACwAIAA2ADoAMAAwAFwAIgApAFwAbgBSAGUAdAB1AHIAbgBzADoAIAB7ADIAMAAxADQALAAgADIALAAgADIANQAsACAAMAAuADIANQB9AFwAbgBcAG4AUABBAFIAUwBFAF8ATABJAFQARQBSAEEAUgBZAF8ARABBAFQARQAoAFwAIgBEAGUAYwAgADMAMQAsACAAMgAwADIAMwAsACAAMgA0ADoAMAAwAFwAIgApAFwAbgBSAGUAdAB1AHIAbgBzADoAIAB7ADIAMAAyADMALAAgADEAMgAsACAAMwAxACwAIAAxAH0AXABuAFwAbgBQAEEAUgBTAEUAXwBMAEkAVABFAFIAQQBSAFkAXwBEAEEAVABFACgAXAAiAEYAZQBiACAAMgA1AFwAIgApAFwAbgBSAGUAdAB1AHIAbgBzADoAIAB7AFwAIgBcACIAIAAsACAAMgAsACAAMgA1ACwAIABcACIAXAAiAH0AXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAFAAQQBSAFMARQBfAEwASQBUAEUAUgBBAFIAWQBfAEQAQQBUAEUAIAA9ACAATABBAE0AQgBEAEEAKABMAGkAdABlAHIAYQByAHkARABhAHQAZQAsAFwAbgAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIABmAG4AUABhAHIAcwBlAEQAYQB0AGUALAAgAEwAQQBNAEIARABBACgAXwBsAGkAdABEAGEAdABlACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAF8AbABpAHQARABhAHQAZQAgAD0AIABcACIAXAAiACwAIAB7AFwAIgBcACIALAAgAFwAIgBcACIALAAgAFwAIgBcACIALAAgAFwAIgBcACIAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHAAYQByAHQAcwAsACAAVABSAEkATQAoAFQARQBYAFQAUwBQAEwASQBUACgAXwBsAGkAdABEAGEAdABlACwAIABcACIALABcACIAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGMAbwBsAHMALAAgAEMATwBMAFUATQBOAFMAKABfAHAAYQByAHQAcwApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAUwAoAF8AYwBvAGwAcwAgAD0AIAAxACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBwAGEAcgB0ADEALAAgAEkATgBEAEUAWAAoAF8AcABhAHIAdABzACwAIAAxACwAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAcABhAGMAZQBQAG8AcwAsACAASQBGAEUAUgBSAE8AUgAoAEYASQBOAEQAKABcACIAIABcACIALAAgAF8AcABhAHIAdAAxACkALAAgADAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAF8AcwBwAGEAYwBlAFAAbwBzACAAPQAgADAALAAgAHsAIwBWAEEATABVAEUAIQAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AbwBuAHQAaAAsACAAUABBAFIAUwBFAF8ATQBPAE4AVABIACgATABFAEYAVAAoAF8AcABhAHIAdAAxACwAIABfAHMAcABhAGMAZQBQAG8AcwAgAC0AIAAxACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHIAZQBtAGEAaQBuACwAIABNAEkARAAoAF8AcABhAHIAdAAxACwAIABfAHMAcABhAGMAZQBQAG8AcwAgACsAIAAxACwAIABMAEUATgAoAF8AcABhAHIAdAAxACkAIAAtACAAXwBzAHAAYQBjAGUAUABvAHMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAZQBuAG8AdABlAGQAWQBlAGEAcgAsACAASQBGAEUAUgBSAE8AUgAoAEYASQBOAEQAKABcACIAQwBcACIALAAgAF8AcgBlAG0AYQBpAG4AKQAsACAAMAApACAAPgAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB2AGEAbAAsACAASQBGACgAXwBkAGUAbgBvAHQAZQBkAFkAZQBhAHIALAAgAFAAQQBSAFMARQBfAEwASQBUAEUAUgBBAFIAWQBfAFkARQBBAFIAKABfAHIAZQBtAGEAaQBuACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAE4AVAAoAFYAQQBMAFUARQAoAF8AcgBlAG0AYQBpAG4AKQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAIABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQAsACAASQBGAFMAKABfAGQAZQBuAG8AdABlAGQAWQBlAGEAcgAsACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdgBhAGwAIAA8AD0AIAAwACwAIAB7ACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdgBhAGwAIAA8AD0AIAAzADEALAAgAF8AdgBhAGwALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAIABcACIAXAAiAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AeQBlAGEAcgAsACAASQBGAFMAKABfAGQAZQBuAG8AdABlAGQAWQBlAGEAcgAsACAAXwB2AGEAbAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdgBhAGwAIAA8AD0AIAAzADEALAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAIABfAHYAYQBsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXwB5AGUAYQByACwAIABfAG0AbwBuAHQAaAAsACAAXwBkAGEAeQAsACAAXAAiAFwAIgApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYwBvAGwAcwAgAD0AIAAyACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBwADEALAAgAEkATgBEAEUAWAAoAF8AcABhAHIAdABzACwAIAAxACwAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAcABhAGMAZQBQAG8AcwAsACAASQBGAEUAUgBSAE8AUgAoAEYASQBOAEQAKABcACIAIABcACIALAAgAF8AcAAxACkALAAgADAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAF8AcwBwAGEAYwBlAFAAbwBzACAAPQAgADAALAAgAHsAIwBWAEEATABVAEUAIQAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AbwBuAHQAaAAsACAAUABBAFIAUwBFAF8ATQBPAE4AVABIACgATABFAEYAVAAoAF8AcAAxACwAIABfAHMAcABhAGMAZQBQAG8AcwAgAC0AIAAxACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAYQB5ACwAIABJAE4AVAAoAFYAQQBMAFUARQAoAE0ASQBEACgAXwBwADEALAAgAF8AcwBwAGEAYwBlAFAAbwBzACAAKwAgADEALAAgAEwARQBOACgAXwBwADEAKQAgAC0AIABfAHMAcABhAGMAZQBQAG8AcwApACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHAAMgAsACAASQBOAEQARQBYACgAXwBwAGEAcgB0AHMALAAgADEALAAgADIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAcgB5AFQAaQBtAGUALAAgAEQAQQBUAEUAVgBBAEwAVQBFACgAXwBwADIAKQAgACsAIABUAEkATQBFAFYAQQBMAFUARQAoAF8AcAAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AGkAbQBlACwAIABJAEYARQBSAFIATwBSACgAXwB0AHIAeQBUAGkAbQBlACwAIABcACIAXAAiACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AGUAYQByACwAIABJAEYAKABJAFMARQBSAFIATwBSACgAXwB0AHIAeQBUAGkAbQBlACkALAAgAFAAQQBSAFMARQBfAEwASQBUAEUAUgBBAFIAWQBfAFkARQBBAFIAKABfAHAAMgApACwAIABcACIAXAAiACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABfAHkAZQBhAHIALAAgAF8AbQBvAG4AdABoACwAIABfAGQAYQB5ACwAIABfAHQAaQBtAGUAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGMAbwBsAHMAIAA9ACAAMwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AeQBlAGEAcgAsACAAUABBAFIAUwBFAF8ATABJAFQARQBSAEEAUgBZAF8AWQBFAEEAUgAoAEkATgBEAEUAWAAoAF8AcABhAHIAdABzACwAIAAxACwAIAAyACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdABpAG0AZQAsACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdABpAG0AZQBQAGEAcgB0ACwAIABJAE4ARABFAFgAKABfAHAAYQByAHQAcwAsACAAMQAsACAAMwApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABEAEEAVABFAFYAQQBMAFUARQAoAF8AdABpAG0AZQBQAGEAcgB0ACkAIAArACAAVABJAE0ARQBWAEEATABVAEUAKABfAHQAaQBtAGUAUABhAHIAdAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHAAMQAsACAASQBOAEQARQBYACgAXwBwAGEAcgB0AHMALAAgADEALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBwAGEAYwBlAFAAbwBzACwAIABJAEYARQBSAFIATwBSACgARgBJAE4ARAAoAFwAIgAgAFwAIgAsACAAXwBwADEAKQAsACAAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBzAHAAYQBjAGUAUABvAHMAIAA9ACAAMAAsACAAewAjAFYAQQBMAFUARQAhACwAIABcACIAXAAiACwAIABcACIAXAAiACwAIABcACIAXAAiAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbQBvAG4AdABoACwAIABQAEEAUgBTAEUAXwBNAE8ATgBUAEgAKABMAEUARgBUACgAXwBwADEALAAgAF8AcwBwAGEAYwBlAFAAbwBzACAALQAgADEAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkALAAgAEkATgBUACgAVgBBAEwAVQBFACgATQBJAEQAKABfAHAAMQAsACAAXwBzAHAAYQBjAGUAUABvAHMAIAArACAAMQAsACAATABFAE4AKABfAHAAMQApACAALQAgAF8AcwBwAGEAYwBlAFAAbwBzACkAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXwB5AGUAYQByACwAIABfAG0AbwBuAHQAaAAsACAAXwBkAGEAeQAsACAAXwB0AGkAbQBlACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABSAFUARQAsACAAewAjAFYAQQBMAFUARQAhACwAIABcACIAXAAiACwAIABcACIAXAAiACwAIABcACIAXAAiAH0AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIABfAHIAZQBzAHUAbAB0ACwAIABSAEUARABVAEMARQAoAFwAIgBcACIALAAgAEwAaQB0AGUAcgBhAHIAeQBEAGEAdABlACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwAQQBNAEIARABBACgAXwBhAGMAYwAsACAAXwBjAHUAcgByAGUAbgB0ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcABhAHIAdABzACwAIABmAG4AUABhAHIAcwBlAEQAYQB0AGUAKABfAGMAdQByAHIAZQBuAHQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVgBTAFQAQQBDAEsAKABfAGEAYwBjACwAIABfAHAAYQByAHQAcwApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIABEAFIATwBQACgAXwByAGUAcwB1AGwAdAAsACAAMQApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFAAQQBSAFMARQBfAFUAUwBfAEQAQQBUAEUAXABuAFwAbgBQAGEAcgBzAGUAcwAgAGEAIABVAFMAIABmAG8AcgBtAGEAdABlAGQAIABkAGEAdABlACAAaQBuAHQAbwAgAHIAZQBzAHAAZQBjAHQAaQB2AGUAIABwAGEAcgB0AHMAIABvAGYAIAB5AGUAYQByACwAIABtAG8AbgB0AGgALAAgAGQAYQB5ACAAYQBuAGQAIAB0AGkAbQBlACAAbwBmACAAZABhAHkALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAaQBuAHQAZQBnAGUAcgAgACAAIAAgACAAIAAgACAAIAB8ACAAWQBlAGEAcgBcAG4AIAAyACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADEALgAuADEAMgBdACAAfAAgAE0AbwBuAHQAaABcAG4AIAAzACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADEALgAuADMAMQBdACAAfAAgAEQAYQB5AFwAbgAgADQAIAB8ACAAZABlAGMAaQBtAGEAbAAgAFsAMAAuAC4AMQApACAAIAB8ACAAVABpAG0AZQBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFUAUwBEAGEAdABlACAAfAAgAHQAZQB4AHQAIAB8ACAARABhAHQAZQAgAGkAbgAgAFUAUwAgAGYAbwByAG0AYQB0ACAAaQBlAC4AIABNAE0ALwBkAGQALwB5AHkAeQB5ACAAaABoADoAbQBtADoAcwBzAFwAbgBcAG4ARQB4AGEAbQBwAGwAZQBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBQAEEAUgBTAEUAXwBVAFMAXwBEAEEAVABFACgAXAAiADEALwAyADUALwAyADAAMQA0ACAANgA6ADAAMABcACIAKQBcAG4AUgBlAHQAdQByAG4AcwA6ACAAewAyADAAMQA0ACwAIAAxACwAIAAyADUALAAgADAALgAyADUAfQBcAG4AXABuAFAAQQBSAFMARQBfAFUAUwBfAEQAQQBUAEUAKABcACIAMQAyAC8AMwAxAC8AMgAwADIAMwAgADIANAA6ADAAMABcACIAKQBcAG4AUgBlAHQAdQByAG4AcwA6ACAAewAyADAAMgAzACwAIAAxADIALAAgADMAMQAsACAAMQB9AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBQAEEAUgBTAEUAXwBVAFMAXwBEAEEAVABFACAAPQAgAEwAQQBNAEIARABBACgAVQBTAEQAYQB0AGUALABcAG4AIAAgACAAIABJAEYAKABVAFMARABhAHQAZQAgAD0AIABcACIAXAAiACwAIAB7AFwAIgBcACIALAAgAFwAIgBcACIALAAgAFwAIgBcACIALAAgAFwAIgBcACIAfQAsAFwAbgAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAZgBuAEkAbgB2AGEAbABpAGQAQwBoAGEAcgBzACwAIABMAEEATQBCAEQAQQAoAF8AdABlAHgAdAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGMAaABhAHIAUwBlAHQALAAgAFwAIgAgACwALQAuAC8AMAAxADIAMwA0ADUANgA3ADgAOQA6AEEATQBQAFQAYQBtAHAAXwBcACIAIAAmACAAVQBOAEkAQwBIAEEAUgAoADgANwAyADIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBlAHMAYwBhAHAAZQBUAGUAeAB0ACwAIABTAFUAQgBTAFQASQBUAFUAVABFACgAUwBVAEIAUwBUAEkAVABVAFQARQAoAF8AdABlAHgAdAAsACAAXAAiACYAXAAiACwAIABcACIAJgBhAG0AcAA7AFwAIgApACwAIABcACIAPABcACIALAAgAFwAIgAmAGwAdAA7AFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHgAbQBsACwAIABcACIAPAB0AD4APABzAD4AXAAiACAAJgAgAF8AZQBzAGMAYQBwAGUAVABlAHgAdAAgACYAIABcACIAPAAvAHMAPgA8AC8AdAA+AFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB4AHAAYQB0AGgALAAgAFwAIgAvAC8AcwBbAHQAcgBhAG4AcwBsAGEAdABlACgALgAsACcAXAAiACAAJgAgAF8AYwBoAGEAcgBTAGUAdAAgACYAIABcACIAJwAsACcAJwApAD0AJwAnAF0AXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAFMARQBSAFIATwBSACgARgBJAEwAVABFAFIAWABNAEwAKABfAHgAbQBsACwAIABfAHgAcABhAHQAaAApACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAZgBuAEMAbwB1AG4AdABDAGgAYQByAHMALAAgAEwAQQBNAEIARABBACgAQwBoAGEAcgBBAHIAcgBhAHkALAAgAFQAZQB4AHQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAZQB4AHQAIAA9ACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwByAGUAbQBvAHYAZQBkACwAIABSAEUARABVAEMARQAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAZQB4AHQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABDAGgAYQByAEEAcgByAGEAeQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwAQQBNAEIARABBACgAXwBhAGMAYwAsACAAXwBjAHUAcgByACwAIABTAFUAQgBTAFQASQBUAFUAVABFACgAXwBhAGMAYwAsACAAXwBjAHUAcgByACwAIABcACIAXAAiACkAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUATgAoAFQAZQB4AHQAKQAgAC0AIABMAEUATgAoAF8AcgBlAG0AbwB2AGUAZAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABmAG4ARgBpAG4AZABOAHQAaABDAGgAYQByAFAAbwBzACwAIABMAEEATQBCAEQAQQAoAEMAaABhAHIAcwAsACAAVABlAHgAdAAsACAATgAsACAAWwBTAHQAYQByAHQAUABvAHMAXQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAE4AKABTAHQAYQByAHQAUABvAHMAKQAgAD4AIABMAEUATgAoAFQAZQB4AHQAKQAsACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBmAHIAbwBtAFAAbwBzACwAIABJAEYAKABOACgAUwB0AGEAcgB0AFAAbwBzACkAIAA8AD0AIAAwACwAIAAwACwAIABOACgAUwB0AGEAcgB0AFAAbwBzACkAIAAtACAAMQApACwAIABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AGUAeAB0ACwAIABJAEYAKABfAGYAcgBvAG0AUABvAHMAIAA9ACAAMAAsACAAVABlAHgAdAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFIASQBHAEgAVAAoAFQAZQB4AHQALAAgAEwARQBOACgAVABlAHgAdAApACAALQAgAF8AZgByAG8AbQBQAG8AcwApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYwBoAGEAcgBDAG8AdQBuAHQALAAgAEwARQBOACgAQwBoAGEAcgBzACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBuACwAIABJAE4AVAAoAE4AKABOACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKAAoAF8AYwBoAGEAcgBDAG8AdQBuAHQAIAA9ACAAMAApACAAKwAgACgAXwBuACAAPQAgADAAKQAsACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGMAaABhAHIAcwAsACAATQBJAEQAKABDAGgAYQByAHMALAAgAFMARQBRAFUARQBOAEMARQAoADEALAAgAF8AYwBoAGEAcgBDAG8AdQBuAHQAKQAsACAAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGYAaQBuAGQAQwBvAHUAbgB0ACwAIABmAG4AQwBvAHUAbgB0AEMAaABhAHIAcwAoAF8AYwBoAGEAcgBzACwAIABfAHQAZQB4AHQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBmAGkAbgBkAEMAbwB1AG4AdAAgADwAIABBAEIAUwAoAF8AbgApACwAIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAbgB0AGgAIABjAGEAbgAgAGMAbwB1AG4AdAAgAGYAcgBvAG0AIABlAG4AZAAgAGIAYQBjAGsAdwBhAHIAZABzAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbgB0AGgALAAgAEkARgAoAF8AbgAgAD4AIAAwACwAIABfAG4ALAAgAF8AZgBpAG4AZABDAG8AdQBuAHQAIAArACAAXwBuACAAKwAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbgB0AGgAUABvAHMALAAgAFIARQBEAFUAQwBFACgAMAAsACAAUwBFAFEAVQBFAE4AQwBFACgAMQAsACAAXwBuAHQAaAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEEATQBCAEQAQQAoAF8AYQBjAGMALAAgAF8AYwB1AHIAcgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAGEAYwBjACAAPAAgADAALAAgAC0AMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG4AZQB4AHQAUABvAHMAQwBoAGEAcgBzACwAIABJAEYARQBSAFIATwBSACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEYASQBOAEQAKABfAGMAaABhAHIAcwAsACAAXwB0AGUAeAB0ACwAIABfAGEAYwBjACAAKwAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAwAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBuAGUAeAB0AFAAbwBzACwAIABNAEkATgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABGAEkATABUAEUAUgAoAF8AbgBlAHgAdABQAG8AcwBDAGgAYQByAHMALAAgAF8AbgBlAHgAdABQAG8AcwBDAGgAYQByAHMAIAA+ACAAMAAsACAAMAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBuAGUAeAB0AFAAbwBzACAAPQAgADAALAAgAC0AMQAsACAAXwBuAGUAeAB0AFAAbwBzACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAF8AbgB0AGgAUABvAHMAIAA+ACAAMAAsACAAXwBuAHQAaABQAG8AcwAgACsAIABfAGYAcgBvAG0AUABvAHMAIAAsACAAMAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABmAG4AWQBlAGEAcgBWAGEAbAB1AGUALAAgAEwAQQBNAEIARABBACgAXwB0AGUAeAB0ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYwBoAGEAcgAxACwAIABMAEUARgBUACgAXwB0AGUAeAB0ACwAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBpAGcAbgAsACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBjAGgAYQByADEAIAA9ACAAXAAiACsAXAAiACwAIAAxACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYwBoAGEAcgAxACAAPQAgAFwAIgAtAFwAIgAsACAALQAxACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFUATgBJAEMATwBEAEUAKABfAGMAaABhAHIAMQApACAAPQAgADgANwAyADIALAAgAC0AMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAIABcACIAXAAiAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBzAGkAZwBuACAAPQAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBOAFQAKABWAEEATABVAEUAKABfAHQAZQB4AHQAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBpAGcAbgAgACoAIABJAE4AVAAoAFYAQQBMAFUARQAoAFIASQBHAEgAVAAoAF8AdABlAHgAdAAsACAATABFAE4AKABfAHQAZQB4AHQAKQAgAC0AMQApACkAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAZgBuAEkAbgB2AGEAbABpAGQAQwBoAGEAcgBzACgAVQBTAEQAYQB0AGUAKQAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBwAG8AcwAxACwAIABmAG4ARgBpAG4AZABOAHQAaABDAGgAYQByAFAAbwBzACgAXAAiACwALgAvAC0AXwBcACIALAAgAFUAUwBEAGEAdABlACwAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcABvAHMAMgAsACAAZgBuAEYAaQBuAGQATgB0AGgAQwBoAGEAcgBQAG8AcwAoAFwAIgAsAC4ALwAtAF8AXAAiACwAIABVAFMARABhAHQAZQAsACAAMgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHAAbwBzADMALAAgAEkARgAoAF8AcABvAHMAMgAgAD0AIAAwACwAIAAwACwAIABmAG4ARgBpAG4AZABOAHQAaABDAGgAYQByAFAAbwBzACgAXAAiACwALgAvAC0AXwBUACAAXAAiACwAIABVAFMARABhAHQAZQAsACAAMQAsACAAXwBwAG8AcwAyACAAKwAgADIAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHAAbwBzADQALAAgAEkARgAoAF8AcABvAHMAMwAgAD0AIAAwACwAIAAwACwAIABmAG4ARgBpAG4AZABOAHQAaABDAGgAYQByAFAAbwBzACgAXAAiADAAMQAyADMANAA1ADYANwA4ADkAXAAiACwAIABVAFMARABhAHQAZQAsACAAMQAsACAATQBBAFgAKABfAHAAbwBzADIALAAgAF8AcABvAHMAMwApACAAKwAgADEAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AbwBuAHQAaAAsACAASQBGACgAXwBwAG8AcwAxACAAPQAgADAALAAgACMAVgBBAEwAVQBFACEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBOAFQAKABWAEEATABVAEUAKABMAEUARgBUACgAVQBTAEQAYQB0AGUALAAgAF8AcABvAHMAMQAgAC0AIAAxACkAKQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQAsACAASQBGACgAXwBwAG8AcwAyACAAPQAgADAALAAgACMAVgBBAEwAVQBFACEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBOAFQAKABWAEEATABVAEUAKABNAEkARAAoAFUAUwBEAGEAdABlACwAIABfAHAAbwBzADEAIAArACAAMQAsACAAXwBwAG8AcwAyACAALQAgAF8AcABvAHMAMQAgAC0AIAAxACkAKQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AGUAYQByACwAIABmAG4AWQBlAGEAcgBWAGEAbAB1AGUAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBwAG8AcwAzACAAPQAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABSAEkARwBIAFQAKABVAFMARABhAHQAZQAsACAATABFAE4AKABVAFMARABhAHQAZQApACAALQAgAF8AcABvAHMAMgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATQBJAEQAKABVAFMARABhAHQAZQAsACAAXwBwAG8AcwAyACAAKwAgADEALAAgAF8AcABvAHMAMwAgAC0AIABfAHAAbwBzADIAIAAtACAAMQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AGkAbQBlACwAIABJAEYAKABfAHAAbwBzADQAIAA9ACAAMAAsACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdABpAG0AZQBQAGEAcgB0ACwAIABSAEkARwBIAFQAKABVAFMARABhAHQAZQAsACAATABFAE4AKABVAFMARABhAHQAZQApACAALQAgAF8AcABvAHMANAAgACsAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABEAEEAVABFAFYAQQBMAFUARQAoAF8AdABpAG0AZQBQAGEAcgB0ACkAIAArACAAVABJAE0ARQBWAEEATABVAEUAKABfAHQAaQBtAGUAUABhAHIAdAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABfAHkAZQBhAHIALAAgAF8AbQBvAG4AdABoACwAIABfAGQAYQB5ACwAIABfAHQAaQBtAGUAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBQAEEAUgBTAEUAXwBNAEkATABfAEQAVABHAFwAbgBcAG4AUABhAHIAcwBlAHMAIABhACAAZABhAHQAZQAtAHQAaQBtAGUAIABnAHIAbwB1AHAAIABpAG4AIAB0AGgAZQAgAGYAbwByAG0AYQB0ACAAdQBzAGUAZAAgAGIAeQAgAFUAUwAgAE0AaQBsAGkAdABhAHIAeQAgAG0AZQBzAHMAYQBnAGUAIAB0AHIAYQBmAGYAaQBjACwAIABpAG4AdABvACAAcgBlAHMAcABlAGMAdABpAHYAZQAgAHAAYQByAHQAcwAgAG8AZgAgAHkAZQBhAHIALABcAG4AbQBvAG4AdABoACwAIABkAGEAeQAsACAAdABpAG0AZQAgAG8AZgAgAGQAYQB5ACAAYQBuAGQAIAB0AGkAbQBlACAAegBvAG4AZQAgAG8AZgBmAHMAZQB0ACAAaQBuACAAbQBpAG4AdQB0AGUAcwAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABpAG4AdABlAGcAZQByACAAWwAxADkANQAxAC4ALgAyADAANQAwAF0AIAB8ACAAWQBlAGEAcgBcAG4AIAAyACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADEALgAuADEAMgBdACAAIAAgACAAIAAgAHwAIABNAG8AbgB0AGgAXABuACAAMwAgAHwAIABpAG4AdABlAGcAZQByACAAWwAxAC4ALgAzADEAXQAgACAAIAAgACAAIAB8ACAARABhAHkAXABuACAANAAgAHwAIABkAGUAYwBpAG0AYQBsACAAWwAwAC4ALgAxACkAIAAgACAAIAAgACAAIAB8ACAAVABpAG0AZQBcAG4AIAA1ACAAfAAgAGQAZQBjAGkAbQBhAGwAIABbAC0AOQAwADAALgAuADkAMAAwAF0AIAAgAHwAIABUAGkAbQBlACAAegBvAG4AZQAgAG8AZgBmAHMAZQB0ACAAbQBpAG4AdQB0AGUAcwBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEQAVABHACAAfAAgAHQAZQB4AHQAIAB8ACAARABhAHQAZQAtAHQAaQBtAGUAIABnAHIAbwB1AHAAIABpAG4AIABVAFMAIABNAGkAbABpAHQAYQByAHkAIABmAG8AcgBtAGEAdAAgAGkAZQAuACAAZABkAEgASABtAG0AcwBzAFoAbQBtAG0AWQBZAFwAbgBcAG4ARQB4AGEAbQBwAGwAZQBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBQAEEAUgBTAEUAXwBNAEkATABfAEQAVABHACgAXAAiADEAMgAgADEANQAgADMAMAAgADQANQAgAEIAIABNAEEAWQAgADIAMwBcACIAKQBcAG4AUgBlAHQAdQByAG4AcwA6ACAAewAyADAAMgAzACwAIAA1ACwAIAAxADIALAAgADAALgA3ADcAMQAxADgAMAA1ADUALAAgADEAMgAwAH0AXABuAFwAbgBQAEEAUgBTAEUAXwBNAEkATABfAEQAVABHACgAXAAiADAANQAwADYANAA1ADEANQBLAEoAVQBOADAAMABcACIAKQBcAG4AUgBlAHQAdQByAG4AcwA6ACAAewAyADAAMAAwACwAIAA2ACwAIAA1ACwAIAAwAC4AMgA4ADEANAAyADMANgAxADEALAAgADYAMAAwAH0AXABuAFwAbgBQAEEAUgBTAEUAXwBNAEkATABfAEQAVABHACgAXAAiADEANQAwADYAMAAwAFoAXAAiACkAXABuAFIAZQB0AHUAcgBuAHMAOgAgAHsAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAMQA1ACwAIAAwAC4AMgA1ACwAIAAwAH0AXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAFAAQQBSAFMARQBfAE0ASQBMAF8ARABUAEcAIAA9ACAATABBAE0AQgBEAEEAKABEAFQARwAsAFwAbgAgACAAIAAgAEkARgAoAEQAVABHACAAPQAgAFwAIgBcACIALAAgAHsAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgB9ACwAXABuACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABmAG4ASQBuAHYAYQBsAGkAZABDAGgAYQByAHMALAAgAEwAQQBNAEIARABBACgAXwB0AGUAeAB0ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYwBoAGEAcgBTAGUAdAAsACAAXAAiADAAMQAyADMANAA1ADYANwA4ADkAQQBCAEMARABFAEYARwBIAEkASgBLAEwATQBOAE8AUABRAFIAUwBUAFUAVgBXAFgAWQBaAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBlAHMAYwBhAHAAZQBUAGUAeAB0ACwAIABTAFUAQgBTAFQASQBUAFUAVABFACgAUwBVAEIAUwBUAEkAVABVAFQARQAoAF8AdABlAHgAdAAsACAAXAAiACYAXAAiACwAIABcACIAJgBhAG0AcAA7AFwAIgApACwAIABcACIAPABcACIALAAgAFwAIgAmAGwAdAA7AFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHgAbQBsACwAIABcACIAPAB0AD4APABzAD4AXAAiACAAJgAgAF8AZQBzAGMAYQBwAGUAVABlAHgAdAAgACYAIABcACIAPAAvAHMAPgA8AC8AdAA+AFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB4AHAAYQB0AGgALAAgAFwAIgAvAC8AcwBbAHQAcgBhAG4AcwBsAGEAdABlACgALgAsACcAXAAiACAAJgAgAF8AYwBoAGEAcgBTAGUAdAAgACYAIABcACIAJwAsACcAJwApAD0AJwAnAF0AXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAFMARQBSAFIATwBSACgARgBJAEwAVABFAFIAWABNAEwAKABfAHgAbQBsACwAIABfAHgAcABhAHQAaAApACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAZgBuAFkAZQBhAHIALAAgAEwAQQBNAEIARABBACgAXwBzAFkAZQBhAHIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AHkALAAgAFYAQQBMAFUARQAoAF8AcwBZAGUAYQByACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAF8AeQB5ACAAPAAgADUAMQAsACAAMgAwADAAMAAgACsAIABfAHkAeQAsACAAMQA5ADAAMAAgACsAIABfAHkAeQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAGYAbgBUAGkAbQBlACwAIABMAEEATQBCAEQAQQAoAF8AaABvAHUAcgAsACAAXwBtAGkAbgB1AHQAZQAsACAAXwBzAGUAYwBvAG4AZAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAF8AVgBBAEwASQBEAF8AVABJAE0ARQAoAF8AaABvAHUAcgAsACAAXwBtAGkAbgB1AHQAZQAsACAAXwBzAGUAYwBvAG4AZAApACkALAAgAHsAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoAE4AKABfAGgAbwB1AHIAKQAgAC8AIAAyADQAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACsAIAAoAE4AKABfAG0AaQBuAHUAdABlACkAIAAvACAAMQA0ADQAMAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKwAgACgATgAoAF8AcwBlAGMAbwBuAGQAKQAgAC8AIAA4ADYANAAwADAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABmAG4AUABhAHIAcwBlAFQAWgAsACAATABBAE0AQgBEAEEAKABfAHQAegBDAGgAYQByACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYwBvAGQAZQAsACAAQwBPAEQARQAoAF8AdAB6AEMAaABhAHIAKQAgAC0AIAA2ADQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYwBvAGQAZQAgAD0AIAAyADYALAAgADAALAAgAC8ALwAgAFoAIAA9ACAAVQBUAEMAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYwBvAGQAZQAgAD0AIAAxADAALAAgAFwAIgBcACIALAAgAC8ALwAgAEoAIAA9ACAATABvAGMAYQBsACAAVABpAG0AZQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBjAG8AZABlACAAPAA9ACAAMAAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBjAG8AZABlACAAPAA9ACAAOQAsACAAXwBjAG8AZABlACAAKgAgADYAMAAsACAALwAvACAAQQBCAEMARABFAEYARwBIAEkAIAAtAD4AIAArADEALgAuACsAOQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBjAG8AZABlACAAPAA9ACAAMQAzACwAIAAoAF8AYwBvAGQAZQAgAC0AIAAxACkAIAAqACAANgAwACwAIAAgAC8ALwAgAEsATABNACAALQA+ACAAKwAxADAALgAuACsAMQAyAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGMAbwBkAGUAIAA8AD0AIAAyADUALAAgACgAMQAzACAALQAgAF8AYwBvAGQAZQApACAAKgAgADYAMAAsACAALwAvACAATgBPAFAAUQBSAFMAVABVAFYAVwBYAFkAIAAtAD4AIAAtADEALgAuAC0AMQAyAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAIAB7ACMAVgBBAEwAVQBFACEAfQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAZgBuAFAAYQByAHMAZQBGAHUAbABsACwAIABMAEEATQBCAEQAQQAoAF8ARABUAEcALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQAsACAAVgBBAEwAVQBFACgATABFAEYAVAAoAF8ARABUAEcALAAgADIAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AbwBuAHQAaAAsACAAUABBAFIAUwBFAF8ATQBPAE4AVABIACgATQBJAEQAKABfAEQAVABHACwAIAAxADAALAAgADMAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIALAAgAGYAbgBZAGUAYQByACgAUgBJAEcASABUACgAXwBEAFQARwAsACAAMgApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAF8AVgBBAEwASQBEAF8ARABBAFQARQAoAF8AeQBlAGEAcgAsACAAXwBtAG8AbgB0AGgALAAgAF8AZABhAHkALAAgADAAKQApACwAIAB7ACMAVgBBAEwAVQBFACEALAAgACMAVgBBAEwAVQBFACEALAAgACMAVgBBAEwAVQBFACEALAAgACMAVgBBAEwAVQBFACEALAAgACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AaABvAHUAcgAsACAAVgBBAEwAVQBFACgATQBJAEQAKABfAEQAVABHACwAIAAzACwAIAAyACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbQBpAG4AdQB0AGUALAAgAFYAQQBMAFUARQAoAE0ASQBEACgAXwBEAFQARwAsACAANQAsACAAMgApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAZQBjAG8AbgBkACwAIABWAEEATABVAEUAKABNAEkARAAoAF8ARABUAEcALAAgADcALAAgADIAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AGkAbQBlACwAIABmAG4AVABpAG0AZQAoAF8AaABvAHUAcgAsACAAXwBtAGkAbgB1AHQAZQAsACAAXwBzAGUAYwBvAG4AZAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AHoALAAgAGYAbgBQAGEAcgBzAGUAVABaACgATQBJAEQAKABfAEQAVABHACwAIAA5ACwAIAAxACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAF8AVgBBAEwASQBEAF8AVABJAE0ARQAoAF8AaABvAHUAcgAsACAAXwBtAGkAbgB1AHQAZQAsACAAXwBzAGUAYwBvAG4AZAApACkALAAgAHsAIwBWAEEATABVAEUAIQAsACAAIwBWAEEATABVAEUAIQAsACAAIwBWAEEATABVAEUAIQAsACAAIwBWAEEATABVAEUAIQAsACAAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBtAG8AbgB0AGgALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAaQBtAGUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AHoAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAGYAbgBQAGEAcgBzAGUAUwBoAG8AcgB0ACwAIABMAEEATQBCAEQAQQAoAF8ARABUAEcALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQAsACAAVgBBAEwAVQBFACgATABFAEYAVAAoAF8ARABUAEcALAAgADIAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AbwBuAHQAaAAsACAAUABBAFIAUwBFAF8ATQBPAE4AVABIACgATQBJAEQAKABfAEQAVABHACwAIAA4ACwAIAAzACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AGUAYQByACwAIABmAG4AWQBlAGEAcgAoAFIASQBHAEgAVAAoAF8ARABUAEcALAAgADIAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBfAFYAQQBMAEkARABfAEQAQQBUAEUAKABfAHkAZQBhAHIALAAgAF8AbQBvAG4AdABoACwAIABfAGQAYQB5ACwAIAAwACkAKQAsACAAewAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGgAbwB1AHIALAAgAFYAQQBMAFUARQAoAE0ASQBEACgAXwBEAFQARwAsACAAMwAsACAAMgApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AaQBuAHUAdABlACwAIABWAEEATABVAEUAKABNAEkARAAoAF8ARABUAEcALAAgADUALAAgADIAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AHoALAAgAGYAbgBQAGEAcgBzAGUAVABaACgATQBJAEQAKABfAEQAVABHACwAIAA3ACwAIAAxACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAF8AVgBBAEwASQBEAF8AVABJAE0ARQAoAF8AaABvAHUAcgAsACAAXwBtAGkAbgB1AHQAZQAsACAAXAAiAFwAIgApACkALAAgAHsAIwBWAEEATABVAEUAIQAsACAAIwBWAEEATABVAEUAIQAsACAAIwBWAEEATABVAEUAIQAsACAAIwBWAEEATABVAEUAIQAsACAAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBtAG8AbgB0AGgALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAEkATQBFACgAXwBoAG8AdQByACwAIABfAG0AaQBuAHUAdABlACwAIAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AHoAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAGYAbgBQAGEAcgBzAGUAUABsAGEAbgAsACAATABBAE0AQgBEAEEAKABfAEQAVABHACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkALAAgAFYAQQBMAFUARQAoAEwARQBGAFQAKABfAEQAVABHACwAIAAyACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBoAG8AdQByACwAIABWAEEATABVAEUAKABNAEkARAAoAF8ARABUAEcALAAgADMALAAgADIAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AaQBuAHUAdABlACwAIABWAEEATABVAEUAKABNAEkARAAoAF8ARABUAEcALAAgADUALAAgADIAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegAsACAAZgBuAFAAYQByAHMAZQBUAFoAKABNAEkARAAoAF8ARABUAEcALAAgADcALAAgADEAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBfAFYAQQBMAEkARABfAFQASQBNAEUAKABfAGgAbwB1AHIALAAgAF8AbQBpAG4AdQB0AGUALAAgAFwAIgBcACIAKQApACwAIAB7ACMAVgBBAEwAVQBFACEALAAgACMAVgBBAEwAVQBFACEALAAgACMAVgBBAEwAVQBFACEALAAgACMAVgBBAEwAVQBFACEALAAgACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQASQBNAEUAKABfAGgAbwB1AHIALAAgAF8AbQBpAG4AdQB0AGUALAAgADAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdAB6AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAEQAVABHACwAIABTAFUAQgBTAFQASQBUAFUAVABFACgARABUAEcALAAgAFwAIgAgAFwAIgAsACAAXAAiAFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAGYAbgBJAG4AdgBhAGwAaQBkAEMAaABhAHIAcwAoAF8ARABUAEcAKQAsACAAewAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBsAGUAbgAsACAATABFAE4AKABfAEQAVABHACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZgBtAHQALAAgAEkARgBTACgAXwBsAGUAbgAgAD0AIAAxADQALAAgADEALAAgAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGwAZQBuACAAPQAgADEAMgAsACAAMgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGwAZQBuACAAPQAgADcALAAgADMALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABSAFUARQAsACAAMABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAF8AZgBtAHQAIAA9ACAAMAAsACAAewAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGYAbQB0ACAAPQAgADEALAAgAGYAbgBQAGEAcgBzAGUARgB1AGwAbAAoAF8ARABUAEcAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZgBtAHQAIAA9ACAAMgAsACAAZgBuAFAAYQByAHMAZQBTAGgAbwByAHQAKABfAEQAVABHACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGYAbQB0ACAAPQAgADMALAAgAGYAbgBQAGEAcgBzAGUAUABsAGEAbgAoAF8ARABUAEcAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAFwAbgBcAG4AXABuAFwAbgBcAG4AXABuAFwAbgBcAG4AXABuAFwAbgBcAG4ALwAqACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwBcAG4AIwAgAFQARQBYAFQAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACoALwBcAG4AXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBXAEUARQBLAEQAQQBZAF8ATgBBAE0ARQBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIABuAGEAbQBlACAAbwBmACAAYQBuACAASQBTAE8AIABkAGEAeQAgAG8AZgAgAHcAZQBlAGsAIABuAHUAbQBiAGUAcgAgAGEAcwAgAHQAZQB4AHQALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAdABlAHgAdAAgAHwAIABXAGUAZQBrAGQAYQB5AFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ASQBTAE8AVwBlAGUAawBEAGEAeQAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAWwAxAC4ALgA3AF0AIAB8ACAASQBTAE8AIABkAGEAeQAgAG8AZgAgAHcAZQBlAGsAIABuAHUAbQBiAGUAcgBcAG4AWwBTAGgAbwByAHQAXQAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABzAHcAaQB0AGMAaAAgACAAIAAgACAAIAAgACAAIAB8ACAAUgBlAHQAdQByAG4AIABzAGgAbwByAHQAIABmAG8AcgBtAGEAdAAgAE0AbwBuAC4ALgBTAHUAbgBcAG4AWwBJAG4AdABlAHIAbgBhAHQAaQBvAG4AYQBsAEUAbgBnAGwAaQBzAGgAXQAgAHwAIABzAHcAaQB0AGMAaAAgACAAIAAgACAAIAAgACAAIAB8ACAASQBuAHQAZQByAG4AYQB0AGkAbwBuAGEAbAAgAEUAbgBnAGwAaQBzAGgAIABpAG4AcwB0AGUAYQBkACAAbwBmACAAbABvAGMAYQBsACAAbABhAG4AZwB1AGEAZwBlACAAcwBlAHQAIABpAG4AIABFAHgAYwBlAGwAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAFcARQBFAEsARABBAFkAXwBOAEEATQBFACAAPQAgAEwAQQBNAEIARABBACgASQBTAE8AVwBlAGUAawBEAGEAeQAsACAAWwBTAGgAbwByAHQAXQAsACAAWwBJAG4AdABlAHIAbgBhAHQAaQBvAG4AYQBsAEUAbgBnAGwAaQBzAGgAXQAsAFwAbgAgACAAIAAgAEkARgAoAEkAUwBPAFcAZQBlAGsARABhAHkAIAA9ACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABJAFMATwBXAGUAZQBrAEQAYQB5ACkAKQAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHUAcwBlAFMAaABvAHIAdAAsACAATgAoAFMAaABvAHIAdAApACAAPAA+ACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdQBzAGUATABvAGMAYQBsAEwAYQBuAGcALAAgAE4AKABJAG4AdABlAHIAbgBhAHQAaQBvAG4AYQBsAEUAbgBnAGwAaQBzAGgAKQAgAD0AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBpAHMAbwBEAG8AVwAsACAATQBPAEQAKABJAE4AVAAoAEkAUwBPAFcAZQBlAGsARABhAHkAKQAgAC0AIAAxACwAIAA3ACkAIAArACAAMQAsACAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwB1AHMAZQBMAG8AYwBhAGwATABhAG4AZwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5ADIAawByAGUAZgBEAGEAeQAsACAAMwA2ADUAMgA3ACAAKwAgAF8AaQBzAG8ARABvAFcALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBmAG0AdAAsACAASQBGACgAXwB1AHMAZQBTAGgAbwByAHQALAAgAFwAIgBkAGQAZABcACIALAAgAFwAIgBkAGQAZABkAFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQARQBYAFQAKABfAHkAMgBrAHIAZQBmAEQAYQB5ACwAIABfAGYAbQB0ACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB1AHMAZQBTAGgAbwByAHQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAQwBIAE8ATwBTAEUAKABfAGkAcwBvAEQAbwBXACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiAE0AbwBuAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBUAHUAZQBcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAVwBlAGQAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiAFQAaAB1AFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBGAHIAaQBcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAUwBhAHQAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiAFMAdQBuAFwAIgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABDAEgATwBPAFMARQAoAF8AaQBzAG8ARABvAFcALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIATQBvAG4AZABhAHkAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiAFQAdQBlAHMAZABhAHkAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiAFcAZQBkAG4AZQBzAGQAYQB5AFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBUAGgAdQByAHMAZABhAHkAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiAEYAcgBpAGQAYQB5AFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBTAGEAdAB1AHIAZABhAHkAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiAFMAdQBuAGQAYQB5AFwAIgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAE0ATwBOAFQASABfAE4AQQBNAEUAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAYQAgAG0AbwBuAHQAaAAgAGEAcwAgAHQAZQB4AHQALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAdABlAHgAdAAgAHwAIABNAG8AbgB0AGgAIABuAGEAbQBlAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ATQBvAG4AdABoACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAWwAxAC4ALgAxADIAXQAgAHwAIABNAG8AbgB0AGgAXABuAFsAUwBoAG8AcgB0AF0AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAcwB3AGkAdABjAGgAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAUgBlAHQAdQByAG4AIABzAGgAbwByAHQAIABmAG8AcgBtAGEAdAAgAEoAYQBuAC4ALgBEAGUAYwBcAG4AWwBJAG4AdABlAHIAbgBhAHQAaQBvAG4AYQBsAEUAbgBnAGwAaQBzAGgAXQAgAHwAIABzAHcAaQB0AGMAaAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABJAG4AdABlAHIAbgBhAHQAaQBvAG4AYQBsACAARQBuAGcAbABpAHMAaAAgAGkAbgBzAHQAZQBhAGQAIABvAGYAIABsAG8AYwBhAGwAIABsAGEAbgBnAHUAYQBnAGUAIABzAGUAdAAgAGkAbgAgAEUAeABjAGUAbABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ATQBPAE4AVABIAF8ATgBBAE0ARQAgAD0AIABMAEEATQBCAEQAQQAoAE0AbwBuAHQAaAAsACAAWwBTAGgAbwByAHQAXQAsACAAWwBJAG4AdABlAHIAbgBhAHQAaQBvAG4AYQBsAEUAbgBnAGwAaQBzAGgAXQAsAFwAbgAgACAAIAAgAEkARgAoAE0AbwBuAHQAaAAgAD0AIABcACIAXAAiACwAIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAE0AbwBuAHQAaAApACkALAAgACMAVgBBAEwAVQBFACEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHUAcwBlAFMAaABvAHIAdAAsACAATgAoAFMAaABvAHIAdAApACAAPAA+ACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdQBzAGUATABvAGMAYQBsAEwAYQBuAGcALAAgAE4AKABJAG4AdABlAHIAbgBhAHQAaQBvAG4AYQBsAEUAbgBnAGwAaQBzAGgAKQAgAD0AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBtAG8AbgB0AGgALAAgAEkATgBUACgATQBvAG4AdABoACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAHUAcwBlAEwAbwBjAGEAbABMAGEAbgBnACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAYQB5AE8AZgBNAG8AbgB0AGgALAAgAEQAQQBUAEUAKAAyADAAMAAwACwAIABfAG0AbwBuAHQAaAAsACAAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZgBtAHQALAAgAEkARgAoAF8AdQBzAGUAUwBoAG8AcgB0ACwAIABcACIATQBNAE0AXAAiACwAIABcACIATQBNAE0ATQBcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAEUAWABUACgAXwBkAGEAeQBPAGYATQBvAG4AdABoACwAIABfAGYAbQB0ACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB1AHMAZQBTAGgAbwByAHQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBOAEQARQBYACgAewBcACIASgBhAG4AXAAiADsAIABcACIARgBlAGIAXAAiADsAIABcACIATQBhAHIAXAAiADsAIABcACIAQQBwAHIAXAAiADsAIABcACIATQBhAHkAXAAiADsAIABcACIASgB1AG4AXAAiADsAIABcACIASgB1AGwAXAAiADsAIABcACIAQQB1AGcAXAAiADsAIABcACIAUwBlAHAAXAAiADsAIABcACIATwBjAHQAXAAiADsAIABcACIATgBvAHYAXAAiADsAIABcACIARABlAGMAXAAiAH0ALAAgAF8AbQBvAG4AdABoACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBOAEQARQBYACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAewBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBKAGEAbgB1AGEAcgB5AFwAIgA7AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiAEYAZQBiAHIAdQBhAHIAeQBcACIAOwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBNAGEAcgBjAGgAXAAiADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAQQBwAHIAaQBsAFwAIgA7AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiAE0AYQB5AFwAIgA7AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiAEoAdQBuAGUAXAAiADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIASgB1AGwAeQBcACIAOwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBBAHUAZwB1AHMAdABcACIAOwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBTAGUAcAB0AGUAbQBiAGUAcgBcACIAOwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBPAGMAdABvAGIAZQByAFwAIgA7AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiAE4AbwB2AGUAbQBiAGUAcgBcACIAOwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBEAGUAYwBlAG0AYgBlAHIAXAAiAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AbwBuAHQAaABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEYATwBSAE0AQQBUAF8ASQBTAE8AXwBEAEEAVABFAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAGEAIABkAGEAdABlACAAYQBzACAAdABlAHgAdAAgAGkAbgAgAEkAUwBPACAAZgBvAHIAbQBhAHQALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAdABlAHgAdAAgAHwAIABJAFMATwAgAGYAbwByAG0AYQB0AHQAZQBkACAAZABhAHQAZQBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFkAZQBhAHIAQwBFACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgACAAIAAgACAAIAAgACAAIAB8ACAATgBvAHQAZQAgAHQAaABhAHQAIAAxACAAQgBDACAAPQAgADAAIABDAEUALAAgADIAIABCAEMAIAA9ACAALQAxACAAQwBFAFwAbgBNAG8AbgB0AGgAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADEALgAuADEAMgBdACAAfABcAG4ARABhAHkAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAWwAxAC4ALgAzADEAXQAgAHwAXABuAFsAVABpAG0AZQBdACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgAFsAMAAuAC4AMQApACAAIAB8ACAAVABpAG0AZQAgAG8AZgAgAGQAYQB5ACAAYQBzACAAZABlAGMAaQBtAGEAbAAgAGYAcgBhAGMAdABpAG8AbgAgAG8AZgAgAGEAIABkAGEAeQAuAFwAbgBbAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdABdACAAfAAgAGQAZQBjAGkAbQBhAGwAIAAgACAAIAAgACAAIAAgACAAfAAgAFQAaQBtAGUAIAB6AG8AbgBlACAAbwBmAGYAcwBlAHQAIABpAG4AIABtAGkAbgB1AHQAZQBzACAAZgByAG8AbQAgAFUAVABDAC4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAWwAtADkAMAAwAC4ALgA5ADAAMABdACAAIAAgACAAIAB8ACAAQQBzAHMAdQBtAGUAZAAgAHQAbwAgAGIAZQAgAFUAVABDACAAaQBmACAAbwBtAG0AaQB0AHQAZQBkAC4AXABuAFsAUAByAGUAYwBpAHMAaQBvAG4AXQAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgACAAIAAgACAAIAAgACAAIAB8ACAAUwBlAGwAZQBjAHQAIABwAHIAZQBjAGkAcwBpAG8AbgAgAGwAZQB2AGUAbABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAMAAgAC0AIABGAGwAbwBhAHQAaQBuAGcAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADEAIAAtACAARABhAHkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADIAIAAtACAASABvAHUAcgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAMwAgAC0AIABNAGkAbgB1AHQAZQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAANAAgAC0AIABTAGUAYwBvAG4AZABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAANQAgAC0AIABNAGkAbABsAGkAcwBlAGMAbwBuAGQAXABuAFsATgBvAFoAdQBsAHUAXQAgACAAIAAgACAAIAAgACAAIAB8ACAAcwB3AGkAdABjAGgAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAVQBzAGUAIAArADAAMAA6ADAAMAAgAGkAbgBzAHQAZQBhAGQAIABvAGYAIABaACAAZgBvAHIAIABVAFQAQwAgAHQAaQBtAGUAIAB6AG8AbgBlAC4AXABuAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0AIAB8ACAAcwB3AGkAdABjAGgAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAQwBhAGwAYwB1AGwAYQB0AGUAIABmAG8AcgAgAHQAaABlACAASgB1AGwAaQBhAG4AIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuACAARABlAGYAYQB1AGwAdAAgAGkAcwAgAEcAcgBlAGcAbwByAGkAYQBuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AIABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ARgBPAFIATQBBAFQAXwBJAFMATwBfAEQAQQBUAEUAIAA9ACAATABBAE0AQgBEAEEAKABZAGUAYQByAEMARQAsACAATQBvAG4AdABoACwAIABEAGEAeQAsACAAWwBUAGkAbQBlAF0ALAAgAFsAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0AF0ALAAgAFsAUAByAGUAYwBpAHMAaQBvAG4AXQAsACAAWwBOAG8AWgB1AGwAdQBdACwAIABbAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACwAXABuACAAIAAgACAASQBGACgAKABZAGUAYQByAEMARQAgAD0AIABcACIAXAAiACkAIAAqACAAKABNAG8AbgB0AGgAIAA9ACAAXAAiAFwAIgApACAAKgAgACgARABhAHkAIAA9ACAAXAAiAFwAIgApACwAIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAFkAZQBhAHIAQwBFACkAKQAgACsAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAE0AbwBuAHQAaAApACkAIAArACAATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABEAGEAeQApACkALAAgAHsAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAF8AVgBBAEwASQBEAF8ARABBAFQARQAoAFkAZQBhAHIAQwBFACwAIABNAG8AbgB0AGgALAAgAEQAYQB5ACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQApACwAIAB7ACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABmAG4AUgBlAHMAbwBsAHYAZQBUAGkAbQBlACwAIABMAEEATQBCAEQAQQAoAF8AdABpAG0AZQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAF8AdABpAG0AZQApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAFkAZQBhAHIAQwBFACwAIABNAG8AbgB0AGgALAAgAEQAYQB5ACwAIABcACIAXAAiACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB1AHMAZQBQAHIAZQBjAGkAcwBpAG8AbgAsACAASQBGACgATgAoAFAAcgBlAGMAaQBzAGkAbwBuACkAIAA+ACAANQAsACAANQAsACAANAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABSAEUAUwBPAEwAVgBFAF8ARABBAFQARQAoAFkAZQBhAHIAQwBFACwAIABNAG8AbgB0AGgALAAgAEQAYQB5ACwAIABfAHQAaQBtAGUALAAgAF8AdQBzAGUAUAByAGUAYwBpAHMAaQBvAG4ALAAgAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAZgBuAEYAbwByAG0AYQB0AFkAZQBhAHIALAAgAEwAQQBNAEIARABBACgAXwB5AGUAYQByACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AGUAYQByAEYAbQB0ACwAIABJAEYAKAAoAF8AeQBlAGEAcgAgAD4APQAgADEAMAAwADAAKQAgACoAIAAoAF8AeQBlAGEAcgAgADwAPQAgADkAOQA5ADkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiADAAMAAwADAAOwBcACIAIAAmACAAVQBOAEkAQwBIAEEAUgAoADgANwAyADIAKQAgACYAIABcACIAMAAwADAAMABcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgArADAAMAAwADAAOwBcACIAIAAmACAAVQBOAEkAQwBIAEEAUgAoADgANwAyADIAKQAgACYAIABcACIAMAAwADAAMAA7ACsAMAAwADAAMABcACIAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQARQBYAFQAKABfAHkAZQBhAHIALAAgAF8AeQBlAGEAcgBGAG0AdAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAGYAbgBGAG8AcgBtAGEAdABUAGkAbQBlACwAIABMAEEATQBCAEQAQQAoAF8AdABpAG0AZQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAF8AdABpAG0AZQApACkALAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAcgBvAHUAbgBkACAAdABvACAAbQBpAGwAbABpAHMAZQBvAG4AZABzACwAIABzAGMAYQBsAGUAIAB0AG8AIABzAGUAYwBvAG4AZABzAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGUAYwBvAG4AZABzACwAIABSAE8AVQBOAEQAKABfAHQAaQBtAGUAIAAqACAAOAA2ADQAMAAwACwAIAAzACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBoAG8AdwBQAHIAZQBjAGkAcwBpAG8AbgAsACAASQBGACgATgAoAFAAcgBlAGMAaQBzAGkAbwBuACkAIAA+ACAAMAAsACAAUAByAGUAYwBpAHMAaQBvAG4ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGAFMAKABfAHMAZQBjAG8AbgBkAHMAIAA9ACAAMAAsACAAMgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAE0ATwBEACgAXwBzAGUAYwBvAG4AZABzACwAIAAxACkAIAA+ACAAMAAsACAANQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAE0ATwBEACgAXwBzAGUAYwBvAG4AZABzACAALwAgADYAMAAsACAAMQApACAAPgAgADAALAAgADQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABNAE8ARAAoAF8AcwBlAGMAbwBuAGQAcwAgAC8AIAAzADYAMAAwACwAIAAxACkAIAA+ACAAMAAsACAAMwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALAAgADIAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAHMAaABvAHcAUAByAGUAYwBpAHMAaQBvAG4AIAA9ACAAMQAsACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZgBtAHQALAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaABvAHcAUAByAGUAYwBpAHMAaQBvAG4AIAA9ACAAMgAsACAAXAAiAEgASABcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBoAG8AdwBQAHIAZQBjAGkAcwBpAG8AbgAgAD0AIAAzACwAIABcACIASABIADoAbQBtAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGgAbwB3AFAAcgBlAGMAaQBzAGkAbwBuACAAPQAgADQALAAgAFwAIgBIAEgAOgBtAG0AOgBzAHMAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAIABcACIASABIADoAbQBtADoAcwBzAC4AMAAwADAAXAAiAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAVABcACIAIAAmACAAVABFAFgAVAAoAF8AdABpAG0AZQAsACAAXwBmAG0AdAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAGYAbgBGAG8AcgBtAGEAdABUAFoALAAgAEwAQQBNAEIARABBACgAXwB0AHoAbwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAF8AdAB6AG8AKQApACwAIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAKABfAHQAegBvACAAPQAgADAAKQAgACoAIAAoAE4AKABOAG8AWgB1AGwAdQApACAAPQAgADAAKQAsACAAXAAiAFoAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBGAG0AdAAsACAASQBGACgATQBPAEQAKABfAHQAegBvACwAIAAxACkAIAA9ACAAMAAsACAAXAAiAEgASAA6AG0AbQBcACIALAAgAFwAIgBIAEgAOgBtAG0AOgBzAHMAXAAiACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGkAZwBuACwAIABJAEYAKABfAHQAegBvACAAPgA9ACAAMAAsACAAXAAiACsAXAAiACwAIABVAE4ASQBDAEgAQQBSACgAOAA3ADIAMgApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGkAZwBuACAAJgAgAFQARQBYAFQAKABBAEIAUwAoAF8AdAB6AG8AKQAgAC8AIAAxADQANAAwACwAIABfAHQAegBGAG0AdAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcgBEAGEAdABlACwAIABmAG4AUgBlAHMAbwBsAHYAZQBUAGkAbQBlACgAVABpAG0AZQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAWQBlAGEAcgAsACAAZgBuAEYAbwByAG0AYQB0AFkAZQBhAHIAKABJAE4ARABFAFgAKABfAHIARABhAHQAZQAsACAAMQAsACAAMQApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBNAG8AbgB0AGgALAAgAFQARQBYAFQAKABJAE4ARABFAFgAKABfAHIARABhAHQAZQAsACAAMQAsACAAMgApACwAIABcACIAMAAwAFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMARABhAHkALAAgAFQARQBYAFQAKABJAE4ARABFAFgAKABfAHIARABhAHQAZQAsACAAMQAsACAAMwApACwAIABcACIAMAAwAFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAVABpAG0AZQAsACAAZgBuAEYAbwByAG0AYQB0AFQAaQBtAGUAKABJAE4ARABFAFgAKABfAHIARABhAHQAZQAsACAAMQAsACAANAApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBUAFoALAAgAGYAbgBGAG8AcgBtAGEAdABUAFoAKABUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAQwBPAE4AQwBBAFQAKABfAHMAWQBlAGEAcgAsACAAXAAiAC0AXAAiACwAIABfAHMATQBvAG4AdABoACwAIABcACIALQBcACIALAAgAF8AcwBEAGEAeQAsACAAXwBzAFQAaQBtAGUALAAgAF8AcwBUAFoAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ARgBPAFIATQBBAFQAXwBMAEkAVABFAFIAQQBSAFkAXwBZAEUAQQBSAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAGEAIAB5AGUAYQByACAAZgBvAHIAbQBhAHQAdABlAGQAIABpAG4AIABsAGkAdABlAHIAYQByAHkAIABzAHQAeQBsAGUALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAdABlAHgAdAAgAHwAIABMAGkAdABlAHIAYQByAHkAIAB5AGUAYQByAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AWQBlAGEAcgBDAEUAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIABOAG8AdABlACAAdABoAGEAdAAgADEAIABCAEMAIAA9ACAAMAAgAEMARQAsACAAMgAgAEIAQwAgAD0AIAAtADEAIABDAEUAXABuAFsAQQBsAHcAYQB5AHMAUwBoAG8AdwBFAHIAYQBdACAAfAAgAHMAdwBpAHQAYwBoACAAIAB8ACAAQQBsAHcAYQB5AHMAIABhAHAAcABsAHkAIABCAEMARQAvAEMARQAgAHMAdQBmAGYAaQB4AC4AIABJAGYAIABuAG8AdAAgAHUAcwBlAGQALAAgAG8AbgBsAHkAIAB5AGUAYQByAHMAIABsAGUAcwBzACAAdABoAGEAbgAgADEAMAAwADAAIABzAGgAbwB3ACAAYQBuACAAZQByAGEALgBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ARgBPAFIATQBBAFQAXwBMAEkAVABFAFIAQQBSAFkAXwBZAEUAQQBSACAAPQAgAEwAQQBNAEIARABBACgAWQBlAGEAcgBDAEUALAAgAFsAQQBsAHcAYQB5AHMAUwBoAG8AdwBFAHIAYQBdACwAXABuACAAIAAgACAASQBGACgAWQBlAGEAcgBDAEUAIAA9ACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AGUAYQByAEMARQAsACAASQBOAFQAKABZAGUAYQByAEMARQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AaQBzAEMARQAsACAAXwB5AGUAYQByAEMARQAgAD4APQAgADEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AGUAYQByACwAIABJAEYAKABfAGkAcwBDAEUALAAgAF8AeQBlAGEAcgBDAEUALAAgADEAIAAtACAAXwB5AGUAYQByAEMARQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwB1AGYAZgBpAHgALAAgAEkARgBTACgATgBPAFQAKABfAGkAcwBDAEUAKQAsACAAXAAiACAAQgBDAEUAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AGUAYQByAEMARQAgADwAIAAxADAAMAAwACwAIABcACIAIABDAEUAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATgAoAEEAbAB3AGEAeQBzAFMAaABvAHcARQByAGEAKQAgADwAPgAgADAALAAgAFwAIgAgAEMARQBcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAIABcACIAXAAiAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AeQBlAGEAcgAgACYAIABfAHMAdQBmAGYAaQB4AFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBGAE8AUgBNAEEAVABfAEwASQBUAEUAUgBBAFIAWQBfAEQAQQBUAEUAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAYQAgAGQAYQB0AGUAIABmAG8AcgBtAGEAdAB0AGUAZAAgAGkAbgAgAGwAaQB0AGUAcgBhAHIAeQAgAHMAdAB5AGwAZQAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIAB0AGUAeAB0ACAAfAAgAEwAaQB0AGUAcgBhAHIAeQAgAGQAYQB0AGUAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBZAGUAYQByAEMARQAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAAgACAAIAAgACAAIAAgACAAfAAgAE4AbwB0AGUAIAB0AGgAYQB0ACAAMQAgAEIAQwAgAD0AIAAwACAAQwBFACwAIAAyACAAQgBDACAAPQAgAC0AMQAgAEMARQBcAG4ATQBvAG4AdABoACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAWwAxAC4ALgAxADIAXQAgAHwAXABuAEQAYQB5ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMQAuAC4AMwAxAF0AIAB8AFwAbgBbAFQAaQBtAGUAXQAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIABbADAALgAuADEAKQAgACAAfAAgAFQAaQBtAGUAIABvAGYAIABkAGEAeQAgAGEAcwAgAGQAZQBjAGkAbQBhAGwAIABmAHIAYQBjAHQAaQBvAG4AIABvAGYAIABhACAAZABhAHkALgBcAG4AWwBTAGgAbwByAHQAXQAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABzAHcAaQB0AGMAaAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABSAGUAdAB1AHIAbgAgAHMAaABvAHIAdAAgAGYAbwByAG0AYQB0ACAASgBhAG4ALgAuAEQAZQBjAFwAbgBbAEkAbgB0AGUAcgBuAGEAdABpAG8AbgBhAGwARQBuAGcAbABpAHMAaABdACAAfAAgAHMAdwBpAHQAYwBoACAAIAAgACAAIAAgACAAIAAgACAAfAAgAFUAcwBlACAAdABoAGUAIABJAG4AdABlAHIAbgBhAHQAaQBvAG4AYQBsACAARQBuAGcAbABpAHMAaAAgAGkAbgBzAHQAZQBhAGQAIABvAGYAIABsAG8AYwBhAGwAIABsAGEAbgBnAHUAYQBnAGUAIABzAGUAdAAgAGkAbgAgAEUAeABjAGUAbABcAG4AWwBBAGwAdwBhAHkAcwBTAGgAbwB3AEUAcgBhAF0AIAAgACAAIAAgACAAIAAgAHwAIABzAHcAaQB0AGMAaAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABBAGwAdwBhAHkAcwAgAGEAcABwAGwAeQAgAEIAQwBFAC8AQwBFACAAcwB1AGYAZgBpAHgALgAgAEkAZgAgAG4AbwB0ACAAdQBzAGUAZAAsACAAbwBuAGwAeQAgAHkAZQBhAHIAcwAgAGwAZQBzAHMAIAB0AGgAYQBuACAAMQAwADAAMABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABzAGgAbwB3ACAAYQBuACAAZQByAGEALgBcAG4AWwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAgACAAIAAgACAAIAAgAHwAIABzAHcAaQB0AGMAaAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABDAGEAbABjAHUAbABhAHQAZQAgAGYAbwByACAAdABoAGUAIABKAHUAbABpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AIABEAGUAZgBhAHUAbAB0ACAAaQBzACAARwByAGUAZwBvAHIAaQBhAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ARgBPAFIATQBBAFQAXwBMAEkAVABFAFIAQQBSAFkAXwBEAEEAVABFACAAPQAgAEwAQQBNAEIARABBACgAWQBlAGEAcgBDAEUALAAgAE0AbwBuAHQAaAAsACAARABhAHkALAAgAFsAVABpAG0AZQBdACwAIABbAFMAaABvAHIAdABdACwAIABbAEkAbgB0AGUAcgBuAGEAdABpAG8AbgBhAGwARQBuAGcAbABpAHMAaABdACwAIABbAEEAbAB3AGEAeQBzAFMAaABvAHcARQByAGEAXQAsACAAWwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAsAFwAbgAgACAAIAAgAEkARgAoACgAWQBlAGEAcgBDAEUAIAA9ACAAXAAiAFwAIgApACAAKgAgACgATQBvAG4AdABoACAAPQAgAFwAIgBcACIAKQAgACoAIAAoAEQAYQB5ACAAPQAgAFwAIgBcACIAKQAsACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABNAG8AbgB0AGgAKQApACAAKwAgACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABZAGUAYQByAEMARQApACkAIAAqACAATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABEAGEAeQApACkAKQAsACAAIwBWAEEATABVAEUAIQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AeQBlAGEAcgBDAEUALAAgAEkARgAoAFkAZQBhAHIAQwBFACAAPQAgAFwAIgBcACIALAAgADIAMAAwADAALAAgAFkAZQBhAHIAQwBFACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAYQB5ACwAIABJAEYAKABEAGEAeQAgAD0AIABcACIAXAAiACwAIAAxACwAIABEAGEAeQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgATgBPAFQAKABJAFMAXwBWAEEATABJAEQAXwBEAEEAVABFACgAXwB5AGUAYQByAEMARQAsACAATQBvAG4AdABoACwAIABfAGQAYQB5ACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQApACwAIAAjAFYAQQBMAFUARQAhACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHIARABhAHQAZQAsACAASQBGACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABUAGkAbQBlACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXwB5AGUAYQByAEMARQAsACAATQBvAG4AdABoACwAIABfAGQAYQB5ACwAIABcACIAXAAiACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABSAEUAUwBPAEwAVgBFAF8ARABBAFQARQAoAF8AeQBlAGEAcgBDAEUALAAgAE0AbwBuAHQAaAAsACAAXwBkAGEAeQAsACAAVABpAG0AZQAsACAAMwAsACAASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAE0AbwBuAHQAaAAsACAATQBPAE4AVABIAF8ATgBBAE0ARQAoAEkATgBEAEUAWAAoAF8AcgBEAGEAdABlACwAIAAxACwAIAAyACkALAAgAFMAaABvAHIAdAAsACAASQBuAHQAZQByAG4AYQB0AGkAbwBuAGEAbABFAG4AZwBsAGkAcwBoACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAEQAYQB5ACwAIABJAEYAKABJAFMATgBVAE0AQgBFAFIAKABEAGEAeQApACwAIABcACIAIABcACIAIAAmACAASQBOAEQARQBYACgAXwByAEQAYQB0AGUALAAgADEALAAgADMAKQAsACAAXAAiAFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBZAGUAYQByACwAIABJAEYAKABJAFMATgBVAE0AQgBFAFIAKABZAGUAYQByAEMARQApACwAIABcACIALAAgAFwAIgAgACYAIABGAE8AUgBNAEEAVABfAEwASQBUAEUAUgBBAFIAWQBfAFkARQBBAFIAKABJAE4ARABFAFgAKABfAHIARABhAHQAZQAsACAAMQAsACAAMQApACwAIABBAGwAdwBhAHkAcwBTAGgAbwB3AEUAcgBhACkALAAgAFwAIgBcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAVABpAG0AZQAsACAASQBGACgASQBTAE4AVQBNAEIARQBSACgAVABpAG0AZQApACwAIABcACIALAAgAFwAIgAgACYAIABUAEUAWABUACgASQBOAEQARQBYACgAXwByAEQAYQB0AGUALAAgADEALAAgADQAKQAsACAAXAAiAGgAOgBtAG0AIABBAE0ALwBQAE0AXAAiACkALAAgAFwAIgBcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABDAE8ATgBDAEEAVAAoAF8AcwBNAG8AbgB0AGgALAAgAF8AcwBEAGEAeQAsACAAXwBzAFkAZQBhAHIALAAgAF8AcwBUAGkAbQBlACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEYATwBSAE0AQQBUAF8AVQBTAF8ARABBAFQARQBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIABhACAAZABhAHQAZQAgAGYAbwByAG0AYQB0AHQAZQBkACAAaQBuACAAdABoAGUAIABVAFMAIABzAHQAeQBsAGUALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAdABlAHgAdAAgAHwAIABVAFMAIABzAHQAeQBsAGUAIABkAGEAdABlAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AWQBlAGEAcgBDAEUAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAIAAgACAAIAAgACAAIAAgAHwAIABOAG8AdABlACAAdABoAGEAdAAgADEAIABCAEMAIAA9ACAAMAAgAEMARQAsACAAMgAgAEIAQwAgAD0AIAAtADEAIABDAEUAXABuAE0AbwBuAHQAaAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMQAuAC4AMQAyAF0AIAB8AFwAbgBEAGEAeQAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADEALgAuADMAMQBdACAAfABcAG4AWwBUAGkAbQBlAF0AIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAWwAwAC4ALgAxACkAIAAgAHwAIABUAGkAbQBlACAAbwBmACAAZABhAHkAIABhAHMAIABkAGUAYwBpAG0AYQBsACAAZgByAGEAYwB0AGkAbwBuACAAbwBmACAAYQAgAGQAYQB5AC4AXABuAFsAUwBlAHAAYQByAGEAdABvAHIAXQAgACAAIAAgACAAIAB8ACAAYwBoAGEAcgAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAQwBoAGEAcgBhAGMAdABlAHIAIABzAGUAcABhAHIAYQB0AG8AcgAgAGYAbwByACAAZABhAHQAZQAgAGUAbABlAG0AZQBuAHQAcwAuACAAWwAsAC4ALwAtAF8AXQBcAG4AWwBQAHIAZQBjAGkAcwBpAG8AbgBdACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAIAAgACAAIAAgACAAIAAgAHwAIABTAGUAbABlAGMAdAAgAHAAcgBlAGMAaQBzAGkAbwBuACAAbABlAHYAZQBsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAwACAALQAgAEYAbABvAGEAdABpAG4AZwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAMQAgAC0AIABEAGEAeQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAMgAgAC0AIABIAG8AdQByAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAzACAALQAgAE0AaQBuAHUAdABlAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAA0ACAALQAgAFMAZQBjAG8AbgBkAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAA1ACAALQAgAE0AaQBsAGwAaQBzAGUAYwBvAG4AZABcAG4AWwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAgAHwAIABzAHcAaQB0AGMAaAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABDAGEAbABjAHUAbABhAHQAZQAgAGYAbwByACAAdABoAGUAIABKAHUAbABpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AIABEAGUAZgBhAHUAbAB0ACAAaQBzACAARwByAGUAZwBvAHIAaQBhAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgAgAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBGAE8AUgBNAEEAVABfAFUAUwBfAEQAQQBUAEUAIAA9ACAATABBAE0AQgBEAEEAKABZAGUAYQByAEMARQAsACAATQBvAG4AdABoACwAIABEAGEAeQAsACAAWwBUAGkAbQBlAF0ALAAgAFsAUwBlAHAAYQByAGEAdABvAHIAXQAsACAAWwBQAHIAZQBjAGkAcwBpAG8AbgBdACwAIABbAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACwAXABuACAAIAAgACAASQBGACgAKABZAGUAYQByAEMARQAgAD0AIABcACIAXAAiACkAIAAqACAAKABNAG8AbgB0AGgAIAA9ACAAXAAiAFwAIgApACAAKgAgACgARABhAHkAIAA9ACAAXAAiAFwAIgApACwAIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAFkAZQBhAHIAQwBFACkAKQAgACsAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAE0AbwBuAHQAaAApACkAIAArACAATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABEAGEAeQApACkALAAgACMAVgBBAEwAVQBFACEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgATgBPAFQAKABJAFMAXwBWAEEATABJAEQAXwBEAEEAVABFACgAWQBlAGEAcgBDAEUALAAgAE0AbwBuAHQAaAAsACAARABhAHkALAAgAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgApACkALAAgACMAVgBBAEwAVQBFACEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAZgBuAEYAbwByAG0AYQB0AFQAaQBtAGUALAAgAEwAQQBNAEIARABBACgAXwB0AGkAbQBlACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgAXwB0AGkAbQBlACkAKQAsACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIAByAG8AdQBuAGQAIAB0AG8AIABtAGkAbABsAGkAcwBlAG8AbgBkAHMALAAgAHMAYwBhAGwAZQAgAHQAbwAgAHMAZQBjAG8AbgBkAHMAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAZQBjAG8AbgBkAHMALAAgAFIATwBVAE4ARAAoAF8AdABpAG0AZQAgACoAIAA4ADYANAAwADAALAAgADMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGgAbwB3AFAAcgBlAGMAaQBzAGkAbwBuACwAIABJAEYAKABOACgAUAByAGUAYwBpAHMAaQBvAG4AKQAgAD4AIAAwACwAIABQAHIAZQBjAGkAcwBpAG8AbgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAUwAoAF8AcwBlAGMAbwBuAGQAcwAgAD0AIAAwACwAIAAzACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATQBPAEQAKABfAHMAZQBjAG8AbgBkAHMALAAgADEAKQAgAD4AIAAwACwAIAA1ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATQBPAEQAKABfAHMAZQBjAG8AbgBkAHMAIAAvACAANgAwACwAIAAxACkAIAA+ACAAMAAsACAANAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALAAgADMAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAHMAaABvAHcAUAByAGUAYwBpAHMAaQBvAG4AIAA9ACAAMQAsACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZgBtAHQALAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaABvAHcAUAByAGUAYwBpAHMAaQBvAG4AIAA9ACAAMgAsACAAXAAiAGgAIABBAE0ALwBQAE0AXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaABvAHcAUAByAGUAYwBpAHMAaQBvAG4AIAA9ACAAMwAsACAAXAAiAGgAOgBtAG0AIABBAE0ALwBQAE0AXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaABvAHcAUAByAGUAYwBpAHMAaQBvAG4AIAA9ACAANAAsACAAXAAiAGgAOgBtAG0AOgBzAHMAIABBAE0ALwBQAE0AXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAIABcACIAaAA6AG0AbQA6AHMAcwAuADAAMAAwACAAQQBNAC8AUABNAFwAIgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiACAAXAAiACAAJgAgAFQARQBYAFQAKABfAHQAaQBtAGUALAAgAF8AZgBtAHQAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAZQBwAGEAcgBhAHQAbwByACwAIABJAEYAKABTAGUAcABhAHIAYQB0AG8AcgAgAD0AIABcACIAXAAiACwAIABcACIALwBcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGMAaABhAHIAMQAsACAATABFAEYAVAAoAFMAZQBwAGEAcgBhAHQAbwByACwAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABJAEYARQBSAFIATwBSACgARgBJAE4ARAAoAF8AYwBoAGEAcgAxACwAIABcACIALAAuAC8ALQBfAFwAIgApACwAIAAwACkAIAA+ACAAMAAsACAAXwBjAGgAYQByADEALAAgAFwAIgAvAFwAIgApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB1AHMAZQBQAHIAZQBjAGkAcwBpAG8AbgAsACAASQBGACgATgAoAFAAcgBlAGMAaQBzAGkAbwBuACkAIAA+AD0AIAA1ACwAIAA1ACwAIAA0ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcgBEAGEAdABlACwAIABJAEYAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAFQAaQBtAGUAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAWQBlAGEAcgBDAEUALAAgAE0AbwBuAHQAaAAsACAARABhAHkALAAgAFwAIgBcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABSAEUAUwBPAEwAVgBFAF8ARABBAFQARQAoAFkAZQBhAHIAQwBFACwAIABNAG8AbgB0AGgALAAgAEQAYQB5ACwAIABUAGkAbQBlACwAIABfAHUAcwBlAFAAcgBlAGMAaQBzAGkAbwBuACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBZAGUAYQByACwAIABUAEUAWABUACgASQBOAEQARQBYACgAXwByAEQAYQB0AGUALAAgADEALAAgADEAKQAsACAAXAAiADAAMAAwADAAOwBcACIAIAAmACAAVQBOAEkAQwBIAEEAUgAoADgANwAyADIAKQAgACYAIABcACIAMAAwADAAMAA7ADAAMAAwADAAXAAiACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBNAG8AbgB0AGgALAAgAEkATgBEAEUAWAAoAF8AcgBEAGEAdABlACwAIAAxACwAIAAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBEAGEAeQAsACAAVABFAFgAVAAoAEkATgBEAEUAWAAoAF8AcgBEAGEAdABlACwAIAAxACwAIAAzACkALAAgAFwAIgAwADAAXAAiACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBUAGkAbQBlACwAIABmAG4ARgBvAHIAbQBhAHQAVABpAG0AZQAoAEkATgBEAEUAWAAoAF8AcgBEAGEAdABlACwAIAAxACwAIAA0ACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAQwBPAE4AQwBBAFQAKABfAHMATQBvAG4AdABoACwAIABfAHMAZQBwAGEAcgBhAHQAbwByACwAIABfAHMARABhAHkALAAgAF8AcwBlAHAAYQByAGEAdABvAHIALAAgAF8AcwBZAGUAYQByACwAIABfAHMAVABpAG0AZQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEYATwBSAE0AQQBUAF8ATQBJAEwAXwBEAFQARwBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIABhACAAZABhAHQAZQAgAGYAbwByAG0AYQB0AHQAZQBkACAAaQBuACAAVQBTACAATQBpAGwAaQB0AGEAcgB5ACAAbQBlAHMAcwBhAGcAZQAgAHQAcgBhAGYAZgBpAGMAIABzAHQAeQBsAGUALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAdABlAHgAdAAgAHwAIABEAFQARwAgAGYAbwByAG0AYQB0AHQAZQBkACAAZABhAHQAZQBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFkAZQBhAHIAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMQA5ADUAMQAuAC4AMgAwADUAMABdACAAfABcAG4ATQBvAG4AdABoACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAWwAxAC4ALgAxADIAXQAgACAAIAAgACAAIAB8AFwAbgBEAGEAeQAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADEALgAuADMAMQBdACAAIAAgACAAIAAgAHwAXABuAFQAaQBtAGUAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgAFsAMAAuAC4AMQApACAAIAAgACAAIAAgACAAfAAgAFQAaQBtAGUAIABvAGYAIABkAGEAeQAgAGEAcwAgAGQAZQBjAGkAbQBhAGwAIABmAHIAYQBjAHQAaQBvAG4AIABvAGYAIABhACAAZABhAHkALgBcAG4AWwBUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQAXQAgAHwAIABkAGUAYwBpAG0AYQBsACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAVABpAG0AZQAgAHoAbwBuAGUAIABvAGYAZgBzAGUAdAAgAGkAbgAgAG0AaQBuAHUAdABlAHMAIABmAHIAbwBtACAAVQBUAEMALgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABbAC0AOQAwADAALgAuADkAMAAwAF0AIAAgACAAIAAgACAAIAAgACAAIAB8ACAAQQBzAHMAdQBtAGUAZAAgAHQAbwAgAGIAZQAgAFUAVABDACAAaQBmACAAbwBtAG0AaQB0AHQAZQBkAC4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAFQAaQBtAGUAIAB3AGkAbABsACAAYgBlACAAYwBvAG4AdgBlAHIAdABlAGQAIABpAGYAIAB0AGgAZQAgAG8AZgBmAHMAZQB0ACAAZABvAGUAcwAgAG4AbwB0ACAAYQBsAGkAZwBuACAAdwBpAHQAaAAgAG0AaQBsAGkAdABhAHIAeQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAdABpAG0AZQAgAHoAbwBuAGUAcwAuAFwAbgBbAFMAaABvAHIAdABdACAAIAAgACAAIAAgACAAIAAgACAAfAAgAHMAdwBpAHQAYwBoACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABTAGgAbwByAHQAIAB0AGkAbQBlACAAZgBvAHIAbQB0ADoAIABoAGgAbQBtACwAIABvAHQAaABlAHIAdwBpAHMAZQA6ACAAaABoAG0AbQBzAHMAXABuAFwAbgBFAHgAYQBtAHAAbABlAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEYATwBSAE0AQQBUAF8ATQBJAEwAXwBEAFQARwAoADIAMAAyADMALAAgADIALAAgADEAMgAsACAAMAAuADcANQAsACAANgAwADAALAAgADEAKQBcAG4AUgBlAHQAdQByAG4AcwA6ACAAMQAyADEAOAAwADAASwBGAEUAQgAyADMAXABuAFwAbgBGAE8AUgBNAEEAVABfAE0ASQBMAF8ARABUAEcAKAAgACwAIAAsACAAMQAyACwAIAAwAC4AMgA1ACkAXABuAFIAZQB0AHUAcgBuAHMAOgAgADEAMgAwADYAMAAwAEoAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEYATwBSAE0AQQBUAF8ATQBJAEwAXwBEAFQARwAgAD0AIABMAEEATQBCAEQAQQAoAFkAZQBhAHIALAAgAE0AbwBuAHQAaAAsACAARABhAHkALAAgAFQAaQBtAGUALAAgAFsAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0AF0ALAAgAFsAUwBoAG8AcgB0AF0ALABcAG4AIAAgACAAIABJAEYAKAAoAFkAZQBhAHIAIAA9ACAAXAAiAFwAIgApACAAKgAgACgATQBvAG4AdABoACAAPQAgAFwAIgBcACIAKQAgACoAIAAoAEQAYQB5ACAAPQAgAFwAIgBcACIAKQAgACoAIAAoAFQAaQBtAGUAIAA9ACAAXAAiAFwAIgApACwAIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEQAYQB5ACkAKQAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGwAbwBjAGEAbAAsACAAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0ACAAPQAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBvACwAIABOACgAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAGYAbgBJAG4AdgBhAGwAaQBkAFAAYQByAGEAbQBzACwAIABMAEEATQBCAEQAQQAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAQQBCAFMAKABfAHQAegBvACkAIAA+ACAAOQAwADAALAAgAFQAUgBVAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgASQBTAE4AVQBNAEIARQBSACgAWQBlAGEAcgApACwAIAAoACgAWQBlAGEAcgAgADwAIAAxADkANQAxACkAIAArACAAKABZAGUAYQByACAAPgAgADIAMAA1ADAAKQApACwAIABGAEEATABTAEUAKQAsACAAVABSAFUARQAsACAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgAKAAoAFkAZQBhAHIAIAA9ACAAXAAiAFwAIgApACAAKgAgACgATQBvAG4AdABoACAAPQAgAFwAIgBcACIAKQApACAAKwAgAE4AKABJAFMAXwBWAEEATABJAEQAXwBEAEEAVABFACgAWQBlAGEAcgAsACAATQBvAG4AdABoACwAIABEAGEAeQAsACAAMAApACkAKQAgAD0AIAAwACwAIABUAFIAVQBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALAAgAEYAQQBMAFMARQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABmAG4ARgBtAHQAVABpAG0AZQAsACAATABBAE0AQgBEAEEAKABfAHQAaQBtAGUALAAgAF8AcwBoAG8AcgB0ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAaQBtAGUARgBtAHQALAAgAEkARgAoAF8AcwBoAG8AcgB0ACwAIABcACIASABIAG0AbQBcACIALAAgAFwAIgBIAEgAbQBtAHMAcwBcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAEUAWABUACgAXwB0AGkAbQBlACwAIABfAHQAaQBtAGUARgBtAHQAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABmAG4AUgBlAHMAbwBsAHYAZQBNAGkAbABpAHQAYQByAHkAVABaACwAIABMAEEATQBCAEQAQQAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBsAG8AYwBhAGwALAAgAEgAUwBUAEEAQwBLACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATgAoAFQAaQBtAGUAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBKAFwAIgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBvACAAPgAgADcAMgAwACwAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBoAGkAZgB0AFQAWgBPACwAIABfAHQAegBvACAALQAgADcAMgAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AGkAbQBlACwAIABOACgAVABpAG0AZQApACAALQAgACgAXwBzAGgAaQBmAHQAVABaAE8AIAAvACAAMQA0ADQAMAApACwAIAAgAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAaQBtAGUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBNAFwAIgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdAB6AG8AIAA8ACAALQA3ADIAMAAsACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaABpAGYAdABUAFoATwAsACAAXwB0AHoAbwAgACsAIAA3ADIAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdABpAG0AZQAsACAATgAoAFQAaQBtAGUAKQAgAC0AIAAoAF8AcwBoAGkAZgB0AFQAWgBPACAALwAgADEANAA0ADAAKQAsACAAIABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AGkAbQBlACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAWQBcACIAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbQBpAGwAaQB0AGEAcgB5AFQAWgBPACwAIABTAEkARwBOACgAXwB0AHoAbwApACAAKgAgAE0AUgBPAFUATgBEACgAQQBCAFMAKABfAHQAegBvACkALAAgADYAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGgAaQBmAHQAVABaAE8ALAAgAF8AdAB6AG8AIAAtACAAXwBtAGkAbABpAHQAYQByAHkAVABaAE8ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAaQBtAGUALAAgAE4AKABUAGkAbQBlACkAIAAtACAAKABfAHMAaABpAGYAdABUAFoATwAgAC8AIAAxADQANAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGkAZAB4ACwAIABJAE4AVAAoAF8AbQBpAGwAaQB0AGEAcgB5AFQAWgBPACAALwAgADYAMAApACAAKwAgADEAMwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbQBpAGwAaQB0AGEAcgB5AFQAWgAsACAAQwBIAE8ATwBTAEUAKABfAGkAZAB4ACwAIABcACIAWQBcACIALAAgAFwAIgBYAFwAIgAsACAAXAAiAFcAXAAiACwAIABcACIAVgBcACIALAAgAFwAIgBVAFwAIgAsACAAXAAiAFQAXAAiACwAIABcACIAUwBcACIALAAgAFwAIgBSAFwAIgAsACAAXAAiAFEAXAAiACwAIABcACIAUABcACIALAAgAFwAIgBPAFwAIgAsACAAXAAiAE4AXAAiACwAIABcACIAWgBcACIALAAgAFwAIgBBAFwAIgAsACAAXAAiAEIAXAAiACwAIABcACIAQwBcACIALAAgAFwAIgBEAFwAIgAsACAAXAAiAEUAXAAiACwAIABcACIARgBcACIALAAgAFwAIgBHAFwAIgAsACAAXAAiAEgAXAAiACwAIABcACIASQBcACIALAAgAFwAIgBLAFwAIgAsACAAXAAiAEwAXAAiACwAIABcACIATQBcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAaQBtAGUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbQBpAGwAaQB0AGEAcgB5AFQAWgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAGYAbgBJAG4AdgBhAGwAaQBkAFAAYQByAGEAbQBzACgAKQAsACAAewBcACIAIwBOAFUATQAhACEAXAAiAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbQBpAGwAaQB0AGEAcgB5AFQAaQBtAGUALAAgAGYAbgBSAGUAcwBvAGwAdgBlAE0AaQBsAGkAdABhAHIAeQBUAFoAKAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcgBEAGEAdABlACwAIABJAEYAKABZAGUAYQByACAAPQAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABSAEUAUwBPAEwAVgBFAF8ARABBAFQARQAoADIAMAAwADAALAAgADMALAAgAEQAYQB5ACwAIABJAE4ARABFAFgAKABfAG0AaQBsAGkAdABhAHIAeQBUAGkAbQBlACwAIAAxACwAIAAxACkALAAgADMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFIARQBTAE8ATABWAEUAXwBEAEEAVABFACgAWQBlAGEAcgAsACAATQBvAG4AdABoACwAIABEAGEAeQAsACAASQBOAEQARQBYACgAXwBtAGkAbABpAHQAYQByAHkAVABpAG0AZQAsACAAMQAsACAAMQApACwAIAAzACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAEQAYQB5ACwAIABUAEUAWABUACgASQBOAEQARQBYACgAXwByAEQAYQB0AGUALAAgADMAKQAsACAAXAAiADAAMABcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABZAGUAYQByACAAPQAgAFwAIgBcACIALAAgAEMATwBOAEMAQQBUACgAXwBzAEQAYQB5ACwAIABmAG4ARgBtAHQAVABpAG0AZQAoAEkATgBEAEUAWAAoAF8AcgBEAGEAdABlACwAIAA0ACkALAAgADEAKQAsACAASQBOAEQARQBYACgAXwBtAGkAbABpAHQAYQByAHkAVABpAG0AZQAsACAAMQAsACAAMgApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAFQAaQBtAGUALAAgAGYAbgBGAG0AdABUAGkAbQBlACgASQBOAEQARQBYACgAXwByAEQAYQB0AGUALAAgADQAKQAsACAATgAoAFMAaABvAHIAdAApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBNAG8AbgB0AGgALAAgAFUAUABQAEUAUgAoAE0ATwBOAFQASABfAE4AQQBNAEUAKABJAE4ARABFAFgAKABfAHIARABhAHQAZQAsACAAMgApACwAIAAxACwAIAAxACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAFkAWQAsACAAUgBJAEcASABUACgAVABFAFgAVAAoAEkATgBEAEUAWAAoAF8AcgBEAGEAdABlACwAIAAxACkALAAgAFwAIgAwADAAXAAiACkALAAgADIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAQwBPAE4AQwBBAFQAKABfAHMARABhAHkALAAgAF8AcwBUAGkAbQBlACwAIABJAE4ARABFAFgAKABfAG0AaQBsAGkAdABhAHIAeQBUAGkAbQBlACwAIAAxACwAIAAyACkALAAgAF8AcwBNAG8AbgB0AGgALAAgAF8AcwBZAFkAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4AXABuAFwAbgBcAG4AXABuAFwAbgBcAG4ALwAqACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwBcAG4AIwAgAEMATwBOAFYARQBSAFMASQBPAE4AUwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACoALwBcAG4AXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ASQBTAE8ARABBAFQARQBfAFQATwBfAEoARABOAF8ATABPAEMAQQBMAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAHQAaABlACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByACAAYQBuAGQAIABsAG8AYwBhAGwAIAB0AGkAbQBlACAAZgBvAHIAIABhACAAZABhAHQAZQAgAGEAbgBkACAAdABpAG0AZQAgAHAAcgBvAHYAaQBkAGUAZAAgAGkAbgAgAEkAUwBPACAAZgBvAHIAbQBhAHQALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAaQBuAHQAZQBnAGUAcgAgACAAIAAgACAAIAAgACAAfAAgAEwAbwBjAGEAbAAgAEoAdQBsAGkAYQBuACAARABhAHkAIABOAHUAbQBiAGUAcgBcAG4AIAAyACAAfAAgAGQAZQBjAGkAbQBhAGwAIABbADAALgAuADEAKQAgAHwAIABMAG8AYwBhAGwAIAB0AGkAbQBlACAAbwBmACAAZABhAHkALgAgAEQAZQBjAGkAbQBhAGwAIABmAHIAYQBjAHQAaQBvAG4AIABvAGYAIABhACAAZABhAHkALAAgAGkAbQBwAGwAaQBjAGkAdABsAHkAIABjAG8AbgB2AGUAcgB0AHMAIAB0AG8AIABFAHgAYwBlAGwAIAB0AGkAbQBlACAAZABhAHQAYQAgAHQAeQBwAGUALgBcAG4AIAAzACAAfAAgAGQAZQBjAGkAbQBhAGwAIAAgACAAIAAgACAAIAAgAHwAIABUAGkAbQBlACAAegBvAG4AZQAgAG8AZgBmAHMAZQB0ACAAbQBpAG4AdQB0AGUAcwAgAGYAcgBvAG0AIABVAFQAQwBcAG4AIAAgACAAfAAgAFsALQA5ADAAMAAuAC4AOQAwADAAXQAgACAAIAAgAHwAIABcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEkAUwBPAEQAYQB0AGUAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAB0AGUAeAB0ACAAIAAgAHwAIABJAFMATwAgAGYAbwByAG0AYQB0AHQAZQBkACAAZABhAHQAZQAsACAAdABpAG0AZQAgAGEAbgBkACAAdABpAG0AZQAgAHoAbwBuAGUAIABvAGYAZgBzAGUAdAAuAFwAbgBbAEYAcgBvAG0ASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0AIAB8ACAAcwB3AGkAdABjAGgAIAB8ACAAQwBhAGwAYwB1AGwAYQB0AGUAIABmAHIAbwBtACAAdABoAGUAIABKAHUAbABpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AIABEAGUAZgBhAHUAbAB0ACAAaQBzACAARwByAGUAZwBvAHIAaQBhAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgAHwAIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuACAAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEkAUwBPAEQAQQBUAEUAXwBUAE8AXwBKAEQATgBfAEwATwBDAEEATAAgAD0AIABMAEEATQBCAEQAQQAoAEkAUwBPAEQAYQB0AGUALAAgAFsARgByAG8AbQBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAsAFwAbgAgACAAIAAgAEkARgAoAEkAUwBPAEQAYQB0AGUAIAA9ACAAXAAiAFwAIgAsACAAewBcACIAXAAiACwAIABcACIAXAAiACwAIABcACIAXAAiAH0ALABcAG4AIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AaQBzAG8ARABhAHQAZQAsACAAUABBAFIAUwBFAF8ASQBTAE8AXwBEAEEAVABFACgASQBTAE8ARABhAHQAZQAsACAARgByAG8AbQBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGoAZABuACwAIABJAEYAKABJAFMARQBSAFIATwBSACgASQBOAEQARQBYACgAXwBpAHMAbwBEAGEAdABlACwAIAAxACwAIAAxACkAKQAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABKAFUATABJAEEATgBfAEQAQQBZAF8ATgBVAE0AQgBFAFIAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkATgBEAEUAWAAoAF8AaQBzAG8ARABhAHQAZQAsACAAMQAsACAAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAE4ARABFAFgAKABfAGkAcwBvAEQAYQB0AGUALAAgADEALAAgADIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBOAEQARQBYACgAXwBpAHMAbwBEAGEAdABlACwAIAAxACwAIAAzACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEYAcgBvAG0ASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AGkAbQBlACwAIABJAEYAKABJAE4ARABFAFgAKABfAGkAcwBvAEQAYQB0AGUALAAgADEALAAgADQAKQAgAD0AIABcACIAXAAiACwAIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGAEUAUgBSAE8AUgAoAE0ATwBEACgASQBOAEQARQBYACgAXwBpAHMAbwBEAGEAdABlACwAIAAxACwAIAA0ACkALAAgADEAKQAsACAAewAjAFYAQQBMAFUARQAhAH0AKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGMAYQByAHIAeQBEAGEAeQAsACAASQBGACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABJAE4ARABFAFgAKABfAGkAcwBvAEQAYQB0AGUALAAgADEALAAgADQAKQApACkALAAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAE4AVAAoAEkATgBEAEUAWAAoAF8AaQBzAG8ARABhAHQAZQAsACAAMQAsACAANAApACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwByAEoARABOACwAIABJAEYARQBSAFIATwBSACgAXwBKAEQATgAgACsAIABfAGMAYQByAHIAeQBEAGEAeQAsACAAewAjAFYAQQBMAFUARQAhAH0AKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegAsACAASQBGAEUAUgBSAE8AUgAoAEkATgBEAEUAWAAoAF8AaQBzAG8ARABhAHQAZQAsACAAMQAsACAANQApACwAIAB7ACMAVgBBAEwAVQBFACEAfQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXwByAEoARABOACwAIABfAHQAaQBtAGUALAAgAF8AdAB6ACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBJAFMATwBEAEEAVABFAF8AVABPAF8ASgBEAEEAVABFAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAHQAaABlACAASgB1AGwAaQBhAG4AIABEAGEAdABlACAAZgBvAHIAIABhACAAZABhAHQAZQAgAGEAbgBkACAAdABpAG0AZQAgAHAAcgBvAHYAaQBkAGUAZAAgAGkAbgAgAEkAUwBPACAAZgBvAHIAbQBhAHQALgBcAG4ATgBvAHQAZQAgAGEAIABKAHUAbABpAGEAbgAgAEQAYQB0AGUAIABpAHMAIABhAGwAdwBhAHkAcwAgAGkAbgAgAFUAVABDAC4AXABuAFwAbgBPAHUAdABwAHUAdABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAASgB1AGwAaQBhAG4AIABEAGEAdABlAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ASQBTAE8ARABhAHQAZQAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAHQAZQB4AHQAIAAgACAAfAAgAEkAUwBPACAAZgBvAHIAbQBhAHQAdABlAGQAIABkAGEAdABlACwAIAB0AGkAbQBlACAAYQBuAGQAIAB0AGkAbQBlACAAegBvAG4AZQAgAG8AZgBmAHMAZQB0AC4AIABJAGYAIAB0AGkAbQBlACAAaQBzACAAbwBtAG0AaQB0AHQAZQBkACwAIABhAHMAcwB1AG0AZQBkAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAB8ACAAdABvACAAYgBlACAAYQB0ACAAMAAwADoAMAAwAC4AIABJAGYAIAB0AGkAbQBlACAAegBvAG4AZQAgAGkAcwAgAG8AbQBtAGkAdAB0AGUAZAAsACAAYQBzAHMAdQBtAGUAZAAgAHQAbwAgAGIAZQAgAFUAVABDAC4AXABuAFsARgByAG8AbQBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAgAHwAIABzAHcAaQB0AGMAaAAgAHwAIABDAGEAbABjAHUAbABhAHQAZQAgAGYAcgBvAG0AIAB0AGgAZQAgAEoAdQBsAGkAYQBuACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgAgAEQAZQBmAGEAdQBsAHQAIABpAHMAIABHAHIAZQBnAG8AcgBpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAB8ACAAYwBhAGwAZQBuAGQAYQByAC4AIABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ASQBTAE8ARABBAFQARQBfAFQATwBfAEoARABBAFQARQAgAD0AIABMAEEATQBCAEQAQQAoAEkAUwBPAEQAYQB0AGUALAAgAFsARgByAG8AbQBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAsAFwAbgAgACAAIAAgAEkARgAoAEkAUwBPAEQAYQB0AGUAIAA9ACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBqAGQAbgBMAG8AYwBhAGwALAAgAEkAUwBPAEQAQQBUAEUAXwBUAE8AXwBKAEQATgBfAEwATwBDAEEATAAoAEkAUwBPAEQAYQB0AGUALAAgAEYAcgBvAG0ASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAASgBEAE4AXwBMAE8AQwBBAEwAXwBUAE8AXwBKAEQAQQBUAEUAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAE4ARABFAFgAKABfAGoAZABuAEwAbwBjAGEAbAAsACwAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABOACgASQBOAEQARQBYACgAXwBqAGQAbgBMAG8AYwBhAGwALAAsACAAMgApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABOACgASQBOAEQARQBYACgAXwBqAGQAbgBMAG8AYwBhAGwALAAsACAAMwApACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBJAFMATwBEAEEAVABFAF8AVABPAF8ARQBEAEEAVABFAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAGEAbgAgAEUAeABjAGUAbAAgAEQAYQB0AGUALwBUAGkAbQBlACAAZgBvAHIAIABhACAAZABhAHQAZQAgAGEAbgBkACAAdABpAG0AZQAgAHAAcgBvAHYAaQBkAGUAZAAgAGkAbgAgAEkAUwBPACAAZgBvAHIAbQBhAHQALgBcAG4ATgBvAHQAZQAgAEUAeABjAGUAbAAgAEQAYQB0AGUALwBUAGkAbQBlACAAdQBzAGUAcwAgAHQAaABlACAARwByAGUAZwBvAHIAaQBhAG4AIABjAGEAbABlAG4AZABhAHIALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIABFAHgAYwBlAGwAIABEAGEAdABlAC8AVABpAG0AZQAuACAAMQA5ADAAMAAtADAAMQAtADAAMQAuAC4AOQA5ADkAOQAtADEAMgAtADMAMQBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEkAUwBPAEQAYQB0AGUAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAB0AGUAeAB0ACAAIAAgAHwAIABJAFMATwAgAGYAbwByAG0AYQB0AHQAZQBkACAAZABhAHQAZQAsACAAdABpAG0AZQAgAGEAbgBkACAAdABpAG0AZQAgAHoAbwBuAGUAIABvAGYAZgBzAGUAdAAuACAASQBmACAAdABpAG0AZQAgAGkAcwAgAG8AbQBtAGkAdAB0AGUAZAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAB8ACAAYQBzAHMAdQBtAGUAZAAgAHQAbwAgAGIAZQAgAGEAdAAgADAAMAA6ADAAMAAuAFwAbgBbAEkAbgBjAGwAdQBkAGUAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0AF0AIAB8ACAAcwB3AGkAdABjAGgAIAB8ACAAUgBlAHQAdQByAG4AIAB0AGkAbQBlACAAegBvAG4AZQAgAG8AZgBmAHMAZQB0ACAAcABhAHIAcwBlAGQAIABmAHIAbwBtACAAdABoAGUAIABJAFMATwBEAGEAdABlAC4AXABuAFsARgByAG8AbQBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAgACAAIAAgAHwAIABzAHcAaQB0AGMAaAAgAHwAIABDAGEAbABjAHUAbABhAHQAZQAgAGYAcgBvAG0AIAB0AGgAZQAgAEoAdQBsAGkAYQBuACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgAgAEQAZQBmAGEAdQBsAHQAIABpAHMAIABHAHIAZQBnAG8AcgBpAGEAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAfAAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEkAUwBPAEQAQQBUAEUAXwBUAE8AXwBFAEQAQQBUAEUAIAA9ACAATABBAE0AQgBEAEEAKABJAFMATwBEAGEAdABlACwAIABbAEkAbgBjAGwAdQBkAGUAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0AF0ALAAgAFsARgByAG8AbQBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAsAFwAbgAgACAAIAAgAEkARgAoAEkAUwBPAEQAYQB0AGUAIAA9ACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwByAGUAdAB1AHIAbgBUAFoATwAsACAATgAoAEkAbgBjAGwAdQBkAGUAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0ACkAIAA8AD4AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AagB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByACwAIABOACgARgByAG8AbQBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAgADwAPgAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBpAHMAbwBEAGEAdABlACwAIABQAEEAUgBTAEUAXwBJAFMATwBfAEQAQQBUAEUAKABJAFMATwBEAGEAdABlACwAIABfAGoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAEkAUwBFAFIAUgBPAFIAKABJAE4ARABFAFgAKABfAGkAcwBvAEQAYQB0AGUALAAgADEALAAgADEAKQApACwAIABJAEYAKABfAHIAZQB0AHUAcgBuAFQAWgBPACwAIABIAFMAVABBAEMASwAoAHsAIwBWAEEATABVAEUAIQB9ACwAIABUAEEASwBFACgAXwBpAHMAbwBEAGEAdABlACwAIAAxACwAIAAtADEAKQApACwAIAB7ACMAVgBBAEwAVQBFACEAfQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZwBEAGEAdABlACwAIABJAEYAKABfAGoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABKAFUATABJAEEATgBfAFQATwBfAEcAUgBFAEcATwBSAEkAQQBOACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBOAEQARQBYACgAXwBpAHMAbwBEAGEAdABlACwAIAAxACwAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAE4ARABFAFgAKABfAGkAcwBvAEQAYQB0AGUALAAgADEALAAgADIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkATgBEAEUAWAAoAF8AaQBzAG8ARABhAHQAZQAsACAAMQAsACAAMwApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAQQBLAEUAKABfAGkAcwBvAEQAYQB0AGUALAAgADEALAAgADMAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZQBEAGEAdABlACwAIABEAEEAVABFACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkATgBEAEUAWAAoAF8AZwBEAGEAdABlACwAIAAxACwAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBOAEQARQBYACgAXwBnAEQAYQB0AGUALAAgADEALAAgADIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAE4ARABFAFgAKABfAGcARABhAHQAZQAsACAAMQAsACAAMwApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBlAEQAYQB0AGUAVABpAG0AZQAsACAAXwBlAEQAYQB0AGUAIAArACAASQBOAEQARQBYACgAXwBpAHMAbwBEAGEAdABlACwAIAAxACwAIAA0ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAF8AcgBlAHQAdQByAG4AVABaAE8ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGUARABhAHQAZQBUAGkAbQBlACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBOAEQARQBYACgAXwBpAHMAbwBEAGEAdABlACwAIAAxACwAIAA1ACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGUARABhAHQAZQBUAGkAbQBlAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ASgBEAEEAVABFAF8AVABPAF8ASQBTAE8ARABBAFQARQBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIABJAFMATwAgAGYAbwByAG0AYQB0ACAAZABhAHQAZQAsACAAdABpAG0AZQAgAGEAbgBkACAAdABpAG0AZQAgAHoAbwBuAGUAIABvAGYAZgBzAGUAdAAgAGYAcgBvAG0AIABhACAAIABKAHUAbABpAGEAbgAgAEQAYQB0AGUALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAdABlAHgAdAAgAHwAIABJAFMATwAgAGQAYQB0AGUALgBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEoARABhAHQAZQAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAASgB1AGwAaQBhAG4AIABEAGEAdABlAC4AIABOAG8AdABlACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMAIABhAHIAZQAgAGEAbAB3AGEAeQBzACAAaQBuACAAVQBUAEMALgBcAG4AWwBUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQAXQAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIABUAGkAbQBlACAAegBvAG4AZQAgAG8AZgBmAHMAZQB0ACAAaQBuACAAbQBpAG4AdQB0AGUAcwAgAGYAcgBvAG0AIABVAFQAQwAuAFwAbgBbAFAAcgBlAGMAaQBzAGkAbwBuAF0AIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAFMAZQBsAGUAYwB0ACAAcAByAGUAYwBpAHMAaQBvAG4AIABsAGUAdgBlAGwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADAAIAAtACAAQQB1AHQAbwBtAGEAdABpAGMAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADEAIAAtACAASABvAHUAcgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAMgAgAC0AIABNAGkAbgB1AHQAZQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAMwAgAC0AIABTAGUAYwBvAG4AZABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAANAAgAC0AIABNAGkAbABsAGkAcwBlAGMAbwBuAGQAXABuAFsATgBvAFoAdQBsAHUAXQAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAHMAdwBpAHQAYwBoACAAIAB8ACAAVQBzAGUAIAArADAAMAA6ADAAMAAgAGkAbgBzAHQAZQBhAGQAIABvAGYAIABaACAAZgBvAHIAIABVAFQAQwAgAHQAaQBtAGUAIAB6AG8AbgBlAC4AXABuAFsAVABvAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACAAfAAgAHMAdwBpAHQAYwBoACAAIAB8ACAAQwBhAGwAYwB1AGwAYQB0AGUAIABpAG4AIAB0AGgAZQAgAEoAdQBsAGkAYQBuACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgAgAEQAZQBmAGEAdQBsAHQAIABpAHMAIABHAHIAZQBnAG8AcgBpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgAGMAYQBsAGUAbgBkAGEAcgAuACAAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEoARABBAFQARQBfAFQATwBfAEkAUwBPAEQAQQBUAEUAIAA9ACAATABBAE0AQgBEAEEAKABKAEQAYQB0AGUALAAgAFsAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0AF0ALAAgAFsAUAByAGUAYwBpAHMAaQBvAG4AXQAsACAAWwBOAG8AWgB1AGwAdQBdACwAIABbAFQAbwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAsAFwAbgAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIABfAHIARABhAHQAZQAsACAAQwBBAEwARQBOAEQAQQBSAF8ARgBSAE8ATQBfAEoARABBAFQARQAoAEoARABhAHQAZQAsACAAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0ACwAIABQAHIAZQBjAGkAcwBpAG8AbgAsACAAVABvAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgApACwAXABuACAAIAAgACAAIAAgACAAIABGAE8AUgBNAEEAVABfAEkAUwBPAF8ARABBAFQARQAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAE4ARABFAFgAKABfAHIARABhAHQAZQAsACAAMQAsACAAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkATgBEAEUAWAAoAF8AcgBEAGEAdABlACwAIAAxACwAIAAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBOAEQARQBYACgAXwByAEQAYQB0AGUALAAgADEALAAgADMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAE4ARABFAFgAKABfAHIARABhAHQAZQAsACAAMQAsACAANAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABQAHIAZQBjAGkAcwBpAG8AbgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABOAG8AWgB1AGwAdQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAG8ASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ASgBEAE4AXwBMAE8AQwBBAEwAXwBUAE8AXwBJAFMATwBEAEEAVABFAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAEkAUwBPACAAZgBvAHIAbQBhAHQAIABkAGEAdABlACwAIAB0AGkAbQBlACAAYQBuAGQAIAB0AGkAbQBlACAAegBvAG4AZQAgAG8AZgBmAHMAZQB0ACAAZgBvAHIAIAB0AGgAZQAgAHAAcgBvAHYAaQBkAGUAZAAgAEoAdQBsAGkAYQBuACAARABhAHkAIABOAHUAbQBiAGUAcgAgAGEAbgBkACAAbABvAGMAYQBsACAAdABpAG0AZQAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIAB0AGUAeAB0ACAAfAAgAEkAUwBPACAAZABhAHQAZQAuAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ATABvAGMAYQBsAEoARABOACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIABMAG8AYwBhAGwAIABKAHUAbABpAGEAbgAgAEQAYQB5ACAATgB1AG0AYgBlAHIALgBcAG4ATABvAGMAYQBsAFQAaQBtAGUAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIABMAG8AYwBhAGwAIAB0AGkAbQBlACAAbwBmACAAZABhAHkAIABhAHMAIABkAGUAYwBpAG0AYQBsACAAZgByAGEAYwB0AGkAbwBuACAAbwBmACAAYQAgAGQAYQB5ACAAbwByACAARQB4AGMAZQBsACAAVABpAG0AZQAgAGQAYQB0AGEAIAB0AHkAcABlAC4AXABuAFsAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0AF0AIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAAVABpAG0AZQAgAHoAbwBuAGUAIABvAGYAZgBzAGUAdAAgAGkAbgAgAG0AaQBuAHUAdABlAHMAIABmAHIAbwBtACAAVQBUAEMALgBcAG4AWwBQAHIAZQBjAGkAcwBpAG8AbgBdACAAIAAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIABTAGUAbABlAGMAdAAgAHAAcgBlAGMAaQBzAGkAbwBuACAAbABlAHYAZQBsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAwACAALQAgAEEAdQB0AG8AbQBhAHQAaQBjAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAxACAALQAgAEgAbwB1AHIAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADIAIAAtACAATQBpAG4AdQB0AGUAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADMAIAAtACAAUwBlAGMAbwBuAGQAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADQAIAAtACAATQBpAGwAbABpAHMAZQBjAG8AbgBkAFwAbgBbAE4AbwBaAHUAbAB1AF0AIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABzAHcAaQB0AGMAaAAgACAAfAAgAFUAcwBlACAAKwAwADAAOgAwADAAIABpAG4AcwB0AGUAYQBkACAAbwBmACAAWgAgAGYAbwByACAAVQBUAEMAIAB0AGkAbQBlACAAegBvAG4AZQAuAFwAbgBbAFQAbwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAgAHwAIABzAHcAaQB0AGMAaAAgACAAfAAgAEMAYQBsAGMAdQBsAGEAdABlACAAaQBuACAAdABoAGUAIABKAHUAbABpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AIABEAGUAZgBhAHUAbAB0ACAAaQBzACAARwByAGUAZwBvAHIAaQBhAG4AIABwAHIAbwBsAGUAcAB0AGkAYwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIABjAGEAbABlAG4AZABhAHIALgAgAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBKAEQATgBfAEwATwBDAEEATABfAFQATwBfAEkAUwBPAEQAQQBUAEUAIAA9ACAATABBAE0AQgBEAEEAKABMAG8AYwBhAGwASgBEAE4ALAAgAEwAbwBjAGEAbABUAGkAbQBlACwAIABbAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdABdACwAIABbAFAAcgBlAGMAaQBzAGkAbwBuAF0ALAAgAFsATgBvAFoAdQBsAHUAXQAsACAAWwBUAG8ASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0ALABcAG4AIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAXwBqAGQAYQB0AGUALAAgAEoARABOAF8ATABPAEMAQQBMAF8AVABPAF8ASgBEAEEAVABFACgATABvAGMAYQBsAEoARABOACwAIABMAG8AYwBhAGwAVABpAG0AZQAsACAATgAoAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdAApACkALABcAG4AIAAgACAAIAAgACAAIAAgAEoARABBAFQARQBfAFQATwBfAEkAUwBPAEQAQQBUAEUAKABfAGoAZABhAHQAZQAsACAAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0ACwAIABQAHIAZQBjAGkAcwBpAG8AbgAsACAATgBvAFoAdQBsAHUALAAgAFQAbwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ARQBEAEEAVABFAF8AVABPAF8ASQBTAE8ARABBAFQARQBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIABJAFMATwAgAGYAbwByAG0AYQB0ACAAZABhAHQAZQAsACAAdABpAG0AZQAgAGEAbgBkACAAdABpAG0AZQAgAHoAbwBuAGUAIABvAGYAZgBzAGUAdAAgAGYAcgBvAG0AIABhAG4AIABFAHgAYwBlAGwAIABEAGEAdABlAC8AVABpAG0AZQAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIAB0AGUAeAB0ACAAfAAgAEkAUwBPACAAZABhAHQAZQAuAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ARQBEAGEAdABlACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIABFAHgAYwBlAGwAIABEAGEAdABlAC8AVABpAG0AZQAuAFwAbgBbAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdABdACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgAFQAaQBtAGUAIAB6AG8AbgBlACAAbwBmAGYAcwBlAHQAIABpAG4AIABtAGkAbgB1AHQAZQBzACAAZgByAG8AbQAgAFUAVABDAC4AXABuAFsAUAByAGUAYwBpAHMAaQBvAG4AXQAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAAUwBlAGwAZQBjAHQAIABwAHIAZQBjAGkAcwBpAG8AbgAgAGwAZQB2AGUAbABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAMAAgAC0AIABBAHUAdABvAG0AYQB0AGkAYwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAMQAgAC0AIABIAG8AdQByAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAyACAALQAgAE0AaQBuAHUAdABlAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAzACAALQAgAFMAZQBjAG8AbgBkAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAA0ACAALQAgAE0AaQBsAGwAaQBzAGUAYwBvAG4AZABcAG4AWwBOAG8AWgB1AGwAdQBdACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAcwB3AGkAdABjAGgAIAAgAHwAIABVAHMAZQAgACsAMAAwADoAMAAwACAAaQBuAHMAdABlAGEAZAAgAG8AZgAgAFoAIABmAG8AcgAgAFUAVABDACAAdABpAG0AZQAgAHoAbwBuAGUALgBcAG4AWwBUAG8ASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0AIAB8ACAAcwB3AGkAdABjAGgAIAAgAHwAIABDAGEAbABjAHUAbABhAHQAZQAgAGkAbgAgAHQAaABlACAASgB1AGwAaQBhAG4AIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuACAARABlAGYAYQB1AGwAdAAgAGkAcwAgAEcAcgBlAGcAbwByAGkAYQBuACAAcAByAG8AbABlAHAAdABpAGMAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAYwBhAGwAZQBuAGQAYQByAC4AIABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ARQBEAEEAVABFAF8AVABPAF8ASQBTAE8ARABBAFQARQAgAD0AIABMAEEATQBCAEQAQQAoAEUARABhAHQAZQAsACAAWwBUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQAXQAsACAAWwBQAHIAZQBjAGkAcwBpAG8AbgBdACwAIABbAE4AbwBaAHUAbAB1AF0ALAAgAFsAVABvAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACwAXABuACAAIAAgACAASQBGACgARQBEAGEAdABlACAAPQAgAFwAIgBcACIALAAgAFwAIgBcACIALAAgAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABFAEQAYQB0AGUAKQApACwAIAB7ACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AeQBlAGEAcgBDAEUALAAgAFkARQBBAFIAKABFAEQAYQB0AGUAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbQBvAG4AdABoACwAIABNAE8ATgBUAEgAKABFAEQAYQB0AGUAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkALAAgAEQAQQBZACgARQBEAGEAdABlACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHIARABhAHQAZQAsACAASQBGACgATgAoAFQAbwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAgAD0AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAF8AeQBlAGEAcgBDAEUALAAgAF8AbQBvAG4AdABoACwAIABfAGQAYQB5ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEcAUgBFAEcATwBSAEkAQQBOAF8AVABPAF8ASgBVAEwASQBBAE4AKABfAHkAZQBhAHIAQwBFACwAIABfAG0AbwBuAHQAaAAsACAAXwBkAGEAeQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAaQBtAGUALAAgAE0ATwBEACgARQBEAGEAdABlACwAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABGAE8AUgBNAEEAVABfAEkAUwBPAF8ARABBAFQARQAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBOAEQARQBYACgAXwByAEQAYQB0AGUALAAgADEALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBOAEQARQBYACgAXwByAEQAYQB0AGUALAAgADEALAAgADIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBOAEQARQBYACgAXwByAEQAYQB0AGUALAAgADEALAAgADMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AGkAbQBlACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFAAcgBlAGMAaQBzAGkAbwBuACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABOAG8AWgB1AGwAdQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABvAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ARQBEAEEAVABFAF8AVABPAF8ASgBEAEEAVABFAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAHQAaABlACAASgB1AGwAaQBhAG4AIABEAGEAdABlACAAZgBvAHIAIAB0AGgAZQAgAHAAcgBvAHYAaQBkAGUAZAAgAEUAeABjAGUAbAAgAEQAYQB0AGUALwBUAGkAbQBlAC4AXABuAFwAbgBPAHUAdABwAHUAdABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAASgB1AGwAaQBhAG4AIABEAGEAdABlAC4AXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBFAEQAYQB0AGUAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgAEUAeABjAGUAbAAgAEQAYQB0AGUALwBUAGkAbQBlAC4AXABuAFsAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0AF0AIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAAVABpAG0AZQAgAHoAbwBuAGUAIABvAGYAZgBzAGUAdAAgAGkAbgAgAG0AaQBuAHUAdABlAHMAIABmAHIAbwBtACAAVQBUAEMALgBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ARQBEAEEAVABFAF8AVABPAF8ASgBEAEEAVABFACAAPQAgAEwAQQBNAEIARABBACgARQBEAGEAdABlACwAIABbAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdABdACwAXABuACAAIAAgACAASQBGACgARQBEAGEAdABlACAAPQAgAFwAIgBcACIALAAgAFwAIgBcACIALAAgAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABFAEQAYQB0AGUAKQApACwAIAB7ACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AeQBlAGEAcgBDAEUALAAgAFkARQBBAFIAKABFAEQAYQB0AGUAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbQBvAG4AdABoACwAIABNAE8ATgBUAEgAKABFAEQAYQB0AGUAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkALAAgAEQAQQBZACgARQBEAGEAdABlACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAaQBtAGUALAAgAE0ATwBEACgARQBEAGEAdABlACwAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABKAFUATABJAEEATgBfAEQAQQBUAEUAKABfAHkAZQBhAHIAQwBFACwAIABfAG0AbwBuAHQAaAAsACAAXwBkAGEAeQAsACAAXwB0AGkAbQBlACwAIABUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQALAAgADAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEUARABBAFQARQBfAFQATwBfAEoARABOAF8ATABPAEMAQQBMAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAHQAaABlACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByACAAYQBuAGQAIABsAG8AYwBhAGwAIAB0AGkAbQBlACAAZgBvAHIAIAB0AGgAZQAgAHAAcgBvAHYAaQBkAGUAZAAgAEUAeABjAGUAbAAgAEQAYQB0AGUALwBUAGkAbQBlAC4AXABuAFwAbgBPAHUAdABwAHUAdABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAATABvAGMAYQBsACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByAFwAbgAgADIAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIABMAG8AYwBhAGwAIAB0AGkAbQBlACAAbwBmACAAZABhAHkALgAgAEQAZQBjAGkAbQBhAGwAIABmAHIAYQBjAHQAaQBvAG4AIABvAGYAIABhACAAZABhAHkALAAgAGkAbQBwAGwAaQBjAGkAdABsAHkAIABjAG8AbgB2AGUAcgB0AHMAIAB0AG8AIABFAHgAYwBlAGwAIAB0AGkAbQBlACAAZABhAHQAYQAgAHQAeQBwAGUALgBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEUARABhAHQAZQAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgAEUAeABjAGUAbAAgAEQAYQB0AGUALwBUAGkAbQBlAC4AXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEUARABBAFQARQBfAFQATwBfAEoARABOAF8ATABPAEMAQQBMACAAPQAgAEwAQQBNAEIARABBACgARQBEAGEAdABlACwAXABuACAAIAAgACAASQBGACgARQBEAGEAdABlACAAPQAgAFwAIgBcACIALAAgAHsAXAAiAFwAIgAsACAAXAAiAFwAIgB9ACwAIABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgARQBEAGEAdABlACkAKQAsACAAewAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhAH0ALAAgAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AeQBlAGEAcgBDAEUALAAgAFkARQBBAFIAKABFAEQAYQB0AGUAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbQBvAG4AdABoACwAIABNAE8ATgBUAEgAKABFAEQAYQB0AGUAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkALAAgAEQAQQBZACgARQBEAGEAdABlACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAaQBtAGUALAAgAE0ATwBEACgARQBEAGEAdABlACwAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGoAZABuACwAIABKAFUATABJAEEATgBfAEQAQQBZAF8ATgBVAE0AQgBFAFIAKABfAHkAZQBhAHIAQwBFACwAIABfAG0AbwBuAHQAaAAsACAAXwBkAGEAeQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABfAGoAZABuACwAIABfAHQAaQBtAGUAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEoARABOAF8ATABPAEMAQQBMAF8AVABPAF8ARQBEAEEAVABFAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAGEAbgAgAEUAeABjAGUAbAAgAEQAYQB0AGUALwBUAGkAbQBlACAAZgBvAHIAIAB0AGgAZQAgAHAAcgBvAHYAaQBkAGUAZAAgAEoAdQBsAGkAYQBuACAARABhAHkAIABOAHUAbQBiAGUAcgAgAGEAbgBkACAAbABvAGMAYQBsACAAdABpAG0AZQAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgAEUAeABjAGUAbAAgAEQAYQB0AGUALwBUAGkAbQBlAC4AXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBMAG8AYwBhAGwASgBEAE4AIAAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIABMAG8AYwBhAGwAIABKAHUAbABpAGEAbgAgAEQAYQB5ACAATgB1AG0AYgBlAHIALgBcAG4ATABvAGMAYQBsAFQAaQBtAGUAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAATABvAGMAYQBsACAAdABpAG0AZQAgAG8AZgAgAGQAYQB5ACAAYQBzACAAZABlAGMAaQBtAGEAbAAgAGYAcgBhAGMAdABpAG8AbgAgAG8AZgAgAGEAIABkAGEAeQAgAG8AcgAgAEUAeABjAGUAbAAgAFQAaQBtAGUAIABkAGEAdABhACAAdAB5AHAAZQAuAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBKAEQATgBfAEwATwBDAEEATABfAFQATwBfAEUARABBAFQARQAgAD0AIABMAEEATQBCAEQAQQAoAEwAbwBjAGEAbABKAEQATgAsACAATABvAGMAYQBsAFQAaQBtAGUALABcAG4AIAAgACAAIABJAEYAKAAoAEwAbwBjAGEAbABKAEQATgAgAD0AIABcACIAXAAiACkAIAAqACAAKABMAG8AYwBhAGwAVABpAG0AZQAgAD0AIABcACIAXAAiACkALAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgATABvAGMAYQBsAEoARABOACkAKQAgACsAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEwAbwBjAGEAbABUAGkAbQBlACkAKQAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgATQBPAEQAKABMAG8AYwBhAGwASgBEAE4ALAAgADEAKQAgAD4AIAAwACwAIAB7ACMATgBVAE0AIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcgBEAGEAdABlACwAIABKAEQATgBfAFQATwBfAEMAQQBMAEUATgBEAEEAUgBfAEQAQQBUAEUAKABMAG8AYwBhAGwASgBEAE4AKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBlAEQAYQB0AGUALAAgAEQAQQBUAEUAKABJAE4ARABFAFgAKABfAHIARABhAHQAZQAsACAAMQAsACAAMQApACwAIABJAE4ARABFAFgAKABfAHIARABhAHQAZQAsACAAMQAsACAAMgApACwAIABJAE4ARABFAFgAKABfAHIARABhAHQAZQAsACAAMQAsACAAMwApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZQBEAGEAdABlACAAKwAgAEwAbwBjAGEAbABUAGkAbQBlAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBKAEQAQQBUAEUAXwBUAE8AXwBFAEQAQQBUAEUAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAYQBuACAARQB4AGMAZQBsACAARABhAHQAZQAvAFQAaQBtAGUAIABmAG8AcgAgAHQAaABlACAAcAByAG8AdgBpAGQAZQBkACAASgB1AGwAaQBhAG4AIABEAGEAdABlAC4AXABuAFwAbgBPAHUAdABwAHUAdABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAARQB4AGMAZQBsACAARABhAHQAZQAvAFQAaQBtAGUALgBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEoARABhAHQAZQAgACAAIAAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgAEoAdQBsAGkAYQBuACAARABhAHQAZQBcAG4AVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0ACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAAVABpAG0AZQAgAHoAbwBuAGUAIABvAGYAZgBzAGUAdAAgAGkAbgAgAG0AaQBuAHUAdABlAHMAIABmAHIAbwBtACAAVQBUAEMALgBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ASgBEAEEAVABFAF8AVABPAF8ARQBEAEEAVABFACAAPQAgAEwAQQBNAEIARABBACgASgBEAGEAdABlACwAIABUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQALABcAG4AIAAgACAAIABJAEYAKABKAEQAYQB0AGUAIAA9ACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABKAEQAYQB0AGUAKQApACwAIAB7ACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AagBkAG4ATABvAGMAYQBsACwAIABKAEQAQQBUAEUAXwBUAE8AXwBKAEQATgBfAEwATwBDAEEATAAoAEoARABhAHQAZQAsACAATgAoAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdAApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABKAEQATgBfAEwATwBDAEEATABfAFQATwBfAEUARABBAFQARQAoAEkATgBEAEUAWAAoAF8AagBkAG4ATABvAGMAYQBsACwAIAAxACwAIAAxACkALAAgAEkATgBEAEUAWAAoAF8AagBkAG4ATABvAGMAYQBsACwAIAAxACwAIAAyACkAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFUAUwBEAEEAVABFAF8AVABPAF8ARQBEAEEAVABFAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAGEAbgAgAEUAeABjAGUAbAAgAEQAYQB0AGUALwBUAGkAbQBlACAAZgBvAHIAIAB0AGgAZQAgAHAAcgBvAHYAaQBkAGUAZAAgAFUAUwAgAGYAbwByAG0AYQB0ACAAZABhAHQAZQAgAGEAbgBkACAAdABpAG0AZQAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgAEUAeABjAGUAbAAgAEQAYQB0AGUALwBUAGkAbQBlAC4AXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBVAFMARABhAHQAZQAgAHwAIAB0AGUAeAB0ACAAfAAgAEQAYQB0AGUAIABpAG4AIABVAFMAIABmAG8AcgBtAGEAdAAgAGkAZQAuACAATQBNAC8AZABkAC8AeQB5AHkAeQAgAGgAaAA6AG0AbQA6AHMAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4AVQBTAEQAQQBUAEUAXwBUAE8AXwBFAEQAQQBUAEUAIAA9ACAATABBAE0AQgBEAEEAKABVAFMARABhAHQAZQAsAFwAbgAgACAAIAAgAEkARgAoAFUAUwBEAGEAdABlACAAPQAgAFwAIgBcACIALAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AVQBTAEQAYQB0AGUALAAgAFAAQQBSAFMARQBfAFUAUwBfAEQAQQBUAEUAKABVAFMARABhAHQAZQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdABpAG0AZQAsACAASQBOAEQARQBYACgAXwBVAFMARABhAHQAZQAsACAAMQAsACAANAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AeQBlAGEAcgAsACAASQBOAEQARQBYACgAXwBVAFMARABhAHQAZQAsACAAMQAsACAAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZQBEAGEAdABlACwAIABJAEYAKABfAHkAZQBhAHIAIAA9ACAAXAAiAFwAIgAsACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEQAQQBUAEUAKABfAHkAZQBhAHIALAAgAEkATgBEAEUAWAAoAF8AVQBTAEQAYQB0AGUALAAgADEALAAgADIAKQAsACAASQBOAEQARQBYACgAXwBVAFMARABhAHQAZQAsACAAMQAsACAAMwApACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBlAEQAYQB0AGUAIAArACAAXwB0AGkAbQBlAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ARQBEAEEAVABFAF8AVABPAF8AVQBTAEQAQQBUAEUAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAYQAgAFUAUwAgAGYAbwByAG0AYQB0ACAAZABhAHQAZQAgAGEAbgBkACAAdABpAG0AZQAgAGYAbwByACAAdABoAGUAIABwAHIAbwB2AGkAZABlAGQAIABFAHgAYwBlAGwAIABEAGEAdABlAC8AVABpAG0AZQAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIAB0AGUAeAB0ACAAfAAgAFUAUwAgAGYAbwByAG0AYQB0ACAAZABhAHQAZQAgAGEAbgBkACAAdABpAG0AZQBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEUARABhAHQAZQAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgAEUAeABjAGUAbAAgAEQAYQB0AGUALwBUAGkAbQBlAC4AXABuAFsAUwBlAHAAYQByAGEAdABvAHIAXQAgAHwAIABjAGgAYQByACAAIAAgACAAfAAgAEMAaABhAHIAYQBjAHQAZQByACAAcwBlAHAAYQByAGEAdABvAHIAIABmAG8AcgAgAGQAYQB0AGUAIABlAGwAZQBtAGUAbgB0AHMALgAgAFsALAAuAC8ALQBfAF0AXABuAFsAUAByAGUAYwBpAHMAaQBvAG4AXQAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAFMAZQBsAGUAYwB0ACAAcAByAGUAYwBpAHMAaQBvAG4AIABsAGUAdgBlAGwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAwACAALQAgAEEAdQB0AG8AbQBhAHQAaQBjAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAMQAgAC0AIABIAG8AdQByAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAMgAgAC0AIABNAGkAbgB1AHQAZQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADMAIAAtACAAUwBlAGMAbwBuAGQAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAA0ACAALQAgAE0AaQBsAGwAaQBzAGUAYwBvAG4AZABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ARQBEAEEAVABFAF8AVABPAF8AVQBTAEQAQQBUAEUAIAA9ACAATABBAE0AQgBEAEEAKABFAEQAYQB0AGUALAAgAFsAUwBlAHAAYQByAGEAdABvAHIAXQAsACAAWwBQAHIAZQBjAGkAcwBpAG8AbgBdACwAXABuACAAIAAgACAASQBGACgARQBEAGEAdABlACAAPQAgAFwAIgBcACIALAAgAFwAIgBcACIALAAgAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABFAEQAYQB0AGUAKQApACwAIAB7ACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AeQBlAGEAcgBDAEUALAAgAFkARQBBAFIAKABFAEQAYQB0AGUAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbQBvAG4AdABoACwAIABNAE8ATgBUAEgAKABFAEQAYQB0AGUAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkALAAgAEQAQQBZACgARQBEAGEAdABlACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAaQBtAGUALAAgAE0ATwBEACgARQBEAGEAdABlACwAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABGAE8AUgBNAEEAVABfAFUAUwBfAEQAQQBUAEUAKABfAHkAZQBhAHIAQwBFACwAIABfAG0AbwBuAHQAaAAsACAAXwBkAGEAeQAsACAAXwB0AGkAbQBlACwAIABTAGUAcABhAHIAYQB0AG8AcgAsACAAUAByAGUAYwBpAHMAaQBvAG4ALAAgADAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAFwAbgAvACoAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjAFwAbgAjACAARQBOAEQAIABDAEEATABFAE4ARABBAFIAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAKgAvAFwAbgAiAH0AXQAsACIAcAByAG8AagBlAGMAdABOAGEAbQBlAHMAIgA6AFsAIgBDAEEATABFAE4ARABBAFIALgBJAFMAXwBMAEUAQQBQAF8AWQBFAEEAUgAiACwAIgBDAEEATABFAE4ARABBAFIALgBJAFMAXwBWAEEATABJAEQAXwBEAEEAVABFACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAEkAUwBfAFYAQQBMAEkARABfAFQASQBNAEUAIgAsACIAQwBBAEwARQBOAEQAQQBSAC4AWQBFAEEAUgBfAEMATwBNAE0ATwBOAF8ARQBSAEEAIgAsACIAQwBBAEwARQBOAEQAQQBSAC4ARABBAFkAUwBfAEkATgBfAFkARQBBAFIAIgAsACIAQwBBAEwARQBOAEQAQQBSAC4ARABBAFkAUwBfAEkATgBfAE0ATwBOAFQASAAiACwAIgBDAEEATABFAE4ARABBAFIALgBKAFUATABJAEEATgBfAEQAQQBZAF8ATgBVAE0AQgBFAFIAIgAsACIAQwBBAEwARQBOAEQAQQBSAC4ASgBEAE4AXwBUAE8AXwBDAEEATABFAE4ARABBAFIAXwBEAEEAVABFACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAEoARABOAF8AVABPAF8ATwBSAEQASQBOAEEATABfAEQAQQBUAEUAIgAsACIAQwBBAEwARQBOAEQAQQBSAC4ATwBSAEQASQBOAEEATABfAEQAQQBUAEUAXwBUAE8AXwBKAEQATgAiACwAIgBDAEEATABFAE4ARABBAFIALgBHAFIARQBHAE8AUgBJAEEATgBfAFQATwBfAEoAVQBMAEkAQQBOACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAEoAVQBMAEkAQQBOAF8AVABPAF8ARwBSAEUARwBPAFIASQBBAE4AIgAsACIAQwBBAEwARQBOAEQAQQBSAC4AUwBFAEMAVQBMAEEAUgBfAEQASQBGAEYARQBSAEUATgBDAEUAIgAsACIAQwBBAEwARQBOAEQAQQBSAC4ARABBAFkAXwBPAEYAXwBXAEUARQBLACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAEMATwBOAFYARQBSAFQAXwBXAEUARQBLAEQAQQBZAF8ATgBVAE0AQgBFAFIAIgAsACIAQwBBAEwARQBOAEQAQQBSAC4AVwBFAEUASwBEAEEAWQBfAE8ARgBfAE0ATwBOAFQASAAiACwAIgBDAEEATABFAE4ARABBAFIALgBXAEUARQBLAFMAXwBJAE4AXwBZAEUAQQBSACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAFcARQBFAEsAXwBEAEEAVABFAF8AVABPAF8ASgBEAE4AIgAsACIAQwBBAEwARQBOAEQAQQBSAC4ASgBEAE4AXwBUAE8AXwBXAEUARQBLAF8ARABBAFQARQAiACwAIgBDAEEATABFAE4ARABBAFIALgBXAEUARQBLAF8ATgBVAE0AQgBFAFIAIgAsACIAQwBBAEwARQBOAEQAQQBSAC4ARABBAFkAUwBfAEkATgBfAFEAVQBBAFIAVABFAFIAIgAsACIAQwBBAEwARQBOAEQAQQBSAC4AUQBVAEEAUgBUAEUAUgBfAEQAQQBUAEUAXwBUAE8AXwBKAEQATgAiACwAIgBDAEEATABFAE4ARABBAFIALgBKAEQATgBfAFQATwBfAFEAVQBBAFIAVABFAFIAXwBEAEEAVABFACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAEoARABOAF8AVQBUAEMAXwBUAE8AXwBKAEQAQQBUAEUAIgAsACIAQwBBAEwARQBOAEQAQQBSAC4ASgBEAE4AXwBMAE8AQwBBAEwAXwBUAE8AXwBKAEQAQQBUAEUAIgAsACIAQwBBAEwARQBOAEQAQQBSAC4ASgBEAEEAVABFAF8AVABPAF8ASgBEAE4AXwBVAFQAQwAiACwAIgBDAEEATABFAE4ARABBAFIALgBKAEQAQQBUAEUAXwBUAE8AXwBKAEQATgBfAEwATwBDAEEATAAiACwAIgBDAEEATABFAE4ARABBAFIALgBKAFUATABJAEEATgBfAEQAQQBUAEUAIgAsACIAQwBBAEwARQBOAEQAQQBSAC4AQwBBAEwARQBOAEQAQQBSAF8ARgBSAE8ATQBfAEoARABBAFQARQAiACwAIgBDAEEATABFAE4ARABBAFIALgBUAEkATQBFAF8ARABFAEMASQBNAEEATABfAFQATwBfAEgATQBTACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAEgATQBTAF8AVABPAF8AVABJAE0ARQBfAEQARQBDAEkATQBBAEwAIgAsACIAQwBBAEwARQBOAEQAQQBSAC4AQQBEAEQAXwBUAEkATQBFAFMAUABBAE4AIgAsACIAQwBBAEwARQBOAEQAQQBSAC4AUgBFAFMATwBMAFYARQBfAEQAQQBUAEUAIgAsACIAQwBBAEwARQBOAEQAQQBSAC4ARABFAEwAVABBAF8ASABPAFUAUgBTACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAEQARQBMAFQAQQBfAE0ASQBOAFUAVABFAFMAIgAsACIAQwBBAEwARQBOAEQAQQBSAC4ARABFAEwAVABBAF8AUwBFAEMATwBOAEQAUwAiACwAIgBDAEEATABFAE4ARABBAFIALgBEAEUATABUAEEAXwBIAE8AVQBSAF8ATQBJAE4AXwBTAEUAQwAiACwAIgBDAEEATABFAE4ARABBAFIALgBEAEUATABUAEEAXwBEAEEAWQBTACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAEQARQBMAFQAQQBfAFcARQBFAEsAUwAiACwAIgBDAEEATABFAE4ARABBAFIALgBEAEUATABUAEEAXwBNAE8ATgBUAEgAUwAiACwAIgBDAEEATABFAE4ARABBAFIALgBEAEUATABUAEEAXwBRAFUAQQBSAFQARQBSAFMAIgAsACIAQwBBAEwARQBOAEQAQQBSAC4ARABFAEwAVABBAF8AWQBFAEEAUgBTACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAEQARQBMAFQAQQBfAFcARQBFAEsAXwBEAEEAWQBTACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAEQARQBMAFQAQQBfAFkARQBBAFIAXwBXAEUARQBLAF8ARABBAFkAUwAiACwAIgBDAEEATABFAE4ARABBAFIALgBEAEUATABUAEEAXwBNAE8ATgBUAEgAXwBEAEEAWQBTACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAEQARQBMAFQAQQBfAFEAVQBBAFIAVABFAFIAXwBEAEEAWQBTACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAEQARQBMAFQAQQBfAEkATgBUAEUAUgBWAEEATAAiACwAIgBDAEEATABFAE4ARABBAFIALgBFAFgAVABFAE4AVABfAE8ARgBfAEQAQQBZAFMAIgAsACIAQwBBAEwARQBOAEQAQQBSAC4ARQBYAFQARQBOAFQAXwBPAEYAXwBXAEUARQBLAFMAIgAsACIAQwBBAEwARQBOAEQAQQBSAC4ARQBYAFQARQBOAFQAXwBPAEYAXwBNAE8ATgBUAEgAUwAiACwAIgBDAEEATABFAE4ARABBAFIALgBFAFgAVABFAE4AVABfAE8ARgBfAFEAVQBBAFIAVABFAFIAUwAiACwAIgBDAEEATABFAE4ARABBAFIALgBFAFgAVABFAE4AVABfAE8ARgBfAFkARQBBAFIAUwAiACwAIgBDAEEATABFAE4ARABBAFIALgBQAEEAUgBTAEUAXwBJAFMATwBfAEQAQQBUAEUAIgAsACIAQwBBAEwARQBOAEQAQQBSAC4AUABBAFIAUwBFAF8AVwBFAEUASwBEAEEAWQAiACwAIgBDAEEATABFAE4ARABBAFIALgBQAEEAUgBTAEUAXwBNAE8ATgBUAEgAIgAsACIAQwBBAEwARQBOAEQAQQBSAC4AUABBAFIAUwBFAF8ATABJAFQARQBSAEEAUgBZAF8AWQBFAEEAUgAiACwAIgBDAEEATABFAE4ARABBAFIALgBQAEEAUgBTAEUAXwBMAEkAVABFAFIAQQBSAFkAXwBEAEEAVABFACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAFAAQQBSAFMARQBfAFUAUwBfAEQAQQBUAEUAIgAsACIAQwBBAEwARQBOAEQAQQBSAC4AUABBAFIAUwBFAF8ATQBJAEwAXwBEAFQARwAiACwAIgBDAEEATABFAE4ARABBAFIALgBXAEUARQBLAEQAQQBZAF8ATgBBAE0ARQAiACwAIgBDAEEATABFAE4ARABBAFIALgBNAE8ATgBUAEgAXwBOAEEATQBFACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAEYATwBSAE0AQQBUAF8ASQBTAE8AXwBEAEEAVABFACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAEYATwBSAE0AQQBUAF8ATABJAFQARQBSAEEAUgBZAF8AWQBFAEEAUgAiACwAIgBDAEEATABFAE4ARABBAFIALgBGAE8AUgBNAEEAVABfAEwASQBUAEUAUgBBAFIAWQBfAEQAQQBUAEUAIgAsACIAQwBBAEwARQBOAEQAQQBSAC4ARgBPAFIATQBBAFQAXwBVAFMAXwBEAEEAVABFACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAEYATwBSAE0AQQBUAF8ATQBJAEwAXwBEAFQARwAiACwAIgBDAEEATABFAE4ARABBAFIALgBJAFMATwBEAEEAVABFAF8AVABPAF8ASgBEAE4AXwBMAE8AQwBBAEwAIgAsACIAQwBBAEwARQBOAEQAQQBSAC4ASQBTAE8ARABBAFQARQBfAFQATwBfAEoARABBAFQARQAiACwAIgBDAEEATABFAE4ARABBAFIALgBJAFMATwBEAEEAVABFAF8AVABPAF8ARQBEAEEAVABFACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAEoARABBAFQARQBfAFQATwBfAEkAUwBPAEQAQQBUAEUAIgAsACIAQwBBAEwARQBOAEQAQQBSAC4ASgBEAE4AXwBMAE8AQwBBAEwAXwBUAE8AXwBJAFMATwBEAEEAVABFACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAEUARABBAFQARQBfAFQATwBfAEkAUwBPAEQAQQBUAEUAIgAsACIAQwBBAEwARQBOAEQAQQBSAC4ARQBEAEEAVABFAF8AVABPAF8ASgBEAEEAVABFACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAEUARABBAFQARQBfAFQATwBfAEoARABOAF8ATABPAEMAQQBMACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAEoARABOAF8ATABPAEMAQQBMAF8AVABPAF8ARQBEAEEAVABFACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAEoARABBAFQARQBfAFQATwBfAEUARABBAFQARQAiACwAIgBDAEEATABFAE4ARABBAFIALgBVAFMARABBAFQARQBfAFQATwBfAEUARABBAFQARQAiACwAIgBDAEEATABFAE4ARABBAFIALgBFAEQAQQBUAEUAXwBUAE8AXwBVAFMARABBAFQARQAiAF0ALAAiAGwAbwBjAGEAbABlACIAOgB7ACIAbABpAHMAdABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHIAbwB3AFMAZQBwAGEAcgBhAHQAbwByACIAOgAiADsAIgAsACIAYwBvAGwAdQBtAG4AUwBlAHAAYQByAGEAdABvAHIAIgA6ACIALAAiACwAIgB0AGgAbwB1AHMAYQBuAGQAcwBTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHQAaABvAHUAcwBhAG4AZABzAFAAbwBzAGkAdABpAG8AbgBzACIAOgBbADMAXQAsACIAZABlAGMAaQBtAGEAbABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAuACIALAAiAGQAYQB0AGUATwByAGQAZQByACIAOgAiAEQATQBZACIALAAiAGMAdQByAHIAZQBuAGMAeQBTAHkAbQBiAG8AbAAiADoAIgAkACIALAAiAGkAcwBDAHUAcgByAGUAbgBjAHkAUwB5AG0AYgBvAGwATABlAGEAZAAiADoAdAByAHUAZQAsACIAaQBzAEMAdQByAHIAZQBuAGMAeQBTAGUAcABCAHkAUwBwAGEAYwBlACIAOgBmAGEAbABzAGUALAAiAHIAbwB3AEwAZQB0AHQAZQByACIAOgAiAFIAIgAsACIAYwBvAGwAdQBtAG4ATABlAHQAdABlAHIAIgA6ACIAQwAiACwAIgByAGMATABlAGYAdABCAHIAYQBjAGsAZQB0ACIAOgAiAFsAIgAsACIAcgBjAFIAaQBnAGgAdABCAHIAYQBjAGsAZQB0ACIAOgAiAF0AIgAsACIAcwB0AGEAdABlAG0AZQBuAHQAUwBlAHAAYQByAGEAdABvAHIAIgA6ACIAOwAiACwAIgBsAG8AYwBhAGwAZQBOAGEAbQBlACIAOgAiAGUAbgAtAHUAcwAiAH0AfQA=</AFEJSONBlob>
+<AFEJSONBlob xmlns="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0">ewAiAHMAYwBoAGUAbQBhACIAOgAiAGgAdAB0AHAAOgAvAC8AcwBjAGgAZQBtAGEAcwAuAGEAZAB2AGEAbgBjAGUAZABmAG8AcgBtAHUAbABhAGUAbgB2AGkAcgBvAG4AbQBlAG4AdAAuAG8AZgBmAGkAYwBlAGEAcABwAHMALgBsAGkAdgBlAC4AYwBvAG0ALwBhAGYAZQBwAHIAbwBqAGUAYwB0AHMALwAwAC4AMgAiACwAIgBmAGkAbABlAHMAIgA6AFsAewAiAHAAYQB0AGgAIgA6ACIALwBwAHIAbwBqAGUAYwB0AHMALwBXAG8AcgBrAGIAbwBvAGsAIgAsACIAdABlAHgAdAAiADoAIgAiAH0ALAB7ACIAcABhAHQAaAAiADoAIgAvAHAAcgBvAGoAZQBjAHQAcwAvAEMAQQBMAEUATgBEAEEAUgAiACwAIgB0AGUAeAB0ACIAOgAiAC8AKgAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAXABuACMAIABDAEEATABFAE4ARABBAFIAIAB2ADEALgAxACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABNAG8AZAB1AGwAZQAgAGYAbwByACAAdwBvAHIAawBpAG4AZwAgAHcAaQB0AGgAIABkAGEAdABlAHMAIABpAG4AIAB0AGgAZQAgAEcAcgBlAGcAbwByAGkAYQBuACAAYQBuAGQAIABKAHUAbABpAGEAbgAgAGMAYQBsAGUAbgBkAGEAcgBzACAAbwB1AHQAcwBpAGQAZQAgAHQAaABlACAAcgBhAG4AZwBlACAAbwBmACAAdABoAGUAIABFAHgAYwBlAGwAIAAgACAAIAAgACMAXABuACMAIABEAGEAdABlAC8AVABpAG0AZQAgAHQAeQBwAGUALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABNAG8AZAB1AGwAZQAgAEQAZQBwAGUAbgBkAGUAbgBjAGkAZQBzADoAIABOAG8AbgBlACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABMAE8ARwBJAEMAQQBMACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIAAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAgACMAXABuACMAIABJAFMAXwBMAEUAQQBQAF8AWQBFAEEAUgAgACAAIAAgACAAIAAgACAAIAAgACAAVABlAHMAdABzACAAaQBmACAAYQAgAHkAZQBhAHIAIABpAG4AYwBsAHUAZABlAHMAIABhACAAbABlAGEAcAAgAGQAYQB5ACAAaQBuACAAdABoAGUAIABnAGkAdgBlAG4AIABjAGEAbABlAG4AZABhAHIALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABJAFMAXwBWAEEATABJAEQAXwBEAEEAVABFACAAIAAgACAAIAAgACAAIAAgACAAVABlAHMAdABzACAAaQBmACAAYQAgAGQAYQB0AGUAIABpAHMAIAB2AGEAbABpAGQAIABmAG8AcgAgAHQAaABlACAAZwBpAHYAZQBuACAAYwBhAGwAZQBuAGQAYQByAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABJAFMAXwBWAEEATABJAEQAXwBUAEkATQBFACAAIAAgACAAIAAgACAAIAAgACAAVABlAHMAdABzACAAaQBmACAAYQAgAHQAaQBtAGUAIABpAHMAIAB2AGEAbABpAGQAIABpAG4AIAB0AGgAZQAgADIANAAgAGgAbwB1AHIAIAB0AGkAbQBlAGsAZQBlAHAAaQBuAGcAIABzAHkAcwB0AGUAbQAuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABDAEEATABFAE4ARABBAFIAIABEAEEAVABFAFMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIAAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAgACMAXABuACMAIABZAEUAQQBSAF8AQwBPAE0ATQBPAE4AXwBFAFIAQQAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHkAZQBhAHIAIAB2AGEAbAB1AGUAIAByAGUAbABhAHQAaQB2AGUAIAB0AG8AIAB0AGgAZQAgAEMAbwBtAG0AbwBuACAARQByAGEALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABEAEEAWQBTAF8ASQBOAF8AWQBFAEEAUgAgACAAIAAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAG4AdQBtAGIAZQByACAAbwBmACAAZABhAHkAcwAgAGkAbgAgAHQAaABlACAAZwBpAHYAZQBuACAAeQBlAGEAcgAgAG8AZgAgAHQAaABlACAAcwBwAGUAYwBpAGYAaQBlAGQAIABjAGEAbABlAG4AZABhAHIALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABEAEEAWQBTAF8ASQBOAF8ATQBPAE4AVABIACAAIAAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAG4AdQBtAGIAZQByACAAbwBmACAAZABhAHkAcwAgAGkAbgAgAHQAaABlACAAZwBpAHYAZQBuACAAbQBvAG4AdABoACAAYQBuAGQAIAB5AGUAYQByACAAbwBmACAAdABoAGUAIABzAHAAZQBjAGkAZgBpAGUAZAAgAGMAYQBsAGUAbgBkAGEAcgAuACAAIAAgACMAXABuACMAIABKAFUATABJAEEATgBfAEQAQQBZAF8ATgBVAE0AQgBFAFIAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByACAAbwBmACAAdABoAGUAIABwAHIAbwB2AGkAZABlAGQAIABkAGEAdABlACAAaQBuACAAdABoAGUAIABzAHAAZQBjAGkAZgBpAGUAZAAgAGMAYQBsAGUAbgBkAGEAcgAuACAAIAAgACMAXABuACMAIABKAEQATgBfAFQATwBfAEMAQQBMAEUATgBEAEEAUgBfAEQAQQBUAEUAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAAZABhAHQAZQAgAGYAcgBvAG0AIAB0AGgAZQAgAGcAaQB2AGUAbgAgAEoAdQBsAGkAYQBuACAARABhAHkAIABOAHUAbQBiAGUAcgAgAGkAbgAgAHQAaABlACAAcwBwAGUAYwBpAGYAaQBlAGQAIABjAGEAbABlAG4AZABhAHIALgAgACAAIAAgACMAXABuACMAIABKAEQATgBfAFQATwBfAE8AUgBEAEkATgBBAEwAXwBEAEEAVABFACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAAeQBlAGEAcgAsACAAbwByAGQAaQBuAGEAbAAgAGQAYQB5ACAAbwBmACAAeQBlAGEAcgAgAGEAbgBkACAAZABhAHkAcwAgAGkAbgAgAHQAaABlACAAeQBlAGEAcgAgAGYAcgBvAG0AIAB0AGgAZQAgAGcAaQB2AGUAbgAgACAAIAAgACAAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByACAAaQBuACAAdABoAGUAIABzAHAAZQBjAGkAZgBpAGUAZAAgAGMAYQBsAGUAbgBkAGEAcgAuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABPAFIARABJAE4AQQBMAF8ARABBAFQARQBfAFQATwBfAEoARABOACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByACAAbwBmACAAdABoAGUAIABwAHIAbwB2AGkAZABlAGQAIABvAHIAZABpAG4AYQBsACAAZABhAHQAZQAgAGkAbgAgAHQAaABlACAAcwBwAGUAYwBpAGYAaQBlAGQAIAAgACAAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAYwBhAGwAZQBuAGQAYQByAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABHAFIARQBHAE8AUgBJAEEATgBfAFQATwBfAEoAVQBMAEkAQQBOACAAIAAgACAAVAByAGEAbgBzAGwAYQB0AGUAcwAgAGEAIABkAGEAdABlACAAaQBuACAAdABoAGUAIABHAHIAZQBnAG8AcgBpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByACAAdABvACAAdABoAGUAIABKAHUAbABpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAYwBhAGwAZQBuAGQAYQByAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABKAFUATABJAEEATgBfAFQATwBfAEcAUgBFAEcATwBSAEkAQQBOACAAIAAgACAAVAByAGEAbgBzAGwAYQB0AGUAcwAgAGEAIABkAGEAdABlACAAaQBuACAAdABoAGUAIABKAHUAbABpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByACAAdABvACAAdABoAGUAIABHAHIAZQBnAG8AcgBpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAYwBhAGwAZQBuAGQAYQByAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABTAEUAQwBVAEwAQQBSAF8ARABJAEYARgBFAFIARQBOAEMARQAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAAbgB1AG0AYgBlAHIAIABvAGYAIABkAGEAeQBzACAAdABoAGUAIABHAHIAZQBnAG8AcgBpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByACAAaQBzACAAYQBoAGUAYQBkACAAbwBmACAAdABoAGUAIAAgACAAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASgB1AGwAaQBhAG4AIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAgAGYAbwByACAAYQAgAGcAaQB2AGUAbgAgAGQAYQB0AGUALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABXAEUARQBLAFMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIAAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAgACMAXABuACMAIABEAEEAWQBfAE8ARgBfAFcARQBFAEsAIAAgACAAIAAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAGEAbgAgAGkAbgB0AGUAZwBlAHIAIABmAG8AcgAgAHQAaABlACAAZABhAHkAIABvAGYAIAB0AGgAZQAgAHcAZQBlAGsAIABmAG8AcgAgAGEAIABnAGkAdgBlAG4AIABKAHUAbABpAGEAbgAgAEQAYQB5ACAATgB1AG0AYgBlAHIALgAgACAAIAAgACAAIAAgACMAXABuACMAIABDAE8ATgBWAEUAUgBUAF8AVwBFAEUASwBEAEEAWQBfAE4AVQBNAEIARQBSACAAUgBlAHQAdQByAG4AcwAgAGEAbgAgAGkAbgB0AGUAZwBlAHIAIABmAG8AcgAgAHQAaABlACAAZABhAHkAIABvAGYAIAB0AGgAZQAgAHcAZQBlAGsAIABmAHIAbwBtACAAdABoAGUAIAB0AHIAYQBkAGkAdABvAG4AYQBsACAAbgB1AG0AYgBlAHIAaQBuAGcAIABzAGMAaABlAG0AZQAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAdABvACAAdABoAGUAIABJAFMATwAgAGQAZQBmAGkAbgBpAHQAaQBvAG4ALAAgAG8AcgAgAHYAaQBjAGUAIAB2AGUAcgBzAGEALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABXAEUARQBLAEQAQQBZAF8ATwBGAF8ATQBPAE4AVABIACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAGEAIABKAHUAbABpAGEAbgAgAEQAYQB5ACAATgB1AG0AYgBlAHIAIABmAG8AcgAgAGEAIABnAGkAdgBlAG4AIABkAGEAeQAgAG8AZgAgAHcAZQBlAGsALAAgAGEAbgBkACAAYQAgAHIAZQBsAGEAdABpAHYAZQAgAHcAZQBlAGsAIABmAG8AcgAgACAAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAdABoAGUAIABtAG8AbgB0AGgAIABhAG4AZAAgAHkAZQBhAHIAIABvAGYAIAB0AGgAZQAgAHMAcABlAGMAaQBmAGkAZQBkACAAYwBhAGwAZQBuAGQAYQByAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABXAEUARQBLAFMAXwBJAE4AXwBZAEUAQQBSACAAIAAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAAYwBvAHUAbgB0ACAAbwBmACAASQBTAE8AIABkAGUAZgBpAG4AZQBkACAAdwBlAGUAawBzACAAaQBuACAAYQAgAGcAaQB2AGUAbgAgAHkAZQBhAHIAIABvAGYAIAB0AGgAZQAgAHMAcABlAGMAaQBmAGkAZQBkACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAYwBhAGwAZQBuAGQAYQByAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABXAEUARQBLAF8ARABBAFQARQBfAFQATwBfAEoARABOACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByACAAbwBmACAAdABoAGUAIABwAHIAbwB2AGkAZABlAGQAIAB3AGUAZQBrACAAZABhAHQAZQAgAGkAbgAgAHQAaABlACAAcwBwAGUAYwBpAGYAaQBlAGQAIAAgACAAIAAgACAAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAYwBhAGwAZQBuAGQAYQByAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABKAEQATgBfAFQATwBfAFcARQBFAEsAXwBEAEEAVABFACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAAeQBlAGEAcgAsACAASQBTAE8AIABkAGUAZgBpAG4AZQBkACAAdwBlAGUAawAgAG4AdQBtAGIAZQByACwAIABkAGEAeQAgAG8AZgAgAHQAaABlACAAdwBlAGUAawAsACAAYQBuAGQAIAB3AGUAZQBrAHMAIABpAG4AIAB0AGgAZQAgACAAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAeQBlAGEAcgAgAGYAbwByACAAdABoAGUAIABnAGkAdgBlAG4AIABKAHUAbABpAGEAbgAgAEQAYQB5ACAATgB1AG0AYgBlAHIAIABpAG4AIAB0AGgAZQAgAHMAcABlAGMAaQBmAGkAZQBkACAAYwBhAGwAZQBuAGQAYQByAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABXAEUARQBLAF8ATgBVAE0AQgBFAFIAIAAgACAAIAAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAASQBTAE8AIABkAGUAZgBpAG4AZQBkACAAdwBlAGUAawAgAG4AdQBtAGIAZQByACAAZgBvAHIAIABhACAAZwBpAHYAZQBuACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByACAAaQBuACAAdABoAGUAIAAgACAAIAAgACAAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAcwBwAGUAYwBpAGYAaQBlAGQAIABjAGEAbABlAG4AZABhAHIALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABRAFUAQQBSAFQARQBSAFMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIAAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAgACMAXABuACMAIABEAEEAWQBTAF8ASQBOAF8AUQBVAEEAUgBUAEUAUgAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAAYwBvAHUAbgB0ACAAbwBmACAAZABhAHkAcwAgAGkAbgAgAGEAIABxAHUAYQByAHQAZQByACAAbwBmACAAYQAgAGcAaQB2AGUAbgAgAHkAZQBhAHIAIABvAGYAIAB0AGgAZQAgAHMAcABlAGMAaQBmAGkAZQBkACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAYwBhAGwAZQBuAGQAYQByAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABKAEQATgBfAFQATwBfAFEAVQBBAFIAVABFAFIAXwBEAEEAVABFACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAAeQBlAGEAcgAsACAAcQB1AGEAcgB0AGUAcgAsACAAZABhAHkAIABvAGYAIABxAHUAYQByAHQAZQByACAAYQBuAGQAIABkAGEAeQBzACAAaQBuACAAdABoAGUAIABxAHUAYQByAHQAZQByACAAZgBvAHIAIAB0AGgAZQAgAGcAaQB2AGUAbgAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByACAAaQBuACAAdABoAGUAIABzAHAAZQBjAGkAZgBpAGUAZAAgAGMAYQBsAGUAbgBkAGEAcgAuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABRAFUAQQBSAFQARQBSAF8ARABBAFQARQBfAFQATwBfAEoARABOACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByACAAbwBmACAAdABoAGUAIABwAHIAbwB2AGkAZABlAGQAIABxAHUAYQByAHQAZQByACAAZABhAHQAZQAgAGkAbgAgAHQAaABlACAAcwBwAGUAYwBpAGYAaQBlAGQAIAAgACAAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAYwBhAGwAZQBuAGQAYQByAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABEAEEAVABFACAAQQBOAEQAIABUAEkATQBFACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIAAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAgACMAXABuACMAIABKAEQATgBfAFUAVABDAF8AVABPAF8ASgBEAEEAVABFACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAASgB1AGwAaQBhAG4AIABEAGEAdABlACAAZwBpAHYAZQBuACAAYQBuACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByACAAYQBuAGQAIAB0AGkAbQBlACAAbwBmACAAZABhAHkAIABpAG4AIABVAFQAQwAuACAAIAAgACAAIAAgACMAXABuACMAIABKAEQATgBfAEwATwBDAEEATABfAFQATwBfAEoARABBAFQARQAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAASgB1AGwAaQBhAG4AIABEAGEAdABlACAAZwBpAHYAZQBuACAAYQAgAGwAbwBjAGEAbAAgAEoAdQBsAGkAYQBuACAARABhAHkAIABOAHUAbQBiAGUAcgAgAGEAbgBkACAAbABvAGMAYQBsACAAdABpAG0AZQAgAG8AZgAgAGQAYQB5ACAAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAdwBpAHQAaAAgAHQAaQBtAGUAIAB6AG8AbgBlACAAbwBmAGYAcwBlAHQAIABpAG4AIABtAGkAbgB1AHQAZQBzAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABKAEQAQQBUAEUAXwBUAE8AXwBKAEQATgBfAFUAVABDACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByACAAYQBuAGQAIAB0AGkAbQBlACAAbwBmACAAZABhAHkAIABpAG4AIABVAFQAQwAgAG8AZgAgAGEAIABnAGkAdgBlAG4AIABKAHUAbABpAGEAbgAgAEQAYQB0AGUALgAgACAAIAAgACMAXABuACMAIABKAEQAQQBUAEUAXwBUAE8AXwBKAEQATgBfAEwATwBDAEEATAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAAbABvAGMAYQBsACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByACAAYQBuAGQAIAB0AGkAbQBlACAAbwBmACAAZABhAHkAIABvAGYAIABhACAAZwBpAHYAZQBuACAASgB1AGwAaQBhAG4AIABEAGEAdABlAC4AIAAgACAAIAAgACMAXABuACMAIABKAFUATABJAEEATgBfAEQAQQBUAEUAIAAgACAAIAAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAASgB1AGwAaQBhAG4AIABEAGEAdABlACAAbwBmACAAdABoAGUAIABwAHIAbwB2AGkAZABlAGQAIABjAGEAbABlAG4AZABhAHIAIABkAGEAdABlACAAYQBuAGQAIAB0AGkAbQBlACAAbwBmACAAZABhAHkALgAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABDAEEATABFAE4ARABBAFIAXwBGAFIATwBNAF8ASgBEAEEAVABFACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAAYwBhAGwAZQBuAGQAYQByACAAZABhAHQAZQAgAGEAbgBkACAAbABvAGMAYQBsACAAdABpAG0AZQAgAG8AZgAgAGQAYQB5ACAAZgBvAHIAIABhACAAZwBpAHYAZQBuACAASgB1AGwAaQBhAG4AIABEAGEAdABlACAAYQBuAGQAIAAgACAAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAdABpAG0AZQAgAHoAbwBuAGUAIABvAGYAZgBzAGUAdAAuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABUAEkATQBFAF8ARABFAEMASQBNAEEATABfAFQATwBfAEgATQBTACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAAMgA0ACAAaABvAHUAcgAgAHQAaQBtAGUAawBlAGUAcABpAG4AZwAgAHIAZQBwAHIAZQBzAGUAbgB0AGEAdABpAG8AbgAgAG8AZgAgAGEAIABkAGUAYwBpAG0AYQBsACAAdABpAG0AZQAgAHYAYQBsAHUAZQAuACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABIAE0AUwBfAFQATwBfAFQASQBNAEUAXwBEAEUAQwBJAE0AQQBMACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAGEAIABkAGUAYwBpAG0AYQBsACAAdABpAG0AZQAgAGEAcwAgAGEAIABmAHIAYQBjAHQAaQBvAG4AIABvAGYAIABhACAAZABhAHkAIABmAHIAbwBtACAAYQAgADIANAAgAGgAbwB1AHIAIAB0AGkAbQBlAGsAZQBlAHAAaQBuAGcAIAB2AGEAbAB1AGUAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAbwBmACAAdABpAG0AZQAuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuAFwAbgAjACAAQQBEAEQAXwBUAEkATQBFAFMAUABBAE4AIAAgACAAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAEoAdQBsAGkAYQBuACAARABhAHQAZQAgAG8AZgAgAHQAaABlACAAYQBkAGQAaQB0AGkAbwBuACAAbwBmACAAdABoAGUAIABwAHIAbwB2AGkAZABlAGQAIABjAGEAbABlAG4AZABhAHIAIABkAGEAdABlACAAYQBuAGQAIAB0AGkAbQBlACAAIAAjAFwAbgAjACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAG8AZgAgAGQAYQB5ACAAYQBuAGQAIABhACAAdABpAG0AZQBzAHAAYQBuACAAYwBvAG0AcABsAGkAYwBhAHQAaQBvAG4ALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAAUgBFAFMATwBMAFYARQBfAEQAQQBUAEUAIAAgACAAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIABhACAAYwBhAGwAZQBuAGQAYQByACAAZABhAHQAZQAgAGYAcgBvAG0AIABwAHIAbwB2AGkAZABlAGQAIABkAGUAYwBpAG0AYQBsACAAeQBlAGEAcgAsACAAbQBvAG4AdABoAHMALAAgAGQAYQB5AHMAIABhAG4AZAAgAHQAaQBtAGUALgAgACAAIAAgACAAIAAjAFwAbgAjACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARABFAEwAVABBACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AIAAjAFwAbgAjACAARABFAEwAVABBAF8ASQBOAFQARQBSAFYAQQBMACAAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHQAaQBtAGUAcwBwAGEAbgAgAGQAaQBmAGYAZQByAGUAbgBjAGUAIABiAGUAdAB3AGUAZQBuACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMAIABpAG4AIAB0AGgAZQAgAHMAcABlAGMAaQBmAGkAZQBkACAAdQBuAGkAdABzAC4AIAAgACAAIAAjAFwAbgAjACAARABFAEwAVABBAF8ASABPAFUAUgBTACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHQAaQBtAGUAcwBwAGEAbgAgAGQAaQBmAGYAZQByAGUAbgBjAGUAIABiAGUAdAB3AGUAZQBuACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMAIABpAG4AIABoAG8AdQByAHMALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARABFAEwAVABBAF8ATQBJAE4AVQBUAEUAUwAgACAAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHQAaQBtAGUAcwBwAGEAbgAgAGQAaQBmAGYAZQByAGUAbgBjAGUAIABiAGUAdAB3AGUAZQBuACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMAIABpAG4AIABtAGkAbgB1AHQAZQBzAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARABFAEwAVABBAF8AUwBFAEMATwBOAEQAUwAgACAAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHQAaQBtAGUAcwBwAGEAbgAgAGQAaQBmAGYAZQByAGUAbgBjAGUAIABiAGUAdAB3AGUAZQBuACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMAIABpAG4AIABzAGUAYwBvAG4AZABzAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARABFAEwAVABBAF8ASABPAFUAUgBfAE0ASQBOAF8AUwBFAEMAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHQAaQBtAGUAcwBwAGEAbgAgAGQAaQBmAGYAZQByAGUAbgBjAGUAIABiAGUAdAB3AGUAZQBuACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMAIABpAG4AIABoAG8AdQByAHMALAAgAG0AaQBuAHUAdABlAHMAIABhAG4AZAAgACAAIAAgACAAIAAjAFwAbgAjACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHMAZQBjAG8AbgBkAHMALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARABFAEwAVABBAF8ARABBAFkAUwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHQAaQBtAGUAcwBwAGEAbgAgAGQAaQBmAGYAZQByAGUAbgBjAGUAIABiAGUAdAB3AGUAZQBuACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMAIABpAG4AIABkAGEAeQBzAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARABFAEwAVABBAF8AVwBFAEUASwBTACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHQAaQBtAGUAcwBwAGEAbgAgAGQAaQBmAGYAZQByAGUAbgBjAGUAIABiAGUAdAB3AGUAZQBuACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMAIABpAG4AIAB3AGUAZQBrAHMALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARABFAEwAVABBAF8ATQBPAE4AVABIAFMAIAAgACAAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHQAaQBtAGUAcwBwAGEAbgAgAGQAaQBmAGYAZQByAGUAbgBjAGUAIABiAGUAdAB3AGUAZQBuACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMAIABpAG4AIABtAG8AbgB0AGgAcwAuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARABFAEwAVABBAF8AUQBVAEEAUgBUAEUAUgBTACAAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHQAaQBtAGUAcwBwAGEAbgAgAGQAaQBmAGYAZQByAGUAbgBjAGUAIABiAGUAdAB3AGUAZQBuACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMAIABpAG4AIABxAHUAYQByAHQAZQByAHMALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARABFAEwAVABBAF8AWQBFAEEAUgBTACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHQAaQBtAGUAcwBwAGEAbgAgAGQAaQBmAGYAZQByAGUAbgBjAGUAIABiAGUAdAB3AGUAZQBuACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMAIABpAG4AIAB5AGUAYQByAHMALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARABFAEwAVABBAF8AVwBFAEUASwBfAEQAQQBZAFMAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHQAaQBtAGUAcwBwAGEAbgAgAGQAaQBmAGYAZQByAGUAbgBjAGUAIABiAGUAdAB3AGUAZQBuACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMAIABpAG4AIAB3AGUAZQBrAHMAIABhAG4AZAAgAGQAYQB5AHMALgAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARABFAEwAVABBAF8AWQBFAEEAUgBfAFcARQBFAEsAXwBEAEEAWQBTACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHQAaQBtAGUAcwBwAGEAbgAgAGQAaQBmAGYAZQByAGUAbgBjAGUAIABiAGUAdAB3AGUAZQBuACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMAIABpAG4AIAB5AGUAYQByAHMALAAgAHcAZQBlAGsAcwAgAGEAbgBkACAAZABhAHkAcwAuACAAIAAjAFwAbgAjACAARABFAEwAVABBAF8ATQBPAE4AVABIAF8ARABBAFkAUwAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHQAaQBtAGUAcwBwAGEAbgAgAGQAaQBmAGYAZQByAGUAbgBjAGUAIABiAGUAdAB3AGUAZQBuACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMAIABpAG4AIABtAG8AbgB0AGgAcwAgAGEAbgBkACAAZABhAHkAcwAuACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARABFAEwAVABBAF8AUQBVAEEAUgBUAEUAUgBfAEQAQQBZAFMAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHQAaQBtAGUAcwBwAGEAbgAgAGQAaQBmAGYAZQByAGUAbgBjAGUAIABiAGUAdAB3AGUAZQBuACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMAIABpAG4AIABxAHUAYQByAHQAZQByAHMAIABhAG4AZAAgAGQAYQB5AHMALgAgACAAIAAgACAAIAAjAFwAbgAjACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARQBYAFQARQBOAFQAUwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AIAAjAFwAbgAjACAARQBYAFQARQBOAFQAXwBPAEYAXwBEAEEAWQBTACAAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAGkAbgBjAGwAdQBzAGkAdgBlACAAZQB4AHQAZQBuAHQAIABvAGYAIABkAGEAeQBzACAAcwBwAGEAbgBuAGUAZAAgAGIAeQAgAHQAdwBvACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARQBYAFQARQBOAFQAXwBPAEYAXwBXAEUARQBLAFMAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAGkAbgBjAGwAdQBzAGkAdgBlACAAZQB4AHQAZQBuAHQAIABvAGYAIAB3AGUAZQBrAHMAIABzAHAAYQBuAG4AZQBkACAAYgB5ACAAdAB3AG8AIABKAHUAbABpAGEAbgAgAEQAYQB0AGUAcwAuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARQBYAFQARQBOAFQAXwBPAEYAXwBNAE8ATgBUAEgAUwAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAGkAbgBjAGwAdQBzAGkAdgBlACAAZQB4AHQAZQBuAHQAIABvAGYAIABtAG8AbgB0AGgAcwAgAHMAcABhAG4AbgBlAGQAIABiAHkAIAB0AHcAbwAgAEoAdQBsAGkAYQBuACAARABhAHQAZQBzAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARQBYAFQARQBOAFQAXwBPAEYAXwBRAFUAQQBSAFQARQBSAFMAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAGkAbgBjAGwAdQBzAGkAdgBlACAAZQB4AHQAZQBuAHQAIABvAGYAIABxAHUAYQByAHQAZQByAHMAIABzAHAAYQBuAG4AZQBkACAAYgB5ACAAdAB3AG8AIABKAHUAbABpAGEAbgAgAEQAYQB0AGUAcwAuACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARQBYAFQARQBOAFQAXwBPAEYAXwBZAEUAQQBSAFMAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAGkAbgBjAGwAdQBzAGkAdgBlACAAZQB4AHQAZQBuAHQAIABvAGYAIAB5AGUAYQByAHMAIABzAHAAYQBuAG4AZQBkACAAYgB5ACAAdAB3AG8AIABKAHUAbABpAGEAbgAgAEQAYQB0AGUAcwAuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAAUABBAFIAUwBJAE4ARwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AIAAjAFwAbgAjACAAUABBAFIAUwBFAF8ASQBTAE8AXwBEAEEAVABFACAAIAAgACAAIAAgACAAIAAgAFAAYQByAHMAZQBzACAAYQBuACAASQBTAE8AIABmAG8AcgBtAGEAdAB0AGUAZAAgAGQAYQB0AGUAIABpAG4AdABvACAAcgBlAHMAcABlAGMAdABpAHYAZQAgAHAAYQByAHQAcwAgAG8AZgAgAHkAZQBhAHIALAAgAG0AbwBuAHQAaAAsACAAZABhAHkALAAgAHQAaQBtAGUAIABvAGYAIAAjAFwAbgAjACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAGQAYQB5ACAAYQBuAGQAIAB0AGkAbQBlACAAegBvAG4AZQAgAG8AZgBmAHMAZQB0ACAAaQBuACAAbQBpAG4AdQB0AGUAcwAgAGYAcgBvAG0AIABVAFQAQwAuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAAUABBAFIAUwBFAF8AVwBFAEUASwBEAEEAWQAgACAAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIABhACAAbgB1AG0AYgBlAHIAIAByAGUAcAByAGUAcwBlAG4AdABpAG4AZwAgAHQAaABlACAAZABhAHkAIABvAGYAIAB0AGgAZQAgAHcAZQBlAGsAIABmAHIAbwBtACAAYQAgAGcAaQB2AGUAbgAgAHQAZQB4AHQAIAB3AGUAZQBrAGQAYQB5ACAAIAAgACAAIAAjAFwAbgAjACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAG4AYQBtAGUALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAAUABBAFIAUwBFAF8ATQBPAE4AVABIACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIABhACAAbgB1AG0AYgBlAHIAIAByAGUAcAByAGUAcwBlAG4AdABpAG4AZwAgAHQAaABlACAAbQBvAG4AdABoACAAbwBmACAAeQBlAGEAcgAgAGYAcgBvAG0AIABhACAAZwBpAHYAZQBuACAAbQBvAG4AdABoACAAbgBhAG0AZQAuACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAAUABBAFIAUwBFAF8ATABJAFQARQBSAEEAUgBZAF8AWQBFAEEAUgAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIABhACAAbgB1AG0AYgBlAHIAIAByAGUAcAByAGUAcwBlAG4AdABpAG4AZwAgAHQAaABlACAAeQBlAGEAcgAgAHIAZQBsAGEAdABpAHYAZQAgAHQAbwAgAHQAaABlACAAYwBvAG0AbQBvAG4AIABlAHIAYQAgAGYAcgBvAG0AIABhACAAZwBpAHYAZQBuACAAIAAjAFwAbgAjACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAGwAaQB0AGUAcgBhAHIAeQAgAHkAZQBhAHIALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAAUABBAFIAUwBFAF8ATABJAFQARQBSAEEAUgBZAF8ARABBAFQARQAgACAAIAAgAFAAYQByAHMAZQBzACAAYQAgAGwAaQB0AGUAcgBhAHIAeQAgAGQAYQB0AGUAIABpAG4AdABvACAAcgBlAHMAcABlAGMAdABpAHYAZQAgAHAAYQByAHQAcwAgAG8AZgAgAHkAZQBhAHIALAAgAG0AbwBuAHQAaAAsACAAZABhAHkAIABhAG4AZAAgAHQAaQBtAGUAIABvAGYAIAAgACAAIAAjAFwAbgAjACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAGQAYQB5AC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAAUABBAFIAUwBFAF8AVQBTAF8ARABBAFQARQAgACAAIAAgACAAIAAgACAAIAAgAFAAYQByAHMAZQBzACAAYQAgAFUAUwAgAGYAbwByAG0AYQB0AHQAZQBkACAAZABhAHQAZQAgAGkAbgB0AG8AIAByAGUAcwBwAGUAYwB0AGkAdgBlACAAcABhAHIAdABzACAAbwBmACAAeQBlAGEAcgAsACAAbQBvAG4AdABoACwAIABkAGEAeQAgAGEAbgBkACAAdABpAG0AZQAgACAAIAAjAFwAbgAjACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAG8AZgAgAGQAYQB5AC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAAUABBAFIAUwBFAF8ATQBJAEwAXwBEAFQARwAgACAAIAAgACAAIAAgACAAIAAgAFAAYQByAHMAZQBzACAAYQAgAGQAYQB0AGUALQB0AGkAbQBlACAAZwByAG8AdQBwACAAaQBuACAAdABoAGUAIABmAG8AcgBtAGEAdAAgAHUAcwBlAGQAIABiAHkAIABVAFMAIABNAGkAbABpAHQAYQByAHkAIABtAGUAcwBzAGEAZwBlACAAdAByAGEAZgBmAGkAYwAsACAAIAAgACAAIAAjAFwAbgAjACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAGkAbgB0AG8AIAByAGUAcwBwAGUAYwB0AGkAdgBlACAAcABhAHIAdABzACAAbwBmACAAeQBlAGEAcgAsACAAbQBvAG4AdABoACwAIABkAGEAeQAsACAAdABpAG0AZQAgAG8AZgAgAGQAYQB5ACAAYQBuAGQAIAB0AGkAbQBlACAAegBvAG4AZQAgAG8AZgBmAHMAZQB0ACAAaQBuACAAIAAjAFwAbgAjACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAG0AaQBuAHUAdABlAHMAIABmAHIAbwBtACAAVQBUAEMALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAAVABFAFgAVAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AIAAjAFwAbgAjACAAVwBFAEUASwBEAEEAWQBfAE4AQQBNAEUAIAAgACAAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIABuAGEAbQBlACAAbwBmACAAYQBuACAASQBTAE8AIABkAGEAeQAgAG8AZgAgAHcAZQBlAGsAIABuAHUAbQBiAGUAcgAgAGEAcwAgAHQAZQB4AHQALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAATQBPAE4AVABIAF8ATgBBAE0ARQAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIABuAGEAbQBlACAAbwBmACAAbQBvAG4AdABoAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARgBPAFIATQBBAFQAXwBJAFMATwBfAEQAQQBUAEUAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIABhACAAZABhAHQAZQAgAGEAcwAgAHQAZQB4AHQAIABpAG4AIABJAFMATwAgAGYAbwByAG0AYQB0AC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARgBPAFIATQBBAFQAXwBMAEkAVABFAFIAQQBSAFkAXwBZAEUAQQBSACAAIAAgAFIAZQB0AHUAcgBuAHMAIABhACAAeQBlAGEAcgAgAGYAbwByAG0AYQB0AHQAZQBkACAAaQBuACAAbABpAHQAZQByAGEAcgB5ACAAcwB0AHkAbABlAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARgBPAFIATQBBAFQAXwBMAEkAVABFAFIAQQBSAFkAXwBEAEEAVABFACAAIAAgAFIAZQB0AHUAcgBuAHMAIABhACAAZABhAHQAZQAgAGYAbwByAG0AYQB0AHQAZQBkACAAaQBuACAAbABpAHQAZQByAGEAcgB5ACAAcwB0AHkAbABlAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARgBPAFIATQBBAFQAXwBVAFMAXwBEAEEAVABFACAAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIABhACAAZABhAHQAZQAgAGYAbwByAG0AYQB0AHQAZQBkACAAaQBuACAAdABoAGUAIABVAFMAIABzAHQAeQBsAGUALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARgBPAFIATQBBAFQAXwBNAEkATABfAEQAVABHACAAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIABhACAAZABhAHQAZQAtAHQAaQBtAGUAIABnAHIAbwB1AHAAIABmAG8AcgBtAGEAdAB0AGUAZAAgAGkAbgAgAFUAUwAgAE0AaQBsAGkAdABhAHIAeQAgAG0AZQBzAHMAYQBnAGUAIAB0AHIAYQBmAGYAaQBjACAAcwB0AHkAbABlAC4AIAAgACAAIAAgACAAIAAjAFwAbgAjACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAAQwBvAG4AdgBlAHIAcwBpAG8AbgBzACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AIAAjAFwAbgAjACAASQBTAE8ARABBAFQARQBfAFQATwBfAEoARABOAF8ATABPAEMAQQBMACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAEoAdQBsAGkAYQBuACAARABhAHkAIABOAHUAbQBiAGUAcgAgAGEAbgBkACAAbABvAGMAYQBsACAAdABpAG0AZQAgAGYAbwByACAAYQAgAGQAYQB0AGUAIABhAG4AZAAgAHQAaQBtAGUAIABwAHIAbwB2AGkAZABlAGQAIABpAG4AIAAgACAAIAAjAFwAbgAjACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkAUwBPACAAZgBvAHIAbQBhAHQALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAASQBTAE8ARABBAFQARQBfAFQATwBfAEoARABBAFQARQAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAEoAdQBsAGkAYQBuACAARABhAHQAZQAgAGYAbwByACAAYQAgAGQAYQB0AGUAIABhAG4AZAAgAHQAaQBtAGUAIABwAHIAbwB2AGkAZABlAGQAIABpAG4AIABJAFMATwAgAGYAbwByAG0AYQB0AC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAASQBTAE8ARABBAFQARQBfAFQATwBfAEUARABBAFQARQAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIABhAG4AIABFAHgAYwBlAGwAIABEAGEAdABlAC8AVABpAG0AZQAgAGYAbwByACAAYQAgAGQAYQB0AGUAIABhAG4AZAAgAHQAaQBtAGUAIABwAHIAbwB2AGkAZABlAGQAIABpAG4AIABJAFMATwAgAGYAbwByAG0AYQB0AC4AIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAASgBEAEEAVABFAF8AVABPAF8ASQBTAE8ARABBAFQARQAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIABJAFMATwAgAGYAbwByAG0AYQB0ACAAZABhAHQAZQAsACAAdABpAG0AZQAgAGEAbgBkACAAdABpAG0AZQAgAHoAbwBuAGUAIABvAGYAZgBzAGUAdAAgAGYAcgBvAG0AIABhACAAIABKAHUAbABpAGEAbgAgAEQAYQB0AGUALgAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAASgBEAE4AXwBMAE8AQwBBAEwAXwBUAE8AXwBJAFMATwBEAEEAVABFACAAIAAgAFIAZQB0AHUAcgBuAHMAIABJAFMATwAgAGYAbwByAG0AYQB0ACAAZABhAHQAZQAsACAAdABpAG0AZQAgAGEAbgBkACAAdABpAG0AZQAgAHoAbwBuAGUAIABvAGYAZgBzAGUAdAAgAGYAbwByACAAdABoAGUAIABwAHIAbwB2AGkAZABlAGQAIABKAHUAbABpAGEAbgAgAEQAYQB5ACAAIAAjAFwAbgAjACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAE4AdQBtAGIAZQByACAAYQBuAGQAIABsAG8AYwBhAGwAIAB0AGkAbQBlAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARQBEAEEAVABFAF8AVABPAF8ASQBTAE8ARABBAFQARQAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIABJAFMATwAgAGYAbwByAG0AYQB0ACAAZABhAHQAZQAsACAAdABpAG0AZQAgAGEAbgBkACAAdABpAG0AZQAgAHoAbwBuAGUAIABvAGYAZgBzAGUAdAAgAGYAcgBvAG0AIABhAG4AIABFAHgAYwBlAGwAIABEAGEAdABlAC8AVABpAG0AZQAuACAAIAAgACAAIAAjAFwAbgAjACAARQBEAEEAVABFAF8AVABPAF8ASgBEAEEAVABFACAAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAEoAdQBsAGkAYQBuACAARABhAHQAZQAgAGYAbwByACAAdABoAGUAIABwAHIAbwB2AGkAZABlAGQAIABFAHgAYwBlAGwAIABEAGEAdABlAC8AVABpAG0AZQAuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARQBEAEEAVABFAF8AVABPAF8ASgBEAE4AXwBMAE8AQwBBAEwAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAEoAdQBsAGkAYQBuACAARABhAHkAIABOAHUAbQBiAGUAcgAgAGEAbgBkACAAbABvAGMAYQBsACAAdABpAG0AZQAgAGYAbwByACAAdABoAGUAIABwAHIAbwB2AGkAZABlAGQAIABFAHgAYwBlAGwAIABEAGEAdABlAC8AVABpAG0AZQAuACAAIAAjAFwAbgAjACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAASgBEAE4AXwBMAE8AQwBBAEwAXwBUAE8AXwBFAEQAQQBUAEUAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIABhAG4AIABFAHgAYwBlAGwAIABEAGEAdABlAC8AVABpAG0AZQAgAGYAbwByACAAdABoAGUAIABwAHIAbwB2AGkAZABlAGQAIABKAHUAbABpAGEAbgAgAEQAYQB5ACAATgB1AG0AYgBlAHIAIABhAG4AZAAgAGwAbwBjAGEAbAAgAHQAaQBtAGUALgAgACAAIAAjAFwAbgAjACAASgBEAEEAVABFAF8AVABPAF8ARQBEAEEAVABFACAAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIABhAG4AIABFAHgAYwBlAGwAIABEAGEAdABlAC8AVABpAG0AZQAgAGYAbwByACAAdABoAGUAIABwAHIAbwB2AGkAZABlAGQAIABKAHUAbABpAGEAbgAgAEQAYQB0AGUALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAAVQBTAEQAQQBUAEUAXwBUAE8AXwBFAEQAQQBUAEUAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIABhAG4AIABFAHgAYwBlAGwAIABEAGEAdABlAC8AVABpAG0AZQAgAGYAbwByACAAdABoAGUAIABwAHIAbwB2AGkAZABlAGQAIABVAFMAIABmAG8AcgBtAGEAdAAgAGQAYQB0AGUAIABhAG4AZAAgAHQAaQBtAGUALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAARQBEAEEAVABFAF8AVABPAF8AVQBTAEQAQQBUAEUAIAAgACAAIAAgACAAIAAgAFIAZQB0AHUAcgBuAHMAIABhACAAVQBTACAAZgBvAHIAbQBhAHQAIABkAGEAdABlACAAYQBuAGQAIAB0AGkAbQBlACAAZgBvAHIAIAB0AGgAZQAgAHAAcgBvAHYAaQBkAGUAZAAgAEUAeABjAGUAbAAgAEQAYQB0AGUALwBUAGkAbQBlAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAKgAvAFwAbgBcAG4AXABuAFwAbgAvACoAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjAFwAbgAjACAATABPAEcASQBDAEEATAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAKgAvAFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEkAUwBfAEwARQBBAFAAXwBZAEUAQQBSAFwAbgBcAG4AVABlAHMAdABzACAAaQBmACAAYQAgAHkAZQBhAHIAIABpAG4AYwBsAHUAZABlAHMAIABhACAAbABlAGEAcAAgAGQAYQB5ACAAaQBuACAAdABoAGUAIABnAGkAdgBlAG4AIABjAGEAbABlAG4AZABhAHIALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAYgBvAG8AbABlAGEAbgAgAHwAIABuAHUAbABsACAAaQBmACAAZQBtAHAAdAB5AFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AWQBlAGEAcgBDAEUAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgAFkAZQBhAHIAIABpAG4AIABDAG8AbQBtAG8AbgAgAEUAcgBhAC4AIABOAG8AdABlACAAdABoAGEAdAAgADEAIABCAEMAIAA9ACAAMAAgAEMARQAsACAAMgAgAEIAQwAgAD0AIAAtADEAIABDAEUAXABuAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0AIAB8ACAAcwB3AGkAdABjAGgAIAAgAHwAIABDAGEAbABjAHUAbABhAHQAZQAgAGYAbwByACAAdABoAGUAIABKAHUAbABpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AIABEAGUAZgBhAHUAbAB0ACAAaQBzACAARwByAGUAZwBvAHIAaQBhAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBJAFMAXwBMAEUAQQBQAF8AWQBFAEEAUgAgAD0AIABMAEEATQBCAEQAQQAoAFkAZQBhAHIAQwBFACwAIABbAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACwAXABuACAAIAAgACAASQBGACgAWQBlAGEAcgBDAEUAIAA9ACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABZAGUAYQByAEMARQApACkALAAgAHsAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AGUAYQByAEMARQAsACAASQBOAFQAKABZAGUAYQByAEMARQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABOACgASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByACkAIAA9ACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGAFMAKABNAE8ARAAoAF8AeQBlAGEAcgBDAEUALAAgADQAMAAwACkAIAA9ACAAMAAsACAAVABSAFUARQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABNAE8ARAAoAF8AeQBlAGEAcgBDAEUALAAgADEAMAAwACkAIAA9ACAAMAAsACAARgBBAEwAUwBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALAAgAE0ATwBEACgAXwB5AGUAYQByAEMARQAsACAANAApACAAPQAgADAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABNAE8ARAAoAF8AeQBlAGEAcgBDAEUALAAgADQAKQAgAD0AIAAwAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEkAUwBfAFYAQQBMAEkARABfAEQAQQBUAEUAXABuAFwAbgBUAGUAcwB0AHMAIABpAGYAIABhACAAZABhAHQAZQAgAGkAcwAgAHYAYQBsAGkAZAAgAGYAbwByACAAdABoAGUAIABnAGkAdgBlAG4AIABjAGEAbABlAG4AZABhAHIALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAYgBvAG8AbABlAGEAbgAgAHwAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBZAGUAYQByAEMARQAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAAgACAAIAAgACAAIAAgACAAfAAgAFkAZQBhAHIAIABpAG4AIABDAG8AbQBtAG8AbgAgAEUAcgBhAC4AIABOAG8AdABlACAAdABoAGEAdAAgADEAIABCAEMAIAA9ACAAMAAgAEMARQAsACAAMgAgAEIAQwAgAD0AIAAtADEAIABDAEUAXABuAE0AbwBuAHQAaAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMQAuAC4AMQAyAF0AIAB8ACAATQBvAG4AdABoACAAbwBmACAAeQBlAGEAcgBcAG4ARABhAHkAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAWwAxAC4ALgAzADIAKQAgAHwAIABEAGEAeQAgAG8AZgAgAG0AbwBuAHQAaABcAG4AWwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAgAHwAIABzAHcAaQB0AGMAaAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABDAGEAbABjAHUAbABhAHQAZQAgAGYAbwByACAAdABoAGUAIABKAHUAbABpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AIABEAGUAZgBhAHUAbAB0ACAAaQBzACAARwByAGUAZwBvAHIAaQBhAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ASQBTAF8AVgBBAEwASQBEAF8ARABBAFQARQAgAD0AIABMAEEATQBCAEQAQQAoAFkAZQBhAHIAQwBFACwAIABNAG8AbgB0AGgALAAgAEQAYQB5ACwAIABbAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACwAXABuACAAIAAgACAASQBGACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABZAGUAYQByAEMARQApACkAIAArACAATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABNAG8AbgB0AGgAKQApACAAKwAgAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgARABhAHkAKQApACwAXABuACAAIAAgACAAIAAgACAAIABGAEEATABTAEUALAAgAC8ALwAgAGMAYQBuAG4AbwB0ACAAbwBtAG0AaQB0ACAAeQBlAGEAcgAsACAAbQBvAG4AdABoACAAbwByACAAZABhAHkAXABuACAAIAAgACAAIAAgACAAIABJAEYAKAAoAE0ATwBEACgAWQBlAGEAcgBDAEUALAAgADEAKQAgAD4AIAAwACkAIAArACAAKABNAE8ARAAoAE0AbwBuAHQAaAAsACAAMQApACAAPgAgADAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABGAEEATABTAEUALAAgAC8ALwAgAHkAZQBhAHIAIABhAG4AZAAgAG0AbwBuAHQAaAAgAGMAYQBuAG4AbwB0ACAAYgBlACAAZgByAGEAYwB0AGkAbwBuAGEAbABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAYQB5ACwAIABJAE4AVAAoAEQAYQB5ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAGQAYQB5ACAAPAAgADEALAAgAEYAQQBMAFMARQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQBzAEkAbgBNAG8AbgB0AGgALAAgAEQAQQBZAFMAXwBJAE4AXwBNAE8ATgBUAEgAKABNAG8AbgB0AGgALAAgAFkAZQBhAHIAQwBFACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABJAFMARQBSAFIATwBSACgAXwBkAGEAeQBzAEkAbgBNAG8AbgB0AGgAKQAsACAARgBBAEwAUwBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQAgADwAPQAgAF8AZABhAHkAcwBJAG4ATQBvAG4AdABoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ASQBTAF8AVgBBAEwASQBEAF8AVABJAE0ARQBcAG4AXABuAFQAZQBzAHQAcwAgAGkAZgAgAGEAIAB0AGkAbQBlACAAaQBzACAAdgBhAGwAaQBkACAAaQBuACAAdABoAGUAIAAyADQAIABoAG8AdQByACAAdABpAG0AZQBrAGUAZQBwAGkAbgBnACAAcwB5AHMAdABlAG0ALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAYgBvAG8AbABlAGEAbgAgAHwAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBIAG8AdQByACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAWwAwAC4ALgAyADQAKQAgAHwAIABGAHIAYQBjAHQAaQBvAG4AYQBsACAAYQBsAGwAbwB3AGUAZAAgAGkAZgAgAG0AaQBuAHUAdABlACAAYQBuAGQAIABzAGUAYwBvAG4AZAAgAGUAbQBwAHQAeQAuAFwAbgBNAGkAbgB1AHQAZQAgAHwAIABkAGUAYwBpAG0AYQBsACAAWwAwAC4ALgA2ADAAKQAgAHwAIABGAHIAYQBjAHQAaQBvAG4AYQBsACAAYQBsAGwAbwB3AGUAZAAgAGkAZgAgAHMAZQBjAG8AbgBkACAAZQBtAHAAdAB5AC4AXABuAFMAZQBjAG8AbgBkACAAfAAgAGQAZQBjAGkAbQBhAGwAIABbADAALgAuADYAMAApACAAfAAgAEYAcgBhAGMAdABpAG8AbgBhAGwAIABhAGwAbABvAHcAZQBkAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBcAG4ASQBTAF8AVgBBAEwASQBEAF8AVABJAE0ARQAgAD0AIABMAEEATQBCAEQAQQAoAEgAbwB1AHIALAAgAE0AaQBuAHUAdABlACwAIABTAGUAYwBvAG4AZAAsAFwAbgAgACAAIAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIABJAFMATgBVAE0AQgBFAFIAKABIAG8AdQByACkAIAAqACAASQBTAE4AVQBNAEIARQBSACgATQBpAG4AdQB0AGUAKQAgACoAIABJAFMATgBVAE0AQgBFAFIAKABTAGUAYwBvAG4AZAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKABNAE8ARAAoAEgAbwB1AHIALAAgADEAKQAgAD4AIAAwACkAIAArACAAKABNAE8ARAAoAE0AaQBuAHUAdABlACwAIAAxACkAIAA+ACAAMAApACwAIABGAEEATABTAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoAEgAbwB1AHIAIAA8ACAAMAApACAAKwAgACgASABvAHUAcgAgAD4AIAAyADMAKQAsACAARgBBAEwAUwBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKABNAGkAbgB1AHQAZQAgADwAIAAwACkAIAArACAAKABNAGkAbgB1AHQAZQAgAD4AIAA1ADkAKQAsACAARgBBAEwAUwBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKABTAGUAYwBvAG4AZAAgADwAIAAwACkAIAArACAAKABTAGUAYwBvAG4AZAAgAD4APQAgADYAMAApACwAIABGAEEATABTAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAIABUAFIAVQBFAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIABJAFMATgBVAE0AQgBFAFIAKABIAG8AdQByACkAIAAqACAASQBTAE4AVQBNAEIARQBSACgATQBpAG4AdQB0AGUAKQAgACoAIAAoAFMAZQBjAG8AbgBkACAAPQAgAFwAIgBcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAUwAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAE0ATwBEACgASABvAHUAcgAsACAAMQApACAAPgAgADAALAAgAEYAQQBMAFMARQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgASABvAHUAcgAgADwAIAAwACkAIAArACAAKABIAG8AdQByACAAPgAgADIAMwApACwAIABGAEEATABTAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoAE0AaQBuAHUAdABlACAAPAAgADAAKQAgACsAIAAoAE0AaQBuAHUAdABlACAAPgA9ACAANgAwACkALAAgAEYAQQBMAFMARQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALAAgAFQAUgBVAEUAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgAEkAUwBOAFUATQBCAEUAUgAoAEgAbwB1AHIAKQAgACoAIAAoAE0AaQBuAHUAdABlACAAPQAgAFwAIgBcACIAKQAgACoAIAAoAFMAZQBjAG8AbgBkACAAPQAgAFwAIgBcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoACgASABvAHUAcgAgAD4APQAgADAAKQAgACoAIAAoAEgAbwB1AHIAIAA8ACAAMgA0ACkAKQAgADwAPgAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACgASABvAHUAcgAgAD0AIABcACIAXAAiACkAIAAqACAASQBTAE4AVQBNAEIARQBSACgATQBpAG4AdQB0AGUAKQAgACoAIABJAFMATgBVAE0AQgBFAFIAKABTAGUAYwBvAG4AZAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATQBPAEQAKABNAGkAbgB1AHQAZQAsACAAMQApACAAPgAgADAALAAgAEYAQQBMAFMARQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgATQBpAG4AdQB0AGUAIAA8ACAAMAApACAAKwAgACgATQBpAG4AdQB0AGUAIAA+ACAANQA5ACkALAAgAEYAQQBMAFMARQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgAUwBlAGMAbwBuAGQAIAA8ACAAMAApACAAKwAgACgAUwBlAGMAbwBuAGQAIAA+AD0AIAA2ADAAKQAsACAARgBBAEwAUwBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABSAFUARQAsACAAVABSAFUARQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAKABIAG8AdQByACAAPQAgAFwAIgBcACIAKQAgACoAIABJAFMATgBVAE0AQgBFAFIAKABNAGkAbgB1AHQAZQApACAAKgAgACgAUwBlAGMAbwBuAGQAIAA9ACAAXAAiAFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgAKABNAGkAbgB1AHQAZQAgAD4APQAgADAAKQAgACoAIAAoAE0AaQBuAHUAdABlACAAPAAgADYAMAApACkAIAA8AD4AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAoAEgAbwB1AHIAIAA9ACAAXAAiAFwAIgApACAAKgAgACgATQBpAG4AdQB0AGUAIAA9ACAAXAAiAFwAIgApACAAKgAgAEkAUwBOAFUATQBCAEUAUgAoAFMAZQBjAG8AbgBkACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKAAoAFMAZQBjAG8AbgBkACAAPgA9ACAAMAApACAAKgAgACgAUwBlAGMAbwBuAGQAIAA8ACAANgAwACkAKQAgADwAPgAgADAALABcAG4AIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALAAgAEYAQQBMAFMARQBcAG4AIAAgACAAIAApAFwAbgApADsAIAAgACAAIAAgACAAIAAgAFwAbgBcAG4AXABuAFwAbgAvACoAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjAFwAbgAjACAAQwBBAEwARQBOAEQAQQBSACAARABBAFQARQBTACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAKgAvAFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFkARQBBAFIAXwBDAE8ATQBNAE8ATgBfAEUAUgBBAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAHkAZQBhAHIAIAB2AGEAbAB1AGUAIAByAGUAbABhAHQAaQB2AGUAIAB0AG8AIAB0AGgAZQAgAEMAbwBtAG0AbwBuACAARQByAGEALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIAAxACAAQwBFACAAPQAgADEALAAgADEAIABCAEMARQAgAD0AIAAwACwAIAAyACAAQgBDAEUAIAA9ACAALQAxAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AWQBlAGEAcgAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADEALgAuAF0AIAB8ACAAUABvAHMAaQB0AGkAdgBlACAAbgBvAG4ALQB6AGUAcgBvACAAaQBuAHQAZQBnAGUAcgAuAFwAbgBCAEMARQAgACAAIAB8ACAAcwB3AGkAdABjAGgAIAAgACAAIAAgACAAIAAgAHwAIABCAGUAZgBvAHIAZQAgAEMAbwBtAG0AbwBuACAARQByAGEALgBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4AWQBFAEEAUgBfAEMATwBNAE0ATwBOAF8ARQBSAEEAIAA9ACAATABBAE0AQgBEAEEAKABZAGUAYQByACwAIABCAEMARQAsAFwAbgAgACAAIAAgAEkARgAoAFkAZQBhAHIAIAA9ACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABZAGUAYQByACkAKQAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIALAAgAEkATgBUACgAWQBlAGEAcgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwB5AGUAYQByACAAPAAgADEALAAgAHsAIwBOAFUATQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAE4AKABCAEMARQApACwAIAAxACAALQAgAF8AeQBlAGEAcgAsACAAXwB5AGUAYQByACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEQAQQBZAFMAXwBJAE4AXwBZAEUAQQBSAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAG4AdQBtAGIAZQByACAAbwBmACAAZABhAHkAcwAgAGkAbgAgAHQAaABlACAAZwBpAHYAZQBuACAAeQBlAGEAcgAgAG8AZgAgAHQAaABlACAAcwBwAGUAYwBpAGYAaQBlAGQAIABjAGEAbABlAG4AZABhAHIALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMwA2ADUALAAzADYANgBdAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AWQBlAGEAcgBDAEUAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAFkAZQBhAHIAIABpAG4AIABDAG8AbQBtAG8AbgAgAEUAcgBhAC4AIABOAG8AdABlACAAdABoAGEAdAAgADEAIABCAEMAIAA9ACAAMAAgAEMARQAsACAAMgAgAEIAQwAgAD0AIAAtADEAIABDAEUAXABuAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0AIAB8ACAAcwB3AGkAdABjAGgAIAAgAHwAIABDAGEAbABjAHUAbABhAHQAZQAgAGYAbwByACAAdABoAGUAIABKAHUAbABpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AIABEAGUAZgBhAHUAbAB0ACAAaQBzACAARwByAGUAZwBvAHIAaQBhAG4AIABwAHIAbwBsAGUAcAB0AGkAYwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgAGMAYQBsAGUAbgBkAGEAcgAuAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBEAEEAWQBTAF8ASQBOAF8AWQBFAEEAUgAgAD0AIABMAEEATQBCAEQAQQAoAFkAZQBhAHIAQwBFACwAIABbAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACwAXABuACAAIAAgACAASQBGACgAWQBlAGEAcgBDAEUAIAA9ACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABZAGUAYQByAEMARQApACkALAAgAHsAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAEkAUwBfAEwARQBBAFAAXwBZAEUAQQBSACgAWQBlAGEAcgBDAEUALAAgAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAMwA2ADYALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAzADYANQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEQAQQBZAFMAXwBJAE4AXwBNAE8ATgBUAEgAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAbgB1AG0AYgBlAHIAIABvAGYAIABkAGEAeQBzACAAaQBuACAAdABoAGUAIABnAGkAdgBlAG4AIABtAG8AbgB0AGgAIABhAG4AZAAgAHkAZQBhAHIAIABvAGYAIAB0AGgAZQAgAHMAcABlAGMAaQBmAGkAZQBkACAAYwBhAGwAZQBuAGQAYQByAC4AXABuAFwAbgBPAHUAdABwAHUAdABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADEALgAuADMAMQBdAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ATQBvAG4AdABoACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAWwAxAC4ALgAxADIAXQAgAHwAIABNAG8AbgB0AGgAIABvAGYAIAB5AGUAYQByAFwAbgBbAFkAZQBhAHIAQwBFAF0AIAAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAAgACAAIAAgACAAIAAgACAAfAAgAFkAZQBhAHIAIABpAG4AIABDAG8AbQBtAG8AbgAgAEUAcgBhAC4AIABOAG8AdABlACAAdABoAGEAdAAgADEAIABCAEMAIAA9ACAAMAAgAEMARQAsACAAMgAgAEIAQwAgAD0AIAAtADEAIABDAEUAXABuAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0AIAB8ACAAcwB3AGkAdABjAGgAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAQwBhAGwAYwB1AGwAYQB0AGUAIABmAG8AcgAgAHQAaABlACAASgB1AGwAaQBhAG4AIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuACAARABlAGYAYQB1AGwAdAAgAGkAcwAgAEcAcgBlAGcAbwByAGkAYQBuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEQAQQBZAFMAXwBJAE4AXwBNAE8ATgBUAEgAIAA9ACAATABBAE0AQgBEAEEAKABNAG8AbgB0AGgALAAgAFsAWQBlAGEAcgBDAEUAXQAsACAAWwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAsAFwAbgAgACAAIAAgAEkARgAoAE0AbwBuAHQAaAA9AFwAIgBcACIALAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgATQBvAG4AdABoACkAKQAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AbwBuAHQAaAAsACAASQBOAFQAKABNAG8AbgB0AGgAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AbwBuAHQAaAAgADwAIAAxACwAIAB7ACMATgBVAE0AIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AbwBuAHQAaAAgAD4AIAAxADIALAAgAHsAIwBOAFUATQAhAH0ALABcAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABGAGUAYgByAHUAYQByAHkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AbwBuAHQAaAAgAD0AIAAyACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBsAGUAYQBwAEQAYQB5ACwAIABJAEYAKABJAFMATgBVAE0AQgBFAFIAKABZAGUAYQByAEMARQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABOACgASQBTAF8ATABFAEEAUABfAFkARQBBAFIAKABZAGUAYQByAEMARQAsACAASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAMABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAMgA4ACAAKwAgAF8AbABlAGEAcABEAGEAeQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAEoAYQBuACwAIABNAGEAcgAsACAAQQBwAHIALAAgAE0AYQB5ACwAIABKAHUAbgAsACAASgB1AGwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AbwBuAHQAaAAgADwAPQAgADcALAAgADMAMAAgACsAIABNAE8ARAAoAF8AbQBvAG4AdABoACwAIAAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAQQB1AGcALAAgAFMAZQBwACwAIABPAGMAdAAsACAATgBvAHYALAAgAEQAZQBjAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABSAFUARQAsACAAMwAxACAALQAgAE0ATwBEACgAXwBtAG8AbgB0AGgALAAgADIAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEoAVQBMAEkAQQBOAF8ARABBAFkAXwBOAFUATQBCAEUAUgBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAEoAdQBsAGkAYQBuACAARABhAHkAIABOAHUAbQBiAGUAcgAgAG8AZgAgAHQAaABlACAAcAByAG8AdgBpAGQAZQBkACAAZABhAHQAZQAgAGkAbgAgAHQAaABlACAAcwBwAGUAYwBpAGYAaQBlAGQAIABjAGEAbABlAG4AZABhAHIALgBcAG4ATgBvAHQAZQAgAHQAaABlACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByACAAaQBzACAAYQBuACAAaQBuAHQAZQBnAGUAcgAgAHQAeQBwAGUAIABhAG4AZAAgAGkAcwAgAGEAbgAgAG8AcgBkAGkAbgBhAGwAIABkAGEAeQAgAG4AdQBtAGIAZQByACAAcgBlAGYAZQByAGUAbgBjAGUAZAAgAGYAcgBvAG0AIABKAGEAbgB1AGEAcgB5ACAAMQAsAFwAbgA0ADcAMQAzACAAQgBDACAAaQBuACAAdABoAGUAIABwAHIAbwBsAGUAcAB0AGkAYwAgAEoAdQBsAGkAYQBuACAAYwBhAGwAZQBuAGQAYQByAC4AIABJAHQAIABkAG8AZQBzACAAbgBvAHQAIABpAG4AYwBsAHUAZABlACAAYQBuAHkAIAB2AGEAbAB1AGUAIABmAG8AcgAgAHQAaQBtAGUAIABvAGYAIABkAGEAeQAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAEoAdQBsAGkAYQBuACAARABhAHkAIABOAHUAbQBiAGUAcgBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFkAZQBhAHIAQwBFACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgACAAIAAgACAAIAAgACAAIAB8ACAAWQBlAGEAcgAgAGkAbgAgAEMAbwBtAG0AbwBuACAARQByAGEALgAgAE4AbwB0AGUAIAB0AGgAYQB0ACAAMQAgAEIAQwAgAD0AIAAwACAAQwBFACwAIAAyACAAQgBDACAAPQAgAC0AMQAgAEMARQBcAG4ATQBvAG4AdABoACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAWwAxAC4ALgAxADIAXQAgAHwAIABNAG8AbgB0AGgAIABvAGYAIAB5AGUAYQByAFwAbgBEAGEAeQAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIABbADEALgAuADMAMgApACAAfAAgAEQAYQB5ACAAbwBmACAAbQBvAG4AdABoAFwAbgBbAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACAAfAAgAHMAdwBpAHQAYwBoACAAIAAgACAAIAAgACAAIAAgACAAfAAgAEMAYQBsAGMAdQBsAGEAdABlACAAZgBvAHIAIAB0AGgAZQAgAEoAdQBsAGkAYQBuACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgAgAEQAZQBmAGEAdQBsAHQAIABpAHMAIABHAHIAZQBnAG8AcgBpAGEAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABwAHIAbwBsAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ASgBVAEwASQBBAE4AXwBEAEEAWQBfAE4AVQBNAEIARQBSACAAPQAgAEwAQQBNAEIARABBACgAWQBlAGEAcgBDAEUALAAgAE0AbwBuAHQAaAAsACAARABhAHkALAAgAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0ALABcAG4AIAAgACAAIABJAEYAKAAoAFkAZQBhAHIAQwBFACAAPQAgAFwAIgBcACIAKQAgACoAIAAoAE0AbwBuAHQAaAAgAD0AIABcACIAXAAiACkAIAAqACAAKABEAGEAeQAgAD0AIABcACIAXAAiACkALAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAF8AVgBBAEwASQBEAF8ARABBAFQARQAoAFkAZQBhAHIAQwBFACwAIABNAG8AbgB0AGgALAAgAEQAYQB5ACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQApACwAIAB7ACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkALAAgAEkATgBUACgARABhAHkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZwByAGUAZwBvAHIAaQBhAG4ALAAgAE4AKABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAgAD0AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBZAEUAQQBSADQAOAAwADEAQgBDAEUALAAgAC0ANAA4ADAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8ARwA0ADgAMAAxAEIAQwBFAF8ASgBEACwAIAAtADMAMgAwADQANQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8ASgA0ADgAMAAxAEIAQwBFAF8ASgBEACwAIAAtADMAMgAwADgAMwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8ARABhAHkAcwBJAG4ANQBNAG8AbgB0AGgAcwBGAHIAbwBtAE0AYQByAGMAaAAsACAAMQA1ADMALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGEALAAgAEkATgBUACgAKAAxADQAIAAtACAATQBvAG4AdABoACkAIAAvACAAMQAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkALAAgACgAWQBlAGEAcgBDAEUAIAAtACAAXwBZAEUAQQBSADQAOAAwADEAQgBDAEUAIAAtACAAXwBhACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0ALAAgACgATQBvAG4AdABoACAAKwAgADEAMgAgACoAIABfAGEAIAAtACAAMwApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB4ACwAIAAzADYANQAgACoAIABfAHkAIAArACAASQBOAFQAKABfAHkAIAAvACAANAApACAAKwAgAEkATgBUACgAKABfAEQAYQB5AHMASQBuADUATQBvAG4AdABoAHMARgByAG8AbQBNAGEAcgBjAGgAIAAqACAAXwBtACAAKwAgADIAKQAgAC8AIAA1ACkAIAArACAAXwBkAGEAeQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBnAHIAZQBnAG8AcgBpAGEAbgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB4ACAAKwAgAF8ARwA0ADgAMAAxAEIAQwBFAF8ASgBEACAALQAgAEkATgBUACgAXwB5ACAALwAgADEAMAAwACkAIAArACAASQBOAFQAKABfAHkAIAAvACAANAAwADAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB4ACAAKwAgAF8ASgA0ADgAMAAxAEIAQwBFAF8ASgBEAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBKAEQATgBfAFQATwBfAEMAQQBMAEUATgBEAEEAUgBfAEQAQQBUAEUAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIABkAGEAdABlACAAZgByAG8AbQAgAHQAaABlACAAZwBpAHYAZQBuACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByACAAaQBuACAAdABoAGUAIABzAHAAZQBjAGkAZgBpAGUAZAAgAGMAYQBsAGUAbgBkAGEAcgAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABpAG4AdABlAGcAZQByACAAIAAgACAAIAAgACAAIAAgAHwAIABZAGUAYQByACAAaQBuACAAQwBvAG0AbQBvAG4AIABFAHIAYQAuACAATgBvAHQAZQAgAHQAaABhAHQAIAAxACAAQgBDACAAPQAgADAAIABDAEUALAAgADIAIABCAEMAIAA9ACAALQAxACAAQwBFAFwAbgAgADIAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMQAuAC4AMQAyAF0AIAB8ACAATQBvAG4AdABoAFwAbgAgADMAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMQAuAC4AMwAxAF0AIAB8ACAARABhAHkAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBKAEQATgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByACAAZgBvAHIAIAB0AGgAZQAgAGMAYQBsAGUAbgBkAGEAcgAgAGQAYQB5AFwAbgBbAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACAAfAAgAHMAdwBpAHQAYwBoACAAIAB8ACAAQwBhAGwAYwB1AGwAYQB0AGUAIABmAG8AcgAgAHQAaABlACAASgB1AGwAaQBhAG4AIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuACAARABlAGYAYQB1AGwAdAAgAGkAcwAgAEcAcgBlAGcAbwByAGkAYQBuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ASgBEAE4AXwBUAE8AXwBDAEEATABFAE4ARABBAFIAXwBEAEEAVABFACAAPQAgAEwAQQBNAEIARABBACgASgBEAE4ALAAgAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0ALABcAG4AIAAgACAAIABJAEYAKABKAEQATgAgAD0AIABcACIAXAAiACwAIAB7AFwAIgBcACIALAAgAFwAIgBcACIALAAgAFwAIgBcACIAfQAsAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABKAEQATgApACkALAAgAHsAIwBWAEEATABVAEUAIQAsACAAIwBWAEEATABVAEUAIQAsACAAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBqAGQAbgAsACAASQBOAFQAKABKAEQATgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBnAHIAZQBnAG8AcgBpAGEAbgAsACAATgAoAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgApACAAPQAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAFkARQBBAFIANAA4ADAAMQBCAEMARQAsACAALQA0ADgAMAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBEAGEAeQBzAEkAbgA0AFkAZQBhAHIALAAgADEANAA2ADEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAEQAYQB5AHMASQBuAFkAZQBhAHIALAAgADMANgA1ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBNAG8AbgB0AGgAQwBvAHIAcgBlAGMAdABpAG8AbgBEAGEAeQBzACwAIAAzADAAOAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8ARABhAHkAcwBJAG4ANABNAG8AbgB0AGgAcwAsACAAMQAyADIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAEQAYQB5AHMASQBuADUATQBvAG4AdABoAHMARgByAG8AbQBNAGEAcgBjAGgALAAgADEANQAzACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBnAHIAZQBnAG8AcgBpAGEAbgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBHADQAOAAwADEAQgBDAEUAXwBKAEQAMAAsACAALQAzADIAMAA0ADUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBHAHIAZQBnAEQAYQB5AHMASQBuADQAMAAwAFkAZQBhAHIALAAgADEANAA2ADAAOQA3ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8ARwByAGUAZwBEAGEAeQBzAEkAbgAxADAAMABZAGUAYQByACwAIAAzADYANQAyADQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQBzADAALAAgAF8AagBkAG4AIAAtACAAXwBHADQAOAAwADEAQgBDAEUAXwBKAEQAMAAgAC0AIAAxACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcQB1AGEAZABDAGUAbgB0ACwAIABJAE4AVAAoAF8AZABhAHkAcwAwACAALwAgAF8ARwByAGUAZwBEAGEAeQBzAEkAbgA0ADAAMABZAGUAYQByACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQBzADEALAAgAF8AZABhAHkAcwAwACAALQAgAF8AcQB1AGEAZABDAGUAbgB0ACAAKgAgAF8ARwByAGUAZwBEAGEAeQBzAEkAbgA0ADAAMABZAGUAYQByACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcgBlAG0AQwBlAG4AdAAsACAASQBOAFQAKAAoAEkATgBUACgAXwBkAGEAeQBzADEAIAAvACAAXwBHAHIAZQBnAEQAYQB5AHMASQBuADEAMAAwAFkAZQBhAHIAKQAgACsAIAAxACkAIAAqACAAMAAuADcANQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkAcwAyACwAIABfAGQAYQB5AHMAMQAgAC0AIABfAHIAZQBtAEMAZQBuAHQAIAAqACAAXwBHAHIAZQBnAEQAYQB5AHMASQBuADEAMAAwAFkAZQBhAHIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBxAHUAYQBkAFkAcgAsACAASQBOAFQAKABfAGQAYQB5AHMAMgAgAC8AIABfAEQAYQB5AHMASQBuADQAWQBlAGEAcgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkAcwAzACwAIABfAGQAYQB5AHMAMgAgAC0AIABfAHEAdQBhAGQAWQByACAAKgAgAF8ARABhAHkAcwBJAG4ANABZAGUAYQByACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcgBlAG0AWQByACwAIABJAE4AVAAoACgASQBOAFQAKABfAGQAYQB5AHMAMwAgAC8AIABfAEQAYQB5AHMASQBuAFkAZQBhAHIAKQAgACsAIAAxACkAIAAqACAAMAAuADcANQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkAcwA0ACwAIABfAGQAYQB5AHMAMwAgAC0AIABfAHIAZQBtAFkAcgAgACoAIABfAEQAYQB5AHMASQBuAFkAZQBhAHIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5ACwAIABfAHEAdQBhAGQAQwBlAG4AdAAgACoAIAA0ADAAMAAgACsAIABfAHIAZQBtAEMAZQBuAHQAIAAqACAAMQAwADAAIAArACAAXwBxAHUAYQBkAFkAcgAgACoAIAA0ACAAKwAgAF8AcgBlAG0AWQByACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbQAsACAASQBOAFQAKAAoAF8AZABhAHkAcwA0ACAAKgAgADUAIAArACAAXwBNAG8AbgB0AGgAQwBvAHIAcgBlAGMAdABpAG8AbgBEAGEAeQBzACkAIAAvACAAXwBEAGEAeQBzAEkAbgA1AE0AbwBuAHQAaABzAEYAcgBvAG0ATQBhAHIAYwBoACkAIAAtACAAMgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAYQB5ACwAIABfAGQAYQB5AHMANAAgAC0AIABJAE4AVAAoACgAXwBtACAAKwAgADQAKQAgACoAIABfAEQAYQB5AHMASQBuADUATQBvAG4AdABoAHMARgByAG8AbQBNAGEAcgBjAGgAIAAvACAANQApACAAKwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAEQAYQB5AHMASQBuADQATQBvAG4AdABoAHMAIAArACAAMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIALAAgAF8AWQBFAEEAUgA0ADgAMAAxAEIAQwBFACAAKwAgAF8AeQAgACsAIABJAE4AVAAoACgAXwBtACAAKwAgADIAKQAgAC8AIAAxADIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AbwBuAHQAaAAsACAATQBPAEQAKABfAG0AIAArACAAMgAsACAAMQAyACkAIAArACAAMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAF8AeQBlAGEAcgAsACAAXwBtAG8AbgB0AGgALAAgAF8AZABhAHkAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8ASgA0ADgAMAAxAEIAQwBFAF8ASgBEADAALAAgAC0AMwAyADAAOAAzACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkAcwAwACwAIABfAGoAZABuACAALQAgAF8ASgA0ADgAMAAxAEIAQwBFAF8ASgBEADAAIAAtACAAMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHEAdQBhAGQAWQByACwAIABJAE4AVAAoAF8AZABhAHkAcwAwACAALwAgAF8ARABhAHkAcwBJAG4ANABZAGUAYQByACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQBzADEALAAgAF8AZABhAHkAcwAwACAALQAgAF8AcQB1AGEAZABZAHIAIAAqACAAXwBEAGEAeQBzAEkAbgA0AFkAZQBhAHIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwByAGUAbQBZAHIALAAgAEkATgBUACgAKABJAE4AVAAoAF8AZABhAHkAcwAxACAALwAgAF8ARABhAHkAcwBJAG4AWQBlAGEAcgApACAAKwAgADEAKQAgACoAIAAwAC4ANwA1ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQBzADIALAAgAF8AZABhAHkAcwAxACAALQAgAF8AcgBlAG0AWQByACAAKgAgAF8ARABhAHkAcwBJAG4AWQBlAGEAcgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkALAAgAF8AcQB1AGEAZABZAHIAIAAqACAANAAgACsAIABfAHIAZQBtAFkAcgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0ALAAgAEkATgBUACgAKABfAGQAYQB5AHMAMgAgACoAIAA1ACAAKwAgAF8ATQBvAG4AdABoAEMAbwByAHIAZQBjAHQAaQBvAG4ARABhAHkAcwApACAALwAgAF8ARABhAHkAcwBJAG4ANQBNAG8AbgB0AGgAcwBGAHIAbwBtAE0AYQByAGMAaAApACAALQAgADIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQAsACAAXwBkAGEAeQBzADIAIAAtACAASQBOAFQAKAAoAF8AbQAgACsAIAA0ACkAIAAqACAAXwBEAGEAeQBzAEkAbgA1AE0AbwBuAHQAaABzAEYAcgBvAG0ATQBhAHIAYwBoACAALwAgADUAKQAgACsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBEAGEAeQBzAEkAbgA0AE0AbwBuAHQAaABzACAAKwAgADEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AGUAYQByACwAIABfAFkARQBBAFIANAA4ADAAMQBCAEMARQAgACsAIABfAHkAIAArACAASQBOAFQAKAAoAF8AbQAgACsAIAAyACkAIAAvACAAMQAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBtAG8AbgB0AGgALAAgAE0ATwBEACgAXwBtACAAKwAgADIALAAgADEAMgApACAAKwAgADEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABfAHkAZQBhAHIALAAgAF8AbQBvAG4AdABoACwAIABfAGQAYQB5ACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBKAEQATgBfAFQATwBfAE8AUgBEAEkATgBBAEwAXwBEAEEAVABFAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAHQAaABlACAAeQBlAGEAcgAsACAAbwByAGQAaQBuAGEAbAAgAGQAYQB5ACAAbwBmACAAeQBlAGEAcgAgAGEAbgBkACAAZABhAHkAcwAgAGkAbgAgAHQAaABlACAAeQBlAGEAcgAgAGYAcgBvAG0AIAB0AGgAZQAgAGcAaQB2AGUAbgAgAEoAdQBsAGkAYQBuACAARABhAHkAIABOAHUAbQBiAGUAcgAgAGkAbgAgAHQAaABlACAAcwBwAGUAYwBpAGYAaQBlAGQAXABuAGMAYQBsAGUAbgBkAGEAcgAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABpAG4AdABlAGcAZQByACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAWQBlAGEAcgAgAGkAbgAgAEMAbwBtAG0AbwBuACAARQByAGEALgAgAE4AbwB0AGUAIAB0AGgAYQB0ACAAMQAgAEIAQwAgAD0AIAAwACAAQwBFACwAIAAyACAAQgBDACAAPQAgAC0AMQAgAEMARQBcAG4AIAAyACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADEALgAuADMANgA2AF0AIAAgAHwAIABPAHIAZABpAG4AYQBsACAAZABhAHkAXABuACAAMwAgAHwAIABpAG4AdABlAGcAZQByACAAWwAzADYANQAsADMANgA2AF0AIAB8ACAARABhAHkAcwAgAGkAbgAgAHkAZQBhAHIAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBKAEQATgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByACAAZgBvAHIAIAB0AGgAZQAgAGMAYQBsAGUAbgBkAGEAcgAgAGQAYQB5AFwAbgBbAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACAAfAAgAHMAdwBpAHQAYwBoACAAIAB8ACAAQwBhAGwAYwB1AGwAYQB0AGUAIABmAG8AcgAgAHQAaABlACAASgB1AGwAaQBhAG4AIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuACAARABlAGYAYQB1AGwAdAAgAGkAcwAgAEcAcgBlAGcAbwByAGkAYQBuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ASgBEAE4AXwBUAE8AXwBPAFIARABJAE4AQQBMAF8ARABBAFQARQAgAD0AIABMAEEATQBCAEQAQQAoAEoARABOACwAIABbAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACwAXABuACAAIAAgACAASQBGACgASgBEAE4AIAA9ACAAXAAiAFwAIgAsACAAewBcACIAXAAiACwAIABcACIAXAAiACwAIABcACIAXAAiAH0ALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgASgBEAE4AKQApACwAIAB7ACMAVgBBAEwAVQBFACEALAAgACMAVgBBAEwAVQBFACEALAAgACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AagBkAG4ALAAgAEkATgBUACgASgBEAE4AKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHQAZQAsACAASgBEAE4AXwBUAE8AXwBDAEEATABFAE4ARABBAFIAXwBEAEEAVABFACgAXwBqAGQAbgAsACAASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIAQwBFACwAIABJAE4ARABFAFgAKABfAGQAYQB0AGUALAAgADEALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AagBkAG4AWQBlAGEAcgBTAHQAYQByAHQALAAgAEoAVQBMAEkAQQBOAF8ARABBAFkAXwBOAFUATQBCAEUAUgAoAF8AeQBlAGEAcgBDAEUALAAgADEALAAgADEALAAgAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBvAHIAZABpAG4AYQBsAEQAYQB5ACwAIABfAGoAZABuACAALQAgAF8AagBkAG4AWQBlAGEAcgBTAHQAYQByAHQAIAArACAAMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkAcwBJAG4AWQBlAGEAcgAsACAARABBAFkAUwBfAEkATgBfAFkARQBBAFIAKABfAHkAZQBhAHIAQwBFACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIAQwBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG8AcgBkAGkAbgBhAGwARABhAHkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkAcwBJAG4AWQBlAGEAcgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBPAFIARABJAE4AQQBMAF8ARABBAFQARQBfAFQATwBfAEoARABOAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAHQAaABlACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByACAAbwBmACAAdABoAGUAIABwAHIAbwB2AGkAZABlAGQAIABvAHIAZABpAG4AYQBsACAAZABhAHQAZQAgAGkAbgAgAHQAaABlACAAcwBwAGUAYwBpAGYAaQBlAGQAIABjAGEAbABlAG4AZABhAHIALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIABKAHUAbABpAGEAbgAgAEQAYQB5ACAATgB1AG0AYgBlAHIAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBZAGUAYQByAEMARQAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAWQBlAGEAcgAgAGkAbgAgAEMAbwBtAG0AbwBuACAARQByAGEALgAgAE4AbwB0AGUAIAB0AGgAYQB0ACAAMQAgAEIAQwAgAD0AIAAwACAAQwBFACwAIAAyACAAQgBDACAAPQAgAC0AMQAgAEMARQBcAG4ATwByAGQAaQBuAGEAbABEAGEAeQAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAWwAxAC4ALgAzADYANgApACAAfAAgAEQAYQB5ACAAbwBmACAAeQBlAGEAcgAsACAAYwBhAHIAcgBpAGUAcwAgAGkAZgAgAHIAYQBuAGcAZQAgAGUAeABjAGUAZQBkAGUAZABcAG4AWwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAgAHwAIABzAHcAaQB0AGMAaAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAEMAYQBsAGMAdQBsAGEAdABlACAAZgBvAHIAIAB0AGgAZQAgAEoAdQBsAGkAYQBuACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgAgAEQAZQBmAGEAdQBsAHQAIABpAHMAIABHAHIAZQBnAG8AcgBpAGEAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAE8AUgBEAEkATgBBAEwAXwBEAEEAVABFAF8AVABPAF8ASgBEAE4AIAA9ACAATABBAE0AQgBEAEEAKABZAGUAYQByAEMARQAsACAATwByAGQAaQBuAGEAbABEAGEAeQAsACAAWwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAsAFwAbgAgACAAIAAgAEkARgAoACgAWQBlAGEAcgBDAEUAIAA9ACAAXAAiAFwAIgApACAAKgAgACgATwByAGQAaQBuAGEAbABEAGEAeQAgAD0AIABcACIAXAAiACkALAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgAWQBlAGEAcgBDAEUAKQApACAAKwAgAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgATwByAGQAaQBuAGEAbABEAGEAeQApACkALAAgAHsAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBvAHIAZABpAG4AYQBsAEQAYQB5ACwAIABJAE4AVAAoAE8AcgBkAGkAbgBhAGwARABhAHkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AagBkAG4AWQBlAGEAcgBTAHQAYQByAHQALAAgAEoAVQBMAEkAQQBOAF8ARABBAFkAXwBOAFUATQBCAEUAUgAoAFkAZQBhAHIAQwBFACwAIAAxACwAIAAxACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AagBkAG4AWQBlAGEAcgBTAHQAYQByAHQAIAArACAAXwBvAHIAZABpAG4AYQBsAEQAYQB5ACAALQAgADEAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBHAFIARQBHAE8AUgBJAEEATgBfAFQATwBfAEoAVQBMAEkAQQBOAFwAbgBcAG4AVAByAGEAbgBzAGwAYQB0AGUAcwAgAGEAIABkAGEAdABlACAAaQBuACAAdABoAGUAIABHAHIAZQBnAG8AcgBpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByACAAdABvACAAdABoAGUAIABKAHUAbABpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AXABuAFwAbgBPAHUAdABwAHUAdABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAGkAbgB0AGUAZwBlAHIAIAAgACAAIAAgACAAIAAgACAAfAAgAFkAZQBhAHIAIABpAG4AIABDAG8AbQBtAG8AbgAgAEUAcgBhAC4AIABOAG8AdABlACAAdABoAGEAdAAgADEAIABCAEMAIAA9ACAAMAAgAEMARQAsACAAMgAgAEIAQwAgAD0AIAAtADEAIABDAEUAXABuACAAMgAgAHwAIABpAG4AdABlAGcAZQByACAAWwAxAC4ALgAxADIAXQAgAHwAIABNAG8AbgB0AGgAXABuACAAMwAgAHwAIABpAG4AdABlAGcAZQByACAAWwAxAC4ALgAzADEAXQAgAHwAIABEAGEAeQBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFkAZQBhAHIAQwBFACAAfAAgAGkAbgB0AGUAZwBlAHIAIAAgACAAIAAgACAAIAAgACAAfAAgAFkAZQBhAHIAIABpAG4AIABDAG8AbQBtAG8AbgAgAEUAcgBhAC4AIABOAG8AdABlACAAdABoAGEAdAAgADEAIABCAEMAIAA9ACAAMAAgAEMARQAsACAAMgAgAEIAQwAgAD0AIAAtADEAIABDAEUAXABuAE0AbwBuAHQAaAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADEALgAuADEAMgBdACAAfAAgAFwAbgBEAGEAeQAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAWwAxAC4ALgAzADIAKQAgAHwAIABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ARwBSAEUARwBPAFIASQBBAE4AXwBUAE8AXwBKAFUATABJAEEATgAgAD0AIABMAEEATQBCAEQAQQAoAFkAZQBhAHIAQwBFACwAIABNAG8AbgB0AGgALAAgAEQAYQB5ACwAXABuACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgAF8ASgBEAE4ALAAgAEoAVQBMAEkAQQBOAF8ARABBAFkAXwBOAFUATQBCAEUAUgAoAFkAZQBhAHIAQwBFACwAIABNAG8AbgB0AGgALAAgAEQAYQB5ACwAIAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgBTACgASQBTAEUAUgBSAE8AUgAoAF8ASgBEAE4AKQAsACAAewAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBKAEQATgAgAD0AIABcACIAXAAiACwAIAB7AFwAIgBcACIALAAgAFwAIgBcACIALAAgAFwAIgBcACIAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAIABKAEQATgBfAFQATwBfAEMAQQBMAEUATgBEAEEAUgBfAEQAQQBUAEUAKABfAEoARABOACwAIAAxACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBKAFUATABJAEEATgBfAFQATwBfAEcAUgBFAEcATwBSAEkAQQBOAFwAbgBcAG4AVAByAGEAbgBzAGwAYQB0AGUAcwAgAGEAIABkAGEAdABlACAAaQBuACAAdABoAGUAIABKAHUAbABpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByACAAdABvACAAdABoAGUAIABHAHIAZQBnAG8AcgBpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AXABuAFwAbgBPAHUAdABwAHUAdABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAGkAbgB0AGUAZwBlAHIAIAAgACAAIAAgACAAIAAgACAAfAAgAFkAZQBhAHIAIABpAG4AIABDAG8AbQBtAG8AbgAgAEUAcgBhAC4AIABOAG8AdABlACAAdABoAGEAdAAgADEAIABCAEMAIAA9ACAAMAAgAEMARQAsACAAMgAgAEIAQwAgAD0AIAAtADEAIABDAEUAXABuACAAMgAgAHwAIABpAG4AdABlAGcAZQByACAAWwAxAC4ALgAxADIAXQAgAHwAIABNAG8AbgB0AGgAXABuACAAMwAgAHwAIABpAG4AdABlAGcAZQByACAAWwAxAC4ALgAzADEAXQAgAHwAIABEAGEAeQBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFkAZQBhAHIAQwBFACAAfAAgAGkAbgB0AGUAZwBlAHIAIAAgACAAIAAgACAAIAAgACAAfAAgAFkAZQBhAHIAIABpAG4AIABDAG8AbQBtAG8AbgAgAEUAcgBhAC4AIABOAG8AdABlACAAdABoAGEAdAAgADEAIABCAEMAIAA9ACAAMAAgAEMARQAsACAAMgAgAEIAQwAgAD0AIAAtADEAIABDAEUAXABuAE0AbwBuAHQAaAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADEALgAuADEAMgBdACAAfAAgAFwAbgBEAGEAeQAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAWwAxAC4ALgAzADIAKQAgAHwAIABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ASgBVAEwASQBBAE4AXwBUAE8AXwBHAFIARQBHAE8AUgBJAEEATgAgAD0AIABMAEEATQBCAEQAQQAoAFkAZQBhAHIAQwBFACwAIABNAG8AbgB0AGgALAAgAEQAYQB5ACwAXABuACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgAF8ASgBEAE4ALAAgAEoAVQBMAEkAQQBOAF8ARABBAFkAXwBOAFUATQBCAEUAUgAoAFkAZQBhAHIAQwBFACwAIABNAG8AbgB0AGgALAAgAEQAYQB5ACwAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgBTACgASQBTAEUAUgBSAE8AUgAoAF8ASgBEAE4AKQAsACAAewAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBKAEQATgAgAD0AIABcACIAXAAiACwAIAB7AFwAIgBcACIALAAgAFwAIgBcACIALAAgAFwAIgBcACIAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAIABKAEQATgBfAFQATwBfAEMAQQBMAEUATgBEAEEAUgBfAEQAQQBUAEUAKABfAEoARABOACwAIAAwACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBTAEUAQwBVAEwAQQBSAF8ARABJAEYARgBFAFIARQBOAEMARQBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAG4AdQBtAGIAZQByACAAbwBmACAAZABhAHkAcwAgAHQAaABlACAARwByAGUAZwBvAHIAaQBhAG4AIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAgAGkAcwAgAGEAaABlAGEAZAAgAG8AZgAgAHQAaABlACAASgB1AGwAaQBhAG4AIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAgAGYAbwByAFwAbgBhACAAZwBpAHYAZQBuACAAZABhAHQAZQAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAEQAYQB5AHMAIABkAGkAZgBmAGUAcgBlAG4AYwBlAC4AIABOAGUAZwBhAHQAaQB2AGUAIAB2AGEAbAB1AGUAcwAgAGEAcgBlACAAdwBoAGUAbgAgAHQAaABlACAASgB1AGwAaQBhAG4AIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGUAcgAgAGkAcwAgAGEAaABlAGEAZAAuAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AWQBlAGEAcgBDAEUAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAAgACAAIAAgACAAIAAgACAAfAAgAFkAZQBhAHIAIABpAG4AIABDAG8AbQBtAG8AbgAgAEUAcgBhAC4AIABOAG8AdABlACAAdABoAGEAdAAgADEAIABCAEMAIAA9ACAAMAAgAEMARQAsACAAMgAgAEIAQwAgAD0AIAAtADEAIABDAEUAXABuAE0AbwBuAHQAaAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAWwAxAC4ALgAxADIAXQAgAHwAIABcAG4ARABhAHkAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIABbADEALgAuADMAMgApACAAfAAgAFwAbgBbAEYAcgBvAG0ASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0AIAB8ACAAcwB3AGkAdABjAGgAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAUAByAG8AdgBpAGQAZQBkACAAZABhAHQAZQAgAGkAcwAgAGkAbgAgAEoAdQBsAGkAYQBuACAAYwBhAGwAZQBuAGQAYQByAC4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABEAGUAZgBhAHUAbAB0ACAAaQBzACAAdABoAGUAIABHAHIAZQBnAG8AcgBpAGEAbgAgAGMAYQBsAGUAbgBkAGEAcgAuAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBTAEUAQwBVAEwAQQBSAF8ARABJAEYARgBFAFIARQBOAEMARQAgAD0AIABMAEEATQBCAEQAQQAoAFkAZQBhAHIAQwBFACwAIABNAG8AbgB0AGgALAAgAEQAYQB5ACwAIABbAEYAcgBvAG0ASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0ALABcAG4AIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAXwBkAGEAeQAsACAASQBOAFQAKABEAGEAeQApACwAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABOACgARgByAG8AbQBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAgAD0AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAEYAcgBvAG0AIABHAHIAZQBnAG8AcgBpAGEAbgAgAGMAYQBsAGUAbgBkAGEAcgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAEoARABOAF8ARwAsACAASgBVAEwASQBBAE4AXwBEAEEAWQBfAE4AVQBNAEIARQBSACgAWQBlAGEAcgBDAEUALAAgAE0AbwBuAHQAaAAsACAAXwBkAGEAeQAsACAAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgASQBTAEUAUgBSAE8AUgAoAF8ASgBEAE4AXwBHACkALAAgAHsAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAEoARABOAF8ARwAgAD0AIABcACIAXAAiACwAIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBKAEQATgBfAEoALAAgAEkARgAoACgATQBvAG4AdABoACAAPQAgADIAKQAgACoAIAAoAF8AZABhAHkAIAA9ACAAMgA5ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAEkAUwBfAEwARQBBAFAAXwBZAEUAQQBSACgAWQBlAGEAcgBDAEUALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABKAFUATABJAEEATgBfAEQAQQBZAF8ATgBVAE0AQgBFAFIAKABZAGUAYQByAEMARQAsACAAMgAsACAAMgA5ACwAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASgBVAEwASQBBAE4AXwBEAEEAWQBfAE4AVQBNAEIARQBSACgAWQBlAGEAcgBDAEUALAAgADIALAAgADIAOAAsACAAMQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASgBVAEwASQBBAE4AXwBEAEEAWQBfAE4AVQBNAEIARQBSACgAWQBlAGEAcgBDAEUALAAgAE0AbwBuAHQAaAAsACAAXwBkAGEAeQAsACAAMQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAEoARABOAF8ASgAgAC0AIABfAEoARABOAF8ARwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAARgByAG8AbQAgAEoAdQBsAGkAYQBuACAAYwBhAGwAZQBuAGQAYQByAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHQAZQBfAEcALAAgAEoAVQBMAEkAQQBOAF8AVABPAF8ARwBSAEUARwBPAFIASQBBAE4AKABZAGUAYQByAEMARQAsACAATQBvAG4AdABoACwAIABfAGQAYQB5ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABJAFMARQBSAFIATwBSACgASQBOAEQARQBYACgAXwBkAGEAdABlAF8ARwAsACAAMQAsACAAMQApACkALAAgAHsAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABJAE4ARABFAFgAKABfAGQAYQB0AGUAXwBHACwAIAAxACwAIAAxACkAIAA9ACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABTAEUAQwBVAEwAQQBSAF8ARABJAEYARgBFAFIARQBOAEMARQAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkATgBEAEUAWAAoAF8AZABhAHQAZQBfAEcALAAgADEALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkATgBEAEUAWAAoAF8AZABhAHQAZQBfAEcALAAgADEALAAgADIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkATgBEAEUAWAAoAF8AZABhAHQAZQBfAEcALAAgADEALAAgADMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAFwAbgBcAG4AXABuAFwAbgBcAG4AXABuAC8AKgAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAXABuACMAIABXAEUARQBLAFMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAqAC8AXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ARABBAFkAXwBPAEYAXwBXAEUARQBLAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAGEAbgAgAGkAbgB0AGUAZwBlAHIAIABmAG8AcgAgAHQAaABlACAAZABhAHkAIABvAGYAIAB0AGgAZQAgAHcAZQBlAGsAIABmAG8AcgAgAGEAIABnAGkAdgBlAG4AIABKAHUAbABpAGEAbgAgAEQAYQB5ACAATgB1AG0AYgBlAHIALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMQAuAC4ANwBdACAAfAAgAEkAUwBPACAAZABhAHkAIABvAGYAIAB3AGUAZQBrACAAbgB1AG0AYgBlAHIAXABuACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAATQBvAG4AZABhAHkALgAuAFMAdQBuAGQAYQB5AFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ASgBEAE4AIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIABKAHUAbABpAGEAbgAgAEQAYQB5ACAATgB1AG0AYgBlAHIAIABmAG8AcgAgAHQAaABlACAAYwBhAGwAZQBuAGQAYQByACAAZABhAHkAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEQAQQBZAF8ATwBGAF8AVwBFAEUASwAgAD0AIABMAEEATQBCAEQAQQAoAEoARABOACwAXABuACAAIAAgACAASQBGACgASgBEAE4AIAA9ACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABKAEQATgApACkALAAgAHsAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBqAGQAbgAsACAASQBOAFQAKABKAEQATgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATQBPAEQAKABfAGoAZABuACwAIAA3ACkAIAArACAAMQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEMATwBOAFYARQBSAFQAXwBXAEUARQBLAEQAQQBZAF8ATgBVAE0AQgBFAFIAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAYQBuACAAaQBuAHQAZQBnAGUAcgAgAGYAbwByACAAdABoAGUAIABkAGEAeQAgAG8AZgAgAHQAaABlACAAdwBlAGUAawAgAGYAcgBvAG0AIAB0AGgAZQAgAHQAcgBhAGQAaQB0AG8AbgBhAGwAIABuAHUAbQBiAGUAcgBpAG4AZwAgAHMAYwBoAGUAbQBlACAAdABvACAAdABoAGUAIABJAFMATwAgAGQAZQBmAGkAbgBpAHQAaQBvAG4ALAAgAG8AcgBcAG4AdgBpAGMAZQAgAHYAZQByAHMAYQAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAFcAZQBlAGsAZABhAHkAIABuAHUAbQBiAGUAcgBcAG4AIAAgACAAfAAgAFsAMQAuAC4ANwBdACAAIAB8ACAAIAAgACAAfAAgAEkAUwBPACAAIAAgACAAIAAgACAAfAAgAFQAcgBhAGQAaQB0AGkAbwBhAGwAXABuACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAgADEAIAB8ACAATQBvAG4AZABhAHkAIAAgACAAIAB8ACAAUwB1AG4AZABhAHkAIABcAG4AIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAyACAAfAAgAFQAdQBlAHMAZABhAHkAIAAgACAAfAAgAE0AbwBuAGQAYQB5ACAAXABuACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgACAAMwAgAHwAIABXAGUAZABuAGUAcwBkAGEAeQAgAHwAIABUAHUAZQBzAGQAYQB5AFwAbgAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAgADQAIAB8ACAAVABoAHUAcgBzAGQAYQB5ACAAIAB8ACAAVwBlAGQAbgBlAHMAZABhAHkAXABuACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgACAANQAgAHwAIABGAHIAaQBkAGEAeQAgACAAIAAgAHwAIABUAGgAdQByAHMAZABhAHkAXABuACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgACAANgAgAHwAIABTAGEAdAB1AHIAZABhAHkAIAAgAHwAIABGAHIAaQBkAGEAeQBcAG4AIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAA3ACAAfAAgAFMAdQBuAGQAYQB5ACAAIAAgACAAfAAgAFMAYQB0AHUAcgBkAGEAeQBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEQAYQB5AE8AZgBXAGUAZQBrACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADEALgAuADcAXQAgAHwAIABEAGEAeQAgAG8AZgAgAHcAZQBlAGsAIABuAHUAbQBiAGUAcgBcAG4AWwBJAFMATwB0AG8AVAByAGEAZABpAHQAaQBvAG4AYQBsAF0AIAB8ACAAcwB3AGkAdABjAGgAIAAgACAAIAAgACAAIAAgACAAfAAgAFIAZQB0AHUAcgBuACAAZABhAHkAIABvAGYAIAB3AGUAZQBrACAAdQBzAGkAbgBnACAAdAByAGEAZABpAHQAaQBvAG4AYQBsACAAbgB1AG0AYgBlAHIAaQBuAGcAIABzAGMAaABlAG0AZQAsACAAYQBzAHMAdQBtAGkAbgBnACAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABEAGEAeQBPAGYAVwBlAGUAawAgAHcAYQBzACAAcAByAG8AdgBpAGQAZQBkACAAYQBjAGMAbwByAGQAaQBuAGcAIAB0AG8AIABJAFMATwAgAGQAZQBmAGkAbgBpAHQAaQBvAG4ALgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAEQAZQBmAGEAdQBsAHQAIABpAHMAIAB0AG8AIAByAGUAdAB1AHIAbgAgAGkAbgAgAEkAUwBPACAAZABlAGYAaQBuAGkAdABpAG8AbgAsACAAYQBzAHMAdQBtAGkAbgBnACAARABhAHkATwBmAFcAZQBlAGsAIAB3AGEAcwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAHAAcgBvAHYAaQBkAGUAZAAgAGEAYwBjAG8AcgBkAGkAbgBnACAAdABvACAAdABoAGUAIAB0AHIAYQBkAGkAdABpAG8AbgBhAGwAIABuAHUAbQBiAGUAcgBpAG4AZwAgAHMAYwBoAGUAbQBlAC4AXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEMATwBOAFYARQBSAFQAXwBXAEUARQBLAEQAQQBZAF8ATgBVAE0AQgBFAFIAIAA9ACAATABBAE0AQgBEAEEAKABEAGEAeQBPAGYAVwBlAGUAawAsACAAWwBJAFMATwB0AG8AVAByAGEAZABpAHQAaQBvAG4AYQBsAF0ALABcAG4AIAAgACAAIABJAEYAKABEAGEAeQBPAGYAVwBlAGUAawAgAD0AIABcACIAXAAiACwAIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEQAYQB5AE8AZgBXAGUAZQBrACkAKQAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGcAaQB2AGUAbgBEAG8AVwAsACAASQBOAFQAKABOACgARABhAHkATwBmAFcAZQBlAGsAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBmAHIAbwBtAEkAUwBPACwAIABOACgASQBTAE8AdABvAFQAcgBhAGQAaQB0AGkAbwBuAGEAbAApACAAPAA+ACAAMAAsACAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGgAaQBmAHQARABvAFcALAAgAF8AZwBpAHYAZQBuAEQAbwB3ACAAKwAgAEkARgAoAF8AZgByAG8AbQBJAFMATwAsACAAMAAsACAALQAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABNAE8ARAAoAF8AcwBoAGkAZgB0AEQAbwB3ACwAIAA3ACkAIAArACAAMQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFcARQBFAEsARABBAFkAXwBPAEYAXwBNAE8ATgBUAEgAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAYQAgAEoAdQBsAGkAYQBuACAARABhAHkAIABOAHUAbQBiAGUAcgAgAGYAbwByACAAYQAgAGcAaQB2AGUAbgAgAGQAYQB5ACAAbwBmACAAdwBlAGUAawAsACAAYQBuAGQAIABhACAAcgBlAGwAYQB0AGkAdgBlACAAdwBlAGUAawAgAGYAbwByACAAdABoAGUAIABtAG8AbgB0AGgAIABhAG4AZAAgAHkAZQBhAHIAIABvAGYAIAB0AGgAZQBcAG4AcwBwAGUAYwBpAGYAaQBlAGQAIABjAGEAbABlAG4AZABhAHIALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIABKAHUAbABpAGEAbgAgAEQAYQB5ACAATgB1AG0AYgBlAHIAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBZAGUAYQByAEMARQAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAAgACAAIAAgACAAIAAgACAAfAAgAFkAZQBhAHIAIABpAG4AIABDAG8AbQBtAG8AbgAgAEUAcgBhAC4AIABOAG8AdABlACAAdABoAGEAdAAgADEAIABCAEMAIAA9ACAAMAAgAEMARQAsACAAMgAgAEIAQwAgAD0AIAAtADEAIABDAEUAXABuAE0AbwBuAHQAaAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMQAuAC4AMQAyAF0AIAB8ACAATQBvAG4AdABoACAAbwBmACAAdABoAGUAIAB5AGUAYQByAFwAbgBXAGUAZQBrAE8AZgBNAG8AbgB0AGgAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAAgACAAIAAgACAAIAAgACAAfAAgAFcAZQBlAGsAIABpAG4AIAB0AGgAZQAgAG0AbwBuAHQAaAAuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAE4AbwB0AGUAIABpAGYAIAB0AGgAZQAgAHIAZQBmAGUAcgBlAG4AYwBlACAAZQB4AGMAZQBlAGQAcwAgAHQAaABlACAAYgBvAHUAbgBkAHMAIABvAGYAIAB0AGgAZQAgAG0AbwBuAHQAaAAsACAAYQBuAG8AdABoAGUAcgAgAG0AbwBuAHQAaABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAB3AGkAbABsACAAYgBlACAAcgBlAHQAdQByAG4AZQBkAC4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAxACAALQAgAGYAaQByAHMAdAAgAHcAZQBlAGsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAyACAALQAgAHMAZQBjAG8AbgBkACAAdwBlAGUAawBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgADMAIAAtACAAdABoAGkAcgBkACAAdwBlAGUAawBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgADQAIAAtACAAZgBvAHUAcgB0AGgAIAB3AGUAZQBrAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAANQAgAC0AIABmAGkAZgB0AGgAIAB3AGUAZQBrAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAMAAgAC0AIABsAGEAcwB0ACAAdwBlAGUAawBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAtADEAIAAtACAAcwBlAGMAbwBuAGQAIAB0AG8AIABsAGEAcwB0ACAAdwBlAGUAawBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAtADIAIAAtACAAdABoAGkAcgBkACAAdABvACAAbABhAHMAdAAgAHcAZQBlAGsAXABuAEkAUwBPAFcAZQBlAGsARABhAHkAIAAgACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgAFsAMQAuAC4ANwBdACAAIAB8ACAASQBTAE8AIABkAGEAeQAgAG8AZgAgAHcAZQBlAGsAIABuAHUAbQBiAGUAcgAgAE0AbwBuAGQAYQB5AC4ALgBTAHUAbgBkAGEAeQBcAG4AWwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAgAHwAIABzAHcAaQB0AGMAaAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABDAGEAbABjAHUAbABhAHQAZQAgAGYAbwByACAAdABoAGUAIABKAHUAbABpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AIABEAGUAZgBhAHUAbAB0ACAAaQBzACAARwByAGUAZwBvAHIAaQBhAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgBcAG4AIAAgACAAIABcAG4ARQB4AGEAbQBwAGwAZQBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBXAEUARQBLAEQAQQBZAF8ATwBGAF8ATQBPAE4AVABIACgAMgAwADIAMwAsACAANgAsACAAMAAsACAANwApAFwAbgBSAGUAdAB1AHIAbgBzADoAIABKAEQATgAgADIANAA2ADAAMQAyADEAIAAoADIANQAvADAANgAvADIAMAAyADMAKQAgAGkAZQAuACAAdABoAGUAIABsAGEAcwB0ACAAUwB1AG4AZABhAHkAIABvAGYAIABKAHUAbgBlACAAMgAwADIAMwBcAG4AXABuAFcARQBFAEsARABBAFkAXwBPAEYAXwBNAE8ATgBUAEgAKAAyADAAMgAzACwAIAAxACwAIAAyACwAIAAyACkAXABuAFIAZQB0AHUAcgBuAHMAOgAgAEoARABOACAAMgA0ADUAOQA5ADUANQAgACgAMQAwAC8AMAAxAC8AMgAwADIAMwApACAAaQBlAC4AIAB0AGgAZQAgAHMAZQBjAG8AbgBkACAAVAB1AGUAcwBkAGEAeQAgAG8AZgAgAEoAYQBuAHUAYQByAHkAIAAyADAAMgAzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBXAEUARQBLAEQAQQBZAF8ATwBGAF8ATQBPAE4AVABIACAAPQAgAEwAQQBNAEIARABBACgAWQBlAGEAcgBDAEUALAAgAE0AbwBuAHQAaAAsACAAVwBlAGUAawBPAGYATQBvAG4AdABoACwAIABJAFMATwBXAGUAZQBrAEQAYQB5ACwAIABbAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACwAXABuACAAIAAgACAASQBGACgAKABZAGUAYQByAEMARQAgAD0AIABcACIAXAAiACkAIAAqACAAKABNAG8AbgB0AGgAIAA9ACAAXAAiAFwAIgApACAAKgAgACgAVwBlAGUAawBPAGYATQBvAG4AdABoACAAPQAgAFwAIgBcACIAKQAgACoAIAAoAEkAUwBPAFcAZQBlAGsARABhAHkAIAA9ACAAXAAiAFwAIgApACwAIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAFkAZQBhAHIAQwBFACkAKQAgACsAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAE0AbwBuAHQAaAApACkAIAArACAATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABXAGUAZQBrAE8AZgBNAG8AbgB0AGgAKQApACAAKwAgAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgASQBTAE8AVwBlAGUAawBEAGEAeQApACkALAAgAHsAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoACgATQBPAEQAKABZAGUAYQByAEMARQAsACAAMQApACAAPgAgADAAKQAgACsAIAAoAE0ATwBEACgATQBvAG4AdABoACwAIAAxACkAIAA+ACAAMAApACAAKwAgACgATQBPAEQAKABXAGUAZQBrAE8AZgBNAG8AbgB0AGgALAAgADEAKQAgAD4AIAAwACkALAAgAHsAIwBOAFUATQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBtAG8AbgB0AGgALAAgAE0AbwBuAHQAaAAgACsAIABOACgAVwBlAGUAawBPAGYATQBvAG4AdABoACAAPAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBpAHMAbwBEAG8AVwAsACAATQBPAEQAKABJAE4AVAAoAEkAUwBPAFcAZQBlAGsARABhAHkAKQAgAC0AIAAxACwAIAA3ACkAIAArACAAMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBmAGkAcgBzAHQATwBmAE0AbwBuAHQAaAAsACAASgBVAEwASQBBAE4AXwBEAEEAWQBfAE4AVQBNAEIARQBSACgAWQBlAGEAcgBDAEUALAAgAF8AbQBvAG4AdABoACwAIAAxACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBmAGkAcgBzAHQARABvAFcALAAgAEQAQQBZAF8ATwBGAF8AVwBFAEUASwAoAF8AZgBpAHIAcwB0AE8AZgBNAG8AbgB0AGgAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBmAGkAcgBzAHQATwBmAE0AbwBuAHQAaAAgACsAIAAoACgAVwBlAGUAawBPAGYATQBvAG4AdABoACAALQAgADEAKQAgACoAIAA3ACkAIAArACAATQBPAEQAKABfAGkAcwBvAEQAbwB3ACAALQAgAF8AZgBpAHIAcwB0AEQAbwBXACwAIAA3ACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFcARQBFAEsAUwBfAEkATgBfAFkARQBBAFIAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIABjAG8AdQBuAHQAIABvAGYAIABJAFMATwAgAGQAZQBmAGkAbgBlAGQAIAB3AGUAZQBrAHMAIABpAG4AIABhACAAZwBpAHYAZQBuACAAeQBlAGEAcgAgAG8AZgAgAHQAaABlACAAcwBwAGUAYwBpAGYAaQBlAGQAIABjAGEAbABlAG4AZABhAHIALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsANQAyACwANQAzAF0AXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBZAGUAYQByAEMARQAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAAWQBlAGEAcgAgAGkAbgAgAEMAbwBtAG0AbwBuACAARQByAGEALgAgAE4AbwB0AGUAIAB0AGgAYQB0ACAAMQAgAEIAQwAgAD0AIAAwACAAQwBFACwAIAAyACAAQgBDACAAPQAgAC0AMQAgAEMARQBcAG4AWwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAgAHwAIABzAHcAaQB0AGMAaAAgACAAfAAgAEMAYQBsAGMAdQBsAGEAdABlACAAZgBvAHIAIAB0AGgAZQAgAEoAdQBsAGkAYQBuACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgAgAEQAZQBmAGEAdQBsAHQAIABpAHMAIABHAHIAZQBnAG8AcgBpAGEAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAFcARQBFAEsAUwBfAEkATgBfAFkARQBBAFIAIAA9ACAATABBAE0AQgBEAEEAKABZAGUAYQByAEMARQAsACAAWwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAsAFwAbgAgACAAIAAgAEkARgAoAFkAZQBhAHIAQwBFACAAPQAgAFwAIgBcACIALAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgAWQBlAGEAcgBDAEUAKQApACwAIAB7ACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZwByAGUAZwBvAHIAaQBhAG4ALAAgAE4AKABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAgAD0AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAZgBuAEwAYQBzAHQAVwBlAGUAawBEAGEAeQBPAGYAWQBlAGEAcgAsACAATABBAE0AQgBEAEEAKABfAHkAZQBhAHIAQwBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAYQB5AFAAcgBlAGMAZQBzAHMAaQBvAG4ALAAgAEkARgAoAF8AZwByAGUAZwBvAHIAaQBhAG4ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIAQwBFACAAKwAgAEkATgBUACgAXwB5AGUAYQByAEMARQAgAC8AIAA0ACkAIAAtACAASQBOAFQAKABfAHkAZQBhAHIAQwBFACAALwAgADEAMAAwACkAIAArACAASQBOAFQAKABfAHkAZQBhAHIAQwBFACAALwAgADQAMAAwACkAIAArACAANgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AeQBlAGEAcgBDAEUAIAArACAASQBOAFQAKABfAHkAZQBhAHIAQwBFACAALwAgADQAKQAgACsAIAA0AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAE0ATwBEACgAXwBkAGEAeQBQAHIAZQBjAGUAcwBzAGkAbwBuACwAIAA3ACkAIAArACAAMQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIAQwBFACwAIABJAE4AVAAoAFkAZQBhAHIAQwBFACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAbwB3AEwAYQBzAHQARABhAHkALAAgAGYAbgBMAGEAcwB0AFcAZQBlAGsARABhAHkATwBmAFkAZQBhAHIAKABfAHkAZQBhAHIAQwBFACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABvAHcATABhAHMAdABEAGEAeQAgAD0AIAA0ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABpAGYAIABsAGEAcwB0ACAAZABhAHkAIABvAGYAIAB5AGUAYQByACAAaQBzACAAYQAgAFQAaAB1AHIAcwBkAGEAeQAsACAAdABoAGUAbgAgAGgAYQBzACAAYQBuACAAZQB4AHQAcgBhACAAdwBlAGUAawBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADUAMwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAG8AdwBMAGEAcwB0AEQAYQB5AFAAcgBlAHYALAAgAGYAbgBMAGEAcwB0AFcAZQBlAGsARABhAHkATwBmAFkAZQBhAHIAKABfAHkAZQBhAHIAQwBFACAALQAgADEAKQAgACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABvAHcATABhAHMAdABEAGEAeQBQAHIAZQB2ACAAPQAgADMALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABpAGYAIABsAGEAcwB0ACAAZABhAHkAIABvAGYAIABwAHIAZQB2AGkAbwB1AHMAIAB5AGUAYQByACAAaQBzACAAYQAgAFcAZQBkAG4AZQBzAGQAYQB5ACwAIAB0AGgAZQBuACAAaABhAHMAIABhAG4AIABlAHgAdAByAGEAIAB3AGUAZQBrAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADUAMwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAG8AdABoAGUAcgB3AGkAcwBlAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADUAMgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFcARQBFAEsAXwBEAEEAVABFAF8AVABPAF8ASgBEAE4AXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIABKAHUAbABpAGEAbgAgAEQAYQB5ACAATgB1AG0AYgBlAHIAIABvAGYAIAB0AGgAZQAgAHAAcgBvAHYAaQBkAGUAZAAgAHcAZQBlAGsAIABkAGEAdABlACAAaQBuACAAdABoAGUAIABzAHAAZQBjAGkAZgBpAGUAZAAgAGMAYQBsAGUAbgBkAGEAcgAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAEoAdQBsAGkAYQBuACAARABhAHkAIABOAHUAbQBiAGUAcgBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFkAZQBhAHIAQwBFACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgACAAIAAgACAAIAAgACAAIAB8ACAAWQBlAGEAcgAgAGkAbgAgAEMAbwBtAG0AbwBuACAARQByAGEALgAgAE4AbwB0AGUAIAB0AGgAYQB0ACAAMQAgAEIAQwAgAD0AIAAwACAAQwBFACwAIAAyACAAQgBDACAAPQAgAC0AMQAgAEMARQBcAG4ASQBTAE8AVwBlAGUAawAgACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAWwAxAC4ALgA1ADMAXQAgAHwAIABJAFMATwAgAGQAZQBmAGkAbgBlAGQAIAB3AGUAZQBrACAAbgB1AG0AYgBlAHIAIABvAGYAIAB0AGgAZQAgAHkAZQBhAHIAXABuAEkAUwBPAFcAZQBlAGsARABhAHkAIAAgACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgAFsAMQAuAC4ANwBdACAAIAB8ACAASQBTAE8AIABkAGUAZgBpAG4AZQBkACAAZABhAHkAIABvAGYAIAB3AGUAZQBrACAATQBvAG4AZABhAHkALgAuAFMAdQBuAGQAYQB5AFwAbgBbAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACAAfAAgAHMAdwBpAHQAYwBoACAAIAAgACAAIAAgACAAIAAgACAAfAAgAEMAYQBsAGMAdQBsAGEAdABlACAAZgBvAHIAIAB0AGgAZQAgAEoAdQBsAGkAYQBuACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgAgAEQAZQBmAGEAdQBsAHQAIABpAHMAIABHAHIAZQBnAG8AcgBpAGEAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBXAEUARQBLAF8ARABBAFQARQBfAFQATwBfAEoARABOACAAPQAgAEwAQQBNAEIARABBACgAWQBlAGEAcgBDAEUALAAgAEkAUwBPAFcAZQBlAGsALAAgAEkAUwBPAFcAZQBlAGsARABhAHkALAAgAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0ALABcAG4AIAAgACAAIABJAEYAKAAoAFkAZQBhAHIAQwBFACAAPQAgAFwAIgBcACIAKQAgACoAIAAoAEkAUwBPAFcAZQBlAGsAIAA9ACAAXAAiAFwAIgApACAAKgAgACgASQBTAE8AVwBlAGUAawBEAGEAeQAgAD0AIABcACIAXAAiACkALAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgAWQBlAGEAcgBDAEUAKQApACAAKwAgAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgASQBTAE8AVwBlAGUAawApACkAIAArACAATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABJAFMATwBXAGUAZQBrAEQAYQB5ACkAKQAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGkAbgB2AGEAbABpAGQALAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABNAE8ARAAoAFkAZQBhAHIAQwBFACwAIAAxACkAIAA+ACAAMAAsACAAVABSAFUARQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATQBPAEQAKABJAFMATwBXAGUAZQBrACwAIAAxACkAIAA+ACAAMAAsACAAVABSAFUARQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBTAE8AVwBlAGUAawAgADwAIAAxACwAIABUAFIAVQBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAFMATwBXAGUAZQBrACAAPgAgADUAMwAsACAAVABSAFUARQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBTAE8AVwBlAGUAawAgAD0AIAA1ADMALAAgACgAVwBFAEUASwBTAF8ASQBOAF8AWQBFAEEAUgAoAFkAZQBhAHIAQwBFACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAgADwAIAA1ADMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABSAFUARQAsACAARgBBAEwAUwBFAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAGkAbgB2AGEAbABpAGQALAAgAHsAIwBOAFUATQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBoAGkAZgB0AEIAeQBXAGUAZQBrAHMALAAgACgASQBTAE8AVwBlAGUAawAgAC0AIAAxACkAIAAqACAANwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaABpAGYAdABEAGEAeQBPAGYAVwBlAGUAawAsACAATQBPAEQAKABJAE4AVAAoAEkAUwBPAFcAZQBlAGsARABhAHkAKQAgAC0AIAAxACwAIAA3ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBqAGQAbgBGAGkAcgBzAHQARABhAHkAWQBlAGEAcgAsACAASgBVAEwASQBBAE4AXwBEAEEAWQBfAE4AVQBNAEIARQBSACgAWQBlAGEAcgBDAEUALAAgADEALAAgADEALAAgAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZgBpAHIAcwB0AFcAZQBlAGsARABhAHkALAAgAEQAQQBZAF8ATwBGAF8AVwBFAEUASwAoAF8AagBkAG4ARgBpAHIAcwB0AEQAYQB5AFkAZQBhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIAQwBvAHIAcgBlAGMAdABpAG8AbgAsACAATQBPAEQAKAA0ACAALQAgAF8AZgBpAHIAcwB0AFcAZQBlAGsARABhAHkALAAgADcAKQAgAC0AIAAzACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AagBkAG4ARgBpAHIAcwB0AEQAYQB5AFkAZQBhAHIAIAArACAAXwB5AGUAYQByAEMAbwByAHIAZQBjAHQAaQBvAG4AIAArACAAXwBzAGgAaQBmAHQAQgB5AFcAZQBlAGsAcwAgACsAIABfAHMAaABpAGYAdABEAGEAeQBPAGYAVwBlAGUAawAgAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ASgBEAE4AXwBUAE8AXwBXAEUARQBLAF8ARABBAFQARQBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHkAZQBhAHIALAAgAEkAUwBPACAAZABlAGYAaQBuAGUAZAAgAHcAZQBlAGsAIABuAHUAbQBiAGUAcgAsACAAZABhAHkAIABvAGYAIAB0AGgAZQAgAHcAZQBlAGsALAAgAGEAbgBkACAAdwBlAGUAawBzACAAaQBuACAAdABoAGUAIAB5AGUAYQByACAAZgBvAHIAIAB0AGgAZQAgAGcAaQB2AGUAbgAgAEoAdQBsAGkAYQBuACAARABhAHkAXABuAE4AdQBtAGIAZQByACAAaQBuACAAdABoAGUAIABzAHAAZQBjAGkAZgBpAGUAZAAgAGMAYQBsAGUAbgBkAGEAcgAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABpAG4AdABlAGcAZQByACAAIAAgACAAIAAgACAAIAAgAHwAIABZAGUAYQByAEMARQBcAG4AIAAyACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADEALgAuADUAMwBdACAAfAAgAEkAUwBPACAAdwBlAGUAawAgAG4AdQBtAGIAZQByAFwAbgAgADMAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMQAuAC4ANwBdACAAIAB8ACAASQBTAE8AIABkAGEAeQAgAG8AZgAgAHcAZQBlAGsAIABNAG8AbgBkAGEAeQAuAC4AUwB1AG4AZABhAHkAXABuACAANAAgAHwAIABpAG4AdABlAGcAZQByACAAWwA1ADIALAA1ADMAXQAgAHwAIABJAFMATwAgAHcAZQBlAGsAcwAgAGkAbgAgAHkAZQBhAHIAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBKAEQATgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByACAAZgBvAHIAIAB0AGgAZQAgAGMAYQBsAGUAbgBkAGEAcgAgAGQAYQB5AFwAbgBbAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACAAfAAgAHMAdwBpAHQAYwBoACAAIAB8ACAAQwBhAGwAYwB1AGwAYQB0AGUAIABmAG8AcgAgAHQAaABlACAASgB1AGwAaQBhAG4AIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuACAARABlAGYAYQB1AGwAdAAgAGkAcwAgAEcAcgBlAGcAbwByAGkAYQBuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ASgBEAE4AXwBUAE8AXwBXAEUARQBLAF8ARABBAFQARQAgAD0AIABMAEEATQBCAEQAQQAoAEoARABOACwAIABbAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACwAXABuACAAIAAgACAASQBGACgASgBEAE4AIAA9ACAAXAAiAFwAIgAsACAAewBcACIAXAAiACwAIABcACIAXAAiACwAIABcACIAXAAiACwAIABcACIAXAAiAH0ALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgASgBEAE4AKQApACwAIAB7ACMAVgBBAEwAVQBFACEALAAgACMAVgBBAEwAVQBFACEALAAgACMAVgBBAEwAVQBFACEALAAgACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AagBkAG4ALAAgAEkATgBUACgASgBEAE4AKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYwBhAGwARABhAHQAZQAsACAASgBEAE4AXwBUAE8AXwBDAEEATABFAE4ARABBAFIAXwBEAEEAVABFACgAXwBqAGQAbgAsACAASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIAQwBFACwAIABJAE4ARABFAFgAKABfAGMAYQBsAEQAYQB0AGUALAAgADEALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkATwBmAFcAZQBlAGsALAAgAEQAQQBZAF8ATwBGAF8AVwBFAEUASwAoAF8AagBkAG4AKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkATwBmAFkAZQBhAHIALAAgAF8AagBkAG4AIAAtACAASgBVAEwASQBBAE4AXwBEAEEAWQBfAE4AVQBNAEIARQBSACgAXwB5AGUAYQByAEMARQAsACAAMQAsACAAMQAsACAASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByACkAIAArACAAMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbgBvAG0AaQBuAGEAbABXAGUAZQBrACwAIABJAE4AVAAoACgAXwBkAGEAeQBPAGYAWQBlAGEAcgAgAC0AIABfAGQAYQB5AE8AZgBXAGUAZQBrACAAKwAgADEAMAApACAALwAgADcAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABsAGEAcwB0ACAAdwBlAGUAawAgAG8AZgAgAHAAcgBlAHYAaQBvAHUAcwAgAHkAZQBhAHIAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG4AbwBtAGkAbgBhAGwAVwBlAGUAawAgAD0AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB3AGUAZQBrAHMASQBuAFkAZQBhAHIALAAgAFcARQBFAEsAUwBfAEkATgBfAFkARQBBAFIAKABfAHkAZQBhAHIAQwBFACAALQAgADEALAAgAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgApACwAIABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AGUAYQByAEMARQAgAC0AIAAxACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHcAZQBlAGsAcwBJAG4AWQBlAGEAcgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQBPAGYAVwBlAGUAawAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB3AGUAZQBrAHMASQBuAFkAZQBhAHIAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABpAGYAIAB0AGgAaQBzACAAeQBlAGEAcgAgAGQAbwBlAHMAIABuAG8AdAAgAGgAYQB2AGUAIAA1ADMAIAB3AGUAZQBrAHMALAAgAHQAaABlAG4AIABpAHMAIAB0AGgAZQAgAGYAaQByAHMAdAAgAHcAZQBlAGsAIABvAGYAIABmAG8AbABsAG8AdwBpAG4AZwAgAHkAZQBhAHIAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG4AbwBtAGkAbgBhAGwAVwBlAGUAawAgAD0AIAA1ADMALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAVwBFAEUASwBTAF8ASQBOAF8AWQBFAEEAUgAoAF8AeQBlAGEAcgBDAEUALAAgAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgApACAAPQAgADUAMwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIAQwBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAA1ADMALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkATwBmAFcAZQBlAGsALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADUAMwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdwBlAGUAawBzAEkAbgBZAGUAYQByACwAIABXAEUARQBLAFMAXwBJAE4AXwBZAEUAQQBSACgAXwB5AGUAYQByAEMARQAgACsAIAAxACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AGUAYQByAEMARQAgACsAIAAxACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQBPAGYAVwBlAGUAawAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHcAZQBlAGsAcwBJAG4AWQBlAGEAcgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB3AGUAZQBrAHMASQBuAFkAZQBhAHIALAAgAFcARQBFAEsAUwBfAEkATgBfAFkARQBBAFIAKABfAHkAZQBhAHIAQwBFACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIAQwBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG4AbwBtAGkAbgBhAGwAVwBlAGUAawAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQBPAGYAVwBlAGUAawAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB3AGUAZQBrAHMASQBuAFkAZQBhAHIAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFcARQBFAEsAXwBOAFUATQBCAEUAUgBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAEkAUwBPACAAZABlAGYAaQBuAGUAZAAgAHcAZQBlAGsAIABuAHUAbQBiAGUAcgAgAGYAbwByACAAYQAgAGcAaQB2AGUAbgAgAEoAdQBsAGkAYQBuACAARABhAHkAIABOAHUAbQBiAGUAcgAgAGkAbgAgAHQAaABlACAAcwBwAGUAYwBpAGYAaQBlAGQAIABjAGEAbABlAG4AZABhAHIALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMQAuAC4ANQAzAF0AIAB8ACAASQBTAE8AIAB3AGUAZQBrACAAbgB1AG0AYgBlAHIAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBKAEQATgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByAC4AXABuAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0AIAB8ACAAcwB3AGkAdABjAGgAIAAgAHwAIABDAGEAbABjAHUAbABhAHQAZQAgAGYAbwByACAAdABoAGUAIABKAHUAbABpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AIABEAGUAZgBhAHUAbAB0ACAAaQBzACAARwByAGUAZwBvAHIAaQBhAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBXAEUARQBLAF8ATgBVAE0AQgBFAFIAIAA9ACAATABBAE0AQgBEAEEAKABKAEQATgAsACAAWwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAsAFwAbgAgACAAIAAgAEkARgAoAEoARABOACAAPQAgAFwAIgBcACIALAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgASgBEAE4AKQApACwAIAB7ACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdwBlAGUAawBEAGEAdABlACwAIABKAEQATgBfAFQATwBfAFcARQBFAEsAXwBEAEEAVABFACgASgBEAE4ALAAgAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAQwBIAE8ATwBTAEUAQwBPAEwAUwAoAF8AdwBlAGUAawBEAGEAdABlACwAIAAyACkAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAFwAbgBcAG4AXABuAFwAbgBcAG4ALwAqACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwBcAG4AIwAgAFEAVQBBAFIAVABFAFIAUwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACoALwBcAG4AXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBEAEEAWQBTAF8ASQBOAF8AUQBVAEEAUgBUAEUAUgBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAGMAbwB1AG4AdAAgAG8AZgAgAGQAYQB5AHMAIABpAG4AIABhACAAcQB1AGEAcgB0AGUAcgAgAG8AZgAgAGEAIABnAGkAdgBlAG4AIAB5AGUAYQByACAAbwBmACAAdABoAGUAIABzAHAAZQBjAGkAZgBpAGUAZAAgAGMAYQBsAGUAbgBkAGEAcgAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABpAG4AdABlAGcAZQByACAAWwA4ADkALgAuADkAMgBdAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AUQB1AGEAcgB0AGUAcgAgACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAWwAxAC4ALgA0AF0AIAAgAHwAIABRAHUAYQByAHQAZQByACAAbwBmACAAdABoAGUAIAB5AGUAYQByACAAMQAuAC4ANAAsACAAdAByAGEAbgBzAGkAdABpAHYAZQAsACAAZQB4AGMAZQBlAGQAaQBuAGcAIAByAGEAbgBnAGUAIAB3AGkAbABsACAAYwBhAHIAcgB5ACAAdABvACAAeQBlAGEAcgAuAFwAbgBbAEYAaQBzAGMAYQBsAFkAZQBhAHIAQwBFAF0AIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAAgACAAIAAgACAAIAAgACAAfAAgAFkAZQBhAHIAIABpAG4AIABDAG8AbQBtAG8AbgAgAEUAcgBhAC4AIABOAG8AdABlACAAdABoAGEAdAAgADEAIABCAEMAIAA9ACAAMAAgAEMARQAsACAAMgAgAEIAQwAgAD0AIAAtADEAIABDAEUAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAVwBoAGUAbgAgAG0AbwBuAHQAaAAgAG8AZgBmAHMAZQB0ACAAaQBzACAAbgBvAG4ALQB6AGUAcgBvACAAdABoAGUAIABmAGkAcwBjAGEAbAAgAHkAZQBhAHIAIABzAHAAYQBuAHMAIABjAGEAbABlAG4AZABhAHIAIAB5AGUAYQByAHMAIABhAG4AZABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABpAHMAIABkAGUAZgBpAG4AZQBkACAAYQBzACAAdABoAGUAIAB5AGUAYQByACAAdwBoAGUAcgBlACAASgB1AG4AZQAgAGYAYQBsAGwAcwAuAFwAbgBbAE0AbwBuAHQAaABPAGYAZgBzAGUAdABdACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbAC0ANgAuAC4AMwBdACAAfAAgAFEAdQBhAHIAdABlAHIAIABtAG8AbgB0AGgAIABvAGYAZgBzAGUAdAAgAGYAcgBvAG0AIABKAGEAbgB1AGEAcgBhAHkAXABuAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0AIAB8ACAAcwB3AGkAdABjAGgAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAQwBhAGwAYwB1AGwAYQB0AGUAIABmAG8AcgAgAHQAaABlACAASgB1AGwAaQBhAG4AIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuACAARABlAGYAYQB1AGwAdAAgAGkAcwAgAEcAcgBlAGcAbwByAGkAYQBuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AXABuAFwAbgBFAHgAYQBtAHAAbABlAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEQAQQBZAFMAXwBJAE4AXwBRAFUAQQBSAFQARQBSACgAMwAsACAAMgAwADIAMAAsACAALQA2ACkAXABuAFIAZQB0AHUAcgBuAHMAOgAgADkAMQBcAG4AaQAuAGUALgAgADMAcgBkACAAcQB1AGEAcgB0AGUAcgAgAHMAdABhAHIAdABpAG4AZwAgAGYAcgBvAG0AIABKAHUAbAB5ACAAMgAwADEAOQAsACAAbgBhAG0AZQBsAHkAIABKAGEAbgAsACAARgBlAGIALAAgAE0AYQByACAAMgAwADIAMAAgAHcAaQB0AGgAIAAzADEALAAgADIAOQAsACAAMwAxACAAZABhAHkAcwAgAHIAZQBzAHAAZQBjAHQAaQB2AGUAbAB5AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBEAEEAWQBTAF8ASQBOAF8AUQBVAEEAUgBUAEUAUgAgAD0AIABMAEEATQBCAEQAQQAoAFEAdQBhAHIAdABlAHIALAAgAFsARgBpAHMAYwBhAGwAWQBlAGEAcgBDAEUAXQAsACAAWwBNAG8AbgB0AGgATwBmAGYAcwBlAHQAXQAsACAAWwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAsAFwAbgAgACAAIAAgAEkARgAoAFEAdQBhAHIAdABlAHIAIAA9ACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABRAHUAYQByAHQAZQByACkAKQAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgATQBPAEQAKABRAHUAYQByAHQAZQByACwAIAAxACkAIAA+ACAAMAAsACAAewAjAE4AVQBNACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AbwBuAHQAaABPAGYAZgBzAGUAdAAsACAAUgBPAFUATgBEACgATgAoAE0AbwBuAHQAaABPAGYAZgBzAGUAdAApACwAIAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoACgAXwBtAG8AbgB0AGgATwBmAGYAcwBlAHQAIAA8ACAALQA2ACkAIAArACAAKABfAG0AbwBuAHQAaABPAGYAZgBzAGUAdAAgAD4AIAAzACkALAAgAHsAIwBOAFUATQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHEAdQBhAHIAdABlAHIALAAgAE0ATwBEACgASQBOAFQAKABRAHUAYQByAHQAZQByACkAIAAtACAAMQAsACAANAApACwAIAAvAC8AIAAwAC4ALgAzAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkAcwBJAG4AUQB1AGEAcgB0AGUAcgBDAHkAYwBsAGkAYwBhAGwALAAgAHsAOQAwACwAOAA5ACwAOQAyACwAOQAxACwAOQAyACwAOQAyACwAOQAyACwAOQAyACwAOQAxACwAOQAyACwAOQAyACwAOQAwAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHEAdQBhAHIAdABlAHIAVwBpAHQAaABGAGUAYgAsACAASQBOAFQAKABNAE8ARAAoADEAIAAtACAAXwBtAG8AbgB0AGgATwBmAGYAcwBlAHQALAAgADEAMgApACAALwAgADMAKQAsACAAIAAvAC8AIAAwAC4ALgAzAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcQB1AGEAcgB0AGUAcgBQAHIAZQBjAGUAcwBzAGkAbwBuACwAIABNAE8ARAAoAF8AbQBvAG4AdABoAE8AZgBmAHMAZQB0ACAAKwAgACgAXwBxAHUAYQByAHQAZQByACAAKgAgADMAKQAsACAAMQAyACkAIAArACAAMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbgBvAG0AaQBuAGEAbABEAGEAeQBzAEkAbgBRAHUAYQByAHQAZQByACwAIABJAE4ARABFAFgAKABfAGQAYQB5AHMASQBuAFEAdQBhAHIAdABlAHIAQwB5AGMAbABpAGMAYQBsACwAIAAxACwAIABfAHEAdQBhAHIAdABlAHIAUAByAGUAYwBlAHMAcwBpAG8AbgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBsAGUAYQBwAEQAYQB5ACwAIABJAEYAKABJAFMATgBVAE0AQgBFAFIAKABGAGkAcwBjAGEAbABZAGUAYQByAEMARQApACAAKgAgACgAXwBxAHUAYQByAHQAZQByAFcAaQB0AGgARgBlAGIAIAA9ACAAXwBxAHUAYQByAHQAZQByACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AeQBlAGEAcgBPAGYARgBlAGIALAAgAEkATgBUACgARgBpAHMAYwBhAGwAWQBlAGEAcgBDAEUAKQAgACsAIABOACgAXwBxAHUAYQByAHQAZQByACAAPQAgADMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABOACgASQBTAF8ATABFAEEAUABfAFkARQBBAFIAKABfAHkAZQBhAHIATwBmAEYAZQBiACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAMABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBuAG8AbQBpAG4AYQBsAEQAYQB5AHMASQBuAFEAdQBhAHIAdABlAHIAIAArACAAXwBsAGUAYQBwAEQAYQB5AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AUQBVAEEAUgBUAEUAUgBfAEQAQQBUAEUAXwBUAE8AXwBKAEQATgBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAEoAdQBsAGkAYQBuACAARABhAHkAIABOAHUAbQBiAGUAcgAgAG8AZgAgAHQAaABlACAAcAByAG8AdgBpAGQAZQBkACAAcQB1AGEAcgB0AGUAcgAgAGQAYQB0AGUAIABpAG4AIAB0AGgAZQAgAHMAcABlAGMAaQBmAGkAZQBkACAAYwBhAGwAZQBuAGQAYQByAC4AXABuAFwAbgBPAHUAdABwAHUAdABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ARgBpAHMAYwBhAGwAWQBlAGEAcgBDAEUAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAIAAgACAAIAAgACAAIAAgAHwAIABZAGUAYQByACAAaQBuACAAQwBvAG0AbQBvAG4AIABFAHIAYQAuACAATgBvAHQAZQAgAHQAaABhAHQAIAAxACAAQgBDACAAPQAgADAAIABDAEUALAAgADIAIABCAEMAIAA9ACAALQAxACAAQwBFAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAFcAaABlAG4AIABtAG8AbgB0AGgAIABvAGYAZgBzAGUAdAAgAGkAcwAgAG4AbwBuAC0AegBlAHIAbwAgAHQAaABlACAAZgBpAHMAYwBhAGwAIAB5AGUAYQByACAAcwBwAGEAbgBzACAAYwBhAGwAZQBuAGQAYQByACAAeQBlAGEAcgBzACAAYQBuAGQAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAaQBzACAAZABlAGYAaQBuAGUAZAAgAGEAcwAgAHQAaABlACAAeQBlAGEAcgAgAHcAaABlAHIAZQAgAEoAdQBuAGUAIABmAGEAbABsAHMALgBcAG4AUQB1AGEAcgB0AGUAcgAgACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAWwAxAC4ALgA0AF0AIAAgAHwAIABRAHUAYQByAHQAZQByACAAbwBmACAAdABoAGUAIAB5AGUAYQByACAAMQAuAC4ANAAsACAAdAByAGEAbgBzAGkAdABpAHYAZQAsACAAZQB4AGMAZQBlAGQAaQBuAGcAIAByAGEAbgBnAGUAIAB3AGkAbABsACAAYwBhAHIAcgB5ACAAdABvACAAeQBlAGEAcgAuAFwAbgBEAGEAeQBPAGYAUQB1AGEAcgB0AGUAcgAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIABbADEALgAuADkAMgBdACAAfAAgAE8AcgBkAGkAbgBhAGwAIABkAGEAeQAgAG8AZgAgAHQAaABlACAAcQB1AGEAcgB0AGUAcgAsACAAZQB4AGMAZQBlAGQAaQBuAGcAIAByAGEAbgBnAGUAIAB3AGkAbABsACAAYwBhAHIAcgB5AFwAbgBbAE0AbwBuAHQAaABPAGYAZgBzAGUAdABdACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbAC0ANgAuAC4AMwBdACAAfAAgAFEAdQBhAHIAdABlAHIAIABtAG8AbgB0AGgAIABvAGYAZgBzAGUAdAAgAGYAcgBvAG0AIABKAGEAbgB1AGEAcgB5AFwAbgBbAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACAAfAAgAHMAdwBpAHQAYwBoACAAIAAgACAAIAAgACAAIAAgACAAfAAgAEMAYQBsAGMAdQBsAGEAdABlACAAZgBvAHIAIAB0AGgAZQAgAEoAdQBsAGkAYQBuACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgAgAEQAZQBmAGEAdQBsAHQAIABpAHMAIABHAHIAZQBnAG8AcgBpAGEAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBRAFUAQQBSAFQARQBSAF8ARABBAFQARQBfAFQATwBfAEoARABOACAAPQAgAEwAQQBNAEIARABBACgARgBpAHMAYwBhAGwAWQBlAGEAcgBDAEUALAAgAFEAdQBhAHIAdABlAHIALAAgAEQAYQB5AE8AZgBRAHUAYQByAHQAZQByACwAIABbAE0AbwBuAHQAaABPAGYAZgBzAGUAdABdACwAIABbAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACwAXABuACAAIAAgACAASQBGACgAKABGAGkAcwBjAGEAbABZAGUAYQByAEMARQAgAD0AIABcACIAXAAiACkAIAAqACAAKABRAHUAYQByAHQAZQByACAAPQAgAFwAIgBcACIAKQAgACoAIAAoAEQAYQB5AE8AZgBRAHUAYQByAHQAZQByACAAPQAgAFwAIgBcACIAKQAsACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABGAGkAcwBjAGEAbABZAGUAYQByAEMARQApACkAIAArACAATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABRAHUAYQByAHQAZQByACkAKQAgACsAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEQAYQB5AE8AZgBRAHUAYQByAHQAZQByACkAKQAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgATQBPAEQAKABRAHUAYQByAHQAZQByACwAIAAxACkAIAA+ACAAMAAsACAAewAjAE4AVQBNACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AbwBuAHQAaABPAGYAZgBzAGUAdAAsACAAUgBPAFUATgBEACgATgAoAE0AbwBuAHQAaABPAGYAZgBzAGUAdAApACwAIAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoACgAXwBtAG8AbgB0AGgATwBmAGYAcwBlAHQAIAA8ACAALQA2ACkAIAArACAAKABfAG0AbwBuAHQAaABPAGYAZgBzAGUAdAAgAD4AIAAzACkALAAgAHsAIwBOAFUATQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGYAaQBzAGMAYQBsAFkAZQBhAHIAQwBFACwAIABJAE4AVAAoAEYAaQBzAGMAYQBsAFkAZQBhAHIAQwBFACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHEAdQBhAHIAdABlAHIALAAgAEkATgBUACgAUQB1AGEAcgB0AGUAcgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGgAaQBmAHQATQBvAG4AdABoACwAIAAoAF8AcQB1AGEAcgB0AGUAcgAgAC0AIAAxACkAIAAqACAAMwAgACsAIABfAG0AbwBuAHQAaABPAGYAZgBzAGUAdAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AeQBlAGEAcgBDAEUALAAgAF8AZgBpAHMAYwBhAGwAWQBlAGEAcgBDAEUAIAArACAASQBOAFQAKABfAHMAaABpAGYAdABNAG8AbgB0AGgAIAAvACAAMQAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AbwBuAHQAaAAsACAATQBPAEQAKABfAHMAaABpAGYAdABNAG8AbgB0AGgALAAgADEAMgApACAAKwAgADEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGYAaQByAHMAdABEAGEAeQBPAGYAUQB1AGEAcgB0AGUAcgAsACAASgBVAEwASQBBAE4AXwBEAEEAWQBfAE4AVQBNAEIARQBSACgAXwB5AGUAYQByAEMARQAsACAAXwBtAG8AbgB0AGgALAAgADEALAAgAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBmAGkAcgBzAHQARABhAHkATwBmAFEAdQBhAHIAdABlAHIAIAAtACAAMQAgACsAIABJAE4AVAAoAEQAYQB5AE8AZgBRAHUAYQByAHQAZQByACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAIAAgACAAIABcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEoARABOAF8AVABPAF8AUQBVAEEAUgBUAEUAUgBfAEQAQQBUAEUAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIABmAGkAcwBjAGEAbAAgAHkAZQBhAHIALAAgAHEAdQBhAHIAdABlAHIALAAgAGQAYQB5ACAAbwBmACAAcQB1AGEAcgB0AGUAcgAgAGEAbgBkACAAZABhAHkAcwAgAGkAbgAgAHQAaABlACAAcQB1AGEAcgB0AGUAcgAgAGYAbwByACAAdABoAGUAIABnAGkAdgBlAG4AIABKAHUAbABpAGEAbgAgAEQAYQB5ACAATgB1AG0AYgBlAHIAXABuAGkAbgAgAHQAaABlACAAcwBwAGUAYwBpAGYAaQBlAGQAIABjAGEAbABlAG4AZABhAHIALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAaQBuAHQAZQBnAGUAcgAgACAAIAAgACAAIAAgACAAIAAgAHwAIABGAGkAcwBjAGEAbABZAGUAYQByAEMARQBcAG4AIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAVwBoAGUAbgAgAG0AbwBuAHQAaAAgAG8AZgBmAHMAZQB0ACAAaQBzACAAbgBvAG4ALQB6AGUAcgBvACAAdABoAGUAIABmAGkAcwBjAGEAbAAgAHkAZQBhAHIAIABzAHAAYQBuAHMAIABjAGEAbABlAG4AZABhAHIAIAB5AGUAYQByAHMAIABhAG4AZABcAG4AIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAaQBzACAAZABlAGYAaQBuAGUAZAAgAGEAcwAgAHQAaABlACAAeQBlAGEAcgAgAHcAaABlAHIAZQAgAEoAdQBuAGUAIABmAGEAbABsAHMALgBcAG4AIAAyACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADEALgAuADQAXQAgACAAIAB8ACAAUQB1AGEAcgB0AGUAcgBcAG4AIAAzACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADEALgAuADkAMgBdACAAIAB8ACAARABhAHkAIABvAGYAIABxAHUAYQByAHQAZQByAFwAbgAgADQAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAOAA5AC4ALgA5ADIAXQAgAHwAIABEAGEAeQBzACAAaQBuACAAcQB1AGEAcgB0AGUAcgBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEoARABOACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgACAAIAAgACAAIAAgACAAIAB8ACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByACAAZgBvAHIAIAB0AGgAZQAgAGMAYQBsAGUAbgBkAGEAcgAgAGQAYQB5AFwAbgBbAE0AbwBuAHQAaABPAGYAZgBzAGUAdABdACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbAC0ANgAuAC4AMwBdACAAfAAgAFEAdQBhAHIAdABlAHIAIABtAG8AbgB0AGgAIABvAGYAZgBzAGUAdAAgAGYAcgBvAG0AIABKAGEAbgB1AGEAcgB5AC4AXABuAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0AIAB8ACAAcwB3AGkAdABjAGgAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAQwBhAGwAYwB1AGwAYQB0AGUAIABmAG8AcgAgAHQAaABlACAASgB1AGwAaQBhAG4AIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuACAARABlAGYAYQB1AGwAdAAgAGkAcwAgAEcAcgBlAGcAbwByAGkAYQBuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEoARABOAF8AVABPAF8AUQBVAEEAUgBUAEUAUgBfAEQAQQBUAEUAIAA9ACAATABBAE0AQgBEAEEAKABKAEQATgAsACAAWwBNAG8AbgB0AGgATwBmAGYAcwBlAHQAXQAsACAAWwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAsAFwAbgAgACAAIAAgAEkARgAoAEoARABOACAAPQAgAFwAIgBcACIALAAgAHsAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgB9ACwAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEoARABOACkAKQAsACAAewAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AbwBuAHQAaABPAGYAZgBzAGUAdAAsACAAUgBPAFUATgBEACgATgAoAE0AbwBuAHQAaABPAGYAZgBzAGUAdAApACwAIAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKAAoAF8AbQBvAG4AdABoAE8AZgBmAHMAZQB0ACAAPAAgAC0ANgApACAAKwAgACgAXwBtAG8AbgB0AGgATwBmAGYAcwBlAHQAIAA+ACAAMwApACwAIAB7ACMATgBVAE0AIQAsACAAIwBOAFUATQAhACwAIAAjAE4AVQBNACEALAAgACMATgBVAE0AIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGoAZABuACwAIABJAE4AVAAoAEoARABOACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBjAGEAbABEAGEAdABlACwAIABKAEQATgBfAFQATwBfAEMAQQBMAEUATgBEAEEAUgBfAEQAQQBUAEUAKABfAGoAZABuACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaABpAGYAdABNAG8AbgB0AGgALAAgAEkATgBEAEUAWAAoAF8AYwBhAGwARABhAHQAZQAsACAAMQAsACAAMgApACAALQAgADEAIAAtACAAXwBtAG8AbgB0AGgATwBmAGYAcwBlAHQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBmAGkAcwBjAGEAbABZAGUAYQByACwAIABJAE4ARABFAFgAKABfAGMAYQBsAEQAYQB0AGUALAAgADEALAAgADEAKQAgACsAIABJAE4AVAAoAF8AcwBoAGkAZgB0AE0AbwBuAHQAaAAgAC8AIAAxADIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHoAZQByAG8AQgBhAHMAZQBkAEYAaQBzAGMAYQBsAE0AbwBuAHQAaAAsACAATQBPAEQAKABfAHMAaABpAGYAdABNAG8AbgB0AGgALAAgADEAMgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcQB1AGEAcgB0AGUAcgAsACAASQBOAFQAKABfAHoAZQByAG8AQgBhAHMAZQBkAEYAaQBzAGMAYQBsAE0AbwBuAHQAaAAgAC8AIAAzACkAIAArACAAMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGoAZABuAEYAaQByAHMAdABEAGEAeQBRAHUAYQByAHQAZQByACwAIABRAFUAQQBSAFQARQBSAF8ARABBAFQARQBfAFQATwBfAEoARABOACgAXwBmAGkAcwBjAGEAbABZAGUAYQByACwAIABfAHEAdQBhAHIAdABlAHIALAAgADEALAAgAF8AbQBvAG4AdABoAE8AZgBmAHMAZQB0ACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAYQB5AE8AZgBRAHUAYQByAHQAZQByACwAIABfAGoAZABuACAALQAgAF8AagBkAG4ARgBpAHIAcwB0AEQAYQB5AFEAdQBhAHIAdABlAHIAIAArACAAMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAYQB5AHMASQBuAFEAdQBhAHIAdABlAHIALAAgAEQAQQBZAFMAXwBJAE4AXwBRAFUAQQBSAFQARQBSACgAXwBxAHUAYQByAHQAZQByACwAIABfAGYAaQBzAGMAYQBsAFkAZQBhAHIALAAgAF8AbQBvAG4AdABoAE8AZgBmAHMAZQB0ACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZgBpAHMAYwBhAGwAWQBlAGEAcgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcQB1AGEAcgB0AGUAcgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkATwBmAFEAdQBhAHIAdABlAHIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAYQB5AHMASQBuAFEAdQBhAHIAdABlAHIAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAFwAbgBcAG4AXABuAFwAbgBcAG4AXABuAFwAbgBcAG4ALwAqACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwBcAG4AIwAgAEQAQQBUAEUAIABBAE4ARAAgAFQASQBNAEUAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACoALwBcAG4AXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBKAEQATgBfAFUAVABDAF8AVABPAF8ASgBEAEEAVABFAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAHQAaABlACAASgB1AGwAaQBhAG4AIABEAGEAdABlACAAZwBpAHYAZQBuACAAYQBuACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByACAAYQBuAGQAIAB0AGkAbQBlACAAbwBmACAAZABhAHkAIABpAG4AIABVAFQAQwAuAFwAbgBOAG8AdABlACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMAIABhAHIAZQAgAGEAbAB3AGEAeQBzACAAaQBuACAAVQBUAEMALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIABKAHUAbABpAGEAbgAgAEQAYQB0AGUAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBKAEQATgAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAIAAgACAAIAAgACAAIAB8ACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByAC4AXABuAFsAVABpAG0AZQBVAFQAQwBdACAAfAAgAGQAZQBjAGkAbQBhAGwAIABbADAALgAuADEAKQAgAHwAIABUAGkAbQBlACAAbwBmACAAZABhAHkAIABpAG4AIABVAFQAQwAgAGEAcwAgAGQAZQBjAGkAbQBhAGwAIABmAHIAYQBjAHQAaQBvAG4AIABvAHIAIABFAHgAYwBlAGwAIABEAGEAdABlAC8AVABpAG0AZQAgAHQAeQBwAGUALgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAEMAYQByAHIAaQBlAHMAIABpAGYAIAByAGEAbgBnAGUAIABpAHMAIABlAHgAYwBlAGUAZABlAGQALgBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ASgBEAE4AXwBVAFQAQwBfAFQATwBfAEoARABBAFQARQAgAD0AIABMAEEATQBCAEQAQQAoAEoARABOACwAIABbAFQAaQBtAGUAVQBUAEMAXQAsAFwAbgAgACAAIAAgAEkARgAoACgASgBEAE4AIAA9ACAAXAAiAFwAIgApACAAKgAgACgAVABpAG0AZQBVAFQAQwAgAD0AIABcACIAXAAiACkALAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgASgBEAE4AKQApACAAKwAgACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABUAGkAbQBlAFUAVABDACkAKQAgACoAIAAoAFQAaQBtAGUAVQBUAEMAIAA8AD4AIABcACIAXAAiACkAKQAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgATQBPAEQAKABKAEQATgAsACAAMQApACAAPgAgADAALAAgAHsAIwBOAFUATQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABKAEQATgAgAC0AIAAwAC4ANQAgACsAIABOACgAVABpAG0AZQBVAFQAQwApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBKAEQATgBfAEwATwBDAEEATABfAFQATwBfAEoARABBAFQARQBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAEoAdQBsAGkAYQBuACAARABhAHQAZQAgAGcAaQB2AGUAbgAgAGEAIABsAG8AYwBhAGwAIABKAHUAbABpAGEAbgAgAEQAYQB5ACAATgB1AG0AYgBlAHIAIABhAG4AZAAgAGwAbwBjAGEAbAAgAHQAaQBtAGUAIABvAGYAIABkAGEAeQAgAHcAaQB0AGgAIAB0AGkAbQBlACAAegBvAG4AZQAgAG8AZgBmAHMAZQB0ACAAaQBuAFwAbgBtAGkAbgB1AHQAZQBzAC4AIABOAG8AdABlACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMAIABhAHIAZQAgAGEAbAB3AGEAeQBzACAAaQBuACAAVQBUAEMALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIABKAHUAbABpAGEAbgAgAEQAYQB0AGUAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBMAG8AYwBhAGwASgBEAE4AIAAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAAgACAAIAAgACAAIAAgAHwAIABMAG8AYwBhAGwAIABKAHUAbABpAGEAbgAgAEQAYQB5ACAATgB1AG0AYgBlAHIALgBcAG4ATABvAGMAYQBsAFQAaQBtAGUAIAAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAWwAwAC4ALgAxACkAIAB8ACAATABvAGMAYQBsACAAdABpAG0AZQAgAG8AZgAgAGQAYQB5ACAAYQBzACAAZABlAGMAaQBtAGEAbAAgAGYAcgBhAGMAdABpAG8AbgAgAG8AcgAgAEUAeABjAGUAbAAgAEQAYQB0AGUALwBUAGkAbQBlACAAdAB5AHAAZQAuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABDAGEAcgByAGkAZQBzACAAaQBzACAAcgBhAG4AZwBlACAAaQBzACAAZQB4AGMAZQBlAGQAZQBkAC4AXABuAFsAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0AF0AIAB8ACAAZABlAGMAaQBtAGEAbAAgACAAIAAgACAAIAAgACAAfAAgAFQAaQBtAGUAIAB6AG8AbgBlACAAbwBmAGYAcwBlAHQAIABpAG4AIABtAGkAbgB1AHQAZQBzACAAZgByAG8AbQAgAFUAVABDAC4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAWwAtADkAMAAwAC4ALgA5ADAAMABdACAAIAAgACAAfAAgAEEAcwBzAHUAbQBlAGQAIAB0AG8AIABiAGUAIABVAFQAQwAgAGkAZgAgAG8AbQBtAGkAdAB0AGUAZAAuAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBKAEQATgBfAEwATwBDAEEATABfAFQATwBfAEoARABBAFQARQAgAD0AIABMAEEATQBCAEQAQQAoAEwAbwBjAGEAbABKAEQATgAsACAATABvAGMAYQBsAFQAaQBtAGUALAAgAFsAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0AF0ALABcAG4AIAAgACAAIABJAEYAKAAoAEwAbwBjAGEAbABKAEQATgAgAD0AIABcACIAXAAiACkAIAAqACAAKABMAG8AYwBhAGwAVABpAG0AZQAgAD0AIABcACIAXAAiACkALAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgATABvAGMAYQBsAEoARABOACkAKQAgACsAIAAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgATABvAGMAYQBsAFQAaQBtAGUAKQApACAAKgAgACgATABvAGMAYQBsAFQAaQBtAGUAIAA8AD4AIABcACIAXAAiACkAKQAgACsAIAAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0ACkAKQAgACoAIAAoAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdAAgADwAPgAgAFwAIgBcACIAKQApACwAIAB7ACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABNAE8ARAAoAEwAbwBjAGEAbABKAEQATgAsACAAMQApACAAPgAgADAALAAgAHsAIwBOAFUATQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AHoAbwAsACAATgAoAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdAApACAALwAgADEANAA0ADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAEEAQgBTACgAXwB0AHoAbwApACAAPgAgADAALgA2ADIANQAsACAAewAjAE4AVQBNACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAG8AYwBhAGwASgBEAE4AIAAtACAAMAAuADUAIAArACAATgAoAEwAbwBjAGEAbABUAGkAbQBlACkAIAAtACAAXwB0AHoAbwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEoARABBAFQARQBfAFQATwBfAEoARABOAF8AVQBUAEMAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIABKAHUAbABpAGEAbgAgAEQAYQB5ACAATgB1AG0AYgBlAHIAIABhAG4AZAAgAHQAaQBtAGUAIABvAGYAIABkAGEAeQAgAGkAbgAgAFUAVABDACAAbwBmACAAYQAgAGcAaQB2AGUAbgAgAEoAdQBsAGkAYQBuACAARABhAHQAZQAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABpAG4AdABlAGcAZQByACAAIAAgACAAIAAgACAAIAB8ACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByAFwAbgAgADIAIAB8ACAAZABlAGMAaQBtAGEAbAAgAFsAMAAuAC4AMQApACAAfAAgAFQAaQBtAGUAIABvAGYAIABkAGEAeQAgAGkAbgAgAFUAVABDAC4AIABEAGUAYwBpAG0AYQBsACAAZgByAGEAYwB0AGkAbwBuACwAIABpAG0AcABsAGkAYwBpAHQAbAB5ACAAYwBvAG4AdgBlAHIAdABzACAAdABvACAARQB4AGMAZQBsACAARABhAHQAZQAvAFQAaQBtAGUAIAB0AHkAcABlAC4AXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBKAEQAYQB0AGUAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIABKAHUAbABpAGEAbgAgAEQAYQB0AGUAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEoARABBAFQARQBfAFQATwBfAEoARABOAF8AVQBUAEMAIAA9ACAATABBAE0AQgBEAEEAKABKAEQAYQB0AGUALABcAG4AIAAgACAAIABJAEYAKABKAEQAYQB0AGUAIAA9ACAAXAAiAFwAIgAsACAAewBcACIAXAAiACwAIABcACIAXAAiAH0ALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgASgBEAGEAdABlACkAKQAsACAAewAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaABpAGYAdABVAFQAQwAsACAASgBEAGEAdABlACAAKwAgADAALgA1ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBKAEQATgAsACAASQBOAFQAKABfAHMAaABpAGYAdABVAFQAQwApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBVAFQAQwAsACAAXwBzAGgAaQBmAHQAVQBUAEMAIAAtACAAXwBKAEQATgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXwBKAEQATgAsACAAXwBVAFQAQwApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ASgBEAEEAVABFAF8AVABPAF8ASgBEAE4AXwBMAE8AQwBBAEwAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIABsAG8AYwBhAGwAIABKAHUAbABpAGEAbgAgAEQAYQB5ACAATgB1AG0AYgBlAHIAIABhAG4AZAAgAHQAaQBtAGUAIABvAGYAIABkAGEAeQAgAG8AZgAgAGEAIABnAGkAdgBlAG4AIABKAHUAbABpAGEAbgAgAEQAYQB0AGUALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAaQBuAHQAZQBnAGUAcgAgACAAIAAgACAAIAAgACAAfAAgAEwAbwBjAGEAbAAgAEoAdQBsAGkAYQBuACAARABhAHkAIABOAHUAbQBiAGUAcgBcAG4AIAAyACAAfAAgAGQAZQBjAGkAbQBhAGwAIABbADAALgAuADEAKQAgAHwAIABMAG8AYwBhAGwAIAB0AGkAbQBlACAAbwBmACAAZABhAHkALgAgAEQAZQBjAGkAbQBhAGwAIABmAHIAYQBjAHQAaQBvAG4ALAAgAGkAbQBwAGwAaQBjAGkAdABsAHkAIABjAG8AbgB2AGUAcgB0AHMAIAB0AG8AIABFAHgAYwBlAGwAIABEAGEAdABlAC8AVABpAG0AZQAgAHQAeQBwAGUALgBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEoARABhAHQAZQAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgACAAIAAgACAAfAAgAEoAdQBsAGkAYQBuACAARABhAHQAZQBcAG4AWwBUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQAXQAgAHwAIABkAGUAYwBpAG0AYQBsACAAIAAgACAAIAB8ACAAVABpAG0AZQAgAHoAbwBuAGUAIABvAGYAZgBzAGUAdAAgAGkAbgAgAG0AaQBuAHUAdABlAHMAIABmAHIAbwBtACAAVQBUAEMALgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABbAC0AOQAwADAALgAuADkAMAAwAF0AIAB8ACAAQQBzAHMAdQBtAGUAZAAgAHQAbwAgAGIAZQAgAFUAVABDACAAaQBmACAAbwBtAG0AaQB0AHQAZQBkAC4AXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEoARABBAFQARQBfAFQATwBfAEoARABOAF8ATABPAEMAQQBMACAAPQAgAEwAQQBNAEIARABBACgASgBEAGEAdABlACwAIABbAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdABdACwAXABuACAAIAAgACAASQBGACgASgBEAGEAdABlACAAPQAgAFwAIgBcACIALAAgAHsAXAAiAFwAIgAsACAAXAAiAFwAIgB9ACwAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEoARABhAHQAZQApACkAIAArACAAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdAApACkAIAAqACAAKABUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQAIAA8AD4AIABcACIAXAAiACkAKQAsACAAewAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBvACwAIABOACgAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0ACkAIAAvACAAMQA0ADQAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAEEAQgBTACgAXwB0AHoAbwApACAAPgAgADAALgA2ADIANQAsACAAewAjAE4AVQBNACEALAAgACMATgBVAE0AIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGgAaQBmAHQATABvAGMAYQBsACwAIABKAEQAYQB0AGUAIAArACAAMAAuADUAIAArACAAXwB0AHoAbwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGwAbwBjAGEAbABKAEQATgAsACAASQBOAFQAKABfAHMAaABpAGYAdABMAG8AYwBhAGwAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGwAbwBjAGEAbABUAGkAbQBlACwAIABfAHMAaABpAGYAdABMAG8AYwBhAGwAIAAtACAAXwBsAG8AYwBhAGwASgBEAE4ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABfAGwAbwBjAGEAbABKAEQATgAsACAAXwBsAG8AYwBhAGwAVABpAG0AZQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ASgBVAEwASQBBAE4AXwBEAEEAVABFAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAHQAaABlACAASgB1AGwAaQBhAG4AIABEAGEAdABlACAAbwBmACAAdABoAGUAIABwAHIAbwB2AGkAZABlAGQAIABjAGEAbABlAG4AZABhAHIAIABkAGEAdABlACAAYQBuAGQAIAB0AGkAbQBlACAAbwBmACAAZABhAHkALgBcAG4ATgBvAHQAZQAgAEoAdQBsAGkAYQBuACAARABhAHQAZQBzACAAYQByAGUAIABhAGwAdwBhAHkAcwAgAGkAbgAgAFUAVABDAC4AXABuAFwAbgBPAHUAdABwAHUAdABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAASgB1AGwAaQBhAG4AIABEAGEAdABlAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AWQBlAGEAcgBDAEUAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAIAAgACAAIAAgACAAIAAgAHwAIABZAGUAYQByACAAaQBuACAAQwBvAG0AbQBvAG4AIABFAHIAYQAuACAATgBvAHQAZQAgAHQAaABhAHQAIAAxACAAQgBDACAAPQAgADAAIABDAEUALAAgADIAIABCAEMAIAA9ACAALQAxACAAQwBFAFwAbgBNAG8AbgB0AGgAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADEALgAuADEAMgBdACAAfAAgAE0AbwBuAHQAaABcAG4ARABhAHkAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAWwAxAC4ALgAzADEAXQAgAHwAIABEAGEAeQBcAG4AVABpAG0AZQAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAWwAwAC4ALgAxACkAIAAgAHwAIABUAGkAbQBlACAAbwBmACAAZABhAHkAIABhAHMAIABkAGUAYwBpAG0AYQBsACAAZgByAGEAYwB0AGkAbwBuACAAbwByACAARQB4AGMAZQBsACAARABhAHQAZQAvAFQAaQBtAGUAIAB0AHkAcABlAC4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAQwBhAHIAcgBpAGUAcwAgAGkAZgAgAHIAYQBuAGcAZQAgAGkAcwAgAGUAeABjAGUAZQBkAGUAZAAuAFwAbgBbAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdABdACAAfAAgAGQAZQBjAGkAbQBhAGwAIAAgACAAIAAgACAAIAAgACAAfAAgAFQAaQBtAGUAIAB6AG8AbgBlACAAbwBmAGYAcwBlAHQAIABpAG4AIABtAGkAbgB1AHQAZQBzACAAZgByAG8AbQAgAFUAVABDAC4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAWwAtADkAMAAwAC4ALgA5ADAAMABdACAAIAAgACAAIAB8ACAAQQBzAHMAdQBtAGUAZAAgAHQAbwAgAGIAZQAgAFUAVABDACAAaQBmACAAbwBtAG0AaQB0AHQAZQBkAC4AXABuAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0AIAB8ACAAcwB3AGkAdABjAGgAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAQwBhAGwAYwB1AGwAYQB0AGUAIABpAG4AIAB0AGgAZQAgAEoAdQBsAGkAYQBuACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgAgAEQAZQBmAGEAdQBsAHQAIABpAHMAIABHAHIAZQBnAG8AcgBpAGEAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBKAFUATABJAEEATgBfAEQAQQBUAEUAIAA9ACAATABBAE0AQgBEAEEAKABZAGUAYQByAEMARQAsACAATQBvAG4AdABoACwAIABEAGEAeQAsACAAVABpAG0AZQAsACAAWwBUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQAXQAsACAAWwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAsAFwAbgAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAF8AVgBBAEwASQBEAF8ARABBAFQARQAoAFkAZQBhAHIAQwBFACwAIABNAG8AbgB0AGgALAAgAEQAYQB5ACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQApACwAIAB7ACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgATQBPAEQAKABEAGEAeQAsACAAMQApACAAPgAgADAALAAgAHsAIwBOAFUATQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBvACwAIABOACgAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABBAEIAUwAoAF8AdAB6AG8AKQAgAD4AIAA5ADAAMAAsACAAewAjAE4AVQBNACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkAUABhAHIAdAAsACAASQBOAFQAKABOACgAVABpAG0AZQApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AG8AZAAsACAATgAoAFQAaQBtAGUAKQAgAC0AIABfAGQAYQB5AFAAYQByAHQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBqAGQAbgAsACAAXwBkAGEAeQBQAGEAcgB0ACAAKwAgAEoAVQBMAEkAQQBOAF8ARABBAFkAXwBOAFUATQBCAEUAUgAoAFkAZQBhAHIAQwBFACwAIABNAG8AbgB0AGgALAAgAEQAYQB5ACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABKAEQATgBfAEwATwBDAEEATABfAFQATwBfAEoARABBAFQARQAoAF8AagBkAG4ALAAgAF8AdABvAGQALAAgAF8AdAB6AG8AKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEMAQQBMAEUATgBEAEEAUgBfAEYAUgBPAE0AXwBKAEQAQQBUAEUAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIABjAGEAbABlAG4AZABhAHIAIABkAGEAdABlACAAYQBuAGQAIABsAG8AYwBhAGwAIAB0AGkAbQBlACAAbwBmACAAZABhAHkAIABmAG8AcgAgAGEAIABnAGkAdgBlAG4AIABKAHUAbABpAGEAbgAgAEQAYQB0AGUAIABhAG4AZAAgAHQAaQBtAGUAIAB6AG8AbgBlACAAbwBmAGYAcwBlAHQALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAaQBuAHQAZQBnAGUAcgAgACAAIAAgACAAIAAgACAAIAB8ACAAWQBlAGEAcgBDAEUAXABuACAAMgAgAHwAIABpAG4AdABlAGcAZQByACAAWwAxAC4ALgAxADIAXQAgAHwAIABNAG8AbgB0AGgAXABuACAAMwAgAHwAIABpAG4AdABlAGcAZQByACAAWwAxAC4ALgAzADEAXQAgAHwAIABEAGEAeQBcAG4AIAA0ACAAfAAgAGQAZQBjAGkAbQBhAGwAIABbADAALgAuADEAKQAgACAAfAAgAEwAbwBjAGEAbAAgAHQAaQBtAGUAIABvAGYAIABkAGEAeQAuACAARABlAGMAaQBtAGEAbAAgAGYAcgBhAGMAdABpAG8AbgAsACAAaQBtAHAAbABpAGMAaQB0AGwAeQAgAGMAbwBuAHYAZQByAHQAcwAgAHQAbwAgAEUAeABjAGUAbAAgAEQAYQB0AGUALwBUAGkAbQBlACAAdAB5AHAAZQAuAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ASgBEAGEAdABlACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAIAAgACAAIAB8ACAASgB1AGwAaQBhAG4AIABEAGEAdABlAC4AIABOAG8AdABlACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMAIABhAHIAZQAgAGEAbAB3AGEAeQBzACAAaQBuACAAVQBUAEMALgBcAG4AWwBUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQAXQAgAHwAIABkAGUAYwBpAG0AYQBsACAAIAAgACAAIAB8ACAAVABpAG0AZQAgAHoAbwBuAGUAIABvAGYAZgBzAGUAdAAgAGkAbgAgAG0AaQBuAHUAdABlAHMAIABmAHIAbwBtACAAVQBUAEMALgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABbAC0AOQAwADAALgAuADkAMAAwAF0AIAB8ACAAQQBzAHMAdQBtAGUAZAAgAHQAbwAgAGIAZQAgAFUAVABDACAAaQBmACAAbwBtAG0AaQB0AHQAZQBkAC4AXABuAFsAUAByAGUAYwBpAHMAaQBvAG4AXQAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgACAAIAAgACAAfAAgAFMAZQBsAGUAYwB0ACAAcAByAGUAYwBpAHMAaQBvAG4AIABsAGUAdgBlAGwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAwACAALQAgAEYAbABvAGEAdABpAG4AZwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADEAIAAtACAARABhAHkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAyACAALQAgAEgAbwB1AHIAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAzACAALQAgAE0AaQBuAHUAdABlAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAANAAgAC0AIABTAGUAYwBvAG4AZABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADUAIAAtACAATQBpAGwAbABpAHMAZQBjAG8AbgBkAFwAbgBbAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACAAfAAgAHMAdwBpAHQAYwBoACAAIAAgACAAIAAgAHwAIABDAGEAbABjAHUAbABhAHQAZQAgAGkAbgAgAHQAaABlACAASgB1AGwAaQBhAG4AIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuACAARABlAGYAYQB1AGwAdAAgAGkAcwAgAEcAcgBlAGcAbwByAGkAYQBuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBDAEEATABFAE4ARABBAFIAXwBGAFIATwBNAF8ASgBEAEEAVABFACAAPQAgAEwAQQBNAEIARABBACgASgBEAGEAdABlACwAIABbAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdABdACwAIABbAFAAcgBlAGMAaQBzAGkAbwBuAF0ALAAgAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0ALABcAG4AIAAgACAAIABJAEYAKABKAEQAYQB0AGUAIAA9ACAAXAAiAFwAIgAsACAAewBcACIAXAAiACwAIABcACIAXAAiACwAIABcACIAXAAiACwAIABcACIAXAAiAH0ALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgASgBEAGEAdABlACkAKQAsACAAewAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGoAZABuAEwAbwBjAGEAbAAsACAASgBEAEEAVABFAF8AVABPAF8ASgBEAE4AXwBMAE8AQwBBAEwAKABKAEQAYQB0AGUALAAgAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgASQBTAEUAUgBSAE8AUgAoAEkATgBEAEUAWAAoAF8AagBkAG4ATABvAGMAYQBsACwAIAAxACwAIAAxACkAKQAsACAAewAjAE4AVQBNACEALAAgACMATgBVAE0AIQAsACAAIwBOAFUATQAhACwAIAAjAE4AVQBNACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBwAHIAZQBjAGkAcwBpAG8AbgAsACAATgAoAFAAcgBlAGMAaQBzAGkAbwBuACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBsAG8AYwBhAGwAVABpAG0AZQAsACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHAAcgBlAGMAaQBzAGkAbwBuACAAPAA9ACAAMAAsACAASQBOAEQARQBYACgAXwBqAGQAbgBMAG8AYwBhAGwALAAgADEALAAgADIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcAByAGUAYwBpAHMAaQBvAG4AIAA9ACAAMQAsACAAUgBPAFUATgBEACgASQBOAEQARQBYACgAXwBqAGQAbgBMAG8AYwBhAGwALAAgADEALAAgADIAKQAsACAAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBwAHIAZQBjAGkAcwBpAG8AbgAgAD0AIAAyACwAIABSAE8AVQBOAEQAKABJAE4ARABFAFgAKABfAGoAZABuAEwAbwBjAGEAbAAsACAAMQAsACAAMgApACAAKgAgADIANAAsACAAMAApACAALwAgADIANAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcAByAGUAYwBpAHMAaQBvAG4AIAA9ACAAMwAsACAAUgBPAFUATgBEACgASQBOAEQARQBYACgAXwBqAGQAbgBMAG8AYwBhAGwALAAgADEALAAgADIAKQAgACoAIAAxADQANAAwACwAIAAwACkAIAAvACAAMQA0ADQAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcAByAGUAYwBpAHMAaQBvAG4AIAA9ACAANAAsACAAUgBPAFUATgBEACgASQBOAEQARQBYACgAXwBqAGQAbgBMAG8AYwBhAGwALAAgADEALAAgADIAKQAgACoAIAA4ADYANAAwADAALAAgADAAKQAgAC8AIAA4ADYANAAwADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAIABSAE8AVQBOAEQAKABJAE4ARABFAFgAKABfAGoAZABuAEwAbwBjAGEAbAAsACAAMQAsACAAMgApACAAKgAgADgANgA0ADAAMAAsACAAMwApACAALwAgADgANgA0ADAAMABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHIATABvAGMAYQBsAFQAaQBtAGUALAAgAE0ATwBEACgAXwBsAG8AYwBhAGwAVABpAG0AZQAsACAAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcgBKAEQATgAsACAASQBOAEQARQBYACgAXwBqAGQAbgBMAG8AYwBhAGwALAAgADEALAAgADEAKQAgACsAIABJAE4AVAAoAF8AbABvAGMAYQBsAFQAaQBtAGUAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGwAbwBjAGEAbABEAGEAdABlACwAIABKAEQATgBfAFQATwBfAEMAQQBMAEUATgBEAEEAUgBfAEQAQQBUAEUAKABfAHIASgBEAE4ALAAgAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXwBsAG8AYwBhAGwARABhAHQAZQAsACAAXwByAEwAbwBjAGEAbABUAGkAbQBlACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBUAEkATQBFAF8ARABFAEMASQBNAEEATABfAFQATwBfAEgATQBTAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAHQAaABlACAAMgA0ACAAaABvAHUAcgAgAHQAaQBtAGUAawBlAGUAcABpAG4AZwAgAHIAZQBwAHIAZQBzAGUAbgB0AGEAdABpAG8AbgAgAG8AZgAgAGEAIABkAGUAYwBpAG0AYQBsACAAdABpAG0AZQAgAHYAYQBsAHUAZQAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABpAG4AdABlAGcAZQByACAAWwAtADEALAAwACwAMQBdACAAfAAgAFMAaQBnAG4AXABuACAAMgAgAHwAIABpAG4AdABlAGcAZQByACAAWwAwAC4ALgBdACAAIAAgACAAfAAgAEgAbwB1AHIAcwBcAG4AIAAzACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADAALgAuADUAOQBdACAAIAB8ACAATQBpAG4AdQB0AGUAcwBcAG4AIAA0ACAAfAAgAGQAZQBjAGkAbQBhAGwAIABbADAALgAuADYAMAApACAAIAB8ACAAUwBlAGMAbwBuAGQAcwBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFQAaQBtAGUAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIABUAGkAbQBlACAAYQBzACAAZgByAGEAYwB0AGkAbwBuACAAbwBmACAAYQAgAGQAYQB5ACAAKAAyADQAIABoAG8AdQByAHMAKQAuACAASQBtAHAAbABpAGMAaQB0AGwAeQAgAGMAbwBuAHYAZQByAHQAcwAgAGYAcgBvAG0AIABFAHgAYwBlAGwAIABEAGEAdABlAC8AVABpAG0AZQAgAHQAeQBwAGUAIABmAG8AcgBcAG4AIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgAG4AbwBuAC0AbgBlAGcAYQB0AGkAdgBlACAAdgBhAGwAdQBlAHMALgAgAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBUAEkATQBFAF8ARABFAEMASQBNAEEATABfAFQATwBfAEgATQBTACAAPQAgAEwAQQBNAEIARABBACgAVABpAG0AZQAsAFwAbgAgACAAIAAgAEkARgAoAFQAaQBtAGUAIAA9ACAAXAAiAFwAIgAsACAAewBcACIAXAAiACwAIABcACIAXAAiACwAIABcACIAXAAiACwAIABcACIAXAAiAH0ALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgAVABpAG0AZQApACkALAAgAHsAIwBWAEEATABVAEUAIQAsACAAIwBWAEEATABVAEUAIQAsACAAIwBWAEEATABVAEUAIQAsACAAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAcgBvAHUAbgBkACAAdABvACAAbQBpAGwAbABpAHMAZQBjAG8AbgBkAHMALAAgAHMAYwBhAGwAZQAgAHQAbwAgAHMAZQBjAG8AbgBkAHMAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGUAYwBvAG4AZABzACwAIABSAE8AVQBOAEQAKABUAGkAbQBlACAAKgAgADgANgA0ADAAMAAsACAAMwApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBzAGUAYwBvAG4AZABzACAAPQAgADAALAAgAHsAMAAsACAAMAAsACAAMAAsACAAMAB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaQBnAG4ALAAgAFMASQBHAE4AKABfAHMAZQBjAG8AbgBkAHMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGEAYgBzAFMAZQBjAG8AbgBkAHMALAAgAEEAQgBTACgAXwBzAGUAYwBvAG4AZABzACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGUAYwBvAG4AZABQAGEAcgB0ACwAIABNAE8ARAAoAF8AYQBiAHMAUwBlAGMAbwBuAGQAcwAsACAANgAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBtAGkAbgB1AHQAZQBzACwAIABJAE4AVAAoACgAXwBhAGIAcwBTAGUAYwBvAG4AZABzACAALQAgAF8AcwBlAGMAbwBuAGQAUABhAHIAdAApACAALwAgADYAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbQBpAG4AdQB0AGUAUABhAHIAdAAsACAATQBPAEQAKABfAG0AaQBuAHUAdABlAHMALAAgADYAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AaABvAHUAcgBQAGEAcgB0ACwAIABJAE4AVAAoACgAXwBtAGkAbgB1AHQAZQBzACAALQAgAF8AbQBpAG4AdQB0AGUAUABhAHIAdAApACAALwAgADYAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGkAZwBuACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBoAG8AdQByAFAAYQByAHQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AaQBuAHUAdABlAFAAYQByAHQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAZQBjAG8AbgBkAFAAYQByAHQAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBIAE0AUwBfAFQATwBfAFQASQBNAEUAXwBEAEUAQwBJAE0AQQBMAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAGEAIABkAGUAYwBpAG0AYQBsACAAdABpAG0AZQAgAGEAcwAgAGEAIABmAHIAYQBjAHQAaQBvAG4AIABvAGYAIABhACAAZABhAHkAIABmAHIAbwBtACAAYQAgADIANAAgAGgAbwB1AHIAIAB0AGkAbQBlAGsAZQBlAHAAaQBuAGcAIAB2AGEAbAB1AGUAIABvAGYAIAB0AGkAbQBlAC4AXABuAFwAbgBPAHUAdABwAHUAdABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAASQBtAHAAbABpAGMAaQB0AGwAeQAgAGMAbwBuAHYAZQByAHQAcwAgAHQAbwAgAEUAeABjAGUAbAAgAEQAYQB0AGUALwBUAGkAbQBlACAAdAB5AHAAZQAgAGYAbwByACAAbgBvAG4ALQBuAGUAZwBhAHQAaQB2AGUAIAB2AGEAbAB1AGUAcwAuAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AUwBpAGcAbgAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAWwAtADEALAAwACwAMQBdACAAfABcAG4ASABvAHUAcgBzACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAWwAwAC4ALgBdACAAIAAgACAAfABcAG4ATQBpAG4AdQB0AGUAcwAgAHwAIABpAG4AdABlAGcAZQByACAAWwAwAC4ALgA1ADkAXQAgACAAfABcAG4AUwBlAGMAbwBuAGQAcwAgAHwAIABkAGUAYwBpAG0AYQBsACAAWwAwAC4ALgA2ADAAKQAgACAAfABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ASABNAFMAXwBUAE8AXwBUAEkATQBFAF8ARABFAEMASQBNAEEATAAgAD0AIABMAEEATQBCAEQAQQAoAFMAaQBnAG4ALAAgAEgAbwB1AHIAcwAsACAATQBpAG4AdQB0AGUAcwAsACAAUwBlAGMAbwBuAGQAcwAsAFwAbgAgACAAIAAgAEkARgAoACgASABvAHUAcgBzACAAPQAgAFwAIgBcACIAKQAgACoAIAAoAE0AaQBuAHUAdABlAHMAIAA9ACAAXAAiAFwAIgApACAAKgAgACgAUwBlAGMAbwBuAGQAcwAgAD0AIABcACIAXAAiACkALAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABTAGkAZwBuACkAKQAgACoAIAAoAFMAaQBnAG4AIAA8AD4AIABcACIAXAAiACkAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKwAgACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABIAG8AdQByAHMAKQApACAAKgAgACgASABvAHUAcgBzACAAPAA+ACAAXAAiAFwAIgApACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACsAIAAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgATQBpAG4AdQB0AGUAcwApACkAIAAqACAAKABNAGkAbgB1AHQAZQBzACAAPAA+ACAAXAAiAFwAIgApACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACsAIAAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgAUwBlAGMAbwBuAGQAcwApACkAIAAqACAAKABTAGUAYwBvAG4AZABzACAAPAA+ACAAXAAiAFwAIgApACkALAAgAHsAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBoAG8AdQByAHMALAAgAE4AKABIAG8AdQByAHMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbQBpAG4AdQB0AGUAcwAsACAATgAoAE0AaQBuAHUAdABlAHMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBlAGMAbwBuAGQAcwAsACAATgAoAFMAZQBjAG8AbgBkAHMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoACgAXwBoAG8AdQByAHMAIAA9ACAAMAApACAAKgAgACgAXwBtAGkAbgB1AHQAZQBzACAAPQAgADAAKQAgACoAIAAoAF8AcwBlAGMAbwBuAGQAcwAgAD0AIAAwACkALAAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBpAGcAbgAsACAASQBGACgATgAoAFMAaQBnAG4AKQAgADwAIAAwACwAIAAtADEALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaQBnAG4AIAAqACAAKAAoAF8AaABvAHUAcgBzACAALwAgADIANAApACAAKwAgACgAXwBtAGkAbgB1AHQAZQBzACAALwAgADEANAA0ADAAKQAgACsAIAAoAF8AcwBlAGMAbwBuAGQAcwAgAC8AIAA4ADYANAAwADAAKQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AQQBEAEQAXwBUAEkATQBFAFMAUABBAE4AXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIABKAHUAbABpAGEAbgAgAEQAYQB0AGUAIABvAGYAIAB0AGgAZQAgAGEAZABkAGkAdABpAG8AbgAgAG8AZgAgAHQAaABlACAAcAByAG8AdgBpAGQAZQBkACAAYwBhAGwAZQBuAGQAYQByACAAZABhAHQAZQAgAGEAbgBkACAAdABpAG0AZQAgAG8AZgAgAGQAYQB5ACAAYQBuAGQAIABhACAAdABpAG0AZQBzAHAAYQBuACAAYwBvAG0AcABsAGkAYwBhAHQAaQBvAG4ALgBcAG4ATgBvAHQAZQAgAEoAdQBsAGkAYQBuACAARABhAHQAZQBzACAAYQByAGUAIABhAGwAdwBhAHkAcwAgAGkAbgAgAFUAVABDAC4AXABuAFwAbgBPAHUAdABwAHUAdABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAASgB1AGwAaQBhAG4AIABEAGEAdABlAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AWQBlAGEAcgBDAEUAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAIAAgACAAIAAgACAAIAAgAHwAIABZAGUAYQByACAAaQBuACAAQwBvAG0AbQBvAG4AIABFAHIAYQAuACAATgBvAHQAZQAgAHQAaABhAHQAIAAxACAAQgBDACAAPQAgADAAIABDAEUALAAgADIAIABCAEMAIAA9ACAALQAxACAAQwBFAFwAbgBNAG8AbgB0AGgAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADEALgAuADEAMgBdACAAfAAgAE0AbwBuAHQAaABcAG4ARABhAHkAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAWwAxAC4ALgAzADEAXQAgAHwAIABEAGEAeQBcAG4AVABpAG0AZQAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAWwAwAC4ALgAxACkAIAAgAHwAIABMAG8AYwBhAGwAIAB0AGkAbQBlACAAbwBmACAAZABhAHkAIABhAHMAIABkAGUAYwBpAG0AYQBsACAAZgByAGEAYwB0AGkAbwBuACAAbwByACAARQB4AGMAZQBsACAARABhAHQAZQAvAFQAaQBtAGUAIAB0AHkAcABlAC4AXABuAEEAZABkAFkAZQBhAHIAcwAgACAAIAAgACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgACAAIAAgACAAIAAgACAAIAB8ACAAQQBkAGQAIAB5AGUAYQByAHMAIAB0AGkAbQBlAHMAcABhAG4ALgAgAEYAcgBhAGMAdABpAG8AbgBhAGwAIABwAGEAcgB0ACAAYwBhAHIAcgBpAGUAcwAgAHQAbwAgAG0AbwBuAHQAaAAgAGEAbgBkACAAZABhAHkALgBcAG4AQQBkAGQATQBvAG4AdABoAHMAIAAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAIAAgACAAIAAgACAAIAAgAHwAIABBAGQAZAAgAG0AbwBuAHQAaABzACAAdABpAG0AZQBzAHAAYQBuAC4AIABGAHIAYQBjAHQAaQBvAG4AYQBsACAAcABhAHIAdAAgAGMAYQByAHIAaQBlAHMAIAB0AG8AIABkAGEAeQAuAFwAbgBBAGQAZABEAGEAeQBzACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAAgACAAIAAgACAAIAAgACAAfAAgAEEAZABkACAAZABhAHkAcwAgAHQAaQBtAGUAcwBwAGEAbgAuACAARgByAGEAYwB0AGkAbwBuAGEAbAAgAHAAYQByAHQAIABjAGEAcgByAGkAZQBzACAAdABvACAAdABpAG0AZQAuAFwAbgBBAGQAZABUAGkAbQBlACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAAgACAAIAAgACAAIAAgACAAfAAgAEEAZABkACAAdABpAG0AZQBzAHAAYQBuAC4AXABuAFsAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0AF0AIAB8ACAAZABlAGMAaQBtAGEAbAAgACAAIAAgACAAIAAgACAAIAB8ACAAVABpAG0AZQAgAHoAbwBuAGUAIABvAGYAZgBzAGUAdAAgAGkAbgAgAG0AaQBuAHUAdABlAHMAIABmAHIAbwBtACAAVQBUAEMALgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABbAC0AOQAwADAALgAuADkAMAAwAF0AIAAgACAAIAAgAHwAIABBAHMAcwB1AG0AZQBkACAAdABvACAAYgBlACAAVQBUAEMAIABpAGYAIABvAG0AbQBpAHQAdABlAGQALgBcAG4AWwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAgAHwAIABzAHcAaQB0AGMAaAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABDAGEAbABjAHUAbABhAHQAZQAgAGkAbgAgAHQAaABlACAASgB1AGwAaQBhAG4AIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuACAARABlAGYAYQB1AGwAdAAgAGkAcwAgAEcAcgBlAGcAbwByAGkAYQBuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEEARABEAF8AVABJAE0ARQBTAFAAQQBOACAAPQAgAEwAQQBNAEIARABBACgAWQBlAGEAcgBDAEUALAAgAE0AbwBuAHQAaAAsACAARABhAHkALAAgAFQAaQBtAGUALAAgAEEAZABkAFkAZQBhAHIAcwAsACAAQQBkAGQATQBvAG4AdABoAHMALAAgAEEAZABkAEQAYQB5AHMALAAgAEEAZABkAFQAaQBtAGUALAAgAFsAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0AF0ALAAgAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0ALABcAG4AIAAgACAAIABJAEYAKAAoAFkAZQBhAHIAQwBFACAAPQAgAFwAIgBcACIAKQAgACoAIAAoAE0AbwBuAHQAaAAgAD0AIABcACIAXAAiACkAIAAqACAAKABEAGEAeQAgAD0AIABcACIAXAAiACkAIAAqACAAKABUAGkAbQBlACAAPQAgAFwAIgBcACIAKQAsACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABZAGUAYQByAEMARQApACkAIAArACAATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABNAG8AbgB0AGgAKQApACAAKwAgAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgARABhAHkAKQApACwAIAB7ACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBfAFYAQQBMAEkARABfAEQAQQBUAEUAKABZAGUAYQByAEMARQAsACAATQBvAG4AdABoACwAIABEAGEAeQAsACAASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByACkAKQAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABNAE8ARAAoAEQAYQB5ACwAIAAxACkAIAA+ACAAMAAsACAAewAjAE4AVQBNACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AHoAbwAsACAATgAoAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAEEAQgBTACgAXwB0AHoAbwApACAAPgAgADkAMAAwACwAIAB7ACMATgBVAE0AIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYQBkAGQAWQBlAGEAcgBzACwAIABJAE4AVAAoAE4AKABBAGQAZABZAGUAYQByAHMAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGYAQQBkAGQAWQBlAGEAcgBzACwAIABOACgAQQBkAGQAWQBlAGEAcgBzACkAIAAtACAAXwBhAGQAZABZAGUAYQByAHMALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBNAG8AbgB0AGgAcwAsACAATgAoAEEAZABkAE0AbwBuAHQAaABzACkAIAArACAAKABfAGYAQQBkAGQAWQBlAGEAcgBzACAAKgAgADEAMgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGEAZABkAE0AbwBuAHQAaABzACwAIABJAE4AVAAoAF8AcwBNAG8AbgB0AGgAcwApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGYAQQBkAGQATQBvAG4AdABoAHMALAAgAF8AcwBNAG8AbgB0AGgAcwAgAC0AIABfAGEAZABkAE0AbwBuAHQAaABzACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHoATQBvAG4AdABoAHMALAAgAE0AbwBuAHQAaAAgACsAIABfAGEAZABkAE0AbwBuAHQAaABzACAALQAgADEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcgBNAG8AbgB0AGgALAAgAE0ATwBEACgAXwB6AE0AbwBuAHQAaABzACwAIAAxADIAKQAgACsAIAAxACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHIAWQBlAGEAcgAsACAAWQBlAGEAcgBDAEUAIAArACAAXwBhAGQAZABZAGUAYQByAHMAIAArACAASQBOAFQAKABfAHoATQBvAG4AdABoAHMAIAAvACAAMQAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYQB2AGcARABhAHkAcwBNAG8AbgB0AGgALAAgAEkARgAoAE4AKABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsACAAMwAwAC4ANAAzADcANQAsACAAMwAwAC4ANAAzADYAOAA3ADUAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBtAEQAYQB5AHMALAAgAFIATwBVAE4ARAAoAF8AZgBBAGQAZABNAG8AbgB0AGgAcwAgACoAIABfAGEAdgBnAEQAYQB5AHMATQBvAG4AdABoACwAIAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYgBhAHMAZQBKAEQAYQB0AGUALAAgAEoAVQBMAEkAQQBOAF8ARABBAFQARQAoAF8AcgBZAGUAYQByACwAIABfAHIATQBvAG4AdABoACwAIAAxACwAIAAwACwAIABfAHQAegBvACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAgAC0AIAAxACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMARABhAHkAcwAsACAARABhAHkAIAArACAAXwBtAEQAYQB5AHMAIAArACAATgAoAEEAZABkAEQAYQB5AHMAKQAgACsAIABOACgAVABpAG0AZQApACAAKwAgAE4AKABBAGQAZABUAGkAbQBlACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYgBhAHMAZQBKAEQAYQB0AGUAIAArACAAXwBzAEQAYQB5AHMAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFIARQBTAE8ATABWAEUAXwBEAEEAVABFAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAGEAIABjAGEAbABlAG4AZABhAHIAIABkAGEAdABlACAAZgByAG8AbQAgAHAAcgBvAHYAaQBkAGUAZAAgAGQAZQBjAGkAbQBhAGwAIAB5AGUAYQByACwAIABtAG8AbgB0AGgAcwAsACAAZABhAHkAcwAgAGEAbgBkACAAdABpAG0AZQAuAFwAbgBOAG8AdABlACAAbQBvAG4AdABoAHMAIABhAG4AZAAgAGQAYQB5AHMAIABhAHIAZQAgAG4AbwB0ACAAYgBvAHUAbgBkAGUAZAAgAGIAeQAgAHQAaABlACAAYwBhAGwAZQBuAGQAYQByAC4AXABuAFwAbgBPAHUAdABwAHUAdABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAGkAbgB0AGUAZwBlAHIAIAAgACAAIAAgACAAIAAgACAAfAAgAFkAZQBhAHIAQwBFAFwAbgAgADIAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMQAuAC4AMQAyAF0AIAB8ACAATQBvAG4AdABoAFwAbgAgADMAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMQAuAC4AMwAxAF0AIAB8ACAARABhAHkAXABuACAANAAgAHwAIABkAGUAYwBpAG0AYQBsACAAWwAwAC4ALgAxACkAXQAgAHwAIABMAG8AYwBhAGwAIAB0AGkAbQBlACAAbwBmACAAZABhAHkALgAgAEQAZQBjAGkAbQBhAGwAIABmAHIAYQBjAHQAaQBvAG4ALAAgAGkAbQBwAGwAaQBjAGkAdABsAHkAIABjAG8AbgB2AGUAcgB0AHMAIAB0AG8AIABFAHgAYwBlAGwAIABEAGEAdABlAC8AVABpAG0AZQAgAHQAeQBwAGUALgBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFkAZQBhAHIAQwBFACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIABZAGUAYQByACAAaQBuACAAQwBvAG0AbQBvAG4AIABFAHIAYQAuACAATgBvAHQAZQAgAHQAaABhAHQAIAAxACAAQgBDACAAPQAgADAAIABDAEUALAAgADIAIABCAEMAIAA9ACAALQAxACAAQwBFAFwAbgBNAG8AbgB0AGgAcwAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAATQBvAG4AdABoAHMAXABuAEQAYQB5AHMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIABEAGEAeQBzAFwAbgBUAGkAbQBlACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAATABvAGMAYQBsACAAdABpAG0AZQAgAG8AZgAgAGQAYQB5ACAAYQBzACAAZABlAGMAaQBtAGEAbAAgAGYAcgBhAGMAdABpAG8AbgAgAG8AcgAgAEUAeABjAGUAbAAgAEQAYQB0AGUALwBUAGkAbQBlACAAdAB5AHAAZQAuAFwAbgBbAFAAcgBlAGMAaQBzAGkAbwBuAF0AIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAAUwBlAGwAZQBjAHQAIABwAHIAZQBjAGkAcwBpAG8AbgAgAGwAZQB2AGUAbABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAwACAALQAgAEYAbABvAGEAdABpAG4AZwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAxACAALQAgAEQAYQB5AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADIAIAAtACAASABvAHUAcgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAzACAALQAgAE0AaQBuAHUAdABlAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADQAIAAtACAAUwBlAGMAbwBuAGQAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAANQAgAC0AIABNAGkAbABsAGkAcwBlAGMAbwBuAGQAXABuAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0AIAB8ACAAcwB3AGkAdABjAGgAIAAgAHwAIABDAGEAbABjAHUAbABhAHQAZQAgAGkAbgAgAHQAaABlACAASgB1AGwAaQBhAG4AIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuACAARABlAGYAYQB1AGwAdAAgAGkAcwAgAEcAcgBlAGcAbwByAGkAYQBuACAAcAByAG8AbABlAHAAdABpAGMAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIABjAGEAbABlAG4AZABhAHIALgBcAG4AXABuAEUAeABhAG0AcABsAGUAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AUgBFAFMATwBMAFYARQBfAEQAQQBUAEUAKAAyADAAMgAzACwAIAAyADUALAAgADMAMwAuADUALAAgAC0AMQAuADUAKQBcAG4AUgBlAHQAdQByAG4AcwA6ACAAewAyADAAMgA1ACwAIAAyACwAIAAxACwAIAAwAH0AXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAFIARQBTAE8ATABWAEUAXwBEAEEAVABFACAAPQAgAEwAQQBNAEIARABBACgAWQBlAGEAcgBDAEUALAAgAE0AbwBuAHQAaABzACwAIABEAGEAeQBzACwAIABUAGkAbQBlACwAIABbAFAAcgBlAGMAaQBzAGkAbwBuAF0ALAAgAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0ALABcAG4AIAAgACAAIABJAEYAKAAoAFkAZQBhAHIAQwBFACAAPQAgAFwAIgBcACIAKQAgACoAIAAoAE0AbwBuAHQAaABzACAAPQAgAFwAIgBcACIAKQAgACoAIAAoAEQAYQB5AHMAIAA9ACAAXAAiAFwAIgApACAAKgAgACgAVABpAG0AZQAgAD0AIABcACIAXAAiACkALAAgAHsAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgB9ACwAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAFkAZQBhAHIAQwBFACkAKQAgACsAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAE0AbwBuAHQAaABzACkAKQAgACsAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEQAYQB5AHMAKQApACwAIAB7ACMAVgBBAEwAVQBFACEALAAgACMAVgBBAEwAVQBFACEALAAgACMAVgBBAEwAVQBFACEALAAgACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AeQBlAGEAcgBDAEUALAAgAEkATgBUACgAWQBlAGEAcgBDAEUAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYQBkAGQAWQBlAGEAcgBzACwAIABZAGUAYQByAEMARQAgAC0AIABfAHkAZQBhAHIAQwBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBhAGQAZABNAG8AbgB0AGgAcwAsACAATQBvAG4AdABoAHMAIAAtACAAMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYQBkAGQARABhAHkAcwAsACAARABhAHkAcwAgAC0AIAAxACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBqAEQAYQB0AGUALAAgAEEARABEAF8AVABJAE0ARQBTAFAAQQBOACgAXwB5AGUAYQByAEMARQAsACAAMQAsACAAMQAsACAAMAAsACAAXwBhAGQAZABZAGUAYQByAHMALAAgAF8AYQBkAGQATQBvAG4AdABoAHMALAAgAF8AYQBkAGQARABhAHkAcwAsACAAVABpAG0AZQAsACAAMAAsACAASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABDAEEATABFAE4ARABBAFIAXwBGAFIATwBNAF8ASgBEAEEAVABFACgAXwBqAEQAYQB0AGUALAAgADAALAAgAFAAcgBlAGMAaQBzAGkAbwBuACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAFwAbgBcAG4AXABuAFwAbgAvACoAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjAFwAbgAjACAARABFAEwAVABBAFMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAKgAvAFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEQARQBMAFQAQQBfAEgATwBVAFIAUwBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHQAaQBtAGUAcwBwAGEAbgAgAGQAaQBmAGYAZQByAGUAbgBjAGUAIABiAGUAdAB3AGUAZQBuACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMAIABpAG4AIABoAG8AdQByAHMALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIABEAGkAZgBmAGUAcgBlAG4AYwBlACAAaQBuACAAaABvAHUAcgBzAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ASgBEAGEAdABlADEAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIABcAG4ASgBEAGEAdABlADIAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ARABFAEwAVABBAF8ASABPAFUAUgBTACAAPQAgAEwAQQBNAEIARABBACgASgBEAGEAdABlADEALAAgAEoARABhAHQAZQAyACwAXABuACAAIAAgACAASQBGACgAKABKAEQAYQB0AGUAMQAgAD0AIABcACIAXAAiACkAIAAqACAAKABKAEQAYQB0AGUAMgAgAD0AIABcACIAXAAiACkALAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgASgBEAGEAdABlADEAKQApACAAKwAgAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgASgBEAGEAdABlADIAKQApACwAIAB7ACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoAEoARABhAHQAZQAyACAALQAgAEoARABhAHQAZQAxACkAIAAqACAAMgA0AFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ARABFAEwAVABBAF8ATQBJAE4AVQBUAEUAUwBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHQAaQBtAGUAcwBwAGEAbgAgAGQAaQBmAGYAZQByAGUAbgBjAGUAIABiAGUAdAB3AGUAZQBuACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMAIABpAG4AIABtAGkAbgB1AHQAZQBzAC4AXABuAFwAbgBPAHUAdABwAHUAdABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAARABpAGYAZgBlAHIAZQBuAGMAZQAgAGkAbgAgAG0AaQBuAHUAdABlAHMAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBKAEQAYQB0AGUAMQAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgAFwAbgBKAEQAYQB0AGUAMgAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBEAEUATABUAEEAXwBNAEkATgBVAFQARQBTACAAPQAgAEwAQQBNAEIARABBACgASgBEAGEAdABlADEALAAgAEoARABhAHQAZQAyACwAXABuACAAIAAgACAASQBGACgAKABKAEQAYQB0AGUAMQAgAD0AIABcACIAXAAiACkAIAAqACAAKABKAEQAYQB0AGUAMgAgAD0AIABcACIAXAAiACkALAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgASgBEAGEAdABlADEAKQApACAAKwAgAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgASgBEAGEAdABlADIAKQApACwAIAB7ACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoAEoARABhAHQAZQAyACAALQAgAEoARABhAHQAZQAxACkAIAAqACAAMQA0ADQAMABcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEQARQBMAFQAQQBfAFMARQBDAE8ATgBEAFMAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIAB0AGkAbQBlAHMAcABhAG4AIABkAGkAZgBmAGUAcgBlAG4AYwBlACAAYgBlAHQAdwBlAGUAbgAgAEoAdQBsAGkAYQBuACAARABhAHQAZQBzACAAaQBuACAAcwBlAGMAbwBuAGQAcwAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgAEQAaQBmAGYAZQByAGUAbgBjAGUAIABpAG4AIABzAGUAYwBvAG4AZABzAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ASgBEAGEAdABlADEAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIABcAG4ASgBEAGEAdABlADIAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ARABFAEwAVABBAF8AUwBFAEMATwBOAEQAUwAgAD0AIABMAEEATQBCAEQAQQAoAEoARABhAHQAZQAxACwAIABKAEQAYQB0AGUAMgAsAFwAbgAgACAAIAAgAEkARgAoACgASgBEAGEAdABlADEAIAA9ACAAXAAiAFwAIgApACAAKgAgACgASgBEAGEAdABlADIAIAA9ACAAXAAiAFwAIgApACwAIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEoARABhAHQAZQAxACkAKQAgACsAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEoARABhAHQAZQAyACkAKQAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKABKAEQAYQB0AGUAMgAgAC0AIABKAEQAYQB0AGUAMQApACAAKgAgADgANgA0ADAAMABcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEQARQBMAFQAQQBfAEgATwBVAFIAXwBNAEkATgBfAFMARQBDAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAHQAaABlACAAdABpAG0AZQBzAHAAYQBuACAAZABpAGYAZgBlAHIAZQBuAGMAZQAgAGIAZQB0AHcAZQBlAG4AIABKAHUAbABpAGEAbgAgAEQAYQB0AGUAcwAgAGkAbgAgAGgAbwB1AHIAcwAsACAAbQBpAG4AdQB0AGUAcwAgAGEAbgBkACAAcwBlAGMAbwBuAGQAcwAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABpAG4AdABlAGcAZQByACAAWwAtADEALAAwACwAMQBdACAAfAAgAFMAaQBnAG4AXABuACAAMgAgAHwAIABpAG4AdABlAGcAZQByACAAWwAwAC4ALgBdACAAIAAgACAAfAAgAEQAZQBsAHQAYQAgAGgAbwB1AHIAcwBcAG4AIAAzACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADAALgAuADUAOQBdACAAIAB8ACAARABlAGwAdABhACAAbQBpAG4AdQB0AGUAcwBcAG4AIAA0ACAAfAAgAGQAZQBjAGkAbQBhAGwAIABbADAALgAuADYAMAApACAAIAB8ACAARABlAGwAdABhACAAcwBlAGMAbwBuAGQAcwBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEoARABhAHQAZQAxACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAAXABuAEoARABhAHQAZQAyACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEQARQBMAFQAQQBfAEgATwBVAFIAXwBNAEkATgBfAFMARQBDACAAPQAgAEwAQQBNAEIARABBACgASgBEAGEAdABlADEALAAgAEoARABhAHQAZQAyACwAXABuACAAIAAgACAASQBGACgAKABKAEQAYQB0AGUAMQAgAD0AIABcACIAXAAiACkAIAAqACAAKABKAEQAYQB0AGUAMgAgAD0AIABcACIAXAAiACkALAAgAHsAXAAiAFwAIgAsAFwAIgBcACIALABcACIAXAAiACwAXAAiAFwAIgB9ACwAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEoARABhAHQAZQAxACkAKQAgACsAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEoARABhAHQAZQAyACkAKQAsACAAewAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABJAE0ARQBfAEQARQBDAEkATQBBAEwAXwBUAE8AXwBIAE0AUwAoAEoARABhAHQAZQAyACAALQAgAEoARABhAHQAZQAxACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBEAEUATABUAEEAXwBEAEEAWQBTAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAHQAaABlACAAdABpAG0AZQBzAHAAYQBuACAAZABpAGYAZgBlAHIAZQBuAGMAZQAgAGIAZQB0AHcAZQBlAG4AIABKAHUAbABpAGEAbgAgAEQAYQB0AGUAcwAgAGkAbgAgAGQAYQB5AHMALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIABEAGkAZgBmAGUAcgBlAG4AYwBlACAAaQBuACAAZABhAHkAcwBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEoARABhAHQAZQAxACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAAXABuAEoARABhAHQAZQAyACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEQARQBMAFQAQQBfAEQAQQBZAFMAIAA9ACAATABBAE0AQgBEAEEAKABKAEQAYQB0AGUAMQAsACAASgBEAGEAdABlADIALABcAG4AIAAgACAAIABJAEYAKAAoAEoARABhAHQAZQAxACAAPQAgAFwAIgBcACIAKQAgACoAIAAoAEoARABhAHQAZQAyACAAPQAgAFwAIgBcACIAKQAsACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABKAEQAYQB0AGUAMQApACkAIAArACAATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABKAEQAYQB0AGUAMgApACkALAAgAHsAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgASgBEAGEAdABlADIAIAAtACAASgBEAGEAdABlADEAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEQARQBMAFQAQQBfAFcARQBFAEsAUwBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHQAaQBtAGUAcwBwAGEAbgAgAGQAaQBmAGYAZQByAGUAbgBjAGUAIABiAGUAdAB3AGUAZQBuACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMAIABpAG4AIAB3AGUAZQBrAHMALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIABEAGkAZgBmAGUAcgBlAG4AYwBlACAAaQBuACAAdwBlAGUAawBzAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ASgBEAGEAdABlADEAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAXABuAEoARABhAHQAZQAyACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBEAEUATABUAEEAXwBXAEUARQBLAFMAIAA9ACAATABBAE0AQgBEAEEAKABKAEQAYQB0AGUAMQAsACAASgBEAGEAdABlADIALABcAG4AIAAgACAAIABJAEYAKAAoAEoARABhAHQAZQAxACAAPQAgAFwAIgBcACIAKQAgACoAIAAoAEoARABhAHQAZQAyACAAPQAgAFwAIgBcACIAKQAsACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABKAEQAYQB0AGUAMQApACkAIAArACAATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABKAEQAYQB0AGUAMgApACkALAAgAHsAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgASgBEAGEAdABlADIAIAAtACAASgBEAGEAdABlADEAKQAgAC8AIAA3AFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ARABFAEwAVABBAF8ATQBPAE4AVABIAFMAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIAB0AGkAbQBlAHMAcABhAG4AIABkAGkAZgBmAGUAcgBlAG4AYwBlACAAYgBlAHQAdwBlAGUAbgAgAEoAdQBsAGkAYQBuACAARABhAHQAZQBzACAAaQBuACAAbQBvAG4AdABoAHMALgBcAG4AVwBoAGUAcgBlACAAdABoAGUAIABkAGkAZgBmAGUAcgBlAG4AYwBlACAAaQBuAGMAbAB1AGQAZQBzACAAcABhAHIAdABpAGEAbAAgAG0AbwBuAHQAaABzACwAIAB0AGgAZQAgAGYAcgBhAGMAdABpAG8AbgAgAGkAcwAgAGMAYQBsAGMAdQBsAGEAdABlAGQAIABvAG4AIAB0AGgAZQAgAGIAYQBzAGkAcwAgAG8AZgAgAGQAYQB5AHMAIABpAG4AIAB0AGgAZQAgAG0AbwBuAHQAaABcAG4AbwBmACAAdABoAGUAIABjAGEAbABlAG4AZABhAHIALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIABEAGkAZgBmAGUAcgBlAG4AYwBlACAAaQBuACAAbQBvAG4AdABoAHMAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBKAEQAYQB0AGUAMQAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAAgACAAIAAgAHwAXABuAEoARABhAHQAZQAyACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgACAAIAAgACAAfABcAG4AWwBUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQAXQAgAHwAIABkAGUAYwBpAG0AYQBsACAAIAAgACAAIAB8ACAAVABpAG0AZQAgAHoAbwBuAGUAIABvAGYAZgBzAGUAdAAgAGkAbgAgAG0AaQBuAHUAdABlAHMAIABmAHIAbwBtACAAVQBUAEMALgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABbAC0AOQAwADAALgAuADkAMAAwAF0AIAB8ACAAQQBzAHMAdQBtAGUAZAAgAHQAbwAgAGIAZQAgAFUAVABDACAAaQBmACAAbwBtAG0AaQB0AHQAZQBkAC4AXABuAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0AIAB8ACAAcwB3AGkAdABjAGgAIAAgACAAIAAgACAAfAAgAEMAYQBsAGMAdQBsAGEAdABlACAAaQBuACAAdABoAGUAIABKAHUAbABpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AIABEAGUAZgBhAHUAbAB0ACAAaQBzACAARwByAGUAZwBvAHIAaQBhAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEQARQBMAFQAQQBfAE0ATwBOAFQASABTACAAPQAgAEwAQQBNAEIARABBACgASgBEAGEAdABlADEALAAgAEoARABhAHQAZQAyACwAIABbAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdABdACwAIABbAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACwAXABuACAAIAAgACAASQBGACgAKABKAEQAYQB0AGUAMQAgAD0AIABcACIAXAAiACkAIAAqACAAKABKAEQAYQB0AGUAMgAgAD0AIABcACIAXAAiACkALAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgASgBEAGEAdABlADEAKQApACAAKwAgAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgASgBEAGEAdABlADIAKQApACwAIAB7ACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdAB6AG8ALAAgAE4AKABUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAEEAQgBTACgAXwB0AHoAbwApACAAPgAgADkAMAAwACwAIAB7ACMATgBVAE0AIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaQBnAG4ALAAgAEkARgAoAEoARABhAHQAZQAyACAAPgA9ACAASgBEAGEAdABlADEALAAgADEALAAgAC0AMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AagBkAG4ATABvAGMAYQBsAF8AUwB0AGEAcgB0ACwAIABKAEQAQQBUAEUAXwBUAE8AXwBKAEQATgBfAEwATwBDAEEATAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAF8AcwBpAGcAbgAgAD0AIAAxACwAIABKAEQAYQB0AGUAMQAsACAASgBEAGEAdABlADIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdAB6AG8AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBqAGQAbgBMAG8AYwBhAGwAXwBFAG4AZAAsACAASgBEAEEAVABFAF8AVABPAF8ASgBEAE4AXwBMAE8AQwBBAEwAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAHMAaQBnAG4AIAA9ACAAMQAsACAASgBEAGEAdABlADIALAAgAEoARABhAHQAZQAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBvAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHQAZQBfAFMAdABhAHIAdAAsACAASgBEAE4AXwBUAE8AXwBDAEEATABFAE4ARABBAFIAXwBEAEEAVABFACgASQBOAEQARQBYACgAXwBqAGQAbgBMAG8AYwBhAGwAXwBTAHQAYQByAHQALAAgADEALAAgADEAKQAsACAASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAdABlAF8ARQBuAGQALAAgAEoARABOAF8AVABPAF8AQwBBAEwARQBOAEQAQQBSAF8ARABBAFQARQAoAEkATgBEAEUAWAAoAF8AagBkAG4ATABvAGMAYQBsAF8ARQBuAGQALAAgADEALAAgADEAKQAsACAASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGUAbAB0AGEAWQBlAGEAcgAsACAASQBOAEQARQBYACgAXwBkAGEAdABlAF8ARQBuAGQALAAgADEALAAgADEAKQAgAC0AIABJAE4ARABFAFgAKABfAGQAYQB0AGUAXwBTAHQAYQByAHQALAAgADEALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAZQBsAHQAYQBNAG8AbgB0AGgALAAgAEkATgBEAEUAWAAoAF8AZABhAHQAZQBfAEUAbgBkACwAIAAxACwAIAAyACkAIAAtACAASQBOAEQARQBYACgAXwBkAGEAdABlAF8AUwB0AGEAcgB0ACwAIAAxACwAIAAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGkAZgBmAE0AbwBuAHQAaABzACwAIAAoAF8AZABlAGwAdABhAFkAZQBhAHIAIAAqACAAMQAyACkAIAArACAAXwBkAGUAbAB0AGEATQBvAG4AdABoACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkAcwBNAG8AbgB0AGgAXwBTAHQAYQByAHQALAAgAEQAQQBZAFMAXwBJAE4AXwBNAE8ATgBUAEgAKABJAE4ARABFAFgAKABfAGQAYQB0AGUAXwBTAHQAYQByAHQALAAgADEALAAgADIAKQAsACAASQBOAEQARQBYACgAXwBkAGEAdABlAF8AUwB0AGEAcgB0ACwAIAAxACwAIAAxACkALAAgAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkAcwBNAG8AbgB0AGgAXwBFAG4AZAAsACAARABBAFkAUwBfAEkATgBfAE0ATwBOAFQASAAoAEkATgBEAEUAWAAoAF8AZABhAHQAZQBfAEUAbgBkACwAIAAxACwAIAAyACkALAAgAEkATgBEAEUAWAAoAF8AZABhAHQAZQBfAEUAbgBkACwAIAAxACwAIAAxACkALAAgAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcABhAHIAdABpAGEAbABNAG8AbgB0AGgAXwBTAHQAYQByAHQALAAgACgASQBOAEQARQBYACgAXwBkAGEAdABlAF8AUwB0AGEAcgB0ACwAIAAxACwAIAAzACkAIAAtACAAMQAgACsAIABJAE4ARABFAFgAKABfAGoAZABuAEwAbwBjAGEAbABfAFMAdABhAHIAdAAsACAAMQAsACAAMgApACkAIAAvACAAXwBkAGEAeQBzAE0AbwBuAHQAaABfAFMAdABhAHIAdAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHAAYQByAHQAaQBhAGwATQBvAG4AdABoAF8ARQBuAGQALAAgACgASQBOAEQARQBYACgAXwBkAGEAdABlAF8ARQBuAGQALAAgADEALAAgADMAKQAgAC0AIAAxACAAKwAgAEkATgBEAEUAWAAoAF8AagBkAG4ATABvAGMAYQBsAF8ARQBuAGQALAAgADEALAAgADIAKQApACAALwAgAF8AZABhAHkAcwBNAG8AbgB0AGgAXwBFAG4AZAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaQBnAG4AIAAqACAAKABfAGQAaQBmAGYATQBvAG4AdABoAHMAIAAtACAAXwBwAGEAcgB0AGkAYQBsAE0AbwBuAHQAaABfAFMAdABhAHIAdAAgACsAIABfAHAAYQByAHQAaQBhAGwATQBvAG4AdABoAF8ARQBuAGQAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEQARQBMAFQAQQBfAFEAVQBBAFIAVABFAFIAUwBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHQAaQBtAGUAcwBwAGEAbgAgAGQAaQBmAGYAZQByAGUAbgBjAGUAIABiAGUAdAB3AGUAZQBuACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMAIABpAG4AIABxAHUAYQByAHQAZQByAHMALgBcAG4AVwBoAGUAcgBlACAAdABoAGUAIABkAGkAZgBmAGUAcgBlAG4AYwBlACAAaQBuAGMAbAB1AGQAZQBzACAAcABhAHIAdABpAGEAbAAgAHEAdQBhAHIAdABlAHIAcwAsACAAdABoAGUAIABmAHIAYQBjAHQAaQBvAG4AIABpAHMAIABjAGEAbABjAHUAbABhAHQAZQBkACAAbwBuACAAdABoAGUAIABiAGEAcwBpAHMAIABvAGYAIABkAGEAeQBzACAAaQBuACAAdABoAGUAXABuAHEAdQBhAHIAdABlAHIAIABvAGYAIAB0AGgAZQAgAGMAYQBsAGUAbgBkAGEAcgAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgAEQAaQBmAGYAZQByAGUAbgBjAGUAIABpAG4AIABxAHUAYQByAHQAZQByAHMAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBKAEQAYQB0AGUAMQAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAAgACAAIAAgACAAIAAgACAAfAAgAFwAbgBKAEQAYQB0AGUAMgAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAAgACAAIAAgACAAIAAgACAAfAAgAFwAbgBbAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdABdACAAfAAgAGQAZQBjAGkAbQBhAGwAIAAgACAAIAAgACAAIAAgACAAfAAgAFQAaQBtAGUAIAB6AG8AbgBlACAAbwBmAGYAcwBlAHQAIABpAG4AIABtAGkAbgB1AHQAZQBzACAAZgByAG8AbQAgAFUAVABDAC4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAWwAtADkAMAAwAC4ALgA5ADAAMABdACAAIAAgACAAIAB8ACAAQQBzAHMAdQBtAGUAZAAgAHQAbwAgAGIAZQAgAFUAVABDACAAaQBmACAAbwBtAG0AaQB0AHQAZQBkAC4AXABuAFsATQBvAG4AdABoAE8AZgBmAHMAZQB0AF0AIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsALQA2AC4ALgAzAF0AIAB8ACAAUQB1AGEAcgB0AGUAcgAgAG0AbwBuAHQAaAAgAG8AZgBmAHMAZQB0ACAAZgByAG8AbQAgAEoAYQBuAHUAYQByAHkALgBcAG4AWwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAgAHwAIABzAHcAaQB0AGMAaAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABDAGEAbABjAHUAbABhAHQAZQAgAGkAbgAgAHQAaABlACAASgB1AGwAaQBhAG4AIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuACAARABlAGYAYQB1AGwAdAAgAGkAcwAgAEcAcgBlAGcAbwByAGkAYQBuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEQARQBMAFQAQQBfAFEAVQBBAFIAVABFAFIAUwAgAD0AIABMAEEATQBCAEQAQQAoAEoARABhAHQAZQAxACwAIABKAEQAYQB0AGUAMgAsACAAWwBUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQAXQAsACAAWwBNAG8AbgB0AGgATwBmAGYAcwBlAHQAXQAsACAAWwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAsAFwAbgAgACAAIAAgAEkARgAoACgASgBEAGEAdABlADEAIAA9ACAAXAAiAFwAIgApACAAKgAgACgASgBEAGEAdABlADIAIAA9ACAAXAAiAFwAIgApACwAIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEoARABhAHQAZQAxACkAKQAgACsAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEoARABhAHQAZQAyACkAKQAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBvACwAIABOACgAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AbwBuAHQAaABPAGYAZgBzAGUAdAAsACAAUgBPAFUATgBEACgATgAoAE0AbwBuAHQAaABPAGYAZgBzAGUAdAApACwAIAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKAAoAEEAQgBTACgAXwB0AHoAbwApACAAPgAgADkAMAAwACkAIAArACAAKABfAG0AbwBuAHQAaABPAGYAZgBzAGUAdAAgADwAIAAtADYAKQAgACsAIAAoAF8AbQBvAG4AdABoAE8AZgBmAHMAZQB0ACAAPgAgADMAKQAsACAAewAjAE4AVQBNACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGkAZwBuACwAIABJAEYAKABKAEQAYQB0AGUAMgAgAD4APQAgAEoARABhAHQAZQAxACwAIAAxACwAIAAtADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGoAZABuAEwAbwBjAGEAbABfAFMAdABhAHIAdAAsACAASgBEAEEAVABFAF8AVABPAF8ASgBEAE4AXwBMAE8AQwBBAEwAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAHMAaQBnAG4AIAA9ACAAMQAsACAASgBEAGEAdABlADEALAAgAEoARABhAHQAZQAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBvAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AagBkAG4ATABvAGMAYQBsAF8ARQBuAGQALAAgAEoARABBAFQARQBfAFQATwBfAEoARABOAF8ATABPAEMAQQBMACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBzAGkAZwBuACAAPQAgADEALAAgAEoARABhAHQAZQAyACwAIABKAEQAYQB0AGUAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AHoAbwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHEAdQBhAHIAdABlAHIARABhAHQAZQBfAFMAdABhAHIAdAAsACAASgBEAE4AXwBUAE8AXwBRAFUAQQBSAFQARQBSAF8ARABBAFQARQAoAEkATgBEAEUAWAAoAF8AagBkAG4ATABvAGMAYQBsAF8AUwB0AGEAcgB0ACwAIAAxACwAIAAxACkALAAgAF8AbQBvAG4AdABoAE8AZgBmAHMAZQB0ACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHEAdQBhAHIAdABlAHIARABhAHQAZQBfAEUAbgBkACwAIABKAEQATgBfAFQATwBfAFEAVQBBAFIAVABFAFIAXwBEAEEAVABFACgASQBOAEQARQBYACgAXwBqAGQAbgBMAG8AYwBhAGwAXwBFAG4AZAAsACAAMQAsACAAMQApACwAIABfAG0AbwBuAHQAaABPAGYAZgBzAGUAdAAsACAASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGUAbAB0AGEAWQBlAGEAcgAsACAASQBOAEQARQBYACgAXwBxAHUAYQByAHQAZQByAEQAYQB0AGUAXwBFAG4AZAAsACAAMQAsACAAMQApACAALQAgAEkATgBEAEUAWAAoAF8AcQB1AGEAcgB0AGUAcgBEAGEAdABlAF8AUwB0AGEAcgB0ACwAIAAxACwAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGUAbAB0AGEAUQB1AGEAcgB0AGUAcgAsACAASQBOAEQARQBYACgAXwBxAHUAYQByAHQAZQByAEQAYQB0AGUAXwBFAG4AZAAsACAAMQAsACAAMgApACAALQAgAEkATgBEAEUAWAAoAF8AcQB1AGEAcgB0AGUAcgBEAGEAdABlAF8AUwB0AGEAcgB0ACwAIAAxACwAIAAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGkAZgBmAFEAdQBhAHIAdABlAHIAcwAsACAAKABfAGQAZQBsAHQAYQBZAGUAYQByACAAKgAgADQAKQAgACsAIABfAGQAZQBsAHQAYQBRAHUAYQByAHQAZQByACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcABhAHIAdABpAGEAbABRAHUAYQByAHQAZQByAF8AUwB0AGEAcgB0ACwAIAAoAEkATgBEAEUAWAAoAF8AcQB1AGEAcgB0AGUAcgBEAGEAdABlAF8AUwB0AGEAcgB0ACwAIAAxACwAIAAzACkAIAAtACAAMQAgACsAIABJAE4ARABFAFgAKABfAGoAZABuAEwAbwBjAGEAbABfAFMAdABhAHIAdAAsACAAMQAsACAAMgApACkAIAAvACAASQBOAEQARQBYACgAXwBxAHUAYQByAHQAZQByAEQAYQB0AGUAXwBTAHQAYQByAHQALAAgADEALAAgADQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHAAYQByAHQAaQBhAGwAUQB1AGEAcgB0AGUAcgBfAEUAbgBkACwAIAAoAEkATgBEAEUAWAAoAF8AcQB1AGEAcgB0AGUAcgBEAGEAdABlAF8ARQBuAGQALAAgADEALAAgADMAKQAgAC0AIAAxACAAKwAgAEkATgBEAEUAWAAoAF8AagBkAG4ATABvAGMAYQBsAF8ARQBuAGQALAAgADEALAAgADIAKQApACAALwAgAEkATgBEAEUAWAAoAF8AcQB1AGEAcgB0AGUAcgBEAGEAdABlAF8ARQBuAGQALAAgADEALAAgADQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaQBnAG4AIAAqACAAKABfAGQAaQBmAGYAUQB1AGEAcgB0AGUAcgBzACAALQAgAF8AcABhAHIAdABpAGEAbABRAHUAYQByAHQAZQByAF8AUwB0AGEAcgB0ACAAKwAgAF8AcABhAHIAdABpAGEAbABRAHUAYQByAHQAZQByAF8ARQBuAGQAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEQARQBMAFQAQQBfAFkARQBBAFIAUwBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHQAaQBtAGUAcwBwAGEAbgAgAGQAaQBmAGYAZQByAGUAbgBjAGUAIABiAGUAdAB3AGUAZQBuACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMAIABpAG4AIAB5AGUAYQByAHMALgBcAG4AVwBoAGUAcgBlACAAdABoAGUAIABkAGkAZgBmAGUAcgBlAG4AYwBlACAAaQBuAGMAbAB1AGQAZQBzACAAcABhAHIAdABpAGEAbAAgAHkAZQBhAHIAcwAsACAAdABoAGUAIABmAHIAYQBjAHQAaQBvAG4AIABpAHMAIABjAGEAbABjAHUAbABhAHQAZQBkACAAbwBuACAAdABoAGUAIABiAGEAcwBpAHMAIABvAGYAIABkAGEAeQBzACAAaQBuACAAdABoAGUAXABuAHkAZQBhAHIAIABvAGYAIAB0AGgAZQAgAGMAYQBsAGUAbgBkAGEAcgAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgAEQAaQBmAGYAZQByAGUAbgBjAGUAIABpAG4AIAB5AGUAYQByAHMAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBKAEQAYQB0AGUAMQAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAAgACAAIAAgAHwAIABcAG4ASgBEAGEAdABlADIAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAIAAgACAAIAB8ACAAXABuAFsAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0AF0AIAB8ACAAZABlAGMAaQBtAGEAbAAgACAAIAAgACAAfAAgAFQAaQBtAGUAIAB6AG8AbgBlACAAbwBmAGYAcwBlAHQAIABpAG4AIABtAGkAbgB1AHQAZQBzACAAZgByAG8AbQAgAFUAVABDAC4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAWwAtADkAMAAwAC4ALgA5ADAAMABdACAAfAAgAEEAcwBzAHUAbQBlAGQAIAB0AG8AIABiAGUAIABVAFQAQwAgAGkAZgAgAG8AbQBtAGkAdAB0AGUAZAAuAFwAbgBbAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACAAfAAgAHMAdwBpAHQAYwBoACAAIAAgACAAIAAgAHwAIABDAGEAbABjAHUAbABhAHQAZQAgAGkAbgAgAHQAaABlACAASgB1AGwAaQBhAG4AIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuACAARABlAGYAYQB1AGwAdAAgAGkAcwAgAEcAcgBlAGcAbwByAGkAYQBuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBEAEUATABUAEEAXwBZAEUAQQBSAFMAIAA9ACAATABBAE0AQgBEAEEAKABKAEQAYQB0AGUAMQAsACAASgBEAGEAdABlADIALAAgAFsAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0AF0ALAAgAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0ALABcAG4AIAAgACAAIABJAEYAKAAoAEoARABhAHQAZQAxACAAPQAgAFwAIgBcACIAKQAgACoAIAAoAEoARABhAHQAZQAyACAAPQAgAFwAIgBcACIAKQAsACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABKAEQAYQB0AGUAMQApACkAIAArACAATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABKAEQAYQB0AGUAMgApACkALAAgAHsAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AHoAbwAsACAATgAoAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAQQBCAFMAKABfAHQAegBvACkAIAA+ACAAOQAwADAALAAgAHsAIwBOAFUATQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBpAGcAbgAsACAASQBGACgASgBEAGEAdABlADIAIAA+AD0AIABKAEQAYQB0AGUAMQAsACAAMQAsACAALQAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBqAGQAbgBMAG8AYwBhAGwAXwBTAHQAYQByAHQALAAgAEoARABBAFQARQBfAFQATwBfAEoARABOAF8ATABPAEMAQQBMACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBzAGkAZwBuACAAPQAgADEALAAgAEoARABhAHQAZQAxACwAIABKAEQAYQB0AGUAMgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AHoAbwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGoAZABuAEwAbwBjAGEAbABfAEUAbgBkACwAIABKAEQAQQBUAEUAXwBUAE8AXwBKAEQATgBfAEwATwBDAEEATAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAF8AcwBpAGcAbgAgAD0AIAAxACwAIABKAEQAYQB0AGUAMgAsACAASgBEAGEAdABlADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdAB6AG8AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBvAHIAZABpAG4AYQBsAEQAYQB0AGUAXwBTAHQAYQByAHQALAAgAEoARABOAF8AVABPAF8ATwBSAEQASQBOAEEATABfAEQAQQBUAEUAKABJAE4ARABFAFgAKABfAGoAZABuAEwAbwBjAGEAbABfAFMAdABhAHIAdAAsACAAMQAsACAAMQApACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG8AcgBkAGkAbgBhAGwARABhAHQAZQBfAEUAbgBkACwAIABKAEQATgBfAFQATwBfAE8AUgBEAEkATgBBAEwAXwBEAEEAVABFACgASQBOAEQARQBYACgAXwBqAGQAbgBMAG8AYwBhAGwAXwBFAG4AZAAsACAAMQAsACAAMQApACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAZQBsAHQAYQBZAGUAYQByACwAIABJAE4ARABFAFgAKABfAG8AcgBkAGkAbgBhAGwARABhAHQAZQBfAEUAbgBkACwAIAAxACwAIAAxACkAIAAtACAASQBOAEQARQBYACgAXwBvAHIAZABpAG4AYQBsAEQAYQB0AGUAXwBTAHQAYQByAHQALAAgADEALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHAAYQByAHQAaQBhAGwAWQBlAGEAcgBfAFMAdABhAHIAdAAsACAAKABJAE4ARABFAFgAKABfAG8AcgBkAGkAbgBhAGwARABhAHQAZQBfAFMAdABhAHIAdAAsACAAMQAsACAAMgApACAALQAgADEAIAArACAASQBOAEQARQBYACgAXwBqAGQAbgBMAG8AYwBhAGwAXwBTAHQAYQByAHQALAAgADEALAAgADIAKQApACAALwAgAEkATgBEAEUAWAAoAF8AbwByAGQAaQBuAGEAbABEAGEAdABlAF8AUwB0AGEAcgB0ACwAIAAxACwAIAAzACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBwAGEAcgB0AGkAYQBsAFkAZQBhAHIAXwBFAG4AZAAsACAAKABJAE4ARABFAFgAKABfAG8AcgBkAGkAbgBhAGwARABhAHQAZQBfAEUAbgBkACwAIAAxACwAIAAyACkAIAAtACAAMQAgACsAIABJAE4ARABFAFgAKABfAGoAZABuAEwAbwBjAGEAbABfAEUAbgBkACwAIAAxACwAIAAyACkAKQAgAC8AIABJAE4ARABFAFgAKABfAG8AcgBkAGkAbgBhAGwARABhAHQAZQBfAEUAbgBkACwAIAAxACwAIAAzACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGkAZwBuACAAKgAgACgAXwBkAGUAbAB0AGEAWQBlAGEAcgAgAC0AIABfAHAAYQByAHQAaQBhAGwAWQBlAGEAcgBfAFMAdABhAHIAdAAgACsAIABfAHAAYQByAHQAaQBhAGwAWQBlAGEAcgBfAEUAbgBkACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ARABFAEwAVABBAF8AVwBFAEUASwBfAEQAQQBZAFMAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIAB0AGkAbQBlAHMAcABhAG4AIABkAGkAZgBmAGUAcgBlAG4AYwBlACAAYgBlAHQAdwBlAGUAbgAgAEoAdQBsAGkAYQBuACAARABhAHQAZQBzACAAaQBuACAAdwBlAGUAawBzACAAYQBuAGQAIABkAGEAeQBzAC4AXABuAFwAbgBPAHUAdABwAHUAdABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbAC0AMQAsADAALAAxAF0AIAB8ACAAUwBpAGcAbgBcAG4AIAAzACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADAALgAuAF0AIAAgACAAIAB8ACAARABlAGwAdABhACAAdwBlAGUAawBzACAAXABuACAANAAgAHwAIABkAGUAYwBpAG0AYQBsACAAWwAwAC4ALgA3ACkAIAAgACAAfAAgAEQAZQBsAHQAYQAgAGQAYQB5AHMAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBKAEQAYQB0AGUAMQAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgAFwAbgBKAEQAYQB0AGUAMgAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBEAEUATABUAEEAXwBXAEUARQBLAF8ARABBAFkAUwAgAD0AIABMAEEATQBCAEQAQQAoAEoARABhAHQAZQAxACwAIABKAEQAYQB0AGUAMgAsAFwAbgAgACAAIAAgAEkARgAoACgASgBEAGEAdABlADEAIAA9ACAAXAAiAFwAIgApACAAKgAgACgASgBEAGEAdABlADIAIAA9ACAAXAAiAFwAIgApACwAIAB7AFwAIgBcACIALAAgAFwAIgBcACIALAAgAFwAIgBcACIAfQAsAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABKAEQAYQB0AGUAMQApACkAIAArACAATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABKAEQAYQB0AGUAMgApACkALAAgAHsAIwBWAEEATABVAEUAIQAsACAAIwBWAEEATABVAEUAIQAsACAAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGkAZgBmAEQAYQB5AHMALAAgACgASgBEAGEAdABlADIAIAAtACAASgBEAGEAdABlADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAF8AZABpAGYAZgBEAGEAeQBzACAAPQAgADAALAAgAHsAMAAsACAAMAAsACAAMAB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaQBnAG4ALAAgAEkARgAoAF8AZABpAGYAZgBEAGEAeQBzACAAPgA9ACAAMAAsACAAMQAsACAALQAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBhAGIAcwBEAGkAZgBmAEQAYQB5AHMALAAgAF8AcwBpAGcAbgAgACoAIABfAGQAaQBmAGYARABhAHkAcwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAZQBsAHQAYQBXAGUAZQBrACwAIABJAE4AVAAoAF8AYQBiAHMARABpAGYAZgBEAGEAeQBzACAALwAgADcAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAZQBsAHQAYQBEAGEAeQAsACAATQBPAEQAKABfAGEAYgBzAEQAaQBmAGYARABhAHkAcwAsACAANwApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGkAZwBuACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGUAbAB0AGEAVwBlAGUAawAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABlAGwAdABhAEQAYQB5AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ARABFAEwAVABBAF8AWQBFAEEAUgBfAFcARQBFAEsAXwBEAEEAWQBTAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAHQAaABlACAAdABpAG0AZQBzAHAAYQBuACAAZABpAGYAZgBlAHIAZQBuAGMAZQAgAGIAZQB0AHcAZQBlAG4AIABKAHUAbABpAGEAbgAgAEQAYQB0AGUAcwAgAGkAbgAgAHkAZQBhAHIAcwAsACAAdwBlAGUAawBzACwAIABhAG4AZAAgAGQAYQB5AHMALgBcAG4ATgBvAHQAZQAgAHQAaABlACAAbgB1AG0AYgBlAHIAIABvAGYAIAB3AGUAZQBrAHMAIABwAGUAcgAgAHkAZQBhAHIAIABhAG4AIAB2AGEAcgB5ACAAYgBlAHQAdwBlAGUAbgAgADUAMgAgAGEAbgBkACAANQAzAC4AIABJAGYAIABhAG4AIABhAGIAcwBvAGwAdQB0AGUAIABuAHUAbQBiAGUAcgAgAG8AZgAgAHcAZQBlAGsAcwAgAGkAcwAgAGIAZQBpAG4AZwAgAHMAbwB1AGcAaAB0AFwAbgB0AGgAZQBuACAAdQBzAGUAIABlAGkAdABoAGUAcgAgAEQARQBMAFQAQQBfAFcARQBFAEsAXwBEAEEAWQBTACAAbwByACAARABFAEwAVABBAF8AVwBFAEUASwBTACAAZgB1AG4AYwB0AGkAbwBuAHMALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsALQAxACwAMAAsADEAXQAgAHwAIABTAGkAZwBuAFwAbgAgADIAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMAAuAC4AXQAgACAAIAAgAHwAIABEAGUAbAB0AGEAIAB5AGUAYQByAHMAXABuACAAMwAgAHwAIABpAG4AdABlAGcAZQByACAAWwAwAC4ALgA1ADIAXQAgACAAfAAgAEQAZQBsAHQAYQAgAHcAZQBlAGsAcwAgAFwAbgAgADQAIAB8ACAAZABlAGMAaQBtAGEAbAAgAFsAMAAuAC4ANwApACAAIAAgAHwAIABEAGUAbAB0AGEAIABkAGEAeQBzAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ASgBEAGEAdABlADEAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAIAAgACAAIAB8ACAAXABuAEoARABhAHQAZQAyACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgACAAIAAgACAAfAAgAFwAbgBbAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdABdACAAfAAgAGQAZQBjAGkAbQBhAGwAIAAgACAAIAAgAHwAIABUAGkAbQBlACAAegBvAG4AZQAgAG8AZgBmAHMAZQB0ACAAaQBuACAAbQBpAG4AdQB0AGUAcwAgAGYAcgBvAG0AIABVAFQAQwAuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAFsALQA5ADAAMAAuAC4AOQAwADAAXQAgAHwAIABBAHMAcwB1AG0AZQBkACAAdABvACAAYgBlACAAVQBUAEMAIABpAGYAIABvAG0AbQBpAHQAdABlAGQALgBcAG4AWwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAgAHwAIABzAHcAaQB0AGMAaAAgACAAIAAgACAAIAB8ACAAQwBhAGwAYwB1AGwAYQB0AGUAIABpAG4AIAB0AGgAZQAgAEoAdQBsAGkAYQBuACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgAgAEQAZQBmAGEAdQBsAHQAIABpAHMAIABHAHIAZQBnAG8AcgBpAGEAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ARABFAEwAVABBAF8AWQBFAEEAUgBfAFcARQBFAEsAXwBEAEEAWQBTACAAPQAgAEwAQQBNAEIARABBACgASgBEAGEAdABlADEALAAgAEoARABhAHQAZQAyACwAIABbAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdABdACwAIABbAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACwAXABuACAAIAAgACAASQBGACgAKABKAEQAYQB0AGUAMQAgAD0AIABcACIAXAAiACkAIAAqACAAKABKAEQAYQB0AGUAMgAgAD0AIABcACIAXAAiACkALAAgAHsAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgB9ACwAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEoARABhAHQAZQAxACkAKQAgACsAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEoARABhAHQAZQAyACkAKQAsACAAewAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBvACwAIABOACgAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABBAEIAUwAoAF8AdAB6AG8AKQAgAD4AIAA5ADAAMAAsACAAewAjAE4AVQBNACEALAAgACMATgBVAE0AIQAsACAAIwBOAFUATQAhACwAIAAjAE4AVQBNACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgASgBEAGEAdABlADIAIAA9ACAASgBEAGEAdABlADEALAAgAHsAMAAsACAAMAAsACAAMAAsACAAMAB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGkAZwBuACwAIABJAEYAKABKAEQAYQB0AGUAMgAgAD4APQAgAEoARABhAHQAZQAxACwAIAAxACwAIAAtADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AagBkAG4ATABvAGMAYQBsAF8AUwB0AGEAcgB0ACwAIABKAEQAQQBUAEUAXwBUAE8AXwBKAEQATgBfAEwATwBDAEEATAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBzAGkAZwBuACAAPQAgADEALAAgAEoARABhAHQAZQAxACwAIABKAEQAYQB0AGUAMgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBvAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGoAZABuAEwAbwBjAGEAbABfAEUAbgBkACwAIABKAEQAQQBUAEUAXwBUAE8AXwBKAEQATgBfAEwATwBDAEEATAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBzAGkAZwBuACAAPQAgADEALAAgAEoARABhAHQAZQAyACwAIABKAEQAYQB0AGUAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBvAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB3AGUAZQBrAEQAYQB0AGUAXwBTAHQAYQByAHQALAAgAEoARABOAF8AVABPAF8AVwBFAEUASwBfAEQAQQBUAEUAKABJAE4ARABFAFgAKABfAGoAZABuAEwAbwBjAGEAbABfAFMAdABhAHIAdAAsACAAMQAsACAAMQApACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdwBlAGUAawBEAGEAdABlAF8ARQBuAGQALAAgAEoARABOAF8AVABPAF8AVwBFAEUASwBfAEQAQQBUAEUAKABJAE4ARABFAFgAKABfAGoAZABuAEwAbwBjAGEAbABfAEUAbgBkACwAIAAxACwAIAAxACkALAAgAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGUAbAB0AGEAWQBlAGEAcgAsACAASQBOAEQARQBYACgAXwB3AGUAZQBrAEQAYQB0AGUAXwBFAG4AZAAsACAAMQAsACAAMQApACAALQAgAEkATgBEAEUAWAAoAF8AdwBlAGUAawBEAGEAdABlAF8AUwB0AGEAcgB0ACwAIAAxACwAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAZQBsAHQAYQBXAGUAZQBrACwAIABJAE4ARABFAFgAKABfAHcAZQBlAGsARABhAHQAZQBfAEUAbgBkACwAIAAxACwAIAAyACkAIAAtACAASQBOAEQARQBYACgAXwB3AGUAZQBrAEQAYQB0AGUAXwBTAHQAYQByAHQALAAgADEALAAgADIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABlAGwAdABhAEQAYQB5ACwAIABJAE4ARABFAFgAKABfAHcAZQBlAGsARABhAHQAZQBfAEUAbgBkACwAIAAxACwAIAAzACkAIAAtACAASQBOAEQARQBYACgAXwB3AGUAZQBrAEQAYQB0AGUAXwBTAHQAYQByAHQALAAgADEALAAgADMAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACsAIABJAE4ARABFAFgAKABfAGoAZABuAEwAbwBjAGEAbABfAEUAbgBkACwAIAAxACwAIAAyACkAIAAtACAASQBOAEQARQBYACgAXwBqAGQAbgBMAG8AYwBhAGwAXwBTAHQAYQByAHQALAAgADEALAAgADIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAZQBsAHQAYQBEAGEAeQAyACwAIABNAE8ARAAoAF8AZABlAGwAdABhAEQAYQB5ACwAIAA3ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAZQBsAHQAYQBXAGUAZQBrADIALAAgAF8AZABlAGwAdABhAFcAZQBlAGsAIAArACAASQBOAFQAKABfAGQAZQBsAHQAYQBEAGEAeQAgAC8AIAA3ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAGQAZQBsAHQAYQBXAGUAZQBrADIAIAA+AD0AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaQBnAG4ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGUAbAB0AGEAWQBlAGEAcgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAZQBsAHQAYQBXAGUAZQBrADIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGUAbAB0AGEARABhAHkAMgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBpAGcAbgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAZQBsAHQAYQBZAGUAYQByACAALQAgADEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGUAbAB0AGEAVwBlAGUAawAyACAAKwAgAEkATgBEAEUAWAAoAF8AdwBlAGUAawBEAGEAdABlAF8AUwB0AGEAcgB0ACwAIAAxACwAIAA0ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGUAbAB0AGEARABhAHkAMgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEQARQBMAFQAQQBfAE0ATwBOAFQASABfAEQAQQBZAFMAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIAB0AGkAbQBlAHMAcABhAG4AIABkAGkAZgBmAGUAcgBlAG4AYwBlACAAYgBlAHQAdwBlAGUAbgAgAEoAdQBsAGkAYQBuACAARABhAHQAZQBzACAAaQBuACAAbQBvAG4AdABoAHMAIABhAG4AZAAgAGQAYQB5AHMALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsALQAxACwAMAAsADEAXQAgAHwAIABTAGkAZwBuAFwAbgAgADIAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMAAuAC4AXQAgACAAIAAgAHwAIABEAGUAbAB0AGEAIABtAG8AbgB0AGgAcwBcAG4AIAAzACAAfAAgAGQAZQBjAGkAbQBhAGwAIABbADAALgAuADMAMQApACAAIAB8ACAARABlAGwAdABhACAAZABhAHkAcwBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEoARABhAHQAZQAxACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgACAAIAAgACAAfAAgAFwAbgBKAEQAYQB0AGUAMgAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAAgACAAIAAgAHwAIABcAG4AWwBUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQAXQAgAHwAIABkAGUAYwBpAG0AYQBsACAAIAAgACAAIAB8ACAAVABpAG0AZQAgAHoAbwBuAGUAIABvAGYAZgBzAGUAdAAgAGkAbgAgAG0AaQBuAHUAdABlAHMAIABmAHIAbwBtACAAVQBUAEMALgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABbAC0AOQAwADAALgAuADkAMAAwAF0AIAB8ACAAQQBzAHMAdQBtAGUAZAAgAHQAbwAgAGIAZQAgAFUAVABDACAAaQBmACAAbwBtAG0AaQB0AHQAZQBkAC4AXABuAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0AIAB8ACAAcwB3AGkAdABjAGgAIAAgACAAIAAgACAAfAAgAEMAYQBsAGMAdQBsAGEAdABlACAAaQBuACAAdABoAGUAIABKAHUAbABpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AIABEAGUAZgBhAHUAbAB0ACAAaQBzACAARwByAGUAZwBvAHIAaQBhAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEQARQBMAFQAQQBfAE0ATwBOAFQASABfAEQAQQBZAFMAIAA9ACAATABBAE0AQgBEAEEAKABKAEQAYQB0AGUAMQAsACAASgBEAGEAdABlADIALAAgAFsAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0AF0ALAAgAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0ALABcAG4AIAAgACAAIABJAEYAKAAoAEoARABhAHQAZQAxACAAPQAgAFwAIgBcACIAKQAgACoAIAAoAEoARABhAHQAZQAyACAAPQAgAFwAIgBcACIAKQAsACAAewBcACIAXAAiACwAIABcACIAXAAiACwAIABcACIAXAAiAH0ALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgASgBEAGEAdABlADEAKQApACAAKwAgAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgASgBEAGEAdABlADIAKQApACwAIAB7ACMAVgBBAEwAVQBFACEALAAgACMAVgBBAEwAVQBFACEALAAgACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdAB6AG8ALAAgAE4AKABUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAEEAQgBTACgAXwB0AHoAbwApACAAPgAgADkAMAAwACwAIAB7ACMATgBVAE0AIQAsACAAIwBOAFUATQAhACwAIAAjAE4AVQBNACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgASgBEAGEAdABlADIAIAA9ACAASgBEAGEAdABlADEALAAgAHsAMAAsACAAMAAsACAAMAB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGkAZwBuACwAIABJAEYAKABKAEQAYQB0AGUAMgAgAD4APQAgAEoARABhAHQAZQAxACwAIAAxACwAIAAtADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AagBkAG4ATABvAGMAYQBsAF8AUwB0AGEAcgB0ACwAIABKAEQAQQBUAEUAXwBUAE8AXwBKAEQATgBfAEwATwBDAEEATAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBzAGkAZwBuACAAPQAgADEALAAgAEoARABhAHQAZQAxACwAIABKAEQAYQB0AGUAMgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBvAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGoAZABuAEwAbwBjAGEAbABfAEUAbgBkACwAIABKAEQAQQBUAEUAXwBUAE8AXwBKAEQATgBfAEwATwBDAEEATAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBzAGkAZwBuACAAPQAgADEALAAgAEoARABhAHQAZQAyACwAIABKAEQAYQB0AGUAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBvAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAdABlAF8AUwB0AGEAcgB0ACwAIABKAEQATgBfAFQATwBfAEMAQQBMAEUATgBEAEEAUgBfAEQAQQBUAEUAKABJAE4ARABFAFgAKABfAGoAZABuAEwAbwBjAGEAbABfAFMAdABhAHIAdAAsACAAMQAsACAAMQApACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHQAZQBfAEUAbgBkACwAIABKAEQATgBfAFQATwBfAEMAQQBMAEUATgBEAEEAUgBfAEQAQQBUAEUAKABJAE4ARABFAFgAKABfAGoAZABuAEwAbwBjAGEAbABfAEUAbgBkACwAIAAxACwAIAAxACkALAAgAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGUAbAB0AGEAWQBlAGEAcgAsACAASQBOAEQARQBYACgAXwBkAGEAdABlAF8ARQBuAGQALAAgADEALAAgADEAKQAgAC0AIABJAE4ARABFAFgAKABfAGQAYQB0AGUAXwBTAHQAYQByAHQALAAgADEALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABlAGwAdABhAE0AbwBuAHQAaAAsACAASQBOAEQARQBYACgAXwBkAGEAdABlAF8ARQBuAGQALAAgADEALAAgADIAKQAgAC0AIABJAE4ARABFAFgAKABfAGQAYQB0AGUAXwBTAHQAYQByAHQALAAgADEALAAgADIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABpAGYAZgBNAG8AbgB0AGgAcwAsACAAKABfAGQAZQBsAHQAYQBZAGUAYQByACAAKgAgADEAMgApACAAKwAgAF8AZABlAGwAdABhAE0AbwBuAHQAaAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABlAGwAdABhAEQAYQB5ACwAIABJAE4ARABFAFgAKABfAGQAYQB0AGUAXwBFAG4AZAAsACAAMQAsACAAMwApACAALQAgAEkATgBEAEUAWAAoAF8AZABhAHQAZQBfAFMAdABhAHIAdAAsACAAMQAsACAAMwApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKwAgAEkATgBEAEUAWAAoAF8AagBkAG4ATABvAGMAYQBsAF8ARQBuAGQALAAgADEALAAgADIAKQAgAC0AIABJAE4ARABFAFgAKABfAGoAZABuAEwAbwBjAGEAbABfAFMAdABhAHIAdAAsACAAMQAsACAAMgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAF8AZABlAGwAdABhAEQAYQB5ACAAPAAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkAcwBNAG8AbgB0AGgAXwBTAHQAYQByAHQALAAgAEQAQQBZAFMAXwBJAE4AXwBNAE8ATgBUAEgAKABJAE4ARABFAFgAKABfAGQAYQB0AGUAXwBTAHQAYQByAHQALAAgADEALAAgADIAKQAsACAASQBOAEQARQBYACgAXwBkAGEAdABlAF8AUwB0AGEAcgB0ACwAIAAxACwAIAAxACkALAAgAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGkAZwBuACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGkAZgBmAE0AbwBuAHQAaABzACAALQAgADEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAYQB5AHMATQBvAG4AdABoAF8AUwB0AGEAcgB0ACAAKwAgAF8AZABlAGwAdABhAEQAYQB5AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGkAZwBuACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABpAGYAZgBNAG8AbgB0AGgAcwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAZQBsAHQAYQBEAGEAeQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEQARQBMAFQAQQBfAFEAVQBBAFIAVABFAFIAXwBEAEEAWQBTAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAHQAaABlACAAdABpAG0AZQBzAHAAYQBuACAAZABpAGYAZgBlAHIAZQBuAGMAZQAgAGIAZQB0AHcAZQBlAG4AIABKAHUAbABpAGEAbgAgAEQAYQB0AGUAcwAgAGkAbgAgAHEAdQBhAHIAdABlAHIAcwAgAGEAbgBkACAAZABhAHkAcwAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABpAG4AdABlAGcAZQByACAAWwAtADEALAAwACwAMQBdACAAfAAgAFMAaQBnAG4AXABuACAAMgAgAHwAIABpAG4AdABlAGcAZQByACAAWwAwAC4ALgBdACAAIAAgACAAfAAgAEQAZQBsAHQAYQAgAHEAdQBhAHIAdABlAHIAcwBcAG4AIAAzACAAfAAgAGQAZQBjAGkAbQBhAGwAIABbADAALgAuADkAMgApACAAIAB8ACAARABlAGwAdABhACAAZABhAHkAcwBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEoARABhAHQAZQAxACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgACAAIAAgACAAIAAgACAAIAB8ACAAXABuAEoARABhAHQAZQAyACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgACAAIAAgACAAIAAgACAAIAB8ACAAXABuAFsAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0AF0AIAB8ACAAZABlAGMAaQBtAGEAbAAgACAAIAAgACAAIAAgACAAIAB8ACAAVABpAG0AZQAgAHoAbwBuAGUAIABvAGYAZgBzAGUAdAAgAGkAbgAgAG0AaQBuAHUAdABlAHMAIABmAHIAbwBtACAAVQBUAEMALgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABbAC0AOQAwADAALgAuADkAMAAwAF0AIAAgACAAIAAgAHwAIABBAHMAcwB1AG0AZQBkACAAdABvACAAYgBlACAAVQBUAEMAIABpAGYAIABvAG0AbQBpAHQAdABlAGQALgBcAG4AWwBNAG8AbgB0AGgATwBmAGYAcwBlAHQAXQAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAWwAtADYALgAuADMAXQAgAHwAIABRAHUAYQByAHQAZQByACAAbQBvAG4AdABoACAAbwBmAGYAcwBlAHQAIABmAHIAbwBtACAASgBhAG4AdQBhAHIAeQAuAFwAbgBbAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACAAfAAgAHMAdwBpAHQAYwBoACAAIAAgACAAIAAgACAAIAAgACAAfAAgAEMAYQBsAGMAdQBsAGEAdABlACAAaQBuACAAdABoAGUAIABKAHUAbABpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AIABEAGUAZgBhAHUAbAB0ACAAaQBzACAARwByAGUAZwBvAHIAaQBhAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ARABFAEwAVABBAF8AUQBVAEEAUgBUAEUAUgBfAEQAQQBZAFMAIAA9ACAATABBAE0AQgBEAEEAKABKAEQAYQB0AGUAMQAsACAASgBEAGEAdABlADIALAAgAFsAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0AF0ALAAgAFsATQBvAG4AdABoAE8AZgBmAHMAZQB0AF0ALAAgAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0ALABcAG4AIAAgACAAIABJAEYAKAAoAEoARABhAHQAZQAxACAAPQAgAFwAIgBcACIAKQAgACoAIAAoAEoARABhAHQAZQAyACAAPQAgAFwAIgBcACIAKQAsACAAewBcACIAXAAiACwAIABcACIAXAAiACwAIABcACIAXAAiAH0ALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgASgBEAGEAdABlADEAKQApACAAKwAgAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgASgBEAGEAdABlADIAKQApACwAIAB7ACMAVgBBAEwAVQBFACEALAAgACMAVgBBAEwAVQBFACEALAAgACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdAB6AG8ALAAgAE4AKABUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbQBvAG4AdABoAE8AZgBmAHMAZQB0ACwAIABSAE8AVQBOAEQAKABOACgATQBvAG4AdABoAE8AZgBmAHMAZQB0ACkALAAgADAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoACgAQQBCAFMAKABfAHQAegBvACkAIAA+ACAAOQAwADAAKQAgACsAIAAoAF8AbQBvAG4AdABoAE8AZgBmAHMAZQB0ACAAPAAgAC0ANgApACAAKwAgACgAXwBtAG8AbgB0AGgATwBmAGYAcwBlAHQAIAA+ACAAMwApACwAIAB7ACMATgBVAE0AIQAsACAAIwBOAFUATQAhACwAIAAjAE4AVQBNACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgASgBEAGEAdABlADIAIAA9ACAASgBEAGEAdABlADEALAAgAHsAIAAwACwAIAAwACAALAAwAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaQBnAG4ALAAgAEkARgAoAEoARABhAHQAZQAxACAAPgAgAEoARABhAHQAZQAyACwAIAAtADEALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AagBkAG4ATABvAGMAYQBsAF8AUwB0AGEAcgB0ACwAIABKAEQAQQBUAEUAXwBUAE8AXwBKAEQATgBfAEwATwBDAEEATAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBzAGkAZwBuACAAPQAgADEALAAgAEoARABhAHQAZQAxACwAIABKAEQAYQB0AGUAMgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBvAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGoAZABuAEwAbwBjAGEAbABfAEUAbgBkACwAIABKAEQAQQBUAEUAXwBUAE8AXwBKAEQATgBfAEwATwBDAEEATAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBzAGkAZwBuACAAPQAgADEALAAgAEoARABhAHQAZQAyACwAIABKAEQAYQB0AGUAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBvAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHEAdQBhAHIAdABlAHIARABhAHQAZQBfAFMAdABhAHIAdAAsACAASgBEAE4AXwBUAE8AXwBRAFUAQQBSAFQARQBSAF8ARABBAFQARQAoAEkATgBEAEUAWAAoAF8AagBkAG4ATABvAGMAYQBsAF8AUwB0AGEAcgB0ACwAIAAxACwAIAAxACkALAAgAF8AbQBvAG4AdABoAE8AZgBmAHMAZQB0ACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcQB1AGEAcgB0AGUAcgBEAGEAdABlAF8ARQBuAGQALAAgAEoARABOAF8AVABPAF8AUQBVAEEAUgBUAEUAUgBfAEQAQQBUAEUAKABJAE4ARABFAFgAKABfAGoAZABuAEwAbwBjAGEAbABfAEUAbgBkACwAIAAxACwAIAAxACkALAAgAF8AbQBvAG4AdABoAE8AZgBmAHMAZQB0ACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABlAGwAdABhAFkAZQBhAHIALAAgAEkATgBEAEUAWAAoAF8AcQB1AGEAcgB0AGUAcgBEAGEAdABlAF8ARQBuAGQALAAgADEALAAgADEAKQAgAC0AIABJAE4ARABFAFgAKABfAHEAdQBhAHIAdABlAHIARABhAHQAZQBfAFMAdABhAHIAdAAsACAAMQAsACAAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGUAbAB0AGEAUQB1AGEAcgB0AGUAcgAsACAASQBOAEQARQBYACgAXwBxAHUAYQByAHQAZQByAEQAYQB0AGUAXwBFAG4AZAAsACAAMQAsACAAMgApACAALQAgAEkATgBEAEUAWAAoAF8AcQB1AGEAcgB0AGUAcgBEAGEAdABlAF8AUwB0AGEAcgB0ACwAIAAxACwAIAAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAaQBmAGYAUQB1AGEAcgB0AGUAcgBzACwAIAAoAF8AZABlAGwAdABhAFkAZQBhAHIAIAAqACAANAApACAAKwAgAF8AZABlAGwAdABhAFEAdQBhAHIAdABlAHIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAZQBsAHQAYQBEAGEAeQAsACAASQBOAEQARQBYACgAXwBxAHUAYQByAHQAZQByAEQAYQB0AGUAXwBFAG4AZAAsACAAMQAsACAAMwApACAALQAgAEkATgBEAEUAWAAoAF8AcQB1AGEAcgB0AGUAcgBEAGEAdABlAF8AUwB0AGEAcgB0ACwAIAAxACwAIAAzACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAArACAASQBOAEQARQBYACgAXwBqAGQAbgBMAG8AYwBhAGwAXwBFAG4AZAAsACAAMQAsACAAMgApACAALQAgAEkATgBEAEUAWAAoAF8AagBkAG4ATABvAGMAYQBsAF8AUwB0AGEAcgB0ACwAIAAxACwAIAAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBkAGUAbAB0AGEARABhAHkAIAA8ACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQBzAFEAdQBhAHIAdABlAHIAXwBTAHQAYQByAHQALAAgAEkATgBEAEUAWAAoAF8AcQB1AGEAcgB0AGUAcgBEAGEAdABlAF8AUwB0AGEAcgB0ACwAIAAxACwAIAA0ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaQBnAG4ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAaQBmAGYAUQB1AGEAcgB0AGUAcgBzACAALQAgADEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAYQB5AHMAUQB1AGEAcgB0AGUAcgBfAFMAdABhAHIAdAAgACsAIABfAGQAZQBsAHQAYQBEAGEAeQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBpAGcAbgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAaQBmAGYAUQB1AGEAcgB0AGUAcgBzACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABlAGwAdABhAEQAYQB5AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ARABFAEwAVABBAF8ASQBOAFQARQBSAFYAQQBMAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAHQAaABlACAAdABpAG0AZQBzAHAAYQBuACAAZABpAGYAZgBlAHIAZQBuAGMAZQAgAGIAZQB0AHcAZQBlAG4AIABKAHUAbABpAGEAbgAgAEQAYQB0AGUAcwAgAGkAbgAgAHQAaABlACAAcwBwAGUAYwBpAGYAaQBlAGQAIAB1AG4AaQB0AHMALgBcAG4AXABuAE8AdQB0AHAAdQB0ACAAdwBoAGUAcgBlACAAVQBuAGkAdABzACAAPQAgAEgALAAgAE4ALAAgAFMALAAgAEQALAAgAFcALAAgAE0ALAAgAFEALAAgAFkAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgAEQAZQBsAHQAYQAgAHUAbgBpAHQAcwAgAGQAZQBjAGkAbQBhAGwAXABuAFwAbgBPAHUAdABwAHUAdAAgAHcAaABlAHIAZQAgAFUAbgBpAHQAcwAgAD0AIABIAE0AUwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbAC0AMQAsADAALAAxAF0AIAB8ACAAUwBpAGcAbgBcAG4AIAAyACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADAALgAuAF0AIAAgACAAIAB8ACAARABlAGwAdABhACAAaABvAHUAcgBzAFwAbgAgADMAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMAAuAC4ANQA5AF0AIAAgAHwAIABEAGUAbAB0AGEAIABtAGkAbgB1AHQAZQBzAFwAbgAgADQAIAB8ACAAZABlAGMAaQBtAGEAbAAgAFsAMAAuAC4ANgAwACkAIAAgAHwAIABEAGUAbAB0AGEAIABzAGUAYwBvAG4AZABzAFwAbgBcAG4ATwB1AHQAcAB1AHQAIAB3AGgAZQByAGUAIABVAG4AaQB0AHMAIAA9ACAARABIAE0AUwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbAC0AMQAsADAALAAxAF0AIAB8ACAAUwBpAGcAbgBcAG4AIAAyACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADAALgAuAF0AIAAgACAAIAB8ACAARABlAGwAdABhACAAZABhAHkAcwBcAG4AIAAzACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADAALgAuADIAMwBdACAAIAB8ACAARABlAGwAdABhACAAaABvAHUAcgBzAFwAbgAgADQAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMAAuAC4ANQA5AF0AIAAgAHwAIABEAGUAbAB0AGEAIABtAGkAbgB1AHQAZQBzAFwAbgAgADUAIAB8ACAAZABlAGMAaQBtAGEAbAAgAFsAMAAuAC4ANgAwACkAIAAgAHwAIABEAGUAbAB0AGEAIABzAGUAYwBvAG4AZABzAFwAbgBcAG4ATwB1AHQAcAB1AHQAIAB3AGgAZQByAGUAIABVAG4AaQB0AHMAIAA9ACAAVwBEACwAIABNAEQALAAgAFEARABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbAC0AMQAsADAALAAxAF0AIAAgACAAIAAgAHwAIABTAGkAZwBuAFwAbgAgADIAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMAAuAC4AXQAgACAAIAAgACAAIAAgACAAfAAgAEQAZQBsAHQAYQAgAHcAZQBlAGsAcwAvAG0AbwBuAHQAaABzAC8AcQB1AGEAcgB0AGUAcgBzAFwAbgAgADMAIAB8ACAAZABlAGMAaQBtAGEAbAAgAFsAMAAuAC4ANwAvADMAMQAvADkAMgApACAAfAAgAEQAZQBsAHQAYQAgAGQAYQB5AHMAXABuAFwAbgBPAHUAdABwAHUAdAAgAHcAaABlAHIAZQAgAFUAbgBpAHQAcwAgAD0AIABZAFcARAAsACAAWQBNAEQALAAgAFkAUQBEAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsALQAxACwAMAAsADEAXQAgACAAIAAgACAAfAAgAFMAaQBnAG4AXABuACAAMgAgAHwAIABpAG4AdABlAGcAZQByACAAWwAwAC4ALgBdACAAIAAgACAAIAAgACAAIAB8ACAARABlAGwAdABhACAAeQBlAGEAcgBzAFwAbgAgADMAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMAAuAC4ANQAyAC8AMQAyAC8ANABdACAAfAAgAEQAZQBsAHQAYQAgAHcAZQBlAGsAcwAvAG0AbwBuAHQAaABzAC8AcQB1AGEAcgB0AGUAcgBzAFwAbgAgADQAIAB8ACAAZABlAGMAaQBtAGEAbAAgAFsAMAAuAC4ANwAvADMAMQAvADkAMgApACAAfAAgAEQAZQBsAHQAYQAgAGQAYQB5AHMAXABuAFwAbgBPAHUAdABwAHUAdAAgAHcAaABlAHIAZQAgAFUAbgBpAHQAcwAgAD0AIABZAE0ARABIAE0AUwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbAC0AMQAsADAALAAxAF0AIAB8ACAAUwBpAGcAbgBcAG4AIAAyACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADAALgAuAF0AIAAgACAAIAB8ACAARABlAGwAdABhACAAeQBlAGEAcgBzAFwAbgAgADMAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMAAuAC4AMQAyAF0AIAAgAHwAIABEAGUAbAB0AGEAIABtAG8AbgB0AGgAcwBcAG4AIAA0ACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADAALgAuADMAMABdACAAIAB8ACAARABlAGwAdABhACAAZABhAHkAcwBcAG4AIAA1ACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADAALgAuADIAMwBdACAAIAB8ACAARABlAGwAdABhACAAaABvAHUAcgBzAFwAbgAgADYAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMAAuAC4ANQA5AF0AIAAgAHwAIABEAGUAbAB0AGEAIABtAGkAbgB1AHQAZQBzAFwAbgAgADcAIAB8ACAAZABlAGMAaQBtAGEAbAAgAFsAMAAuAC4ANgAwACkAIAAgAHwAIABEAGUAbAB0AGEAIABzAGUAYwBvAG4AZABzAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AVQBuAGkAdABzACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAB0AGUAeAB0ACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAASAAgAC0AIABoAG8AdQByAHMAIABkAGUAYwBpAG0AYQBsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIABOACAALQAgAG0AaQBuAHUAdABlAHMAIABkAGUAYwBpAG0AYQBsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIABTACAALQAgAHMAZQBjAG8AbgBkAHMAIABkAGUAYwBpAG0AYQBsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIABEACAALQAgAGQAYQB5AHMAIABkAGUAYwBpAG0AYQBsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIABXACAALQAgAHcAZQBlAGsAcwAgAGQAZQBjAGkAbQBhAGwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgAE0AIAAtACAAbQBvAG4AdABoAHMAIABkAGUAYwBpAG0AYQBsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIABRACAALQAgAHEAdQBhAHIAdABlAHIAcwAgAGQAZQBjAGkAbQBhAGwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgAFkAIAAtACAAeQBlAGEAcgBzACAAZABlAGMAaQBtAGEAbABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIABIAE0AUwAgAC0AIABoAG8AdQByAHMALAAgAG0AaQBuAHUAdABlAHMALAAgAHMAZQBjAG8AbgBkAHMAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgAEQASABNAFMAIAAtACAAZABhAHkAcwAsACAAaABvAHUAcgBzACwAIABtAGkAbgB1AHQAZQBzACwAIABzAGUAYwBvAG4AZABzAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAVwBEACAALQAgAHcAZQBlAGsAcwAgAGEAbgBkACAAZABhAHkAcwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgAE0ARAAgAC0AIABtAG8AbgB0AGgAcwAgAGEAbgBkACAAZABhAHkAcwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgAFEARAAgAC0AIABxAHUAYQByAHQAZQByAHMAIABhAG4AZAAgAGQAYQB5AHMAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAWQBXAEQAIAAtACAAeQBlAGEAcgBzACwAIAB3AGUAZQBrAHMALAAgAGQAYQB5AHMAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAWQBNAEQAIAAtACAAeQBlAGEAcgBzACwAIABtAG8AbgB0AGgAcwAsACAAZABhAHkAcwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIABZAFEARAAgAC0AIAB5AGUAYQByAHMALAAgAHEAdQBhAHIAdABlAHIAcwAsACAAZABhAHkAcwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABZAE0ARABIAE0AUwAgAC0AIAB5AGUAYQByAHMALAAgAG0AbwBuAHQAaABzACwAIABkAGEAeQBzACwAIABoAG8AdQByAHMALAAgAG0AaQBuAHUAdABlAHMALAAgAHMAZQBjAG8AbgBkAHMAXABuAEoARABhAHQAZQAxACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgACAAIAAgACAAIAAgACAAIAB8ACAAXABuAEoARABhAHQAZQAyACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgACAAIAAgACAAIAAgACAAIAB8ACAAXABuAFsAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0AF0AIAB8ACAAZABlAGMAaQBtAGEAbAAgACAAIAAgACAAIAAgACAAIAB8ACAAVABpAG0AZQAgAHoAbwBuAGUAIABvAGYAZgBzAGUAdAAgAGkAbgAgAG0AaQBuAHUAdABlAHMAIABmAHIAbwBtACAAVQBUAEMALgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABbAC0AOQAwADAALgAuADkAMAAwAF0AIAAgACAAIAAgAHwAIABBAHMAcwB1AG0AZQBkACAAdABvACAAYgBlACAAVQBUAEMAIABpAGYAIABvAG0AbQBpAHQAdABlAGQALgBcAG4AWwBNAG8AbgB0AGgATwBmAGYAcwBlAHQAXQAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAWwAtADYALgAuADMAXQAgAHwAIABRAHUAYQByAHQAZQByACAAbQBvAG4AdABoACAAbwBmAGYAcwBlAHQAIABmAHIAbwBtACAASgBhAG4AdQBhAHIAeQAuAFwAbgBbAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACAAfAAgAHMAdwBpAHQAYwBoACAAIAAgACAAIAAgACAAIAAgACAAfAAgAEMAYQBsAGMAdQBsAGEAdABlACAAaQBuACAAdABoAGUAIABKAHUAbABpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AIABEAGUAZgBhAHUAbAB0ACAAaQBzACAARwByAGUAZwBvAHIAaQBhAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ARABFAEwAVABBAF8ASQBOAFQARQBSAFYAQQBMACAAPQAgAEwAQQBNAEIARABBACgAVQBuAGkAdABzACwAIABKAEQAYQB0AGUAMQAsACAASgBEAGEAdABlADIALAAgAFsAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0AF0ALAAgAFsATQBvAG4AdABoAE8AZgBmAHMAZQB0AF0ALAAgAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0ALABcAG4AIAAgACAAIABJAEYAUwAoAFwAbgAgACAAIAAgACAAIAAgACAAVQBuAGkAdABzACAAPQAgAFwAIgBcACIALAAgAHsAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIABVAG4AaQB0AHMAIAA9ACAAXAAiAEgAXAAiACwAIABEAEUATABUAEEAXwBIAE8AVQBSAFMAKABKAEQAYQB0AGUAMQAsACAASgBEAGEAdABlADIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAVQBuAGkAdABzACAAPQAgAFwAIgBOAFwAIgAsACAARABFAEwAVABBAF8ATQBJAE4AVQBUAEUAUwAoAEoARABhAHQAZQAxACwAIABKAEQAYQB0AGUAMgApACwAXABuACAAIAAgACAAIAAgACAAIABVAG4AaQB0AHMAIAA9ACAAXAAiAFMAXAAiACwAIABEAEUATABUAEEAXwBTAEUAQwBPAE4ARABTACgASgBEAGEAdABlADEALAAgAEoARABhAHQAZQAyACkALABcAG4AIAAgACAAIAAgACAAIAAgAFUAbgBpAHQAcwAgAD0AIABcACIASABNAFMAXAAiACwAIABEAEUATABUAEEAXwBIAE8AVQBSAF8ATQBJAE4AXwBTAEUAQwAoAEoARABhAHQAZQAxACwAIABKAEQAYQB0AGUAMgApACwAXABuACAAIAAgACAAIAAgACAAIABVAG4AaQB0AHMAIAA9ACAAXAAiAEQAXAAiACwAIABEAEUATABUAEEAXwBEAEEAWQBTACgASgBEAGEAdABlADEALAAgAEoARABhAHQAZQAyACkALABcAG4AIAAgACAAIAAgACAAIAAgAFUAbgBpAHQAcwAgAD0AIABcACIAVwBcACIALAAgAEQARQBMAFQAQQBfAFcARQBFAEsAUwAoAEoARABhAHQAZQAxACwAIABKAEQAYQB0AGUAMgApACwAXABuACAAIAAgACAAIAAgACAAIABVAG4AaQB0AHMAIAA9ACAAXAAiAE0AXAAiACwAIABEAEUATABUAEEAXwBNAE8ATgBUAEgAUwAoAEoARABhAHQAZQAxACwAIABKAEQAYQB0AGUAMgAsACAAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0ACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAVQBuAGkAdABzACAAPQAgAFwAIgBRAFwAIgAsACAARABFAEwAVABBAF8AUQBVAEEAUgBUAEUAUgBTACgASgBEAGEAdABlADEALAAgAEoARABhAHQAZQAyACwAIABUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQALAAgAE0AbwBuAHQAaABPAGYAZgBzAGUAdAAsACAASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByACkALABcAG4AIAAgACAAIAAgACAAIAAgAFUAbgBpAHQAcwAgAD0AIABcACIAWQBcACIALAAgAEQARQBMAFQAQQBfAFkARQBBAFIAUwAoAEoARABhAHQAZQAxACwAIABKAEQAYQB0AGUAMgAsACAAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0ACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAVQBuAGkAdABzACAAPQAgAFwAIgBXAEQAXAAiACwAIABEAEUATABUAEEAXwBXAEUARQBLAF8ARABBAFkAUwAoAEoARABhAHQAZQAxACwAIABKAEQAYQB0AGUAMgApACwAXABuACAAIAAgACAAIAAgACAAIABVAG4AaQB0AHMAIAA9ACAAXAAiAFkAVwBEAFwAIgAsACAARABFAEwAVABBAF8AWQBFAEEAUgBfAFcARQBFAEsAXwBEAEEAWQBTACgASgBEAGEAdABlADEALAAgAEoARABhAHQAZQAyACwAIABUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQALAAgAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgApACwAXABuACAAIAAgACAAIAAgACAAIABVAG4AaQB0AHMAIAA9ACAAXAAiAE0ARABcACIALAAgAEQARQBMAFQAQQBfAE0ATwBOAFQASABfAEQAQQBZAFMAKABKAEQAYQB0AGUAMQAsACAASgBEAGEAdABlADIALAAgAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdAAsACAASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByACkALABcAG4AIAAgACAAIAAgACAAIAAgAFUAbgBpAHQAcwAgAD0AIABcACIAUQBEAFwAIgAsACAARABFAEwAVABBAF8AUQBVAEEAUgBUAEUAUgBfAEQAQQBZAFMAKABKAEQAYQB0AGUAMQAsACAASgBEAGEAdABlADIALAAgAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdAAsACAATQBvAG4AdABoAE8AZgBmAHMAZQB0ACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAVQBuAGkAdABzACAAPQAgAFwAIgBEAEgATQBTAFwAIgAsACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGgAbQBzACwAIABEAEUATABUAEEAXwBIAE8AVQBSAF8ATQBJAE4AXwBTAEUAQwAoAEoARABhAHQAZQAxACwAIABKAEQAYQB0AGUAMgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQBzACwAIABJAE4AVAAoAEkATgBEAEUAWAAoAF8AaABtAHMALAAgADEALAAgADIAKQAgAC8AIAAyADQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AaABvAHUAcgBzACwAIABJAE4ARABFAFgAKABfAGgAbQBzACwAIAAxACwAIAAyACkAIAAtACAAXwBkAGEAeQBzACAAKgAgADIANAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAE4ARABFAFgAKABfAGgAbQBzACwAIAAxACwAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkAcwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBoAG8AdQByAHMALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkATgBEAEUAWAAoAF8AaABtAHMALAAgADEALAAgADMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBOAEQARQBYACgAXwBoAG0AcwAsACAAMQAsACAANAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgAFUAbgBpAHQAcwAgAD0AIABcACIAWQBNAEQAXAAiACwAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbQBvAG4AdABoAEQAYQB5AHMALAAgAEQARQBMAFQAQQBfAE0ATwBOAFQASABfAEQAQQBZAFMAKABKAEQAYQB0AGUAMQAsACAASgBEAGEAdABlADIALAAgAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdAAsACAASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIAcwAsACAASQBOAFQAKABJAE4ARABFAFgAKABfAG0AbwBuAHQAaABEAGEAeQBzACwAIAAxACwAIAAyACkAIAAvACAAMQAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AbwBuAHQAaABzACwAIABJAE4ARABFAFgAKABfAG0AbwBuAHQAaABEAGEAeQBzACwAIAAxACwAIAAyACkAIAAtACAAXwB5AGUAYQByAHMAIAAqACAAMQAyACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkATgBEAEUAWAAoAF8AbQBvAG4AdABoAEQAYQB5AHMALAAgADEALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AGUAYQByAHMALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbQBvAG4AdABoAHMALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkATgBEAEUAWAAoAF8AbQBvAG4AdABoAEQAYQB5AHMALAAgADEALAAgADMAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIABVAG4AaQB0AHMAIAA9ACAAXAAiAFkAUQBEAFwAIgAsACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHEAdQBhAHIAdABlAHIARABhAHkAcwAsACAARABFAEwAVABBAF8AUQBVAEEAUgBUAEUAUgBfAEQAQQBZAFMAKABKAEQAYQB0AGUAMQAsACAASgBEAGEAdABlADIALAAgAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdAAsACAASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIAcwAsACAASQBOAFQAKABJAE4ARABFAFgAKABfAHEAdQBhAHIAdABlAHIARABhAHkAcwAsACAAMQAsACAAMgApACAALwAgADQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcQB1AGEAcgB0AGUAcgBzACwAIABJAE4ARABFAFgAKABfAHEAdQBhAHIAdABlAHIARABhAHkAcwAsACAAMQAsACAAMgApACAALQAgAF8AeQBlAGEAcgBzACAAKgAgADQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBOAEQARQBYACgAXwBxAHUAYQByAHQAZQByAEQAYQB5AHMALAAgADEALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AGUAYQByAHMALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcQB1AGEAcgB0AGUAcgBzACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAE4ARABFAFgAKABfAHEAdQBhAHIAdABlAHIARABhAHkAcwAsACAAMQAsACAAMwApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgAFUAbgBpAHQAcwAgAD0AIABcACIAWQBNAEQASABNAFMAXAAiACwAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbQBvAG4AdABoAEQAYQB5AHMALAAgAEQARQBMAFQAQQBfAE0ATwBOAFQASABfAEQAQQBZAFMAKABKAEQAYQB0AGUAMQAsACAASgBEAGEAdABlADIALAAgAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdAAsACAASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIAcwAsACAASQBOAFQAKABJAE4ARABFAFgAKABfAG0AbwBuAHQAaABEAGEAeQBzACwAIAAxACwAIAAyACkAIAAvACAAMQAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AbwBuAHQAaABzACwAIABJAE4ARABFAFgAKABfAG0AbwBuAHQAaABEAGEAeQBzACwAIAAxACwAIAAyACkAIAAtACAAXwB5AGUAYQByAHMAIAAqACAAMQAyACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQBzACwAIABJAE4AVAAoAEkATgBEAEUAWAAoAF8AbQBvAG4AdABoAEQAYQB5AHMALAAgADEALAAgADMAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AGkAbQBlACwAIABJAE4ARABFAFgAKABfAG0AbwBuAHQAaABEAGEAeQBzACwAIAAxACwAIAAzACkAIAAtACAAXwBkAGEAeQBzACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBoAG0AcwAsACAAVABJAE0ARQBfAEQARQBDAEkATQBBAEwAXwBUAE8AXwBIAE0AUwAoAF8AdABpAG0AZQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkATgBEAEUAWAAoAF8AbQBvAG4AdABoAEQAYQB5AHMALAAgADEALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AGUAYQByAHMALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbQBvAG4AdABoAHMALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkAcwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAARABSAE8AUAAoAF8AaABtAHMALAAsACAAMQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALAAgAHsAIwBWAEEATABVAEUAIQB9AFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAFwAbgBcAG4AXABuAFwAbgBcAG4AXABuAFwAbgBcAG4AXABuAFwAbgBcAG4ALwAqACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwBcAG4AIwAgAEUAWABUAEUATgBUAFMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACoALwBcAG4AXABuAFwAbgBcAG4AXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBFAFgAVABFAE4AVABfAE8ARgBfAEQAQQBZAFMAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIABpAG4AYwBsAHUAcwBpAHYAZQAgAGUAeAB0AGUAbgB0ACAAbwBmACAAZABhAHkAcwAgAHMAcABhAG4AbgBlAGQAIABiAHkAIAB0AHcAbwAgAEoAdQBsAGkAYQBuACAARABhAHQAZQBzAC4AXABuAFwAbgBPAHUAdABwAHUAdABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAARQB4AHQAZQBuAHQAIABvAGYAIABkAGEAeQBzAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ASgBEAGEAdABlADEAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAIAAgACAAIAB8ACAAXABuAEoARABhAHQAZQAyACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgACAAIAAgACAAfAAgAFwAbgBbAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdABdACAAfAAgAGQAZQBjAGkAbQBhAGwAIAAgACAAIAAgAHwAIABUAGkAbQBlACAAegBvAG4AZQAgAG8AZgBmAHMAZQB0ACAAaQBuACAAbQBpAG4AdQB0AGUAcwAgAGYAcgBvAG0AIABVAFQAQwAuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAFsALQA5ADAAMAAuAC4AOQAwADAAXQAgAHwAIABBAHMAcwB1AG0AZQBkACAAdABvACAAYgBlACAAVQBUAEMAIABpAGYAIABvAG0AbQBpAHQAdABlAGQALgBcAG4AXABuAEUAeABhAG0AcABsAGUAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ARQBYAFQARQBOAFQAXwBEAEEAWQBTACgASgBVAEwASQBBAE4AXwBEAEEAVABFACgAMgAwADIAMwAsADEALAAxACwAVABJAE0ARQAoADIAMwAsADUAOQAsADUANQApACkALAAgAEoAVQBMAEkAQQBOAF8ARABBAFQARQAoADIAMAAyADMALAAxACwAMgAsAFQASQBNAEUAKAAwACwAMAAsADUAKQApACkAXABuAD0AIAAyACAAIABpAC4AZQAuACAAMgAgAGQAYQB5AHMAIABiAGUAYwBhAHUAcwBlACAAdABoAGUAIAAxADAAIABzAGUAYwBvAG4AZAAgAHQAaQBtAGUAcwBwAGEAbgAgAGMAcgBvAHMAcwBlAHMAIAB0AGgAZQAgAGQAYQB5ACAAYgBvAHUAbgBkAGEAcgB5AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBFAFgAVABFAE4AVABfAE8ARgBfAEQAQQBZAFMAIAA9ACAATABBAE0AQgBEAEEAKABKAEQAYQB0AGUAMQAsACAASgBEAGEAdABlADIALAAgAFsAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0AF0ALABcAG4AIAAgACAAIABJAEYAKAAoAEoARABhAHQAZQAxACAAPQAgAFwAIgBcACIAKQAgACoAIAAoAEoARABhAHQAZQAyACAAPQAgAFwAIgBcACIAKQAsACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABKAEQAYQB0AGUAMQApACkAIAArACAATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABKAEQAYQB0AGUAMgApACkALAAgAHsAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AHoAbwAsACAATgAoAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAQQBCAFMAKABfAHQAegBvACkAIAA+ACAAOQAwADAALAAgAHsAIwBOAFUATQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBpAGcAbgAsACAASQBGACgASgBEAGEAdABlADIAIAA+AD0AIABKAEQAYQB0AGUAMQAsACAAMQAsACAALQAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBqAGQAbgBMAG8AYwBhAGwAMQAsACAASgBEAEEAVABFAF8AVABPAF8ASgBEAE4AXwBMAE8AQwBBAEwAKABKAEQAYQB0AGUAMQAsACAAXwB0AHoAbwApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AagBkAG4ATABvAGMAYQBsADIALAAgAEoARABBAFQARQBfAFQATwBfAEoARABOAF8ATABPAEMAQQBMACgASgBEAGEAdABlADIALAAgAF8AdAB6AG8AKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAZQBsAHQAYQBEAGEAeQAsACAASQBOAEQARQBYACgAXwBqAGQAbgBMAG8AYwBhAGwAMgAsACAAMQAsACAAMQApACAALQAgAEkATgBEAEUAWAAoAF8AagBkAG4ATABvAGMAYQBsADEALAAgADEALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaQBnAG4AIAAqACAAKABBAEIAUwAoAF8AZABlAGwAdABhAEQAYQB5ACkAIAArACAAMQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEUAWABUAEUATgBUAF8ATwBGAF8AVwBFAEUASwBTAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAHQAaABlACAAaQBuAGMAbAB1AHMAaQB2AGUAIABlAHgAdABlAG4AdAAgAG8AZgAgAHcAZQBlAGsAcwAgAHMAcABhAG4AbgBlAGQAIABiAHkAIAB0AHcAbwAgAEoAdQBsAGkAYQBuACAARABhAHQAZQBzAC4AXABuAFwAbgBPAHUAdABwAHUAdABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAARQB4AHQAZQBuAHQAIABvAGYAIAB3AGUAZQBrAHMAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBKAEQAYQB0AGUAMQAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAAgACAAIAAgAHwAIABcAG4ASgBEAGEAdABlADIAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAIAAgACAAIAB8ACAAXABuAFsAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0AF0AIAB8ACAAZABlAGMAaQBtAGEAbAAgACAAIAAgACAAfAAgAFQAaQBtAGUAIAB6AG8AbgBlACAAbwBmAGYAcwBlAHQAIABpAG4AIABtAGkAbgB1AHQAZQBzACAAZgByAG8AbQAgAFUAVABDAC4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAWwAtADkAMAAwAC4ALgA5ADAAMABdACAAfAAgAEEAcwBzAHUAbQBlAGQAIAB0AG8AIABiAGUAIABVAFQAQwAgAGkAZgAgAG8AbQBtAGkAdAB0AGUAZAAuAFwAbgBcAG4ARQB4AGEAbQBwAGwAZQBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBFAFgAVABFAE4AVABfAEQAQQBZAFMAKABKAFUATABJAEEATgBfAEQAQQBUAEUAKAAyADAAMgAzACwANgAsADQALABUAEkATQBFACgAMgAzACwANQA5ACwANQA1ACkAKQAsACAASgBVAEwASQBBAE4AXwBEAEEAVABFACgAMgAwADIAMwAsADYALAA1ACwAVABJAE0ARQAoADAALAAwACwANQApACkAKQBcAG4APQAgADIAIAAgAGkALgBlAC4AIAAyACAAdwBlAGUAawBzACAAYgBlAGMAYQB1AHMAZQAgAHQAaABlACAAMQAwACAAcwBlAGMAbwBuAGQAIAB0AGkAbQBlAHMAcABhAG4AIABjAHIAbwBzAHMAZQBzACAAdABoAGUAIAB3AGUAZQBrACAAYgBvAHUAbgBkAGEAcgB5AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBFAFgAVABFAE4AVABfAE8ARgBfAFcARQBFAEsAUwAgAD0AIABMAEEATQBCAEQAQQAoAEoARABhAHQAZQAxACwAIABKAEQAYQB0AGUAMgAsACAAWwBUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQAXQAsAFwAbgAgACAAIAAgAEkARgAoACgASgBEAGEAdABlADEAIAA9ACAAXAAiAFwAIgApACAAKgAgACgASgBEAGEAdABlADIAIAA9ACAAXAAiAFwAIgApACwAIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEoARABhAHQAZQAxACkAKQAgACsAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEoARABhAHQAZQAyACkAKQAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBvACwAIABOACgAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABBAEIAUwAoAF8AdAB6AG8AKQAgAD4AIAA5ADAAMAAsACAAewAjAE4AVQBNACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGkAZwBuACwAIABJAEYAKABKAEQAYQB0AGUAMgAgAD4APQAgAEoARABhAHQAZQAxACwAIAAxACwAIAAtADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGoAZABuAEwAbwBjAGEAbABfAFMAdABhAHIAdAAsACAASgBEAEEAVABFAF8AVABPAF8ASgBEAE4AXwBMAE8AQwBBAEwAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAHMAaQBnAG4AIAA9ACAAMQAsACAASgBEAGEAdABlADEALAAgAEoARABhAHQAZQAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBvAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AagBkAG4ATABvAGMAYQBsAF8ARQBuAGQALAAgAEoARABBAFQARQBfAFQATwBfAEoARABOAF8ATABPAEMAQQBMACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBzAGkAZwBuACAAPQAgADEALAAgAEoARABhAHQAZQAyACwAIABKAEQAYQB0AGUAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AHoAbwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGoAZABuAE0AbwBuAGQAYQB5AF8AUwB0AGEAcgB0ACwAIABJAE4ARABFAFgAKABfAGoAZABuAEwAbwBjAGEAbABfAFMAdABhAHIAdAAsACAAMQAsACAAMQApACAAKwAgADEAIAAtACAARABBAFkAXwBPAEYAXwBXAEUARQBLACgASQBOAEQARQBYACgAXwBqAGQAbgBMAG8AYwBhAGwAXwBTAHQAYQByAHQALAAgADEALAAgADEAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AagBkAG4ATQBvAG4AZABhAHkAXwBFAG4AZAAsACAASQBOAEQARQBYACgAXwBqAGQAbgBMAG8AYwBhAGwAXwBFAG4AZAAsACAAMQAsACAAMQApACAAKwAgADEAIAAtACAARABBAFkAXwBPAEYAXwBXAEUARQBLACgASQBOAEQARQBYACgAXwBqAGQAbgBMAG8AYwBhAGwAXwBFAG4AZAAsACAAMQAsACAAMQApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGkAZwBuACAAKgAgAEkATgBUACgAKABfAGoAZABuAE0AbwBuAGQAYQB5AF8ARQBuAGQAIAAtACAAXwBqAGQAbgBNAG8AbgBkAGEAeQBfAFMAdABhAHIAdAApACAALwAgADcAIAArACAAMQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ARQBYAFQARQBOAFQAXwBPAEYAXwBNAE8ATgBUAEgAUwBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAGkAbgBjAGwAdQBzAGkAdgBlACAAZQB4AHQAZQBuAHQAIABvAGYAIABtAG8AbgB0AGgAcwAgAHMAcABhAG4AbgBlAGQAIABiAHkAIAB0AHcAbwAgAEoAdQBsAGkAYQBuACAARABhAHQAZQBzAC4AXABuAFwAbgBPAHUAdABwAHUAdABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAARQB4AHQAZQBuAHQAIABvAGYAIABtAG8AbgB0AGgAcwBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEoARABhAHQAZQAxACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgACAAIAAgACAAfABcAG4ASgBEAGEAdABlADIAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAIAAgACAAIAB8AFwAbgBbAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdABdACAAfAAgAGQAZQBjAGkAbQBhAGwAIAAgACAAIAAgAHwAIABUAGkAbQBlACAAegBvAG4AZQAgAG8AZgBmAHMAZQB0ACAAaQBuACAAbQBpAG4AdQB0AGUAcwAgAGYAcgBvAG0AIABVAFQAQwAuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAFsALQA5ADAAMAAuAC4AOQAwADAAXQAgAHwAIABBAHMAcwB1AG0AZQBkACAAdABvACAAYgBlACAAVQBUAEMAIABpAGYAIABvAG0AbQBpAHQAdABlAGQALgBcAG4AWwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAgAHwAIABzAHcAaQB0AGMAaAAgACAAIAAgACAAIAB8ACAAQwBhAGwAYwB1AGwAYQB0AGUAIABpAG4AIAB0AGgAZQAgAEoAdQBsAGkAYQBuACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgAgAEQAZQBmAGEAdQBsAHQAIABpAHMAIABHAHIAZQBnAG8AcgBpAGEAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ARQBYAFQARQBOAFQAXwBPAEYAXwBNAE8ATgBUAEgAUwAgAD0AIABMAEEATQBCAEQAQQAoAEoARABhAHQAZQAxACwAIABKAEQAYQB0AGUAMgAsACAAWwBUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQAXQAsACAAWwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAsAFwAbgAgACAAIAAgAEkARgAoACgASgBEAGEAdABlADEAIAA9ACAAXAAiAFwAIgApACAAKgAgACgASgBEAGEAdABlADIAIAA9ACAAXAAiAFwAIgApACwAIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEoARABhAHQAZQAxACkAKQAgACsAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEoARABhAHQAZQAyACkAKQAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBvACwAIABOACgAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABBAEIAUwAoAF8AdAB6AG8AKQAgAD4AIAA5ADAAMAAsACAAewAjAE4AVQBNACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGkAZwBuACwAIABJAEYAKABKAEQAYQB0AGUAMgAgAD4APQAgAEoARABhAHQAZQAxACwAIAAxACwAIAAtADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGoAZABuAEwAbwBjAGEAbABfAFMAdABhAHIAdAAsACAASgBEAEEAVABFAF8AVABPAF8ASgBEAE4AXwBMAE8AQwBBAEwAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAHMAaQBnAG4AIAA9ACAAMQAsACAASgBEAGEAdABlADEALAAgAEoARABhAHQAZQAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBvAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AagBkAG4ATABvAGMAYQBsAF8ARQBuAGQALAAgAEoARABBAFQARQBfAFQATwBfAEoARABOAF8ATABPAEMAQQBMACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBzAGkAZwBuACAAPQAgADEALAAgAEoARABhAHQAZQAyACwAIABKAEQAYQB0AGUAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AHoAbwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAYQB0AGUAXwBTAHQAYQByAHQALAAgAEoARABOAF8AVABPAF8AQwBBAEwARQBOAEQAQQBSAF8ARABBAFQARQAoAEkATgBEAEUAWAAoAF8AagBkAG4ATABvAGMAYQBsAF8AUwB0AGEAcgB0ACwAIAAxACwAIAAxACkALAAgAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHQAZQBfAEUAbgBkACwAIABKAEQATgBfAFQATwBfAEMAQQBMAEUATgBEAEEAUgBfAEQAQQBUAEUAKABJAE4ARABFAFgAKABfAGoAZABuAEwAbwBjAGEAbABfAEUAbgBkACwAIAAxACwAIAAxACkALAAgAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABlAGwAdABhAFkAZQBhAHIALAAgAEkATgBEAEUAWAAoAF8AZABhAHQAZQBfAEUAbgBkACwAIAAxACwAIAAxACkAIAAtACAASQBOAEQARQBYACgAXwBkAGEAdABlAF8AUwB0AGEAcgB0ACwAIAAxACwAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGUAbAB0AGEATQBvAG4AdABoACwAIABJAE4ARABFAFgAKABfAGQAYQB0AGUAXwBFAG4AZAAsACAAMQAsACAAMgApACAALQAgAEkATgBEAEUAWAAoAF8AZABhAHQAZQBfAFMAdABhAHIAdAAsACAAMQAsACAAMgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABpAGYAZgBNAG8AbgB0AGgAcwAsACAAKABfAGQAZQBsAHQAYQBZAGUAYQByACAAKgAgADEAMgApACAAKwAgAF8AZABlAGwAdABhAE0AbwBuAHQAaAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaQBnAG4AIAAqACAAKABfAGQAaQBmAGYATQBvAG4AdABoAHMAIAArACAAMQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ARQBYAFQARQBOAFQAXwBPAEYAXwBRAFUAQQBSAFQARQBSAFMAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIABpAG4AYwBsAHUAcwBpAHYAZQAgAGUAeAB0AGUAbgB0ACAAbwBmACAAcQB1AGEAcgB0AGUAcgBzACAAcwBwAGEAbgBuAGUAZAAgAGIAeQAgAHQAdwBvACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIABFAHgAdABlAG4AdAAgAG8AZgAgAHEAdQBhAHIAdABlAHIAcwBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEoARABhAHQAZQAxACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgACAAIAAgACAAIAAgACAAIAB8AFwAbgBKAEQAYQB0AGUAMgAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAAgACAAIAAgACAAIAAgACAAfABcAG4AWwBUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQAXQAgAHwAIABkAGUAYwBpAG0AYQBsACAAIAAgACAAIAAgACAAIAAgAHwAIABUAGkAbQBlACAAegBvAG4AZQAgAG8AZgBmAHMAZQB0ACAAaQBuACAAbQBpAG4AdQB0AGUAcwAgAGYAcgBvAG0AIABVAFQAQwAuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAFsALQA5ADAAMAAuAC4AOQAwADAAXQAgACAAIAAgACAAfAAgAEEAcwBzAHUAbQBlAGQAIAB0AG8AIABiAGUAIABVAFQAQwAgAGkAZgAgAG8AbQBtAGkAdAB0AGUAZAAuAFwAbgBbAE0AbwBuAHQAaABPAGYAZgBzAGUAdABdACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbAC0ANgAuAC4AMwBdACAAfAAgAFEAdQBhAHIAdABlAHIAIABtAG8AbgB0AGgAIABvAGYAZgBzAGUAdAAgAGYAcgBvAG0AIABKAGEAbgB1AGEAcgB5AC4AXABuAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0AIAB8ACAAcwB3AGkAdABjAGgAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAQwBhAGwAYwB1AGwAYQB0AGUAIABpAG4AIAB0AGgAZQAgAEoAdQBsAGkAYQBuACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgAgAEQAZQBmAGEAdQBsAHQAIABpAHMAIABHAHIAZQBnAG8AcgBpAGEAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBFAFgAVABFAE4AVABfAE8ARgBfAFEAVQBBAFIAVABFAFIAUwAgAD0AIABMAEEATQBCAEQAQQAoAEoARABhAHQAZQAxACwAIABKAEQAYQB0AGUAMgAsACAAWwBUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQAXQAsACAAWwBNAG8AbgB0AGgATwBmAGYAcwBlAHQAXQAsACAAWwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAsAFwAbgAgACAAIAAgAEkARgAoACgASgBEAGEAdABlADEAIAA9ACAAXAAiAFwAIgApACAAKgAgACgASgBEAGEAdABlADIAIAA9ACAAXAAiAFwAIgApACwAIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEoARABhAHQAZQAxACkAKQAgACsAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEoARABhAHQAZQAyACkAKQAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBvACwAIABOACgAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AbwBuAHQAaABPAGYAZgBzAGUAdAAsACAAUgBPAFUATgBEACgATgAoAE0AbwBuAHQAaABPAGYAZgBzAGUAdAApACwAIAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKAAoAEEAQgBTACgAXwB0AHoAbwApACAAPgAgADkAMAAwACkAIAArACAAKABfAG0AbwBuAHQAaABPAGYAZgBzAGUAdAAgADwAIAAtADYAKQAgACsAIAAoAF8AbQBvAG4AdABoAE8AZgBmAHMAZQB0ACAAPgAgADMAKQAsACAAewAjAE4AVQBNACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGkAZwBuACwAIABJAEYAKABKAEQAYQB0AGUAMgAgAD4APQAgAEoARABhAHQAZQAxACwAIAAxACwAIAAtADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGoAZABuAEwAbwBjAGEAbABfAFMAdABhAHIAdAAsACAASgBEAEEAVABFAF8AVABPAF8ASgBEAE4AXwBMAE8AQwBBAEwAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAHMAaQBnAG4AIAA9ACAAMQAsACAASgBEAGEAdABlADEALAAgAEoARABhAHQAZQAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBvAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AagBkAG4ATABvAGMAYQBsAF8ARQBuAGQALAAgAEoARABBAFQARQBfAFQATwBfAEoARABOAF8ATABPAEMAQQBMACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBzAGkAZwBuACAAPQAgADEALAAgAEoARABhAHQAZQAyACwAIABKAEQAYQB0AGUAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AHoAbwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHEAdQBhAHIAdABlAHIARABhAHQAZQBfAFMAdABhAHIAdAAsACAASgBEAE4AXwBUAE8AXwBRAFUAQQBSAFQARQBSAF8ARABBAFQARQAoAEkATgBEAEUAWAAoAF8AagBkAG4ATABvAGMAYQBsAF8AUwB0AGEAcgB0ACwAIAAxACwAIAAxACkALAAgAF8AbQBvAG4AdABoAE8AZgBmAHMAZQB0ACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHEAdQBhAHIAdABlAHIARABhAHQAZQBfAEUAbgBkACwAIABKAEQATgBfAFQATwBfAFEAVQBBAFIAVABFAFIAXwBEAEEAVABFACgASQBOAEQARQBYACgAXwBqAGQAbgBMAG8AYwBhAGwAXwBFAG4AZAAsACAAMQAsACAAMQApACwAIABfAG0AbwBuAHQAaABPAGYAZgBzAGUAdAAsACAASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGUAbAB0AGEAWQBlAGEAcgAsACAASQBOAEQARQBYACgAXwBxAHUAYQByAHQAZQByAEQAYQB0AGUAXwBFAG4AZAAsACAAMQAsACAAMQApACAALQAgAEkATgBEAEUAWAAoAF8AcQB1AGEAcgB0AGUAcgBEAGEAdABlAF8AUwB0AGEAcgB0ACwAIAAxACwAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGUAbAB0AGEAUQB1AGEAcgB0AGUAcgAsACAASQBOAEQARQBYACgAXwBxAHUAYQByAHQAZQByAEQAYQB0AGUAXwBFAG4AZAAsACAAMQAsACAAMgApACAALQAgAEkATgBEAEUAWAAoAF8AcQB1AGEAcgB0AGUAcgBEAGEAdABlAF8AUwB0AGEAcgB0ACwAIAAxACwAIAAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGkAZgBmAFEAdQBhAHIAdABlAHIAcwAsACAAKABfAGQAZQBsAHQAYQBZAGUAYQByACAAKgAgADQAKQAgACsAIABfAGQAZQBsAHQAYQBRAHUAYQByAHQAZQByACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBpAGcAbgAgACoAIAAoAF8AZABpAGYAZgBRAHUAYQByAHQAZQByAHMAIAArACAAMQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ARQBYAFQARQBOAFQAXwBPAEYAXwBZAEUAQQBSAFMAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIABpAG4AYwBsAHUAcwBpAHYAZQAgAGUAeAB0AGUAbgB0ACAAbwBmACAAeQBlAGEAcgBzACAAcwBwAGEAbgBuAGUAZAAgAGIAeQAgAHQAdwBvACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIABFAHgAdABlAG4AdAAgAG8AZgAgAHEAdQBhAHIAdABlAHIAcwBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEoARABhAHQAZQAxACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgACAAIAAgACAAIAAgACAAIAB8AFwAbgBKAEQAYQB0AGUAMgAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAAgACAAIAAgACAAIAAgACAAfABcAG4AWwBUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQAXQAgAHwAIABkAGUAYwBpAG0AYQBsACAAIAAgACAAIAAgACAAIAAgAHwAIABUAGkAbQBlACAAegBvAG4AZQAgAG8AZgBmAHMAZQB0ACAAaQBuACAAbQBpAG4AdQB0AGUAcwAgAGYAcgBvAG0AIABVAFQAQwAuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAFsALQA5ADAAMAAuAC4AOQAwADAAXQAgACAAIAAgACAAfAAgAEEAcwBzAHUAbQBlAGQAIAB0AG8AIABiAGUAIABVAFQAQwAgAGkAZgAgAG8AbQBtAGkAdAB0AGUAZAAuAFwAbgBbAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACAAfAAgAHMAdwBpAHQAYwBoACAAIAAgACAAIAAgACAAIAAgACAAfAAgAEMAYQBsAGMAdQBsAGEAdABlACAAaQBuACAAdABoAGUAIABKAHUAbABpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AIABEAGUAZgBhAHUAbAB0ACAAaQBzACAARwByAGUAZwBvAHIAaQBhAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ARQBYAFQARQBOAFQAXwBPAEYAXwBZAEUAQQBSAFMAIAA9ACAATABBAE0AQgBEAEEAKABKAEQAYQB0AGUAMQAsACAASgBEAGEAdABlADIALAAgAFsAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0AF0ALAAgAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0ALABcAG4AIAAgACAAIABJAEYAKAAoAEoARABhAHQAZQAxACAAPQAgAFwAIgBcACIAKQAgACoAIAAoAEoARABhAHQAZQAyACAAPQAgAFwAIgBcACIAKQAsACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABKAEQAYQB0AGUAMQApACkAIAArACAATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABKAEQAYQB0AGUAMgApACkALAAgAHsAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AHoAbwAsACAATgAoAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAKABBAEIAUwAoAF8AdAB6AG8AKQAgAD4AIAA5ADAAMAApACwAIAB7ACMATgBVAE0AIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaQBnAG4ALAAgAEkARgAoAEoARABhAHQAZQAyACAAPgA9ACAASgBEAGEAdABlADEALAAgADEALAAgAC0AMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AagBkAG4ATABvAGMAYQBsAF8AUwB0AGEAcgB0ACwAIABKAEQAQQBUAEUAXwBUAE8AXwBKAEQATgBfAEwATwBDAEEATAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAF8AcwBpAGcAbgAgAD0AIAAxACwAIABKAEQAYQB0AGUAMQAsACAASgBEAGEAdABlADIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdAB6AG8AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBqAGQAbgBMAG8AYwBhAGwAXwBFAG4AZAAsACAASgBEAEEAVABFAF8AVABPAF8ASgBEAE4AXwBMAE8AQwBBAEwAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAHMAaQBnAG4AIAA9ACAAMQAsACAASgBEAGEAdABlADIALAAgAEoARABhAHQAZQAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBvAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHQAZQBfAFMAdABhAHIAdAAsACAASgBEAE4AXwBUAE8AXwBDAEEATABFAE4ARABBAFIAXwBEAEEAVABFACgASQBOAEQARQBYACgAXwBqAGQAbgBMAG8AYwBhAGwAXwBTAHQAYQByAHQALAAgADEALAAgADEAKQAsACAASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAdABlAF8ARQBuAGQALAAgAEoARABOAF8AVABPAF8AQwBBAEwARQBOAEQAQQBSAF8ARABBAFQARQAoAEkATgBEAEUAWAAoAF8AagBkAG4ATABvAGMAYQBsAF8ARQBuAGQALAAgADEALAAgADEAKQAsACAASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGUAbAB0AGEAWQBlAGEAcgAsACAASQBOAEQARQBYACgAXwBkAGEAdABlAF8ARQBuAGQALAAgADEALAAgADEAKQAgAC0AIABJAE4ARABFAFgAKABfAGQAYQB0AGUAXwBTAHQAYQByAHQALAAgADEALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaQBnAG4AIAAqACAAKABfAGQAZQBsAHQAYQBZAGUAYQByACAAKwAgADEAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAFwAbgBcAG4AXABuAFwAbgBcAG4AXABuAC8AKgAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAXABuACMAIABQAEEAUgBTAEkATgBHACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAqAC8AXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AUABBAFIAUwBFAF8ASQBTAE8AXwBEAEEAVABFAFwAbgBcAG4AUABhAHIAcwBlAHMAIABhAG4AIABJAFMATwAgAGYAbwByAG0AYQB0AHQAZQBkACAAZABhAHQAZQAgAGkAbgB0AG8AIAByAGUAcwBwAGUAYwB0AGkAdgBlACAAcABhAHIAdABzACAAbwBmACAAeQBlAGEAcgAsACAAbQBvAG4AdABoACwAIABkAGEAeQAsACAAdABpAG0AZQAgAG8AZgAgAGQAYQB5ACAAYQBuAGQAIAB0AGkAbQBlACAAegBvAG4AZQAgAG8AZgBmAHMAZQB0AFwAbgBpAG4AIABtAGkAbgB1AHQAZQBzACAAZgByAG8AbQAgAFUAVABDAC4AXABuAFwAbgBPAHUAdABwAHUAdABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAGkAbgB0AGUAZwBlAHIAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAWQBlAGEAcgBcAG4AIAAyACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADEALgAuADEAMgBdACAAIAAgACAAIAB8ACAATQBvAG4AdABoAFwAbgAgADMAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMQAuAC4AMwAxAF0AIAAgACAAIAAgAHwAIABEAGEAeQBcAG4AIAA0ACAAfAAgAGQAZQBjAGkAbQBhAGwAIABbADAALgAuADEAKQAgACAAIAAgACAAIAB8ACAAVABpAG0AZQBcAG4AIAA1ACAAfAAgAGQAZQBjAGkAbQBhAGwAIABbAC0AOQAwADAALgAuADkAMAAwAF0AIAB8ACAAVABpAG0AZQAgAHoAbwBuAGUAIABvAGYAZgBzAGUAdAAgAG0AaQBuAHUAdABlAHMAIABmAHIAbwBtACAAVQBUAEMAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBJAFMATwBEAGEAdABlACAAIAAgACAAIAAgACAAIAAgACAAfAAgAHQAZQB4AHQAIAAgACAAfAAgAEQAYQB0AGUAIABpAG4AIABJAFMATwAgAGYAbwByAG0AYQB0ACAAaQBlAC4AIAB5AHkAeQB5AC0ATQBNAC0AZABkAFQAaABoADoAbQBtADoAcwBzACsAaABoADoAbQBtAFwAbgBbAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACAAfAAgAHMAdwBpAHQAYwBoACAAfAAgAEMAYQBsAGMAdQBsAGEAdABlACAAaQBuACAAdABoAGUAIABKAHUAbABpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AIABEAGUAZgBhAHUAbAB0ACAAaQBzACAARwByAGUAZwBvAHIAaQBhAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAB8ACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgBcAG4AXABuAEUAeABhAG0AcABsAGUAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AUABBAFIAUwBFAF8ASQBTAE8AXwBEAEEAVABFACgAXAAiADIAMAAyADMALQAwADUALQAyADMAXAAiACkAXABuAFIAZQB0AHUAcgBuAHMAOgAgAHsAMgAwADIAMwAsACAANQAsACAAMgAzACwAIABcACIAXAAiACwAIABcACIAXAAiAH0AXABuAFwAbgBQAEEAUgBTAEUAXwBJAFMATwBfAEQAQQBUAEUAKABcACIAMgAwADIAMwAtADAANQAtADIAMwBUADAANgA6ADAAMABcACIAKQBcAG4AUgBlAHQAdQByAG4AcwA6ACAAewAyADAAMgAzACwAIAA1ACwAIAAyADMALAAgADAALgAyADUALAAgAFwAIgBcACIAfQBcAG4AXABuAFAAQQBSAFMARQBfAEkAUwBPAF8ARABBAFQARQAoAFwAIgAyADAAMgAzAC0AMAA1AC0AMgAzAFQAMAA2ADoAMAAwACsAMAA5ADoAMwAwAFwAIgApAFwAbgBSAGUAdAB1AHIAbgBzADoAIAB7ADIAMAAyADMALAAgADUALAAgADIAMwAsACAAMAAuADIANQAsACAANQA3ADAAfQBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4AUABBAFIAUwBFAF8ASQBTAE8AXwBEAEEAVABFACAAPQAgAEwAQQBNAEIARABBACgASQBTAE8ARABhAHQAZQAsACAAWwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAsAFwAbgAgACAAIAAgAEkARgAoAEkAUwBPAEQAYQB0AGUAIAA9ACAAXAAiAFwAIgAsACAAewBcACIAXAAiACwAIABcACIAXAAiACwAIABcACIAXAAiACwAIABcACIAXAAiACwAIABcACIAXAAiAH0ALABcAG4AIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAGYAbgBDAG8AdQBuAHQAQwBoAGEAcgBzACwAIABMAEEATQBCAEQAQQAoAEMAaABhAHIAQQByAHIAYQB5ACwAIABUAGUAeAB0ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAGUAeAB0ACAAPQAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcgBlAG0AbwB2AGUAZAAsACAAUgBFAEQAVQBDAEUAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAGUAeAB0ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAQwBoAGEAcgBBAHIAcgBhAHkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEEATQBCAEQAQQAoAF8AYQBjAGMALAAgAF8AYwB1AHIAcgAsACAAUwBVAEIAUwBUAEkAVABVAFQARQAoAF8AYQBjAGMALAAgAF8AYwB1AHIAcgAsACAAXAAiAFwAIgApACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAE4AKABUAGUAeAB0ACkAIAAtACAATABFAE4AKABfAHIAZQBtAG8AdgBlAGQAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAZgBuAEYAaQBuAGQATgB0AGgAQwBoAGEAcgBQAG8AcwAsACAATABBAE0AQgBEAEEAKABDAGgAYQByAHMALAAgAFQAZQB4AHQALAAgAE4ALAAgAFsAUwB0AGEAcgB0AFAAbwBzAF0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABOACgAUwB0AGEAcgB0AFAAbwBzACkAIAA+ACAATABFAE4AKABUAGUAeAB0ACkALAAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZgByAG8AbQBQAG8AcwAsACAASQBGACgATgAoAFMAdABhAHIAdABQAG8AcwApACAAPAA9ACAAMAAsACAAMAAsACAATgAoAFMAdABhAHIAdABQAG8AcwApACAALQAgADEAKQAsACAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdABlAHgAdAAsACAASQBGACgAXwBmAHIAbwBtAFAAbwBzACAAPQAgADAALAAgAFQAZQB4AHQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABSAEkARwBIAFQAKABUAGUAeAB0ACwAIABMAEUATgAoAFQAZQB4AHQAKQAgAC0AIABfAGYAcgBvAG0AUABvAHMAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGMAaABhAHIAQwBvAHUAbgB0ACwAIABMAEUATgAoAEMAaABhAHIAcwApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbgAsACAASQBOAFQAKABOACgATgApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAKABfAGMAaABhAHIAQwBvAHUAbgB0ACAAPQAgADAAKQAgACsAIAAoAF8AbgAgAD0AIAAwACkALAAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBjAGgAYQByAHMALAAgAE0ASQBEACgAQwBoAGEAcgBzACwAIABTAEUAUQBVAEUATgBDAEUAKAAxACwAIABfAGMAaABhAHIAQwBvAHUAbgB0ACkALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBmAGkAbgBkAEMAbwB1AG4AdAAsACAAZgBuAEMAbwB1AG4AdABDAGgAYQByAHMAKABfAGMAaABhAHIAcwAsACAAXwB0AGUAeAB0ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAF8AZgBpAG4AZABDAG8AdQBuAHQAIAA8ACAAQQBCAFMAKABfAG4AKQAsACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAG4AdABoACAAYwBhAG4AIABjAG8AdQBuAHQAIABmAHIAbwBtACAAZQBuAGQAIABiAGEAYwBrAHcAYQByAGQAcwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG4AdABoACwAIABJAEYAKABfAG4AIAA+ACAAMAAsACAAXwBuACwAIABfAGYAaQBuAGQAQwBvAHUAbgB0ACAAKwAgAF8AbgAgACsAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG4AdABoAFAAbwBzACwAIABSAEUARABVAEMARQAoADAALAAgAFMARQBRAFUARQBOAEMARQAoADEALAAgAF8AbgB0AGgAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABBAE0AQgBEAEEAKABfAGEAYwBjACwAIABfAGMAdQByAHIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBhAGMAYwAgADwAIAAwACwAIAAtADEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBuAGUAeAB0AFAAbwBzAEMAaABhAHIAcwAsACAASQBGAEUAUgBSAE8AUgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABGAEkATgBEACgAXwBjAGgAYQByAHMALAAgAF8AdABlAHgAdAAsACAAXwBhAGMAYwAgACsAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAMABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbgBlAHgAdABQAG8AcwAsACAATQBJAE4AKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAARgBJAEwAVABFAFIAKABfAG4AZQB4AHQAUABvAHMAQwBoAGEAcgBzACwAIABfAG4AZQB4AHQAUABvAHMAQwBoAGEAcgBzACAAPgAgADAALAAgADAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAF8AbgBlAHgAdABQAG8AcwAgAD0AIAAwACwAIAAtADEALAAgAF8AbgBlAHgAdABQAG8AcwApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAG4AdABoAFAAbwBzACAAPgAgADAALAAgAF8AbgB0AGgAUABvAHMAIAArACAAXwBmAHIAbwBtAFAAbwBzACAALAAgADAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAZgBuAEkAbgB2AGEAbABpAGQAQwBoAGEAcgBzACwAIABMAEEATQBCAEQAQQAoAF8AdABlAHgAdAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGMAaABhAHIAUwBlAHQALAAgAFwAIgArACwALQAuADAAMQAyADMANAA1ADYANwA4ADkAOgBUAFcAWgBcACIAIAAmACAAVQBOAEkAQwBIAEEAUgAoADgANwAyADIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBlAHMAYwBhAHAAZQBUAGUAeAB0ACwAIABTAFUAQgBTAFQASQBUAFUAVABFACgAUwBVAEIAUwBUAEkAVABVAFQARQAoAF8AdABlAHgAdAAsACAAXAAiACYAXAAiACwAIABcACIAJgBhAG0AcAA7AFwAIgApACwAIABcACIAPABcACIALAAgAFwAIgAmAGwAdAA7AFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHgAbQBsACwAIABcACIAPAB0AD4APABzAD4AXAAiACAAJgAgAF8AZQBzAGMAYQBwAGUAVABlAHgAdAAgACYAIABcACIAPAAvAHMAPgA8AC8AdAA+AFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB4AHAAYQB0AGgALAAgAFwAIgAvAC8AcwBbAHQAcgBhAG4AcwBsAGEAdABlACgALgAsACcAXAAiACAAJgAgAF8AYwBoAGEAcgBTAGUAdAAgACYAIABcACIAJwAsACcAJwApAD0AJwAnAF0AXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAFMARQBSAFIATwBSACgARgBJAEwAVABFAFIAWABNAEwAKABfAHgAbQBsACwAIABfAHgAcABhAHQAaAApACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAZgBuAFAAYQByAHMAZQBEAGEAdABlACwAIABMAEEATQBCAEQAQQAoAF8AZABhAHQAZQBQAGEAcgB0ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZgBpAHIAcwB0AEMAaABhAHIALAAgAEwARQBGAFQAKABfAGQAYQB0AGUAUABhAHIAdAAsACAAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGkAcwBTAGkAZwBuAGUAZAAsACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBmAGkAcgBzAHQAQwBoAGEAcgAgAD0AIABcACIAKwBcACIALAAgAFQAUgBVAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBmAGkAcgBzAHQAQwBoAGEAcgAgAD0AIABcACIALQBcACIALAAgAFQAUgBVAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBmAGkAcgBzAHQAQwBoAGEAcgAgAD0AIABVAE4ASQBDAEgAQQBSACgAOAA3ADIAMgApACwAIABUAFIAVQBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALAAgAEYAQQBMAFMARQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBpAGcAbgAsACAASQBGACgAXwBpAHMAUwBpAGcAbgBlAGQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGYAaQByAHMAdABDAGgAYQByACAAPQAgAFwAIgAtAFwAIgAsACAALQAxACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBmAGkAcgBzAHQAQwBoAGEAcgAgAD0AIABVAE4ASQBDAEgAQQBSACgAOAA3ADIAMgApACwAIAAtADEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAIAAxAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAIAAxAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB1AG4AUwBpAGcAbgBlAGQALAAgAEkARgAoAF8AaQBzAFMAaQBnAG4AZQBkACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFIASQBHAEgAVAAoAF8AZABhAHQAZQBQAGEAcgB0ACwAIABMAEUATgAoAF8AZABhAHQAZQBQAGEAcgB0ACkAIAAtACAAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHQAZQBQAGEAcgB0AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBwAG8AcwAxACwAIABJAEYARQBSAFIATwBSACgARgBJAE4ARAAoAFwAIgAtAFwAIgAsACAAXwB1AG4AUwBpAGcAbgBlAGQAKQAsACAAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAHAAbwBzADEAIAA8ACAANQAsACAAewAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHAAbwBzADIALAAgAEkARgBFAFIAUgBPAFIAKABGAEkATgBEACgAXAAiAC0AXAAiACwAIABfAHUAbgBTAGkAZwBuAGUAZAAsACAAXwBwAG8AcwAxACAAKwAgADEAKQAsACAAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBwAG8AcwAyACAALQAgAF8AcABvAHMAMQAgADwAPgAgADMALAAgAHsAIwBWAEEATABVAEUAIQAsACAAIwBWAEEATABVAEUAIQAsACAAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIALAAgAF8AcwBpAGcAbgAgACoAIABJAE4AVAAoAFYAQQBMAFUARQAoAEwARQBGAFQAKABfAHUAbgBTAGkAZwBuAGUAZAAsACAAXwBwAG8AcwAxACAALQAgADEAKQApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBtAG8AbgB0AGgALAAgAEkATgBUACgAVgBBAEwAVQBFACgATQBJAEQAKABfAHUAbgBTAGkAZwBuAGUAZAAsACAAXwBwAG8AcwAxACAAKwAgADEALAAgAF8AcABvAHMAMgAtACAAXwBwAG8AcwAxACAALQAgADEAKQApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQAsACAASQBOAFQAKABWAEEATABVAEUAKABSAEkARwBIAFQAKABfAHUAbgBTAGkAZwBuAGUAZAAsACAATABFAE4AKABfAHUAbgBTAGkAZwBuAGUAZAApACAALQAgAF8AcABvAHMAMgApACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABJAFMAXwBWAEEATABJAEQAXwBEAEEAVABFACgAXwB5AGUAYQByACwAIABfAG0AbwBuAHQAaAAsACAAXwBkAGEAeQAsACAASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAF8AeQBlAGEAcgAsACAAXwBtAG8AbgB0AGgALAAgAF8AZABhAHkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHsAIwBWAEEATABVAEUAIQAsACAAIwBWAEEATABVAEUAIQAsACAAIwBWAEEATABVAEUAIQB9AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABmAG4AVABpAG0AZQBEAGUAYwBpAG0AYQBsACwAIABMAEEATQBCAEQAQQAoAF8AaABvAHUAcgAsACAAXwBtAGkAbgB1AHQAZQAsACAAXwBzAGUAYwBvAG4AZAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGkAcwBJAG4AVgBhAGwAaQBkACwAIABJAEYAUwAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGgAbwB1AHIAIAA8ACAAMAAsACAAVABSAFUARQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGgAbwB1AHIAIAA+ACAAMgA0ACwAIABUAFIAVQBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgAXwBoAG8AdQByACAAPQAgADIANAApACAAKgAgACgAKABfAG0AaQBuAHUAdABlACAAPgAgADAAKQAgACsAIAAoAF8AcwBlAGMAbwBuAGQAIAA+ACAAMAApACkALAAgAFQAUgBVAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBtAGkAbgB1AHQAZQAgADwAIAAwACwAIABUAFIAVQBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbQBpAG4AdQB0AGUAIAA+AD0AIAA2ADAALAAgAFQAUgBVAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGUAYwBvAG4AZAAgADwAIAAwACwAIABUAFIAVQBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBlAGMAbwBuAGQAIAA+AD0AIAA2ADAALAAgAFQAUgBVAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABSAFUARQAsACAARgBBAEwAUwBFAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAF8AaQBzAEkAbgB2AGEAbABpAGQALAAgAHsAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgAXwBoAG8AdQByACAALwAgADIANAApACAAKwAgACgAXwBtAGkAbgB1AHQAZQAvACAAMQA0ADQAMAApACAAKwAgACgAXwBzAGUAYwBvAG4AZAAgAC8AIAA4ADYANAAwADAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAZgBuAFAAYQByAHMAZQBUAGkAbQBlACwAIABMAEEATQBCAEQAQQAoAF8AdABpAG0AZQBQAGEAcgB0ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbABlAG4ALAAgAEwARQBOACgAXwB0AGkAbQBlAFAAYQByAHQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBsAGUAbgAgAD0AIAAyACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAGYAbgBUAGkAbQBlAEQAZQBjAGkAbQBhAGwAKABWAEEATABVAEUAKABfAHQAaQBtAGUAUABhAHIAdAApACwAIAAwACwAIAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBsAGUAbgAgAD0AIAA1ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAE0ASQBEACgAXwB0AGkAbQBlAFAAYQByAHQALAAgADMALAAgADEAKQAgADwAPgAgAFwAIgA6AFwAIgAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABmAG4AVABpAG0AZQBEAGUAYwBpAG0AYQBsACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABWAEEATABVAEUAKABMAEUARgBUACgAXwB0AGkAbQBlAFAAYQByAHQALAAgADIAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABWAEEATABVAEUAKABSAEkARwBIAFQAKABfAHQAaQBtAGUAUABhAHIAdAAsACAAMgApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGwAZQBuACAAPQAgADgALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgATQBJAEQAKABfAHQAaQBtAGUAUABhAHIAdAAsACAAMwAsACAAMQApACAAPAA+ACAAXAAiADoAXAAiACwAIAB7ACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAE0ASQBEACgAXwB0AGkAbQBlAFAAYQByAHQALAAgADYALAAgADEAKQAgADwAPgAgAFwAIgA6AFwAIgAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAGYAbgBUAGkAbQBlAEQAZQBjAGkAbQBhAGwAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVgBBAEwAVQBFACgATABFAEYAVAAoAF8AdABpAG0AZQBQAGEAcgB0ACwAIAAyACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABWAEEATABVAEUAKABNAEkARAAoAF8AdABpAG0AZQBQAGEAcgB0ACwAIAA0ACwAIAAyACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABWAEEATABVAEUAKABSAEkARwBIAFQAKABfAHQAaQBtAGUAUABhAHIAdAAsACAAMgApACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKABfAGwAZQBuACAAPgA9ACAAMQAwACkAIAAqACAAKABfAGwAZQBuACAAPAA9ACAAMQAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgATQBJAEQAKABfAHQAaQBtAGUAUABhAHIAdAAsACAAMwAsACAAMQApACAAPAA+ACAAXAAiADoAXAAiACwAIAB7ACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAE0ASQBEACgAXwB0AGkAbQBlAFAAYQByAHQALAAgADYALAAgADEAKQAgADwAPgAgAFwAIgA6AFwAIgAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAE0ASQBEACgAXwB0AGkAbQBlAFAAYQByAHQALAAgADkALAAgADEAKQAgADwAPgAgAFwAIgAuAFwAIgAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGkAbgB0AFMAZQBjACwAIABJAE4AVAAoAFYAQQBMAFUARQAoAE0ASQBEACgAXwB0AGkAbQBlAFAAYQByAHQALAAgADcALAAgADIAKQApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAZQBjAFAAbABhAGMAZQBzACwAIABfAGwAZQBuACAALQAgADkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGYAcgBhAGMAUwBlAGMALAAgAEkATgBUACgAVgBBAEwAVQBFACgAUgBJAEcASABUACgAXwB0AGkAbQBlAFAAYQByAHQALAAgAF8AZABlAGMAUABsAGEAYwBlAHMAKQApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAZQBjAFMAZQBjACwAIABfAGkAbgB0AFMAZQBjACAAKwAgACgAXwBmAHIAYQBjAFMAZQBjACAALwAgACgAMQAwACAAXgAgAF8AZABlAGMAUABsAGEAYwBlAHMAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAZgBuAFQAaQBtAGUARABlAGMAaQBtAGEAbAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVgBBAEwAVQBFACgATABFAEYAVAAoAF8AdABpAG0AZQBQAGEAcgB0ACwAIAAyACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVgBBAEwAVQBFACgATQBJAEQAKABfAHQAaQBtAGUAUABhAHIAdAAsACAANAAsACAAMgApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABlAGMAUwBlAGMAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAIAB7ACMAVgBBAEwAVQBFACEAfQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABmAG4AVABaAG0AaQBuAHUAdABlAHMALAAgAEwAQQBNAEIARABBACgAXwBzAGkAZwBuACwAIABfAGgAbwB1AHIALAAgAF8AbQBpAG4AdQB0AGUALAAgAF8AcwBlAGMAbwBuAGQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBhAGIAcwBNAGkAbgBzACwAIAAoAF8AaABvAHUAcgAgACoAIAA2ADAAKQAgACsAIABfAG0AaQBuAHUAdABlACAAKwAgACgAXwBzAGUAYwBvAG4AZAAgAC8AIAA2ADAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBhAGIAcwBNAGkAbgBzACAAPgAgADkAMAAwACwAIAB7ACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaQBnAG4AIAAqACAAXwBhAGIAcwBNAGkAbgBzAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABmAG4AUABhAHIAcwBlAFQAWgAsACAATABBAE0AQgBEAEEAKABfAFQAWgBwAGEAcgB0ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAVQBQAFAARQBSACgAXwBUAFoAcABhAHIAdAApACAAPQAgAFwAIgBaAFwAIgAsACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBmAGkAcgBzAHQAQwBoAGEAcgAsACAATABFAEYAVAAoAF8AVABaAHAAYQByAHQALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaQBnAG4ALAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBmAGkAcgBzAHQAQwBoAGEAcgAgAD0AIABcACIALQBcACIALAAgAC0AMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZgBpAHIAcwB0AEMAaABhAHIAIAA9ACAAVQBOAEkAQwBIAEEAUgAoADgANwAyADIAKQAsACAALQAxACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABSAFUARQAsACAAMQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGwAZQBuACwAIABMAEUATgAoAF8AVABaAHAAYQByAHQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAUwAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbABlAG4AIAA9ACAAMwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAGYAbgBUAFoAbQBpAG4AdQB0AGUAcwAoAF8AcwBpAGcAbgAsACAAVgBBAEwAVQBFACgAUgBJAEcASABUACgAXwBUAFoAcABhAHIAdAAsACAAMgApACkALAAgADAALAAgADAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbABlAG4AIAA9ACAANgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAE0ASQBEACgAXwBUAFoAcABhAHIAdAAsACAANAAsACAAMQApACAAPAA+ACAAXAAiADoAXAAiACwAIAB7ACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAZgBuAFQAWgBtAGkAbgB1AHQAZQBzACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBpAGcAbgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABWAEEATABVAEUAKABNAEkARAAoAF8AVABaAHAAYQByAHQALAAgADIALAAgADIAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFYAQQBMAFUARQAoAFIASQBHAEgAVAAoAF8AVABaAHAAYQByAHQALAAgADIAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGwAZQBuACAAPQAgADkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABNAEkARAAoAF8AVABaAHAAYQByAHQALAAgADQALAAgADEAKQAgADwAPgAgAFwAIgA6AFwAIgAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAE0ASQBEACgAXwBUAFoAcABhAHIAdAAsACAANwAsACAAMQApACAAPAA+ACAAXAAiADoAXAAiACwAIAB7ACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABmAG4AVABaAG0AaQBuAHUAdABlAHMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaQBnAG4ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABWAEEATABVAEUAKABNAEkARAAoAF8AVABaAHAAYQByAHQALAAgADIALAAgADIAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVgBBAEwAVQBFACgATQBJAEQAKABfAFQAWgBwAGEAcgB0ACwAIAA1ACwAIAAyACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFYAQQBMAFUARQAoAFIASQBHAEgAVAAoAF8AVABaAHAAYQByAHQALAAgADIAKQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABSAFUARQAsACAAewAjAFYAQQBMAFUARQAhAH0AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAGYAbgBJAG4AdgBhAGwAaQBkAEMAaABhAHIAcwAoAEkAUwBPAEQAYQB0AGUAKQAsACAAewAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBUAHAAbwBzACwAIABJAEYARQBSAFIATwBSACgARgBJAE4ARAAoAFwAIgBUAFwAIgAsACAASQBTAE8ARABhAHQAZQApACwAIAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAF8AVABwAG8AcwAgAD0AIAAwACwAIABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABmAG4AUABhAHIAcwBlAEQAYQB0AGUAKABJAFMATwBEAGEAdABlACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiAFwAIgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHQAZQAsACAAZgBuAFAAYQByAHMAZQBEAGEAdABlACgATABFAEYAVAAoAEkAUwBPAEQAYQB0AGUALAAgAF8AVABwAG8AcwAgAC0AIAAxACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AVABaAHAAbwBzACwAIABmAG4ARgBpAG4AZABOAHQAaABDAGgAYQByAFAAbwBzACgAXAAiAFoAKwAtAFwAIgAgACYAIABVAE4ASQBDAEgAQQBSACgAOAA3ADIAMgApACwAIABJAFMATwBEAGEAdABlACwAIAAtADEALAAgAF8AVABwAG8AcwApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBUAFoAcABvAHMAIAA9ACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAZgBuAFAAYQByAHMAZQBEAGEAdABlACgATABFAEYAVAAoAEkAUwBPAEQAYQB0AGUALAAgAF8AVABwAG8AcwAgAC0AIAAxACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABmAG4AUABhAHIAcwBlAFQAaQBtAGUAKABSAEkARwBIAFQAKABJAFMATwBEAGEAdABlACwAIABMAEUATgAoAEkAUwBPAEQAYQB0AGUAKQAgAC0AIABfAFQAcABvAHMAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBcACIAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABmAG4AUABhAHIAcwBlAEQAYQB0AGUAKABMAEUARgBUACgASQBTAE8ARABhAHQAZQAsACAAXwBUAHAAbwBzACAALQAgADEAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAGYAbgBQAGEAcgBzAGUAVABpAG0AZQAoAE0ASQBEACgASQBTAE8ARABhAHQAZQAsACAAXwBUAHAAbwBzACAAKwAgADEALAAgAF8AVABaAFAAbwBzACAALQAgAF8AVABwAG8AcwAgAC0AIAAxACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABmAG4AUABhAHIAcwBlAFQAWgAoAFIASQBHAEgAVAAoAEkAUwBPAEQAYQB0AGUALAAgAEwARQBOACgASQBTAE8ARABhAHQAZQApACAALQAgAF8AVABaAHAAbwBzACAAKwAgADEAKQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AUABBAFIAUwBFAF8AVwBFAEUASwBEAEEAWQBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIABhACAAbgB1AG0AYgBlAHIAIAByAGUAcAByAGUAcwBlAG4AdABpAG4AZwAgAHQAaABlACAAZABhAHkAIABvAGYAIAB0AGgAZQAgAHcAZQBlAGsAIABmAHIAbwBtACAAYQAgAGcAaQB2AGUAbgAgAHQAZQB4AHQAIAB3AGUAZQBrAGQAYQB5ACAAbgBhAG0AZQAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAEQAYQB5ACAAbwBmACAAdwBlAGUAawBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEQAYQB5AE8AZgBXAGUAZQBrACAAIAAgACAAIAAgACAAfAAgAHQAZQB4AHQAIAAgACAAIAB8ACAARABhAHkAIABvAGYAIAB3AGUAZQBrACAAbgBhAG0AZQBcAG4AWwBOAHUAbQBiAGUAcgBTAGMAaABlAG0AZQBdACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIABSAGUAdAB1AHIAbgAgAGQAYQB5ACAAbwBmACAAdwBlAGUAawAgAHUAcwBpAG4AZwAgAG4AdQBtAGIAZQByAGkAbgBnACAAcwBjAGgAZQBtAGUAOgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAMQAgAC0AIAAxAC4ALgA3ACAAUwB1AG4AZABhAHkALgAuAFMAYQB0AHUAcgBkAGEAeQAgACgAZABlAGYAYQB1AGwAdAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAyACAALQAgADEALgAuADcAIABNAG8AbgBkAGEAeQAuAC4AUwB1AG4AZABhAHkAIAAgACAAKABJAFMATwAgADgANgAwADEAIABkAGUAZgBpAG4AaQB0AGkAbwBuACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADMAIAAtACAAMAAuAC4ANgAgAE0AbwBuAGQAYQB5AC4ALgBTAHUAbgBkAGEAeQBcAG4ARQB4AGEAbQBwAGwAZQBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBQAEEAUgBTAEUAXwBXAEUARQBLAEQAQQBZACgAXAAiAFMAYQB0AHUAcgBkAGEAeQBcACIAKQBcAG4AUgBlAHQAdQByAG4AcwA6ACAANwBcAG4AXABuAFAAQQBSAFMARQBfAFcARQBFAEsARABBAFkAKABcACIATQBvAG4AXAAiACwAIAAzACkAXABuAFIAZQB0AHUAcgBuAHMAOgAgADAAXABuAFwAbgBQAEEAUgBTAEUAXwBXAEUARQBLAEQAQQBZACgAXAAiAFQAaAB1AHIAcwBcACIALAAgADEAKQBcAG4AUgBlAHQAdQByAG4AcwA6ACAAIwBWAEEATABVAEUAIQBcAG4AXABuAFAAQQBSAFMARQBfAFcARQBFAEsARABBAFkAKABcACIAVgBlAG4AXAAiACwAIAAyACkAXABuAFIAZQB0AHUAcgBuAHMAOgAgADUAIAAoAGkAZgAgAGwAbwBjAGEAbAAgAGwAYQBuAGcAdQBhAGcAZQAgAGkAcwAgAHMAZQB0ACAAdABvACAASQB0AGEAbABpAGEAbgApAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBQAEEAUgBTAEUAXwBXAEUARQBLAEQAQQBZACAAPQAgAEwAQQBNAEIARABBACgARABhAHkATwBmAFcAZQBlAGsALAAgAFsATgB1AG0AYgBlAHIAUwBjAGgAZQBtAGUAXQAsAFwAbgAgACAAIAAgAEkARgAoAEQAYQB5AE8AZgBXAGUAZQBrACAAPQAgAFwAIgBcACIALAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAGYAbgBNAGEAdABjAGgASQBuAHQARQBuAGcALAAgAEwAQQBNAEIARABBACgARABvAFcALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAG8AdwAsACAASQBGACgATABFAE4AKABEAGEAeQBPAGYAVwBlAGUAawApACAAPQAgADMALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAWABNAEEAVABDAEgAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABEAGEAeQBPAGYAVwBlAGUAawAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAUwB1AG4AXAAiADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIATQBvAG4AXAAiADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAVAB1AGUAXAAiADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAVwBlAGQAXAAiADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAVABoAHUAXAAiADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIARgByAGkAXAAiADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAUwBhAHQAXAAiAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAH0AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAWABNAEEAVABDAEgAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABEAGEAeQBPAGYAVwBlAGUAawAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAUwB1AG4AZABhAHkAXAAiADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIATQBvAG4AZABhAHkAXAAiADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAVAB1AGUAcwBkAGEAeQBcACIAOwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBXAGUAZABuAGUAcwBkAGEAeQBcACIAOwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBUAGgAdQByAHMAZABhAHkAXAAiADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIARgByAGkAZABhAHkAXAAiADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAUwBhAHQAdQByAGQAYQB5AFwAIgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB9AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGAE4AQQAoAF8AZABvAHcALAAgADAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAGYAbgBNAGEAdABjAGgATABvAGMAYQBsAEwAYQBuAGcALAAgAEwAQQBNAEIARABBACgARABvAFcALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQBzACwAIABTAEUAUQBVAEUATgBDAEUAKAA3ACwAIAAxACwAIAAzADYANQAyADcAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAG8AdwAsACAASQBGACgATABFAE4AKABEAGEAeQBPAGYAVwBlAGUAawApACAAPQAgADMALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAWABNAEEAVABDAEgAKABEAGEAeQBPAGYAVwBlAGUAawAsACAAVABFAFgAVAAoAF8AZABhAHkAcwAsACAAXAAiAGQAZABkAFwAIgApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAWABNAEEAVABDAEgAKABEAGEAeQBPAGYAVwBlAGUAawAsACAAVABFAFgAVAAoAF8AZABhAHkAcwAsACAAXAAiAGQAZABkAGQAXAAiACkAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgBOAEEAKABfAGQAbwB3ACwAIAAwACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAcgBhAGQARABvAFcALAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBpAGQAeAAsACAAZgBuAE0AYQB0AGMAaABJAG4AdABFAG4AZwAoAEQAYQB5AE8AZgBXAGUAZQBrACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAGkAZAB4ACAAPgAgADAALAAgAF8AaQBkAHgALAAgAGYAbgBNAGEAdABjAGgATABvAGMAYQBsAEwAYQBuAGcAKABEAGEAeQBPAGYAVwBlAGUAawApACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGMAaABlAG0AZQAsACAASQBOAFQAKABOACgATgB1AG0AYgBlAHIAUwBjAGgAZQBtAGUAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AHIAYQBkAEQAbwBXACAAPQAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAVgBBAEwAVQBFACEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAYwBoAGUAbQBlACAAPAA9ACAAMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AHIAYQBkAEQAbwBXACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGMAaABlAG0AZQAgAD4APQAgADMALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAE0ATwBEACgAXwB0AHIAYQBkAEQAbwBXACAALQAgADIALAAgADcAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAE0ATwBEACgAXwB0AHIAYQBkAEQAbwBXACAALQAgADIALAAgADcAKQAgACsAIAAxAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBQAEEAUgBTAEUAXwBNAE8ATgBUAEgAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAYQAgAG4AdQBtAGIAZQByACAAcgBlAHAAcgBlAHMAZQBuAHQAaQBuAGcAIAB0AGgAZQAgAG0AbwBuAHQAaAAgAG8AZgAgAHkAZQBhAHIAIABmAHIAbwBtACAAYQAgAGcAaQB2AGUAbgAgAHQAZQB4AHQAIABtAG8AbgB0AGgAIABuAGEAbQBlAC4AXABuAFwAbgBPAHUAdABwAHUAdABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADEALgAuADEAMgBdACAAfAAgAE0AbwBuAHQAaABcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAE0AbwBuAHQAaABOAGEAbQBlACAAfAAgAHQAZQB4AHQAIAB8ACAATQBvAG4AdABoACAAbgBhAG0AZQBcAG4AXABuAEUAeABhAG0AcABsAGUAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AUABBAFIAUwBFAF8ATQBPAE4AVABIACgAXAAiAEYAZQBiAFwAIgApAFwAbgBSAGUAdAB1AHIAbgBzADoAIAAyAFwAbgBcAG4AUABBAFIAUwBFAF8ATQBPAE4AVABIACgAXAAiAEoAYQBuAHUAYQByAHkAXAAiACkAXABuAFIAZQB0AHUAcgBuAHMAOgAgADEAXABuAFwAbgBQAEEAUgBTAEUAXwBNAE8ATgBUAEgAKABcACIASgBcACIAKQBcAG4AUgBlAHQAdQByAG4AcwA6ACAAIwBWAEEATABVAEUAIQBcAG4AXABuAFAAQQBSAFMARQBfAE0ATwBOAFQASAAoAFwAIgBNAGEAcgB6AG8AXAAiACkAXABuAFIAZQB0AHUAcgBuAHMAOgAgADMAIAAoAGkAZgAgAGwAbwBjAGEAbAAgAGwAYQBuAGcAdQBhAGcAZQAgAGkAcwAgAHMAZQB0ACAAdABvACAASQB0AGEAbABpAGEAbgApAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBQAEEAUgBTAEUAXwBNAE8ATgBUAEgAIAA9ACAATABBAE0AQgBEAEEAKABNAG8AbgB0AGgATgBhAG0AZQAsAFwAbgAgACAAIAAgAEkARgAoAE0AbwBuAHQAaABOAGEAbQBlACAAPQAgAFwAIgBcACIALAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdAByAHkATQBvAG4AdABoACwAIABNAG8AbgB0AGgATgBhAG0AZQAgACYAIABcACIAIAAyADAAMAAwAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABNAE8ATgBUAEgAKABEAEEAVABFAFYAQQBMAFUARQAoAF8AdAByAHkATQBvAG4AdABoACkAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AUABBAFIAUwBFAF8ATABJAFQARQBSAEEAUgBZAF8AWQBFAEEAUgBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIABhACAAbgB1AG0AYgBlAHIAIAByAGUAcAByAGUAcwBlAG4AdABpAG4AZwAgAHQAaABlACAAeQBlAGEAcgAgAHIAZQBsAGEAdABpAHYAZQAgAHQAbwAgAHQAaABlACAAYwBvAG0AbQBvAG4AIABlAHIAYQAgAGYAcgBvAG0AIABhACAAZwBpAHYAZQBuACAAbABpAHQAZQByAGEAcgB5ACAAeQBlAGEAcgAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAFkAZQBhAHIAQwBFAC4AIABOAG8AdABlACAAdABoAGEAdAAgADEAIABCAEMAIAA9ACAAMAAgAEMARQAsACAAMgAgAEIAQwAgAD0AIAAtADEAIABDAEUAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBMAGkAdABlAHIAYQByAHkAWQBlAGEAcgAgAHwAIAB0AGUAeAB0ACAAfAAgAEwAaQB0AGUAcgBhAHIAeQAgAHkAZQBhAHIAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAFAAQQBSAFMARQBfAEwASQBUAEUAUgBBAFIAWQBfAFkARQBBAFIAIAA9ACAATABBAE0AQgBEAEEAKABMAGkAdABlAHIAYQByAHkAWQBlAGEAcgAsAFwAbgAgACAAIAAgAEkARgAoAEwAaQB0AGUAcgBhAHIAeQBZAGUAYQByACAAPQAgAFwAIgBcACIALAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAGYAbgBZAGUAYQByAFYAYQBsAHUAZQAsACAATABBAE0AQgBEAEEAKABfAHQAZQB4AHQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBjAGgAYQByADEALAAgAEwARQBGAFQAKABfAHQAZQB4AHQALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGkAZwBuACwAIABJAEYAUwAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGMAaABhAHIAMQAgAD0AIABcACIAKwBcACIALAAgADEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBjAGgAYQByADEAIAA9ACAAXAAiAC0AXAAiACwAIAAtADEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVQBOAEkAQwBPAEQARQAoAF8AYwBoAGEAcgAxACkAIAA9ACAAOAA3ADIAMgAsACAALQAxACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALAAgAFwAIgBcACIAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAHMAaQBnAG4AIAA9ACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAE4AVAAoAFYAQQBMAFUARQAoAF8AdABlAHgAdAApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGkAZwBuACAAKgAgAEkATgBUACgAVgBBAEwAVQBFACgAUgBJAEcASABUACgAXwB0AGUAeAB0ACwAIABMAEUATgAoAF8AdABlAHgAdAApACAALQAxACkAKQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGwAaQB0AFkAZQBhAHIALAAgAFMAVQBCAFMAVABJAFQAVQBUAEUAKABTAFUAQgBTAFQASQBUAFUAVABFACgATABpAHQAZQByAGEAcgB5AFkAZQBhAHIALAAgAFwAIgAsAFwAIgAsACAAXAAiAFwAIgApACwAIABcACIAIABcACIALAAgAFwAIgBcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIAQwBFACwAIABJAEYAUwAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFIASQBHAEgAVAAoAF8AbABpAHQAWQBlAGEAcgAsACAAMwApACAAPQAgAFwAIgBCAEMARQBcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBZAGUAYQByACwAIABMAEUARgBUACgAXwBsAGkAdABZAGUAYQByACwAIABMAEUATgAoAF8AbABpAHQAWQBlAGEAcgApACAALQAgADMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAxACAALQAgAGYAbgBZAGUAYQByAFYAYQBsAHUAZQAoAF8AcwBZAGUAYQByACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAUgBJAEcASABUACgAXwBsAGkAdABZAGUAYQByACwAIAAyACkAIAA9ACAAXAAiAEMARQBcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBZAGUAYQByACwAIABMAEUARgBUACgAXwBsAGkAdABZAGUAYQByACwAIABMAEUATgAoAF8AbABpAHQAWQBlAGEAcgApACAALQAgADIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABmAG4AWQBlAGEAcgBWAGEAbAB1AGUAKABfAHMAWQBlAGEAcgApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALAAgAGYAbgBZAGUAYQByAFYAYQBsAHUAZQAoAF8AbABpAHQAWQBlAGEAcgApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYARQBSAFIATwBSACgAXwB5AGUAYQByAEMARQAsACAAewAjAFYAQQBMAFUARQAhAH0AKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AUABBAFIAUwBFAF8ATABJAFQARQBSAEEAUgBZAF8ARABBAFQARQBcAG4AXABuAFAAYQByAHMAZQBzACAAYQAgAGwAaQB0AGUAcgBhAHIAeQAgAGQAYQB0AGUAIABpAG4AdABvACAAcgBlAHMAcABlAGMAdABpAHYAZQAgAHAAYQByAHQAcwAgAG8AZgAgAHkAZQBhAHIALAAgAG0AbwBuAHQAaAAsACAAZABhAHkAIABhAG4AZAAgAHQAaQBtAGUAIABvAGYAIABkAGEAeQAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABpAG4AdABlAGcAZQByACAAIAAgACAAIAAgACAAIAAgAHwAIABZAGUAYQByAFwAbgAgADIAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMQAuAC4AMQAyAF0AIAB8ACAATQBvAG4AdABoAFwAbgAgADMAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMQAuAC4AMwAxAF0AIAB8ACAARABhAHkAXABuACAANAAgAHwAIABkAGUAYwBpAG0AYQBsACAAWwAwAC4ALgAxACkAIAAgAHwAIABUAGkAbQBlAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ATABpAHQAZQByAGEAcgB5AEQAYQB0AGUAIAB8ACAAdABlAHgAdAAgAHwAIABMAGkAdABlAHIAYQByAHkAIABkAGEAdABlACAAYQBuAGQAIAB0AGkAbQBlAFwAbgBcAG4ARQB4AGEAbQBwAGwAZQBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBQAEEAUgBTAEUAXwBMAEkAVABFAFIAQQBSAFkAXwBEAEEAVABFACgAXAAiAEYAZQBiACAAMgA1ACwAIAAyADAAMQA0ACwAIAA2ADoAMAAwAFwAIgApAFwAbgBSAGUAdAB1AHIAbgBzADoAIAB7ADIAMAAxADQALAAgADIALAAgADIANQAsACAAMAAuADIANQB9AFwAbgBcAG4AUABBAFIAUwBFAF8ATABJAFQARQBSAEEAUgBZAF8ARABBAFQARQAoAFwAIgBEAGUAYwAgADMAMQAsACAAMgAwADIAMwAsACAAMgA0ADoAMAAwAFwAIgApAFwAbgBSAGUAdAB1AHIAbgBzADoAIAB7ADIAMAAyADMALAAgADEAMgAsACAAMwAxACwAIAAxAH0AXABuAFwAbgBQAEEAUgBTAEUAXwBMAEkAVABFAFIAQQBSAFkAXwBEAEEAVABFACgAXAAiAEYAZQBiACAAMgA1AFwAIgApAFwAbgBSAGUAdAB1AHIAbgBzADoAIAB7AFwAIgBcACIAIAAsACAAMgAsACAAMgA1ACwAIABcACIAXAAiAH0AXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAFAAQQBSAFMARQBfAEwASQBUAEUAUgBBAFIAWQBfAEQAQQBUAEUAIAA9ACAATABBAE0AQgBEAEEAKABMAGkAdABlAHIAYQByAHkARABhAHQAZQAsAFwAbgAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIABmAG4AUABhAHIAcwBlAEQAYQB0AGUALAAgAEwAQQBNAEIARABBACgAXwBsAGkAdABEAGEAdABlACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAF8AbABpAHQARABhAHQAZQAgAD0AIABcACIAXAAiACwAIAB7AFwAIgBcACIALAAgAFwAIgBcACIALAAgAFwAIgBcACIALAAgAFwAIgBcACIAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHAAYQByAHQAcwAsACAAVABSAEkATQAoAFQARQBYAFQAUwBQAEwASQBUACgAXwBsAGkAdABEAGEAdABlACwAIABcACIALABcACIAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGMAbwBsAHMALAAgAEMATwBMAFUATQBOAFMAKABfAHAAYQByAHQAcwApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAUwAoAF8AYwBvAGwAcwAgAD0AIAAxACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBwAGEAcgB0ADEALAAgAEkATgBEAEUAWAAoAF8AcABhAHIAdABzACwAIAAxACwAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAcABhAGMAZQBQAG8AcwAsACAASQBGAEUAUgBSAE8AUgAoAEYASQBOAEQAKABcACIAIABcACIALAAgAF8AcABhAHIAdAAxACkALAAgADAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAF8AcwBwAGEAYwBlAFAAbwBzACAAPQAgADAALAAgAHsAIwBWAEEATABVAEUAIQAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AbwBuAHQAaAAsACAAUABBAFIAUwBFAF8ATQBPAE4AVABIACgATABFAEYAVAAoAF8AcABhAHIAdAAxACwAIABfAHMAcABhAGMAZQBQAG8AcwAgAC0AIAAxACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHIAZQBtAGEAaQBuACwAIABNAEkARAAoAF8AcABhAHIAdAAxACwAIABfAHMAcABhAGMAZQBQAG8AcwAgACsAIAAxACwAIABMAEUATgAoAF8AcABhAHIAdAAxACkAIAAtACAAXwBzAHAAYQBjAGUAUABvAHMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAZQBuAG8AdABlAGQAWQBlAGEAcgAsACAASQBGAEUAUgBSAE8AUgAoAEYASQBOAEQAKABcACIAQwBcACIALAAgAF8AcgBlAG0AYQBpAG4AKQAsACAAMAApACAAPgAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB2AGEAbAAsACAASQBGACgAXwBkAGUAbgBvAHQAZQBkAFkAZQBhAHIALAAgAFAAQQBSAFMARQBfAEwASQBUAEUAUgBBAFIAWQBfAFkARQBBAFIAKABfAHIAZQBtAGEAaQBuACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAE4AVAAoAFYAQQBMAFUARQAoAF8AcgBlAG0AYQBpAG4AKQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAIABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQAsACAASQBGAFMAKABfAGQAZQBuAG8AdABlAGQAWQBlAGEAcgAsACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdgBhAGwAIAA8AD0AIAAwACwAIAB7ACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdgBhAGwAIAA8AD0AIAAzADEALAAgAF8AdgBhAGwALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAIABcACIAXAAiAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AeQBlAGEAcgAsACAASQBGAFMAKABfAGQAZQBuAG8AdABlAGQAWQBlAGEAcgAsACAAXwB2AGEAbAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdgBhAGwAIAA8AD0AIAAzADEALAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAIABfAHYAYQBsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXwB5AGUAYQByACwAIABfAG0AbwBuAHQAaAAsACAAXwBkAGEAeQAsACAAXAAiAFwAIgApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYwBvAGwAcwAgAD0AIAAyACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBwADEALAAgAEkATgBEAEUAWAAoAF8AcABhAHIAdABzACwAIAAxACwAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAcABhAGMAZQBQAG8AcwAsACAASQBGAEUAUgBSAE8AUgAoAEYASQBOAEQAKABcACIAIABcACIALAAgAF8AcAAxACkALAAgADAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAF8AcwBwAGEAYwBlAFAAbwBzACAAPQAgADAALAAgAHsAIwBWAEEATABVAEUAIQAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AbwBuAHQAaAAsACAAUABBAFIAUwBFAF8ATQBPAE4AVABIACgATABFAEYAVAAoAF8AcAAxACwAIABfAHMAcABhAGMAZQBQAG8AcwAgAC0AIAAxACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAYQB5ACwAIABJAE4AVAAoAFYAQQBMAFUARQAoAE0ASQBEACgAXwBwADEALAAgAF8AcwBwAGEAYwBlAFAAbwBzACAAKwAgADEALAAgAEwARQBOACgAXwBwADEAKQAgAC0AIABfAHMAcABhAGMAZQBQAG8AcwApACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHAAMgAsACAASQBOAEQARQBYACgAXwBwAGEAcgB0AHMALAAgADEALAAgADIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAcgB5AFQAaQBtAGUALAAgAEQAQQBUAEUAVgBBAEwAVQBFACgAXwBwADIAKQAgACsAIABUAEkATQBFAFYAQQBMAFUARQAoAF8AcAAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AGkAbQBlACwAIABJAEYARQBSAFIATwBSACgAXwB0AHIAeQBUAGkAbQBlACwAIABcACIAXAAiACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AGUAYQByACwAIABJAEYAKABJAFMARQBSAFIATwBSACgAXwB0AHIAeQBUAGkAbQBlACkALAAgAFAAQQBSAFMARQBfAEwASQBUAEUAUgBBAFIAWQBfAFkARQBBAFIAKABfAHAAMgApACwAIABcACIAXAAiACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABfAHkAZQBhAHIALAAgAF8AbQBvAG4AdABoACwAIABfAGQAYQB5ACwAIABfAHQAaQBtAGUAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGMAbwBsAHMAIAA9ACAAMwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AeQBlAGEAcgAsACAAUABBAFIAUwBFAF8ATABJAFQARQBSAEEAUgBZAF8AWQBFAEEAUgAoAEkATgBEAEUAWAAoAF8AcABhAHIAdABzACwAIAAxACwAIAAyACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdABpAG0AZQAsACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdABpAG0AZQBQAGEAcgB0ACwAIABJAE4ARABFAFgAKABfAHAAYQByAHQAcwAsACAAMQAsACAAMwApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABEAEEAVABFAFYAQQBMAFUARQAoAF8AdABpAG0AZQBQAGEAcgB0ACkAIAArACAAVABJAE0ARQBWAEEATABVAEUAKABfAHQAaQBtAGUAUABhAHIAdAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHAAMQAsACAASQBOAEQARQBYACgAXwBwAGEAcgB0AHMALAAgADEALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBwAGEAYwBlAFAAbwBzACwAIABJAEYARQBSAFIATwBSACgARgBJAE4ARAAoAFwAIgAgAFwAIgAsACAAXwBwADEAKQAsACAAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBzAHAAYQBjAGUAUABvAHMAIAA9ACAAMAAsACAAewAjAFYAQQBMAFUARQAhACwAIABcACIAXAAiACwAIABcACIAXAAiACwAIABcACIAXAAiAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbQBvAG4AdABoACwAIABQAEEAUgBTAEUAXwBNAE8ATgBUAEgAKABMAEUARgBUACgAXwBwADEALAAgAF8AcwBwAGEAYwBlAFAAbwBzACAALQAgADEAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkALAAgAEkATgBUACgAVgBBAEwAVQBFACgATQBJAEQAKABfAHAAMQAsACAAXwBzAHAAYQBjAGUAUABvAHMAIAArACAAMQAsACAATABFAE4AKABfAHAAMQApACAALQAgAF8AcwBwAGEAYwBlAFAAbwBzACkAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXwB5AGUAYQByACwAIABfAG0AbwBuAHQAaAAsACAAXwBkAGEAeQAsACAAXwB0AGkAbQBlACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABSAFUARQAsACAAewAjAFYAQQBMAFUARQAhACwAIABcACIAXAAiACwAIABcACIAXAAiACwAIABcACIAXAAiAH0AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIABfAHIAZQBzAHUAbAB0ACwAIABSAEUARABVAEMARQAoAFwAIgBcACIALAAgAEwAaQB0AGUAcgBhAHIAeQBEAGEAdABlACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwAQQBNAEIARABBACgAXwBhAGMAYwAsACAAXwBjAHUAcgByAGUAbgB0ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcABhAHIAdABzACwAIABmAG4AUABhAHIAcwBlAEQAYQB0AGUAKABfAGMAdQByAHIAZQBuAHQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVgBTAFQAQQBDAEsAKABfAGEAYwBjACwAIABfAHAAYQByAHQAcwApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIABEAFIATwBQACgAXwByAGUAcwB1AGwAdAAsACAAMQApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFAAQQBSAFMARQBfAFUAUwBfAEQAQQBUAEUAXABuAFwAbgBQAGEAcgBzAGUAcwAgAGEAIABVAFMAIABmAG8AcgBtAGEAdABlAGQAIABkAGEAdABlACAAaQBuAHQAbwAgAHIAZQBzAHAAZQBjAHQAaQB2AGUAIABwAGEAcgB0AHMAIABvAGYAIAB5AGUAYQByACwAIABtAG8AbgB0AGgALAAgAGQAYQB5ACAAYQBuAGQAIAB0AGkAbQBlACAAbwBmACAAZABhAHkALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAaQBuAHQAZQBnAGUAcgAgACAAIAAgACAAIAAgACAAIAB8ACAAWQBlAGEAcgBcAG4AIAAyACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADEALgAuADEAMgBdACAAfAAgAE0AbwBuAHQAaABcAG4AIAAzACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADEALgAuADMAMQBdACAAfAAgAEQAYQB5AFwAbgAgADQAIAB8ACAAZABlAGMAaQBtAGEAbAAgAFsAMAAuAC4AMQApACAAIAB8ACAAVABpAG0AZQBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFUAUwBEAGEAdABlACAAfAAgAHQAZQB4AHQAIAB8ACAARABhAHQAZQAgAGkAbgAgAFUAUwAgAGYAbwByAG0AYQB0ACAAaQBlAC4AIABNAE0ALwBkAGQALwB5AHkAeQB5ACAAaABoADoAbQBtADoAcwBzAFwAbgBcAG4ARQB4AGEAbQBwAGwAZQBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBQAEEAUgBTAEUAXwBVAFMAXwBEAEEAVABFACgAXAAiADEALwAyADUALwAyADAAMQA0ACAANgA6ADAAMABcACIAKQBcAG4AUgBlAHQAdQByAG4AcwA6ACAAewAyADAAMQA0ACwAIAAxACwAIAAyADUALAAgADAALgAyADUAfQBcAG4AXABuAFAAQQBSAFMARQBfAFUAUwBfAEQAQQBUAEUAKABcACIAMQAyAC8AMwAxAC8AMgAwADIAMwAgADIANAA6ADAAMABcACIAKQBcAG4AUgBlAHQAdQByAG4AcwA6ACAAewAyADAAMgAzACwAIAAxADIALAAgADMAMQAsACAAMQB9AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBQAEEAUgBTAEUAXwBVAFMAXwBEAEEAVABFACAAPQAgAEwAQQBNAEIARABBACgAVQBTAEQAYQB0AGUALABcAG4AIAAgACAAIABJAEYAKABVAFMARABhAHQAZQAgAD0AIABcACIAXAAiACwAIAB7AFwAIgBcACIALAAgAFwAIgBcACIALAAgAFwAIgBcACIALAAgAFwAIgBcACIAfQAsAFwAbgAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAZgBuAEkAbgB2AGEAbABpAGQAQwBoAGEAcgBzACwAIABMAEEATQBCAEQAQQAoAF8AdABlAHgAdAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGMAaABhAHIAUwBlAHQALAAgAFwAIgAgACwALQAuAC8AMAAxADIAMwA0ADUANgA3ADgAOQA6AEEATQBQAFQAYQBtAHAAXwBcACIAIAAmACAAVQBOAEkAQwBIAEEAUgAoADgANwAyADIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBlAHMAYwBhAHAAZQBUAGUAeAB0ACwAIABTAFUAQgBTAFQASQBUAFUAVABFACgAUwBVAEIAUwBUAEkAVABVAFQARQAoAF8AdABlAHgAdAAsACAAXAAiACYAXAAiACwAIABcACIAJgBhAG0AcAA7AFwAIgApACwAIABcACIAPABcACIALAAgAFwAIgAmAGwAdAA7AFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHgAbQBsACwAIABcACIAPAB0AD4APABzAD4AXAAiACAAJgAgAF8AZQBzAGMAYQBwAGUAVABlAHgAdAAgACYAIABcACIAPAAvAHMAPgA8AC8AdAA+AFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB4AHAAYQB0AGgALAAgAFwAIgAvAC8AcwBbAHQAcgBhAG4AcwBsAGEAdABlACgALgAsACcAXAAiACAAJgAgAF8AYwBoAGEAcgBTAGUAdAAgACYAIABcACIAJwAsACcAJwApAD0AJwAnAF0AXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAFMARQBSAFIATwBSACgARgBJAEwAVABFAFIAWABNAEwAKABfAHgAbQBsACwAIABfAHgAcABhAHQAaAApACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAZgBuAEMAbwB1AG4AdABDAGgAYQByAHMALAAgAEwAQQBNAEIARABBACgAQwBoAGEAcgBBAHIAcgBhAHkALAAgAFQAZQB4AHQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAZQB4AHQAIAA9ACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwByAGUAbQBvAHYAZQBkACwAIABSAEUARABVAEMARQAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAZQB4AHQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABDAGgAYQByAEEAcgByAGEAeQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwAQQBNAEIARABBACgAXwBhAGMAYwAsACAAXwBjAHUAcgByACwAIABTAFUAQgBTAFQASQBUAFUAVABFACgAXwBhAGMAYwAsACAAXwBjAHUAcgByACwAIABcACIAXAAiACkAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUATgAoAFQAZQB4AHQAKQAgAC0AIABMAEUATgAoAF8AcgBlAG0AbwB2AGUAZAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABmAG4ARgBpAG4AZABOAHQAaABDAGgAYQByAFAAbwBzACwAIABMAEEATQBCAEQAQQAoAEMAaABhAHIAcwAsACAAVABlAHgAdAAsACAATgAsACAAWwBTAHQAYQByAHQAUABvAHMAXQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAE4AKABTAHQAYQByAHQAUABvAHMAKQAgAD4AIABMAEUATgAoAFQAZQB4AHQAKQAsACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBmAHIAbwBtAFAAbwBzACwAIABJAEYAKABOACgAUwB0AGEAcgB0AFAAbwBzACkAIAA8AD0AIAAwACwAIAAwACwAIABOACgAUwB0AGEAcgB0AFAAbwBzACkAIAAtACAAMQApACwAIABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AGUAeAB0ACwAIABJAEYAKABfAGYAcgBvAG0AUABvAHMAIAA9ACAAMAAsACAAVABlAHgAdAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFIASQBHAEgAVAAoAFQAZQB4AHQALAAgAEwARQBOACgAVABlAHgAdAApACAALQAgAF8AZgByAG8AbQBQAG8AcwApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYwBoAGEAcgBDAG8AdQBuAHQALAAgAEwARQBOACgAQwBoAGEAcgBzACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBuACwAIABJAE4AVAAoAE4AKABOACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKAAoAF8AYwBoAGEAcgBDAG8AdQBuAHQAIAA9ACAAMAApACAAKwAgACgAXwBuACAAPQAgADAAKQAsACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGMAaABhAHIAcwAsACAATQBJAEQAKABDAGgAYQByAHMALAAgAFMARQBRAFUARQBOAEMARQAoADEALAAgAF8AYwBoAGEAcgBDAG8AdQBuAHQAKQAsACAAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGYAaQBuAGQAQwBvAHUAbgB0ACwAIABmAG4AQwBvAHUAbgB0AEMAaABhAHIAcwAoAF8AYwBoAGEAcgBzACwAIABfAHQAZQB4AHQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBmAGkAbgBkAEMAbwB1AG4AdAAgADwAIABBAEIAUwAoAF8AbgApACwAIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAbgB0AGgAIABjAGEAbgAgAGMAbwB1AG4AdAAgAGYAcgBvAG0AIABlAG4AZAAgAGIAYQBjAGsAdwBhAHIAZABzAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbgB0AGgALAAgAEkARgAoAF8AbgAgAD4AIAAwACwAIABfAG4ALAAgAF8AZgBpAG4AZABDAG8AdQBuAHQAIAArACAAXwBuACAAKwAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbgB0AGgAUABvAHMALAAgAFIARQBEAFUAQwBFACgAMAAsACAAUwBFAFEAVQBFAE4AQwBFACgAMQAsACAAXwBuAHQAaAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEEATQBCAEQAQQAoAF8AYQBjAGMALAAgAF8AYwB1AHIAcgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAGEAYwBjACAAPAAgADAALAAgAC0AMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG4AZQB4AHQAUABvAHMAQwBoAGEAcgBzACwAIABJAEYARQBSAFIATwBSACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEYASQBOAEQAKABfAGMAaABhAHIAcwAsACAAXwB0AGUAeAB0ACwAIABfAGEAYwBjACAAKwAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAwAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBuAGUAeAB0AFAAbwBzACwAIABNAEkATgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABGAEkATABUAEUAUgAoAF8AbgBlAHgAdABQAG8AcwBDAGgAYQByAHMALAAgAF8AbgBlAHgAdABQAG8AcwBDAGgAYQByAHMAIAA+ACAAMAAsACAAMAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBuAGUAeAB0AFAAbwBzACAAPQAgADAALAAgAC0AMQAsACAAXwBuAGUAeAB0AFAAbwBzACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAF8AbgB0AGgAUABvAHMAIAA+ACAAMAAsACAAXwBuAHQAaABQAG8AcwAgACsAIABfAGYAcgBvAG0AUABvAHMAIAAsACAAMAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABmAG4AWQBlAGEAcgBWAGEAbAB1AGUALAAgAEwAQQBNAEIARABBACgAXwB0AGUAeAB0ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYwBoAGEAcgAxACwAIABMAEUARgBUACgAXwB0AGUAeAB0ACwAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBpAGcAbgAsACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBjAGgAYQByADEAIAA9ACAAXAAiACsAXAAiACwAIAAxACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYwBoAGEAcgAxACAAPQAgAFwAIgAtAFwAIgAsACAALQAxACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFUATgBJAEMATwBEAEUAKABfAGMAaABhAHIAMQApACAAPQAgADgANwAyADIALAAgAC0AMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAIABcACIAXAAiAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBzAGkAZwBuACAAPQAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBOAFQAKABWAEEATABVAEUAKABfAHQAZQB4AHQAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBpAGcAbgAgACoAIABJAE4AVAAoAFYAQQBMAFUARQAoAFIASQBHAEgAVAAoAF8AdABlAHgAdAAsACAATABFAE4AKABfAHQAZQB4AHQAKQAgAC0AMQApACkAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAZgBuAEkAbgB2AGEAbABpAGQAQwBoAGEAcgBzACgAVQBTAEQAYQB0AGUAKQAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBwAG8AcwAxACwAIABmAG4ARgBpAG4AZABOAHQAaABDAGgAYQByAFAAbwBzACgAXAAiACwALgAvAC0AXwBcACIALAAgAFUAUwBEAGEAdABlACwAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcABvAHMAMgAsACAAZgBuAEYAaQBuAGQATgB0AGgAQwBoAGEAcgBQAG8AcwAoAFwAIgAsAC4ALwAtAF8AXAAiACwAIABVAFMARABhAHQAZQAsACAAMgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHAAbwBzADMALAAgAEkARgAoAF8AcABvAHMAMgAgAD0AIAAwACwAIAAwACwAIABmAG4ARgBpAG4AZABOAHQAaABDAGgAYQByAFAAbwBzACgAXAAiACwALgAvAC0AXwBUACAAXAAiACwAIABVAFMARABhAHQAZQAsACAAMQAsACAAXwBwAG8AcwAyACAAKwAgADIAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHAAbwBzADQALAAgAEkARgAoAF8AcABvAHMAMwAgAD0AIAAwACwAIAAwACwAIABmAG4ARgBpAG4AZABOAHQAaABDAGgAYQByAFAAbwBzACgAXAAiADAAMQAyADMANAA1ADYANwA4ADkAXAAiACwAIABVAFMARABhAHQAZQAsACAAMQAsACAATQBBAFgAKABfAHAAbwBzADIALAAgAF8AcABvAHMAMwApACAAKwAgADEAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AbwBuAHQAaAAsACAASQBGACgAXwBwAG8AcwAxACAAPQAgADAALAAgACMAVgBBAEwAVQBFACEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBOAFQAKABWAEEATABVAEUAKABMAEUARgBUACgAVQBTAEQAYQB0AGUALAAgAF8AcABvAHMAMQAgAC0AIAAxACkAKQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQAsACAASQBGACgAXwBwAG8AcwAyACAAPQAgADAALAAgACMAVgBBAEwAVQBFACEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBOAFQAKABWAEEATABVAEUAKABNAEkARAAoAFUAUwBEAGEAdABlACwAIABfAHAAbwBzADEAIAArACAAMQAsACAAXwBwAG8AcwAyACAALQAgAF8AcABvAHMAMQAgAC0AIAAxACkAKQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AGUAYQByACwAIABmAG4AWQBlAGEAcgBWAGEAbAB1AGUAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBwAG8AcwAzACAAPQAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABSAEkARwBIAFQAKABVAFMARABhAHQAZQAsACAATABFAE4AKABVAFMARABhAHQAZQApACAALQAgAF8AcABvAHMAMgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATQBJAEQAKABVAFMARABhAHQAZQAsACAAXwBwAG8AcwAyACAAKwAgADEALAAgAF8AcABvAHMAMwAgAC0AIABfAHAAbwBzADIAIAAtACAAMQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AGkAbQBlACwAIABJAEYAKABfAHAAbwBzADQAIAA9ACAAMAAsACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdABpAG0AZQBQAGEAcgB0ACwAIABSAEkARwBIAFQAKABVAFMARABhAHQAZQAsACAATABFAE4AKABVAFMARABhAHQAZQApACAALQAgAF8AcABvAHMANAAgACsAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABEAEEAVABFAFYAQQBMAFUARQAoAF8AdABpAG0AZQBQAGEAcgB0ACkAIAArACAAVABJAE0ARQBWAEEATABVAEUAKABfAHQAaQBtAGUAUABhAHIAdAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABfAHkAZQBhAHIALAAgAF8AbQBvAG4AdABoACwAIABfAGQAYQB5ACwAIABfAHQAaQBtAGUAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBQAEEAUgBTAEUAXwBNAEkATABfAEQAVABHAFwAbgBcAG4AUABhAHIAcwBlAHMAIABhACAAZABhAHQAZQAtAHQAaQBtAGUAIABnAHIAbwB1AHAAIABpAG4AIAB0AGgAZQAgAGYAbwByAG0AYQB0ACAAdQBzAGUAZAAgAGIAeQAgAFUAUwAgAE0AaQBsAGkAdABhAHIAeQAgAG0AZQBzAHMAYQBnAGUAIAB0AHIAYQBmAGYAaQBjACwAIABpAG4AdABvACAAcgBlAHMAcABlAGMAdABpAHYAZQAgAHAAYQByAHQAcwAgAG8AZgAgAHkAZQBhAHIALABcAG4AbQBvAG4AdABoACwAIABkAGEAeQAsACAAdABpAG0AZQAgAG8AZgAgAGQAYQB5ACAAYQBuAGQAIAB0AGkAbQBlACAAegBvAG4AZQAgAG8AZgBmAHMAZQB0ACAAaQBuACAAbQBpAG4AdQB0AGUAcwAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABpAG4AdABlAGcAZQByACAAWwAxADkANQAxAC4ALgAyADAANQAwAF0AIAB8ACAAWQBlAGEAcgBcAG4AIAAyACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADEALgAuADEAMgBdACAAIAAgACAAIAAgAHwAIABNAG8AbgB0AGgAXABuACAAMwAgAHwAIABpAG4AdABlAGcAZQByACAAWwAxAC4ALgAzADEAXQAgACAAIAAgACAAIAB8ACAARABhAHkAXABuACAANAAgAHwAIABkAGUAYwBpAG0AYQBsACAAWwAwAC4ALgAxACkAIAAgACAAIAAgACAAIAB8ACAAVABpAG0AZQBcAG4AIAA1ACAAfAAgAGQAZQBjAGkAbQBhAGwAIABbAC0AOQAwADAALgAuADkAMAAwAF0AIAAgAHwAIABUAGkAbQBlACAAegBvAG4AZQAgAG8AZgBmAHMAZQB0ACAAbQBpAG4AdQB0AGUAcwBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEQAVABHACAAfAAgAHQAZQB4AHQAIAB8ACAARABhAHQAZQAtAHQAaQBtAGUAIABnAHIAbwB1AHAAIABpAG4AIABVAFMAIABNAGkAbABpAHQAYQByAHkAIABmAG8AcgBtAGEAdAAgAGkAZQAuACAAZABkAEgASABtAG0AcwBzAFoAbQBtAG0AWQBZAFwAbgBcAG4ARQB4AGEAbQBwAGwAZQBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBQAEEAUgBTAEUAXwBNAEkATABfAEQAVABHACgAXAAiADEAMgAgADEANQAgADMAMAAgADQANQAgAEIAIABNAEEAWQAgADIAMwBcACIAKQBcAG4AUgBlAHQAdQByAG4AcwA6ACAAewAyADAAMgAzACwAIAA1ACwAIAAxADIALAAgADAALgA3ADcAMQAxADgAMAA1ADUALAAgADEAMgAwAH0AXABuAFwAbgBQAEEAUgBTAEUAXwBNAEkATABfAEQAVABHACgAXAAiADAANQAwADYANAA1ADEANQBLAEoAVQBOADAAMABcACIAKQBcAG4AUgBlAHQAdQByAG4AcwA6ACAAewAyADAAMAAwACwAIAA2ACwAIAA1ACwAIAAwAC4AMgA4ADEANAAyADMANgAxADEALAAgADYAMAAwAH0AXABuAFwAbgBQAEEAUgBTAEUAXwBNAEkATABfAEQAVABHACgAXAAiADEANQAwADYAMAAwAFoAXAAiACkAXABuAFIAZQB0AHUAcgBuAHMAOgAgAHsAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAMQA1ACwAIAAwAC4AMgA1ACwAIAAwAH0AXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAFAAQQBSAFMARQBfAE0ASQBMAF8ARABUAEcAIAA9ACAATABBAE0AQgBEAEEAKABEAFQARwAsAFwAbgAgACAAIAAgAEkARgAoAEQAVABHACAAPQAgAFwAIgBcACIALAAgAHsAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgB9ACwAXABuACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABmAG4ASQBuAHYAYQBsAGkAZABDAGgAYQByAHMALAAgAEwAQQBNAEIARABBACgAXwB0AGUAeAB0ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYwBoAGEAcgBTAGUAdAAsACAAXAAiADAAMQAyADMANAA1ADYANwA4ADkAQQBCAEMARABFAEYARwBIAEkASgBLAEwATQBOAE8AUABRAFIAUwBUAFUAVgBXAFgAWQBaAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBlAHMAYwBhAHAAZQBUAGUAeAB0ACwAIABTAFUAQgBTAFQASQBUAFUAVABFACgAUwBVAEIAUwBUAEkAVABVAFQARQAoAF8AdABlAHgAdAAsACAAXAAiACYAXAAiACwAIABcACIAJgBhAG0AcAA7AFwAIgApACwAIABcACIAPABcACIALAAgAFwAIgAmAGwAdAA7AFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHgAbQBsACwAIABcACIAPAB0AD4APABzAD4AXAAiACAAJgAgAF8AZQBzAGMAYQBwAGUAVABlAHgAdAAgACYAIABcACIAPAAvAHMAPgA8AC8AdAA+AFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB4AHAAYQB0AGgALAAgAFwAIgAvAC8AcwBbAHQAcgBhAG4AcwBsAGEAdABlACgALgAsACcAXAAiACAAJgAgAF8AYwBoAGEAcgBTAGUAdAAgACYAIABcACIAJwAsACcAJwApAD0AJwAnAF0AXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAFMARQBSAFIATwBSACgARgBJAEwAVABFAFIAWABNAEwAKABfAHgAbQBsACwAIABfAHgAcABhAHQAaAApACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAZgBuAFkAZQBhAHIALAAgAEwAQQBNAEIARABBACgAXwBzAFkAZQBhAHIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AHkALAAgAFYAQQBMAFUARQAoAF8AcwBZAGUAYQByACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAF8AeQB5ACAAPAAgADUAMQAsACAAMgAwADAAMAAgACsAIABfAHkAeQAsACAAMQA5ADAAMAAgACsAIABfAHkAeQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAGYAbgBUAGkAbQBlACwAIABMAEEATQBCAEQAQQAoAF8AaABvAHUAcgAsACAAXwBtAGkAbgB1AHQAZQAsACAAXwBzAGUAYwBvAG4AZAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAF8AVgBBAEwASQBEAF8AVABJAE0ARQAoAF8AaABvAHUAcgAsACAAXwBtAGkAbgB1AHQAZQAsACAAXwBzAGUAYwBvAG4AZAApACkALAAgAHsAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoAE4AKABfAGgAbwB1AHIAKQAgAC8AIAAyADQAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACsAIAAoAE4AKABfAG0AaQBuAHUAdABlACkAIAAvACAAMQA0ADQAMAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKwAgACgATgAoAF8AcwBlAGMAbwBuAGQAKQAgAC8AIAA4ADYANAAwADAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABmAG4AUABhAHIAcwBlAFQAWgAsACAATABBAE0AQgBEAEEAKABfAHQAegBDAGgAYQByACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYwBvAGQAZQAsACAAQwBPAEQARQAoAF8AdAB6AEMAaABhAHIAKQAgAC0AIAA2ADQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYwBvAGQAZQAgAD0AIAAyADYALAAgADAALAAgAC8ALwAgAFoAIAA9ACAAVQBUAEMAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYwBvAGQAZQAgAD0AIAAxADAALAAgAFwAIgBcACIALAAgAC8ALwAgAEoAIAA9ACAATABvAGMAYQBsACAAVABpAG0AZQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBjAG8AZABlACAAPAA9ACAAMAAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBjAG8AZABlACAAPAA9ACAAOQAsACAAXwBjAG8AZABlACAAKgAgADYAMAAsACAALwAvACAAQQBCAEMARABFAEYARwBIAEkAIAAtAD4AIAArADEALgAuACsAOQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBjAG8AZABlACAAPAA9ACAAMQAzACwAIAAoAF8AYwBvAGQAZQAgAC0AIAAxACkAIAAqACAANgAwACwAIAAgAC8ALwAgAEsATABNACAALQA+ACAAKwAxADAALgAuACsAMQAyAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGMAbwBkAGUAIAA8AD0AIAAyADUALAAgACgAMQAzACAALQAgAF8AYwBvAGQAZQApACAAKgAgADYAMAAsACAALwAvACAATgBPAFAAUQBSAFMAVABVAFYAVwBYAFkAIAAtAD4AIAAtADEALgAuAC0AMQAyAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAIAB7ACMAVgBBAEwAVQBFACEAfQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAZgBuAFAAYQByAHMAZQBGAHUAbABsACwAIABMAEEATQBCAEQAQQAoAF8ARABUAEcALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQAsACAAVgBBAEwAVQBFACgATABFAEYAVAAoAF8ARABUAEcALAAgADIAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AbwBuAHQAaAAsACAAUABBAFIAUwBFAF8ATQBPAE4AVABIACgATQBJAEQAKABfAEQAVABHACwAIAAxADAALAAgADMAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIALAAgAGYAbgBZAGUAYQByACgAUgBJAEcASABUACgAXwBEAFQARwAsACAAMgApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAF8AVgBBAEwASQBEAF8ARABBAFQARQAoAF8AeQBlAGEAcgAsACAAXwBtAG8AbgB0AGgALAAgAF8AZABhAHkALAAgADAAKQApACwAIAB7ACMAVgBBAEwAVQBFACEALAAgACMAVgBBAEwAVQBFACEALAAgACMAVgBBAEwAVQBFACEALAAgACMAVgBBAEwAVQBFACEALAAgACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AaABvAHUAcgAsACAAVgBBAEwAVQBFACgATQBJAEQAKABfAEQAVABHACwAIAAzACwAIAAyACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbQBpAG4AdQB0AGUALAAgAFYAQQBMAFUARQAoAE0ASQBEACgAXwBEAFQARwAsACAANQAsACAAMgApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAZQBjAG8AbgBkACwAIABWAEEATABVAEUAKABNAEkARAAoAF8ARABUAEcALAAgADcALAAgADIAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AGkAbQBlACwAIABmAG4AVABpAG0AZQAoAF8AaABvAHUAcgAsACAAXwBtAGkAbgB1AHQAZQAsACAAXwBzAGUAYwBvAG4AZAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AHoALAAgAGYAbgBQAGEAcgBzAGUAVABaACgATQBJAEQAKABfAEQAVABHACwAIAA5ACwAIAAxACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAF8AVgBBAEwASQBEAF8AVABJAE0ARQAoAF8AaABvAHUAcgAsACAAXwBtAGkAbgB1AHQAZQAsACAAXwBzAGUAYwBvAG4AZAApACkALAAgAHsAIwBWAEEATABVAEUAIQAsACAAIwBWAEEATABVAEUAIQAsACAAIwBWAEEATABVAEUAIQAsACAAIwBWAEEATABVAEUAIQAsACAAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBtAG8AbgB0AGgALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAaQBtAGUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AHoAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAGYAbgBQAGEAcgBzAGUAUwBoAG8AcgB0ACwAIABMAEEATQBCAEQAQQAoAF8ARABUAEcALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQAsACAAVgBBAEwAVQBFACgATABFAEYAVAAoAF8ARABUAEcALAAgADIAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AbwBuAHQAaAAsACAAUABBAFIAUwBFAF8ATQBPAE4AVABIACgATQBJAEQAKABfAEQAVABHACwAIAA4ACwAIAAzACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AGUAYQByACwAIABmAG4AWQBlAGEAcgAoAFIASQBHAEgAVAAoAF8ARABUAEcALAAgADIAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBfAFYAQQBMAEkARABfAEQAQQBUAEUAKABfAHkAZQBhAHIALAAgAF8AbQBvAG4AdABoACwAIABfAGQAYQB5ACwAIAAwACkAKQAsACAAewAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGgAbwB1AHIALAAgAFYAQQBMAFUARQAoAE0ASQBEACgAXwBEAFQARwAsACAAMwAsACAAMgApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AaQBuAHUAdABlACwAIABWAEEATABVAEUAKABNAEkARAAoAF8ARABUAEcALAAgADUALAAgADIAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AHoALAAgAGYAbgBQAGEAcgBzAGUAVABaACgATQBJAEQAKABfAEQAVABHACwAIAA3ACwAIAAxACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAF8AVgBBAEwASQBEAF8AVABJAE0ARQAoAF8AaABvAHUAcgAsACAAXwBtAGkAbgB1AHQAZQAsACAAXAAiAFwAIgApACkALAAgAHsAIwBWAEEATABVAEUAIQAsACAAIwBWAEEATABVAEUAIQAsACAAIwBWAEEATABVAEUAIQAsACAAIwBWAEEATABVAEUAIQAsACAAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBtAG8AbgB0AGgALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAEkATQBFACgAXwBoAG8AdQByACwAIABfAG0AaQBuAHUAdABlACwAIAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AHoAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAGYAbgBQAGEAcgBzAGUAUABsAGEAbgAsACAATABBAE0AQgBEAEEAKABfAEQAVABHACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkALAAgAFYAQQBMAFUARQAoAEwARQBGAFQAKABfAEQAVABHACwAIAAyACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBoAG8AdQByACwAIABWAEEATABVAEUAKABNAEkARAAoAF8ARABUAEcALAAgADMALAAgADIAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AaQBuAHUAdABlACwAIABWAEEATABVAEUAKABNAEkARAAoAF8ARABUAEcALAAgADUALAAgADIAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegAsACAAZgBuAFAAYQByAHMAZQBUAFoAKABNAEkARAAoAF8ARABUAEcALAAgADcALAAgADEAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBfAFYAQQBMAEkARABfAFQASQBNAEUAKABfAGgAbwB1AHIALAAgAF8AbQBpAG4AdQB0AGUALAAgAFwAIgBcACIAKQApACwAIAB7ACMAVgBBAEwAVQBFACEALAAgACMAVgBBAEwAVQBFACEALAAgACMAVgBBAEwAVQBFACEALAAgACMAVgBBAEwAVQBFACEALAAgACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQASQBNAEUAKABfAGgAbwB1AHIALAAgAF8AbQBpAG4AdQB0AGUALAAgADAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdAB6AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAEQAVABHACwAIABTAFUAQgBTAFQASQBUAFUAVABFACgARABUAEcALAAgAFwAIgAgAFwAIgAsACAAXAAiAFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAGYAbgBJAG4AdgBhAGwAaQBkAEMAaABhAHIAcwAoAF8ARABUAEcAKQAsACAAewAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBsAGUAbgAsACAATABFAE4AKABfAEQAVABHACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZgBtAHQALAAgAEkARgBTACgAXwBsAGUAbgAgAD0AIAAxADQALAAgADEALAAgAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGwAZQBuACAAPQAgADEAMgAsACAAMgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGwAZQBuACAAPQAgADcALAAgADMALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABSAFUARQAsACAAMABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAF8AZgBtAHQAIAA9ACAAMAAsACAAewAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGYAbQB0ACAAPQAgADEALAAgAGYAbgBQAGEAcgBzAGUARgB1AGwAbAAoAF8ARABUAEcAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZgBtAHQAIAA9ACAAMgAsACAAZgBuAFAAYQByAHMAZQBTAGgAbwByAHQAKABfAEQAVABHACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGYAbQB0ACAAPQAgADMALAAgAGYAbgBQAGEAcgBzAGUAUABsAGEAbgAoAF8ARABUAEcAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAFwAbgBcAG4AXABuAFwAbgBcAG4AXABuAFwAbgBcAG4AXABuAFwAbgBcAG4ALwAqACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwBcAG4AIwAgAFQARQBYAFQAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACoALwBcAG4AXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBXAEUARQBLAEQAQQBZAF8ATgBBAE0ARQBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIABuAGEAbQBlACAAbwBmACAAYQBuACAASQBTAE8AIABkAGEAeQAgAG8AZgAgAHcAZQBlAGsAIABuAHUAbQBiAGUAcgAgAGEAcwAgAHQAZQB4AHQALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAdABlAHgAdAAgAHwAIABXAGUAZQBrAGQAYQB5AFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ASQBTAE8AVwBlAGUAawBEAGEAeQAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAWwAxAC4ALgA3AF0AIAB8ACAASQBTAE8AIABkAGEAeQAgAG8AZgAgAHcAZQBlAGsAIABuAHUAbQBiAGUAcgBcAG4AWwBTAGgAbwByAHQAXQAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABzAHcAaQB0AGMAaAAgACAAIAAgACAAIAAgACAAIAB8ACAAUgBlAHQAdQByAG4AIABzAGgAbwByAHQAIABmAG8AcgBtAGEAdAAgAE0AbwBuAC4ALgBTAHUAbgBcAG4AWwBJAG4AdABlAHIAbgBhAHQAaQBvAG4AYQBsAEUAbgBnAGwAaQBzAGgAXQAgAHwAIABzAHcAaQB0AGMAaAAgACAAIAAgACAAIAAgACAAIAB8ACAASQBuAHQAZQByAG4AYQB0AGkAbwBuAGEAbAAgAEUAbgBnAGwAaQBzAGgAIABpAG4AcwB0AGUAYQBkACAAbwBmACAAbABvAGMAYQBsACAAbABhAG4AZwB1AGEAZwBlACAAcwBlAHQAIABpAG4AIABFAHgAYwBlAGwAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAFcARQBFAEsARABBAFkAXwBOAEEATQBFACAAPQAgAEwAQQBNAEIARABBACgASQBTAE8AVwBlAGUAawBEAGEAeQAsACAAWwBTAGgAbwByAHQAXQAsACAAWwBJAG4AdABlAHIAbgBhAHQAaQBvAG4AYQBsAEUAbgBnAGwAaQBzAGgAXQAsAFwAbgAgACAAIAAgAEkARgAoAEkAUwBPAFcAZQBlAGsARABhAHkAIAA9ACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABJAFMATwBXAGUAZQBrAEQAYQB5ACkAKQAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHUAcwBlAFMAaABvAHIAdAAsACAATgAoAFMAaABvAHIAdAApACAAPAA+ACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdQBzAGUATABvAGMAYQBsAEwAYQBuAGcALAAgAE4AKABJAG4AdABlAHIAbgBhAHQAaQBvAG4AYQBsAEUAbgBnAGwAaQBzAGgAKQAgAD0AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBpAHMAbwBEAG8AVwAsACAATQBPAEQAKABJAE4AVAAoAEkAUwBPAFcAZQBlAGsARABhAHkAKQAgAC0AIAAxACwAIAA3ACkAIAArACAAMQAsACAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwB1AHMAZQBMAG8AYwBhAGwATABhAG4AZwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5ADIAawByAGUAZgBEAGEAeQAsACAAMwA2ADUAMgA3ACAAKwAgAF8AaQBzAG8ARABvAFcALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBmAG0AdAAsACAASQBGACgAXwB1AHMAZQBTAGgAbwByAHQALAAgAFwAIgBkAGQAZABcACIALAAgAFwAIgBkAGQAZABkAFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQARQBYAFQAKABfAHkAMgBrAHIAZQBmAEQAYQB5ACwAIABfAGYAbQB0ACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB1AHMAZQBTAGgAbwByAHQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAQwBIAE8ATwBTAEUAKABfAGkAcwBvAEQAbwBXACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiAE0AbwBuAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBUAHUAZQBcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAVwBlAGQAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiAFQAaAB1AFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBGAHIAaQBcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAUwBhAHQAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiAFMAdQBuAFwAIgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABDAEgATwBPAFMARQAoAF8AaQBzAG8ARABvAFcALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIATQBvAG4AZABhAHkAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiAFQAdQBlAHMAZABhAHkAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiAFcAZQBkAG4AZQBzAGQAYQB5AFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBUAGgAdQByAHMAZABhAHkAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiAEYAcgBpAGQAYQB5AFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBTAGEAdAB1AHIAZABhAHkAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiAFMAdQBuAGQAYQB5AFwAIgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAE0ATwBOAFQASABfAE4AQQBNAEUAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAYQAgAG0AbwBuAHQAaAAgAGEAcwAgAHQAZQB4AHQALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAdABlAHgAdAAgAHwAIABNAG8AbgB0AGgAIABuAGEAbQBlAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ATQBvAG4AdABoACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAWwAxAC4ALgAxADIAXQAgAHwAIABNAG8AbgB0AGgAXABuAFsAUwBoAG8AcgB0AF0AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAcwB3AGkAdABjAGgAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAUgBlAHQAdQByAG4AIABzAGgAbwByAHQAIABmAG8AcgBtAGEAdAAgAEoAYQBuAC4ALgBEAGUAYwBcAG4AWwBJAG4AdABlAHIAbgBhAHQAaQBvAG4AYQBsAEUAbgBnAGwAaQBzAGgAXQAgAHwAIABzAHcAaQB0AGMAaAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABJAG4AdABlAHIAbgBhAHQAaQBvAG4AYQBsACAARQBuAGcAbABpAHMAaAAgAGkAbgBzAHQAZQBhAGQAIABvAGYAIABsAG8AYwBhAGwAIABsAGEAbgBnAHUAYQBnAGUAIABzAGUAdAAgAGkAbgAgAEUAeABjAGUAbABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ATQBPAE4AVABIAF8ATgBBAE0ARQAgAD0AIABMAEEATQBCAEQAQQAoAE0AbwBuAHQAaAAsACAAWwBTAGgAbwByAHQAXQAsACAAWwBJAG4AdABlAHIAbgBhAHQAaQBvAG4AYQBsAEUAbgBnAGwAaQBzAGgAXQAsAFwAbgAgACAAIAAgAEkARgAoAE0AbwBuAHQAaAAgAD0AIABcACIAXAAiACwAIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAE0AbwBuAHQAaAApACkALAAgACMAVgBBAEwAVQBFACEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHUAcwBlAFMAaABvAHIAdAAsACAATgAoAFMAaABvAHIAdAApACAAPAA+ACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdQBzAGUATABvAGMAYQBsAEwAYQBuAGcALAAgAE4AKABJAG4AdABlAHIAbgBhAHQAaQBvAG4AYQBsAEUAbgBnAGwAaQBzAGgAKQAgAD0AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBtAG8AbgB0AGgALAAgAEkATgBUACgATQBvAG4AdABoACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAHUAcwBlAEwAbwBjAGEAbABMAGEAbgBnACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAYQB5AE8AZgBNAG8AbgB0AGgALAAgAEQAQQBUAEUAKAAyADAAMAAwACwAIABfAG0AbwBuAHQAaAAsACAAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZgBtAHQALAAgAEkARgAoAF8AdQBzAGUAUwBoAG8AcgB0ACwAIABcACIATQBNAE0AXAAiACwAIABcACIATQBNAE0ATQBcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAEUAWABUACgAXwBkAGEAeQBPAGYATQBvAG4AdABoACwAIABfAGYAbQB0ACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB1AHMAZQBTAGgAbwByAHQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBOAEQARQBYACgAewBcACIASgBhAG4AXAAiADsAIABcACIARgBlAGIAXAAiADsAIABcACIATQBhAHIAXAAiADsAIABcACIAQQBwAHIAXAAiADsAIABcACIATQBhAHkAXAAiADsAIABcACIASgB1AG4AXAAiADsAIABcACIASgB1AGwAXAAiADsAIABcACIAQQB1AGcAXAAiADsAIABcACIAUwBlAHAAXAAiADsAIABcACIATwBjAHQAXAAiADsAIABcACIATgBvAHYAXAAiADsAIABcACIARABlAGMAXAAiAH0ALAAgAF8AbQBvAG4AdABoACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBOAEQARQBYACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAewBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBKAGEAbgB1AGEAcgB5AFwAIgA7AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiAEYAZQBiAHIAdQBhAHIAeQBcACIAOwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBNAGEAcgBjAGgAXAAiADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAQQBwAHIAaQBsAFwAIgA7AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiAE0AYQB5AFwAIgA7AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiAEoAdQBuAGUAXAAiADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIASgB1AGwAeQBcACIAOwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBBAHUAZwB1AHMAdABcACIAOwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBTAGUAcAB0AGUAbQBiAGUAcgBcACIAOwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBPAGMAdABvAGIAZQByAFwAIgA7AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiAE4AbwB2AGUAbQBiAGUAcgBcACIAOwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBEAGUAYwBlAG0AYgBlAHIAXAAiAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AbwBuAHQAaABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEYATwBSAE0AQQBUAF8ASQBTAE8AXwBEAEEAVABFAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAGEAIABkAGEAdABlACAAYQBzACAAdABlAHgAdAAgAGkAbgAgAEkAUwBPACAAZgBvAHIAbQBhAHQALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAdABlAHgAdAAgAHwAIABJAFMATwAgAGYAbwByAG0AYQB0AHQAZQBkACAAZABhAHQAZQBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFkAZQBhAHIAQwBFACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgACAAIAAgACAAIAAgACAAIAB8ACAATgBvAHQAZQAgAHQAaABhAHQAIAAxACAAQgBDACAAPQAgADAAIABDAEUALAAgADIAIABCAEMAIAA9ACAALQAxACAAQwBFAFwAbgBNAG8AbgB0AGgAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADEALgAuADEAMgBdACAAfABcAG4ARABhAHkAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAWwAxAC4ALgAzADEAXQAgAHwAXABuAFsAVABpAG0AZQBdACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgAFsAMAAuAC4AMQApACAAIAB8ACAAVABpAG0AZQAgAG8AZgAgAGQAYQB5ACAAYQBzACAAZABlAGMAaQBtAGEAbAAgAGYAcgBhAGMAdABpAG8AbgAgAG8AZgAgAGEAIABkAGEAeQAuAFwAbgBbAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdABdACAAfAAgAGQAZQBjAGkAbQBhAGwAIAAgACAAIAAgACAAIAAgACAAfAAgAFQAaQBtAGUAIAB6AG8AbgBlACAAbwBmAGYAcwBlAHQAIABpAG4AIABtAGkAbgB1AHQAZQBzACAAZgByAG8AbQAgAFUAVABDAC4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAWwAtADkAMAAwAC4ALgA5ADAAMABdACAAIAAgACAAIAB8ACAAQQBzAHMAdQBtAGUAZAAgAHQAbwAgAGIAZQAgAFUAVABDACAAaQBmACAAbwBtAG0AaQB0AHQAZQBkAC4AXABuAFsAUAByAGUAYwBpAHMAaQBvAG4AXQAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgACAAIAAgACAAIAAgACAAIAB8ACAAUwBlAGwAZQBjAHQAIABwAHIAZQBjAGkAcwBpAG8AbgAgAGwAZQB2AGUAbAAsACAAZABlAGYAYQB1AGwAdAAgAGkAcwAgADMAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADAAIAAtACAARgBsAG8AYQB0AHMAIABmAHIAbwBtACAAbQBpAG4AdQB0AGUAIAB0AG8AIABtAGkAbABsAGkAcwBlAGMAbwBuAGQAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADEAIAAtACAARABhAHkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADIAIAAtACAASABvAHUAcgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAMwAgAC0AIABNAGkAbgB1AHQAZQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAANAAgAC0AIABTAGUAYwBvAG4AZABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAANQAgAC0AIABNAGkAbABsAGkAcwBlAGMAbwBuAGQAXABuAFsATgBvAFoAdQBsAHUAXQAgACAAIAAgACAAIAAgACAAIAB8ACAAcwB3AGkAdABjAGgAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAVQBzAGUAIAArADAAMAA6ADAAMAAgAGkAbgBzAHQAZQBhAGQAIABvAGYAIABaACAAZgBvAHIAIABVAFQAQwAgAHQAaQBtAGUAIAB6AG8AbgBlAC4AXABuAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0AIAB8ACAAcwB3AGkAdABjAGgAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAQwBhAGwAYwB1AGwAYQB0AGUAIABmAG8AcgAgAHQAaABlACAASgB1AGwAaQBhAG4AIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuACAARABlAGYAYQB1AGwAdAAgAGkAcwAgAEcAcgBlAGcAbwByAGkAYQBuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AIABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ARgBPAFIATQBBAFQAXwBJAFMATwBfAEQAQQBUAEUAIAA9ACAATABBAE0AQgBEAEEAKABZAGUAYQByAEMARQAsACAATQBvAG4AdABoACwAIABEAGEAeQAsACAAWwBUAGkAbQBlAF0ALAAgAFsAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0AF0ALAAgAFsAUAByAGUAYwBpAHMAaQBvAG4AXQAsACAAWwBOAG8AWgB1AGwAdQBdACwAIABbAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACwAXABuACAAIAAgACAASQBGACgAKABZAGUAYQByAEMARQAgAD0AIABcACIAXAAiACkAIAAqACAAKABNAG8AbgB0AGgAIAA9ACAAXAAiAFwAIgApACAAKgAgACgARABhAHkAIAA9ACAAXAAiAFwAIgApACwAIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAFkAZQBhAHIAQwBFACkAKQAgACsAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAE0AbwBuAHQAaAApACkAIAArACAATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABEAGEAeQApACkALAAgAHsAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAF8AVgBBAEwASQBEAF8ARABBAFQARQAoAFkAZQBhAHIAQwBFACwAIABNAG8AbgB0AGgALAAgAEQAYQB5ACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQApACwAIAB7ACMAVgBBAEwAVQBFACEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABmAG4ARgBvAHIAbQBhAHQAWQBlAGEAcgAsACAATABBAE0AQgBEAEEAKABfAHkAZQBhAHIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIARgBtAHQALAAgAEkARgAoACgAXwB5AGUAYQByACAAPgA9ACAAMQAwADAAMAApACAAKgAgACgAXwB5AGUAYQByACAAPAA9ACAAOQA5ADkAOQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAMAAwADAAMAA7AFwAIgAgACYAIABVAE4ASQBDAEgAQQBSACgAOAA3ADIAMgApACAAJgAgAFwAIgAwADAAMAAwAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiACsAMAAwADAAMAA7AFwAIgAgACYAIABVAE4ASQBDAEgAQQBSACgAOAA3ADIAMgApACAAJgAgAFwAIgAwADAAMAAwADsAKwAwADAAMAAwAFwAIgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABFAFgAVAAoAF8AeQBlAGEAcgAsACAAXwB5AGUAYQByAEYAbQB0ACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAZgBuAEYAbwByAG0AYQB0AFQAaQBtAGUALAAgAEwAQQBNAEIARABBACgAXwB0AGkAbQBlACwAIABfAHAAcgBlAGMAaQBzAGkAbwBuACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAF8AcAByAGUAYwBpAHMAaQBvAG4AIAA9ACAAMQAsACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaABvAHcAUAByAGUAYwBpAHMAaQBvAG4ALAAgAEkARgAoAF8AcAByAGUAYwBpAHMAaQBvAG4AIAA+ACAAMQAsACAAXwBwAHIAZQBjAGkAcwBpAG8AbgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAHIAbwB1AG4AZAAgAHQAbwAgAG0AaQBsAGwAaQBzAGUAbwBuAGQAcwAsACAAcwBjAGEAbABlACAAdABvACAAcwBlAGMAbwBuAGQAcwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAZQBjAG8AbgBkAHMALAAgAFIATwBVAE4ARAAoAF8AdABpAG0AZQAgACoAIAA4ADYANAAwADAALAAgADMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAZQBjAG8AbgBkAHMAIAA9ACAAMAAsACAAMwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATQBPAEQAKABfAHMAZQBjAG8AbgBkAHMALAAgADEAKQAgAD4AIAAwACwAIAA1ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABNAE8ARAAoAF8AcwBlAGMAbwBuAGQAcwAgAC8AIAA2ADAALAAgADEAKQAgAD4AIAAwACwAIAA0ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAIAAzAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAHMAaABvAHcAUAByAGUAYwBpAHMAaQBvAG4AIAA9ACAAMQAsACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZgBtAHQALAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaABvAHcAUAByAGUAYwBpAHMAaQBvAG4AIAA9ACAAMgAsACAAXAAiAEgASABcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBoAG8AdwBQAHIAZQBjAGkAcwBpAG8AbgAgAD0AIAAzACwAIABcACIASABIADoAbQBtAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGgAbwB3AFAAcgBlAGMAaQBzAGkAbwBuACAAPQAgADQALAAgAFwAIgBIAEgAOgBtAG0AOgBzAHMAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAIABcACIASABIADoAbQBtADoAcwBzAC4AMAAwADAAXAAiAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAVABcACIAIAAmACAAVABFAFgAVAAoAF8AdABpAG0AZQAsACAAXwBmAG0AdAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAGYAbgBGAG8AcgBtAGEAdABUAFoALAAgAEwAQQBNAEIARABBACgAXwB0AHoAbwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAF8AdAB6AG8AKQApACwAIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAKABfAHQAegBvACAAPQAgADAAKQAgACoAIAAoAE4AKABOAG8AWgB1AGwAdQApACAAPQAgADAAKQAsACAAXAAiAFoAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBGAG0AdAAsACAASQBGACgATQBPAEQAKABfAHQAegBvACwAIAAxACkAIAA9ACAAMAAsACAAXAAiAEgASAA6AG0AbQBcACIALAAgAFwAIgBIAEgAOgBtAG0AOgBzAHMAXAAiACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGkAZwBuACwAIABJAEYAKABfAHQAegBvACAAPgA9ACAAMAAsACAAXAAiACsAXAAiACwAIABVAE4ASQBDAEgAQQBSACgAOAA3ADIAMgApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGkAZwBuACAAJgAgAFQARQBYAFQAKABBAEIAUwAoAF8AdAB6AG8AKQAgAC8AIAAxADQANAAwACwAIABfAHQAegBGAG0AdAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AaABhAHMAVABpAG0AZQAsACAAKAAoAE0ATwBEACgARABhAHkALAAgADEAKQAgAD4AIAAwACkAIAArACAASQBTAE4AVQBNAEIARQBSACgAVABpAG0AZQApACkAIAA+ACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB1AHMAZQBQAHIAZQBjAGkAcwBpAG8AbgAsACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATgBPAFQAKABfAGgAYQBzAFQAaQBtAGUAKQAsACAAMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAFAAcgBlAGMAaQBzAGkAbwBuACkAKQAsACAAMwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAIABJAE4AVAAoAFAAcgBlAGMAaQBzAGkAbwBuACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwByAEQAYQB0AGUALAAgAFIARQBTAE8ATABWAEUAXwBEAEEAVABFACgAWQBlAGEAcgBDAEUALAAgAE0AbwBuAHQAaAAsACAARABhAHkALAAgAFQAaQBtAGUALAAgAF8AdQBzAGUAUAByAGUAYwBpAHMAaQBvAG4ALAAgAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAWQBlAGEAcgAsACAAZgBuAEYAbwByAG0AYQB0AFkAZQBhAHIAKABJAE4ARABFAFgAKABfAHIARABhAHQAZQAsACAAMQAsACAAMQApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBNAG8AbgB0AGgALAAgAFQARQBYAFQAKABJAE4ARABFAFgAKABfAHIARABhAHQAZQAsACAAMQAsACAAMgApACwAIABcACIAMAAwAFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMARABhAHkALAAgAFQARQBYAFQAKABJAE4ARABFAFgAKABfAHIARABhAHQAZQAsACAAMQAsACAAMwApACwAIABcACIAMAAwAFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAVABpAG0AZQAsACAAZgBuAEYAbwByAG0AYQB0AFQAaQBtAGUAKABJAE4ARABFAFgAKABfAHIARABhAHQAZQAsACAAMQAsACAANAApACwAIABfAHUAcwBlAFAAcgBlAGMAaQBzAGkAbwBuACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBUAFoALAAgAGYAbgBGAG8AcgBtAGEAdABUAFoAKABUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAQwBPAE4AQwBBAFQAKABfAHMAWQBlAGEAcgAsACAAXAAiAC0AXAAiACwAIABfAHMATQBvAG4AdABoACwAIABcACIALQBcACIALAAgAF8AcwBEAGEAeQAsACAAXwBzAFQAaQBtAGUALAAgAF8AcwBUAFoAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ARgBPAFIATQBBAFQAXwBMAEkAVABFAFIAQQBSAFkAXwBZAEUAQQBSAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAGEAIAB5AGUAYQByACAAZgBvAHIAbQBhAHQAdABlAGQAIABpAG4AIABsAGkAdABlAHIAYQByAHkAIABzAHQAeQBsAGUALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAdABlAHgAdAAgAHwAIABMAGkAdABlAHIAYQByAHkAIAB5AGUAYQByAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AWQBlAGEAcgBDAEUAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIABOAG8AdABlACAAdABoAGEAdAAgADEAIABCAEMAIAA9ACAAMAAgAEMARQAsACAAMgAgAEIAQwAgAD0AIAAtADEAIABDAEUAXABuAFsAQQBsAHcAYQB5AHMAUwBoAG8AdwBFAHIAYQBdACAAfAAgAHMAdwBpAHQAYwBoACAAIAB8ACAAQQBsAHcAYQB5AHMAIABhAHAAcABsAHkAIABCAEMARQAvAEMARQAgAHMAdQBmAGYAaQB4AC4AIABJAGYAIABuAG8AdAAgAHUAcwBlAGQALAAgAG8AbgBsAHkAIAB5AGUAYQByAHMAIABsAGUAcwBzACAAdABoAGEAbgAgADEAMAAwADAAIABzAGgAbwB3ACAAYQBuACAAZQByAGEALgBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ARgBPAFIATQBBAFQAXwBMAEkAVABFAFIAQQBSAFkAXwBZAEUAQQBSACAAPQAgAEwAQQBNAEIARABBACgAWQBlAGEAcgBDAEUALAAgAFsAQQBsAHcAYQB5AHMAUwBoAG8AdwBFAHIAYQBdACwAXABuACAAIAAgACAASQBGACgAWQBlAGEAcgBDAEUAIAA9ACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AGUAYQByAEMARQAsACAASQBOAFQAKABZAGUAYQByAEMARQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AaQBzAEMARQAsACAAXwB5AGUAYQByAEMARQAgAD4APQAgADEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AGUAYQByACwAIABJAEYAKABfAGkAcwBDAEUALAAgAF8AeQBlAGEAcgBDAEUALAAgADEAIAAtACAAXwB5AGUAYQByAEMARQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwB1AGYAZgBpAHgALAAgAEkARgBTACgATgBPAFQAKABfAGkAcwBDAEUAKQAsACAAXAAiACAAQgBDAEUAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AGUAYQByAEMARQAgADwAIAAxADAAMAAwACwAIABcACIAIABDAEUAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATgAoAEEAbAB3AGEAeQBzAFMAaABvAHcARQByAGEAKQAgADwAPgAgADAALAAgAFwAIgAgAEMARQBcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAIABcACIAXAAiAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AeQBlAGEAcgAgACYAIABfAHMAdQBmAGYAaQB4AFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBGAE8AUgBNAEEAVABfAEwASQBUAEUAUgBBAFIAWQBfAEQAQQBUAEUAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAYQAgAGQAYQB0AGUAIABmAG8AcgBtAGEAdAB0AGUAZAAgAGkAbgAgAGwAaQB0AGUAcgBhAHIAeQAgAHMAdAB5AGwAZQAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIAB0AGUAeAB0ACAAfAAgAEwAaQB0AGUAcgBhAHIAeQAgAGQAYQB0AGUAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBZAGUAYQByAEMARQAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAAgACAAIAAgACAAIAAgACAAfAAgAE4AbwB0AGUAIAB0AGgAYQB0ACAAMQAgAEIAQwAgAD0AIAAwACAAQwBFACwAIAAyACAAQgBDACAAPQAgAC0AMQAgAEMARQBcAG4ATQBvAG4AdABoACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAWwAxAC4ALgAxADIAXQAgAHwAXABuAEQAYQB5ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMQAuAC4AMwAxAF0AIAB8AFwAbgBbAFQAaQBtAGUAXQAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIABbADAALgAuADEAKQAgACAAfAAgAFQAaQBtAGUAIABvAGYAIABkAGEAeQAgAGEAcwAgAGQAZQBjAGkAbQBhAGwAIABmAHIAYQBjAHQAaQBvAG4AIABvAGYAIABhACAAZABhAHkALgBcAG4AWwBTAGgAbwByAHQAXQAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABzAHcAaQB0AGMAaAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABSAGUAdAB1AHIAbgAgAHMAaABvAHIAdAAgAGYAbwByAG0AYQB0ACAASgBhAG4ALgAuAEQAZQBjAFwAbgBbAEkAbgB0AGUAcgBuAGEAdABpAG8AbgBhAGwARQBuAGcAbABpAHMAaABdACAAfAAgAHMAdwBpAHQAYwBoACAAIAAgACAAIAAgACAAIAAgACAAfAAgAFUAcwBlACAAdABoAGUAIABJAG4AdABlAHIAbgBhAHQAaQBvAG4AYQBsACAARQBuAGcAbABpAHMAaAAgAGkAbgBzAHQAZQBhAGQAIABvAGYAIABsAG8AYwBhAGwAIABsAGEAbgBnAHUAYQBnAGUAIABzAGUAdAAgAGkAbgAgAEUAeABjAGUAbABcAG4AWwBBAGwAdwBhAHkAcwBTAGgAbwB3AEUAcgBhAF0AIAAgACAAIAAgACAAIAAgAHwAIABzAHcAaQB0AGMAaAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABBAGwAdwBhAHkAcwAgAGEAcABwAGwAeQAgAEIAQwBFAC8AQwBFACAAcwB1AGYAZgBpAHgALgAgAEkAZgAgAG4AbwB0ACAAdQBzAGUAZAAsACAAbwBuAGwAeQAgAHkAZQBhAHIAcwAgAGwAZQBzAHMAIAB0AGgAYQBuACAAMQAwADAAMABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABzAGgAbwB3ACAAYQBuACAAZQByAGEALgBcAG4AWwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAgACAAIAAgACAAIAAgAHwAIABzAHcAaQB0AGMAaAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABDAGEAbABjAHUAbABhAHQAZQAgAGYAbwByACAAdABoAGUAIABKAHUAbABpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AIABEAGUAZgBhAHUAbAB0ACAAaQBzACAARwByAGUAZwBvAHIAaQBhAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ARgBPAFIATQBBAFQAXwBMAEkAVABFAFIAQQBSAFkAXwBEAEEAVABFACAAPQAgAEwAQQBNAEIARABBACgAWQBlAGEAcgBDAEUALAAgAE0AbwBuAHQAaAAsACAARABhAHkALAAgAFsAVABpAG0AZQBdACwAIABbAFMAaABvAHIAdABdACwAIABbAEkAbgB0AGUAcgBuAGEAdABpAG8AbgBhAGwARQBuAGcAbABpAHMAaABdACwAIABbAEEAbAB3AGEAeQBzAFMAaABvAHcARQByAGEAXQAsACAAWwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAsAFwAbgAgACAAIAAgAEkARgAoACgAWQBlAGEAcgBDAEUAIAA9ACAAXAAiAFwAIgApACAAKgAgACgATQBvAG4AdABoACAAPQAgAFwAIgBcACIAKQAgACoAIAAoAEQAYQB5ACAAPQAgAFwAIgBcACIAKQAsACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABNAG8AbgB0AGgAKQApACAAKwAgACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABZAGUAYQByAEMARQApACkAIAAqACAATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABEAGEAeQApACkAKQAsACAAIwBWAEEATABVAEUAIQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AeQBlAGEAcgBDAEUALAAgAEkARgAoAFkAZQBhAHIAQwBFACAAPQAgAFwAIgBcACIALAAgADIAMAAwADAALAAgAFkAZQBhAHIAQwBFACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAYQB5ACwAIABJAEYAKABEAGEAeQAgAD0AIABcACIAXAAiACwAIAAxACwAIABEAGEAeQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgATgBPAFQAKABJAFMAXwBWAEEATABJAEQAXwBEAEEAVABFACgAXwB5AGUAYQByAEMARQAsACAATQBvAG4AdABoACwAIABfAGQAYQB5ACwAIABKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQApACwAIAAjAFYAQQBMAFUARQAhACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHIARABhAHQAZQAsACAASQBGACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABUAGkAbQBlACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXwB5AGUAYQByAEMARQAsACAATQBvAG4AdABoACwAIABfAGQAYQB5ACwAIABcACIAXAAiACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABSAEUAUwBPAEwAVgBFAF8ARABBAFQARQAoAF8AeQBlAGEAcgBDAEUALAAgAE0AbwBuAHQAaAAsACAAXwBkAGEAeQAsACAAVABpAG0AZQAsACAAMwAsACAASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAE0AbwBuAHQAaAAsACAATQBPAE4AVABIAF8ATgBBAE0ARQAoAEkATgBEAEUAWAAoAF8AcgBEAGEAdABlACwAIAAxACwAIAAyACkALAAgAFMAaABvAHIAdAAsACAASQBuAHQAZQByAG4AYQB0AGkAbwBuAGEAbABFAG4AZwBsAGkAcwBoACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAEQAYQB5ACwAIABJAEYAKABJAFMATgBVAE0AQgBFAFIAKABEAGEAeQApACwAIABcACIAIABcACIAIAAmACAASQBOAEQARQBYACgAXwByAEQAYQB0AGUALAAgADEALAAgADMAKQAsACAAXAAiAFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBZAGUAYQByACwAIABJAEYAKABJAFMATgBVAE0AQgBFAFIAKABZAGUAYQByAEMARQApACwAIABcACIALAAgAFwAIgAgACYAIABGAE8AUgBNAEEAVABfAEwASQBUAEUAUgBBAFIAWQBfAFkARQBBAFIAKABJAE4ARABFAFgAKABfAHIARABhAHQAZQAsACAAMQAsACAAMQApACwAIABBAGwAdwBhAHkAcwBTAGgAbwB3AEUAcgBhACkALAAgAFwAIgBcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAVABpAG0AZQAsACAASQBGACgASQBTAE4AVQBNAEIARQBSACgAVABpAG0AZQApACwAIABcACIALAAgAFwAIgAgACYAIABUAEUAWABUACgASQBOAEQARQBYACgAXwByAEQAYQB0AGUALAAgADEALAAgADQAKQAsACAAXAAiAGgAOgBtAG0AIABBAE0ALwBQAE0AXAAiACkALAAgAFwAIgBcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABDAE8ATgBDAEEAVAAoAF8AcwBNAG8AbgB0AGgALAAgAF8AcwBEAGEAeQAsACAAXwBzAFkAZQBhAHIALAAgAF8AcwBUAGkAbQBlACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEYATwBSAE0AQQBUAF8AVQBTAF8ARABBAFQARQBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIABhACAAZABhAHQAZQAgAGYAbwByAG0AYQB0AHQAZQBkACAAaQBuACAAdABoAGUAIABVAFMAIABzAHQAeQBsAGUALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAdABlAHgAdAAgAHwAIABVAFMAIABzAHQAeQBsAGUAIABkAGEAdABlAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AWQBlAGEAcgBDAEUAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAIAAgACAAIAAgACAAIAAgAHwAIABOAG8AdABlACAAdABoAGEAdAAgADEAIABCAEMAIAA9ACAAMAAgAEMARQAsACAAMgAgAEIAQwAgAD0AIAAtADEAIABDAEUAXABuAE0AbwBuAHQAaAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAFsAMQAuAC4AMQAyAF0AIAB8AFwAbgBEAGEAeQAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADEALgAuADMAMQBdACAAfABcAG4AWwBUAGkAbQBlAF0AIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAWwAwAC4ALgAxACkAIAAgAHwAIABUAGkAbQBlACAAbwBmACAAZABhAHkAIABhAHMAIABkAGUAYwBpAG0AYQBsACAAZgByAGEAYwB0AGkAbwBuACAAbwBmACAAYQAgAGQAYQB5AC4AXABuAFsAUwBlAHAAYQByAGEAdABvAHIAXQAgACAAIAAgACAAIAB8ACAAYwBoAGEAcgAgACAAIAAgAFsALAAuAC8ALQBfAF0AIAB8ACAAQwBoAGEAcgBhAGMAdABlAHIAIABzAGUAcABhAHIAYQB0AG8AcgAgAGYAbwByACAAZABhAHQAZQAgAGUAbABlAG0AZQBuAHQAcwAuAFwAbgBbAFAAcgBlAGMAaQBzAGkAbwBuAF0AIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAAgACAAIAAgACAAIAAgACAAfAAgAFMAZQBsAGUAYwB0ACAAcAByAGUAYwBpAHMAaQBvAG4AIABsAGUAdgBlAGwALAAgAGQAZQBmAGEAdQBsAHQAIABpAHMAIAAzAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAwACAALQAgAEYAbABvAGEAdABzACAAZgByAG8AbQAgAG0AaQBuAHUAdABlACAAdABvACAAbQBpAGwAbABpAHMAZQBjAG8AbgBkAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAxACAALQAgAEQAYQB5AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAyACAALQAgAEgAbwB1AHIAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADMAIAAtACAATQBpAG4AdQB0AGUAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADQAIAAtACAAUwBlAGMAbwBuAGQAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADUAIAAtACAATQBpAGwAbABpAHMAZQBjAG8AbgBkAFwAbgBbAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACAAfAAgAHMAdwBpAHQAYwBoACAAIAAgACAAIAAgACAAIAAgACAAfAAgAEMAYQBsAGMAdQBsAGEAdABlACAAZgBvAHIAIAB0AGgAZQAgAEoAdQBsAGkAYQBuACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgAgAEQAZQBmAGEAdQBsAHQAIABpAHMAIABHAHIAZQBnAG8AcgBpAGEAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuACAAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEYATwBSAE0AQQBUAF8AVQBTAF8ARABBAFQARQAgAD0AIABMAEEATQBCAEQAQQAoAFkAZQBhAHIAQwBFACwAIABNAG8AbgB0AGgALAAgAEQAYQB5ACwAIABbAFQAaQBtAGUAXQAsACAAWwBTAGUAcABhAHIAYQB0AG8AcgBdACwAIABbAFAAcgBlAGMAaQBzAGkAbwBuAF0ALAAgAFsASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0ALABcAG4AIAAgACAAIABJAEYAKAAoAFkAZQBhAHIAQwBFACAAPQAgAFwAIgBcACIAKQAgACoAIAAoAE0AbwBuAHQAaAAgAD0AIABcACIAXAAiACkAIAAqACAAKABEAGEAeQAgAD0AIABcACIAXAAiACkALAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgAWQBlAGEAcgBDAEUAKQApACAAKwAgAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgATQBvAG4AdABoACkAKQAgACsAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEQAYQB5ACkAKQAsACAAIwBWAEEATABVAEUAIQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBfAFYAQQBMAEkARABfAEQAQQBUAEUAKABZAGUAYQByAEMARQAsACAATQBvAG4AdABoACwAIABEAGEAeQAsACAASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByACkAKQAsACAAIwBWAEEATABVAEUAIQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABmAG4ARgBvAHIAbQBhAHQAVABpAG0AZQAsACAATABBAE0AQgBEAEEAKABfAHQAaQBtAGUALAAgAF8AcAByAGUAYwBpAHMAaQBvAG4ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBwAHIAZQBjAGkAcwBpAG8AbgAgAD0AIAAxACwAIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBoAG8AdwBQAHIAZQBjAGkAcwBpAG8AbgAsACAASQBGACgAXwBwAHIAZQBjAGkAcwBpAG8AbgAgAD4AIAAxACwAIABfAHAAcgBlAGMAaQBzAGkAbwBuACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAcgBvAHUAbgBkACAAdABvACAAbQBpAGwAbABpAHMAZQBvAG4AZABzACwAIABzAGMAYQBsAGUAIAB0AG8AIABzAGUAYwBvAG4AZABzAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBlAGMAbwBuAGQAcwAsACAAUgBPAFUATgBEACgAXwB0AGkAbQBlACAAKgAgADgANgA0ADAAMAAsACAAMwApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBlAGMAbwBuAGQAcwAgAD0AIAAwACwAIAAzACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABNAE8ARAAoAF8AcwBlAGMAbwBuAGQAcwAsACAAMQApACAAPgAgADAALAAgADUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAE0ATwBEACgAXwBzAGUAYwBvAG4AZABzACAALwAgADYAMAAsACAAMQApACAAPgAgADAALAAgADQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALAAgADMAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAF8AcwBoAG8AdwBQAHIAZQBjAGkAcwBpAG8AbgAgAD0AIAAxACwAIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBmAG0AdAAsACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBoAG8AdwBQAHIAZQBjAGkAcwBpAG8AbgAgAD0AIAAyACwAIABcACIAaAAgAEEATQAvAFAATQBcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBoAG8AdwBQAHIAZQBjAGkAcwBpAG8AbgAgAD0AIAAzACwAIABcACIAaAA6AG0AbQAgAEEATQAvAFAATQBcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBoAG8AdwBQAHIAZQBjAGkAcwBpAG8AbgAgAD0AIAA0ACwAIABcACIAaAA6AG0AbQA6AHMAcwAgAEEATQAvAFAATQBcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALAAgAFwAIgBoADoAbQBtADoAcwBzAC4AMAAwADAAIABBAE0ALwBQAE0AXAAiAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAIABcACIAIAAmACAAVABFAFgAVAAoAF8AdABpAG0AZQAsACAAXwBmAG0AdAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBlAHAAYQByAGEAdABvAHIALAAgAEkARgAoAFMAZQBwAGEAcgBhAHQAbwByACAAPQAgAFwAIgBcACIALAAgAFwAIgAvAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYwBoAGEAcgAxACwAIABMAEUARgBUACgAUwBlAHAAYQByAGEAdABvAHIALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAEkARgBFAFIAUgBPAFIAKABGAEkATgBEACgAXwBjAGgAYQByADEALAAgAFwAIgAsAC4ALwAtAF8AXAAiACkALAAgADAAKQAgAD4AIAAwACwAIABfAGMAaABhAHIAMQAsACAAXAAiAC8AXAAiACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGgAYQBzAFQAaQBtAGUALAAgACgAKABNAE8ARAAoAEQAYQB5ACwAIAAxACkAIAA+ACAAMAApACAAKwAgAEkAUwBOAFUATQBCAEUAUgAoAFQAaQBtAGUAKQApACAAPgAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdQBzAGUAUAByAGUAYwBpAHMAaQBvAG4ALAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAE4ATwBUACgAXwBoAGEAcwBUAGkAbQBlACkALAAgADEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABQAHIAZQBjAGkAcwBpAG8AbgApACkALAAgADMALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABSAFUARQAsACAASQBOAFQAKABQAHIAZQBjAGkAcwBpAG8AbgApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwByAEQAYQB0AGUALAAgAFIARQBTAE8ATABWAEUAXwBEAEEAVABFACgAWQBlAGEAcgBDAEUALAAgAE0AbwBuAHQAaAAsACAARABhAHkALAAgAFQAaQBtAGUALAAgAF8AdQBzAGUAUAByAGUAYwBpAHMAaQBvAG4ALAAgAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAWQBlAGEAcgAsACAAVABFAFgAVAAoAEkATgBEAEUAWAAoAF8AcgBEAGEAdABlACwAIAAxACwAIAAxACkALAAgAFwAIgAwADAAMAAwADsAXAAiACAAJgAgAFUATgBJAEMASABBAFIAKAA4ADcAMgAyACkAIAAmACAAXAAiADAAMAAwADAAOwAwADAAMAAwAFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMATQBvAG4AdABoACwAIABJAE4ARABFAFgAKABfAHIARABhAHQAZQAsACAAMQAsACAAMgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMARABhAHkALAAgAFQARQBYAFQAKABJAE4ARABFAFgAKABfAHIARABhAHQAZQAsACAAMQAsACAAMwApACwAIABcACIAMAAwAFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAVABpAG0AZQAsACAAZgBuAEYAbwByAG0AYQB0AFQAaQBtAGUAKABJAE4ARABFAFgAKABfAHIARABhAHQAZQAsACAAMQAsACAANAApACwAIABfAHUAcwBlAFAAcgBlAGMAaQBzAGkAbwBuACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEMATwBOAEMAQQBUACgAXwBzAE0AbwBuAHQAaAAsACAAXwBzAGUAcABhAHIAYQB0AG8AcgAsACAAXwBzAEQAYQB5ACwAIABfAHMAZQBwAGEAcgBhAHQAbwByACwAIABfAHMAWQBlAGEAcgAsACAAXwBzAFQAaQBtAGUAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ARgBPAFIATQBBAFQAXwBNAEkATABfAEQAVABHAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAGEAIABkAGEAdABlACAAZgBvAHIAbQBhAHQAdABlAGQAIABpAG4AIABVAFMAIABNAGkAbABpAHQAYQByAHkAIABtAGUAcwBzAGEAZwBlACAAdAByAGEAZgBmAGkAYwAgAHMAdAB5AGwAZQAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIAB0AGUAeAB0ACAAfAAgAEQAVABHACAAZgBvAHIAbQBhAHQAdABlAGQAIABkAGEAdABlAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AWQBlAGEAcgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAIAAgACAAIAAgACAAIAAgAHwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAWwAxADkANQAxAC4ALgAyADAANQAwAF0AIAAgACAAIAB8AFwAbgBNAG8AbgB0AGgAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIABbADEALgAuADEAMgBdACAAfABcAG4ARABhAHkAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAWwAxAC4ALgAzADEAXQAgAHwAXABuAFQAaQBtAGUAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgAFsAMAAuAC4AMQApACAAIAB8ACAAVABpAG0AZQAgAG8AZgAgAGQAYQB5ACAAYQBzACAAZABlAGMAaQBtAGEAbAAgAGYAcgBhAGMAdABpAG8AbgAgAG8AZgAgAGEAIABkAGEAeQAuAFwAbgBbAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdABdACAAfAAgAGQAZQBjAGkAbQBhAGwAIAAgACAAIAAgACAAIAAgACAAfAAgAFQAaQBtAGUAIAB6AG8AbgBlACAAbwBmAGYAcwBlAHQAIABpAG4AIABtAGkAbgB1AHQAZQBzACAAZgByAG8AbQAgAFUAVABDAC4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAWwAtADkAMAAwAC4ALgA5ADAAMABdACAAIAAgACAAIAB8ACAAQQBzAHMAdQBtAGUAZAAgAHQAbwAgAGIAZQAgAFUAVABDACAAaQBmACAAbwBtAG0AaQB0AHQAZQBkAC4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAVABpAG0AZQAgAHcAaQBsAGwAIABiAGUAIABjAG8AbgB2AGUAcgB0AGUAZAAgAGkAZgAgAHQAaABlACAAbwBmAGYAcwBlAHQAIABkAG8AZQBzACAAbgBvAHQAIABhAGwAaQBnAG4AIAB3AGkAdABoACAAbQBpAGwAaQB0AGEAcgB5AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAHQAaQBtAGUAIAB6AG8AbgBlAHMALgBcAG4AWwBTAGgAbwByAHQAXQAgACAAIAAgACAAIAAgACAAIAAgAHwAIABzAHcAaQB0AGMAaAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABTAGgAbwByAHQAIAB0AGkAbQBlACAAZgBvAHIAbQB0ADoAIABoAGgAbQBtACwAIABvAHQAaABlAHIAdwBpAHMAZQA6ACAAaABoAG0AbQBzAHMAXABuAFwAbgBFAHgAYQBtAHAAbABlAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEYATwBSAE0AQQBUAF8ATQBJAEwAXwBEAFQARwAoADIAMAAyADMALAAgADIALAAgADEAMgAsACAAMAAuADcANQAsACAANgAwADAALAAgADEAKQBcAG4AUgBlAHQAdQByAG4AcwA6ACAAMQAyADEAOAAwADAASwBGAEUAQgAyADMAXABuAFwAbgBGAE8AUgBNAEEAVABfAE0ASQBMAF8ARABUAEcAKAAgACwAIAAsACAAMQAyACwAIAAwAC4AMgA1ACkAXABuAFIAZQB0AHUAcgBuAHMAOgAgADEAMgAwADYAMAAwAEoAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEYATwBSAE0AQQBUAF8ATQBJAEwAXwBEAFQARwAgAD0AIABMAEEATQBCAEQAQQAoAFkAZQBhAHIALAAgAE0AbwBuAHQAaAAsACAARABhAHkALAAgAFQAaQBtAGUALAAgAFsAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0AF0ALAAgAFsAUwBoAG8AcgB0AF0ALABcAG4AIAAgACAAIABJAEYAKAAoAFkAZQBhAHIAIAA9ACAAXAAiAFwAIgApACAAKgAgACgATQBvAG4AdABoACAAPQAgAFwAIgBcACIAKQAgACoAIAAoAEQAYQB5ACAAPQAgAFwAIgBcACIAKQAgACoAIAAoAFQAaQBtAGUAIAA9ACAAXAAiAFwAIgApACwAIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEQAYQB5ACkAKQAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGwAbwBjAGEAbAAsACAAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0ACAAPQAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBvACwAIABOACgAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAGYAbgBJAG4AdgBhAGwAaQBkAFAAYQByAGEAbQBzACwAIABMAEEATQBCAEQAQQAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAQQBCAFMAKABfAHQAegBvACkAIAA+ACAAOQAwADAALAAgAFQAUgBVAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgASQBTAE4AVQBNAEIARQBSACgAWQBlAGEAcgApACwAIAAoACgAWQBlAGEAcgAgADwAIAAxADkANQAxACkAIAArACAAKABZAGUAYQByACAAPgAgADIAMAA1ADAAKQApACwAIABGAEEATABTAEUAKQAsACAAVABSAFUARQAsACAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgAKAAoAFkAZQBhAHIAIAA9ACAAXAAiAFwAIgApACAAKgAgACgATQBvAG4AdABoACAAPQAgAFwAIgBcACIAKQApACAAKwAgAE4AKABJAFMAXwBWAEEATABJAEQAXwBEAEEAVABFACgAWQBlAGEAcgAsACAATQBvAG4AdABoACwAIABEAGEAeQAsACAAMAApACkAKQAgAD0AIAAwACwAIABUAFIAVQBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALAAgAEYAQQBMAFMARQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABmAG4ARgBtAHQAVABpAG0AZQAsACAATABBAE0AQgBEAEEAKABfAHQAaQBtAGUALAAgAF8AcwBoAG8AcgB0ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAaQBtAGUARgBtAHQALAAgAEkARgAoAF8AcwBoAG8AcgB0ACwAIABcACIASABIAG0AbQBcACIALAAgAFwAIgBIAEgAbQBtAHMAcwBcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAEUAWABUACgAXwB0AGkAbQBlACwAIABfAHQAaQBtAGUARgBtAHQAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABmAG4AUgBlAHMAbwBsAHYAZQBNAGkAbABpAHQAYQByAHkAVABaACwAIABMAEEATQBCAEQAQQAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBsAG8AYwBhAGwALAAgAEgAUwBUAEEAQwBLACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATgAoAFQAaQBtAGUAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBKAFwAIgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBvACAAPgAgADcAMgAwACwAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBoAGkAZgB0AFQAWgBPACwAIABfAHQAegBvACAALQAgADcAMgAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AGkAbQBlACwAIABOACgAVABpAG0AZQApACAALQAgACgAXwBzAGgAaQBmAHQAVABaAE8AIAAvACAAMQA0ADQAMAApACwAIAAgAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAaQBtAGUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBNAFwAIgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdAB6AG8AIAA8ACAALQA3ADIAMAAsACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaABpAGYAdABUAFoATwAsACAAXwB0AHoAbwAgACsAIAA3ADIAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdABpAG0AZQAsACAATgAoAFQAaQBtAGUAKQAgAC0AIAAoAF8AcwBoAGkAZgB0AFQAWgBPACAALwAgADEANAA0ADAAKQAsACAAIABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AGkAbQBlACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAWQBcACIAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbQBpAGwAaQB0AGEAcgB5AFQAWgBPACwAIABTAEkARwBOACgAXwB0AHoAbwApACAAKgAgAE0AUgBPAFUATgBEACgAQQBCAFMAKABfAHQAegBvACkALAAgADYAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGgAaQBmAHQAVABaAE8ALAAgAF8AdAB6AG8AIAAtACAAXwBtAGkAbABpAHQAYQByAHkAVABaAE8ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAaQBtAGUALAAgAE4AKABUAGkAbQBlACkAIAAtACAAKABfAHMAaABpAGYAdABUAFoATwAgAC8AIAAxADQANAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGkAZAB4ACwAIABJAE4AVAAoAF8AbQBpAGwAaQB0AGEAcgB5AFQAWgBPACAALwAgADYAMAApACAAKwAgADEAMwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbQBpAGwAaQB0AGEAcgB5AFQAWgAsACAAQwBIAE8ATwBTAEUAKABfAGkAZAB4ACwAIABcACIAWQBcACIALAAgAFwAIgBYAFwAIgAsACAAXAAiAFcAXAAiACwAIABcACIAVgBcACIALAAgAFwAIgBVAFwAIgAsACAAXAAiAFQAXAAiACwAIABcACIAUwBcACIALAAgAFwAIgBSAFwAIgAsACAAXAAiAFEAXAAiACwAIABcACIAUABcACIALAAgAFwAIgBPAFwAIgAsACAAXAAiAE4AXAAiACwAIABcACIAWgBcACIALAAgAFwAIgBBAFwAIgAsACAAXAAiAEIAXAAiACwAIABcACIAQwBcACIALAAgAFwAIgBEAFwAIgAsACAAXAAiAEUAXAAiACwAIABcACIARgBcACIALAAgAFwAIgBHAFwAIgAsACAAXAAiAEgAXAAiACwAIABcACIASQBcACIALAAgAFwAIgBLAFwAIgAsACAAXAAiAEwAXAAiACwAIABcACIATQBcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAaQBtAGUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbQBpAGwAaQB0AGEAcgB5AFQAWgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAGYAbgBJAG4AdgBhAGwAaQBkAFAAYQByAGEAbQBzACgAKQAsACAAewBcACIAIwBOAFUATQAhACEAXAAiAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbQBpAGwAaQB0AGEAcgB5AFQAaQBtAGUALAAgAGYAbgBSAGUAcwBvAGwAdgBlAE0AaQBsAGkAdABhAHIAeQBUAFoAKAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcgBEAGEAdABlACwAIABJAEYAKABZAGUAYQByACAAPQAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABSAEUAUwBPAEwAVgBFAF8ARABBAFQARQAoADIAMAAwADAALAAgADMALAAgAEQAYQB5ACwAIABJAE4ARABFAFgAKABfAG0AaQBsAGkAdABhAHIAeQBUAGkAbQBlACwAIAAxACwAIAAxACkALAAgADMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFIARQBTAE8ATABWAEUAXwBEAEEAVABFACgAWQBlAGEAcgAsACAATQBvAG4AdABoACwAIABEAGEAeQAsACAASQBOAEQARQBYACgAXwBtAGkAbABpAHQAYQByAHkAVABpAG0AZQAsACAAMQAsACAAMQApACwAIAAzACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAEQAYQB5ACwAIABUAEUAWABUACgASQBOAEQARQBYACgAXwByAEQAYQB0AGUALAAgADMAKQAsACAAXAAiADAAMABcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABZAGUAYQByACAAPQAgAFwAIgBcACIALAAgAEMATwBOAEMAQQBUACgAXwBzAEQAYQB5ACwAIABmAG4ARgBtAHQAVABpAG0AZQAoAEkATgBEAEUAWAAoAF8AcgBEAGEAdABlACwAIAA0ACkALAAgADEAKQAsACAASQBOAEQARQBYACgAXwBtAGkAbABpAHQAYQByAHkAVABpAG0AZQAsACAAMQAsACAAMgApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAFQAaQBtAGUALAAgAGYAbgBGAG0AdABUAGkAbQBlACgASQBOAEQARQBYACgAXwByAEQAYQB0AGUALAAgADQAKQAsACAATgAoAFMAaABvAHIAdAApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBNAG8AbgB0AGgALAAgAFUAUABQAEUAUgAoAE0ATwBOAFQASABfAE4AQQBNAEUAKABJAE4ARABFAFgAKABfAHIARABhAHQAZQAsACAAMgApACwAIAAxACwAIAAxACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAFkAWQAsACAAUgBJAEcASABUACgAVABFAFgAVAAoAEkATgBEAEUAWAAoAF8AcgBEAGEAdABlACwAIAAxACkALAAgAFwAIgAwADAAXAAiACkALAAgADIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAQwBPAE4AQwBBAFQAKABfAHMARABhAHkALAAgAF8AcwBUAGkAbQBlACwAIABJAE4ARABFAFgAKABfAG0AaQBsAGkAdABhAHIAeQBUAGkAbQBlACwAIAAxACwAIAAyACkALAAgAF8AcwBNAG8AbgB0AGgALAAgAF8AcwBZAFkAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4AXABuAFwAbgBcAG4AXABuAFwAbgBcAG4ALwAqACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwBcAG4AIwAgAEMATwBOAFYARQBSAFMASQBPAE4AUwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACoALwBcAG4AXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ASQBTAE8ARABBAFQARQBfAFQATwBfAEoARABOAF8ATABPAEMAQQBMAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAHQAaABlACAASgB1AGwAaQBhAG4AIABEAGEAeQAgAE4AdQBtAGIAZQByACAAYQBuAGQAIABsAG8AYwBhAGwAIAB0AGkAbQBlACAAZgBvAHIAIABhACAAZABhAHQAZQAgAGEAbgBkACAAdABpAG0AZQAgAHAAcgBvAHYAaQBkAGUAZAAgAGkAbgAgAEkAUwBPACAAZgBvAHIAbQBhAHQALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAaQBuAHQAZQBnAGUAcgAgACAAIAAgACAAIAAgACAAfAAgAEwAbwBjAGEAbAAgAEoAdQBsAGkAYQBuACAARABhAHkAIABOAHUAbQBiAGUAcgBcAG4AIAAyACAAfAAgAGQAZQBjAGkAbQBhAGwAIABbADAALgAuADEAKQAgAHwAIABMAG8AYwBhAGwAIAB0AGkAbQBlACAAbwBmACAAZABhAHkALgAgAEQAZQBjAGkAbQBhAGwAIABmAHIAYQBjAHQAaQBvAG4AIABvAGYAIABhACAAZABhAHkALAAgAGkAbQBwAGwAaQBjAGkAdABsAHkAIABjAG8AbgB2AGUAcgB0AHMAIAB0AG8AIABFAHgAYwBlAGwAIAB0AGkAbQBlACAAZABhAHQAYQAgAHQAeQBwAGUALgBcAG4AIAAzACAAfAAgAGQAZQBjAGkAbQBhAGwAIAAgACAAIAAgACAAIAAgAHwAIABUAGkAbQBlACAAegBvAG4AZQAgAG8AZgBmAHMAZQB0ACAAbQBpAG4AdQB0AGUAcwAgAGYAcgBvAG0AIABVAFQAQwBcAG4AIAAgACAAfAAgAFsALQA5ADAAMAAuAC4AOQAwADAAXQAgACAAIAAgAHwAIABcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEkAUwBPAEQAYQB0AGUAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAB0AGUAeAB0ACAAIAAgAHwAIABJAFMATwAgAGYAbwByAG0AYQB0AHQAZQBkACAAZABhAHQAZQAsACAAdABpAG0AZQAgAGEAbgBkACAAdABpAG0AZQAgAHoAbwBuAGUAIABvAGYAZgBzAGUAdAAuAFwAbgBbAEYAcgBvAG0ASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0AIAB8ACAAcwB3AGkAdABjAGgAIAB8ACAAQwBhAGwAYwB1AGwAYQB0AGUAIABmAHIAbwBtACAAdABoAGUAIABKAHUAbABpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AIABEAGUAZgBhAHUAbAB0ACAAaQBzACAARwByAGUAZwBvAHIAaQBhAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgAHwAIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuACAAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEkAUwBPAEQAQQBUAEUAXwBUAE8AXwBKAEQATgBfAEwATwBDAEEATAAgAD0AIABMAEEATQBCAEQAQQAoAEkAUwBPAEQAYQB0AGUALAAgAFsARgByAG8AbQBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAsAFwAbgAgACAAIAAgAEkARgAoAEkAUwBPAEQAYQB0AGUAIAA9ACAAXAAiAFwAIgAsACAAewBcACIAXAAiACwAIABcACIAXAAiACwAIABcACIAXAAiAH0ALABcAG4AIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AaQBzAG8ARABhAHQAZQAsACAAUABBAFIAUwBFAF8ASQBTAE8AXwBEAEEAVABFACgASQBTAE8ARABhAHQAZQAsACAARgByAG8AbQBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGoAZABuACwAIABJAEYAKABJAFMARQBSAFIATwBSACgASQBOAEQARQBYACgAXwBpAHMAbwBEAGEAdABlACwAIAAxACwAIAAxACkAKQAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABKAFUATABJAEEATgBfAEQAQQBZAF8ATgBVAE0AQgBFAFIAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkATgBEAEUAWAAoAF8AaQBzAG8ARABhAHQAZQAsACAAMQAsACAAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAE4ARABFAFgAKABfAGkAcwBvAEQAYQB0AGUALAAgADEALAAgADIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBOAEQARQBYACgAXwBpAHMAbwBEAGEAdABlACwAIAAxACwAIAAzACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEYAcgBvAG0ASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AGkAbQBlACwAIABJAEYAKABJAE4ARABFAFgAKABfAGkAcwBvAEQAYQB0AGUALAAgADEALAAgADQAKQAgAD0AIABcACIAXAAiACwAIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGAEUAUgBSAE8AUgAoAE0ATwBEACgASQBOAEQARQBYACgAXwBpAHMAbwBEAGEAdABlACwAIAAxACwAIAA0ACkALAAgADEAKQAsACAAewAjAFYAQQBMAFUARQAhAH0AKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGMAYQByAHIAeQBEAGEAeQAsACAASQBGACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABJAE4ARABFAFgAKABfAGkAcwBvAEQAYQB0AGUALAAgADEALAAgADQAKQApACkALAAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAE4AVAAoAEkATgBEAEUAWAAoAF8AaQBzAG8ARABhAHQAZQAsACAAMQAsACAANAApACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwByAEoARABOACwAIABJAEYARQBSAFIATwBSACgAXwBKAEQATgAgACsAIABfAGMAYQByAHIAeQBEAGEAeQAsACAAewAjAFYAQQBMAFUARQAhAH0AKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegAsACAASQBGAEUAUgBSAE8AUgAoAEkATgBEAEUAWAAoAF8AaQBzAG8ARABhAHQAZQAsACAAMQAsACAANQApACwAIAB7ACMAVgBBAEwAVQBFACEAfQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXwByAEoARABOACwAIABfAHQAaQBtAGUALAAgAF8AdAB6ACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBJAFMATwBEAEEAVABFAF8AVABPAF8ASgBEAEEAVABFAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAHQAaABlACAASgB1AGwAaQBhAG4AIABEAGEAdABlACAAZgBvAHIAIABhACAAZABhAHQAZQAgAGEAbgBkACAAdABpAG0AZQAgAHAAcgBvAHYAaQBkAGUAZAAgAGkAbgAgAEkAUwBPACAAZgBvAHIAbQBhAHQALgBcAG4ATgBvAHQAZQAgAGEAIABKAHUAbABpAGEAbgAgAEQAYQB0AGUAIABpAHMAIABhAGwAdwBhAHkAcwAgAGkAbgAgAFUAVABDAC4AXABuAFwAbgBPAHUAdABwAHUAdABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAASgB1AGwAaQBhAG4AIABEAGEAdABlAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ASQBTAE8ARABhAHQAZQAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAHQAZQB4AHQAIAAgACAAfAAgAEkAUwBPACAAZgBvAHIAbQBhAHQAdABlAGQAIABkAGEAdABlACwAIAB0AGkAbQBlACAAYQBuAGQAIAB0AGkAbQBlACAAegBvAG4AZQAgAG8AZgBmAHMAZQB0AC4AIABJAGYAIAB0AGkAbQBlACAAaQBzACAAbwBtAG0AaQB0AHQAZQBkACwAIABhAHMAcwB1AG0AZQBkAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAB8ACAAdABvACAAYgBlACAAYQB0ACAAMAAwADoAMAAwAC4AIABJAGYAIAB0AGkAbQBlACAAegBvAG4AZQAgAGkAcwAgAG8AbQBtAGkAdAB0AGUAZAAsACAAYQBzAHMAdQBtAGUAZAAgAHQAbwAgAGIAZQAgAFUAVABDAC4AXABuAFsARgByAG8AbQBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAgAHwAIABzAHcAaQB0AGMAaAAgAHwAIABDAGEAbABjAHUAbABhAHQAZQAgAGYAcgBvAG0AIAB0AGgAZQAgAEoAdQBsAGkAYQBuACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgAgAEQAZQBmAGEAdQBsAHQAIABpAHMAIABHAHIAZQBnAG8AcgBpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAB8ACAAYwBhAGwAZQBuAGQAYQByAC4AIABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ASQBTAE8ARABBAFQARQBfAFQATwBfAEoARABBAFQARQAgAD0AIABMAEEATQBCAEQAQQAoAEkAUwBPAEQAYQB0AGUALAAgAFsARgByAG8AbQBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAsAFwAbgAgACAAIAAgAEkARgAoAEkAUwBPAEQAYQB0AGUAIAA9ACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBqAGQAbgBMAG8AYwBhAGwALAAgAEkAUwBPAEQAQQBUAEUAXwBUAE8AXwBKAEQATgBfAEwATwBDAEEATAAoAEkAUwBPAEQAYQB0AGUALAAgAEYAcgBvAG0ASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAASgBEAE4AXwBMAE8AQwBBAEwAXwBUAE8AXwBKAEQAQQBUAEUAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAE4ARABFAFgAKABfAGoAZABuAEwAbwBjAGEAbAAsACwAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABOACgASQBOAEQARQBYACgAXwBqAGQAbgBMAG8AYwBhAGwALAAsACAAMgApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABOACgASQBOAEQARQBYACgAXwBqAGQAbgBMAG8AYwBhAGwALAAsACAAMwApACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBJAFMATwBEAEEAVABFAF8AVABPAF8ARQBEAEEAVABFAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAGEAbgAgAEUAeABjAGUAbAAgAEQAYQB0AGUALwBUAGkAbQBlACAAZgBvAHIAIABhACAAZABhAHQAZQAgAGEAbgBkACAAdABpAG0AZQAgAHAAcgBvAHYAaQBkAGUAZAAgAGkAbgAgAEkAUwBPACAAZgBvAHIAbQBhAHQALgBcAG4ATgBvAHQAZQAgAEUAeABjAGUAbAAgAEQAYQB0AGUALwBUAGkAbQBlACAAdQBzAGUAcwAgAHQAaABlACAARwByAGUAZwBvAHIAaQBhAG4AIABjAGEAbABlAG4AZABhAHIALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAZABlAGMAaQBtAGEAbAAgACAAIAAgACAAIAB8ACAARQB4AGMAZQBsACAARABhAHQAZQAvAFQAaQBtAGUALgBcAG4AIAAgACAAfAAgAFsAMQAuAC4AMgA5ADUAOAA0ADYANgApACAAfAAgADEAOQAwADAALQAwADEALQAwADEALgAuADkAOQA5ADkALQAxADIALQAzADEAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBJAFMATwBEAGEAdABlACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAdABlAHgAdAAgACAAIAB8ACAASQBTAE8AIABmAG8AcgBtAGEAdAB0AGUAZAAgAGQAYQB0AGUALAAgAHQAaQBtAGUAIABhAG4AZAAgAHQAaQBtAGUAIAB6AG8AbgBlACAAbwBmAGYAcwBlAHQALgAgAEkAZgAgAHQAaQBtAGUAIABpAHMAIABvAG0AbQBpAHQAdABlAGQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAfAAgAGEAcwBzAHUAbQBlAGQAIAB0AG8AIABiAGUAIABhAHQAIAAwADAAOgAwADAALgBcAG4AWwBJAG4AYwBsAHUAZABlAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdABdACAAfAAgAHMAdwBpAHQAYwBoACAAfAAgAFIAZQB0AHUAcgBuACAAdABpAG0AZQAgAHoAbwBuAGUAIABvAGYAZgBzAGUAdAAgAHAAYQByAHMAZQBkACAAZgByAG8AbQAgAHQAaABlACAASQBTAE8ARABhAHQAZQAuAFwAbgBbAEYAcgBvAG0ASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0AIAAgACAAIAB8ACAAcwB3AGkAdABjAGgAIAB8ACAAQwBhAGwAYwB1AGwAYQB0AGUAIABmAHIAbwBtACAAdABoAGUAIABKAHUAbABpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AIABEAGUAZgBhAHUAbAB0ACAAaQBzACAARwByAGUAZwBvAHIAaQBhAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgAHwAIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBJAFMATwBEAEEAVABFAF8AVABPAF8ARQBEAEEAVABFACAAPQAgAEwAQQBNAEIARABBACgASQBTAE8ARABhAHQAZQAsACAAWwBJAG4AYwBsAHUAZABlAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdABdACwAIABbAEYAcgBvAG0ASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0ALABcAG4AIAAgACAAIABJAEYAKABJAFMATwBEAGEAdABlACAAPQAgAFwAIgBcACIALAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcgBlAHQAdQByAG4AVABaAE8ALAAgAE4AKABJAG4AYwBsAHUAZABlAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdAApACAAPAA+ACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgAsACAATgAoAEYAcgBvAG0ASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByACkAIAA8AD4AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AaQBzAG8ARABhAHQAZQAsACAAUABBAFIAUwBFAF8ASQBTAE8AXwBEAEEAVABFACgASQBTAE8ARABhAHQAZQAsACAAXwBqAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABJAFMARQBSAFIATwBSACgASQBOAEQARQBYACgAXwBpAHMAbwBEAGEAdABlACwAIAAxACwAIAAxACkAKQAsACAASQBGACgAXwByAGUAdAB1AHIAbgBUAFoATwAsACAASABTAFQAQQBDAEsAKAB7ACMAVgBBAEwAVQBFACEAfQAsACAAVABBAEsARQAoAF8AaQBzAG8ARABhAHQAZQAsACAAMQAsACAALQAxACkAKQAsACAAewAjAFYAQQBMAFUARQAhAH0AKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGcARABhAHQAZQAsACAASQBGACgAXwBqAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASgBVAEwASQBBAE4AXwBUAE8AXwBHAFIARQBHAE8AUgBJAEEATgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkATgBEAEUAWAAoAF8AaQBzAG8ARABhAHQAZQAsACAAMQAsACAAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBOAEQARQBYACgAXwBpAHMAbwBEAGEAdABlACwAIAAxACwAIAAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAE4ARABFAFgAKABfAGkAcwBvAEQAYQB0AGUALAAgADEALAAgADMAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAEEASwBFACgAXwBpAHMAbwBEAGEAdABlACwAIAAxACwAIAAzACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGUARABhAHQAZQAsACAARABBAFQARQAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAE4ARABFAFgAKABfAGcARABhAHQAZQAsACAAMQAsACAAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkATgBEAEUAWAAoAF8AZwBEAGEAdABlACwAIAAxACwAIAAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBOAEQARQBYACgAXwBnAEQAYQB0AGUALAAgADEALAAgADMAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZQBEAGEAdABlAFQAaQBtAGUALAAgAF8AZQBEAGEAdABlACAAKwAgAEkATgBEAEUAWAAoAF8AaQBzAG8ARABhAHQAZQAsACAAMQAsACAANAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAHIAZQB0AHUAcgBuAFQAWgBPACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBlAEQAYQB0AGUAVABpAG0AZQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkATgBEAEUAWAAoAF8AaQBzAG8ARABhAHQAZQAsACAAMQAsACAANQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBlAEQAYQB0AGUAVABpAG0AZQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEoARABBAFQARQBfAFQATwBfAEkAUwBPAEQAQQBUAEUAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAASQBTAE8AIABmAG8AcgBtAGEAdAAgAGQAYQB0AGUALAAgAHQAaQBtAGUAIABhAG4AZAAgAHQAaQBtAGUAIAB6AG8AbgBlACAAbwBmAGYAcwBlAHQAIABmAHIAbwBtACAAYQAgACAASgB1AGwAaQBhAG4AIABEAGEAdABlAC4AXABuAFwAbgBPAHUAdABwAHUAdABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAHQAZQB4AHQAIAB8ACAASQBTAE8AIABkAGEAdABlAC4AXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBKAEQAYQB0AGUAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAIAAgACAAIAB8ACAASgB1AGwAaQBhAG4AIABEAGEAdABlAC4AIABOAG8AdABlACAASgB1AGwAaQBhAG4AIABEAGEAdABlAHMAIABhAHIAZQAgAGEAbAB3AGEAeQBzACAAaQBuACAAVQBUAEMALgBcAG4AWwBUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQAXQAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgACAAIAAgACAAfAAgAFQAaQBtAGUAIAB6AG8AbgBlACAAbwBmAGYAcwBlAHQAIABpAG4AIABtAGkAbgB1AHQAZQBzACAAZgByAG8AbQAgAFUAVABDAC4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAFsALQA5ADAAMAAuAC4AOQAwADAAXQAgAHwAIABBAHMAcwB1AG0AZQBkACAAdABvACAAYgBlACAAVQBUAEMAIABpAGYAIABvAG0AbQBpAHQAdABlAGQALgBcAG4AWwBQAHIAZQBjAGkAcwBpAG8AbgBdACAAIAAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgACAAIAAgACAAfAAgAFMAZQBsAGUAYwB0ACAAcAByAGUAYwBpAHMAaQBvAG4AIABsAGUAdgBlAGwALAAgAGQAZQBmAGEAdQBsAHQAIABpAHMAIAAzAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADAAIAAtACAARgBsAG8AYQB0AHMAIABmAHIAbwBtACAAbQBpAG4AdQB0AGUAIAB0AG8AIABtAGkAbABsAGkAcwBlAGMAbwBuAGQAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAMQAgAC0AIABEAGEAeQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAyACAALQAgAEgAbwB1AHIAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAMwAgAC0AIABNAGkAbgB1AHQAZQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAA0ACAALQAgAFMAZQBjAG8AbgBkAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADUAIAAtACAATQBpAGwAbABpAHMAZQBjAG8AbgBkAFwAbgBbAE4AbwBaAHUAbAB1AF0AIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABzAHcAaQB0AGMAaAAgACAAIAAgACAAIAB8ACAAVQBzAGUAIAArADAAMAA6ADAAMAAgAGkAbgBzAHQAZQBhAGQAIABvAGYAIABaACAAZgBvAHIAIABVAFQAQwAgAHQAaQBtAGUAIAB6AG8AbgBlAC4AXABuAFsAVABvAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACAAfAAgAHMAdwBpAHQAYwBoACAAIAAgACAAIAAgAHwAIABDAGEAbABjAHUAbABhAHQAZQAgAGYAbwByACAAdABoAGUAIABKAHUAbABpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AIABEAGUAZgBhAHUAbAB0ACAAaQBzACAARwByAGUAZwBvAHIAaQBhAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuACAAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEoARABBAFQARQBfAFQATwBfAEkAUwBPAEQAQQBUAEUAIAA9ACAATABBAE0AQgBEAEEAKABKAEQAYQB0AGUALAAgAFsAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0AF0ALAAgAFsAUAByAGUAYwBpAHMAaQBvAG4AXQAsACAAWwBOAG8AWgB1AGwAdQBdACwAIABbAFQAbwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAsAFwAbgAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIABfAHIARABhAHQAZQAsACAAQwBBAEwARQBOAEQAQQBSAF8ARgBSAE8ATQBfAEoARABBAFQARQAoAEoARABhAHQAZQAsACAAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0ACwAIABQAHIAZQBjAGkAcwBpAG8AbgAsACAAVABvAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgApACwAXABuACAAIAAgACAAIAAgACAAIABGAE8AUgBNAEEAVABfAEkAUwBPAF8ARABBAFQARQAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAE4ARABFAFgAKABfAHIARABhAHQAZQAsACAAMQAsACAAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkATgBEAEUAWAAoAF8AcgBEAGEAdABlACwAIAAxACwAIAAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBOAEQARQBYACgAXwByAEQAYQB0AGUALAAgADEALAAgADMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAE4ARABFAFgAKABfAHIARABhAHQAZQAsACAAMQAsACAANAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABQAHIAZQBjAGkAcwBpAG8AbgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABOAG8AWgB1AGwAdQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAG8ASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ASgBEAE4AXwBMAE8AQwBBAEwAXwBUAE8AXwBJAFMATwBEAEEAVABFAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAEkAUwBPACAAZgBvAHIAbQBhAHQAIABkAGEAdABlACwAIAB0AGkAbQBlACAAYQBuAGQAIAB0AGkAbQBlACAAegBvAG4AZQAgAG8AZgBmAHMAZQB0ACAAZgBvAHIAIAB0AGgAZQAgAHAAcgBvAHYAaQBkAGUAZAAgAEoAdQBsAGkAYQBuACAARABhAHkAIABOAHUAbQBiAGUAcgAgAGEAbgBkACAAbABvAGMAYQBsACAAdABpAG0AZQAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIAB0AGUAeAB0ACAAfAAgAEkAUwBPACAAZABhAHQAZQAuAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ATABvAGMAYQBsAEoARABOACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgACAAIAAgACAAfAAgAEwAbwBjAGEAbAAgAEoAdQBsAGkAYQBuACAARABhAHkAIABOAHUAbQBiAGUAcgAuAFwAbgBMAG8AYwBhAGwAVABpAG0AZQAgACAAIAAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAIAAgACAAIAB8ACAATABvAGMAYQBsACAAdABpAG0AZQAgAG8AZgAgAGQAYQB5ACAAYQBzACAAZABlAGMAaQBtAGEAbAAgAGYAcgBhAGMAdABpAG8AbgAgAG8AZgAgAGEAIABkAGEAeQAgAG8AcgAgAEUAeABjAGUAbAAgAFQAaQBtAGUAIABkAGEAdABhACAAdAB5AHAAZQAuAFwAbgBbAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdABdACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAIAAgACAAIAB8ACAAVABpAG0AZQAgAHoAbwBuAGUAIABvAGYAZgBzAGUAdAAgAGkAbgAgAG0AaQBuAHUAdABlAHMAIABmAHIAbwBtACAAVQBUAEMALgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAWwAtADkAMAAwAC4ALgA5ADAAMABdACAAfAAgAEEAcwBzAHUAbQBlAGQAIAB0AG8AIABiAGUAIABVAFQAQwAgAGkAZgAgAG8AbQBtAGkAdAB0AGUAZAAuAFwAbgBbAFAAcgBlAGMAaQBzAGkAbwBuAF0AIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAIAAgACAAIAB8ACAAUwBlAGwAZQBjAHQAIABwAHIAZQBjAGkAcwBpAG8AbgAgAGwAZQB2AGUAbAAsACAAZABlAGYAYQB1AGwAdAAgAGkAcwAgADMAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAMAAgAC0AIABGAGwAbwBhAHQAcwAgAGYAcgBvAG0AIABtAGkAbgB1AHQAZQAgAHQAbwAgAG0AaQBsAGwAaQBzAGUAYwBvAG4AZABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAxACAALQAgAEQAYQB5AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADIAIAAtACAASABvAHUAcgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAzACAALQAgAE0AaQBuAHUAdABlAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADQAIAAtACAAUwBlAGMAbwBuAGQAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAANQAgAC0AIABNAGkAbABsAGkAcwBlAGMAbwBuAGQAXABuAFsATgBvAFoAdQBsAHUAXQAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAHMAdwBpAHQAYwBoACAAIAAgACAAIAAgAHwAIABVAHMAZQAgACsAMAAwADoAMAAwACAAaQBuAHMAdABlAGEAZAAgAG8AZgAgAFoAIABmAG8AcgAgAFUAVABDACAAdABpAG0AZQAgAHoAbwBuAGUALgBcAG4AWwBUAG8ASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0AIAB8ACAAcwB3AGkAdABjAGgAIAAgACAAIAAgACAAfAAgAEMAYQBsAGMAdQBsAGEAdABlACAAaQBuACAAdABoAGUAIABKAHUAbABpAGEAbgAgAHAAcgBvAGwAZQBwAHQAaQBjACAAYwBhAGwAZQBuAGQAYQByAC4AIABEAGUAZgBhAHUAbAB0ACAAaQBzACAARwByAGUAZwBvAHIAaQBhAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuACAAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEoARABOAF8ATABPAEMAQQBMAF8AVABPAF8ASQBTAE8ARABBAFQARQAgAD0AIABMAEEATQBCAEQAQQAoAEwAbwBjAGEAbABKAEQATgAsACAATABvAGMAYQBsAFQAaQBtAGUALAAgAFsAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0AF0ALAAgAFsAUAByAGUAYwBpAHMAaQBvAG4AXQAsACAAWwBOAG8AWgB1AGwAdQBdACwAIABbAFQAbwBKAHUAbABpAGEAbgBDAGEAbABlAG4AZABhAHIAXQAsAFwAbgAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIABfAGoAZABhAHQAZQAsACAASgBEAE4AXwBMAE8AQwBBAEwAXwBUAE8AXwBKAEQAQQBUAEUAKABMAG8AYwBhAGwASgBEAE4ALAAgAEwAbwBjAGEAbABUAGkAbQBlACwAIABOACgAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0ACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAASgBEAEEAVABFAF8AVABPAF8ASQBTAE8ARABBAFQARQAoAF8AagBkAGEAdABlACwAIABUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQALAAgAFAAcgBlAGMAaQBzAGkAbwBuACwAIABOAG8AWgB1AGwAdQAsACAAVABvAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBFAEQAQQBUAEUAXwBUAE8AXwBJAFMATwBEAEEAVABFAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAEkAUwBPACAAZgBvAHIAbQBhAHQAIABkAGEAdABlACwAIAB0AGkAbQBlACAAYQBuAGQAIAB0AGkAbQBlACAAegBvAG4AZQAgAG8AZgBmAHMAZQB0ACAAZgByAG8AbQAgAGEAbgAgAEUAeABjAGUAbAAgAEQAYQB0AGUALwBUAGkAbQBlAC4AXABuAFwAbgBPAHUAdABwAHUAdABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAHQAZQB4AHQAIAB8ACAASQBTAE8AIABkAGEAdABlAC4AXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBFAEQAYQB0AGUAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAIAAgACAAIAB8ACAARQB4AGMAZQBsACAARABhAHQAZQAvAFQAaQBtAGUALgBcAG4AWwBUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQAXQAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgACAAIAAgACAAfAAgAFQAaQBtAGUAIAB6AG8AbgBlACAAbwBmAGYAcwBlAHQAIABpAG4AIABtAGkAbgB1AHQAZQBzACAAZgByAG8AbQAgAFUAVABDAC4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAFsALQA5ADAAMAAuAC4AOQAwADAAXQAgAHwAIABBAHMAcwB1AG0AZQBkACAAdABvACAAYgBlACAAVQBUAEMAIABpAGYAIABvAG0AbQBpAHQAdABlAGQALgBcAG4AWwBQAHIAZQBjAGkAcwBpAG8AbgBdACAAIAAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgACAAIAAgACAAfAAgAFMAZQBsAGUAYwB0ACAAcAByAGUAYwBpAHMAaQBvAG4AIABsAGUAdgBlAGwALAAgAGQAZQBmAGEAdQBsAHQAIABpAHMAIAAzAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADAAIAAtACAARgBsAG8AYQB0AHMAIABmAHIAbwBtACAAbQBpAG4AdQB0AGUAIAB0AG8AIABtAGkAbABsAGkAcwBlAGMAbwBuAGQAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAMQAgAC0AIABEAGEAeQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAyACAALQAgAEgAbwB1AHIAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAMwAgAC0AIABNAGkAbgB1AHQAZQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAA0ACAALQAgAFMAZQBjAG8AbgBkAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADUAIAAtACAATQBpAGwAbABpAHMAZQBjAG8AbgBkAFwAbgBbAE4AbwBaAHUAbAB1AF0AIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABzAHcAaQB0AGMAaAAgACAAIAAgACAAIAB8ACAAVQBzAGUAIAArADAAMAA6ADAAMAAgAGkAbgBzAHQAZQBhAGQAIABvAGYAIABaACAAZgBvAHIAIABVAFQAQwAgAHQAaQBtAGUAIAB6AG8AbgBlAC4AXABuAFsAVABvAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgBdACAAfAAgAHMAdwBpAHQAYwBoACAAIAAgACAAIAAgAHwAIABDAGEAbABjAHUAbABhAHQAZQAgAGkAbgAgAHQAaABlACAASgB1AGwAaQBhAG4AIABwAHIAbwBsAGUAcAB0AGkAYwAgAGMAYQBsAGUAbgBkAGEAcgAuACAARABlAGYAYQB1AGwAdAAgAGkAcwAgAEcAcgBlAGcAbwByAGkAYQBuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAcAByAG8AbABlAHAAdABpAGMAIABjAGEAbABlAG4AZABhAHIALgAgAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBFAEQAQQBUAEUAXwBUAE8AXwBJAFMATwBEAEEAVABFACAAPQAgAEwAQQBNAEIARABBACgARQBEAGEAdABlACwAIABbAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdABdACwAIABbAFAAcgBlAGMAaQBzAGkAbwBuAF0ALAAgAFsATgBvAFoAdQBsAHUAXQAsACAAWwBUAG8ASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAF0ALABcAG4AIAAgACAAIABJAEYAKABFAEQAYQB0AGUAIAA9ACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEUARABhAHQAZQApACkALAAgAHsAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AGUAYQByAEMARQAsACAAWQBFAEEAUgAoAEUARABhAHQAZQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBtAG8AbgB0AGgALAAgAE0ATwBOAFQASAAoAEUARABhAHQAZQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQAsACAARABBAFkAKABFAEQAYQB0AGUAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcgBEAGEAdABlACwAIABJAEYAKABOACgAVABvAEoAdQBsAGkAYQBuAEMAYQBsAGUAbgBkAGEAcgApACAAPQAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXwB5AGUAYQByAEMARQAsACAAXwBtAG8AbgB0AGgALAAgAF8AZABhAHkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAARwBSAEUARwBPAFIASQBBAE4AXwBUAE8AXwBKAFUATABJAEEATgAoAF8AeQBlAGEAcgBDAEUALAAgAF8AbQBvAG4AdABoACwAIABfAGQAYQB5ACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdABpAG0AZQAsACAATQBPAEQAKABFAEQAYQB0AGUALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEYATwBSAE0AQQBUAF8ASQBTAE8AXwBEAEEAVABFACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAE4ARABFAFgAKABfAHIARABhAHQAZQAsACAAMQAsACAAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAE4ARABFAFgAKABfAHIARABhAHQAZQAsACAAMQAsACAAMgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAE4ARABFAFgAKABfAHIARABhAHQAZQAsACAAMQAsACAAMwApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAaQBtAGUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAUAByAGUAYwBpAHMAaQBvAG4ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAE4AbwBaAHUAbAB1ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAG8ASgB1AGwAaQBhAG4AQwBhAGwAZQBuAGQAYQByAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBFAEQAQQBUAEUAXwBUAE8AXwBKAEQAQQBUAEUAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIABKAHUAbABpAGEAbgAgAEQAYQB0AGUAIABmAG8AcgAgAHQAaABlACAAcAByAG8AdgBpAGQAZQBkACAARQB4AGMAZQBsACAARABhAHQAZQAvAFQAaQBtAGUALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIABKAHUAbABpAGEAbgAgAEQAYQB0AGUALgBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEUARABhAHQAZQAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAAgACAAIAAgAHwAIABFAHgAYwBlAGwAIABEAGEAdABlAC8AVABpAG0AZQAuAFwAbgBbAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdABdACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAIAAgACAAIAB8ACAAVABpAG0AZQAgAHoAbwBuAGUAIABvAGYAZgBzAGUAdAAgAGkAbgAgAG0AaQBuAHUAdABlAHMAIABmAHIAbwBtACAAVQBUAEMALgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAWwAtADkAMAAwAC4ALgA5ADAAMABdACAAfAAgAEEAcwBzAHUAbQBlAGQAIAB0AG8AIABiAGUAIABVAFQAQwAgAGkAZgAgAG8AbQBtAGkAdAB0AGUAZAAuAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBFAEQAQQBUAEUAXwBUAE8AXwBKAEQAQQBUAEUAIAA9ACAATABBAE0AQgBEAEEAKABFAEQAYQB0AGUALAAgAFsAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0AF0ALABcAG4AIAAgACAAIABJAEYAKABFAEQAYQB0AGUAIAA9ACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEUARABhAHQAZQApACkALAAgAHsAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AGUAYQByAEMARQAsACAAWQBFAEEAUgAoAEUARABhAHQAZQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBtAG8AbgB0AGgALAAgAE0ATwBOAFQASAAoAEUARABhAHQAZQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQAsACAARABBAFkAKABFAEQAYQB0AGUAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdABpAG0AZQAsACAATQBPAEQAKABFAEQAYQB0AGUALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEoAVQBMAEkAQQBOAF8ARABBAFQARQAoAF8AeQBlAGEAcgBDAEUALAAgAF8AbQBvAG4AdABoACwAIABfAGQAYQB5ACwAIABfAHQAaQBtAGUALAAgAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdAAsACAAMAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ARQBEAEEAVABFAF8AVABPAF8ASgBEAE4AXwBMAE8AQwBBAEwAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIABKAHUAbABpAGEAbgAgAEQAYQB5ACAATgB1AG0AYgBlAHIAIABhAG4AZAAgAGwAbwBjAGEAbAAgAHQAaQBtAGUAIABmAG8AcgAgAHQAaABlACAAcAByAG8AdgBpAGQAZQBkACAARQB4AGMAZQBsACAARABhAHQAZQAvAFQAaQBtAGUALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAaQBuAHQAZQBnAGUAcgAgACAAIAAgACAAIAAgACAAfAAgAEwAbwBjAGEAbAAgAEoAdQBsAGkAYQBuACAARABhAHkAIABOAHUAbQBiAGUAcgBcAG4AIAAyACAAfAAgAGQAZQBjAGkAbQBhAGwAIABbADAALgAuADEAKQAgAHwAIABMAG8AYwBhAGwAIAB0AGkAbQBlACAAbwBmACAAZABhAHkALgAgAEQAZQBjAGkAbQBhAGwAIABmAHIAYQBjAHQAaQBvAG4AIABvAGYAIABhACAAZABhAHkALAAgAGkAbQBwAGwAaQBjAGkAdABsAHkAIABjAG8AbgB2AGUAcgB0AHMAIAB0AG8AIABFAHgAYwBlAGwAIABEAGEAdABlAC8AVABpAG0AZQAgAHQAeQBwAGUALgBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEUARABhAHQAZQAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgAEUAeABjAGUAbAAgAEQAYQB0AGUALwBUAGkAbQBlAC4AXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEUARABBAFQARQBfAFQATwBfAEoARABOAF8ATABPAEMAQQBMACAAPQAgAEwAQQBNAEIARABBACgARQBEAGEAdABlACwAXABuACAAIAAgACAASQBGACgARQBEAGEAdABlACAAPQAgAFwAIgBcACIALAAgAHsAXAAiAFwAIgAsACAAXAAiAFwAIgB9ACwAIABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgARQBEAGEAdABlACkAKQAsACAAewAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhAH0ALAAgAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AeQBlAGEAcgBDAEUALAAgAFkARQBBAFIAKABFAEQAYQB0AGUAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbQBvAG4AdABoACwAIABNAE8ATgBUAEgAKABFAEQAYQB0AGUAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkALAAgAEQAQQBZACgARQBEAGEAdABlACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAaQBtAGUALAAgAE0ATwBEACgARQBEAGEAdABlACwAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGoAZABuACwAIABKAFUATABJAEEATgBfAEQAQQBZAF8ATgBVAE0AQgBFAFIAKABfAHkAZQBhAHIAQwBFACwAIABfAG0AbwBuAHQAaAAsACAAXwBkAGEAeQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABfAGoAZABuACwAIABfAHQAaQBtAGUAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEoARABOAF8ATABPAEMAQQBMAF8AVABPAF8ARQBEAEEAVABFAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAGEAbgAgAEUAeABjAGUAbAAgAEQAYQB0AGUALwBUAGkAbQBlACAAZgBvAHIAIAB0AGgAZQAgAHAAcgBvAHYAaQBkAGUAZAAgAEoAdQBsAGkAYQBuACAARABhAHkAIABOAHUAbQBiAGUAcgAgAGEAbgBkACAAbABvAGMAYQBsACAAdABpAG0AZQAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgAEUAeABjAGUAbAAgAEQAYQB0AGUALwBUAGkAbQBlAC4AXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBMAG8AYwBhAGwASgBEAE4AIAAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIABMAG8AYwBhAGwAIABKAHUAbABpAGEAbgAgAEQAYQB5ACAATgB1AG0AYgBlAHIALgBcAG4ATABvAGMAYQBsAFQAaQBtAGUAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAATABvAGMAYQBsACAAdABpAG0AZQAgAG8AZgAgAGQAYQB5ACAAYQBzACAAZABlAGMAaQBtAGEAbAAgAGYAcgBhAGMAdABpAG8AbgAgAG8AZgAgAGEAIABkAGEAeQAgAG8AcgAgAEUAeABjAGUAbAAgAEQAYQB0AGUALwBUAGkAbQBlACAAdAB5AHAAZQAuAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBKAEQATgBfAEwATwBDAEEATABfAFQATwBfAEUARABBAFQARQAgAD0AIABMAEEATQBCAEQAQQAoAEwAbwBjAGEAbABKAEQATgAsACAATABvAGMAYQBsAFQAaQBtAGUALABcAG4AIAAgACAAIABJAEYAKAAoAEwAbwBjAGEAbABKAEQATgAgAD0AIABcACIAXAAiACkAIAAqACAAKABMAG8AYwBhAGwAVABpAG0AZQAgAD0AIABcACIAXAAiACkALAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgATABvAGMAYQBsAEoARABOACkAKQAgACsAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEwAbwBjAGEAbABUAGkAbQBlACkAKQAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgATQBPAEQAKABMAG8AYwBhAGwASgBEAE4ALAAgADEAKQAgAD4AIAAwACwAIAB7ACMATgBVAE0AIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcgBEAGEAdABlACwAIABKAEQATgBfAFQATwBfAEMAQQBMAEUATgBEAEEAUgBfAEQAQQBUAEUAKABMAG8AYwBhAGwASgBEAE4AKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBlAEQAYQB0AGUALAAgAEQAQQBUAEUAKABJAE4ARABFAFgAKABfAHIARABhAHQAZQAsACAAMQAsACAAMQApACwAIABJAE4ARABFAFgAKABfAHIARABhAHQAZQAsACAAMQAsACAAMgApACwAIABJAE4ARABFAFgAKABfAHIARABhAHQAZQAsACAAMQAsACAAMwApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZQBEAGEAdABlACAAKwAgAEwAbwBjAGEAbABUAGkAbQBlAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBKAEQAQQBUAEUAXwBUAE8AXwBFAEQAQQBUAEUAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAYQBuACAARQB4AGMAZQBsACAARABhAHQAZQAvAFQAaQBtAGUAIABmAG8AcgAgAHQAaABlACAAcAByAG8AdgBpAGQAZQBkACAASgB1AGwAaQBhAG4AIABEAGEAdABlAC4AXABuAFwAbgBPAHUAdABwAHUAdABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAARQB4AGMAZQBsACAARABhAHQAZQAvAFQAaQBtAGUALgBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEoARABhAHQAZQAgACAAIAAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAIAAgACAAIAB8ACAASgB1AGwAaQBhAG4AIABEAGEAdABlAFwAbgBUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQAIAB8ACAAZABlAGMAaQBtAGEAbAAgACAAIAAgACAAfAAgAFQAaQBtAGUAIAB6AG8AbgBlACAAbwBmAGYAcwBlAHQAIABpAG4AIABtAGkAbgB1AHQAZQBzACAAZgByAG8AbQAgAFUAVABDAC4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABbAC0AOQAwADAALgAuADkAMAAwAF0AIAB8ACAAQQBzAHMAdQBtAGUAZAAgAHQAbwAgAGIAZQAgAFUAVABDACAAaQBmACAAbwBtAG0AaQB0AHQAZQBkAC4AXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEoARABBAFQARQBfAFQATwBfAEUARABBAFQARQAgAD0AIABMAEEATQBCAEQAQQAoAEoARABhAHQAZQAsACAAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0ACwAXABuACAAIAAgACAASQBGACgASgBEAGEAdABlACAAPQAgAFwAIgBcACIALAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgASgBEAGEAdABlACkAKQAsACAAewAjAFYAQQBMAFUARQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGoAZABuAEwAbwBjAGEAbAAsACAASgBEAEEAVABFAF8AVABPAF8ASgBEAE4AXwBMAE8AQwBBAEwAKABKAEQAYQB0AGUALAAgAE4AKABUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASgBEAE4AXwBMAE8AQwBBAEwAXwBUAE8AXwBFAEQAQQBUAEUAKABJAE4ARABFAFgAKABfAGoAZABuAEwAbwBjAGEAbAAsACAAMQAsACAAMQApACwAIABJAE4ARABFAFgAKABfAGoAZABuAEwAbwBjAGEAbAAsACAAMQAsACAAMgApACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBVAFMARABBAFQARQBfAFQATwBfAEUARABBAFQARQBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIABhAG4AIABFAHgAYwBlAGwAIABEAGEAdABlAC8AVABpAG0AZQAgAGYAbwByACAAdABoAGUAIABwAHIAbwB2AGkAZABlAGQAIABVAFMAIABmAG8AcgBtAGEAdAAgAGQAYQB0AGUAIABhAG4AZAAgAHQAaQBtAGUALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIABFAHgAYwBlAGwAIABEAGEAdABlAC8AVABpAG0AZQAuAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AVQBTAEQAYQB0AGUAIAB8ACAAdABlAHgAdAAgAHwAIABEAGEAdABlACAAaQBuACAAVQBTACAAZgBvAHIAbQBhAHQAIABpAGUALgAgAE0ATQAvAGQAZAAvAHkAeQB5AHkAIABoAGgAOgBtAG0AOgBzAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAFUAUwBEAEEAVABFAF8AVABPAF8ARQBEAEEAVABFACAAPQAgAEwAQQBNAEIARABBACgAVQBTAEQAYQB0AGUALABcAG4AIAAgACAAIABJAEYAKABVAFMARABhAHQAZQAgAD0AIABcACIAXAAiACwAIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAFUAUwBEAGEAdABlACwAIABQAEEAUgBTAEUAXwBVAFMAXwBEAEEAVABFACgAVQBTAEQAYQB0AGUAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAaQBtAGUALAAgAEkATgBEAEUAWAAoAF8AVQBTAEQAYQB0AGUALAAgADEALAAgADQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIALAAgAEkATgBEAEUAWAAoAF8AVQBTAEQAYQB0AGUALAAgADEALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGUARABhAHQAZQAsACAASQBGACgAXwB5AGUAYQByACAAPQAgAFwAIgBcACIALAAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABEAEEAVABFACgAXwB5AGUAYQByACwAIABJAE4ARABFAFgAKABfAFUAUwBEAGEAdABlACwAIAAxACwAIAAyACkALAAgAEkATgBEAEUAWAAoAF8AVQBTAEQAYQB0AGUALAAgADEALAAgADMAKQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZQBEAGEAdABlACAAKwAgAF8AdABpAG0AZQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEUARABBAFQARQBfAFQATwBfAFUAUwBEAEEAVABFAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAGEAIABVAFMAIABmAG8AcgBtAGEAdAAgAGQAYQB0AGUAIABhAG4AZAAgAHQAaQBtAGUAIABmAG8AcgAgAHQAaABlACAAcAByAG8AdgBpAGQAZQBkACAARQB4AGMAZQBsACAARABhAHQAZQAvAFQAaQBtAGUALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAdABlAHgAdAAgAHwAIABVAFMAIABmAG8AcgBtAGEAdAAgAGQAYQB0AGUAIABhAG4AZAAgAHQAaQBtAGUAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBFAEQAYQB0AGUAIAAgACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgACAAIAAgACAAIAB8ACAARQB4AGMAZQBsACAARABhAHQAZQAvAFQAaQBtAGUALgBcAG4AWwBTAGUAcABhAHIAYQB0AG8AcgBdACAAfAAgAGMAaABhAHIAIABbACwALgAvAC0AXwBdACAAfAAgAEMAaABhAHIAYQBjAHQAZQByACAAcwBlAHAAYQByAGEAdABvAHIAIABmAG8AcgAgAGQAYQB0AGUAIABlAGwAZQBtAGUAbgB0AHMALgBcAG4AWwBQAHIAZQBjAGkAcwBpAG8AbgBdACAAfAAgAGkAbgB0AGUAZwBlAHIAIAAgACAAIAAgACAAfAAgAFMAZQBsAGUAYwB0ACAAcAByAGUAYwBpAHMAaQBvAG4AIABsAGUAdgBlAGwALAAgAGQAZQBmAGEAdQBsAHQAIABpAHMAIAAzAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADAAIAAtACAARgBsAG8AYQB0AHMAIABmAHIAbwBtACAAbQBpAG4AdQB0AGUAIAB0AG8AIABtAGkAbABsAGkAcwBlAGMAbwBuAGQAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAMQAgAC0AIABEAGEAeQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAyACAALQAgAEgAbwB1AHIAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAMwAgAC0AIABNAGkAbgB1AHQAZQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAA0ACAALQAgAFMAZQBjAG8AbgBkAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADUAIAAtACAATQBpAGwAbABpAHMAZQBjAG8AbgBkAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBFAEQAQQBUAEUAXwBUAE8AXwBVAFMARABBAFQARQAgAD0AIABMAEEATQBCAEQAQQAoAEUARABhAHQAZQAsACAAWwBTAGUAcABhAHIAYQB0AG8AcgBdACwAIABbAFAAcgBlAGMAaQBzAGkAbwBuAF0ALABcAG4AIAAgACAAIABJAEYAKABFAEQAYQB0AGUAIAA9ACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEUARABhAHQAZQApACkALAAgAHsAIwBWAEEATABVAEUAIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AGUAYQByAEMARQAsACAAWQBFAEEAUgAoAEUARABhAHQAZQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBtAG8AbgB0AGgALAAgAE0ATwBOAFQASAAoAEUARABhAHQAZQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQAsACAARABBAFkAKABFAEQAYQB0AGUAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdABpAG0AZQAsACAATQBPAEQAKABFAEQAYQB0AGUALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEYATwBSAE0AQQBUAF8AVQBTAF8ARABBAFQARQAoAF8AeQBlAGEAcgBDAEUALAAgAF8AbQBvAG4AdABoACwAIABfAGQAYQB5ACwAIABfAHQAaQBtAGUALAAgAFMAZQBwAGEAcgBhAHQAbwByACwAIABQAHIAZQBjAGkAcwBpAG8AbgAsACAAMAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4AXABuAC8AKgAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAXABuACMAIABFAE4ARAAgAEMAQQBMAEUATgBEAEEAUgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAqAC8AXABuACIAfQBdACwAIgBwAHIAbwBqAGUAYwB0AE4AYQBtAGUAcwAiADoAWwAiAEMAQQBMAEUATgBEAEEAUgAuAEkAUwBfAEwARQBBAFAAXwBZAEUAQQBSACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAEkAUwBfAFYAQQBMAEkARABfAEQAQQBUAEUAIgAsACIAQwBBAEwARQBOAEQAQQBSAC4ASQBTAF8AVgBBAEwASQBEAF8AVABJAE0ARQAiACwAIgBDAEEATABFAE4ARABBAFIALgBZAEUAQQBSAF8AQwBPAE0ATQBPAE4AXwBFAFIAQQAiACwAIgBDAEEATABFAE4ARABBAFIALgBEAEEAWQBTAF8ASQBOAF8AWQBFAEEAUgAiACwAIgBDAEEATABFAE4ARABBAFIALgBEAEEAWQBTAF8ASQBOAF8ATQBPAE4AVABIACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAEoAVQBMAEkAQQBOAF8ARABBAFkAXwBOAFUATQBCAEUAUgAiACwAIgBDAEEATABFAE4ARABBAFIALgBKAEQATgBfAFQATwBfAEMAQQBMAEUATgBEAEEAUgBfAEQAQQBUAEUAIgAsACIAQwBBAEwARQBOAEQAQQBSAC4ASgBEAE4AXwBUAE8AXwBPAFIARABJAE4AQQBMAF8ARABBAFQARQAiACwAIgBDAEEATABFAE4ARABBAFIALgBPAFIARABJAE4AQQBMAF8ARABBAFQARQBfAFQATwBfAEoARABOACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAEcAUgBFAEcATwBSAEkAQQBOAF8AVABPAF8ASgBVAEwASQBBAE4AIgAsACIAQwBBAEwARQBOAEQAQQBSAC4ASgBVAEwASQBBAE4AXwBUAE8AXwBHAFIARQBHAE8AUgBJAEEATgAiACwAIgBDAEEATABFAE4ARABBAFIALgBTAEUAQwBVAEwAQQBSAF8ARABJAEYARgBFAFIARQBOAEMARQAiACwAIgBDAEEATABFAE4ARABBAFIALgBEAEEAWQBfAE8ARgBfAFcARQBFAEsAIgAsACIAQwBBAEwARQBOAEQAQQBSAC4AQwBPAE4AVgBFAFIAVABfAFcARQBFAEsARABBAFkAXwBOAFUATQBCAEUAUgAiACwAIgBDAEEATABFAE4ARABBAFIALgBXAEUARQBLAEQAQQBZAF8ATwBGAF8ATQBPAE4AVABIACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAFcARQBFAEsAUwBfAEkATgBfAFkARQBBAFIAIgAsACIAQwBBAEwARQBOAEQAQQBSAC4AVwBFAEUASwBfAEQAQQBUAEUAXwBUAE8AXwBKAEQATgAiACwAIgBDAEEATABFAE4ARABBAFIALgBKAEQATgBfAFQATwBfAFcARQBFAEsAXwBEAEEAVABFACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAFcARQBFAEsAXwBOAFUATQBCAEUAUgAiACwAIgBDAEEATABFAE4ARABBAFIALgBEAEEAWQBTAF8ASQBOAF8AUQBVAEEAUgBUAEUAUgAiACwAIgBDAEEATABFAE4ARABBAFIALgBRAFUAQQBSAFQARQBSAF8ARABBAFQARQBfAFQATwBfAEoARABOACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAEoARABOAF8AVABPAF8AUQBVAEEAUgBUAEUAUgBfAEQAQQBUAEUAIgAsACIAQwBBAEwARQBOAEQAQQBSAC4ASgBEAE4AXwBVAFQAQwBfAFQATwBfAEoARABBAFQARQAiACwAIgBDAEEATABFAE4ARABBAFIALgBKAEQATgBfAEwATwBDAEEATABfAFQATwBfAEoARABBAFQARQAiACwAIgBDAEEATABFAE4ARABBAFIALgBKAEQAQQBUAEUAXwBUAE8AXwBKAEQATgBfAFUAVABDACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAEoARABBAFQARQBfAFQATwBfAEoARABOAF8ATABPAEMAQQBMACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAEoAVQBMAEkAQQBOAF8ARABBAFQARQAiACwAIgBDAEEATABFAE4ARABBAFIALgBDAEEATABFAE4ARABBAFIAXwBGAFIATwBNAF8ASgBEAEEAVABFACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAFQASQBNAEUAXwBEAEUAQwBJAE0AQQBMAF8AVABPAF8ASABNAFMAIgAsACIAQwBBAEwARQBOAEQAQQBSAC4ASABNAFMAXwBUAE8AXwBUAEkATQBFAF8ARABFAEMASQBNAEEATAAiACwAIgBDAEEATABFAE4ARABBAFIALgBBAEQARABfAFQASQBNAEUAUwBQAEEATgAiACwAIgBDAEEATABFAE4ARABBAFIALgBSAEUAUwBPAEwAVgBFAF8ARABBAFQARQAiACwAIgBDAEEATABFAE4ARABBAFIALgBEAEUATABUAEEAXwBIAE8AVQBSAFMAIgAsACIAQwBBAEwARQBOAEQAQQBSAC4ARABFAEwAVABBAF8ATQBJAE4AVQBUAEUAUwAiACwAIgBDAEEATABFAE4ARABBAFIALgBEAEUATABUAEEAXwBTAEUAQwBPAE4ARABTACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAEQARQBMAFQAQQBfAEgATwBVAFIAXwBNAEkATgBfAFMARQBDACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAEQARQBMAFQAQQBfAEQAQQBZAFMAIgAsACIAQwBBAEwARQBOAEQAQQBSAC4ARABFAEwAVABBAF8AVwBFAEUASwBTACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAEQARQBMAFQAQQBfAE0ATwBOAFQASABTACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAEQARQBMAFQAQQBfAFEAVQBBAFIAVABFAFIAUwAiACwAIgBDAEEATABFAE4ARABBAFIALgBEAEUATABUAEEAXwBZAEUAQQBSAFMAIgAsACIAQwBBAEwARQBOAEQAQQBSAC4ARABFAEwAVABBAF8AVwBFAEUASwBfAEQAQQBZAFMAIgAsACIAQwBBAEwARQBOAEQAQQBSAC4ARABFAEwAVABBAF8AWQBFAEEAUgBfAFcARQBFAEsAXwBEAEEAWQBTACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAEQARQBMAFQAQQBfAE0ATwBOAFQASABfAEQAQQBZAFMAIgAsACIAQwBBAEwARQBOAEQAQQBSAC4ARABFAEwAVABBAF8AUQBVAEEAUgBUAEUAUgBfAEQAQQBZAFMAIgAsACIAQwBBAEwARQBOAEQAQQBSAC4ARABFAEwAVABBAF8ASQBOAFQARQBSAFYAQQBMACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAEUAWABUAEUATgBUAF8ATwBGAF8ARABBAFkAUwAiACwAIgBDAEEATABFAE4ARABBAFIALgBFAFgAVABFAE4AVABfAE8ARgBfAFcARQBFAEsAUwAiACwAIgBDAEEATABFAE4ARABBAFIALgBFAFgAVABFAE4AVABfAE8ARgBfAE0ATwBOAFQASABTACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAEUAWABUAEUATgBUAF8ATwBGAF8AUQBVAEEAUgBUAEUAUgBTACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAEUAWABUAEUATgBUAF8ATwBGAF8AWQBFAEEAUgBTACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAFAAQQBSAFMARQBfAEkAUwBPAF8ARABBAFQARQAiACwAIgBDAEEATABFAE4ARABBAFIALgBQAEEAUgBTAEUAXwBXAEUARQBLAEQAQQBZACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAFAAQQBSAFMARQBfAE0ATwBOAFQASAAiACwAIgBDAEEATABFAE4ARABBAFIALgBQAEEAUgBTAEUAXwBMAEkAVABFAFIAQQBSAFkAXwBZAEUAQQBSACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAFAAQQBSAFMARQBfAEwASQBUAEUAUgBBAFIAWQBfAEQAQQBUAEUAIgAsACIAQwBBAEwARQBOAEQAQQBSAC4AUABBAFIAUwBFAF8AVQBTAF8ARABBAFQARQAiACwAIgBDAEEATABFAE4ARABBAFIALgBQAEEAUgBTAEUAXwBNAEkATABfAEQAVABHACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAFcARQBFAEsARABBAFkAXwBOAEEATQBFACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAE0ATwBOAFQASABfAE4AQQBNAEUAIgAsACIAQwBBAEwARQBOAEQAQQBSAC4ARgBPAFIATQBBAFQAXwBJAFMATwBfAEQAQQBUAEUAIgAsACIAQwBBAEwARQBOAEQAQQBSAC4ARgBPAFIATQBBAFQAXwBMAEkAVABFAFIAQQBSAFkAXwBZAEUAQQBSACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAEYATwBSAE0AQQBUAF8ATABJAFQARQBSAEEAUgBZAF8ARABBAFQARQAiACwAIgBDAEEATABFAE4ARABBAFIALgBGAE8AUgBNAEEAVABfAFUAUwBfAEQAQQBUAEUAIgAsACIAQwBBAEwARQBOAEQAQQBSAC4ARgBPAFIATQBBAFQAXwBNAEkATABfAEQAVABHACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAEkAUwBPAEQAQQBUAEUAXwBUAE8AXwBKAEQATgBfAEwATwBDAEEATAAiACwAIgBDAEEATABFAE4ARABBAFIALgBJAFMATwBEAEEAVABFAF8AVABPAF8ASgBEAEEAVABFACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAEkAUwBPAEQAQQBUAEUAXwBUAE8AXwBFAEQAQQBUAEUAIgAsACIAQwBBAEwARQBOAEQAQQBSAC4ASgBEAEEAVABFAF8AVABPAF8ASQBTAE8ARABBAFQARQAiACwAIgBDAEEATABFAE4ARABBAFIALgBKAEQATgBfAEwATwBDAEEATABfAFQATwBfAEkAUwBPAEQAQQBUAEUAIgAsACIAQwBBAEwARQBOAEQAQQBSAC4ARQBEAEEAVABFAF8AVABPAF8ASQBTAE8ARABBAFQARQAiACwAIgBDAEEATABFAE4ARABBAFIALgBFAEQAQQBUAEUAXwBUAE8AXwBKAEQAQQBUAEUAIgAsACIAQwBBAEwARQBOAEQAQQBSAC4ARQBEAEEAVABFAF8AVABPAF8ASgBEAE4AXwBMAE8AQwBBAEwAIgAsACIAQwBBAEwARQBOAEQAQQBSAC4ASgBEAE4AXwBMAE8AQwBBAEwAXwBUAE8AXwBFAEQAQQBUAEUAIgAsACIAQwBBAEwARQBOAEQAQQBSAC4ASgBEAEEAVABFAF8AVABPAF8ARQBEAEEAVABFACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAFUAUwBEAEEAVABFAF8AVABPAF8ARQBEAEEAVABFACIALAAiAEMAQQBMAEUATgBEAEEAUgAuAEUARABBAFQARQBfAFQATwBfAFUAUwBEAEEAVABFACIAXQAsACIAbABvAGMAYQBsAGUAIgA6AHsAIgBsAGkAcwB0AFMAZQBwAGEAcgBhAHQAbwByACIAOgAiACwAIgAsACIAcgBvAHcAUwBlAHAAYQByAGEAdABvAHIAIgA6ACIAOwAiACwAIgBjAG8AbAB1AG0AbgBTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHQAaABvAHUAcwBhAG4AZABzAFMAZQBwAGEAcgBhAHQAbwByACIAOgAiACwAIgAsACIAdABoAG8AdQBzAGEAbgBkAHMAUABvAHMAaQB0AGkAbwBuAHMAIgA6AFsAMwBdACwAIgBkAGUAYwBpAG0AYQBsAFMAZQBwAGEAcgBhAHQAbwByACIAOgAiAC4AIgAsACIAZABhAHQAZQBPAHIAZABlAHIAIgA6ACIARABNAFkAIgAsACIAYwB1AHIAcgBlAG4AYwB5AFMAeQBtAGIAbwBsACIAOgAiACQAIgAsACIAaQBzAEMAdQByAHIAZQBuAGMAeQBTAHkAbQBiAG8AbABMAGUAYQBkACIAOgB0AHIAdQBlACwAIgBpAHMAQwB1AHIAcgBlAG4AYwB5AFMAZQBwAEIAeQBTAHAAYQBjAGUAIgA6AGYAYQBsAHMAZQAsACIAcgBvAHcATABlAHQAdABlAHIAIgA6ACIAUgAiACwAIgBjAG8AbAB1AG0AbgBMAGUAdAB0AGUAcgAiADoAIgBDACIALAAiAHIAYwBMAGUAZgB0AEIAcgBhAGMAawBlAHQAIgA6ACIAWwAiACwAIgByAGMAUgBpAGcAaAB0AEIAcgBhAGMAawBlAHQAIgA6ACIAXQAiACwAIgBzAHQAYQB0AGUAbQBlAG4AdABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgA7ACIALAAiAGwAbwBjAGEAbABlAE4AYQBtAGUAIgA6ACIAZQBuAC0AdQBzACIAfQB9AA==</AFEJSONBlob>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>